<commit_message>
[Fonds de solidarite] Add 2020-05-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1155,10 +1155,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>9381</v>
+        <v>9414</v>
       </c>
       <c r="D2">
-        <v>11981531</v>
+        <v>12024389</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1251,10 +1251,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>3969</v>
+        <v>3984</v>
       </c>
       <c r="D5">
-        <v>5852242</v>
+        <v>5874148</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -1315,10 +1315,10 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>1980</v>
+        <v>1986</v>
       </c>
       <c r="D7">
-        <v>2879233</v>
+        <v>2887161</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1443,10 +1443,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>6516</v>
+        <v>6526</v>
       </c>
       <c r="D11">
-        <v>8291101</v>
+        <v>8302848</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1539,10 +1539,10 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>2141</v>
+        <v>2145</v>
       </c>
       <c r="D14">
-        <v>3147069</v>
+        <v>3153069</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1603,10 +1603,10 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="D16">
-        <v>1269273</v>
+        <v>1273773</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1699,10 +1699,10 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>8588</v>
+        <v>8599</v>
       </c>
       <c r="D19">
-        <v>10715685</v>
+        <v>10729151</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1795,10 +1795,10 @@
         <v>11</v>
       </c>
       <c r="C22">
-        <v>3181</v>
+        <v>3188</v>
       </c>
       <c r="D22">
-        <v>4686226</v>
+        <v>4696461</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1859,10 +1859,10 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="D24">
-        <v>1496428</v>
+        <v>1501072</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1955,10 +1955,10 @@
         <v>11</v>
       </c>
       <c r="C27">
-        <v>3364</v>
+        <v>3373</v>
       </c>
       <c r="D27">
-        <v>4467298</v>
+        <v>4479900</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -2019,10 +2019,10 @@
         <v>11</v>
       </c>
       <c r="C29">
-        <v>1039</v>
+        <v>1042</v>
       </c>
       <c r="D29">
-        <v>1518879</v>
+        <v>1522212</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2083,10 +2083,10 @@
         <v>11</v>
       </c>
       <c r="C31">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D31">
-        <v>488759</v>
+        <v>491759</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2115,10 +2115,10 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D32">
-        <v>340069</v>
+        <v>343069</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2211,10 +2211,10 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <v>13308</v>
+        <v>13326</v>
       </c>
       <c r="D35">
-        <v>16662388</v>
+        <v>16681856</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2339,10 +2339,10 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>5221</v>
+        <v>5233</v>
       </c>
       <c r="D39">
-        <v>7702305</v>
+        <v>7718471</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2403,10 +2403,10 @@
         <v>11</v>
       </c>
       <c r="C41">
-        <v>2441</v>
+        <v>2446</v>
       </c>
       <c r="D41">
-        <v>3551502</v>
+        <v>3558476</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2499,10 +2499,10 @@
         <v>11</v>
       </c>
       <c r="C44">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D44">
-        <v>259255</v>
+        <v>260755</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2531,10 +2531,10 @@
         <v>11</v>
       </c>
       <c r="C45">
-        <v>5121</v>
+        <v>5127</v>
       </c>
       <c r="D45">
-        <v>6636165</v>
+        <v>6642512</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2627,10 +2627,10 @@
         <v>11</v>
       </c>
       <c r="C48">
-        <v>1807</v>
+        <v>1812</v>
       </c>
       <c r="D48">
-        <v>2643659</v>
+        <v>2651159</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2691,10 +2691,10 @@
         <v>11</v>
       </c>
       <c r="C50">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D50">
-        <v>924712</v>
+        <v>927712</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2787,10 +2787,10 @@
         <v>11</v>
       </c>
       <c r="C53">
-        <v>21792</v>
+        <v>21840</v>
       </c>
       <c r="D53">
-        <v>28520201</v>
+        <v>28577087</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2851,10 +2851,10 @@
         <v>11</v>
       </c>
       <c r="C55">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D55">
-        <v>77798</v>
+        <v>79298</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2883,10 +2883,10 @@
         <v>11</v>
       </c>
       <c r="C56">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D56">
-        <v>64500</v>
+        <v>66000</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2915,10 +2915,10 @@
         <v>11</v>
       </c>
       <c r="C57">
-        <v>8263</v>
+        <v>8286</v>
       </c>
       <c r="D57">
-        <v>12205946</v>
+        <v>12238775</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2979,10 +2979,10 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>3130</v>
+        <v>3137</v>
       </c>
       <c r="D59">
-        <v>4553667</v>
+        <v>4564167</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -3139,10 +3139,10 @@
         <v>11</v>
       </c>
       <c r="C64">
-        <v>27787</v>
+        <v>27831</v>
       </c>
       <c r="D64">
-        <v>35929808</v>
+        <v>35984108</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -3203,10 +3203,10 @@
         <v>11</v>
       </c>
       <c r="C66">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D66">
-        <v>20984</v>
+        <v>23145</v>
       </c>
       <c r="E66" t="s">
         <v>12</v>
@@ -3235,10 +3235,10 @@
         <v>11</v>
       </c>
       <c r="C67">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D67">
-        <v>71061</v>
+        <v>72006</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
@@ -3267,10 +3267,10 @@
         <v>11</v>
       </c>
       <c r="C68">
-        <v>12148</v>
+        <v>12168</v>
       </c>
       <c r="D68">
-        <v>17918348</v>
+        <v>17946876</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -3331,10 +3331,10 @@
         <v>11</v>
       </c>
       <c r="C70">
-        <v>5779</v>
+        <v>5793</v>
       </c>
       <c r="D70">
-        <v>8405567</v>
+        <v>8425217</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
@@ -3363,10 +3363,10 @@
         <v>11</v>
       </c>
       <c r="C71">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D71">
-        <v>259663</v>
+        <v>262218</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
@@ -3427,10 +3427,10 @@
         <v>11</v>
       </c>
       <c r="C73">
-        <v>15153</v>
+        <v>15189</v>
       </c>
       <c r="D73">
-        <v>19427215</v>
+        <v>19466677</v>
       </c>
       <c r="E73" t="s">
         <v>12</v>
@@ -3491,10 +3491,10 @@
         <v>11</v>
       </c>
       <c r="C75">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D75">
-        <v>106648</v>
+        <v>108148</v>
       </c>
       <c r="E75" t="s">
         <v>12</v>
@@ -3523,10 +3523,10 @@
         <v>11</v>
       </c>
       <c r="C76">
-        <v>5839</v>
+        <v>5843</v>
       </c>
       <c r="D76">
-        <v>8631945</v>
+        <v>8637945</v>
       </c>
       <c r="E76" t="s">
         <v>12</v>
@@ -3587,10 +3587,10 @@
         <v>11</v>
       </c>
       <c r="C78">
-        <v>3106</v>
+        <v>3112</v>
       </c>
       <c r="D78">
-        <v>4523833</v>
+        <v>4532833</v>
       </c>
       <c r="E78" t="s">
         <v>12</v>
@@ -3683,10 +3683,10 @@
         <v>11</v>
       </c>
       <c r="C81">
-        <v>13009</v>
+        <v>13030</v>
       </c>
       <c r="D81">
-        <v>16518885</v>
+        <v>16545789</v>
       </c>
       <c r="E81" t="s">
         <v>12</v>
@@ -3811,10 +3811,10 @@
         <v>11</v>
       </c>
       <c r="C85">
-        <v>5924</v>
+        <v>5933</v>
       </c>
       <c r="D85">
-        <v>8720545</v>
+        <v>8734045</v>
       </c>
       <c r="E85" t="s">
         <v>12</v>
@@ -3843,10 +3843,10 @@
         <v>11</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D86">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E86" t="s">
         <v>12</v>
@@ -3875,10 +3875,10 @@
         <v>11</v>
       </c>
       <c r="C87">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="D87">
-        <v>2889874</v>
+        <v>2896407</v>
       </c>
       <c r="E87" t="s">
         <v>12</v>
@@ -4003,10 +4003,10 @@
         <v>11</v>
       </c>
       <c r="C91">
-        <v>42760</v>
+        <v>42840</v>
       </c>
       <c r="D91">
-        <v>55119033</v>
+        <v>55218537</v>
       </c>
       <c r="E91" t="s">
         <v>12</v>
@@ -4163,10 +4163,10 @@
         <v>11</v>
       </c>
       <c r="C96">
-        <v>20011</v>
+        <v>20047</v>
       </c>
       <c r="D96">
-        <v>29574252</v>
+        <v>29628063</v>
       </c>
       <c r="E96" t="s">
         <v>12</v>
@@ -4227,10 +4227,10 @@
         <v>11</v>
       </c>
       <c r="C98">
-        <v>12472</v>
+        <v>12491</v>
       </c>
       <c r="D98">
-        <v>18101714</v>
+        <v>18129389</v>
       </c>
       <c r="E98" t="s">
         <v>12</v>
@@ -4387,10 +4387,10 @@
         <v>11</v>
       </c>
       <c r="C103">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D103">
-        <v>1044083</v>
+        <v>1047683</v>
       </c>
       <c r="E103" t="s">
         <v>12</v>
@@ -4419,10 +4419,10 @@
         <v>11</v>
       </c>
       <c r="C104">
-        <v>17514</v>
+        <v>17544</v>
       </c>
       <c r="D104">
-        <v>23459758</v>
+        <v>23498878</v>
       </c>
       <c r="E104" t="s">
         <v>12</v>
@@ -4547,10 +4547,10 @@
         <v>11</v>
       </c>
       <c r="C108">
-        <v>6465</v>
+        <v>6482</v>
       </c>
       <c r="D108">
-        <v>9563677</v>
+        <v>9588310</v>
       </c>
       <c r="E108" t="s">
         <v>12</v>
@@ -4611,10 +4611,10 @@
         <v>11</v>
       </c>
       <c r="C110">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="D110">
-        <v>2945681</v>
+        <v>2956181</v>
       </c>
       <c r="E110" t="s">
         <v>12</v>
@@ -4643,10 +4643,10 @@
         <v>11</v>
       </c>
       <c r="C111">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D111">
-        <v>175771</v>
+        <v>176551</v>
       </c>
       <c r="E111" t="s">
         <v>12</v>
@@ -4707,10 +4707,10 @@
         <v>11</v>
       </c>
       <c r="C113">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D113">
-        <v>175934</v>
+        <v>177434</v>
       </c>
       <c r="E113" t="s">
         <v>12</v>
@@ -4739,10 +4739,10 @@
         <v>11</v>
       </c>
       <c r="C114">
-        <v>9304</v>
+        <v>9315</v>
       </c>
       <c r="D114">
-        <v>11815375</v>
+        <v>11830278</v>
       </c>
       <c r="E114" t="s">
         <v>13</v>
@@ -4835,10 +4835,10 @@
         <v>11</v>
       </c>
       <c r="C117">
-        <v>5147</v>
+        <v>5159</v>
       </c>
       <c r="D117">
-        <v>7588399</v>
+        <v>7606111</v>
       </c>
       <c r="E117" t="s">
         <v>13</v>
@@ -4899,10 +4899,10 @@
         <v>11</v>
       </c>
       <c r="C119">
-        <v>1366</v>
+        <v>1370</v>
       </c>
       <c r="D119">
-        <v>1968752</v>
+        <v>1974752</v>
       </c>
       <c r="E119" t="s">
         <v>13</v>
@@ -4963,10 +4963,10 @@
         <v>11</v>
       </c>
       <c r="C121">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D121">
-        <v>258397</v>
+        <v>259897</v>
       </c>
       <c r="E121" t="s">
         <v>13</v>
@@ -4995,10 +4995,10 @@
         <v>11</v>
       </c>
       <c r="C122">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D122">
-        <v>241132</v>
+        <v>244132</v>
       </c>
       <c r="E122" t="s">
         <v>13</v>
@@ -5027,10 +5027,10 @@
         <v>11</v>
       </c>
       <c r="C123">
-        <v>8199</v>
+        <v>8207</v>
       </c>
       <c r="D123">
-        <v>10491343</v>
+        <v>10501769</v>
       </c>
       <c r="E123" t="s">
         <v>13</v>
@@ -5155,10 +5155,10 @@
         <v>11</v>
       </c>
       <c r="C127">
-        <v>4203</v>
+        <v>4216</v>
       </c>
       <c r="D127">
-        <v>6197917</v>
+        <v>6216536</v>
       </c>
       <c r="E127" t="s">
         <v>13</v>
@@ -5219,10 +5219,10 @@
         <v>11</v>
       </c>
       <c r="C129">
-        <v>1231</v>
+        <v>1236</v>
       </c>
       <c r="D129">
-        <v>1789961</v>
+        <v>1797461</v>
       </c>
       <c r="E129" t="s">
         <v>13</v>
@@ -5347,10 +5347,10 @@
         <v>11</v>
       </c>
       <c r="C133">
-        <v>3784</v>
+        <v>3792</v>
       </c>
       <c r="D133">
-        <v>4725162</v>
+        <v>4736575</v>
       </c>
       <c r="E133" t="s">
         <v>13</v>
@@ -5443,10 +5443,10 @@
         <v>11</v>
       </c>
       <c r="C136">
-        <v>1394</v>
+        <v>1398</v>
       </c>
       <c r="D136">
-        <v>2063462</v>
+        <v>2067191</v>
       </c>
       <c r="E136" t="s">
         <v>13</v>
@@ -5571,10 +5571,10 @@
         <v>11</v>
       </c>
       <c r="C140">
-        <v>4683</v>
+        <v>4690</v>
       </c>
       <c r="D140">
-        <v>5923302</v>
+        <v>5932674</v>
       </c>
       <c r="E140" t="s">
         <v>13</v>
@@ -5635,10 +5635,10 @@
         <v>11</v>
       </c>
       <c r="C142">
-        <v>1889</v>
+        <v>1892</v>
       </c>
       <c r="D142">
-        <v>2783570</v>
+        <v>2788029</v>
       </c>
       <c r="E142" t="s">
         <v>13</v>
@@ -5667,10 +5667,10 @@
         <v>11</v>
       </c>
       <c r="C143">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="D143">
-        <v>1311096</v>
+        <v>1315596</v>
       </c>
       <c r="E143" t="s">
         <v>13</v>
@@ -5699,10 +5699,10 @@
         <v>11</v>
       </c>
       <c r="C144">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D144">
-        <v>138178</v>
+        <v>139678</v>
       </c>
       <c r="E144" t="s">
         <v>13</v>
@@ -5763,10 +5763,10 @@
         <v>11</v>
       </c>
       <c r="C146">
-        <v>3512</v>
+        <v>3519</v>
       </c>
       <c r="D146">
-        <v>4504360</v>
+        <v>4510801</v>
       </c>
       <c r="E146" t="s">
         <v>13</v>
@@ -5827,10 +5827,10 @@
         <v>11</v>
       </c>
       <c r="C148">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="D148">
-        <v>1997575</v>
+        <v>2000575</v>
       </c>
       <c r="E148" t="s">
         <v>13</v>
@@ -5955,10 +5955,10 @@
         <v>11</v>
       </c>
       <c r="C152">
-        <v>9789</v>
+        <v>9803</v>
       </c>
       <c r="D152">
-        <v>12519782</v>
+        <v>12536099</v>
       </c>
       <c r="E152" t="s">
         <v>13</v>
@@ -6083,10 +6083,10 @@
         <v>11</v>
       </c>
       <c r="C156">
-        <v>4263</v>
+        <v>4276</v>
       </c>
       <c r="D156">
-        <v>6272760</v>
+        <v>6291514</v>
       </c>
       <c r="E156" t="s">
         <v>13</v>
@@ -6115,10 +6115,10 @@
         <v>11</v>
       </c>
       <c r="C157">
-        <v>1390</v>
+        <v>1393</v>
       </c>
       <c r="D157">
-        <v>2016587</v>
+        <v>2021087</v>
       </c>
       <c r="E157" t="s">
         <v>13</v>
@@ -6211,10 +6211,10 @@
         <v>11</v>
       </c>
       <c r="C160">
-        <v>1863</v>
+        <v>1865</v>
       </c>
       <c r="D160">
-        <v>2390539</v>
+        <v>2392501</v>
       </c>
       <c r="E160" t="s">
         <v>13</v>
@@ -6275,10 +6275,10 @@
         <v>11</v>
       </c>
       <c r="C162">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D162">
-        <v>1471713</v>
+        <v>1473213</v>
       </c>
       <c r="E162" t="s">
         <v>13</v>
@@ -6339,10 +6339,10 @@
         <v>11</v>
       </c>
       <c r="C164">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D164">
-        <v>527339</v>
+        <v>530339</v>
       </c>
       <c r="E164" t="s">
         <v>13</v>
@@ -6435,10 +6435,10 @@
         <v>11</v>
       </c>
       <c r="C167">
-        <v>5658</v>
+        <v>5670</v>
       </c>
       <c r="D167">
-        <v>7186104</v>
+        <v>7199146</v>
       </c>
       <c r="E167" t="s">
         <v>13</v>
@@ -6531,10 +6531,10 @@
         <v>11</v>
       </c>
       <c r="C170">
-        <v>2237</v>
+        <v>2244</v>
       </c>
       <c r="D170">
-        <v>3304482</v>
+        <v>3314982</v>
       </c>
       <c r="E170" t="s">
         <v>13</v>
@@ -6563,10 +6563,10 @@
         <v>11</v>
       </c>
       <c r="C171">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D171">
-        <v>1433241</v>
+        <v>1434741</v>
       </c>
       <c r="E171" t="s">
         <v>13</v>
@@ -6659,10 +6659,10 @@
         <v>11</v>
       </c>
       <c r="C174">
-        <v>10871</v>
+        <v>10888</v>
       </c>
       <c r="D174">
-        <v>13913166</v>
+        <v>13936451</v>
       </c>
       <c r="E174" t="s">
         <v>14</v>
@@ -6723,10 +6723,10 @@
         <v>11</v>
       </c>
       <c r="C176">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D176">
-        <v>159502</v>
+        <v>162502</v>
       </c>
       <c r="E176" t="s">
         <v>14</v>
@@ -6755,10 +6755,10 @@
         <v>11</v>
       </c>
       <c r="C177">
-        <v>5101</v>
+        <v>5113</v>
       </c>
       <c r="D177">
-        <v>7533009</v>
+        <v>7551009</v>
       </c>
       <c r="E177" t="s">
         <v>14</v>
@@ -6787,10 +6787,10 @@
         <v>11</v>
       </c>
       <c r="C178">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D178">
-        <v>1108412</v>
+        <v>1109912</v>
       </c>
       <c r="E178" t="s">
         <v>14</v>
@@ -6883,10 +6883,10 @@
         <v>11</v>
       </c>
       <c r="C181">
-        <v>16333</v>
+        <v>16360</v>
       </c>
       <c r="D181">
-        <v>21025697</v>
+        <v>21059995</v>
       </c>
       <c r="E181" t="s">
         <v>14</v>
@@ -6979,10 +6979,10 @@
         <v>11</v>
       </c>
       <c r="C184">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D184">
-        <v>249452</v>
+        <v>250952</v>
       </c>
       <c r="E184" t="s">
         <v>14</v>
@@ -7011,10 +7011,10 @@
         <v>11</v>
       </c>
       <c r="C185">
-        <v>7082</v>
+        <v>7094</v>
       </c>
       <c r="D185">
-        <v>10447607</v>
+        <v>10464017</v>
       </c>
       <c r="E185" t="s">
         <v>14</v>
@@ -7075,10 +7075,10 @@
         <v>11</v>
       </c>
       <c r="C187">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="D187">
-        <v>2395507</v>
+        <v>2397007</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
@@ -7171,10 +7171,10 @@
         <v>11</v>
       </c>
       <c r="C190">
-        <v>17248</v>
+        <v>17280</v>
       </c>
       <c r="D190">
-        <v>22189153</v>
+        <v>22231132</v>
       </c>
       <c r="E190" t="s">
         <v>14</v>
@@ -7299,10 +7299,10 @@
         <v>11</v>
       </c>
       <c r="C194">
-        <v>9859</v>
+        <v>9886</v>
       </c>
       <c r="D194">
-        <v>14559457</v>
+        <v>14598769</v>
       </c>
       <c r="E194" t="s">
         <v>14</v>
@@ -7363,10 +7363,10 @@
         <v>11</v>
       </c>
       <c r="C196">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="D196">
-        <v>2327369</v>
+        <v>2330369</v>
       </c>
       <c r="E196" t="s">
         <v>14</v>
@@ -7395,10 +7395,10 @@
         <v>11</v>
       </c>
       <c r="C197">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D197">
-        <v>272691</v>
+        <v>275106</v>
       </c>
       <c r="E197" t="s">
         <v>14</v>
@@ -7427,10 +7427,10 @@
         <v>11</v>
       </c>
       <c r="C198">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D198">
-        <v>356937</v>
+        <v>359937</v>
       </c>
       <c r="E198" t="s">
         <v>14</v>
@@ -7459,10 +7459,10 @@
         <v>11</v>
       </c>
       <c r="C199">
-        <v>15233</v>
+        <v>15257</v>
       </c>
       <c r="D199">
-        <v>19533864</v>
+        <v>19566727</v>
       </c>
       <c r="E199" t="s">
         <v>14</v>
@@ -7619,10 +7619,10 @@
         <v>11</v>
       </c>
       <c r="C204">
-        <v>7527</v>
+        <v>7544</v>
       </c>
       <c r="D204">
-        <v>11097405</v>
+        <v>11122905</v>
       </c>
       <c r="E204" t="s">
         <v>14</v>
@@ -7651,10 +7651,10 @@
         <v>11</v>
       </c>
       <c r="C205">
-        <v>1591</v>
+        <v>1594</v>
       </c>
       <c r="D205">
-        <v>2290119</v>
+        <v>2294619</v>
       </c>
       <c r="E205" t="s">
         <v>14</v>
@@ -7715,10 +7715,10 @@
         <v>11</v>
       </c>
       <c r="C207">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D207">
-        <v>228070</v>
+        <v>229388</v>
       </c>
       <c r="E207" t="s">
         <v>14</v>
@@ -7747,10 +7747,10 @@
         <v>11</v>
       </c>
       <c r="C208">
-        <v>4895</v>
+        <v>4900</v>
       </c>
       <c r="D208">
-        <v>6219123</v>
+        <v>6223865</v>
       </c>
       <c r="E208" t="s">
         <v>15</v>
@@ -7811,10 +7811,10 @@
         <v>11</v>
       </c>
       <c r="C210">
-        <v>1785</v>
+        <v>1788</v>
       </c>
       <c r="D210">
-        <v>2631006</v>
+        <v>2634651</v>
       </c>
       <c r="E210" t="s">
         <v>15</v>
@@ -7875,10 +7875,10 @@
         <v>11</v>
       </c>
       <c r="C212">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="D212">
-        <v>866732</v>
+        <v>872732</v>
       </c>
       <c r="E212" t="s">
         <v>15</v>
@@ -7971,10 +7971,10 @@
         <v>11</v>
       </c>
       <c r="C215">
-        <v>6101</v>
+        <v>6108</v>
       </c>
       <c r="D215">
-        <v>7871325</v>
+        <v>7880695</v>
       </c>
       <c r="E215" t="s">
         <v>15</v>
@@ -8067,10 +8067,10 @@
         <v>11</v>
       </c>
       <c r="C218">
-        <v>2834</v>
+        <v>2837</v>
       </c>
       <c r="D218">
-        <v>4183383</v>
+        <v>4187883</v>
       </c>
       <c r="E218" t="s">
         <v>15</v>
@@ -8099,10 +8099,10 @@
         <v>11</v>
       </c>
       <c r="C219">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="D219">
-        <v>1971113</v>
+        <v>1974113</v>
       </c>
       <c r="E219" t="s">
         <v>15</v>
@@ -8195,10 +8195,10 @@
         <v>11</v>
       </c>
       <c r="C222">
-        <v>3480</v>
+        <v>3485</v>
       </c>
       <c r="D222">
-        <v>4389477</v>
+        <v>4396677</v>
       </c>
       <c r="E222" t="s">
         <v>15</v>
@@ -8291,10 +8291,10 @@
         <v>11</v>
       </c>
       <c r="C225">
-        <v>1340</v>
+        <v>1343</v>
       </c>
       <c r="D225">
-        <v>1975709</v>
+        <v>1980209</v>
       </c>
       <c r="E225" t="s">
         <v>15</v>
@@ -8355,10 +8355,10 @@
         <v>11</v>
       </c>
       <c r="C227">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="D227">
-        <v>652008</v>
+        <v>656508</v>
       </c>
       <c r="E227" t="s">
         <v>15</v>
@@ -8451,10 +8451,10 @@
         <v>11</v>
       </c>
       <c r="C230">
-        <v>11170</v>
+        <v>11183</v>
       </c>
       <c r="D230">
-        <v>14244009</v>
+        <v>14260554</v>
       </c>
       <c r="E230" t="s">
         <v>15</v>
@@ -8547,10 +8547,10 @@
         <v>11</v>
       </c>
       <c r="C233">
-        <v>5197</v>
+        <v>5214</v>
       </c>
       <c r="D233">
-        <v>7662048</v>
+        <v>7686469</v>
       </c>
       <c r="E233" t="s">
         <v>15</v>
@@ -8579,10 +8579,10 @@
         <v>11</v>
       </c>
       <c r="C234">
-        <v>1501</v>
+        <v>1503</v>
       </c>
       <c r="D234">
-        <v>2171800</v>
+        <v>2173651</v>
       </c>
       <c r="E234" t="s">
         <v>15</v>
@@ -8675,10 +8675,10 @@
         <v>11</v>
       </c>
       <c r="C237">
-        <v>5781</v>
+        <v>5788</v>
       </c>
       <c r="D237">
-        <v>7347328</v>
+        <v>7357078</v>
       </c>
       <c r="E237" t="s">
         <v>15</v>
@@ -8771,10 +8771,10 @@
         <v>11</v>
       </c>
       <c r="C240">
-        <v>2606</v>
+        <v>2610</v>
       </c>
       <c r="D240">
-        <v>3835018</v>
+        <v>3841018</v>
       </c>
       <c r="E240" t="s">
         <v>15</v>
@@ -8803,10 +8803,10 @@
         <v>11</v>
       </c>
       <c r="C241">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="D241">
-        <v>1106470</v>
+        <v>1110970</v>
       </c>
       <c r="E241" t="s">
         <v>15</v>
@@ -8867,10 +8867,10 @@
         <v>11</v>
       </c>
       <c r="C243">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D243">
-        <v>102447</v>
+        <v>105147</v>
       </c>
       <c r="E243" t="s">
         <v>15</v>
@@ -8899,10 +8899,10 @@
         <v>11</v>
       </c>
       <c r="C244">
-        <v>9824</v>
+        <v>9843</v>
       </c>
       <c r="D244">
-        <v>12346386</v>
+        <v>12368508</v>
       </c>
       <c r="E244" t="s">
         <v>15</v>
@@ -8995,10 +8995,10 @@
         <v>11</v>
       </c>
       <c r="C247">
-        <v>4760</v>
+        <v>4771</v>
       </c>
       <c r="D247">
-        <v>7029846</v>
+        <v>7044957</v>
       </c>
       <c r="E247" t="s">
         <v>15</v>
@@ -9027,10 +9027,10 @@
         <v>11</v>
       </c>
       <c r="C248">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="D248">
-        <v>3059667</v>
+        <v>3061167</v>
       </c>
       <c r="E248" t="s">
         <v>15</v>
@@ -9091,10 +9091,10 @@
         <v>11</v>
       </c>
       <c r="C250">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D250">
-        <v>158731</v>
+        <v>160231</v>
       </c>
       <c r="E250" t="s">
         <v>15</v>
@@ -9123,10 +9123,10 @@
         <v>11</v>
       </c>
       <c r="C251">
-        <v>4966</v>
+        <v>4975</v>
       </c>
       <c r="D251">
-        <v>6487970</v>
+        <v>6498983</v>
       </c>
       <c r="E251" t="s">
         <v>16</v>
@@ -9219,10 +9219,10 @@
         <v>11</v>
       </c>
       <c r="C254">
-        <v>2048</v>
+        <v>2054</v>
       </c>
       <c r="D254">
-        <v>3007923</v>
+        <v>3014824</v>
       </c>
       <c r="E254" t="s">
         <v>16</v>
@@ -9251,10 +9251,10 @@
         <v>11</v>
       </c>
       <c r="C255">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="D255">
-        <v>1865495</v>
+        <v>1868495</v>
       </c>
       <c r="E255" t="s">
         <v>16</v>
@@ -9347,10 +9347,10 @@
         <v>11</v>
       </c>
       <c r="C258">
-        <v>6526</v>
+        <v>6539</v>
       </c>
       <c r="D258">
-        <v>8567699</v>
+        <v>8586963</v>
       </c>
       <c r="E258" t="s">
         <v>16</v>
@@ -9475,10 +9475,10 @@
         <v>11</v>
       </c>
       <c r="C262">
-        <v>2183</v>
+        <v>2193</v>
       </c>
       <c r="D262">
-        <v>3207637</v>
+        <v>3220600</v>
       </c>
       <c r="E262" t="s">
         <v>16</v>
@@ -9507,10 +9507,10 @@
         <v>11</v>
       </c>
       <c r="C263">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="D263">
-        <v>2355552</v>
+        <v>2357052</v>
       </c>
       <c r="E263" t="s">
         <v>16</v>
@@ -9603,10 +9603,10 @@
         <v>11</v>
       </c>
       <c r="C266">
-        <v>4421</v>
+        <v>4428</v>
       </c>
       <c r="D266">
-        <v>5554580</v>
+        <v>5557631</v>
       </c>
       <c r="E266" t="s">
         <v>17</v>
@@ -9731,10 +9731,10 @@
         <v>11</v>
       </c>
       <c r="C270">
-        <v>1501</v>
+        <v>1505</v>
       </c>
       <c r="D270">
-        <v>2221283</v>
+        <v>2227283</v>
       </c>
       <c r="E270" t="s">
         <v>17</v>
@@ -9827,10 +9827,10 @@
         <v>11</v>
       </c>
       <c r="C273">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D273">
-        <v>39243</v>
+        <v>40743</v>
       </c>
       <c r="E273" t="s">
         <v>17</v>
@@ -9859,10 +9859,10 @@
         <v>11</v>
       </c>
       <c r="C274">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D274">
-        <v>39271</v>
+        <v>43771</v>
       </c>
       <c r="E274" t="s">
         <v>17</v>
@@ -9891,10 +9891,10 @@
         <v>11</v>
       </c>
       <c r="C275">
-        <v>4636</v>
+        <v>4646</v>
       </c>
       <c r="D275">
-        <v>5900124</v>
+        <v>5913018</v>
       </c>
       <c r="E275" t="s">
         <v>17</v>
@@ -9987,10 +9987,10 @@
         <v>11</v>
       </c>
       <c r="C278">
-        <v>2051</v>
+        <v>2058</v>
       </c>
       <c r="D278">
-        <v>3019970</v>
+        <v>3029841</v>
       </c>
       <c r="E278" t="s">
         <v>17</v>
@@ -10019,10 +10019,10 @@
         <v>11</v>
       </c>
       <c r="C279">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="D279">
-        <v>1143800</v>
+        <v>1154300</v>
       </c>
       <c r="E279" t="s">
         <v>17</v>
@@ -10115,10 +10115,10 @@
         <v>11</v>
       </c>
       <c r="C282">
-        <v>18381</v>
+        <v>18415</v>
       </c>
       <c r="D282">
-        <v>23449176</v>
+        <v>23493792</v>
       </c>
       <c r="E282" t="s">
         <v>17</v>
@@ -10275,10 +10275,10 @@
         <v>11</v>
       </c>
       <c r="C287">
-        <v>10624</v>
+        <v>10654</v>
       </c>
       <c r="D287">
-        <v>15677989</v>
+        <v>15719815</v>
       </c>
       <c r="E287" t="s">
         <v>17</v>
@@ -10371,10 +10371,10 @@
         <v>11</v>
       </c>
       <c r="C290">
-        <v>4886</v>
+        <v>4904</v>
       </c>
       <c r="D290">
-        <v>7099496</v>
+        <v>7125608</v>
       </c>
       <c r="E290" t="s">
         <v>17</v>
@@ -10435,10 +10435,10 @@
         <v>11</v>
       </c>
       <c r="C292">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D292">
-        <v>417334</v>
+        <v>418834</v>
       </c>
       <c r="E292" t="s">
         <v>17</v>
@@ -10467,10 +10467,10 @@
         <v>11</v>
       </c>
       <c r="C293">
-        <v>11642</v>
+        <v>11666</v>
       </c>
       <c r="D293">
-        <v>14693965</v>
+        <v>14721697</v>
       </c>
       <c r="E293" t="s">
         <v>17</v>
@@ -10563,10 +10563,10 @@
         <v>11</v>
       </c>
       <c r="C296">
-        <v>6432</v>
+        <v>6457</v>
       </c>
       <c r="D296">
-        <v>9500724</v>
+        <v>9536494</v>
       </c>
       <c r="E296" t="s">
         <v>17</v>
@@ -10627,10 +10627,10 @@
         <v>11</v>
       </c>
       <c r="C298">
-        <v>2952</v>
+        <v>2963</v>
       </c>
       <c r="D298">
-        <v>4297081</v>
+        <v>4311963</v>
       </c>
       <c r="E298" t="s">
         <v>17</v>
@@ -10723,10 +10723,10 @@
         <v>11</v>
       </c>
       <c r="C301">
-        <v>2448</v>
+        <v>2452</v>
       </c>
       <c r="D301">
-        <v>3106900</v>
+        <v>3111135</v>
       </c>
       <c r="E301" t="s">
         <v>17</v>
@@ -10819,10 +10819,10 @@
         <v>11</v>
       </c>
       <c r="C304">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="D304">
-        <v>1496716</v>
+        <v>1498216</v>
       </c>
       <c r="E304" t="s">
         <v>17</v>
@@ -10979,10 +10979,10 @@
         <v>11</v>
       </c>
       <c r="C309">
-        <v>8310</v>
+        <v>8321</v>
       </c>
       <c r="D309">
-        <v>10501091</v>
+        <v>10516891</v>
       </c>
       <c r="E309" t="s">
         <v>17</v>
@@ -11107,10 +11107,10 @@
         <v>11</v>
       </c>
       <c r="C313">
-        <v>4250</v>
+        <v>4257</v>
       </c>
       <c r="D313">
-        <v>6278218</v>
+        <v>6287918</v>
       </c>
       <c r="E313" t="s">
         <v>17</v>
@@ -11171,10 +11171,10 @@
         <v>11</v>
       </c>
       <c r="C315">
-        <v>1558</v>
+        <v>1566</v>
       </c>
       <c r="D315">
-        <v>2247257</v>
+        <v>2256886</v>
       </c>
       <c r="E315" t="s">
         <v>17</v>
@@ -11267,10 +11267,10 @@
         <v>11</v>
       </c>
       <c r="C318">
-        <v>10696</v>
+        <v>10717</v>
       </c>
       <c r="D318">
-        <v>13476067</v>
+        <v>13500219</v>
       </c>
       <c r="E318" t="s">
         <v>17</v>
@@ -11363,10 +11363,10 @@
         <v>11</v>
       </c>
       <c r="C321">
-        <v>4871</v>
+        <v>4887</v>
       </c>
       <c r="D321">
-        <v>7202773</v>
+        <v>7224445</v>
       </c>
       <c r="E321" t="s">
         <v>17</v>
@@ -11427,10 +11427,10 @@
         <v>11</v>
       </c>
       <c r="C323">
-        <v>1813</v>
+        <v>1816</v>
       </c>
       <c r="D323">
-        <v>2633562</v>
+        <v>2638062</v>
       </c>
       <c r="E323" t="s">
         <v>17</v>
@@ -11523,10 +11523,10 @@
         <v>11</v>
       </c>
       <c r="C326">
-        <v>2604</v>
+        <v>2608</v>
       </c>
       <c r="D326">
-        <v>3323940</v>
+        <v>3328543</v>
       </c>
       <c r="E326" t="s">
         <v>17</v>
@@ -11619,10 +11619,10 @@
         <v>11</v>
       </c>
       <c r="C329">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="D329">
-        <v>1361233</v>
+        <v>1365129</v>
       </c>
       <c r="E329" t="s">
         <v>17</v>
@@ -11651,10 +11651,10 @@
         <v>11</v>
       </c>
       <c r="C330">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D330">
-        <v>523453</v>
+        <v>524953</v>
       </c>
       <c r="E330" t="s">
         <v>17</v>
@@ -11747,10 +11747,10 @@
         <v>11</v>
       </c>
       <c r="C333">
-        <v>13648</v>
+        <v>13681</v>
       </c>
       <c r="D333">
-        <v>17166679</v>
+        <v>17202015</v>
       </c>
       <c r="E333" t="s">
         <v>17</v>
@@ -11843,10 +11843,10 @@
         <v>11</v>
       </c>
       <c r="C336">
-        <v>6353</v>
+        <v>6366</v>
       </c>
       <c r="D336">
-        <v>9409866</v>
+        <v>9428299</v>
       </c>
       <c r="E336" t="s">
         <v>17</v>
@@ -11907,10 +11907,10 @@
         <v>11</v>
       </c>
       <c r="C338">
-        <v>4023</v>
+        <v>4030</v>
       </c>
       <c r="D338">
-        <v>5875217</v>
+        <v>5885717</v>
       </c>
       <c r="E338" t="s">
         <v>17</v>
@@ -11971,10 +11971,10 @@
         <v>11</v>
       </c>
       <c r="C340">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D340">
-        <v>194339</v>
+        <v>197339</v>
       </c>
       <c r="E340" t="s">
         <v>17</v>
@@ -12003,10 +12003,10 @@
         <v>11</v>
       </c>
       <c r="C341">
-        <v>6960</v>
+        <v>6969</v>
       </c>
       <c r="D341">
-        <v>8744746</v>
+        <v>8756008</v>
       </c>
       <c r="E341" t="s">
         <v>17</v>
@@ -12099,10 +12099,10 @@
         <v>11</v>
       </c>
       <c r="C344">
-        <v>3543</v>
+        <v>3556</v>
       </c>
       <c r="D344">
-        <v>5212281</v>
+        <v>5230548</v>
       </c>
       <c r="E344" t="s">
         <v>17</v>
@@ -12163,10 +12163,10 @@
         <v>11</v>
       </c>
       <c r="C346">
-        <v>1176</v>
+        <v>1181</v>
       </c>
       <c r="D346">
-        <v>1715338</v>
+        <v>1721552</v>
       </c>
       <c r="E346" t="s">
         <v>17</v>
@@ -12195,10 +12195,10 @@
         <v>11</v>
       </c>
       <c r="C347">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D347">
-        <v>101628</v>
+        <v>103438</v>
       </c>
       <c r="E347" t="s">
         <v>17</v>
@@ -12259,10 +12259,10 @@
         <v>11</v>
       </c>
       <c r="C349">
-        <v>13542</v>
+        <v>13636</v>
       </c>
       <c r="D349">
-        <v>18358361</v>
+        <v>18487120</v>
       </c>
       <c r="E349" t="s">
         <v>18</v>
@@ -12387,10 +12387,10 @@
         <v>11</v>
       </c>
       <c r="C353">
-        <v>4259</v>
+        <v>4266</v>
       </c>
       <c r="D353">
-        <v>6282442</v>
+        <v>6291862</v>
       </c>
       <c r="E353" t="s">
         <v>18</v>
@@ -12451,10 +12451,10 @@
         <v>11</v>
       </c>
       <c r="C355">
-        <v>3333</v>
+        <v>3354</v>
       </c>
       <c r="D355">
-        <v>4813815</v>
+        <v>4844868</v>
       </c>
       <c r="E355" t="s">
         <v>18</v>
@@ -12515,10 +12515,10 @@
         <v>11</v>
       </c>
       <c r="C357">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D357">
-        <v>278311</v>
+        <v>281311</v>
       </c>
       <c r="E357" t="s">
         <v>18</v>
@@ -12579,10 +12579,10 @@
         <v>11</v>
       </c>
       <c r="C359">
-        <v>2873</v>
+        <v>2884</v>
       </c>
       <c r="D359">
-        <v>3953810</v>
+        <v>3970010</v>
       </c>
       <c r="E359" t="s">
         <v>19</v>
@@ -12611,10 +12611,10 @@
         <v>11</v>
       </c>
       <c r="C360">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="D360">
-        <v>1247754</v>
+        <v>1253754</v>
       </c>
       <c r="E360" t="s">
         <v>19</v>
@@ -12675,10 +12675,10 @@
         <v>11</v>
       </c>
       <c r="C362">
-        <v>1026</v>
+        <v>1034</v>
       </c>
       <c r="D362">
-        <v>1491016</v>
+        <v>1503016</v>
       </c>
       <c r="E362" t="s">
         <v>19</v>
@@ -12771,10 +12771,10 @@
         <v>11</v>
       </c>
       <c r="C365">
-        <v>7125</v>
+        <v>7135</v>
       </c>
       <c r="D365">
-        <v>8898799</v>
+        <v>8912523</v>
       </c>
       <c r="E365" t="s">
         <v>20</v>
@@ -12867,10 +12867,10 @@
         <v>11</v>
       </c>
       <c r="C368">
-        <v>2583</v>
+        <v>2586</v>
       </c>
       <c r="D368">
-        <v>3805106</v>
+        <v>3809606</v>
       </c>
       <c r="E368" t="s">
         <v>20</v>
@@ -12931,10 +12931,10 @@
         <v>11</v>
       </c>
       <c r="C370">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D370">
-        <v>1713449</v>
+        <v>1714342</v>
       </c>
       <c r="E370" t="s">
         <v>20</v>
@@ -13027,10 +13027,10 @@
         <v>11</v>
       </c>
       <c r="C373">
-        <v>37535</v>
+        <v>37598</v>
       </c>
       <c r="D373">
-        <v>46928109</v>
+        <v>47011572</v>
       </c>
       <c r="E373" t="s">
         <v>20</v>
@@ -13123,10 +13123,10 @@
         <v>11</v>
       </c>
       <c r="C376">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D376">
-        <v>250435</v>
+        <v>251935</v>
       </c>
       <c r="E376" t="s">
         <v>20</v>
@@ -13155,10 +13155,10 @@
         <v>11</v>
       </c>
       <c r="C377">
-        <v>16781</v>
+        <v>16814</v>
       </c>
       <c r="D377">
-        <v>24708759</v>
+        <v>24755495</v>
       </c>
       <c r="E377" t="s">
         <v>20</v>
@@ -13219,10 +13219,10 @@
         <v>11</v>
       </c>
       <c r="C379">
-        <v>7956</v>
+        <v>7971</v>
       </c>
       <c r="D379">
-        <v>11566443</v>
+        <v>11587691</v>
       </c>
       <c r="E379" t="s">
         <v>20</v>
@@ -13251,10 +13251,10 @@
         <v>11</v>
       </c>
       <c r="C380">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D380">
-        <v>324892</v>
+        <v>327892</v>
       </c>
       <c r="E380" t="s">
         <v>20</v>
@@ -13283,10 +13283,10 @@
         <v>11</v>
       </c>
       <c r="C381">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D381">
-        <v>533795</v>
+        <v>538295</v>
       </c>
       <c r="E381" t="s">
         <v>20</v>
@@ -13347,10 +13347,10 @@
         <v>11</v>
       </c>
       <c r="C383">
-        <v>11668</v>
+        <v>11688</v>
       </c>
       <c r="D383">
-        <v>14856798</v>
+        <v>14884897</v>
       </c>
       <c r="E383" t="s">
         <v>20</v>
@@ -13411,10 +13411,10 @@
         <v>11</v>
       </c>
       <c r="C385">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D385">
-        <v>117444</v>
+        <v>118944</v>
       </c>
       <c r="E385" t="s">
         <v>20</v>
@@ -13443,10 +13443,10 @@
         <v>11</v>
       </c>
       <c r="C386">
-        <v>5093</v>
+        <v>5114</v>
       </c>
       <c r="D386">
-        <v>7526847</v>
+        <v>7556358</v>
       </c>
       <c r="E386" t="s">
         <v>20</v>
@@ -13507,10 +13507,10 @@
         <v>11</v>
       </c>
       <c r="C388">
-        <v>2977</v>
+        <v>2980</v>
       </c>
       <c r="D388">
-        <v>4339966</v>
+        <v>4344466</v>
       </c>
       <c r="E388" t="s">
         <v>20</v>
@@ -13571,10 +13571,10 @@
         <v>11</v>
       </c>
       <c r="C390">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D390">
-        <v>112565</v>
+        <v>114065</v>
       </c>
       <c r="E390" t="s">
         <v>20</v>
@@ -13603,10 +13603,10 @@
         <v>11</v>
       </c>
       <c r="C391">
-        <v>20679</v>
+        <v>20708</v>
       </c>
       <c r="D391">
-        <v>25582029</v>
+        <v>25620922</v>
       </c>
       <c r="E391" t="s">
         <v>20</v>
@@ -13699,10 +13699,10 @@
         <v>11</v>
       </c>
       <c r="C394">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D394">
-        <v>244203</v>
+        <v>245703</v>
       </c>
       <c r="E394" t="s">
         <v>20</v>
@@ -13731,10 +13731,10 @@
         <v>11</v>
       </c>
       <c r="C395">
-        <v>7932</v>
+        <v>7954</v>
       </c>
       <c r="D395">
-        <v>11687330</v>
+        <v>11719210</v>
       </c>
       <c r="E395" t="s">
         <v>20</v>
@@ -13795,10 +13795,10 @@
         <v>11</v>
       </c>
       <c r="C397">
-        <v>3229</v>
+        <v>3239</v>
       </c>
       <c r="D397">
-        <v>4700846</v>
+        <v>4714695</v>
       </c>
       <c r="E397" t="s">
         <v>20</v>
@@ -13827,10 +13827,10 @@
         <v>11</v>
       </c>
       <c r="C398">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D398">
-        <v>242465</v>
+        <v>245465</v>
       </c>
       <c r="E398" t="s">
         <v>20</v>
@@ -13859,10 +13859,10 @@
         <v>11</v>
       </c>
       <c r="C399">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D399">
-        <v>242869</v>
+        <v>243468</v>
       </c>
       <c r="E399" t="s">
         <v>20</v>
@@ -13891,10 +13891,10 @@
         <v>11</v>
       </c>
       <c r="C400">
-        <v>8812</v>
+        <v>8835</v>
       </c>
       <c r="D400">
-        <v>10938784</v>
+        <v>10967032</v>
       </c>
       <c r="E400" t="s">
         <v>20</v>
@@ -14019,10 +14019,10 @@
         <v>11</v>
       </c>
       <c r="C404">
-        <v>2947</v>
+        <v>2952</v>
       </c>
       <c r="D404">
-        <v>4361540</v>
+        <v>4369040</v>
       </c>
       <c r="E404" t="s">
         <v>20</v>
@@ -14051,10 +14051,10 @@
         <v>11</v>
       </c>
       <c r="C405">
-        <v>1289</v>
+        <v>1295</v>
       </c>
       <c r="D405">
-        <v>1867389</v>
+        <v>1874041</v>
       </c>
       <c r="E405" t="s">
         <v>20</v>
@@ -14083,10 +14083,10 @@
         <v>11</v>
       </c>
       <c r="C406">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D406">
-        <v>102502</v>
+        <v>104002</v>
       </c>
       <c r="E406" t="s">
         <v>20</v>
@@ -14115,10 +14115,10 @@
         <v>11</v>
       </c>
       <c r="C407">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D407">
-        <v>194045</v>
+        <v>197045</v>
       </c>
       <c r="E407" t="s">
         <v>20</v>
@@ -14147,10 +14147,10 @@
         <v>11</v>
       </c>
       <c r="C408">
-        <v>24545</v>
+        <v>24638</v>
       </c>
       <c r="D408">
-        <v>33130177</v>
+        <v>33256848</v>
       </c>
       <c r="E408" t="s">
         <v>21</v>
@@ -14307,10 +14307,10 @@
         <v>11</v>
       </c>
       <c r="C413">
-        <v>8976</v>
+        <v>9009</v>
       </c>
       <c r="D413">
-        <v>13236125</v>
+        <v>13284682</v>
       </c>
       <c r="E413" t="s">
         <v>21</v>
@@ -14339,10 +14339,10 @@
         <v>11</v>
       </c>
       <c r="C414">
-        <v>2291</v>
+        <v>2300</v>
       </c>
       <c r="D414">
-        <v>3320096</v>
+        <v>3333482</v>
       </c>
       <c r="E414" t="s">
         <v>21</v>
@@ -14403,10 +14403,10 @@
         <v>11</v>
       </c>
       <c r="C416">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D416">
-        <v>294215</v>
+        <v>297215</v>
       </c>
       <c r="E416" t="s">
         <v>21</v>
@@ -14435,10 +14435,10 @@
         <v>11</v>
       </c>
       <c r="C417">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D417">
-        <v>215066</v>
+        <v>216566</v>
       </c>
       <c r="E417" t="s">
         <v>21</v>
@@ -14467,10 +14467,10 @@
         <v>11</v>
       </c>
       <c r="C418">
-        <v>8997</v>
+        <v>9016</v>
       </c>
       <c r="D418">
-        <v>11988811</v>
+        <v>12014981</v>
       </c>
       <c r="E418" t="s">
         <v>22</v>
@@ -14531,10 +14531,10 @@
         <v>11</v>
       </c>
       <c r="C420">
-        <v>4137</v>
+        <v>4147</v>
       </c>
       <c r="D420">
-        <v>6054347</v>
+        <v>6069347</v>
       </c>
       <c r="E420" t="s">
         <v>22</v>
@@ -14563,10 +14563,10 @@
         <v>11</v>
       </c>
       <c r="C421">
-        <v>2581</v>
+        <v>2588</v>
       </c>
       <c r="D421">
-        <v>3734785</v>
+        <v>3743585</v>
       </c>
       <c r="E421" t="s">
         <v>22</v>
@@ -14659,10 +14659,10 @@
         <v>11</v>
       </c>
       <c r="C424">
-        <v>3012</v>
+        <v>3036</v>
       </c>
       <c r="D424">
-        <v>4265629</v>
+        <v>4300309</v>
       </c>
       <c r="E424" t="s">
         <v>23</v>
@@ -14691,10 +14691,10 @@
         <v>11</v>
       </c>
       <c r="C425">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="D425">
-        <v>1130943</v>
+        <v>1136943</v>
       </c>
       <c r="E425" t="s">
         <v>23</v>
@@ -14819,10 +14819,10 @@
         <v>11</v>
       </c>
       <c r="C429">
-        <v>13541</v>
+        <v>13559</v>
       </c>
       <c r="D429">
-        <v>17274347</v>
+        <v>17297908</v>
       </c>
       <c r="E429" t="s">
         <v>24</v>
@@ -14947,10 +14947,10 @@
         <v>11</v>
       </c>
       <c r="C433">
-        <v>6064</v>
+        <v>6073</v>
       </c>
       <c r="D433">
-        <v>8920161</v>
+        <v>8933575</v>
       </c>
       <c r="E433" t="s">
         <v>24</v>
@@ -14979,10 +14979,10 @@
         <v>11</v>
       </c>
       <c r="C434">
-        <v>2090</v>
+        <v>2093</v>
       </c>
       <c r="D434">
-        <v>3013761</v>
+        <v>3018261</v>
       </c>
       <c r="E434" t="s">
         <v>24</v>
@@ -15011,10 +15011,10 @@
         <v>11</v>
       </c>
       <c r="C435">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D435">
-        <v>274321</v>
+        <v>275821</v>
       </c>
       <c r="E435" t="s">
         <v>24</v>
@@ -15075,10 +15075,10 @@
         <v>11</v>
       </c>
       <c r="C437">
-        <v>9104</v>
+        <v>9118</v>
       </c>
       <c r="D437">
-        <v>11552385</v>
+        <v>11571182</v>
       </c>
       <c r="E437" t="s">
         <v>24</v>
@@ -15203,10 +15203,10 @@
         <v>11</v>
       </c>
       <c r="C441">
-        <v>3984</v>
+        <v>3997</v>
       </c>
       <c r="D441">
-        <v>5881721</v>
+        <v>5899846</v>
       </c>
       <c r="E441" t="s">
         <v>24</v>
@@ -15235,10 +15235,10 @@
         <v>11</v>
       </c>
       <c r="C442">
-        <v>1706</v>
+        <v>1713</v>
       </c>
       <c r="D442">
-        <v>2469035</v>
+        <v>2478364</v>
       </c>
       <c r="E442" t="s">
         <v>24</v>
@@ -15331,10 +15331,10 @@
         <v>11</v>
       </c>
       <c r="C445">
-        <v>8837</v>
+        <v>8851</v>
       </c>
       <c r="D445">
-        <v>11392040</v>
+        <v>11410118</v>
       </c>
       <c r="E445" t="s">
         <v>24</v>
@@ -15459,10 +15459,10 @@
         <v>11</v>
       </c>
       <c r="C449">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="D449">
-        <v>5261855</v>
+        <v>5263355</v>
       </c>
       <c r="E449" t="s">
         <v>24</v>
@@ -15587,10 +15587,10 @@
         <v>11</v>
       </c>
       <c r="C453">
-        <v>4798</v>
+        <v>4803</v>
       </c>
       <c r="D453">
-        <v>6262307</v>
+        <v>6268693</v>
       </c>
       <c r="E453" t="s">
         <v>24</v>
@@ -15683,10 +15683,10 @@
         <v>11</v>
       </c>
       <c r="C456">
-        <v>1735</v>
+        <v>1740</v>
       </c>
       <c r="D456">
-        <v>2555105</v>
+        <v>2562505</v>
       </c>
       <c r="E456" t="s">
         <v>24</v>
@@ -15811,10 +15811,10 @@
         <v>11</v>
       </c>
       <c r="C460">
-        <v>17631</v>
+        <v>17670</v>
       </c>
       <c r="D460">
-        <v>22014681</v>
+        <v>22063579</v>
       </c>
       <c r="E460" t="s">
         <v>24</v>
@@ -15907,10 +15907,10 @@
         <v>11</v>
       </c>
       <c r="C463">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D463">
-        <v>131095</v>
+        <v>132595</v>
       </c>
       <c r="E463" t="s">
         <v>24</v>
@@ -15939,10 +15939,10 @@
         <v>11</v>
       </c>
       <c r="C464">
-        <v>7448</v>
+        <v>7472</v>
       </c>
       <c r="D464">
-        <v>10992459</v>
+        <v>11027858</v>
       </c>
       <c r="E464" t="s">
         <v>24</v>
@@ -16003,10 +16003,10 @@
         <v>11</v>
       </c>
       <c r="C466">
-        <v>2943</v>
+        <v>2952</v>
       </c>
       <c r="D466">
-        <v>4288475</v>
+        <v>4301611</v>
       </c>
       <c r="E466" t="s">
         <v>24</v>
@@ -16035,10 +16035,10 @@
         <v>11</v>
       </c>
       <c r="C467">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D467">
-        <v>196516</v>
+        <v>198016</v>
       </c>
       <c r="E467" t="s">
         <v>24</v>
@@ -16067,10 +16067,10 @@
         <v>11</v>
       </c>
       <c r="C468">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D468">
-        <v>344196</v>
+        <v>345696</v>
       </c>
       <c r="E468" t="s">
         <v>24</v>
@@ -16099,10 +16099,10 @@
         <v>11</v>
       </c>
       <c r="C469">
-        <v>7060</v>
+        <v>7072</v>
       </c>
       <c r="D469">
-        <v>8804650</v>
+        <v>8817771</v>
       </c>
       <c r="E469" t="s">
         <v>25</v>
@@ -16227,10 +16227,10 @@
         <v>11</v>
       </c>
       <c r="C473">
-        <v>2508</v>
+        <v>2509</v>
       </c>
       <c r="D473">
-        <v>3688301</v>
+        <v>3689801</v>
       </c>
       <c r="E473" t="s">
         <v>25</v>
@@ -16291,10 +16291,10 @@
         <v>11</v>
       </c>
       <c r="C475">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D475">
-        <v>68112</v>
+        <v>71112</v>
       </c>
       <c r="E475" t="s">
         <v>25</v>
@@ -16355,10 +16355,10 @@
         <v>11</v>
       </c>
       <c r="C477">
-        <v>17755</v>
+        <v>17775</v>
       </c>
       <c r="D477">
-        <v>22399088</v>
+        <v>22425871</v>
       </c>
       <c r="E477" t="s">
         <v>25</v>
@@ -16483,10 +16483,10 @@
         <v>11</v>
       </c>
       <c r="C481">
-        <v>7330</v>
+        <v>7335</v>
       </c>
       <c r="D481">
-        <v>10818088</v>
+        <v>10825588</v>
       </c>
       <c r="E481" t="s">
         <v>25</v>
@@ -16547,10 +16547,10 @@
         <v>11</v>
       </c>
       <c r="C483">
-        <v>1975</v>
+        <v>1978</v>
       </c>
       <c r="D483">
-        <v>2856292</v>
+        <v>2860792</v>
       </c>
       <c r="E483" t="s">
         <v>25</v>
@@ -16643,10 +16643,10 @@
         <v>11</v>
       </c>
       <c r="C486">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D486">
-        <v>234637</v>
+        <v>236137</v>
       </c>
       <c r="E486" t="s">
         <v>25</v>
@@ -16675,10 +16675,10 @@
         <v>11</v>
       </c>
       <c r="C487">
-        <v>4725</v>
+        <v>4732</v>
       </c>
       <c r="D487">
-        <v>6088405</v>
+        <v>6096791</v>
       </c>
       <c r="E487" t="s">
         <v>25</v>
@@ -16739,10 +16739,10 @@
         <v>11</v>
       </c>
       <c r="C489">
-        <v>1807</v>
+        <v>1809</v>
       </c>
       <c r="D489">
-        <v>2669293</v>
+        <v>2672293</v>
       </c>
       <c r="E489" t="s">
         <v>25</v>
@@ -16803,10 +16803,10 @@
         <v>11</v>
       </c>
       <c r="C491">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D491">
-        <v>1226253</v>
+        <v>1227753</v>
       </c>
       <c r="E491" t="s">
         <v>25</v>
@@ -16899,10 +16899,10 @@
         <v>11</v>
       </c>
       <c r="C494">
-        <v>2276</v>
+        <v>2279</v>
       </c>
       <c r="D494">
-        <v>2820792</v>
+        <v>2823419</v>
       </c>
       <c r="E494" t="s">
         <v>25</v>
@@ -16963,10 +16963,10 @@
         <v>11</v>
       </c>
       <c r="C496">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D496">
-        <v>762429</v>
+        <v>763929</v>
       </c>
       <c r="E496" t="s">
         <v>25</v>
@@ -17027,10 +17027,10 @@
         <v>11</v>
       </c>
       <c r="C498">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D498">
-        <v>393435</v>
+        <v>396435</v>
       </c>
       <c r="E498" t="s">
         <v>25</v>
@@ -17123,10 +17123,10 @@
         <v>11</v>
       </c>
       <c r="C501">
-        <v>5799</v>
+        <v>5812</v>
       </c>
       <c r="D501">
-        <v>7396824</v>
+        <v>7414480</v>
       </c>
       <c r="E501" t="s">
         <v>25</v>
@@ -17251,10 +17251,10 @@
         <v>11</v>
       </c>
       <c r="C505">
-        <v>2407</v>
+        <v>2413</v>
       </c>
       <c r="D505">
-        <v>3564242</v>
+        <v>3570863</v>
       </c>
       <c r="E505" t="s">
         <v>25</v>
@@ -17283,10 +17283,10 @@
         <v>11</v>
       </c>
       <c r="C506">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D506">
-        <v>672242</v>
+        <v>672938</v>
       </c>
       <c r="E506" t="s">
         <v>25</v>
@@ -17379,10 +17379,10 @@
         <v>11</v>
       </c>
       <c r="C509">
-        <v>11899</v>
+        <v>11916</v>
       </c>
       <c r="D509">
-        <v>14774817</v>
+        <v>14797219</v>
       </c>
       <c r="E509" t="s">
         <v>25</v>
@@ -17507,10 +17507,10 @@
         <v>11</v>
       </c>
       <c r="C513">
-        <v>3715</v>
+        <v>3720</v>
       </c>
       <c r="D513">
-        <v>5444737</v>
+        <v>5450969</v>
       </c>
       <c r="E513" t="s">
         <v>25</v>
@@ -17571,10 +17571,10 @@
         <v>11</v>
       </c>
       <c r="C515">
-        <v>1415</v>
+        <v>1417</v>
       </c>
       <c r="D515">
-        <v>2050144</v>
+        <v>2053144</v>
       </c>
       <c r="E515" t="s">
         <v>25</v>
@@ -17635,10 +17635,10 @@
         <v>11</v>
       </c>
       <c r="C517">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D517">
-        <v>190936</v>
+        <v>193936</v>
       </c>
       <c r="E517" t="s">
         <v>25</v>
@@ -17667,10 +17667,10 @@
         <v>11</v>
       </c>
       <c r="C518">
-        <v>43175</v>
+        <v>43243</v>
       </c>
       <c r="D518">
-        <v>54799581</v>
+        <v>54878912</v>
       </c>
       <c r="E518" t="s">
         <v>25</v>
@@ -17795,10 +17795,10 @@
         <v>11</v>
       </c>
       <c r="C522">
-        <v>17620</v>
+        <v>17664</v>
       </c>
       <c r="D522">
-        <v>25977797</v>
+        <v>26040543</v>
       </c>
       <c r="E522" t="s">
         <v>25</v>
@@ -17859,10 +17859,10 @@
         <v>11</v>
       </c>
       <c r="C524">
-        <v>8082</v>
+        <v>8098</v>
       </c>
       <c r="D524">
-        <v>11688250</v>
+        <v>11710553</v>
       </c>
       <c r="E524" t="s">
         <v>25</v>
@@ -17923,10 +17923,10 @@
         <v>11</v>
       </c>
       <c r="C526">
-        <v>1112</v>
+        <v>1118</v>
       </c>
       <c r="D526">
-        <v>1603491</v>
+        <v>1611756</v>
       </c>
       <c r="E526" t="s">
         <v>25</v>
@@ -17987,10 +17987,10 @@
         <v>11</v>
       </c>
       <c r="C528">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D528">
-        <v>648066</v>
+        <v>649566</v>
       </c>
       <c r="E528" t="s">
         <v>25</v>
@@ -18019,10 +18019,10 @@
         <v>11</v>
       </c>
       <c r="C529">
-        <v>6716</v>
+        <v>6728</v>
       </c>
       <c r="D529">
-        <v>8332965</v>
+        <v>8347632</v>
       </c>
       <c r="E529" t="s">
         <v>25</v>
@@ -18115,10 +18115,10 @@
         <v>11</v>
       </c>
       <c r="C532">
-        <v>2829</v>
+        <v>2835</v>
       </c>
       <c r="D532">
-        <v>4159054</v>
+        <v>4168054</v>
       </c>
       <c r="E532" t="s">
         <v>25</v>
@@ -18179,10 +18179,10 @@
         <v>11</v>
       </c>
       <c r="C534">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="D534">
-        <v>1387888</v>
+        <v>1390888</v>
       </c>
       <c r="E534" t="s">
         <v>25</v>
@@ -18243,10 +18243,10 @@
         <v>11</v>
       </c>
       <c r="C536">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D536">
-        <v>108633</v>
+        <v>111633</v>
       </c>
       <c r="E536" t="s">
         <v>25</v>
@@ -18275,10 +18275,10 @@
         <v>11</v>
       </c>
       <c r="C537">
-        <v>11021</v>
+        <v>11039</v>
       </c>
       <c r="D537">
-        <v>13785017</v>
+        <v>13805130</v>
       </c>
       <c r="E537" t="s">
         <v>25</v>
@@ -18403,10 +18403,10 @@
         <v>11</v>
       </c>
       <c r="C541">
-        <v>4594</v>
+        <v>4605</v>
       </c>
       <c r="D541">
-        <v>6740347</v>
+        <v>6755523</v>
       </c>
       <c r="E541" t="s">
         <v>25</v>
@@ -18467,10 +18467,10 @@
         <v>11</v>
       </c>
       <c r="C543">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D543">
-        <v>2006330</v>
+        <v>2007830</v>
       </c>
       <c r="E543" t="s">
         <v>25</v>
@@ -18499,10 +18499,10 @@
         <v>11</v>
       </c>
       <c r="C544">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D544">
-        <v>235810</v>
+        <v>237310</v>
       </c>
       <c r="E544" t="s">
         <v>25</v>
@@ -18563,10 +18563,10 @@
         <v>11</v>
       </c>
       <c r="C546">
-        <v>7218</v>
+        <v>7234</v>
       </c>
       <c r="D546">
-        <v>9028036</v>
+        <v>9047132</v>
       </c>
       <c r="E546" t="s">
         <v>25</v>
@@ -18627,10 +18627,10 @@
         <v>11</v>
       </c>
       <c r="C548">
-        <v>2886</v>
+        <v>2887</v>
       </c>
       <c r="D548">
-        <v>4256475</v>
+        <v>4257975</v>
       </c>
       <c r="E548" t="s">
         <v>25</v>
@@ -18691,10 +18691,10 @@
         <v>11</v>
       </c>
       <c r="C550">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="D550">
-        <v>1536426</v>
+        <v>1537926</v>
       </c>
       <c r="E550" t="s">
         <v>25</v>
@@ -18723,10 +18723,10 @@
         <v>11</v>
       </c>
       <c r="C551">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D551">
-        <v>200170</v>
+        <v>201670</v>
       </c>
       <c r="E551" t="s">
         <v>25</v>
@@ -18787,10 +18787,10 @@
         <v>11</v>
       </c>
       <c r="C553">
-        <v>18086</v>
+        <v>18121</v>
       </c>
       <c r="D553">
-        <v>22873013</v>
+        <v>22912694</v>
       </c>
       <c r="E553" t="s">
         <v>25</v>
@@ -18883,10 +18883,10 @@
         <v>11</v>
       </c>
       <c r="C556">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D556">
-        <v>101554</v>
+        <v>103054</v>
       </c>
       <c r="E556" t="s">
         <v>25</v>
@@ -18915,10 +18915,10 @@
         <v>11</v>
       </c>
       <c r="C557">
-        <v>8377</v>
+        <v>8396</v>
       </c>
       <c r="D557">
-        <v>12315357</v>
+        <v>12343857</v>
       </c>
       <c r="E557" t="s">
         <v>25</v>
@@ -18979,10 +18979,10 @@
         <v>11</v>
       </c>
       <c r="C559">
-        <v>2613</v>
+        <v>2621</v>
       </c>
       <c r="D559">
-        <v>3769428</v>
+        <v>3781428</v>
       </c>
       <c r="E559" t="s">
         <v>25</v>
@@ -19043,10 +19043,10 @@
         <v>11</v>
       </c>
       <c r="C561">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="D561">
-        <v>504889</v>
+        <v>512389</v>
       </c>
       <c r="E561" t="s">
         <v>25</v>
@@ -19075,10 +19075,10 @@
         <v>11</v>
       </c>
       <c r="C562">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D562">
-        <v>423148</v>
+        <v>427339</v>
       </c>
       <c r="E562" t="s">
         <v>25</v>
@@ -19107,10 +19107,10 @@
         <v>11</v>
       </c>
       <c r="C563">
-        <v>7289</v>
+        <v>7301</v>
       </c>
       <c r="D563">
-        <v>9134355</v>
+        <v>9146704</v>
       </c>
       <c r="E563" t="s">
         <v>25</v>
@@ -19203,10 +19203,10 @@
         <v>11</v>
       </c>
       <c r="C566">
-        <v>3152</v>
+        <v>3161</v>
       </c>
       <c r="D566">
-        <v>4639340</v>
+        <v>4652840</v>
       </c>
       <c r="E566" t="s">
         <v>25</v>
@@ -19235,10 +19235,10 @@
         <v>11</v>
       </c>
       <c r="C567">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D567">
-        <v>1029316</v>
+        <v>1032316</v>
       </c>
       <c r="E567" t="s">
         <v>25</v>
@@ -19299,10 +19299,10 @@
         <v>11</v>
       </c>
       <c r="C569">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D569">
-        <v>199546</v>
+        <v>201046</v>
       </c>
       <c r="E569" t="s">
         <v>25</v>
@@ -19331,10 +19331,10 @@
         <v>11</v>
       </c>
       <c r="C570">
-        <v>3915</v>
+        <v>3921</v>
       </c>
       <c r="D570">
-        <v>4693476</v>
+        <v>4700007</v>
       </c>
       <c r="E570" t="s">
         <v>26</v>
@@ -19395,10 +19395,10 @@
         <v>11</v>
       </c>
       <c r="C572">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="D572">
-        <v>1550537</v>
+        <v>1553537</v>
       </c>
       <c r="E572" t="s">
         <v>26</v>
@@ -19427,10 +19427,10 @@
         <v>11</v>
       </c>
       <c r="C573">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D573">
-        <v>867806</v>
+        <v>872306</v>
       </c>
       <c r="E573" t="s">
         <v>26</v>
@@ -19459,10 +19459,10 @@
         <v>11</v>
       </c>
       <c r="C574">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D574">
-        <v>119816</v>
+        <v>125816</v>
       </c>
       <c r="E574" t="s">
         <v>26</v>
@@ -19523,10 +19523,10 @@
         <v>11</v>
       </c>
       <c r="C576">
-        <v>10095</v>
+        <v>10108</v>
       </c>
       <c r="D576">
-        <v>12422322</v>
+        <v>12437886</v>
       </c>
       <c r="E576" t="s">
         <v>26</v>
@@ -19651,10 +19651,10 @@
         <v>11</v>
       </c>
       <c r="C580">
-        <v>3551</v>
+        <v>3562</v>
       </c>
       <c r="D580">
-        <v>5218952</v>
+        <v>5235452</v>
       </c>
       <c r="E580" t="s">
         <v>26</v>
@@ -19683,10 +19683,10 @@
         <v>11</v>
       </c>
       <c r="C581">
-        <v>2110</v>
+        <v>2112</v>
       </c>
       <c r="D581">
-        <v>3089675</v>
+        <v>3092675</v>
       </c>
       <c r="E581" t="s">
         <v>26</v>
@@ -19811,10 +19811,10 @@
         <v>11</v>
       </c>
       <c r="C585">
-        <v>6992</v>
+        <v>7001</v>
       </c>
       <c r="D585">
-        <v>8997870</v>
+        <v>9008880</v>
       </c>
       <c r="E585" t="s">
         <v>26</v>
@@ -19907,10 +19907,10 @@
         <v>11</v>
       </c>
       <c r="C588">
-        <v>2521</v>
+        <v>2527</v>
       </c>
       <c r="D588">
-        <v>3704897</v>
+        <v>3713897</v>
       </c>
       <c r="E588" t="s">
         <v>26</v>
@@ -20035,10 +20035,10 @@
         <v>11</v>
       </c>
       <c r="C592">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D592">
-        <v>137671</v>
+        <v>139171</v>
       </c>
       <c r="E592" t="s">
         <v>26</v>
@@ -20067,10 +20067,10 @@
         <v>11</v>
       </c>
       <c r="C593">
-        <v>19530</v>
+        <v>19546</v>
       </c>
       <c r="D593">
-        <v>24265956</v>
+        <v>24283511</v>
       </c>
       <c r="E593" t="s">
         <v>26</v>
@@ -20195,10 +20195,10 @@
         <v>11</v>
       </c>
       <c r="C597">
-        <v>8622</v>
+        <v>8634</v>
       </c>
       <c r="D597">
-        <v>12694065</v>
+        <v>12712065</v>
       </c>
       <c r="E597" t="s">
         <v>26</v>
@@ -20259,10 +20259,10 @@
         <v>11</v>
       </c>
       <c r="C599">
-        <v>3843</v>
+        <v>3847</v>
       </c>
       <c r="D599">
-        <v>5579861</v>
+        <v>5585602</v>
       </c>
       <c r="E599" t="s">
         <v>26</v>
@@ -20323,10 +20323,10 @@
         <v>11</v>
       </c>
       <c r="C601">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D601">
-        <v>365426</v>
+        <v>366926</v>
       </c>
       <c r="E601" t="s">
         <v>26</v>
@@ -20355,10 +20355,10 @@
         <v>11</v>
       </c>
       <c r="C602">
-        <v>4653</v>
+        <v>4662</v>
       </c>
       <c r="D602">
-        <v>5862939</v>
+        <v>5874705</v>
       </c>
       <c r="E602" t="s">
         <v>26</v>
@@ -20451,10 +20451,10 @@
         <v>11</v>
       </c>
       <c r="C605">
-        <v>1753</v>
+        <v>1760</v>
       </c>
       <c r="D605">
-        <v>2576866</v>
+        <v>2585865</v>
       </c>
       <c r="E605" t="s">
         <v>26</v>
@@ -20483,10 +20483,10 @@
         <v>11</v>
       </c>
       <c r="C606">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D606">
-        <v>1037457</v>
+        <v>1040457</v>
       </c>
       <c r="E606" t="s">
         <v>26</v>
@@ -20515,10 +20515,10 @@
         <v>11</v>
       </c>
       <c r="C607">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D607">
-        <v>276094</v>
+        <v>277420</v>
       </c>
       <c r="E607" t="s">
         <v>26</v>
@@ -20547,10 +20547,10 @@
         <v>11</v>
       </c>
       <c r="C608">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D608">
-        <v>124931</v>
+        <v>127931</v>
       </c>
       <c r="E608" t="s">
         <v>26</v>
@@ -20579,10 +20579,10 @@
         <v>11</v>
       </c>
       <c r="C609">
-        <v>32434</v>
+        <v>32497</v>
       </c>
       <c r="D609">
-        <v>40702277</v>
+        <v>40778370</v>
       </c>
       <c r="E609" t="s">
         <v>26</v>
@@ -20707,10 +20707,10 @@
         <v>11</v>
       </c>
       <c r="C613">
-        <v>13906</v>
+        <v>13928</v>
       </c>
       <c r="D613">
-        <v>20462889</v>
+        <v>20494998</v>
       </c>
       <c r="E613" t="s">
         <v>26</v>
@@ -20803,10 +20803,10 @@
         <v>11</v>
       </c>
       <c r="C616">
-        <v>7579</v>
+        <v>7593</v>
       </c>
       <c r="D616">
-        <v>10989890</v>
+        <v>11010005</v>
       </c>
       <c r="E616" t="s">
         <v>26</v>
@@ -20867,10 +20867,10 @@
         <v>11</v>
       </c>
       <c r="C618">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D618">
-        <v>349634</v>
+        <v>351134</v>
       </c>
       <c r="E618" t="s">
         <v>26</v>
@@ -20899,10 +20899,10 @@
         <v>11</v>
       </c>
       <c r="C619">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D619">
-        <v>755369</v>
+        <v>758369</v>
       </c>
       <c r="E619" t="s">
         <v>26</v>
@@ -20931,10 +20931,10 @@
         <v>11</v>
       </c>
       <c r="C620">
-        <v>6619</v>
+        <v>6628</v>
       </c>
       <c r="D620">
-        <v>8391013</v>
+        <v>8402673</v>
       </c>
       <c r="E620" t="s">
         <v>26</v>
@@ -21059,10 +21059,10 @@
         <v>11</v>
       </c>
       <c r="C624">
-        <v>2385</v>
+        <v>2389</v>
       </c>
       <c r="D624">
-        <v>3504405</v>
+        <v>3510405</v>
       </c>
       <c r="E624" t="s">
         <v>26</v>
@@ -21123,10 +21123,10 @@
         <v>11</v>
       </c>
       <c r="C626">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="D626">
-        <v>1079104</v>
+        <v>1082104</v>
       </c>
       <c r="E626" t="s">
         <v>26</v>
@@ -21251,10 +21251,10 @@
         <v>11</v>
       </c>
       <c r="C630">
-        <v>34611</v>
+        <v>34664</v>
       </c>
       <c r="D630">
-        <v>43211739</v>
+        <v>43274148</v>
       </c>
       <c r="E630" t="s">
         <v>26</v>
@@ -21443,10 +21443,10 @@
         <v>11</v>
       </c>
       <c r="C636">
-        <v>14630</v>
+        <v>14657</v>
       </c>
       <c r="D636">
-        <v>21558883</v>
+        <v>21597439</v>
       </c>
       <c r="E636" t="s">
         <v>26</v>
@@ -21507,10 +21507,10 @@
         <v>11</v>
       </c>
       <c r="C638">
-        <v>8758</v>
+        <v>8770</v>
       </c>
       <c r="D638">
-        <v>12730609</v>
+        <v>12746408</v>
       </c>
       <c r="E638" t="s">
         <v>26</v>
@@ -21571,10 +21571,10 @@
         <v>11</v>
       </c>
       <c r="C640">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="D640">
-        <v>745521</v>
+        <v>753021</v>
       </c>
       <c r="E640" t="s">
         <v>26</v>
@@ -21603,10 +21603,10 @@
         <v>11</v>
       </c>
       <c r="C641">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D641">
-        <v>698001</v>
+        <v>698534</v>
       </c>
       <c r="E641" t="s">
         <v>26</v>
@@ -21667,10 +21667,10 @@
         <v>11</v>
       </c>
       <c r="C643">
-        <v>4630</v>
+        <v>4641</v>
       </c>
       <c r="D643">
-        <v>5772782</v>
+        <v>5789209</v>
       </c>
       <c r="E643" t="s">
         <v>26</v>
@@ -21731,10 +21731,10 @@
         <v>11</v>
       </c>
       <c r="C645">
-        <v>1621</v>
+        <v>1625</v>
       </c>
       <c r="D645">
-        <v>2373229</v>
+        <v>2379229</v>
       </c>
       <c r="E645" t="s">
         <v>26</v>
@@ -21763,10 +21763,10 @@
         <v>11</v>
       </c>
       <c r="C646">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="D646">
-        <v>982556</v>
+        <v>987056</v>
       </c>
       <c r="E646" t="s">
         <v>26</v>
@@ -21859,10 +21859,10 @@
         <v>11</v>
       </c>
       <c r="C649">
-        <v>1772</v>
+        <v>1775</v>
       </c>
       <c r="D649">
-        <v>2276823</v>
+        <v>2281323</v>
       </c>
       <c r="E649" t="s">
         <v>26</v>
@@ -21923,10 +21923,10 @@
         <v>11</v>
       </c>
       <c r="C651">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D651">
-        <v>1070099</v>
+        <v>1073099</v>
       </c>
       <c r="E651" t="s">
         <v>26</v>
@@ -21987,10 +21987,10 @@
         <v>11</v>
       </c>
       <c r="C653">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D653">
-        <v>318993</v>
+        <v>320493</v>
       </c>
       <c r="E653" t="s">
         <v>26</v>
@@ -22019,10 +22019,10 @@
         <v>11</v>
       </c>
       <c r="C654">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D654">
-        <v>63910</v>
+        <v>65190</v>
       </c>
       <c r="E654" t="s">
         <v>26</v>
@@ -22083,10 +22083,10 @@
         <v>11</v>
       </c>
       <c r="C656">
-        <v>13591</v>
+        <v>13622</v>
       </c>
       <c r="D656">
-        <v>17208810</v>
+        <v>17247186</v>
       </c>
       <c r="E656" t="s">
         <v>26</v>
@@ -22211,10 +22211,10 @@
         <v>11</v>
       </c>
       <c r="C660">
-        <v>5044</v>
+        <v>5050</v>
       </c>
       <c r="D660">
-        <v>7401784</v>
+        <v>7410784</v>
       </c>
       <c r="E660" t="s">
         <v>26</v>
@@ -22275,10 +22275,10 @@
         <v>11</v>
       </c>
       <c r="C662">
-        <v>2854</v>
+        <v>2862</v>
       </c>
       <c r="D662">
-        <v>4137854</v>
+        <v>4149854</v>
       </c>
       <c r="E662" t="s">
         <v>26</v>
@@ -22435,10 +22435,10 @@
         <v>11</v>
       </c>
       <c r="C667">
-        <v>8975</v>
+        <v>8989</v>
       </c>
       <c r="D667">
-        <v>11003025</v>
+        <v>11020598</v>
       </c>
       <c r="E667" t="s">
         <v>26</v>
@@ -22531,10 +22531,10 @@
         <v>11</v>
       </c>
       <c r="C670">
-        <v>3482</v>
+        <v>3488</v>
       </c>
       <c r="D670">
-        <v>5107057</v>
+        <v>5116057</v>
       </c>
       <c r="E670" t="s">
         <v>26</v>
@@ -22563,10 +22563,10 @@
         <v>11</v>
       </c>
       <c r="C671">
-        <v>1471</v>
+        <v>1475</v>
       </c>
       <c r="D671">
-        <v>2131734</v>
+        <v>2134885</v>
       </c>
       <c r="E671" t="s">
         <v>26</v>
@@ -22659,10 +22659,10 @@
         <v>11</v>
       </c>
       <c r="C674">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D674">
-        <v>155536</v>
+        <v>157036</v>
       </c>
       <c r="E674" t="s">
         <v>26</v>
@@ -22691,10 +22691,10 @@
         <v>11</v>
       </c>
       <c r="C675">
-        <v>5876</v>
+        <v>5885</v>
       </c>
       <c r="D675">
-        <v>7256879</v>
+        <v>7269577</v>
       </c>
       <c r="E675" t="s">
         <v>26</v>
@@ -22787,10 +22787,10 @@
         <v>11</v>
       </c>
       <c r="C678">
-        <v>2263</v>
+        <v>2269</v>
       </c>
       <c r="D678">
-        <v>3333210</v>
+        <v>3342210</v>
       </c>
       <c r="E678" t="s">
         <v>26</v>
@@ -22915,10 +22915,10 @@
         <v>11</v>
       </c>
       <c r="C682">
-        <v>25974</v>
+        <v>26025</v>
       </c>
       <c r="D682">
-        <v>33220509</v>
+        <v>33278338</v>
       </c>
       <c r="E682" t="s">
         <v>27</v>
@@ -23043,10 +23043,10 @@
         <v>11</v>
       </c>
       <c r="C686">
-        <v>14022</v>
+        <v>14043</v>
       </c>
       <c r="D686">
-        <v>20676915</v>
+        <v>20707449</v>
       </c>
       <c r="E686" t="s">
         <v>27</v>
@@ -23107,10 +23107,10 @@
         <v>11</v>
       </c>
       <c r="C688">
-        <v>3553</v>
+        <v>3558</v>
       </c>
       <c r="D688">
-        <v>5129586</v>
+        <v>5137086</v>
       </c>
       <c r="E688" t="s">
         <v>27</v>
@@ -23139,10 +23139,10 @@
         <v>11</v>
       </c>
       <c r="C689">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D689">
-        <v>524798</v>
+        <v>526298</v>
       </c>
       <c r="E689" t="s">
         <v>27</v>
@@ -23171,10 +23171,10 @@
         <v>11</v>
       </c>
       <c r="C690">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D690">
-        <v>555720</v>
+        <v>560220</v>
       </c>
       <c r="E690" t="s">
         <v>27</v>
@@ -23203,10 +23203,10 @@
         <v>11</v>
       </c>
       <c r="C691">
-        <v>12894</v>
+        <v>12913</v>
       </c>
       <c r="D691">
-        <v>16301592</v>
+        <v>16327276</v>
       </c>
       <c r="E691" t="s">
         <v>27</v>
@@ -23299,10 +23299,10 @@
         <v>11</v>
       </c>
       <c r="C694">
-        <v>6688</v>
+        <v>6700</v>
       </c>
       <c r="D694">
-        <v>9857507</v>
+        <v>9873636</v>
       </c>
       <c r="E694" t="s">
         <v>27</v>
@@ -23363,10 +23363,10 @@
         <v>11</v>
       </c>
       <c r="C696">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="D696">
-        <v>1995816</v>
+        <v>1997901</v>
       </c>
       <c r="E696" t="s">
         <v>27</v>
@@ -23427,10 +23427,10 @@
         <v>11</v>
       </c>
       <c r="C698">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D698">
-        <v>357745</v>
+        <v>362245</v>
       </c>
       <c r="E698" t="s">
         <v>27</v>
@@ -23459,10 +23459,10 @@
         <v>11</v>
       </c>
       <c r="C699">
-        <v>4314</v>
+        <v>4323</v>
       </c>
       <c r="D699">
-        <v>5549243</v>
+        <v>5558120</v>
       </c>
       <c r="E699" t="s">
         <v>27</v>
@@ -23523,10 +23523,10 @@
         <v>11</v>
       </c>
       <c r="C701">
-        <v>2067</v>
+        <v>2069</v>
       </c>
       <c r="D701">
-        <v>3063790</v>
+        <v>3066790</v>
       </c>
       <c r="E701" t="s">
         <v>27</v>
@@ -23555,10 +23555,10 @@
         <v>11</v>
       </c>
       <c r="C702">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D702">
-        <v>573679</v>
+        <v>575179</v>
       </c>
       <c r="E702" t="s">
         <v>27</v>
@@ -23651,10 +23651,10 @@
         <v>11</v>
       </c>
       <c r="C705">
-        <v>8173</v>
+        <v>8183</v>
       </c>
       <c r="D705">
-        <v>10334236</v>
+        <v>10347104</v>
       </c>
       <c r="E705" t="s">
         <v>27</v>
@@ -23747,10 +23747,10 @@
         <v>11</v>
       </c>
       <c r="C708">
-        <v>3545</v>
+        <v>3552</v>
       </c>
       <c r="D708">
-        <v>5220383</v>
+        <v>5230883</v>
       </c>
       <c r="E708" t="s">
         <v>27</v>
@@ -23811,10 +23811,10 @@
         <v>11</v>
       </c>
       <c r="C710">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D710">
-        <v>1241322</v>
+        <v>1242822</v>
       </c>
       <c r="E710" t="s">
         <v>27</v>
@@ -23939,10 +23939,10 @@
         <v>11</v>
       </c>
       <c r="C714">
-        <v>12253</v>
+        <v>12276</v>
       </c>
       <c r="D714">
-        <v>15640547</v>
+        <v>15671255</v>
       </c>
       <c r="E714" t="s">
         <v>27</v>
@@ -24067,10 +24067,10 @@
         <v>11</v>
       </c>
       <c r="C718">
-        <v>6895</v>
+        <v>6899</v>
       </c>
       <c r="D718">
-        <v>10144648</v>
+        <v>10150648</v>
       </c>
       <c r="E718" t="s">
         <v>27</v>
@@ -24131,10 +24131,10 @@
         <v>11</v>
       </c>
       <c r="C720">
-        <v>1306</v>
+        <v>1311</v>
       </c>
       <c r="D720">
-        <v>1882906</v>
+        <v>1890406</v>
       </c>
       <c r="E720" t="s">
         <v>27</v>
@@ -24195,10 +24195,10 @@
         <v>11</v>
       </c>
       <c r="C722">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D722">
-        <v>273000</v>
+        <v>274500</v>
       </c>
       <c r="E722" t="s">
         <v>27</v>
@@ -24227,10 +24227,10 @@
         <v>11</v>
       </c>
       <c r="C723">
-        <v>38723</v>
+        <v>38812</v>
       </c>
       <c r="D723">
-        <v>49974264</v>
+        <v>50085428</v>
       </c>
       <c r="E723" t="s">
         <v>28</v>
@@ -24291,10 +24291,10 @@
         <v>11</v>
       </c>
       <c r="C725">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D725">
-        <v>59070</v>
+        <v>60060</v>
       </c>
       <c r="E725" t="s">
         <v>28</v>
@@ -24387,10 +24387,10 @@
         <v>11</v>
       </c>
       <c r="C728">
-        <v>16162</v>
+        <v>16200</v>
       </c>
       <c r="D728">
-        <v>23822870</v>
+        <v>23877778</v>
       </c>
       <c r="E728" t="s">
         <v>28</v>
@@ -24451,10 +24451,10 @@
         <v>11</v>
       </c>
       <c r="C730">
-        <v>10257</v>
+        <v>10274</v>
       </c>
       <c r="D730">
-        <v>14926438</v>
+        <v>14951882</v>
       </c>
       <c r="E730" t="s">
         <v>28</v>
@@ -24547,10 +24547,10 @@
         <v>11</v>
       </c>
       <c r="C733">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D733">
-        <v>527819</v>
+        <v>528679</v>
       </c>
       <c r="E733" t="s">
         <v>28</v>
@@ -24579,10 +24579,10 @@
         <v>11</v>
       </c>
       <c r="C734">
-        <v>5247</v>
+        <v>5254</v>
       </c>
       <c r="D734">
-        <v>6674474</v>
+        <v>6682937</v>
       </c>
       <c r="E734" t="s">
         <v>28</v>
@@ -24707,10 +24707,10 @@
         <v>11</v>
       </c>
       <c r="C738">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="D738">
-        <v>2950737</v>
+        <v>2956737</v>
       </c>
       <c r="E738" t="s">
         <v>28</v>
@@ -24739,10 +24739,10 @@
         <v>11</v>
       </c>
       <c r="C739">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D739">
-        <v>1306091</v>
+        <v>1307591</v>
       </c>
       <c r="E739" t="s">
         <v>28</v>
@@ -24835,10 +24835,10 @@
         <v>11</v>
       </c>
       <c r="C742">
-        <v>49450</v>
+        <v>49535</v>
       </c>
       <c r="D742">
-        <v>62661258</v>
+        <v>62767596</v>
       </c>
       <c r="E742" t="s">
         <v>28</v>
@@ -24995,10 +24995,10 @@
         <v>11</v>
       </c>
       <c r="C747">
-        <v>22294</v>
+        <v>22350</v>
       </c>
       <c r="D747">
-        <v>32877383</v>
+        <v>32958403</v>
       </c>
       <c r="E747" t="s">
         <v>28</v>
@@ -25059,10 +25059,10 @@
         <v>11</v>
       </c>
       <c r="C749">
-        <v>15537</v>
+        <v>15571</v>
       </c>
       <c r="D749">
-        <v>22623598</v>
+        <v>22670282</v>
       </c>
       <c r="E749" t="s">
         <v>28</v>
@@ -25091,10 +25091,10 @@
         <v>11</v>
       </c>
       <c r="C750">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D750">
-        <v>483976</v>
+        <v>485476</v>
       </c>
       <c r="E750" t="s">
         <v>28</v>
@@ -25123,10 +25123,10 @@
         <v>11</v>
       </c>
       <c r="C751">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D751">
-        <v>1030868</v>
+        <v>1032068</v>
       </c>
       <c r="E751" t="s">
         <v>28</v>
@@ -25155,10 +25155,10 @@
         <v>11</v>
       </c>
       <c r="C752">
-        <v>6725</v>
+        <v>6737</v>
       </c>
       <c r="D752">
-        <v>8913269</v>
+        <v>8929887</v>
       </c>
       <c r="E752" t="s">
         <v>28</v>
@@ -25283,10 +25283,10 @@
         <v>11</v>
       </c>
       <c r="C756">
-        <v>2199</v>
+        <v>2204</v>
       </c>
       <c r="D756">
-        <v>3240773</v>
+        <v>3248273</v>
       </c>
       <c r="E756" t="s">
         <v>28</v>
@@ -25315,10 +25315,10 @@
         <v>11</v>
       </c>
       <c r="C757">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D757">
-        <v>998438</v>
+        <v>1002938</v>
       </c>
       <c r="E757" t="s">
         <v>28</v>
@@ -25443,10 +25443,10 @@
         <v>11</v>
       </c>
       <c r="C761">
-        <v>34435</v>
+        <v>34505</v>
       </c>
       <c r="D761">
-        <v>43427819</v>
+        <v>43512130</v>
       </c>
       <c r="E761" t="s">
         <v>28</v>
@@ -25571,10 +25571,10 @@
         <v>11</v>
       </c>
       <c r="C765">
-        <v>12297</v>
+        <v>12327</v>
       </c>
       <c r="D765">
-        <v>18121690</v>
+        <v>18164802</v>
       </c>
       <c r="E765" t="s">
         <v>28</v>
@@ -25635,10 +25635,10 @@
         <v>11</v>
       </c>
       <c r="C767">
-        <v>7993</v>
+        <v>8017</v>
       </c>
       <c r="D767">
-        <v>11600818</v>
+        <v>11633349</v>
       </c>
       <c r="E767" t="s">
         <v>28</v>
@@ -25699,10 +25699,10 @@
         <v>11</v>
       </c>
       <c r="C769">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D769">
-        <v>473489</v>
+        <v>473831</v>
       </c>
       <c r="E769" t="s">
         <v>28</v>
@@ -25731,10 +25731,10 @@
         <v>11</v>
       </c>
       <c r="C770">
-        <v>16865</v>
+        <v>16883</v>
       </c>
       <c r="D770">
-        <v>21113409</v>
+        <v>21135891</v>
       </c>
       <c r="E770" t="s">
         <v>28</v>
@@ -25859,10 +25859,10 @@
         <v>11</v>
       </c>
       <c r="C774">
-        <v>6856</v>
+        <v>6873</v>
       </c>
       <c r="D774">
-        <v>10096373</v>
+        <v>10121873</v>
       </c>
       <c r="E774" t="s">
         <v>28</v>
@@ -25923,10 +25923,10 @@
         <v>11</v>
       </c>
       <c r="C776">
-        <v>3860</v>
+        <v>3864</v>
       </c>
       <c r="D776">
-        <v>5614152</v>
+        <v>5619260</v>
       </c>
       <c r="E776" t="s">
         <v>28</v>
@@ -25955,10 +25955,10 @@
         <v>11</v>
       </c>
       <c r="C777">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D777">
-        <v>450389</v>
+        <v>451889</v>
       </c>
       <c r="E777" t="s">
         <v>28</v>
@@ -26019,10 +26019,10 @@
         <v>11</v>
       </c>
       <c r="C779">
-        <v>18490</v>
+        <v>18516</v>
       </c>
       <c r="D779">
-        <v>24101743</v>
+        <v>24138123</v>
       </c>
       <c r="E779" t="s">
         <v>29</v>
@@ -26083,10 +26083,10 @@
         <v>11</v>
       </c>
       <c r="C781">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D781">
-        <v>84888</v>
+        <v>86388</v>
       </c>
       <c r="E781" t="s">
         <v>29</v>
@@ -26115,10 +26115,10 @@
         <v>11</v>
       </c>
       <c r="C782">
-        <v>8571</v>
+        <v>8588</v>
       </c>
       <c r="D782">
-        <v>12677195</v>
+        <v>12702695</v>
       </c>
       <c r="E782" t="s">
         <v>29</v>
@@ -26179,10 +26179,10 @@
         <v>11</v>
       </c>
       <c r="C784">
-        <v>6931</v>
+        <v>6946</v>
       </c>
       <c r="D784">
-        <v>10142228</v>
+        <v>10164728</v>
       </c>
       <c r="E784" t="s">
         <v>29</v>
@@ -26211,10 +26211,10 @@
         <v>11</v>
       </c>
       <c r="C785">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D785">
-        <v>126778</v>
+        <v>128278</v>
       </c>
       <c r="E785" t="s">
         <v>29</v>
@@ -26275,10 +26275,10 @@
         <v>11</v>
       </c>
       <c r="C787">
-        <v>28586</v>
+        <v>28656</v>
       </c>
       <c r="D787">
-        <v>37822666</v>
+        <v>37910132</v>
       </c>
       <c r="E787" t="s">
         <v>29</v>
@@ -26403,10 +26403,10 @@
         <v>11</v>
       </c>
       <c r="C791">
-        <v>13935</v>
+        <v>13961</v>
       </c>
       <c r="D791">
-        <v>20574992</v>
+        <v>20613992</v>
       </c>
       <c r="E791" t="s">
         <v>29</v>
@@ -26467,10 +26467,10 @@
         <v>11</v>
       </c>
       <c r="C793">
-        <v>12447</v>
+        <v>12478</v>
       </c>
       <c r="D793">
-        <v>18139991</v>
+        <v>18183084</v>
       </c>
       <c r="E793" t="s">
         <v>29</v>
@@ -26531,10 +26531,10 @@
         <v>11</v>
       </c>
       <c r="C795">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D795">
-        <v>146002</v>
+        <v>147502</v>
       </c>
       <c r="E795" t="s">
         <v>29</v>
@@ -26595,10 +26595,10 @@
         <v>11</v>
       </c>
       <c r="C797">
-        <v>71756</v>
+        <v>71897</v>
       </c>
       <c r="D797">
-        <v>95148852</v>
+        <v>95328434</v>
       </c>
       <c r="E797" t="s">
         <v>29</v>
@@ -26723,10 +26723,10 @@
         <v>11</v>
       </c>
       <c r="C801">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D801">
-        <v>370760</v>
+        <v>373760</v>
       </c>
       <c r="E801" t="s">
         <v>29</v>
@@ -26787,10 +26787,10 @@
         <v>11</v>
       </c>
       <c r="C803">
-        <v>47631</v>
+        <v>47752</v>
       </c>
       <c r="D803">
-        <v>70333060</v>
+        <v>70509355</v>
       </c>
       <c r="E803" t="s">
         <v>29</v>
@@ -26819,10 +26819,10 @@
         <v>11</v>
       </c>
       <c r="C804">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D804">
-        <v>187519</v>
+        <v>189019</v>
       </c>
       <c r="E804" t="s">
         <v>29</v>
@@ -26883,10 +26883,10 @@
         <v>11</v>
       </c>
       <c r="C806">
-        <v>33084</v>
+        <v>33156</v>
       </c>
       <c r="D806">
-        <v>48200008</v>
+        <v>48304636</v>
       </c>
       <c r="E806" t="s">
         <v>29</v>
@@ -27011,10 +27011,10 @@
         <v>11</v>
       </c>
       <c r="C810">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="D810">
-        <v>1525938</v>
+        <v>1530438</v>
       </c>
       <c r="E810" t="s">
         <v>29</v>
@@ -27075,10 +27075,10 @@
         <v>11</v>
       </c>
       <c r="C812">
-        <v>28107</v>
+        <v>28168</v>
       </c>
       <c r="D812">
-        <v>37466571</v>
+        <v>37553439</v>
       </c>
       <c r="E812" t="s">
         <v>29</v>
@@ -27203,10 +27203,10 @@
         <v>11</v>
       </c>
       <c r="C816">
-        <v>13711</v>
+        <v>13744</v>
       </c>
       <c r="D816">
-        <v>20289069</v>
+        <v>20337436</v>
       </c>
       <c r="E816" t="s">
         <v>29</v>
@@ -27267,10 +27267,10 @@
         <v>11</v>
       </c>
       <c r="C818">
-        <v>12716</v>
+        <v>12747</v>
       </c>
       <c r="D818">
-        <v>18633156</v>
+        <v>18678752</v>
       </c>
       <c r="E818" t="s">
         <v>29</v>
@@ -27331,10 +27331,10 @@
         <v>11</v>
       </c>
       <c r="C820">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D820">
-        <v>416881</v>
+        <v>418381</v>
       </c>
       <c r="E820" t="s">
         <v>29</v>
@@ -27363,10 +27363,10 @@
         <v>11</v>
       </c>
       <c r="C821">
-        <v>22548</v>
+        <v>22587</v>
       </c>
       <c r="D821">
-        <v>29355365</v>
+        <v>29398951</v>
       </c>
       <c r="E821" t="s">
         <v>29</v>
@@ -27491,10 +27491,10 @@
         <v>11</v>
       </c>
       <c r="C825">
-        <v>9825</v>
+        <v>9853</v>
       </c>
       <c r="D825">
-        <v>14521831</v>
+        <v>14563831</v>
       </c>
       <c r="E825" t="s">
         <v>29</v>
@@ -27555,10 +27555,10 @@
         <v>11</v>
       </c>
       <c r="C827">
-        <v>7650</v>
+        <v>7667</v>
       </c>
       <c r="D827">
-        <v>11125986</v>
+        <v>11150491</v>
       </c>
       <c r="E827" t="s">
         <v>29</v>
@@ -27651,10 +27651,10 @@
         <v>11</v>
       </c>
       <c r="C830">
-        <v>20301</v>
+        <v>20344</v>
       </c>
       <c r="D830">
-        <v>26883430</v>
+        <v>26940101</v>
       </c>
       <c r="E830" t="s">
         <v>29</v>
@@ -27747,10 +27747,10 @@
         <v>11</v>
       </c>
       <c r="C833">
-        <v>8874</v>
+        <v>8904</v>
       </c>
       <c r="D833">
-        <v>13125783</v>
+        <v>13167835</v>
       </c>
       <c r="E833" t="s">
         <v>29</v>
@@ -27811,10 +27811,10 @@
         <v>11</v>
       </c>
       <c r="C835">
-        <v>8078</v>
+        <v>8111</v>
       </c>
       <c r="D835">
-        <v>11761875</v>
+        <v>11811242</v>
       </c>
       <c r="E835" t="s">
         <v>29</v>
@@ -27907,10 +27907,10 @@
         <v>11</v>
       </c>
       <c r="C838">
-        <v>25307</v>
+        <v>25353</v>
       </c>
       <c r="D838">
-        <v>33505709</v>
+        <v>33565460</v>
       </c>
       <c r="E838" t="s">
         <v>29</v>
@@ -28003,10 +28003,10 @@
         <v>11</v>
       </c>
       <c r="C841">
-        <v>10904</v>
+        <v>10938</v>
       </c>
       <c r="D841">
-        <v>16101338</v>
+        <v>16150891</v>
       </c>
       <c r="E841" t="s">
         <v>29</v>
@@ -28067,10 +28067,10 @@
         <v>11</v>
       </c>
       <c r="C843">
-        <v>10062</v>
+        <v>10086</v>
       </c>
       <c r="D843">
-        <v>14658575</v>
+        <v>14692119</v>
       </c>
       <c r="E843" t="s">
         <v>29</v>
@@ -28099,10 +28099,10 @@
         <v>11</v>
       </c>
       <c r="C844">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D844">
-        <v>134605</v>
+        <v>136105</v>
       </c>
       <c r="E844" t="s">
         <v>29</v>
@@ -28131,10 +28131,10 @@
         <v>11</v>
       </c>
       <c r="C845">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D845">
-        <v>323888</v>
+        <v>325388</v>
       </c>
       <c r="E845" t="s">
         <v>29</v>
@@ -28163,10 +28163,10 @@
         <v>11</v>
       </c>
       <c r="C846">
-        <v>21650</v>
+        <v>21684</v>
       </c>
       <c r="D846">
-        <v>28161631</v>
+        <v>28203817</v>
       </c>
       <c r="E846" t="s">
         <v>29</v>
@@ -28259,10 +28259,10 @@
         <v>11</v>
       </c>
       <c r="C849">
-        <v>10390</v>
+        <v>10416</v>
       </c>
       <c r="D849">
-        <v>15336703</v>
+        <v>15373342</v>
       </c>
       <c r="E849" t="s">
         <v>29</v>
@@ -28323,10 +28323,10 @@
         <v>11</v>
       </c>
       <c r="C851">
-        <v>7582</v>
+        <v>7603</v>
       </c>
       <c r="D851">
-        <v>10991599</v>
+        <v>11021473</v>
       </c>
       <c r="E851" t="s">
         <v>29</v>
@@ -28387,10 +28387,10 @@
         <v>11</v>
       </c>
       <c r="C853">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D853">
-        <v>176359</v>
+        <v>179359</v>
       </c>
       <c r="E853" t="s">
         <v>29</v>
@@ -28419,10 +28419,10 @@
         <v>11</v>
       </c>
       <c r="C854">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D854">
-        <v>175986</v>
+        <v>177486</v>
       </c>
       <c r="E854" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-17 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14955</v>
+        <v>14974</v>
       </c>
       <c r="D2" t="n">
-        <v>18832802</v>
+        <v>18854347</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5884</v>
+        <v>5890</v>
       </c>
       <c r="D6" t="n">
-        <v>8616967</v>
+        <v>8624404</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3038</v>
+        <v>3043</v>
       </c>
       <c r="D8" t="n">
-        <v>4394980</v>
+        <v>4402480</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D11" t="n">
-        <v>426647</v>
+        <v>429647</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9965</v>
+        <v>9975</v>
       </c>
       <c r="D12" t="n">
-        <v>12588214</v>
+        <v>12602318</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3052</v>
+        <v>3055</v>
       </c>
       <c r="D16" t="n">
-        <v>4448440</v>
+        <v>4451828</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="D18" t="n">
-        <v>1912715</v>
+        <v>1915345</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D20" t="n">
-        <v>213784</v>
+        <v>214060</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13088</v>
+        <v>13097</v>
       </c>
       <c r="D21" t="n">
-        <v>16115968</v>
+        <v>16126269</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4629</v>
+        <v>4634</v>
       </c>
       <c r="D25" t="n">
-        <v>6782121</v>
+        <v>6789621</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>5921</v>
+        <v>5937</v>
       </c>
       <c r="D31" t="n">
-        <v>7870234</v>
+        <v>7892619</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1506</v>
+        <v>1508</v>
       </c>
       <c r="D34" t="n">
-        <v>2173046</v>
+        <v>2176046</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D37" t="n">
-        <v>680416</v>
+        <v>681916</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>20145</v>
+        <v>20162</v>
       </c>
       <c r="D40" t="n">
-        <v>24882295</v>
+        <v>24902781</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7364</v>
+        <v>7377</v>
       </c>
       <c r="D46" t="n">
-        <v>10818353</v>
+        <v>10837659</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3575</v>
+        <v>3577</v>
       </c>
       <c r="D48" t="n">
-        <v>5175979</v>
+        <v>5178979</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7592</v>
+        <v>7593</v>
       </c>
       <c r="D52" t="n">
-        <v>9727628</v>
+        <v>9729128</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2626</v>
+        <v>2627</v>
       </c>
       <c r="D56" t="n">
-        <v>3824346</v>
+        <v>3825846</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>32964</v>
+        <v>33002</v>
       </c>
       <c r="D61" t="n">
-        <v>42523266</v>
+        <v>42570242</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>12189</v>
+        <v>12199</v>
       </c>
       <c r="D65" t="n">
-        <v>17895415</v>
+        <v>17908622</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4708</v>
+        <v>4711</v>
       </c>
       <c r="D67" t="n">
-        <v>6809663</v>
+        <v>6814163</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D69" t="n">
-        <v>370961</v>
+        <v>373227</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="D71" t="n">
-        <v>385639</v>
+        <v>392408</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>42295</v>
+        <v>42344</v>
       </c>
       <c r="D73" t="n">
-        <v>54233413</v>
+        <v>54293672</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>17139</v>
+        <v>17147</v>
       </c>
       <c r="D77" t="n">
-        <v>25130175</v>
+        <v>25142175</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>8604</v>
+        <v>8610</v>
       </c>
       <c r="D79" t="n">
-        <v>12429487</v>
+        <v>12438487</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>22699</v>
+        <v>22729</v>
       </c>
       <c r="D84" t="n">
-        <v>28669297</v>
+        <v>28705929</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>8213</v>
+        <v>8223</v>
       </c>
       <c r="D88" t="n">
-        <v>12060642</v>
+        <v>12072696</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4534</v>
+        <v>4536</v>
       </c>
       <c r="D90" t="n">
-        <v>6565907</v>
+        <v>6568907</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D91" t="n">
-        <v>459813</v>
+        <v>461313</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D92" t="n">
-        <v>918973</v>
+        <v>921973</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>20047</v>
+        <v>20059</v>
       </c>
       <c r="D93" t="n">
-        <v>25220204</v>
+        <v>25235136</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D94" t="n">
-        <v>27224</v>
+        <v>27634</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4990,10 +4990,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8544</v>
+        <v>8556</v>
       </c>
       <c r="D97" t="n">
-        <v>12519284</v>
+        <v>12537284</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>3051</v>
+        <v>3053</v>
       </c>
       <c r="D99" t="n">
-        <v>4362957</v>
+        <v>4365957</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5326,10 +5326,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>71639</v>
+        <v>71834</v>
       </c>
       <c r="D104" t="n">
-        <v>91794736</v>
+        <v>92023252</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -5662,10 +5662,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>28571</v>
+        <v>28594</v>
       </c>
       <c r="D111" t="n">
-        <v>41963297</v>
+        <v>41995910</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>18865</v>
+        <v>18881</v>
       </c>
       <c r="D113" t="n">
-        <v>27260109</v>
+        <v>27284109</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5902,10 +5902,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D116" t="n">
-        <v>894108</v>
+        <v>896632</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -6046,10 +6046,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1565</v>
+        <v>1571</v>
       </c>
       <c r="D119" t="n">
-        <v>2204211</v>
+        <v>2210579</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -6094,10 +6094,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>25684</v>
+        <v>25708</v>
       </c>
       <c r="D120" t="n">
-        <v>34002999</v>
+        <v>34029942</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>9138</v>
+        <v>9148</v>
       </c>
       <c r="D124" t="n">
-        <v>13412668</v>
+        <v>13426817</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>2994</v>
+        <v>3000</v>
       </c>
       <c r="D126" t="n">
-        <v>4360644</v>
+        <v>4367232</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>14395</v>
+        <v>14422</v>
       </c>
       <c r="D130" t="n">
-        <v>18013948</v>
+        <v>18046013</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>7297</v>
+        <v>7300</v>
       </c>
       <c r="D133" t="n">
-        <v>10689622</v>
+        <v>10694122</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6814,10 +6814,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>2034</v>
+        <v>2042</v>
       </c>
       <c r="D135" t="n">
-        <v>2913919</v>
+        <v>2921363</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -7054,10 +7054,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>12453</v>
+        <v>12473</v>
       </c>
       <c r="D140" t="n">
-        <v>15625861</v>
+        <v>15648827</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>5900</v>
+        <v>5910</v>
       </c>
       <c r="D144" t="n">
-        <v>8648357</v>
+        <v>8663357</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1819</v>
+        <v>1821</v>
       </c>
       <c r="D146" t="n">
-        <v>2632233</v>
+        <v>2635233</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>5579</v>
+        <v>5585</v>
       </c>
       <c r="D150" t="n">
-        <v>6856484</v>
+        <v>6860710</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>1959</v>
+        <v>1961</v>
       </c>
       <c r="D153" t="n">
-        <v>2872077</v>
+        <v>2875077</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6926</v>
+        <v>6929</v>
       </c>
       <c r="D158" t="n">
-        <v>8635413</v>
+        <v>8639079</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8062,10 +8062,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>2710</v>
+        <v>2712</v>
       </c>
       <c r="D161" t="n">
-        <v>3972773</v>
+        <v>3975773</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D162" t="n">
-        <v>1870481</v>
+        <v>1871981</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>5242</v>
+        <v>5250</v>
       </c>
       <c r="D166" t="n">
-        <v>6631149</v>
+        <v>6638135</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8542,10 +8542,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="D171" t="n">
-        <v>2791408</v>
+        <v>2792908</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -8686,10 +8686,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D174" t="n">
-        <v>156382</v>
+        <v>157882</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -8782,10 +8782,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>14679</v>
+        <v>14700</v>
       </c>
       <c r="D176" t="n">
-        <v>18490028</v>
+        <v>18520771</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -9022,10 +9022,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>6026</v>
+        <v>6036</v>
       </c>
       <c r="D181" t="n">
-        <v>8804550</v>
+        <v>8818950</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -9070,10 +9070,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>2054</v>
+        <v>2057</v>
       </c>
       <c r="D182" t="n">
-        <v>2959780</v>
+        <v>2964280</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D184" t="n">
-        <v>659871</v>
+        <v>664998</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9214,10 +9214,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D185" t="n">
-        <v>507653</v>
+        <v>509153</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>2830</v>
+        <v>2833</v>
       </c>
       <c r="D186" t="n">
-        <v>3574394</v>
+        <v>3576492</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1372</v>
+        <v>1376</v>
       </c>
       <c r="D188" t="n">
-        <v>2008073</v>
+        <v>2014073</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D190" t="n">
-        <v>760169</v>
+        <v>763169</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9646,10 +9646,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>8470</v>
+        <v>8480</v>
       </c>
       <c r="D194" t="n">
-        <v>10612325</v>
+        <v>10624350</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -9886,10 +9886,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>1484</v>
+        <v>1487</v>
       </c>
       <c r="D199" t="n">
-        <v>2139154</v>
+        <v>2143654</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>16068</v>
+        <v>16072</v>
       </c>
       <c r="D203" t="n">
-        <v>20193239</v>
+        <v>20195771</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>7251</v>
+        <v>7258</v>
       </c>
       <c r="D207" t="n">
-        <v>10656877</v>
+        <v>10667377</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10318,10 +10318,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D208" t="n">
-        <v>1655158</v>
+        <v>1656658</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>24387</v>
+        <v>24410</v>
       </c>
       <c r="D211" t="n">
-        <v>30894329</v>
+        <v>30921695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D214" t="n">
-        <v>398715</v>
+        <v>401715</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>9935</v>
+        <v>9941</v>
       </c>
       <c r="D215" t="n">
-        <v>14533891</v>
+        <v>14541330</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>2436</v>
+        <v>2437</v>
       </c>
       <c r="D217" t="n">
-        <v>3519413</v>
+        <v>3520913</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10894,10 +10894,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D220" t="n">
-        <v>711520</v>
+        <v>713020</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>26233</v>
+        <v>26263</v>
       </c>
       <c r="D221" t="n">
-        <v>33245183</v>
+        <v>33283318</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11182,10 +11182,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>13937</v>
+        <v>13948</v>
       </c>
       <c r="D226" t="n">
-        <v>20470642</v>
+        <v>20484837</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>2429</v>
+        <v>2433</v>
       </c>
       <c r="D228" t="n">
-        <v>3486532</v>
+        <v>3492532</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D230" t="n">
-        <v>464185</v>
+        <v>467185</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11422,10 +11422,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D231" t="n">
-        <v>858204</v>
+        <v>864204</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>22555</v>
+        <v>22578</v>
       </c>
       <c r="D232" t="n">
-        <v>28584767</v>
+        <v>28604666</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>10576</v>
+        <v>10583</v>
       </c>
       <c r="D238" t="n">
-        <v>15520538</v>
+        <v>15531038</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11806,10 +11806,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>2329</v>
+        <v>2332</v>
       </c>
       <c r="D239" t="n">
-        <v>3332696</v>
+        <v>3337196</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D242" t="n">
-        <v>497863</v>
+        <v>499751</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>7334</v>
+        <v>7337</v>
       </c>
       <c r="D243" t="n">
-        <v>9206690</v>
+        <v>9209800</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -12190,10 +12190,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>2532</v>
+        <v>2536</v>
       </c>
       <c r="D247" t="n">
-        <v>3719015</v>
+        <v>3724237</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -12286,10 +12286,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="D249" t="n">
-        <v>1314173</v>
+        <v>1318673</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D251" t="n">
-        <v>177745</v>
+        <v>179245</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12430,10 +12430,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>9025</v>
+        <v>9031</v>
       </c>
       <c r="D252" t="n">
-        <v>11534102</v>
+        <v>11541552</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -12718,10 +12718,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="D258" t="n">
-        <v>2896380</v>
+        <v>2901552</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>5156</v>
+        <v>5157</v>
       </c>
       <c r="D261" t="n">
-        <v>6414896</v>
+        <v>6415584</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1888</v>
+        <v>1894</v>
       </c>
       <c r="D264" t="n">
-        <v>2773513</v>
+        <v>2782513</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>17301</v>
+        <v>17327</v>
       </c>
       <c r="D270" t="n">
-        <v>21921392</v>
+        <v>21953281</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13486,10 +13486,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>7444</v>
+        <v>7446</v>
       </c>
       <c r="D274" t="n">
-        <v>10917072</v>
+        <v>10920072</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13582,10 +13582,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>2307</v>
+        <v>2309</v>
       </c>
       <c r="D276" t="n">
-        <v>3313095</v>
+        <v>3316095</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>15136</v>
+        <v>15174</v>
       </c>
       <c r="D281" t="n">
-        <v>18780766</v>
+        <v>18828373</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>6761</v>
+        <v>6767</v>
       </c>
       <c r="D285" t="n">
-        <v>9921642</v>
+        <v>9930080</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3090</v>
+        <v>3093</v>
       </c>
       <c r="D286" t="n">
-        <v>4478485</v>
+        <v>4482985</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>8579</v>
+        <v>8588</v>
       </c>
       <c r="D290" t="n">
-        <v>10792328</v>
+        <v>10805213</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D292" t="n">
-        <v>76870</v>
+        <v>77000</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>3669</v>
+        <v>3673</v>
       </c>
       <c r="D294" t="n">
-        <v>5373783</v>
+        <v>5379783</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="D295" t="n">
-        <v>1661918</v>
+        <v>1664340</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D296" t="n">
-        <v>294839</v>
+        <v>295379</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>8193</v>
+        <v>8197</v>
       </c>
       <c r="D299" t="n">
-        <v>10684715</v>
+        <v>10690715</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14878,10 +14878,10 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>3282</v>
+        <v>3287</v>
       </c>
       <c r="D303" t="n">
-        <v>4794742</v>
+        <v>4802168</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>2057</v>
+        <v>2060</v>
       </c>
       <c r="D304" t="n">
-        <v>2992197</v>
+        <v>2996697</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>9991</v>
+        <v>10001</v>
       </c>
       <c r="D307" t="n">
-        <v>13102594</v>
+        <v>13115602</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3357</v>
+        <v>3360</v>
       </c>
       <c r="D311" t="n">
-        <v>4919219</v>
+        <v>4922353</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>6381</v>
+        <v>6386</v>
       </c>
       <c r="D316" t="n">
-        <v>7928797</v>
+        <v>7935761</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>2171</v>
+        <v>2172</v>
       </c>
       <c r="D320" t="n">
-        <v>3185429</v>
+        <v>3186929</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D322" t="n">
-        <v>1043022</v>
+        <v>1044522</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15934,10 +15934,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>6937</v>
+        <v>6941</v>
       </c>
       <c r="D325" t="n">
-        <v>8713050</v>
+        <v>8716594</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>2931</v>
+        <v>2932</v>
       </c>
       <c r="D329" t="n">
-        <v>4285725</v>
+        <v>4287225</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16318,10 +16318,10 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>29007</v>
+        <v>29053</v>
       </c>
       <c r="D333" t="n">
-        <v>36569136</v>
+        <v>36627594</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -16606,10 +16606,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>15471</v>
+        <v>15484</v>
       </c>
       <c r="D339" t="n">
-        <v>22647085</v>
+        <v>22666285</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>7419</v>
+        <v>7426</v>
       </c>
       <c r="D342" t="n">
-        <v>10696579</v>
+        <v>10706114</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16894,10 +16894,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>3598</v>
+        <v>3601</v>
       </c>
       <c r="D345" t="n">
-        <v>4501837</v>
+        <v>4505643</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>17803</v>
+        <v>17829</v>
       </c>
       <c r="D353" t="n">
-        <v>22214864</v>
+        <v>22241673</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17470,10 +17470,10 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>9244</v>
+        <v>9252</v>
       </c>
       <c r="D357" t="n">
-        <v>13580919</v>
+        <v>13591389</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>4396</v>
+        <v>4406</v>
       </c>
       <c r="D359" t="n">
-        <v>6366635</v>
+        <v>6380532</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>12755</v>
+        <v>12774</v>
       </c>
       <c r="D362" t="n">
-        <v>15961939</v>
+        <v>15989606</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>6082</v>
+        <v>6091</v>
       </c>
       <c r="D366" t="n">
-        <v>8907782</v>
+        <v>8919735</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D369" t="n">
-        <v>935577</v>
+        <v>939464</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>16530</v>
+        <v>16545</v>
       </c>
       <c r="D371" t="n">
-        <v>20666439</v>
+        <v>20676249</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>6790</v>
+        <v>6798</v>
       </c>
       <c r="D374" t="n">
-        <v>9991793</v>
+        <v>10000927</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>2627</v>
+        <v>2630</v>
       </c>
       <c r="D376" t="n">
-        <v>3820641</v>
+        <v>3825141</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D378" t="n">
-        <v>196996</v>
+        <v>198496</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>3830</v>
+        <v>3832</v>
       </c>
       <c r="D380" t="n">
-        <v>4810388</v>
+        <v>4810653</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D383" t="n">
-        <v>1912112</v>
+        <v>1913612</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D386" t="n">
-        <v>93216</v>
+        <v>96216</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>20628</v>
+        <v>20659</v>
       </c>
       <c r="D387" t="n">
-        <v>25670874</v>
+        <v>25710184</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>8902</v>
+        <v>8913</v>
       </c>
       <c r="D390" t="n">
-        <v>13112139</v>
+        <v>13127774</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>5847</v>
+        <v>5850</v>
       </c>
       <c r="D392" t="n">
-        <v>8499954</v>
+        <v>8504454</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D393" t="n">
-        <v>214561</v>
+        <v>219061</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>10314</v>
+        <v>10321</v>
       </c>
       <c r="D395" t="n">
-        <v>12746417</v>
+        <v>12750961</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>5033</v>
+        <v>5039</v>
       </c>
       <c r="D400" t="n">
-        <v>7362410</v>
+        <v>7371410</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>1708</v>
+        <v>1710</v>
       </c>
       <c r="D402" t="n">
-        <v>2483835</v>
+        <v>2486835</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>26085</v>
+        <v>26229</v>
       </c>
       <c r="D405" t="n">
-        <v>35376245</v>
+        <v>35566253</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>6682</v>
+        <v>6698</v>
       </c>
       <c r="D409" t="n">
-        <v>9847374</v>
+        <v>9870874</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>5885</v>
+        <v>5897</v>
       </c>
       <c r="D411" t="n">
-        <v>8523417</v>
+        <v>8541412</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D413" t="n">
-        <v>590549</v>
+        <v>592049</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>6232</v>
+        <v>6289</v>
       </c>
       <c r="D415" t="n">
-        <v>8623575</v>
+        <v>8706226</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>1551</v>
+        <v>1574</v>
       </c>
       <c r="D417" t="n">
-        <v>2282407</v>
+        <v>2316907</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>2095</v>
+        <v>2112</v>
       </c>
       <c r="D419" t="n">
-        <v>3051637</v>
+        <v>3075017</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20542,10 +20542,10 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D421" t="n">
-        <v>109370</v>
+        <v>113870</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>10263</v>
+        <v>10270</v>
       </c>
       <c r="D423" t="n">
-        <v>12683137</v>
+        <v>12690399</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>3591</v>
+        <v>3597</v>
       </c>
       <c r="D426" t="n">
-        <v>5273447</v>
+        <v>5282424</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="D428" t="n">
-        <v>2491087</v>
+        <v>2491691</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -21022,10 +21022,10 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>57371</v>
+        <v>57451</v>
       </c>
       <c r="D431" t="n">
-        <v>71150441</v>
+        <v>71243637</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>23524</v>
+        <v>23541</v>
       </c>
       <c r="D435" t="n">
-        <v>34506678</v>
+        <v>34531898</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>11867</v>
+        <v>11876</v>
       </c>
       <c r="D437" t="n">
-        <v>17207847</v>
+        <v>17220527</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="D441" t="n">
-        <v>1233126</v>
+        <v>1239659</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>17369</v>
+        <v>17382</v>
       </c>
       <c r="D443" t="n">
-        <v>21949263</v>
+        <v>21965751</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21790,10 +21790,10 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>7229</v>
+        <v>7238</v>
       </c>
       <c r="D447" t="n">
-        <v>10625604</v>
+        <v>10638953</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>30156</v>
+        <v>30191</v>
       </c>
       <c r="D452" t="n">
-        <v>36945049</v>
+        <v>36984649</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22222,10 +22222,10 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>10903</v>
+        <v>10910</v>
       </c>
       <c r="D456" t="n">
-        <v>15966017</v>
+        <v>15976055</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>4625</v>
+        <v>4626</v>
       </c>
       <c r="D458" t="n">
-        <v>6711543</v>
+        <v>6713043</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D460" t="n">
-        <v>485995</v>
+        <v>487495</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22462,10 +22462,10 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>13272</v>
+        <v>13289</v>
       </c>
       <c r="D461" t="n">
-        <v>16277733</v>
+        <v>16301396</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>4171</v>
+        <v>4172</v>
       </c>
       <c r="D466" t="n">
-        <v>6132840</v>
+        <v>6134340</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="D468" t="n">
-        <v>2791188</v>
+        <v>2792688</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22942,10 +22942,10 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>30887</v>
+        <v>30990</v>
       </c>
       <c r="D471" t="n">
-        <v>40114238</v>
+        <v>40251769</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -23134,10 +23134,10 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>12527</v>
+        <v>12538</v>
       </c>
       <c r="D475" t="n">
-        <v>18445095</v>
+        <v>18461595</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>10722</v>
+        <v>10732</v>
       </c>
       <c r="D477" t="n">
-        <v>15635716</v>
+        <v>15648746</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D479" t="n">
-        <v>334740</v>
+        <v>337740</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23374,10 +23374,10 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>51265</v>
+        <v>51480</v>
       </c>
       <c r="D480" t="n">
-        <v>67572847</v>
+        <v>67865329</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>20871</v>
+        <v>20900</v>
       </c>
       <c r="D485" t="n">
-        <v>30667771</v>
+        <v>30709306</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>19631</v>
+        <v>19660</v>
       </c>
       <c r="D487" t="n">
-        <v>28503297</v>
+        <v>28546506</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D489" t="n">
-        <v>326608</v>
+        <v>327608</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -23902,10 +23902,10 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>127003</v>
+        <v>127357</v>
       </c>
       <c r="D491" t="n">
-        <v>166988132</v>
+        <v>167458598</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -24190,10 +24190,10 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D497" t="n">
-        <v>23273</v>
+        <v>24773</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -24238,10 +24238,10 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>72881</v>
+        <v>72982</v>
       </c>
       <c r="D498" t="n">
-        <v>107157106</v>
+        <v>107296365</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>52530</v>
+        <v>52622</v>
       </c>
       <c r="D501" t="n">
-        <v>76275393</v>
+        <v>76409428</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24478,10 +24478,10 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D503" t="n">
-        <v>1233162</v>
+        <v>1236162</v>
       </c>
       <c r="E503" t="inlineStr">
         <is>
@@ -24574,10 +24574,10 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>2256</v>
+        <v>2261</v>
       </c>
       <c r="D505" t="n">
-        <v>3182062</v>
+        <v>3188362</v>
       </c>
       <c r="E505" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>35854</v>
+        <v>35921</v>
       </c>
       <c r="D507" t="n">
-        <v>46459386</v>
+        <v>46544569</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24910,10 +24910,10 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>14164</v>
+        <v>14184</v>
       </c>
       <c r="D512" t="n">
-        <v>20833537</v>
+        <v>20856602</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>11638</v>
+        <v>11654</v>
       </c>
       <c r="D514" t="n">
-        <v>16870554</v>
+        <v>16890990</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D516" t="n">
-        <v>403066</v>
+        <v>404566</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25198,10 +25198,10 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>52640</v>
+        <v>52942</v>
       </c>
       <c r="D518" t="n">
-        <v>70295284</v>
+        <v>70709946</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>21141</v>
+        <v>21183</v>
       </c>
       <c r="D522" t="n">
-        <v>31215767</v>
+        <v>31278507</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>20868</v>
+        <v>20897</v>
       </c>
       <c r="D524" t="n">
-        <v>30541865</v>
+        <v>30582911</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25582,10 +25582,10 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D526" t="n">
-        <v>322233</v>
+        <v>325233</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="D527" t="n">
-        <v>967242</v>
+        <v>980742</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>45160</v>
+        <v>45375</v>
       </c>
       <c r="D528" t="n">
-        <v>59599637</v>
+        <v>59893010</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>16212</v>
+        <v>16239</v>
       </c>
       <c r="D531" t="n">
-        <v>23839114</v>
+        <v>23878932</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>16027</v>
+        <v>16052</v>
       </c>
       <c r="D533" t="n">
-        <v>23290741</v>
+        <v>23328223</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -25966,10 +25966,10 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D534" t="n">
-        <v>284167</v>
+        <v>285087</v>
       </c>
       <c r="E534" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>34569</v>
+        <v>34673</v>
       </c>
       <c r="D536" t="n">
-        <v>45627700</v>
+        <v>45775879</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26254,10 +26254,10 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>13055</v>
+        <v>13069</v>
       </c>
       <c r="D540" t="n">
-        <v>19259453</v>
+        <v>19279903</v>
       </c>
       <c r="E540" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>12629</v>
+        <v>12666</v>
       </c>
       <c r="D542" t="n">
-        <v>18349259</v>
+        <v>18399033</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>35833</v>
+        <v>35926</v>
       </c>
       <c r="D545" t="n">
-        <v>46382502</v>
+        <v>46509403</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26686,10 +26686,10 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>14960</v>
+        <v>14984</v>
       </c>
       <c r="D549" t="n">
-        <v>21967419</v>
+        <v>22001052</v>
       </c>
       <c r="E549" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>11637</v>
+        <v>11659</v>
       </c>
       <c r="D551" t="n">
-        <v>16841253</v>
+        <v>16869986</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>38703</v>
+        <v>38734</v>
       </c>
       <c r="D555" t="n">
-        <v>51829668</v>
+        <v>51871227</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>12806</v>
+        <v>12817</v>
       </c>
       <c r="D561" t="n">
-        <v>18814557</v>
+        <v>18829297</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>3338</v>
+        <v>3339</v>
       </c>
       <c r="D562" t="n">
-        <v>4819946</v>
+        <v>4821446</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D567" t="n">
-        <v>454159</v>
+        <v>457159</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27598,10 +27598,10 @@
         </is>
       </c>
       <c r="C568" t="n">
-        <v>14885</v>
+        <v>14912</v>
       </c>
       <c r="D568" t="n">
-        <v>19740753</v>
+        <v>19779305</v>
       </c>
       <c r="E568" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>6291</v>
+        <v>6304</v>
       </c>
       <c r="D572" t="n">
-        <v>9166528</v>
+        <v>9185514</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27886,10 +27886,10 @@
         </is>
       </c>
       <c r="C574" t="n">
-        <v>4203</v>
+        <v>4208</v>
       </c>
       <c r="D574" t="n">
-        <v>6062961</v>
+        <v>6070161</v>
       </c>
       <c r="E574" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D577" t="n">
-        <v>288001</v>
+        <v>292501</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>10815</v>
+        <v>10918</v>
       </c>
       <c r="D579" t="n">
-        <v>15628754</v>
+        <v>15780204</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>1385</v>
+        <v>1392</v>
       </c>
       <c r="D580" t="n">
-        <v>2059078</v>
+        <v>2069578</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>20183</v>
+        <v>20213</v>
       </c>
       <c r="D584" t="n">
-        <v>25404957</v>
+        <v>25439422</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>8471</v>
+        <v>8473</v>
       </c>
       <c r="D589" t="n">
-        <v>12420189</v>
+        <v>12422379</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>3087</v>
+        <v>3092</v>
       </c>
       <c r="D591" t="n">
-        <v>4433868</v>
+        <v>4441368</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D592" t="n">
-        <v>442238</v>
+        <v>445108</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D593" t="n">
-        <v>536084</v>
+        <v>540584</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>13461</v>
+        <v>13484</v>
       </c>
       <c r="D595" t="n">
-        <v>16907905</v>
+        <v>16938376</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -29086,10 +29086,10 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>5498</v>
+        <v>5508</v>
       </c>
       <c r="D599" t="n">
-        <v>8075148</v>
+        <v>8089686</v>
       </c>
       <c r="E599" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>2481</v>
+        <v>2486</v>
       </c>
       <c r="D601" t="n">
-        <v>3577504</v>
+        <v>3585004</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>12772</v>
+        <v>12797</v>
       </c>
       <c r="D604" t="n">
-        <v>16206889</v>
+        <v>16236183</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>4908</v>
+        <v>4912</v>
       </c>
       <c r="D608" t="n">
-        <v>7198907</v>
+        <v>7204907</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>6962</v>
+        <v>6970</v>
       </c>
       <c r="D613" t="n">
-        <v>8983331</v>
+        <v>8994339</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29998,10 +29998,10 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>2422</v>
+        <v>2424</v>
       </c>
       <c r="D618" t="n">
-        <v>3553727</v>
+        <v>3556727</v>
       </c>
       <c r="E618" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>26473</v>
+        <v>26507</v>
       </c>
       <c r="D622" t="n">
-        <v>32698169</v>
+        <v>32743082</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>10445</v>
+        <v>10453</v>
       </c>
       <c r="D626" t="n">
-        <v>15330269</v>
+        <v>15341796</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>4443</v>
+        <v>4453</v>
       </c>
       <c r="D628" t="n">
-        <v>6449497</v>
+        <v>6464497</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30622,10 +30622,10 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D631" t="n">
-        <v>670903</v>
+        <v>673903</v>
       </c>
       <c r="E631" t="inlineStr">
         <is>
@@ -30670,10 +30670,10 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>10504</v>
+        <v>10514</v>
       </c>
       <c r="D632" t="n">
-        <v>12793120</v>
+        <v>12802181</v>
       </c>
       <c r="E632" t="inlineStr">
         <is>
@@ -30910,10 +30910,10 @@
         </is>
       </c>
       <c r="C637" t="n">
-        <v>3469</v>
+        <v>3472</v>
       </c>
       <c r="D637" t="n">
-        <v>5081079</v>
+        <v>5085579</v>
       </c>
       <c r="E637" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="D638" t="n">
-        <v>1493322</v>
+        <v>1499322</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31150,10 +31150,10 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>26204</v>
+        <v>26226</v>
       </c>
       <c r="D642" t="n">
-        <v>32707553</v>
+        <v>32727979</v>
       </c>
       <c r="E642" t="inlineStr">
         <is>
@@ -31342,10 +31342,10 @@
         </is>
       </c>
       <c r="C646" t="n">
-        <v>10212</v>
+        <v>10219</v>
       </c>
       <c r="D646" t="n">
-        <v>15015796</v>
+        <v>15022557</v>
       </c>
       <c r="E646" t="inlineStr">
         <is>
@@ -31438,10 +31438,10 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>2873</v>
+        <v>2875</v>
       </c>
       <c r="D648" t="n">
-        <v>4143149</v>
+        <v>4146149</v>
       </c>
       <c r="E648" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>6970</v>
+        <v>6976</v>
       </c>
       <c r="D652" t="n">
-        <v>8852581</v>
+        <v>8860290</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>2519</v>
+        <v>2521</v>
       </c>
       <c r="D654" t="n">
-        <v>3697603</v>
+        <v>3700603</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31870,10 +31870,10 @@
         </is>
       </c>
       <c r="C657" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D657" t="n">
-        <v>314684</v>
+        <v>316184</v>
       </c>
       <c r="E657" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D659" t="n">
-        <v>196471</v>
+        <v>196973</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>3477</v>
+        <v>3482</v>
       </c>
       <c r="D660" t="n">
-        <v>4234367</v>
+        <v>4240277</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D664" t="n">
-        <v>1071135</v>
+        <v>1072656</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>8576</v>
+        <v>8591</v>
       </c>
       <c r="D669" t="n">
-        <v>10738002</v>
+        <v>10757540</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32686,10 +32686,10 @@
         </is>
       </c>
       <c r="C674" t="n">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="D674" t="n">
-        <v>1010547</v>
+        <v>1012848</v>
       </c>
       <c r="E674" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>17651</v>
+        <v>17668</v>
       </c>
       <c r="D678" t="n">
-        <v>21648657</v>
+        <v>21669072</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>5318</v>
+        <v>5323</v>
       </c>
       <c r="D682" t="n">
-        <v>7770714</v>
+        <v>7778214</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>67024</v>
+        <v>67104</v>
       </c>
       <c r="D688" t="n">
-        <v>84392957</v>
+        <v>84481689</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>24866</v>
+        <v>24895</v>
       </c>
       <c r="D693" t="n">
-        <v>36532065</v>
+        <v>36572931</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>12080</v>
+        <v>12098</v>
       </c>
       <c r="D696" t="n">
-        <v>17415924</v>
+        <v>17441469</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33886,10 +33886,10 @@
         </is>
       </c>
       <c r="C699" t="n">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="D699" t="n">
-        <v>2554817</v>
+        <v>2556317</v>
       </c>
       <c r="E699" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D701" t="n">
-        <v>1403845</v>
+        <v>1405345</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>10119</v>
+        <v>10132</v>
       </c>
       <c r="D702" t="n">
-        <v>12417723</v>
+        <v>12431149</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34174,10 +34174,10 @@
         </is>
       </c>
       <c r="C705" t="n">
-        <v>3901</v>
+        <v>3908</v>
       </c>
       <c r="D705" t="n">
-        <v>5711778</v>
+        <v>5721797</v>
       </c>
       <c r="E705" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D707" t="n">
-        <v>2022517</v>
+        <v>2024017</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D709" t="n">
-        <v>289490</v>
+        <v>292912</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>16268</v>
+        <v>16280</v>
       </c>
       <c r="D710" t="n">
-        <v>20137735</v>
+        <v>20151766</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>6465</v>
+        <v>6469</v>
       </c>
       <c r="D714" t="n">
-        <v>9450193</v>
+        <v>9456193</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34942,10 +34942,10 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>10522</v>
+        <v>10542</v>
       </c>
       <c r="D721" t="n">
-        <v>12997222</v>
+        <v>13023011</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
@@ -35134,10 +35134,10 @@
         </is>
       </c>
       <c r="C725" t="n">
-        <v>3999</v>
+        <v>4002</v>
       </c>
       <c r="D725" t="n">
-        <v>5865170</v>
+        <v>5869218</v>
       </c>
       <c r="E725" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>1477</v>
+        <v>1479</v>
       </c>
       <c r="D727" t="n">
-        <v>2139476</v>
+        <v>2142026</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35374,10 +35374,10 @@
         </is>
       </c>
       <c r="C730" t="n">
-        <v>27142</v>
+        <v>27186</v>
       </c>
       <c r="D730" t="n">
-        <v>33858935</v>
+        <v>33909850</v>
       </c>
       <c r="E730" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>11887</v>
+        <v>11901</v>
       </c>
       <c r="D735" t="n">
-        <v>17396448</v>
+        <v>17416464</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35710,10 +35710,10 @@
         </is>
       </c>
       <c r="C737" t="n">
-        <v>3845</v>
+        <v>3848</v>
       </c>
       <c r="D737" t="n">
-        <v>5501896</v>
+        <v>5506396</v>
       </c>
       <c r="E737" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="D739" t="n">
-        <v>953439</v>
+        <v>967798</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -35950,10 +35950,10 @@
         </is>
       </c>
       <c r="C742" t="n">
-        <v>11042</v>
+        <v>11070</v>
       </c>
       <c r="D742" t="n">
-        <v>13694359</v>
+        <v>13729666</v>
       </c>
       <c r="E742" t="inlineStr">
         <is>
@@ -36094,10 +36094,10 @@
         </is>
       </c>
       <c r="C745" t="n">
-        <v>4364</v>
+        <v>4369</v>
       </c>
       <c r="D745" t="n">
-        <v>6383424</v>
+        <v>6390242</v>
       </c>
       <c r="E745" t="inlineStr">
         <is>
@@ -36142,10 +36142,10 @@
         </is>
       </c>
       <c r="C746" t="n">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="D746" t="n">
-        <v>1492095</v>
+        <v>1493595</v>
       </c>
       <c r="E746" t="inlineStr">
         <is>
@@ -36190,10 +36190,10 @@
         </is>
       </c>
       <c r="C747" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D747" t="n">
-        <v>221660</v>
+        <v>223160</v>
       </c>
       <c r="E747" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D748" t="n">
-        <v>432079</v>
+        <v>432455</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36286,10 +36286,10 @@
         </is>
       </c>
       <c r="C749" t="n">
-        <v>6070</v>
+        <v>6077</v>
       </c>
       <c r="D749" t="n">
-        <v>7153713</v>
+        <v>7159022</v>
       </c>
       <c r="E749" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>15256</v>
+        <v>15266</v>
       </c>
       <c r="D755" t="n">
-        <v>18549367</v>
+        <v>18561147</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>5121</v>
+        <v>5122</v>
       </c>
       <c r="D760" t="n">
-        <v>7505876</v>
+        <v>7506676</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -37102,10 +37102,10 @@
         </is>
       </c>
       <c r="C766" t="n">
-        <v>10467</v>
+        <v>10477</v>
       </c>
       <c r="D766" t="n">
-        <v>13333935</v>
+        <v>13343904</v>
       </c>
       <c r="E766" t="inlineStr">
         <is>
@@ -37246,10 +37246,10 @@
         </is>
       </c>
       <c r="C769" t="n">
-        <v>3725</v>
+        <v>3726</v>
       </c>
       <c r="D769" t="n">
-        <v>5451428</v>
+        <v>5451923</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
@@ -37342,10 +37342,10 @@
         </is>
       </c>
       <c r="C771" t="n">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="D771" t="n">
-        <v>1655721</v>
+        <v>1657221</v>
       </c>
       <c r="E771" t="inlineStr">
         <is>
@@ -37486,10 +37486,10 @@
         </is>
       </c>
       <c r="C774" t="n">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D774" t="n">
-        <v>257442</v>
+        <v>263442</v>
       </c>
       <c r="E774" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>29384</v>
+        <v>29406</v>
       </c>
       <c r="D775" t="n">
-        <v>36289367</v>
+        <v>36315111</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37630,10 +37630,10 @@
         </is>
       </c>
       <c r="C777" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D777" t="n">
-        <v>50350</v>
+        <v>51850</v>
       </c>
       <c r="E777" t="inlineStr">
         <is>
@@ -37726,10 +37726,10 @@
         </is>
       </c>
       <c r="C779" t="n">
-        <v>12301</v>
+        <v>12315</v>
       </c>
       <c r="D779" t="n">
-        <v>18012198</v>
+        <v>18032232</v>
       </c>
       <c r="E779" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>5625</v>
+        <v>5629</v>
       </c>
       <c r="D781" t="n">
-        <v>8129726</v>
+        <v>8135726</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D782" t="n">
-        <v>661672</v>
+        <v>663172</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38014,10 +38014,10 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>6980</v>
+        <v>6985</v>
       </c>
       <c r="D785" t="n">
-        <v>8660867</v>
+        <v>8665276</v>
       </c>
       <c r="E785" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>2496</v>
+        <v>2497</v>
       </c>
       <c r="D791" t="n">
-        <v>3646519</v>
+        <v>3648019</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38350,10 +38350,10 @@
         </is>
       </c>
       <c r="C792" t="n">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="D792" t="n">
-        <v>1488184</v>
+        <v>1493056</v>
       </c>
       <c r="E792" t="inlineStr">
         <is>
@@ -38398,10 +38398,10 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D793" t="n">
-        <v>466708</v>
+        <v>468565</v>
       </c>
       <c r="E793" t="inlineStr">
         <is>
@@ -38494,10 +38494,10 @@
         </is>
       </c>
       <c r="C795" t="n">
-        <v>52073</v>
+        <v>52191</v>
       </c>
       <c r="D795" t="n">
-        <v>65002993</v>
+        <v>65155852</v>
       </c>
       <c r="E795" t="inlineStr">
         <is>
@@ -38734,10 +38734,10 @@
         </is>
       </c>
       <c r="C800" t="n">
-        <v>19754</v>
+        <v>19767</v>
       </c>
       <c r="D800" t="n">
-        <v>28922140</v>
+        <v>28941640</v>
       </c>
       <c r="E800" t="inlineStr">
         <is>
@@ -38878,10 +38878,10 @@
         </is>
       </c>
       <c r="C803" t="n">
-        <v>11507</v>
+        <v>11520</v>
       </c>
       <c r="D803" t="n">
-        <v>16610805</v>
+        <v>16629480</v>
       </c>
       <c r="E803" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>1087</v>
+        <v>1094</v>
       </c>
       <c r="D808" t="n">
-        <v>1513879</v>
+        <v>1523879</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39166,10 +39166,10 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>10051</v>
+        <v>10059</v>
       </c>
       <c r="D809" t="n">
-        <v>12558050</v>
+        <v>12568263</v>
       </c>
       <c r="E809" t="inlineStr">
         <is>
@@ -39358,10 +39358,10 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>3498</v>
+        <v>3503</v>
       </c>
       <c r="D813" t="n">
-        <v>5088299</v>
+        <v>5095799</v>
       </c>
       <c r="E813" t="inlineStr">
         <is>
@@ -39550,10 +39550,10 @@
         </is>
       </c>
       <c r="C817" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D817" t="n">
-        <v>168123</v>
+        <v>171123</v>
       </c>
       <c r="E817" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D819" t="n">
-        <v>299306</v>
+        <v>300806</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39694,10 +39694,10 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>52849</v>
+        <v>52892</v>
       </c>
       <c r="D820" t="n">
-        <v>65539475</v>
+        <v>65588854</v>
       </c>
       <c r="E820" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D825" t="n">
-        <v>120158</v>
+        <v>121658</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -39982,10 +39982,10 @@
         </is>
       </c>
       <c r="C826" t="n">
-        <v>20853</v>
+        <v>20867</v>
       </c>
       <c r="D826" t="n">
-        <v>30602997</v>
+        <v>30621184</v>
       </c>
       <c r="E826" t="inlineStr">
         <is>
@@ -40078,10 +40078,10 @@
         </is>
       </c>
       <c r="C828" t="n">
-        <v>13109</v>
+        <v>13116</v>
       </c>
       <c r="D828" t="n">
-        <v>18997569</v>
+        <v>19006293</v>
       </c>
       <c r="E828" t="inlineStr">
         <is>
@@ -40174,10 +40174,10 @@
         </is>
       </c>
       <c r="C830" t="n">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D830" t="n">
-        <v>1179289</v>
+        <v>1182289</v>
       </c>
       <c r="E830" t="inlineStr">
         <is>
@@ -40222,10 +40222,10 @@
         </is>
       </c>
       <c r="C831" t="n">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="D831" t="n">
-        <v>1394421</v>
+        <v>1397609</v>
       </c>
       <c r="E831" t="inlineStr">
         <is>
@@ -40318,10 +40318,10 @@
         </is>
       </c>
       <c r="C833" t="n">
-        <v>7074</v>
+        <v>7082</v>
       </c>
       <c r="D833" t="n">
-        <v>8719363</v>
+        <v>8727463</v>
       </c>
       <c r="E833" t="inlineStr">
         <is>
@@ -40414,10 +40414,10 @@
         </is>
       </c>
       <c r="C835" t="n">
-        <v>2387</v>
+        <v>2390</v>
       </c>
       <c r="D835" t="n">
-        <v>3481270</v>
+        <v>3484539</v>
       </c>
       <c r="E835" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>995</v>
+        <v>998</v>
       </c>
       <c r="D836" t="n">
-        <v>1441217</v>
+        <v>1445717</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D837" t="n">
-        <v>408097</v>
+        <v>412597</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40606,10 +40606,10 @@
         </is>
       </c>
       <c r="C839" t="n">
-        <v>2963</v>
+        <v>2984</v>
       </c>
       <c r="D839" t="n">
-        <v>3806033</v>
+        <v>3831864</v>
       </c>
       <c r="E839" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="D842" t="n">
-        <v>1604170</v>
+        <v>1607170</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D844" t="n">
-        <v>498190</v>
+        <v>498440</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -40942,10 +40942,10 @@
         </is>
       </c>
       <c r="C846" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D846" t="n">
-        <v>122584</v>
+        <v>124084</v>
       </c>
       <c r="E846" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>20422</v>
+        <v>20432</v>
       </c>
       <c r="D847" t="n">
-        <v>25628995</v>
+        <v>25642400</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41182,10 +41182,10 @@
         </is>
       </c>
       <c r="C851" t="n">
-        <v>7218</v>
+        <v>7221</v>
       </c>
       <c r="D851" t="n">
-        <v>10538196</v>
+        <v>10542696</v>
       </c>
       <c r="E851" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>4284</v>
+        <v>4286</v>
       </c>
       <c r="D853" t="n">
-        <v>6197230</v>
+        <v>6200230</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41422,10 +41422,10 @@
         </is>
       </c>
       <c r="C856" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D856" t="n">
-        <v>500202</v>
+        <v>501702</v>
       </c>
       <c r="E856" t="inlineStr">
         <is>
@@ -41518,10 +41518,10 @@
         </is>
       </c>
       <c r="C858" t="n">
-        <v>13350</v>
+        <v>13362</v>
       </c>
       <c r="D858" t="n">
-        <v>16161401</v>
+        <v>16172279</v>
       </c>
       <c r="E858" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D867" t="n">
-        <v>329166</v>
+        <v>333666</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -41998,10 +41998,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>8924</v>
+        <v>8932</v>
       </c>
       <c r="D868" t="n">
-        <v>10962394</v>
+        <v>10970304</v>
       </c>
       <c r="E868" t="inlineStr">
         <is>
@@ -42142,10 +42142,10 @@
         </is>
       </c>
       <c r="C871" t="n">
-        <v>3193</v>
+        <v>3195</v>
       </c>
       <c r="D871" t="n">
-        <v>4683284</v>
+        <v>4685484</v>
       </c>
       <c r="E871" t="inlineStr">
         <is>
@@ -42190,10 +42190,10 @@
         </is>
       </c>
       <c r="C872" t="n">
-        <v>1384</v>
+        <v>1388</v>
       </c>
       <c r="D872" t="n">
-        <v>1987967</v>
+        <v>1993967</v>
       </c>
       <c r="E872" t="inlineStr">
         <is>
@@ -42238,10 +42238,10 @@
         </is>
       </c>
       <c r="C873" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D873" t="n">
-        <v>161896</v>
+        <v>163396</v>
       </c>
       <c r="E873" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D874" t="n">
-        <v>239159</v>
+        <v>240659</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42334,10 +42334,10 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>40547</v>
+        <v>40582</v>
       </c>
       <c r="D875" t="n">
-        <v>51095643</v>
+        <v>51142115</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>19831</v>
+        <v>19844</v>
       </c>
       <c r="D880" t="n">
-        <v>29093548</v>
+        <v>29111619</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42670,10 +42670,10 @@
         </is>
       </c>
       <c r="C882" t="n">
-        <v>5357</v>
+        <v>5365</v>
       </c>
       <c r="D882" t="n">
-        <v>7714012</v>
+        <v>7725308</v>
       </c>
       <c r="E882" t="inlineStr">
         <is>
@@ -42814,10 +42814,10 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>799</v>
+        <v>805</v>
       </c>
       <c r="D885" t="n">
-        <v>1122312</v>
+        <v>1127381</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
@@ -42862,10 +42862,10 @@
         </is>
       </c>
       <c r="C886" t="n">
-        <v>19502</v>
+        <v>19529</v>
       </c>
       <c r="D886" t="n">
-        <v>24345932</v>
+        <v>24374415</v>
       </c>
       <c r="E886" t="inlineStr">
         <is>
@@ -43006,10 +43006,10 @@
         </is>
       </c>
       <c r="C889" t="n">
-        <v>9255</v>
+        <v>9261</v>
       </c>
       <c r="D889" t="n">
-        <v>13562704</v>
+        <v>13571704</v>
       </c>
       <c r="E889" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="D891" t="n">
-        <v>3014711</v>
+        <v>3016211</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43246,10 +43246,10 @@
         </is>
       </c>
       <c r="C894" t="n">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D894" t="n">
-        <v>777135</v>
+        <v>780135</v>
       </c>
       <c r="E894" t="inlineStr">
         <is>
@@ -43294,10 +43294,10 @@
         </is>
       </c>
       <c r="C895" t="n">
-        <v>6451</v>
+        <v>6453</v>
       </c>
       <c r="D895" t="n">
-        <v>8168609</v>
+        <v>8170559</v>
       </c>
       <c r="E895" t="inlineStr">
         <is>
@@ -43534,10 +43534,10 @@
         </is>
       </c>
       <c r="C900" t="n">
-        <v>2850</v>
+        <v>2851</v>
       </c>
       <c r="D900" t="n">
-        <v>4198353</v>
+        <v>4199853</v>
       </c>
       <c r="E900" t="inlineStr">
         <is>
@@ -43726,10 +43726,10 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>11960</v>
+        <v>11967</v>
       </c>
       <c r="D904" t="n">
-        <v>14939502</v>
+        <v>14949860</v>
       </c>
       <c r="E904" t="inlineStr">
         <is>
@@ -43918,10 +43918,10 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>4938</v>
+        <v>4940</v>
       </c>
       <c r="D908" t="n">
-        <v>7222608</v>
+        <v>7225608</v>
       </c>
       <c r="E908" t="inlineStr">
         <is>
@@ -44110,10 +44110,10 @@
         </is>
       </c>
       <c r="C912" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D912" t="n">
-        <v>190273</v>
+        <v>191773</v>
       </c>
       <c r="E912" t="inlineStr">
         <is>
@@ -44254,10 +44254,10 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>17932</v>
+        <v>17947</v>
       </c>
       <c r="D915" t="n">
-        <v>22527603</v>
+        <v>22543470</v>
       </c>
       <c r="E915" t="inlineStr">
         <is>
@@ -44446,10 +44446,10 @@
         </is>
       </c>
       <c r="C919" t="n">
-        <v>9548</v>
+        <v>9556</v>
       </c>
       <c r="D919" t="n">
-        <v>13967478</v>
+        <v>13978866</v>
       </c>
       <c r="E919" t="inlineStr">
         <is>
@@ -44542,10 +44542,10 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>1921</v>
+        <v>1926</v>
       </c>
       <c r="D921" t="n">
-        <v>2770513</v>
+        <v>2778013</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
@@ -44686,10 +44686,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>7894</v>
+        <v>7903</v>
       </c>
       <c r="D924" t="n">
-        <v>9894186</v>
+        <v>9906505</v>
       </c>
       <c r="E924" t="inlineStr">
         <is>
@@ -44926,10 +44926,10 @@
         </is>
       </c>
       <c r="C929" t="n">
-        <v>2974</v>
+        <v>2977</v>
       </c>
       <c r="D929" t="n">
-        <v>4341071</v>
+        <v>4345571</v>
       </c>
       <c r="E929" t="inlineStr">
         <is>
@@ -44974,10 +44974,10 @@
         </is>
       </c>
       <c r="C930" t="n">
-        <v>1380</v>
+        <v>1384</v>
       </c>
       <c r="D930" t="n">
-        <v>1992330</v>
+        <v>1998329</v>
       </c>
       <c r="E930" t="inlineStr">
         <is>
@@ -45166,10 +45166,10 @@
         </is>
       </c>
       <c r="C934" t="n">
-        <v>60138</v>
+        <v>60219</v>
       </c>
       <c r="D934" t="n">
-        <v>77238227</v>
+        <v>77332274</v>
       </c>
       <c r="E934" t="inlineStr">
         <is>
@@ -45502,10 +45502,10 @@
         </is>
       </c>
       <c r="C941" t="n">
-        <v>23489</v>
+        <v>23516</v>
       </c>
       <c r="D941" t="n">
-        <v>34455032</v>
+        <v>34494025</v>
       </c>
       <c r="E941" t="inlineStr">
         <is>
@@ -45598,10 +45598,10 @@
         </is>
       </c>
       <c r="C943" t="n">
-        <v>15758</v>
+        <v>15776</v>
       </c>
       <c r="D943" t="n">
-        <v>22866235</v>
+        <v>22893235</v>
       </c>
       <c r="E943" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D945" t="n">
-        <v>586073</v>
+        <v>590573</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="D946" t="n">
-        <v>1056548</v>
+        <v>1061048</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45790,10 +45790,10 @@
         </is>
       </c>
       <c r="C947" t="n">
-        <v>75841</v>
+        <v>75925</v>
       </c>
       <c r="D947" t="n">
-        <v>95357764</v>
+        <v>95447088</v>
       </c>
       <c r="E947" t="inlineStr">
         <is>
@@ -45886,10 +45886,10 @@
         </is>
       </c>
       <c r="C949" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D949" t="n">
-        <v>86260</v>
+        <v>87760</v>
       </c>
       <c r="E949" t="inlineStr">
         <is>
@@ -46126,10 +46126,10 @@
         </is>
       </c>
       <c r="C954" t="n">
-        <v>31719</v>
+        <v>31752</v>
       </c>
       <c r="D954" t="n">
-        <v>46554448</v>
+        <v>46602095</v>
       </c>
       <c r="E954" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>23153</v>
+        <v>23177</v>
       </c>
       <c r="D957" t="n">
-        <v>33592580</v>
+        <v>33628580</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46414,10 +46414,10 @@
         </is>
       </c>
       <c r="C960" t="n">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="D960" t="n">
-        <v>2317820</v>
+        <v>2319320</v>
       </c>
       <c r="E960" t="inlineStr">
         <is>
@@ -46462,10 +46462,10 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>9837</v>
+        <v>9841</v>
       </c>
       <c r="D961" t="n">
-        <v>12858440</v>
+        <v>12862654</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D970" t="n">
-        <v>225389</v>
+        <v>226889</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -46942,10 +46942,10 @@
         </is>
       </c>
       <c r="C971" t="n">
-        <v>51536</v>
+        <v>51579</v>
       </c>
       <c r="D971" t="n">
-        <v>64588508</v>
+        <v>64634121</v>
       </c>
       <c r="E971" t="inlineStr">
         <is>
@@ -46990,10 +46990,10 @@
         </is>
       </c>
       <c r="C972" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D972" t="n">
-        <v>39835</v>
+        <v>41335</v>
       </c>
       <c r="E972" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>17478</v>
+        <v>17484</v>
       </c>
       <c r="D976" t="n">
-        <v>25614561</v>
+        <v>25622092</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47278,10 +47278,10 @@
         </is>
       </c>
       <c r="C978" t="n">
-        <v>11744</v>
+        <v>11754</v>
       </c>
       <c r="D978" t="n">
-        <v>17000057</v>
+        <v>17014712</v>
       </c>
       <c r="E978" t="inlineStr">
         <is>
@@ -47326,10 +47326,10 @@
         </is>
       </c>
       <c r="C979" t="n">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D979" t="n">
-        <v>635130</v>
+        <v>636630</v>
       </c>
       <c r="E979" t="inlineStr">
         <is>
@@ -47422,10 +47422,10 @@
         </is>
       </c>
       <c r="C981" t="n">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D981" t="n">
-        <v>893133</v>
+        <v>895002</v>
       </c>
       <c r="E981" t="inlineStr">
         <is>
@@ -47470,10 +47470,10 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>25730</v>
+        <v>25760</v>
       </c>
       <c r="D982" t="n">
-        <v>32049373</v>
+        <v>32082997</v>
       </c>
       <c r="E982" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>9777</v>
+        <v>9791</v>
       </c>
       <c r="D987" t="n">
-        <v>14329360</v>
+        <v>14348905</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47806,10 +47806,10 @@
         </is>
       </c>
       <c r="C989" t="n">
-        <v>5736</v>
+        <v>5742</v>
       </c>
       <c r="D989" t="n">
-        <v>8324219</v>
+        <v>8333219</v>
       </c>
       <c r="E989" t="inlineStr">
         <is>
@@ -47902,10 +47902,10 @@
         </is>
       </c>
       <c r="C991" t="n">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D991" t="n">
-        <v>577173</v>
+        <v>579329</v>
       </c>
       <c r="E991" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-07 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16302</v>
+        <v>16315</v>
       </c>
       <c r="D2" t="n">
-        <v>20495474</v>
+        <v>20511856</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6228</v>
+        <v>6233</v>
       </c>
       <c r="D6" t="n">
-        <v>9109422</v>
+        <v>9116922</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D11" t="n">
-        <v>507708</v>
+        <v>513708</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10948</v>
+        <v>10958</v>
       </c>
       <c r="D12" t="n">
-        <v>13822841</v>
+        <v>13834036</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1451</v>
+        <v>1453</v>
       </c>
       <c r="D18" t="n">
-        <v>2086220</v>
+        <v>2089220</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="D19" t="n">
-        <v>536674</v>
+        <v>545821</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14189</v>
+        <v>14207</v>
       </c>
       <c r="D21" t="n">
-        <v>17414176</v>
+        <v>17429769</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1486,10 +1486,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24" t="n">
-        <v>50924</v>
+        <v>52424</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4933</v>
+        <v>4934</v>
       </c>
       <c r="D25" t="n">
-        <v>7213928</v>
+        <v>7215428</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1630,10 +1630,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="D27" t="n">
-        <v>2455899</v>
+        <v>2457399</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D28" t="n">
-        <v>356659</v>
+        <v>357672</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D30" t="n">
-        <v>466403</v>
+        <v>467903</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6516</v>
+        <v>6542</v>
       </c>
       <c r="D31" t="n">
-        <v>8653069</v>
+        <v>8689865</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="D34" t="n">
-        <v>2314120</v>
+        <v>2315620</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D39" t="n">
-        <v>179114</v>
+        <v>180614</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>21774</v>
+        <v>21797</v>
       </c>
       <c r="D40" t="n">
-        <v>26809521</v>
+        <v>26838971</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7780</v>
+        <v>7789</v>
       </c>
       <c r="D46" t="n">
-        <v>11428362</v>
+        <v>11440960</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3825</v>
+        <v>3827</v>
       </c>
       <c r="D48" t="n">
-        <v>5536155</v>
+        <v>5539155</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D51" t="n">
-        <v>819853</v>
+        <v>821066</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>8116</v>
+        <v>8121</v>
       </c>
       <c r="D52" t="n">
-        <v>10360382</v>
+        <v>10367461</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2775</v>
+        <v>2776</v>
       </c>
       <c r="D56" t="n">
-        <v>4037487</v>
+        <v>4038987</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D59" t="n">
-        <v>271001</v>
+        <v>272501</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>35999</v>
+        <v>36031</v>
       </c>
       <c r="D61" t="n">
-        <v>46352325</v>
+        <v>46389451</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>13112</v>
+        <v>13123</v>
       </c>
       <c r="D66" t="n">
-        <v>19232057</v>
+        <v>19246335</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5140</v>
+        <v>5144</v>
       </c>
       <c r="D68" t="n">
-        <v>7433967</v>
+        <v>7439967</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D72" t="n">
-        <v>478176</v>
+        <v>481176</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>46073</v>
+        <v>46108</v>
       </c>
       <c r="D74" t="n">
-        <v>58922333</v>
+        <v>58967343</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4078,10 +4078,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>18078</v>
+        <v>18087</v>
       </c>
       <c r="D78" t="n">
-        <v>26486682</v>
+        <v>26499739</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9299</v>
+        <v>9312</v>
       </c>
       <c r="D80" t="n">
-        <v>13424741</v>
+        <v>13444049</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D82" t="n">
-        <v>479973</v>
+        <v>481473</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4318,10 +4318,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D83" t="n">
-        <v>17036</v>
+        <v>18536</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D84" t="n">
-        <v>1111180</v>
+        <v>1114180</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>24818</v>
+        <v>24851</v>
       </c>
       <c r="D85" t="n">
-        <v>31292882</v>
+        <v>31335547</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8662</v>
+        <v>8668</v>
       </c>
       <c r="D89" t="n">
-        <v>12715871</v>
+        <v>12723966</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4881</v>
+        <v>4884</v>
       </c>
       <c r="D91" t="n">
-        <v>7055727</v>
+        <v>7060227</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D92" t="n">
-        <v>508622</v>
+        <v>510122</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>21875</v>
+        <v>21901</v>
       </c>
       <c r="D94" t="n">
-        <v>27463967</v>
+        <v>27494630</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -5038,10 +5038,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9138</v>
+        <v>9141</v>
       </c>
       <c r="D98" t="n">
-        <v>13376705</v>
+        <v>13381205</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -5134,10 +5134,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>3307</v>
+        <v>3310</v>
       </c>
       <c r="D100" t="n">
-        <v>4737246</v>
+        <v>4741746</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -5278,10 +5278,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D103" t="n">
-        <v>339543</v>
+        <v>340301</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5326,10 +5326,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D104" t="n">
-        <v>622219</v>
+        <v>623094</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>81228</v>
+        <v>81363</v>
       </c>
       <c r="D105" t="n">
-        <v>104114893</v>
+        <v>104286444</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5614,10 +5614,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D110" t="n">
-        <v>219780</v>
+        <v>221280</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>30527</v>
+        <v>30547</v>
       </c>
       <c r="D112" t="n">
-        <v>44796616</v>
+        <v>44826616</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20736</v>
+        <v>20762</v>
       </c>
       <c r="D114" t="n">
-        <v>29923043</v>
+        <v>29959694</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1873</v>
+        <v>1879</v>
       </c>
       <c r="D121" t="n">
-        <v>2635258</v>
+        <v>2642883</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>27610</v>
+        <v>27630</v>
       </c>
       <c r="D122" t="n">
-        <v>36437788</v>
+        <v>36466789</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D123" t="n">
-        <v>116327</v>
+        <v>117827</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>9848</v>
+        <v>9853</v>
       </c>
       <c r="D126" t="n">
-        <v>14442479</v>
+        <v>14449979</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3255</v>
+        <v>3259</v>
       </c>
       <c r="D128" t="n">
-        <v>4733256</v>
+        <v>4739256</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15677</v>
+        <v>15692</v>
       </c>
       <c r="D132" t="n">
-        <v>19517155</v>
+        <v>19532437</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6814,10 +6814,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7740</v>
+        <v>7745</v>
       </c>
       <c r="D135" t="n">
-        <v>11327564</v>
+        <v>11335064</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>13487</v>
+        <v>13497</v>
       </c>
       <c r="D142" t="n">
-        <v>16854046</v>
+        <v>16867623</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6232</v>
+        <v>6235</v>
       </c>
       <c r="D146" t="n">
-        <v>9130255</v>
+        <v>9134755</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="D148" t="n">
-        <v>2869999</v>
+        <v>2871499</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7582,10 +7582,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D151" t="n">
-        <v>501908</v>
+        <v>504908</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7630,10 +7630,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>5963</v>
+        <v>5971</v>
       </c>
       <c r="D152" t="n">
-        <v>7293358</v>
+        <v>7304762</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="D155" t="n">
-        <v>3016857</v>
+        <v>3018357</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D156" t="n">
-        <v>969827</v>
+        <v>971327</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7420</v>
+        <v>7422</v>
       </c>
       <c r="D160" t="n">
-        <v>9203611</v>
+        <v>9205411</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5597</v>
+        <v>5602</v>
       </c>
       <c r="D168" t="n">
-        <v>7046975</v>
+        <v>7053087</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8638,10 +8638,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="D173" t="n">
-        <v>2958541</v>
+        <v>2960041</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>15915</v>
+        <v>15923</v>
       </c>
       <c r="D178" t="n">
-        <v>20004035</v>
+        <v>20012096</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6377</v>
+        <v>6380</v>
       </c>
       <c r="D183" t="n">
-        <v>9314794</v>
+        <v>9319294</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>2220</v>
+        <v>2224</v>
       </c>
       <c r="D184" t="n">
-        <v>3186491</v>
+        <v>3192491</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3052</v>
+        <v>3058</v>
       </c>
       <c r="D188" t="n">
-        <v>3835567</v>
+        <v>3842191</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D190" t="n">
-        <v>2151030</v>
+        <v>2152242</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9169</v>
+        <v>9189</v>
       </c>
       <c r="D196" t="n">
-        <v>11450053</v>
+        <v>11475143</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>3419</v>
+        <v>3426</v>
       </c>
       <c r="D200" t="n">
-        <v>5023076</v>
+        <v>5033576</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>1606</v>
+        <v>1610</v>
       </c>
       <c r="D201" t="n">
-        <v>2315680</v>
+        <v>2321680</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>17203</v>
+        <v>17216</v>
       </c>
       <c r="D205" t="n">
-        <v>21491431</v>
+        <v>21508086</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>7673</v>
+        <v>7675</v>
       </c>
       <c r="D209" t="n">
-        <v>11268301</v>
+        <v>11271301</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D210" t="n">
-        <v>1773154</v>
+        <v>1774654</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D211" t="n">
-        <v>389366</v>
+        <v>394905</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>26059</v>
+        <v>26079</v>
       </c>
       <c r="D213" t="n">
-        <v>32878423</v>
+        <v>32901891</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>10477</v>
+        <v>10482</v>
       </c>
       <c r="D217" t="n">
-        <v>15301852</v>
+        <v>15309352</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="D219" t="n">
-        <v>3792522</v>
+        <v>3795522</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="D222" t="n">
-        <v>837266</v>
+        <v>843266</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>28391</v>
+        <v>28411</v>
       </c>
       <c r="D223" t="n">
-        <v>35838945</v>
+        <v>35866103</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11230,10 +11230,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D227" t="n">
-        <v>298754</v>
+        <v>300254</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>14707</v>
+        <v>14717</v>
       </c>
       <c r="D228" t="n">
-        <v>21581871</v>
+        <v>21595543</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2645</v>
+        <v>2648</v>
       </c>
       <c r="D230" t="n">
-        <v>3797175</v>
+        <v>3801675</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D233" t="n">
-        <v>1013726</v>
+        <v>1015226</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24211</v>
+        <v>24225</v>
       </c>
       <c r="D234" t="n">
-        <v>30549664</v>
+        <v>30563846</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>11160</v>
+        <v>11162</v>
       </c>
       <c r="D240" t="n">
-        <v>16360749</v>
+        <v>16363749</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2502</v>
+        <v>2503</v>
       </c>
       <c r="D242" t="n">
-        <v>3576347</v>
+        <v>3577847</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12046,10 +12046,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D244" t="n">
-        <v>583843</v>
+        <v>586843</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -12142,10 +12142,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>7853</v>
+        <v>7855</v>
       </c>
       <c r="D246" t="n">
-        <v>9827086</v>
+        <v>9828995</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>2694</v>
+        <v>2697</v>
       </c>
       <c r="D250" t="n">
-        <v>3954150</v>
+        <v>3958650</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12478,10 +12478,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D253" t="n">
-        <v>1451115</v>
+        <v>1452615</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12526,10 +12526,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D254" t="n">
-        <v>279550</v>
+        <v>281050</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>9782</v>
+        <v>9786</v>
       </c>
       <c r="D256" t="n">
-        <v>12477677</v>
+        <v>12482307</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12814,10 +12814,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>4184</v>
+        <v>4189</v>
       </c>
       <c r="D260" t="n">
-        <v>6144028</v>
+        <v>6149170</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>2163</v>
+        <v>2167</v>
       </c>
       <c r="D262" t="n">
-        <v>3131169</v>
+        <v>3137169</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>5523</v>
+        <v>5529</v>
       </c>
       <c r="D265" t="n">
-        <v>6849184</v>
+        <v>6855978</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D270" t="n">
-        <v>1028372</v>
+        <v>1029872</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13342,10 +13342,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D271" t="n">
-        <v>220078</v>
+        <v>221578</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13486,10 +13486,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>19013</v>
+        <v>19028</v>
       </c>
       <c r="D274" t="n">
-        <v>24026477</v>
+        <v>24046316</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>7911</v>
+        <v>7917</v>
       </c>
       <c r="D278" t="n">
-        <v>11599205</v>
+        <v>11608205</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>2490</v>
+        <v>2491</v>
       </c>
       <c r="D280" t="n">
-        <v>3576559</v>
+        <v>3578059</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D281" t="n">
-        <v>709598</v>
+        <v>711098</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D283" t="n">
-        <v>647923</v>
+        <v>649423</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>16543</v>
+        <v>16565</v>
       </c>
       <c r="D285" t="n">
-        <v>20497010</v>
+        <v>20523038</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>7170</v>
+        <v>7173</v>
       </c>
       <c r="D289" t="n">
-        <v>10517497</v>
+        <v>10521112</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>3321</v>
+        <v>3325</v>
       </c>
       <c r="D290" t="n">
-        <v>4813743</v>
+        <v>4819743</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D292" t="n">
-        <v>218202</v>
+        <v>219702</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D293" t="n">
-        <v>465943</v>
+        <v>467443</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>9316</v>
+        <v>9324</v>
       </c>
       <c r="D294" t="n">
-        <v>11707794</v>
+        <v>11719794</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D299" t="n">
-        <v>1810099</v>
+        <v>1811009</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>9174</v>
+        <v>9182</v>
       </c>
       <c r="D304" t="n">
-        <v>11980130</v>
+        <v>11991326</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>3727</v>
+        <v>3732</v>
       </c>
       <c r="D308" t="n">
-        <v>5448349</v>
+        <v>5455849</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2347</v>
+        <v>2349</v>
       </c>
       <c r="D309" t="n">
-        <v>3413568</v>
+        <v>3416568</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>11030</v>
+        <v>11040</v>
       </c>
       <c r="D312" t="n">
-        <v>14482623</v>
+        <v>14497623</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>3771</v>
+        <v>3773</v>
       </c>
       <c r="D316" t="n">
-        <v>5528241</v>
+        <v>5531241</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2693</v>
+        <v>2695</v>
       </c>
       <c r="D318" t="n">
-        <v>3904638</v>
+        <v>3907638</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D320" t="n">
-        <v>230286</v>
+        <v>231786</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6790</v>
+        <v>6794</v>
       </c>
       <c r="D321" t="n">
-        <v>8395064</v>
+        <v>8399105</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D322" t="n">
-        <v>11543</v>
+        <v>13043</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -16174,10 +16174,10 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D330" t="n">
-        <v>173343</v>
+        <v>184273</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>7502</v>
+        <v>7507</v>
       </c>
       <c r="D331" t="n">
-        <v>9392475</v>
+        <v>9397641</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16462,10 +16462,10 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>3125</v>
+        <v>3126</v>
       </c>
       <c r="D336" t="n">
-        <v>4565815</v>
+        <v>4567315</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>31878</v>
+        <v>31919</v>
       </c>
       <c r="D340" t="n">
-        <v>40054205</v>
+        <v>40106450</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>16503</v>
+        <v>16513</v>
       </c>
       <c r="D346" t="n">
-        <v>24132943</v>
+        <v>24147943</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>8018</v>
+        <v>8025</v>
       </c>
       <c r="D349" t="n">
-        <v>11548310</v>
+        <v>11557034</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17182,10 +17182,10 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>777</v>
+        <v>783</v>
       </c>
       <c r="D351" t="n">
-        <v>1096390</v>
+        <v>1105390</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>3880</v>
+        <v>3885</v>
       </c>
       <c r="D352" t="n">
-        <v>4836125</v>
+        <v>4841282</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D355" t="n">
-        <v>2200157</v>
+        <v>2201657</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D359" t="n">
-        <v>117095</v>
+        <v>118595</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>19323</v>
+        <v>19337</v>
       </c>
       <c r="D360" t="n">
-        <v>24095409</v>
+        <v>24112996</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>9882</v>
+        <v>9890</v>
       </c>
       <c r="D364" t="n">
-        <v>14488893</v>
+        <v>14499735</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>4728</v>
+        <v>4732</v>
       </c>
       <c r="D366" t="n">
-        <v>6838802</v>
+        <v>6844355</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="D367" t="n">
-        <v>862969</v>
+        <v>868460</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>13879</v>
+        <v>13889</v>
       </c>
       <c r="D369" t="n">
-        <v>17366820</v>
+        <v>17379286</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>6432</v>
+        <v>6434</v>
       </c>
       <c r="D373" t="n">
-        <v>9416958</v>
+        <v>9419958</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>17947</v>
+        <v>17958</v>
       </c>
       <c r="D378" t="n">
-        <v>22384209</v>
+        <v>22399090</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>7132</v>
+        <v>7135</v>
       </c>
       <c r="D382" t="n">
-        <v>10484079</v>
+        <v>10487715</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>2831</v>
+        <v>2834</v>
       </c>
       <c r="D384" t="n">
-        <v>4118692</v>
+        <v>4123192</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>4076</v>
+        <v>4085</v>
       </c>
       <c r="D388" t="n">
-        <v>5112486</v>
+        <v>5125846</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>22219</v>
+        <v>22238</v>
       </c>
       <c r="D395" t="n">
-        <v>27568492</v>
+        <v>27587902</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>9347</v>
+        <v>9353</v>
       </c>
       <c r="D398" t="n">
-        <v>13759917</v>
+        <v>13768917</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>6192</v>
+        <v>6201</v>
       </c>
       <c r="D400" t="n">
-        <v>9007456</v>
+        <v>9020736</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D401" t="n">
-        <v>237254</v>
+        <v>241754</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>11112</v>
+        <v>11122</v>
       </c>
       <c r="D403" t="n">
-        <v>13702248</v>
+        <v>13714332</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>5323</v>
+        <v>5324</v>
       </c>
       <c r="D408" t="n">
-        <v>7780203</v>
+        <v>7781703</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="D410" t="n">
-        <v>2671989</v>
+        <v>2672364</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>31902</v>
+        <v>31993</v>
       </c>
       <c r="D413" t="n">
-        <v>43227975</v>
+        <v>43352309</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>7765</v>
+        <v>7780</v>
       </c>
       <c r="D417" t="n">
-        <v>11417070</v>
+        <v>11439570</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>7058</v>
+        <v>7073</v>
       </c>
       <c r="D419" t="n">
-        <v>10231955</v>
+        <v>10253817</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20542,10 +20542,10 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D421" t="n">
-        <v>731905</v>
+        <v>734905</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D422" t="n">
-        <v>692443</v>
+        <v>693943</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>8676</v>
+        <v>8747</v>
       </c>
       <c r="D423" t="n">
-        <v>12035029</v>
+        <v>12135796</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2185</v>
+        <v>2198</v>
       </c>
       <c r="D425" t="n">
-        <v>3219470</v>
+        <v>3238820</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>2939</v>
+        <v>2966</v>
       </c>
       <c r="D427" t="n">
-        <v>4292112</v>
+        <v>4331812</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D430" t="n">
-        <v>233586</v>
+        <v>244086</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21022,10 +21022,10 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>10996</v>
+        <v>11007</v>
       </c>
       <c r="D431" t="n">
-        <v>13576104</v>
+        <v>13592027</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D433" t="n">
-        <v>110334</v>
+        <v>111740</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="D436" t="n">
-        <v>2666877</v>
+        <v>2675877</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>62716</v>
+        <v>62791</v>
       </c>
       <c r="D439" t="n">
-        <v>77744271</v>
+        <v>77833000</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>24892</v>
+        <v>24905</v>
       </c>
       <c r="D443" t="n">
-        <v>36489068</v>
+        <v>36507654</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>12894</v>
+        <v>12904</v>
       </c>
       <c r="D445" t="n">
-        <v>18697468</v>
+        <v>18712468</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="D449" t="n">
-        <v>1454169</v>
+        <v>1458294</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>18847</v>
+        <v>18868</v>
       </c>
       <c r="D451" t="n">
-        <v>23823976</v>
+        <v>23851008</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>7694</v>
+        <v>7696</v>
       </c>
       <c r="D455" t="n">
-        <v>11293393</v>
+        <v>11296393</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>4839</v>
+        <v>4848</v>
       </c>
       <c r="D457" t="n">
-        <v>7021422</v>
+        <v>7034922</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22366,10 +22366,10 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D459" t="n">
-        <v>395694</v>
+        <v>397194</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>32165</v>
+        <v>32184</v>
       </c>
       <c r="D460" t="n">
-        <v>39319219</v>
+        <v>39341598</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>11439</v>
+        <v>11443</v>
       </c>
       <c r="D464" t="n">
-        <v>16737481</v>
+        <v>16742770</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>4893</v>
+        <v>4898</v>
       </c>
       <c r="D466" t="n">
-        <v>7099893</v>
+        <v>7107393</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>14370</v>
+        <v>14381</v>
       </c>
       <c r="D469" t="n">
-        <v>17573663</v>
+        <v>17588133</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>4374</v>
+        <v>4377</v>
       </c>
       <c r="D474" t="n">
-        <v>6427567</v>
+        <v>6431024</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23182,10 +23182,10 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="D476" t="n">
-        <v>2979783</v>
+        <v>2981283</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>35838</v>
+        <v>35877</v>
       </c>
       <c r="D479" t="n">
-        <v>46700255</v>
+        <v>46749661</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>13526</v>
+        <v>13535</v>
       </c>
       <c r="D483" t="n">
-        <v>19901294</v>
+        <v>19913518</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>11961</v>
+        <v>11967</v>
       </c>
       <c r="D485" t="n">
-        <v>17457088</v>
+        <v>17466088</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D487" t="n">
-        <v>423226</v>
+        <v>424726</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>62073</v>
+        <v>62165</v>
       </c>
       <c r="D488" t="n">
-        <v>82193284</v>
+        <v>82316043</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>23031</v>
+        <v>23060</v>
       </c>
       <c r="D493" t="n">
-        <v>33793740</v>
+        <v>33835944</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>22348</v>
+        <v>22372</v>
       </c>
       <c r="D495" t="n">
-        <v>32446209</v>
+        <v>32480914</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>150090</v>
+        <v>150347</v>
       </c>
       <c r="D499" t="n">
-        <v>197415728</v>
+        <v>197760444</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>81349</v>
+        <v>81441</v>
       </c>
       <c r="D506" t="n">
-        <v>119513311</v>
+        <v>119647439</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>59785</v>
+        <v>59869</v>
       </c>
       <c r="D509" t="n">
-        <v>86785250</v>
+        <v>86907844</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>2769</v>
+        <v>2770</v>
       </c>
       <c r="D513" t="n">
-        <v>3919926</v>
+        <v>3921260</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>40953</v>
+        <v>41041</v>
       </c>
       <c r="D515" t="n">
-        <v>53227812</v>
+        <v>53348188</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25246,10 +25246,10 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D519" t="n">
-        <v>223599</v>
+        <v>225099</v>
       </c>
       <c r="E519" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>15199</v>
+        <v>15214</v>
       </c>
       <c r="D520" t="n">
-        <v>22328339</v>
+        <v>22349549</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>12885</v>
+        <v>12900</v>
       </c>
       <c r="D522" t="n">
-        <v>18677191</v>
+        <v>18698898</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D524" t="n">
-        <v>461045</v>
+        <v>464045</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25534,10 +25534,10 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D525" t="n">
-        <v>492148</v>
+        <v>493648</v>
       </c>
       <c r="E525" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>65859</v>
+        <v>65978</v>
       </c>
       <c r="D527" t="n">
-        <v>88516866</v>
+        <v>88672541</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>23227</v>
+        <v>23254</v>
       </c>
       <c r="D531" t="n">
-        <v>34274997</v>
+        <v>34314597</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D532" t="n">
-        <v>27000</v>
+        <v>28500</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>24001</v>
+        <v>24027</v>
       </c>
       <c r="D533" t="n">
-        <v>35129631</v>
+        <v>35166691</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="D536" t="n">
-        <v>1210469</v>
+        <v>1213469</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>54814</v>
+        <v>54898</v>
       </c>
       <c r="D537" t="n">
-        <v>72706795</v>
+        <v>72817752</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>17721</v>
+        <v>17746</v>
       </c>
       <c r="D542" t="n">
-        <v>26038840</v>
+        <v>26075526</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>18260</v>
+        <v>18281</v>
       </c>
       <c r="D544" t="n">
-        <v>26541996</v>
+        <v>26572512</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>41400</v>
+        <v>41462</v>
       </c>
       <c r="D547" t="n">
-        <v>54982593</v>
+        <v>55058478</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>14169</v>
+        <v>14188</v>
       </c>
       <c r="D551" t="n">
-        <v>20897329</v>
+        <v>20925496</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>14339</v>
+        <v>14363</v>
       </c>
       <c r="D553" t="n">
-        <v>20826398</v>
+        <v>20856917</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D555" t="n">
-        <v>390930</v>
+        <v>393930</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>41192</v>
+        <v>41224</v>
       </c>
       <c r="D556" t="n">
-        <v>53406921</v>
+        <v>53445764</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D559" t="n">
-        <v>190248</v>
+        <v>191748</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>16147</v>
+        <v>16169</v>
       </c>
       <c r="D560" t="n">
-        <v>23692324</v>
+        <v>23723426</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>12950</v>
+        <v>12971</v>
       </c>
       <c r="D562" t="n">
-        <v>18730143</v>
+        <v>18759847</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D565" t="n">
-        <v>494267</v>
+        <v>495767</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>43687</v>
+        <v>43753</v>
       </c>
       <c r="D566" t="n">
-        <v>58340355</v>
+        <v>58426527</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>13868</v>
+        <v>13883</v>
       </c>
       <c r="D572" t="n">
-        <v>20341228</v>
+        <v>20363440</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>3692</v>
+        <v>3694</v>
       </c>
       <c r="D573" t="n">
-        <v>5325211</v>
+        <v>5328211</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D578" t="n">
-        <v>526251</v>
+        <v>527751</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>17200</v>
+        <v>17223</v>
       </c>
       <c r="D579" t="n">
-        <v>22731008</v>
+        <v>22761148</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>7037</v>
+        <v>7042</v>
       </c>
       <c r="D583" t="n">
-        <v>10233981</v>
+        <v>10241481</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28414,10 +28414,10 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>4902</v>
+        <v>4905</v>
       </c>
       <c r="D585" t="n">
-        <v>7056436</v>
+        <v>7060936</v>
       </c>
       <c r="E585" t="inlineStr">
         <is>
@@ -28510,10 +28510,10 @@
         </is>
       </c>
       <c r="C587" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D587" t="n">
-        <v>377235</v>
+        <v>378731</v>
       </c>
       <c r="E587" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>15222</v>
+        <v>15315</v>
       </c>
       <c r="D590" t="n">
-        <v>22087426</v>
+        <v>22223846</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>1732</v>
+        <v>1735</v>
       </c>
       <c r="D591" t="n">
-        <v>2576530</v>
+        <v>2581030</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>21943</v>
+        <v>21957</v>
       </c>
       <c r="D596" t="n">
-        <v>27529793</v>
+        <v>27550683</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D597" t="n">
-        <v>6977</v>
+        <v>7229</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>8972</v>
+        <v>8974</v>
       </c>
       <c r="D601" t="n">
-        <v>13146197</v>
+        <v>13148508</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29374,10 +29374,10 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="D605" t="n">
-        <v>646199</v>
+        <v>646439</v>
       </c>
       <c r="E605" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>14599</v>
+        <v>14604</v>
       </c>
       <c r="D607" t="n">
-        <v>18304147</v>
+        <v>18310724</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>5777</v>
+        <v>5778</v>
       </c>
       <c r="D611" t="n">
-        <v>8484651</v>
+        <v>8486151</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>2666</v>
+        <v>2668</v>
       </c>
       <c r="D613" t="n">
-        <v>3842587</v>
+        <v>3845587</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D614" t="n">
-        <v>253709</v>
+        <v>255209</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>13723</v>
+        <v>13729</v>
       </c>
       <c r="D616" t="n">
-        <v>17339584</v>
+        <v>17343477</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -30094,10 +30094,10 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>5217</v>
+        <v>5218</v>
       </c>
       <c r="D620" t="n">
-        <v>7646720</v>
+        <v>7648220</v>
       </c>
       <c r="E620" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="D621" t="n">
-        <v>1674068</v>
+        <v>1675991</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D624" t="n">
-        <v>362966</v>
+        <v>364466</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>7471</v>
+        <v>7480</v>
       </c>
       <c r="D625" t="n">
-        <v>9613266</v>
+        <v>9623669</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30574,10 +30574,10 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>2556</v>
+        <v>2558</v>
       </c>
       <c r="D630" t="n">
-        <v>3745106</v>
+        <v>3748106</v>
       </c>
       <c r="E630" t="inlineStr">
         <is>
@@ -30670,10 +30670,10 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D632" t="n">
-        <v>247018</v>
+        <v>248518</v>
       </c>
       <c r="E632" t="inlineStr">
         <is>
@@ -30718,10 +30718,10 @@
         </is>
       </c>
       <c r="C633" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D633" t="n">
-        <v>182456</v>
+        <v>183956</v>
       </c>
       <c r="E633" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>28717</v>
+        <v>28735</v>
       </c>
       <c r="D634" t="n">
-        <v>35373029</v>
+        <v>35391051</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>10997</v>
+        <v>11000</v>
       </c>
       <c r="D638" t="n">
-        <v>16136276</v>
+        <v>16139962</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4804</v>
+        <v>4811</v>
       </c>
       <c r="D640" t="n">
-        <v>6971960</v>
+        <v>6980823</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31198,10 +31198,10 @@
         </is>
       </c>
       <c r="C643" t="n">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D643" t="n">
-        <v>800436</v>
+        <v>801936</v>
       </c>
       <c r="E643" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>11266</v>
+        <v>11276</v>
       </c>
       <c r="D644" t="n">
-        <v>13660187</v>
+        <v>13671054</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="D650" t="n">
-        <v>1586807</v>
+        <v>1588307</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>28185</v>
+        <v>28216</v>
       </c>
       <c r="D654" t="n">
-        <v>35050823</v>
+        <v>35082895</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>10712</v>
+        <v>10722</v>
       </c>
       <c r="D658" t="n">
-        <v>15739964</v>
+        <v>15754964</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>3063</v>
+        <v>3066</v>
       </c>
       <c r="D660" t="n">
-        <v>4416477</v>
+        <v>4420977</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D663" t="n">
-        <v>661147</v>
+        <v>662175</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>7457</v>
+        <v>7467</v>
       </c>
       <c r="D664" t="n">
-        <v>9461739</v>
+        <v>9473999</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D669" t="n">
-        <v>358484</v>
+        <v>361484</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3764</v>
+        <v>3766</v>
       </c>
       <c r="D672" t="n">
-        <v>4561982</v>
+        <v>4563767</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D676" t="n">
-        <v>1141787</v>
+        <v>1143287</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>9270</v>
+        <v>9278</v>
       </c>
       <c r="D681" t="n">
-        <v>11571313</v>
+        <v>11579162</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>3459</v>
+        <v>3463</v>
       </c>
       <c r="D685" t="n">
-        <v>5099017</v>
+        <v>5105017</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D688" t="n">
-        <v>238299</v>
+        <v>239799</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D689" t="n">
-        <v>378069</v>
+        <v>379569</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>19143</v>
+        <v>19156</v>
       </c>
       <c r="D690" t="n">
-        <v>23438473</v>
+        <v>23452454</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>5695</v>
+        <v>5698</v>
       </c>
       <c r="D694" t="n">
-        <v>8318272</v>
+        <v>8322480</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>2237</v>
+        <v>2238</v>
       </c>
       <c r="D696" t="n">
-        <v>3218514</v>
+        <v>3220014</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>74015</v>
+        <v>74097</v>
       </c>
       <c r="D701" t="n">
-        <v>93180958</v>
+        <v>93287118</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>26420</v>
+        <v>26439</v>
       </c>
       <c r="D706" t="n">
-        <v>38795238</v>
+        <v>38822919</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>13089</v>
+        <v>13100</v>
       </c>
       <c r="D709" t="n">
-        <v>18878269</v>
+        <v>18894714</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D710" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="D712" t="n">
-        <v>2773129</v>
+        <v>2774629</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="D714" t="n">
-        <v>1647335</v>
+        <v>1651835</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>11082</v>
+        <v>11092</v>
       </c>
       <c r="D715" t="n">
-        <v>13557228</v>
+        <v>13570748</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>4087</v>
+        <v>4091</v>
       </c>
       <c r="D718" t="n">
-        <v>5979155</v>
+        <v>5984583</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D720" t="n">
-        <v>2138500</v>
+        <v>2140000</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -35038,10 +35038,10 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>17491</v>
+        <v>17511</v>
       </c>
       <c r="D723" t="n">
-        <v>21580263</v>
+        <v>21600605</v>
       </c>
       <c r="E723" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D724" t="n">
-        <v>23064</v>
+        <v>24621</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>6820</v>
+        <v>6824</v>
       </c>
       <c r="D727" t="n">
-        <v>9968829</v>
+        <v>9974829</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35326,10 +35326,10 @@
         </is>
       </c>
       <c r="C729" t="n">
-        <v>2167</v>
+        <v>2171</v>
       </c>
       <c r="D729" t="n">
-        <v>3106538</v>
+        <v>3112538</v>
       </c>
       <c r="E729" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>11442</v>
+        <v>11453</v>
       </c>
       <c r="D734" t="n">
-        <v>14130032</v>
+        <v>14145102</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35854,10 +35854,10 @@
         </is>
       </c>
       <c r="C740" t="n">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D740" t="n">
-        <v>2312534</v>
+        <v>2314034</v>
       </c>
       <c r="E740" t="inlineStr">
         <is>
@@ -35950,10 +35950,10 @@
         </is>
       </c>
       <c r="C742" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D742" t="n">
-        <v>424923</v>
+        <v>426423</v>
       </c>
       <c r="E742" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>29389</v>
+        <v>29411</v>
       </c>
       <c r="D743" t="n">
-        <v>36532810</v>
+        <v>36561557</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>12673</v>
+        <v>12679</v>
       </c>
       <c r="D748" t="n">
-        <v>18548762</v>
+        <v>18557472</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36334,10 +36334,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>4198</v>
+        <v>4199</v>
       </c>
       <c r="D750" t="n">
-        <v>5997619</v>
+        <v>5999119</v>
       </c>
       <c r="E750" t="inlineStr">
         <is>
@@ -36430,10 +36430,10 @@
         </is>
       </c>
       <c r="C752" t="n">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="D752" t="n">
-        <v>1068157</v>
+        <v>1075657</v>
       </c>
       <c r="E752" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D753" t="n">
-        <v>949004</v>
+        <v>952004</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>12248</v>
+        <v>12258</v>
       </c>
       <c r="D755" t="n">
-        <v>15169836</v>
+        <v>15180159</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36718,10 +36718,10 @@
         </is>
       </c>
       <c r="C758" t="n">
-        <v>4644</v>
+        <v>4645</v>
       </c>
       <c r="D758" t="n">
-        <v>6788007</v>
+        <v>6789507</v>
       </c>
       <c r="E758" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D760" t="n">
-        <v>258588</v>
+        <v>259982</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>6677</v>
+        <v>6683</v>
       </c>
       <c r="D762" t="n">
-        <v>7850300</v>
+        <v>7856799</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37102,10 +37102,10 @@
         </is>
       </c>
       <c r="C766" t="n">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="D766" t="n">
-        <v>2469373</v>
+        <v>2470873</v>
       </c>
       <c r="E766" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="D767" t="n">
-        <v>1451844</v>
+        <v>1453344</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37198,10 +37198,10 @@
         </is>
       </c>
       <c r="C768" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D768" t="n">
-        <v>214494</v>
+        <v>215994</v>
       </c>
       <c r="E768" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>16690</v>
+        <v>16708</v>
       </c>
       <c r="D770" t="n">
-        <v>20248402</v>
+        <v>20268209</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>5518</v>
+        <v>5519</v>
       </c>
       <c r="D775" t="n">
-        <v>8085376</v>
+        <v>8086587</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37726,10 +37726,10 @@
         </is>
       </c>
       <c r="C779" t="n">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D779" t="n">
-        <v>526112</v>
+        <v>527612</v>
       </c>
       <c r="E779" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>11313</v>
+        <v>11322</v>
       </c>
       <c r="D781" t="n">
-        <v>14336352</v>
+        <v>14344495</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -38014,10 +38014,10 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>3943</v>
+        <v>3945</v>
       </c>
       <c r="D785" t="n">
-        <v>5765483</v>
+        <v>5768483</v>
       </c>
       <c r="E785" t="inlineStr">
         <is>
@@ -38206,10 +38206,10 @@
         </is>
       </c>
       <c r="C789" t="n">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D789" t="n">
-        <v>730179</v>
+        <v>731679</v>
       </c>
       <c r="E789" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>31931</v>
+        <v>31977</v>
       </c>
       <c r="D791" t="n">
-        <v>39392805</v>
+        <v>39452457</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38494,10 +38494,10 @@
         </is>
       </c>
       <c r="C795" t="n">
-        <v>13146</v>
+        <v>13153</v>
       </c>
       <c r="D795" t="n">
-        <v>19236088</v>
+        <v>19245934</v>
       </c>
       <c r="E795" t="inlineStr">
         <is>
@@ -38590,10 +38590,10 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>6013</v>
+        <v>6017</v>
       </c>
       <c r="D797" t="n">
-        <v>8689230</v>
+        <v>8695230</v>
       </c>
       <c r="E797" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D798" t="n">
-        <v>725817</v>
+        <v>728817</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>7562</v>
+        <v>7570</v>
       </c>
       <c r="D801" t="n">
-        <v>9353393</v>
+        <v>9361796</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -39262,10 +39262,10 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>58439</v>
+        <v>58523</v>
       </c>
       <c r="D811" t="n">
-        <v>73046480</v>
+        <v>73151269</v>
       </c>
       <c r="E811" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>21057</v>
+        <v>21075</v>
       </c>
       <c r="D816" t="n">
-        <v>30808798</v>
+        <v>30834725</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>12534</v>
+        <v>12550</v>
       </c>
       <c r="D819" t="n">
-        <v>18093534</v>
+        <v>18115829</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>1309</v>
+        <v>1312</v>
       </c>
       <c r="D824" t="n">
-        <v>1825685</v>
+        <v>1830185</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>11071</v>
+        <v>11082</v>
       </c>
       <c r="D825" t="n">
-        <v>13805772</v>
+        <v>13820192</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -39982,10 +39982,10 @@
         </is>
       </c>
       <c r="C826" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D826" t="n">
-        <v>15561</v>
+        <v>17061</v>
       </c>
       <c r="E826" t="inlineStr">
         <is>
@@ -40126,10 +40126,10 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>3893</v>
+        <v>3900</v>
       </c>
       <c r="D829" t="n">
-        <v>5660522</v>
+        <v>5671022</v>
       </c>
       <c r="E829" t="inlineStr">
         <is>
@@ -40222,10 +40222,10 @@
         </is>
       </c>
       <c r="C831" t="n">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="D831" t="n">
-        <v>1763049</v>
+        <v>1766049</v>
       </c>
       <c r="E831" t="inlineStr">
         <is>
@@ -40414,10 +40414,10 @@
         </is>
       </c>
       <c r="C835" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D835" t="n">
-        <v>365910</v>
+        <v>367410</v>
       </c>
       <c r="E835" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>58185</v>
+        <v>58238</v>
       </c>
       <c r="D836" t="n">
-        <v>71950213</v>
+        <v>72015412</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>22249</v>
+        <v>22264</v>
       </c>
       <c r="D842" t="n">
-        <v>32648002</v>
+        <v>32668595</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>14243</v>
+        <v>14262</v>
       </c>
       <c r="D844" t="n">
-        <v>20619779</v>
+        <v>20647414</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -40942,10 +40942,10 @@
         </is>
       </c>
       <c r="C846" t="n">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="D846" t="n">
-        <v>1268101</v>
+        <v>1270601</v>
       </c>
       <c r="E846" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>1227</v>
+        <v>1231</v>
       </c>
       <c r="D847" t="n">
-        <v>1708786</v>
+        <v>1714786</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>7701</v>
+        <v>7706</v>
       </c>
       <c r="D849" t="n">
-        <v>9449379</v>
+        <v>9456879</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41182,10 +41182,10 @@
         </is>
       </c>
       <c r="C851" t="n">
-        <v>2560</v>
+        <v>2562</v>
       </c>
       <c r="D851" t="n">
-        <v>3727698</v>
+        <v>3730562</v>
       </c>
       <c r="E851" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D853" t="n">
-        <v>427597</v>
+        <v>429097</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41326,10 +41326,10 @@
         </is>
       </c>
       <c r="C854" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D854" t="n">
-        <v>245155</v>
+        <v>245918</v>
       </c>
       <c r="E854" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>3570</v>
+        <v>3580</v>
       </c>
       <c r="D855" t="n">
-        <v>4616349</v>
+        <v>4628637</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41470,10 +41470,10 @@
         </is>
       </c>
       <c r="C857" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D857" t="n">
-        <v>61992</v>
+        <v>63492</v>
       </c>
       <c r="E857" t="inlineStr">
         <is>
@@ -41518,10 +41518,10 @@
         </is>
       </c>
       <c r="C858" t="n">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D858" t="n">
-        <v>1704082</v>
+        <v>1705582</v>
       </c>
       <c r="E858" t="inlineStr">
         <is>
@@ -41758,10 +41758,10 @@
         </is>
       </c>
       <c r="C863" t="n">
-        <v>22236</v>
+        <v>22257</v>
       </c>
       <c r="D863" t="n">
-        <v>27860393</v>
+        <v>27887937</v>
       </c>
       <c r="E863" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>7714</v>
+        <v>7725</v>
       </c>
       <c r="D867" t="n">
-        <v>11259756</v>
+        <v>11276256</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -42046,10 +42046,10 @@
         </is>
       </c>
       <c r="C869" t="n">
-        <v>4600</v>
+        <v>4608</v>
       </c>
       <c r="D869" t="n">
-        <v>6651421</v>
+        <v>6662151</v>
       </c>
       <c r="E869" t="inlineStr">
         <is>
@@ -42190,10 +42190,10 @@
         </is>
       </c>
       <c r="C872" t="n">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D872" t="n">
-        <v>593794</v>
+        <v>594055</v>
       </c>
       <c r="E872" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>14434</v>
+        <v>14448</v>
       </c>
       <c r="D874" t="n">
-        <v>17406996</v>
+        <v>17421978</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42478,10 +42478,10 @@
         </is>
       </c>
       <c r="C878" t="n">
-        <v>5225</v>
+        <v>5230</v>
       </c>
       <c r="D878" t="n">
-        <v>7620500</v>
+        <v>7627610</v>
       </c>
       <c r="E878" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>2349</v>
+        <v>2351</v>
       </c>
       <c r="D880" t="n">
-        <v>3377003</v>
+        <v>3380003</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42718,10 +42718,10 @@
         </is>
       </c>
       <c r="C883" t="n">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D883" t="n">
-        <v>406885</v>
+        <v>409885</v>
       </c>
       <c r="E883" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>9727</v>
+        <v>9735</v>
       </c>
       <c r="D884" t="n">
-        <v>11955508</v>
+        <v>11965028</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42910,10 +42910,10 @@
         </is>
       </c>
       <c r="C887" t="n">
-        <v>3338</v>
+        <v>3340</v>
       </c>
       <c r="D887" t="n">
-        <v>4890738</v>
+        <v>4893738</v>
       </c>
       <c r="E887" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>44330</v>
+        <v>44358</v>
       </c>
       <c r="D891" t="n">
-        <v>55699957</v>
+        <v>55735119</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>20974</v>
+        <v>20990</v>
       </c>
       <c r="D896" t="n">
-        <v>30755477</v>
+        <v>30777625</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43438,10 +43438,10 @@
         </is>
       </c>
       <c r="C898" t="n">
-        <v>5858</v>
+        <v>5868</v>
       </c>
       <c r="D898" t="n">
-        <v>8440169</v>
+        <v>8455169</v>
       </c>
       <c r="E898" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>21099</v>
+        <v>21124</v>
       </c>
       <c r="D902" t="n">
-        <v>26264723</v>
+        <v>26292309</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43774,10 +43774,10 @@
         </is>
       </c>
       <c r="C905" t="n">
-        <v>9742</v>
+        <v>9750</v>
       </c>
       <c r="D905" t="n">
-        <v>14275869</v>
+        <v>14287869</v>
       </c>
       <c r="E905" t="inlineStr">
         <is>
@@ -43870,10 +43870,10 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>2264</v>
+        <v>2266</v>
       </c>
       <c r="D907" t="n">
-        <v>3244165</v>
+        <v>3247165</v>
       </c>
       <c r="E907" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>7000</v>
+        <v>7006</v>
       </c>
       <c r="D911" t="n">
-        <v>8802191</v>
+        <v>8809529</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>3006</v>
+        <v>3008</v>
       </c>
       <c r="D916" t="n">
-        <v>4427020</v>
+        <v>4430020</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44494,10 +44494,10 @@
         </is>
       </c>
       <c r="C920" t="n">
-        <v>12962</v>
+        <v>12966</v>
       </c>
       <c r="D920" t="n">
-        <v>16161434</v>
+        <v>16165915</v>
       </c>
       <c r="E920" t="inlineStr">
         <is>
@@ -44686,10 +44686,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>5231</v>
+        <v>5233</v>
       </c>
       <c r="D924" t="n">
-        <v>7644180</v>
+        <v>7647180</v>
       </c>
       <c r="E924" t="inlineStr">
         <is>
@@ -44782,10 +44782,10 @@
         </is>
       </c>
       <c r="C926" t="n">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="D926" t="n">
-        <v>1977367</v>
+        <v>1980367</v>
       </c>
       <c r="E926" t="inlineStr">
         <is>
@@ -44974,10 +44974,10 @@
         </is>
       </c>
       <c r="C930" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D930" t="n">
-        <v>356684</v>
+        <v>358184</v>
       </c>
       <c r="E930" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>19228</v>
+        <v>19237</v>
       </c>
       <c r="D931" t="n">
-        <v>24028881</v>
+        <v>24040213</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45310,10 +45310,10 @@
         </is>
       </c>
       <c r="C937" t="n">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="D937" t="n">
-        <v>2960319</v>
+        <v>2961819</v>
       </c>
       <c r="E937" t="inlineStr">
         <is>
@@ -45358,10 +45358,10 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D938" t="n">
-        <v>488147</v>
+        <v>491147</v>
       </c>
       <c r="E938" t="inlineStr">
         <is>
@@ -45406,10 +45406,10 @@
         </is>
       </c>
       <c r="C939" t="n">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D939" t="n">
-        <v>613807</v>
+        <v>616795</v>
       </c>
       <c r="E939" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>8583</v>
+        <v>8586</v>
       </c>
       <c r="D940" t="n">
-        <v>10712407</v>
+        <v>10715120</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>3189</v>
+        <v>3191</v>
       </c>
       <c r="D945" t="n">
-        <v>4651641</v>
+        <v>4654634</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D946" t="n">
-        <v>2150909</v>
+        <v>2152409</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>66781</v>
+        <v>66835</v>
       </c>
       <c r="D950" t="n">
-        <v>85749757</v>
+        <v>85816763</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>25469</v>
+        <v>25484</v>
       </c>
       <c r="D957" t="n">
-        <v>37329817</v>
+        <v>37352317</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46366,10 +46366,10 @@
         </is>
       </c>
       <c r="C959" t="n">
-        <v>17513</v>
+        <v>17530</v>
       </c>
       <c r="D959" t="n">
-        <v>25393228</v>
+        <v>25417242</v>
       </c>
       <c r="E959" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>83347</v>
+        <v>83422</v>
       </c>
       <c r="D963" t="n">
-        <v>104669917</v>
+        <v>104755193</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>33691</v>
+        <v>33708</v>
       </c>
       <c r="D970" t="n">
-        <v>49421902</v>
+        <v>49447106</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -47038,10 +47038,10 @@
         </is>
       </c>
       <c r="C973" t="n">
-        <v>25070</v>
+        <v>25095</v>
       </c>
       <c r="D973" t="n">
-        <v>36359261</v>
+        <v>36396461</v>
       </c>
       <c r="E973" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="D974" t="n">
-        <v>866073</v>
+        <v>871462</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>1974</v>
+        <v>1977</v>
       </c>
       <c r="D976" t="n">
-        <v>2780345</v>
+        <v>2783993</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>10697</v>
+        <v>10704</v>
       </c>
       <c r="D977" t="n">
-        <v>13959740</v>
+        <v>13967791</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47422,10 +47422,10 @@
         </is>
       </c>
       <c r="C981" t="n">
-        <v>3448</v>
+        <v>3453</v>
       </c>
       <c r="D981" t="n">
-        <v>5037276</v>
+        <v>5043922</v>
       </c>
       <c r="E981" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>55746</v>
+        <v>55781</v>
       </c>
       <c r="D987" t="n">
-        <v>69792454</v>
+        <v>69838023</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>18462</v>
+        <v>18469</v>
       </c>
       <c r="D992" t="n">
-        <v>27037283</v>
+        <v>27047783</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -48046,10 +48046,10 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>12563</v>
+        <v>12573</v>
       </c>
       <c r="D994" t="n">
-        <v>18168257</v>
+        <v>18182557</v>
       </c>
       <c r="E994" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>28079</v>
+        <v>28118</v>
       </c>
       <c r="D998" t="n">
-        <v>34942326</v>
+        <v>34991433</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48478,10 +48478,10 @@
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>10453</v>
+        <v>10467</v>
       </c>
       <c r="D1003" t="n">
-        <v>15309495</v>
+        <v>15329750</v>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>6192</v>
+        <v>6196</v>
       </c>
       <c r="D1005" t="n">
-        <v>8978105</v>
+        <v>8984105</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D1006" t="n">
-        <v>743418</v>
+        <v>744918</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-09 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16315</v>
+        <v>16323</v>
       </c>
       <c r="D2" t="n">
-        <v>20511856</v>
+        <v>20522921</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="D6" t="n">
-        <v>9116922</v>
+        <v>9122268</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3281</v>
+        <v>3284</v>
       </c>
       <c r="D8" t="n">
-        <v>4749712</v>
+        <v>4754212</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D11" t="n">
-        <v>513708</v>
+        <v>515208</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10958</v>
+        <v>10963</v>
       </c>
       <c r="D12" t="n">
-        <v>13834036</v>
+        <v>13840056</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D18" t="n">
-        <v>2089220</v>
+        <v>2090720</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14207</v>
+        <v>14217</v>
       </c>
       <c r="D21" t="n">
-        <v>17429769</v>
+        <v>17440448</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1630,10 +1630,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1719</v>
+        <v>1722</v>
       </c>
       <c r="D27" t="n">
-        <v>2457399</v>
+        <v>2461899</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D28" t="n">
-        <v>357672</v>
+        <v>358912</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D30" t="n">
-        <v>467903</v>
+        <v>469403</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6542</v>
+        <v>6545</v>
       </c>
       <c r="D31" t="n">
-        <v>8689865</v>
+        <v>8694275</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="D34" t="n">
-        <v>2315620</v>
+        <v>2317120</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>21797</v>
+        <v>21813</v>
       </c>
       <c r="D40" t="n">
-        <v>26838971</v>
+        <v>26856566</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7789</v>
+        <v>7792</v>
       </c>
       <c r="D46" t="n">
-        <v>11440960</v>
+        <v>11445460</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3827</v>
+        <v>3830</v>
       </c>
       <c r="D48" t="n">
-        <v>5539155</v>
+        <v>5543655</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D51" t="n">
-        <v>821066</v>
+        <v>822566</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>8121</v>
+        <v>8125</v>
       </c>
       <c r="D52" t="n">
-        <v>10367461</v>
+        <v>10372127</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2776</v>
+        <v>2778</v>
       </c>
       <c r="D56" t="n">
-        <v>4038987</v>
+        <v>4041303</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>36031</v>
+        <v>36060</v>
       </c>
       <c r="D61" t="n">
-        <v>46389451</v>
+        <v>46425867</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>13123</v>
+        <v>13128</v>
       </c>
       <c r="D66" t="n">
-        <v>19246335</v>
+        <v>19253835</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5144</v>
+        <v>5147</v>
       </c>
       <c r="D68" t="n">
-        <v>7439967</v>
+        <v>7443815</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D72" t="n">
-        <v>481176</v>
+        <v>482676</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>46108</v>
+        <v>46149</v>
       </c>
       <c r="D74" t="n">
-        <v>58967343</v>
+        <v>59016174</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4078,10 +4078,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>18087</v>
+        <v>18097</v>
       </c>
       <c r="D78" t="n">
-        <v>26499739</v>
+        <v>26513305</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9312</v>
+        <v>9317</v>
       </c>
       <c r="D80" t="n">
-        <v>13444049</v>
+        <v>13451549</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>24851</v>
+        <v>24868</v>
       </c>
       <c r="D85" t="n">
-        <v>31335547</v>
+        <v>31354563</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8668</v>
+        <v>8674</v>
       </c>
       <c r="D89" t="n">
-        <v>12723966</v>
+        <v>12732886</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4884</v>
+        <v>4891</v>
       </c>
       <c r="D91" t="n">
-        <v>7060227</v>
+        <v>7069638</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D93" t="n">
-        <v>1058815</v>
+        <v>1060315</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>21901</v>
+        <v>21917</v>
       </c>
       <c r="D94" t="n">
-        <v>27494630</v>
+        <v>27515519</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -5038,10 +5038,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9141</v>
+        <v>9143</v>
       </c>
       <c r="D98" t="n">
-        <v>13381205</v>
+        <v>13384205</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -5134,10 +5134,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>3310</v>
+        <v>3312</v>
       </c>
       <c r="D100" t="n">
-        <v>4741746</v>
+        <v>4744746</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -5326,10 +5326,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D104" t="n">
-        <v>623094</v>
+        <v>624594</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>81363</v>
+        <v>81430</v>
       </c>
       <c r="D105" t="n">
-        <v>104286444</v>
+        <v>104363624</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>30547</v>
+        <v>30561</v>
       </c>
       <c r="D112" t="n">
-        <v>44826616</v>
+        <v>44846873</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20762</v>
+        <v>20777</v>
       </c>
       <c r="D114" t="n">
-        <v>29959694</v>
+        <v>29982194</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1879</v>
+        <v>1881</v>
       </c>
       <c r="D121" t="n">
-        <v>2642883</v>
+        <v>2645883</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>27630</v>
+        <v>27646</v>
       </c>
       <c r="D122" t="n">
-        <v>36466789</v>
+        <v>36487611</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D123" t="n">
-        <v>117827</v>
+        <v>118956</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6334,10 +6334,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D125" t="n">
-        <v>135605</v>
+        <v>137105</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>9853</v>
+        <v>9857</v>
       </c>
       <c r="D126" t="n">
-        <v>14449979</v>
+        <v>14455979</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6622,10 +6622,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D131" t="n">
-        <v>487482</v>
+        <v>488982</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15692</v>
+        <v>15708</v>
       </c>
       <c r="D132" t="n">
-        <v>19532437</v>
+        <v>19549614</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6814,10 +6814,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7745</v>
+        <v>7750</v>
       </c>
       <c r="D135" t="n">
-        <v>11335064</v>
+        <v>11341635</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2207</v>
+        <v>2209</v>
       </c>
       <c r="D137" t="n">
-        <v>3151110</v>
+        <v>3154110</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7102,10 +7102,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D141" t="n">
-        <v>541999</v>
+        <v>543499</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>13497</v>
+        <v>13506</v>
       </c>
       <c r="D142" t="n">
-        <v>16867623</v>
+        <v>16880085</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6235</v>
+        <v>6237</v>
       </c>
       <c r="D146" t="n">
-        <v>9134755</v>
+        <v>9137755</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7630,10 +7630,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>5971</v>
+        <v>5976</v>
       </c>
       <c r="D152" t="n">
-        <v>7304762</v>
+        <v>7309862</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D156" t="n">
-        <v>971327</v>
+        <v>974327</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7422</v>
+        <v>7426</v>
       </c>
       <c r="D160" t="n">
-        <v>9205411</v>
+        <v>9209161</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>2846</v>
+        <v>2848</v>
       </c>
       <c r="D163" t="n">
-        <v>4173795</v>
+        <v>4175958</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D164" t="n">
-        <v>2008971</v>
+        <v>2009932</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5602</v>
+        <v>5604</v>
       </c>
       <c r="D168" t="n">
-        <v>7053087</v>
+        <v>7055122</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8734,10 +8734,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D175" t="n">
-        <v>996398</v>
+        <v>997472</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>15923</v>
+        <v>15944</v>
       </c>
       <c r="D178" t="n">
-        <v>20012096</v>
+        <v>20034454</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6380</v>
+        <v>6382</v>
       </c>
       <c r="D183" t="n">
-        <v>9319294</v>
+        <v>9322294</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3058</v>
+        <v>3061</v>
       </c>
       <c r="D188" t="n">
-        <v>3842191</v>
+        <v>3845491</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9694,10 +9694,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D195" t="n">
-        <v>67025</v>
+        <v>68525</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9189</v>
+        <v>9195</v>
       </c>
       <c r="D196" t="n">
-        <v>11475143</v>
+        <v>11482026</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>17216</v>
+        <v>17227</v>
       </c>
       <c r="D205" t="n">
-        <v>21508086</v>
+        <v>21518714</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>7675</v>
+        <v>7678</v>
       </c>
       <c r="D209" t="n">
-        <v>11271301</v>
+        <v>11275801</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>26079</v>
+        <v>26095</v>
       </c>
       <c r="D213" t="n">
-        <v>32901891</v>
+        <v>32919425</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D214" t="n">
-        <v>35473</v>
+        <v>36973</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>10482</v>
+        <v>10483</v>
       </c>
       <c r="D217" t="n">
-        <v>15309352</v>
+        <v>15310852</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D218" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>28411</v>
+        <v>28428</v>
       </c>
       <c r="D223" t="n">
-        <v>35866103</v>
+        <v>35885586</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>14717</v>
+        <v>14720</v>
       </c>
       <c r="D228" t="n">
-        <v>21595543</v>
+        <v>21599928</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2648</v>
+        <v>2650</v>
       </c>
       <c r="D230" t="n">
-        <v>3801675</v>
+        <v>3804675</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="D233" t="n">
-        <v>1015226</v>
+        <v>1019228</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24225</v>
+        <v>24237</v>
       </c>
       <c r="D234" t="n">
-        <v>30563846</v>
+        <v>30577910</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>11162</v>
+        <v>11167</v>
       </c>
       <c r="D240" t="n">
-        <v>16363749</v>
+        <v>16371249</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2503</v>
+        <v>2505</v>
       </c>
       <c r="D242" t="n">
-        <v>3577847</v>
+        <v>3580847</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12142,10 +12142,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>7855</v>
+        <v>7862</v>
       </c>
       <c r="D246" t="n">
-        <v>9828995</v>
+        <v>9837056</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>9786</v>
+        <v>9791</v>
       </c>
       <c r="D256" t="n">
-        <v>12482307</v>
+        <v>12488092</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12814,10 +12814,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>4189</v>
+        <v>4193</v>
       </c>
       <c r="D260" t="n">
-        <v>6149170</v>
+        <v>6155170</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>2167</v>
+        <v>2169</v>
       </c>
       <c r="D262" t="n">
-        <v>3137169</v>
+        <v>3140102</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>5529</v>
+        <v>5532</v>
       </c>
       <c r="D265" t="n">
-        <v>6855978</v>
+        <v>6858043</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13198,10 +13198,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="D268" t="n">
-        <v>2944657</v>
+        <v>2947657</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D270" t="n">
-        <v>1029872</v>
+        <v>1031372</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13486,10 +13486,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>19028</v>
+        <v>19041</v>
       </c>
       <c r="D274" t="n">
-        <v>24046316</v>
+        <v>24062909</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13630,10 +13630,10 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D277" t="n">
-        <v>107945</v>
+        <v>109445</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>7917</v>
+        <v>7918</v>
       </c>
       <c r="D278" t="n">
-        <v>11608205</v>
+        <v>11609705</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>2491</v>
+        <v>2492</v>
       </c>
       <c r="D280" t="n">
-        <v>3578059</v>
+        <v>3579559</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D283" t="n">
-        <v>649423</v>
+        <v>650745</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>16565</v>
+        <v>16578</v>
       </c>
       <c r="D285" t="n">
-        <v>20523038</v>
+        <v>20539922</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>7173</v>
+        <v>7178</v>
       </c>
       <c r="D289" t="n">
-        <v>10521112</v>
+        <v>10528612</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>3325</v>
+        <v>3328</v>
       </c>
       <c r="D290" t="n">
-        <v>4819743</v>
+        <v>4823299</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>9324</v>
+        <v>9331</v>
       </c>
       <c r="D294" t="n">
-        <v>11719794</v>
+        <v>11727079</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>3908</v>
+        <v>3910</v>
       </c>
       <c r="D298" t="n">
-        <v>5719832</v>
+        <v>5722832</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>9182</v>
+        <v>9186</v>
       </c>
       <c r="D304" t="n">
-        <v>11991326</v>
+        <v>11996036</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>3732</v>
+        <v>3735</v>
       </c>
       <c r="D308" t="n">
-        <v>5455849</v>
+        <v>5460349</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2349</v>
+        <v>2351</v>
       </c>
       <c r="D309" t="n">
-        <v>3416568</v>
+        <v>3419468</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>11040</v>
+        <v>11053</v>
       </c>
       <c r="D312" t="n">
-        <v>14497623</v>
+        <v>14515336</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>3773</v>
+        <v>3777</v>
       </c>
       <c r="D316" t="n">
-        <v>5531241</v>
+        <v>5537181</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="D318" t="n">
-        <v>3907638</v>
+        <v>3909138</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D320" t="n">
-        <v>231786</v>
+        <v>233286</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6794</v>
+        <v>6801</v>
       </c>
       <c r="D321" t="n">
-        <v>8399105</v>
+        <v>8409391</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>7507</v>
+        <v>7512</v>
       </c>
       <c r="D331" t="n">
-        <v>9397641</v>
+        <v>9404046</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D337" t="n">
-        <v>1844195</v>
+        <v>1845695</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>31919</v>
+        <v>31944</v>
       </c>
       <c r="D340" t="n">
-        <v>40106450</v>
+        <v>40132719</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>16513</v>
+        <v>16518</v>
       </c>
       <c r="D346" t="n">
-        <v>24147943</v>
+        <v>24154379</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>8025</v>
+        <v>8029</v>
       </c>
       <c r="D349" t="n">
-        <v>11557034</v>
+        <v>11563034</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D350" t="n">
-        <v>912945</v>
+        <v>914171</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17182,10 +17182,10 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="D351" t="n">
-        <v>1105390</v>
+        <v>1109890</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>3885</v>
+        <v>3887</v>
       </c>
       <c r="D352" t="n">
-        <v>4841282</v>
+        <v>4842945</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D355" t="n">
-        <v>2201657</v>
+        <v>2203157</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>19337</v>
+        <v>19354</v>
       </c>
       <c r="D360" t="n">
-        <v>24112996</v>
+        <v>24134344</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>9890</v>
+        <v>9895</v>
       </c>
       <c r="D364" t="n">
-        <v>14499735</v>
+        <v>14507235</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>4732</v>
+        <v>4733</v>
       </c>
       <c r="D366" t="n">
-        <v>6844355</v>
+        <v>6844409</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>13889</v>
+        <v>13902</v>
       </c>
       <c r="D369" t="n">
-        <v>17379286</v>
+        <v>17393938</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>6434</v>
+        <v>6436</v>
       </c>
       <c r="D373" t="n">
-        <v>9419958</v>
+        <v>9422958</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18334,10 +18334,10 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>2476</v>
+        <v>2478</v>
       </c>
       <c r="D375" t="n">
-        <v>3558087</v>
+        <v>3561087</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>17958</v>
+        <v>17963</v>
       </c>
       <c r="D378" t="n">
-        <v>22399090</v>
+        <v>22405293</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>7135</v>
+        <v>7136</v>
       </c>
       <c r="D382" t="n">
-        <v>10487715</v>
+        <v>10489215</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>4085</v>
+        <v>4088</v>
       </c>
       <c r="D388" t="n">
-        <v>5125846</v>
+        <v>5129292</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D392" t="n">
-        <v>832272</v>
+        <v>833136</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D394" t="n">
-        <v>118310</v>
+        <v>119810</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>22238</v>
+        <v>22248</v>
       </c>
       <c r="D395" t="n">
-        <v>27587902</v>
+        <v>27599752</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>9353</v>
+        <v>9360</v>
       </c>
       <c r="D398" t="n">
-        <v>13768917</v>
+        <v>13779417</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>6201</v>
+        <v>6203</v>
       </c>
       <c r="D400" t="n">
-        <v>9020736</v>
+        <v>9023736</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>11122</v>
+        <v>11130</v>
       </c>
       <c r="D403" t="n">
-        <v>13714332</v>
+        <v>13721686</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>5324</v>
+        <v>5325</v>
       </c>
       <c r="D408" t="n">
-        <v>7781703</v>
+        <v>7783203</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D411" t="n">
-        <v>197582</v>
+        <v>199082</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>31993</v>
+        <v>32054</v>
       </c>
       <c r="D413" t="n">
-        <v>43352309</v>
+        <v>43432262</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>7780</v>
+        <v>7792</v>
       </c>
       <c r="D417" t="n">
-        <v>11439570</v>
+        <v>11457470</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>7073</v>
+        <v>7088</v>
       </c>
       <c r="D419" t="n">
-        <v>10253817</v>
+        <v>10275127</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>8747</v>
+        <v>8791</v>
       </c>
       <c r="D423" t="n">
-        <v>12135796</v>
+        <v>12200726</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2198</v>
+        <v>2210</v>
       </c>
       <c r="D425" t="n">
-        <v>3238820</v>
+        <v>3256352</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>2966</v>
+        <v>2979</v>
       </c>
       <c r="D427" t="n">
-        <v>4331812</v>
+        <v>4351241</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -20926,10 +20926,10 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D429" t="n">
-        <v>183120</v>
+        <v>186120</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D430" t="n">
-        <v>244086</v>
+        <v>247086</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21022,10 +21022,10 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>11007</v>
+        <v>11019</v>
       </c>
       <c r="D431" t="n">
-        <v>13592027</v>
+        <v>13603731</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>1865</v>
+        <v>1868</v>
       </c>
       <c r="D436" t="n">
-        <v>2675877</v>
+        <v>2680227</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>62791</v>
+        <v>62838</v>
       </c>
       <c r="D439" t="n">
-        <v>77833000</v>
+        <v>77883850</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>24905</v>
+        <v>24913</v>
       </c>
       <c r="D443" t="n">
-        <v>36507654</v>
+        <v>36518620</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>12904</v>
+        <v>12907</v>
       </c>
       <c r="D445" t="n">
-        <v>18712468</v>
+        <v>18716968</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D446" t="n">
-        <v>656056</v>
+        <v>659056</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>18868</v>
+        <v>18881</v>
       </c>
       <c r="D451" t="n">
-        <v>23851008</v>
+        <v>23868117</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D454" t="n">
-        <v>230476</v>
+        <v>231976</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>7696</v>
+        <v>7700</v>
       </c>
       <c r="D455" t="n">
-        <v>11296393</v>
+        <v>11302393</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>4848</v>
+        <v>4851</v>
       </c>
       <c r="D457" t="n">
-        <v>7034922</v>
+        <v>7039422</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22366,10 +22366,10 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D459" t="n">
-        <v>397194</v>
+        <v>397444</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>32184</v>
+        <v>32195</v>
       </c>
       <c r="D460" t="n">
-        <v>39341598</v>
+        <v>39355427</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22558,10 +22558,10 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D463" t="n">
-        <v>445784</v>
+        <v>447284</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>11443</v>
+        <v>11446</v>
       </c>
       <c r="D464" t="n">
-        <v>16742770</v>
+        <v>16747270</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>4898</v>
+        <v>4902</v>
       </c>
       <c r="D466" t="n">
-        <v>7107393</v>
+        <v>7113393</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D468" t="n">
-        <v>546774</v>
+        <v>548253</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>14381</v>
+        <v>14386</v>
       </c>
       <c r="D469" t="n">
-        <v>17588133</v>
+        <v>17592872</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>4377</v>
+        <v>4380</v>
       </c>
       <c r="D474" t="n">
-        <v>6431024</v>
+        <v>6434922</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D477" t="n">
-        <v>196869</v>
+        <v>198369</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23278,10 +23278,10 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D478" t="n">
-        <v>462848</v>
+        <v>464348</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>35877</v>
+        <v>35933</v>
       </c>
       <c r="D479" t="n">
-        <v>46749661</v>
+        <v>46821562</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>13535</v>
+        <v>13546</v>
       </c>
       <c r="D483" t="n">
-        <v>19913518</v>
+        <v>19929300</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>11967</v>
+        <v>11975</v>
       </c>
       <c r="D485" t="n">
-        <v>17466088</v>
+        <v>17476788</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>62165</v>
+        <v>62242</v>
       </c>
       <c r="D488" t="n">
-        <v>82316043</v>
+        <v>82418291</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>23060</v>
+        <v>23081</v>
       </c>
       <c r="D493" t="n">
-        <v>33835944</v>
+        <v>33867084</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>22372</v>
+        <v>22396</v>
       </c>
       <c r="D495" t="n">
-        <v>32480914</v>
+        <v>32516840</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24238,10 +24238,10 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D498" t="n">
-        <v>885101</v>
+        <v>886601</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>150347</v>
+        <v>150578</v>
       </c>
       <c r="D499" t="n">
-        <v>197760444</v>
+        <v>198052522</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>81441</v>
+        <v>81520</v>
       </c>
       <c r="D506" t="n">
-        <v>119647439</v>
+        <v>119762852</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>59869</v>
+        <v>59923</v>
       </c>
       <c r="D509" t="n">
-        <v>86907844</v>
+        <v>86984598</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="D511" t="n">
-        <v>1524607</v>
+        <v>1527607</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>2770</v>
+        <v>2774</v>
       </c>
       <c r="D513" t="n">
-        <v>3921260</v>
+        <v>3926678</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>41041</v>
+        <v>41080</v>
       </c>
       <c r="D515" t="n">
-        <v>53348188</v>
+        <v>53397909</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D516" t="n">
-        <v>30937</v>
+        <v>31779</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>15214</v>
+        <v>15224</v>
       </c>
       <c r="D520" t="n">
-        <v>22349549</v>
+        <v>22364249</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>12900</v>
+        <v>12911</v>
       </c>
       <c r="D522" t="n">
-        <v>18698898</v>
+        <v>18714398</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D524" t="n">
-        <v>464045</v>
+        <v>465446</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>65978</v>
+        <v>66077</v>
       </c>
       <c r="D527" t="n">
-        <v>88672541</v>
+        <v>88810669</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>23254</v>
+        <v>23284</v>
       </c>
       <c r="D531" t="n">
-        <v>34314597</v>
+        <v>34358402</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>24027</v>
+        <v>24054</v>
       </c>
       <c r="D533" t="n">
-        <v>35166691</v>
+        <v>35206129</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D535" t="n">
-        <v>367320</v>
+        <v>368820</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D536" t="n">
-        <v>1213469</v>
+        <v>1214969</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>54898</v>
+        <v>54978</v>
       </c>
       <c r="D537" t="n">
-        <v>72817752</v>
+        <v>72921520</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>17746</v>
+        <v>17760</v>
       </c>
       <c r="D542" t="n">
-        <v>26075526</v>
+        <v>26096526</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>18281</v>
+        <v>18293</v>
       </c>
       <c r="D544" t="n">
-        <v>26572512</v>
+        <v>26590367</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>41462</v>
+        <v>41505</v>
       </c>
       <c r="D547" t="n">
-        <v>55058478</v>
+        <v>55118312</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26734,10 +26734,10 @@
         </is>
       </c>
       <c r="C550" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D550" t="n">
-        <v>237750</v>
+        <v>239250</v>
       </c>
       <c r="E550" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>14188</v>
+        <v>14204</v>
       </c>
       <c r="D551" t="n">
-        <v>20925496</v>
+        <v>20949169</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>14363</v>
+        <v>14382</v>
       </c>
       <c r="D553" t="n">
-        <v>20856917</v>
+        <v>20885178</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D555" t="n">
-        <v>393930</v>
+        <v>395430</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>41224</v>
+        <v>41269</v>
       </c>
       <c r="D556" t="n">
-        <v>53445764</v>
+        <v>53498484</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>16169</v>
+        <v>16179</v>
       </c>
       <c r="D560" t="n">
-        <v>23723426</v>
+        <v>23738426</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>12971</v>
+        <v>12984</v>
       </c>
       <c r="D562" t="n">
-        <v>18759847</v>
+        <v>18779347</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>43753</v>
+        <v>43790</v>
       </c>
       <c r="D566" t="n">
-        <v>58426527</v>
+        <v>58473348</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>13883</v>
+        <v>13896</v>
       </c>
       <c r="D572" t="n">
-        <v>20363440</v>
+        <v>20382249</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>3694</v>
+        <v>3696</v>
       </c>
       <c r="D573" t="n">
-        <v>5328211</v>
+        <v>5330140</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>17223</v>
+        <v>17254</v>
       </c>
       <c r="D579" t="n">
-        <v>22761148</v>
+        <v>22797660</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>7042</v>
+        <v>7046</v>
       </c>
       <c r="D583" t="n">
-        <v>10241481</v>
+        <v>10247481</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28414,10 +28414,10 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>4905</v>
+        <v>4909</v>
       </c>
       <c r="D585" t="n">
-        <v>7060936</v>
+        <v>7066936</v>
       </c>
       <c r="E585" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>15315</v>
+        <v>15353</v>
       </c>
       <c r="D590" t="n">
-        <v>22223846</v>
+        <v>22279946</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>1735</v>
+        <v>1737</v>
       </c>
       <c r="D591" t="n">
-        <v>2581030</v>
+        <v>2584030</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D592" t="n">
-        <v>344302</v>
+        <v>345802</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D594" t="n">
-        <v>71690</v>
+        <v>77690</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>21957</v>
+        <v>21973</v>
       </c>
       <c r="D596" t="n">
-        <v>27550683</v>
+        <v>27570223</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>8974</v>
+        <v>8977</v>
       </c>
       <c r="D601" t="n">
-        <v>13148508</v>
+        <v>13153008</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>14604</v>
+        <v>14613</v>
       </c>
       <c r="D607" t="n">
-        <v>18310724</v>
+        <v>18322064</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>5778</v>
+        <v>5780</v>
       </c>
       <c r="D611" t="n">
-        <v>8486151</v>
+        <v>8489151</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>13729</v>
+        <v>13734</v>
       </c>
       <c r="D616" t="n">
-        <v>17343477</v>
+        <v>17348881</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="D621" t="n">
-        <v>1675991</v>
+        <v>1678855</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>7480</v>
+        <v>7485</v>
       </c>
       <c r="D625" t="n">
-        <v>9623669</v>
+        <v>9629769</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30574,10 +30574,10 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="D630" t="n">
-        <v>3748106</v>
+        <v>3749606</v>
       </c>
       <c r="E630" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>28735</v>
+        <v>28752</v>
       </c>
       <c r="D634" t="n">
-        <v>35391051</v>
+        <v>35412814</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>11000</v>
+        <v>11001</v>
       </c>
       <c r="D638" t="n">
-        <v>16139962</v>
+        <v>16141462</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4811</v>
+        <v>4814</v>
       </c>
       <c r="D640" t="n">
-        <v>6980823</v>
+        <v>6985323</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>11276</v>
+        <v>11283</v>
       </c>
       <c r="D644" t="n">
-        <v>13671054</v>
+        <v>13676576</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>3634</v>
+        <v>3636</v>
       </c>
       <c r="D649" t="n">
-        <v>5319719</v>
+        <v>5322719</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31678,10 +31678,10 @@
         </is>
       </c>
       <c r="C653" t="n">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D653" t="n">
-        <v>316290</v>
+        <v>319290</v>
       </c>
       <c r="E653" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>28216</v>
+        <v>28237</v>
       </c>
       <c r="D654" t="n">
-        <v>35082895</v>
+        <v>35109819</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>10722</v>
+        <v>10724</v>
       </c>
       <c r="D658" t="n">
-        <v>15754964</v>
+        <v>15757964</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>3066</v>
+        <v>3070</v>
       </c>
       <c r="D660" t="n">
-        <v>4420977</v>
+        <v>4426977</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>7467</v>
+        <v>7474</v>
       </c>
       <c r="D664" t="n">
-        <v>9473999</v>
+        <v>9483499</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="D666" t="n">
-        <v>3858707</v>
+        <v>3861707</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32398,10 +32398,10 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D668" t="n">
-        <v>1866821</v>
+        <v>1867872</v>
       </c>
       <c r="E668" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D669" t="n">
-        <v>361484</v>
+        <v>364484</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3766</v>
+        <v>3768</v>
       </c>
       <c r="D672" t="n">
-        <v>4563767</v>
+        <v>4566767</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D680" t="n">
-        <v>204108</v>
+        <v>204932</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>9278</v>
+        <v>9283</v>
       </c>
       <c r="D681" t="n">
-        <v>11579162</v>
+        <v>11585981</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D686" t="n">
-        <v>1075602</v>
+        <v>1077102</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>19156</v>
+        <v>19167</v>
       </c>
       <c r="D690" t="n">
-        <v>23452454</v>
+        <v>23462813</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>5698</v>
+        <v>5699</v>
       </c>
       <c r="D694" t="n">
-        <v>8322480</v>
+        <v>8323980</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>2238</v>
+        <v>2239</v>
       </c>
       <c r="D696" t="n">
-        <v>3220014</v>
+        <v>3221514</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D700" t="n">
-        <v>416690</v>
+        <v>418190</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>74097</v>
+        <v>74156</v>
       </c>
       <c r="D701" t="n">
-        <v>93287118</v>
+        <v>93360823</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>26439</v>
+        <v>26448</v>
       </c>
       <c r="D706" t="n">
-        <v>38822919</v>
+        <v>38836419</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>13100</v>
+        <v>13110</v>
       </c>
       <c r="D709" t="n">
-        <v>18894714</v>
+        <v>18909654</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>1925</v>
+        <v>1927</v>
       </c>
       <c r="D712" t="n">
-        <v>2774629</v>
+        <v>2777047</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>1184</v>
+        <v>1189</v>
       </c>
       <c r="D714" t="n">
-        <v>1651835</v>
+        <v>1659039</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>11092</v>
+        <v>11098</v>
       </c>
       <c r="D715" t="n">
-        <v>13570748</v>
+        <v>13577363</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D720" t="n">
-        <v>2140000</v>
+        <v>2141500</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -35038,10 +35038,10 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>17511</v>
+        <v>17519</v>
       </c>
       <c r="D723" t="n">
-        <v>21600605</v>
+        <v>21610384</v>
       </c>
       <c r="E723" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>6824</v>
+        <v>6826</v>
       </c>
       <c r="D727" t="n">
-        <v>9974829</v>
+        <v>9977829</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35326,10 +35326,10 @@
         </is>
       </c>
       <c r="C729" t="n">
-        <v>2171</v>
+        <v>2173</v>
       </c>
       <c r="D729" t="n">
-        <v>3112538</v>
+        <v>3115538</v>
       </c>
       <c r="E729" t="inlineStr">
         <is>
@@ -35422,10 +35422,10 @@
         </is>
       </c>
       <c r="C731" t="n">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D731" t="n">
-        <v>450989</v>
+        <v>452489</v>
       </c>
       <c r="E731" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>11453</v>
+        <v>11461</v>
       </c>
       <c r="D734" t="n">
-        <v>14145102</v>
+        <v>14154539</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35758,10 +35758,10 @@
         </is>
       </c>
       <c r="C738" t="n">
-        <v>4225</v>
+        <v>4228</v>
       </c>
       <c r="D738" t="n">
-        <v>6193745</v>
+        <v>6198245</v>
       </c>
       <c r="E738" t="inlineStr">
         <is>
@@ -35854,10 +35854,10 @@
         </is>
       </c>
       <c r="C740" t="n">
-        <v>1596</v>
+        <v>1598</v>
       </c>
       <c r="D740" t="n">
-        <v>2314034</v>
+        <v>2317034</v>
       </c>
       <c r="E740" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>29411</v>
+        <v>29435</v>
       </c>
       <c r="D743" t="n">
-        <v>36561557</v>
+        <v>36586956</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36094,10 +36094,10 @@
         </is>
       </c>
       <c r="C745" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D745" t="n">
-        <v>48000</v>
+        <v>49500</v>
       </c>
       <c r="E745" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>12679</v>
+        <v>12682</v>
       </c>
       <c r="D748" t="n">
-        <v>18557472</v>
+        <v>18561366</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>12258</v>
+        <v>12272</v>
       </c>
       <c r="D755" t="n">
-        <v>15180159</v>
+        <v>15194684</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36718,10 +36718,10 @@
         </is>
       </c>
       <c r="C758" t="n">
-        <v>4645</v>
+        <v>4648</v>
       </c>
       <c r="D758" t="n">
-        <v>6789507</v>
+        <v>6793356</v>
       </c>
       <c r="E758" t="inlineStr">
         <is>
@@ -36766,10 +36766,10 @@
         </is>
       </c>
       <c r="C759" t="n">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D759" t="n">
-        <v>1641986</v>
+        <v>1643486</v>
       </c>
       <c r="E759" t="inlineStr">
         <is>
@@ -36862,10 +36862,10 @@
         </is>
       </c>
       <c r="C761" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D761" t="n">
-        <v>517662</v>
+        <v>519162</v>
       </c>
       <c r="E761" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>6683</v>
+        <v>6690</v>
       </c>
       <c r="D762" t="n">
-        <v>7856799</v>
+        <v>7864848</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37246,10 +37246,10 @@
         </is>
       </c>
       <c r="C769" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D769" t="n">
-        <v>206015</v>
+        <v>207515</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>16708</v>
+        <v>16722</v>
       </c>
       <c r="D770" t="n">
-        <v>20268209</v>
+        <v>20285128</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37630,10 +37630,10 @@
         </is>
       </c>
       <c r="C777" t="n">
-        <v>3385</v>
+        <v>3387</v>
       </c>
       <c r="D777" t="n">
-        <v>4944277</v>
+        <v>4947277</v>
       </c>
       <c r="E777" t="inlineStr">
         <is>
@@ -37774,10 +37774,10 @@
         </is>
       </c>
       <c r="C780" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D780" t="n">
-        <v>389848</v>
+        <v>391348</v>
       </c>
       <c r="E780" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>11322</v>
+        <v>11327</v>
       </c>
       <c r="D781" t="n">
-        <v>14344495</v>
+        <v>14350175</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -38014,10 +38014,10 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>3945</v>
+        <v>3947</v>
       </c>
       <c r="D785" t="n">
-        <v>5768483</v>
+        <v>5771483</v>
       </c>
       <c r="E785" t="inlineStr">
         <is>
@@ -38110,10 +38110,10 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D787" t="n">
-        <v>1807912</v>
+        <v>1809412</v>
       </c>
       <c r="E787" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>31977</v>
+        <v>32009</v>
       </c>
       <c r="D791" t="n">
-        <v>39452457</v>
+        <v>39488834</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38590,10 +38590,10 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>6017</v>
+        <v>6019</v>
       </c>
       <c r="D797" t="n">
-        <v>8695230</v>
+        <v>8698230</v>
       </c>
       <c r="E797" t="inlineStr">
         <is>
@@ -38734,10 +38734,10 @@
         </is>
       </c>
       <c r="C800" t="n">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D800" t="n">
-        <v>906273</v>
+        <v>907773</v>
       </c>
       <c r="E800" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>7570</v>
+        <v>7580</v>
       </c>
       <c r="D801" t="n">
-        <v>9361796</v>
+        <v>9373636</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -39262,10 +39262,10 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>58523</v>
+        <v>58581</v>
       </c>
       <c r="D811" t="n">
-        <v>73151269</v>
+        <v>73224406</v>
       </c>
       <c r="E811" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>21075</v>
+        <v>21082</v>
       </c>
       <c r="D816" t="n">
-        <v>30834725</v>
+        <v>30845225</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>12550</v>
+        <v>12555</v>
       </c>
       <c r="D819" t="n">
-        <v>18115829</v>
+        <v>18123329</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39742,10 +39742,10 @@
         </is>
       </c>
       <c r="C821" t="n">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="D821" t="n">
-        <v>636361</v>
+        <v>644695</v>
       </c>
       <c r="E821" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D824" t="n">
-        <v>1830185</v>
+        <v>1831685</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>11082</v>
+        <v>11089</v>
       </c>
       <c r="D825" t="n">
-        <v>13820192</v>
+        <v>13828181</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>58238</v>
+        <v>58273</v>
       </c>
       <c r="D836" t="n">
-        <v>72015412</v>
+        <v>72056213</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>22264</v>
+        <v>22267</v>
       </c>
       <c r="D842" t="n">
-        <v>32668595</v>
+        <v>32672826</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>14262</v>
+        <v>14269</v>
       </c>
       <c r="D844" t="n">
-        <v>20647414</v>
+        <v>20657814</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -40942,10 +40942,10 @@
         </is>
       </c>
       <c r="C846" t="n">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D846" t="n">
-        <v>1270601</v>
+        <v>1272101</v>
       </c>
       <c r="E846" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="D847" t="n">
-        <v>1714786</v>
+        <v>1717786</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>7706</v>
+        <v>7710</v>
       </c>
       <c r="D849" t="n">
-        <v>9456879</v>
+        <v>9462879</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41182,10 +41182,10 @@
         </is>
       </c>
       <c r="C851" t="n">
-        <v>2562</v>
+        <v>2565</v>
       </c>
       <c r="D851" t="n">
-        <v>3730562</v>
+        <v>3735062</v>
       </c>
       <c r="E851" t="inlineStr">
         <is>
@@ -41230,10 +41230,10 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="D852" t="n">
-        <v>1551479</v>
+        <v>1552979</v>
       </c>
       <c r="E852" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>3580</v>
+        <v>3584</v>
       </c>
       <c r="D855" t="n">
-        <v>4628637</v>
+        <v>4633813</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41710,10 +41710,10 @@
         </is>
       </c>
       <c r="C862" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D862" t="n">
-        <v>145155</v>
+        <v>146655</v>
       </c>
       <c r="E862" t="inlineStr">
         <is>
@@ -41758,10 +41758,10 @@
         </is>
       </c>
       <c r="C863" t="n">
-        <v>22257</v>
+        <v>22271</v>
       </c>
       <c r="D863" t="n">
-        <v>27887937</v>
+        <v>27903757</v>
       </c>
       <c r="E863" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>7725</v>
+        <v>7729</v>
       </c>
       <c r="D867" t="n">
-        <v>11276256</v>
+        <v>11282256</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -42046,10 +42046,10 @@
         </is>
       </c>
       <c r="C869" t="n">
-        <v>4608</v>
+        <v>4610</v>
       </c>
       <c r="D869" t="n">
-        <v>6662151</v>
+        <v>6665151</v>
       </c>
       <c r="E869" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>14448</v>
+        <v>14461</v>
       </c>
       <c r="D874" t="n">
-        <v>17421978</v>
+        <v>17437648</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42478,10 +42478,10 @@
         </is>
       </c>
       <c r="C878" t="n">
-        <v>5230</v>
+        <v>5231</v>
       </c>
       <c r="D878" t="n">
-        <v>7627610</v>
+        <v>7629110</v>
       </c>
       <c r="E878" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>9735</v>
+        <v>9739</v>
       </c>
       <c r="D884" t="n">
-        <v>11965028</v>
+        <v>11968265</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -43054,10 +43054,10 @@
         </is>
       </c>
       <c r="C890" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D890" t="n">
-        <v>266389</v>
+        <v>267889</v>
       </c>
       <c r="E890" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>44358</v>
+        <v>44392</v>
       </c>
       <c r="D891" t="n">
-        <v>55735119</v>
+        <v>55772445</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>20990</v>
+        <v>20996</v>
       </c>
       <c r="D896" t="n">
-        <v>30777625</v>
+        <v>30786188</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43438,10 +43438,10 @@
         </is>
       </c>
       <c r="C898" t="n">
-        <v>5868</v>
+        <v>5871</v>
       </c>
       <c r="D898" t="n">
-        <v>8455169</v>
+        <v>8459669</v>
       </c>
       <c r="E898" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D899" t="n">
-        <v>886455</v>
+        <v>887955</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>21124</v>
+        <v>21140</v>
       </c>
       <c r="D902" t="n">
-        <v>26292309</v>
+        <v>26308361</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43774,10 +43774,10 @@
         </is>
       </c>
       <c r="C905" t="n">
-        <v>9750</v>
+        <v>9753</v>
       </c>
       <c r="D905" t="n">
-        <v>14287869</v>
+        <v>14292369</v>
       </c>
       <c r="E905" t="inlineStr">
         <is>
@@ -43870,10 +43870,10 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>2266</v>
+        <v>2267</v>
       </c>
       <c r="D907" t="n">
-        <v>3247165</v>
+        <v>3248665</v>
       </c>
       <c r="E907" t="inlineStr">
         <is>
@@ -43966,10 +43966,10 @@
         </is>
       </c>
       <c r="C909" t="n">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D909" t="n">
-        <v>884433</v>
+        <v>885933</v>
       </c>
       <c r="E909" t="inlineStr">
         <is>
@@ -44014,10 +44014,10 @@
         </is>
       </c>
       <c r="C910" t="n">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D910" t="n">
-        <v>880350</v>
+        <v>881850</v>
       </c>
       <c r="E910" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>7006</v>
+        <v>7010</v>
       </c>
       <c r="D911" t="n">
-        <v>8809529</v>
+        <v>8813292</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>3008</v>
+        <v>3010</v>
       </c>
       <c r="D916" t="n">
-        <v>4430020</v>
+        <v>4433020</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44494,10 +44494,10 @@
         </is>
       </c>
       <c r="C920" t="n">
-        <v>12966</v>
+        <v>12976</v>
       </c>
       <c r="D920" t="n">
-        <v>16165915</v>
+        <v>16175450</v>
       </c>
       <c r="E920" t="inlineStr">
         <is>
@@ -44686,10 +44686,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>5233</v>
+        <v>5236</v>
       </c>
       <c r="D924" t="n">
-        <v>7647180</v>
+        <v>7651678</v>
       </c>
       <c r="E924" t="inlineStr">
         <is>
@@ -44782,10 +44782,10 @@
         </is>
       </c>
       <c r="C926" t="n">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D926" t="n">
-        <v>1980367</v>
+        <v>1981867</v>
       </c>
       <c r="E926" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>19237</v>
+        <v>19248</v>
       </c>
       <c r="D931" t="n">
-        <v>24040213</v>
+        <v>24049207</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45214,10 +45214,10 @@
         </is>
       </c>
       <c r="C935" t="n">
-        <v>10057</v>
+        <v>10058</v>
       </c>
       <c r="D935" t="n">
-        <v>14701576</v>
+        <v>14703076</v>
       </c>
       <c r="E935" t="inlineStr">
         <is>
@@ -45358,10 +45358,10 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D938" t="n">
-        <v>491147</v>
+        <v>492647</v>
       </c>
       <c r="E938" t="inlineStr">
         <is>
@@ -45406,10 +45406,10 @@
         </is>
       </c>
       <c r="C939" t="n">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D939" t="n">
-        <v>616795</v>
+        <v>620294</v>
       </c>
       <c r="E939" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>8586</v>
+        <v>8595</v>
       </c>
       <c r="D940" t="n">
-        <v>10715120</v>
+        <v>10727197</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>3191</v>
+        <v>3192</v>
       </c>
       <c r="D945" t="n">
-        <v>4654634</v>
+        <v>4656134</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D946" t="n">
-        <v>2152409</v>
+        <v>2153309</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>66835</v>
+        <v>66895</v>
       </c>
       <c r="D950" t="n">
-        <v>85816763</v>
+        <v>85891282</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>25484</v>
+        <v>25501</v>
       </c>
       <c r="D957" t="n">
-        <v>37352317</v>
+        <v>37376852</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46366,10 +46366,10 @@
         </is>
       </c>
       <c r="C959" t="n">
-        <v>17530</v>
+        <v>17540</v>
       </c>
       <c r="D959" t="n">
-        <v>25417242</v>
+        <v>25431342</v>
       </c>
       <c r="E959" t="inlineStr">
         <is>
@@ -46462,10 +46462,10 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D961" t="n">
-        <v>697335</v>
+        <v>697823</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
@@ -46510,10 +46510,10 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D962" t="n">
-        <v>1232221</v>
+        <v>1233721</v>
       </c>
       <c r="E962" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>83422</v>
+        <v>83493</v>
       </c>
       <c r="D963" t="n">
-        <v>104755193</v>
+        <v>104839381</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>33708</v>
+        <v>33725</v>
       </c>
       <c r="D970" t="n">
-        <v>49447106</v>
+        <v>49470396</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -47038,10 +47038,10 @@
         </is>
       </c>
       <c r="C973" t="n">
-        <v>25095</v>
+        <v>25115</v>
       </c>
       <c r="D973" t="n">
-        <v>36396461</v>
+        <v>36426461</v>
       </c>
       <c r="E973" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D974" t="n">
-        <v>871462</v>
+        <v>872652</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>1977</v>
+        <v>1980</v>
       </c>
       <c r="D976" t="n">
-        <v>2783993</v>
+        <v>2787617</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>10704</v>
+        <v>10716</v>
       </c>
       <c r="D977" t="n">
-        <v>13967791</v>
+        <v>13982476</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47422,10 +47422,10 @@
         </is>
       </c>
       <c r="C981" t="n">
-        <v>3453</v>
+        <v>3455</v>
       </c>
       <c r="D981" t="n">
-        <v>5043922</v>
+        <v>5046922</v>
       </c>
       <c r="E981" t="inlineStr">
         <is>
@@ -47470,10 +47470,10 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="D982" t="n">
-        <v>1603369</v>
+        <v>1606369</v>
       </c>
       <c r="E982" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>55781</v>
+        <v>55825</v>
       </c>
       <c r="D987" t="n">
-        <v>69838023</v>
+        <v>69893337</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>18469</v>
+        <v>18474</v>
       </c>
       <c r="D992" t="n">
-        <v>27047783</v>
+        <v>27055283</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -48046,10 +48046,10 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>12573</v>
+        <v>12577</v>
       </c>
       <c r="D994" t="n">
-        <v>18182557</v>
+        <v>18188477</v>
       </c>
       <c r="E994" t="inlineStr">
         <is>
@@ -48190,10 +48190,10 @@
         </is>
       </c>
       <c r="C997" t="n">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="D997" t="n">
-        <v>1023924</v>
+        <v>1029924</v>
       </c>
       <c r="E997" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>28118</v>
+        <v>28146</v>
       </c>
       <c r="D998" t="n">
-        <v>34991433</v>
+        <v>35021979</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48478,10 +48478,10 @@
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>10467</v>
+        <v>10473</v>
       </c>
       <c r="D1003" t="n">
-        <v>15329750</v>
+        <v>15338750</v>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>6196</v>
+        <v>6203</v>
       </c>
       <c r="D1005" t="n">
-        <v>8984105</v>
+        <v>8994605</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48670,10 +48670,10 @@
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D1007" t="n">
-        <v>713129</v>
+        <v>716129</v>
       </c>
       <c r="E1007" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-10 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16323</v>
+        <v>16338</v>
       </c>
       <c r="D2" t="n">
-        <v>20522921</v>
+        <v>20540918</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="D6" t="n">
-        <v>9122268</v>
+        <v>9125238</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3284</v>
+        <v>3287</v>
       </c>
       <c r="D8" t="n">
-        <v>4754212</v>
+        <v>4756880</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10963</v>
+        <v>10978</v>
       </c>
       <c r="D12" t="n">
-        <v>13840056</v>
+        <v>13854426</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3223</v>
+        <v>3224</v>
       </c>
       <c r="D16" t="n">
-        <v>4696127</v>
+        <v>4697627</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D18" t="n">
-        <v>2090720</v>
+        <v>2092220</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14217</v>
+        <v>14232</v>
       </c>
       <c r="D21" t="n">
-        <v>17440448</v>
+        <v>17457173</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4934</v>
+        <v>4935</v>
       </c>
       <c r="D25" t="n">
-        <v>7215428</v>
+        <v>7216928</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1630,10 +1630,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="D27" t="n">
-        <v>2461899</v>
+        <v>2462493</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D30" t="n">
-        <v>469403</v>
+        <v>470903</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="D34" t="n">
-        <v>2317120</v>
+        <v>2318620</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>21813</v>
+        <v>21836</v>
       </c>
       <c r="D40" t="n">
-        <v>26856566</v>
+        <v>26876126</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7792</v>
+        <v>7798</v>
       </c>
       <c r="D46" t="n">
-        <v>11445460</v>
+        <v>11454460</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3830</v>
+        <v>3831</v>
       </c>
       <c r="D48" t="n">
-        <v>5543655</v>
+        <v>5545155</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D51" t="n">
-        <v>822566</v>
+        <v>827066</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>8125</v>
+        <v>8132</v>
       </c>
       <c r="D52" t="n">
-        <v>10372127</v>
+        <v>10377641</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2778</v>
+        <v>2779</v>
       </c>
       <c r="D56" t="n">
-        <v>4041303</v>
+        <v>4042043</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="D58" t="n">
-        <v>1441052</v>
+        <v>1443584</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D60" t="n">
-        <v>349961</v>
+        <v>351461</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>36060</v>
+        <v>36089</v>
       </c>
       <c r="D61" t="n">
-        <v>46425867</v>
+        <v>46464294</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>13128</v>
+        <v>13144</v>
       </c>
       <c r="D66" t="n">
-        <v>19253835</v>
+        <v>19277835</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5147</v>
+        <v>5153</v>
       </c>
       <c r="D68" t="n">
-        <v>7443815</v>
+        <v>7452815</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>46149</v>
+        <v>46187</v>
       </c>
       <c r="D74" t="n">
-        <v>59016174</v>
+        <v>59055149</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4078,10 +4078,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>18097</v>
+        <v>18104</v>
       </c>
       <c r="D78" t="n">
-        <v>26513305</v>
+        <v>26523304</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9317</v>
+        <v>9324</v>
       </c>
       <c r="D80" t="n">
-        <v>13451549</v>
+        <v>13460833</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="D84" t="n">
-        <v>1114180</v>
+        <v>1118223</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>24868</v>
+        <v>24901</v>
       </c>
       <c r="D85" t="n">
-        <v>31354563</v>
+        <v>31390628</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8674</v>
+        <v>8676</v>
       </c>
       <c r="D89" t="n">
-        <v>12732886</v>
+        <v>12735886</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4891</v>
+        <v>4895</v>
       </c>
       <c r="D91" t="n">
-        <v>7069638</v>
+        <v>7074639</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D93" t="n">
-        <v>1060315</v>
+        <v>1061815</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>21917</v>
+        <v>21931</v>
       </c>
       <c r="D94" t="n">
-        <v>27515519</v>
+        <v>27531701</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -5038,10 +5038,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9143</v>
+        <v>9149</v>
       </c>
       <c r="D98" t="n">
-        <v>13384205</v>
+        <v>13393205</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -5278,10 +5278,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D103" t="n">
-        <v>340301</v>
+        <v>341301</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>81430</v>
+        <v>81519</v>
       </c>
       <c r="D105" t="n">
-        <v>104363624</v>
+        <v>104466700</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5614,10 +5614,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D110" t="n">
-        <v>221280</v>
+        <v>222780</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>30561</v>
+        <v>30573</v>
       </c>
       <c r="D112" t="n">
-        <v>44846873</v>
+        <v>44864473</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20777</v>
+        <v>20797</v>
       </c>
       <c r="D114" t="n">
-        <v>29982194</v>
+        <v>30009159</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -5950,10 +5950,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D117" t="n">
-        <v>966767</v>
+        <v>969767</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="D121" t="n">
-        <v>2645883</v>
+        <v>2647383</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>27646</v>
+        <v>27666</v>
       </c>
       <c r="D122" t="n">
-        <v>36487611</v>
+        <v>36514011</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>9857</v>
+        <v>9863</v>
       </c>
       <c r="D126" t="n">
-        <v>14455979</v>
+        <v>14464979</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3259</v>
+        <v>3263</v>
       </c>
       <c r="D128" t="n">
-        <v>4739256</v>
+        <v>4744157</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6622,10 +6622,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D131" t="n">
-        <v>488982</v>
+        <v>491802</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15708</v>
+        <v>15722</v>
       </c>
       <c r="D132" t="n">
-        <v>19549614</v>
+        <v>19564614</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6814,10 +6814,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7750</v>
+        <v>7754</v>
       </c>
       <c r="D135" t="n">
-        <v>11341635</v>
+        <v>11347635</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2209</v>
+        <v>2210</v>
       </c>
       <c r="D137" t="n">
-        <v>3154110</v>
+        <v>3155610</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>13506</v>
+        <v>13514</v>
       </c>
       <c r="D142" t="n">
-        <v>16880085</v>
+        <v>16887463</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6237</v>
+        <v>6239</v>
       </c>
       <c r="D146" t="n">
-        <v>9137755</v>
+        <v>9140755</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D150" t="n">
-        <v>153790</v>
+        <v>155290</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7582,10 +7582,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D151" t="n">
-        <v>504908</v>
+        <v>506408</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7630,10 +7630,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>5976</v>
+        <v>5978</v>
       </c>
       <c r="D152" t="n">
-        <v>7309862</v>
+        <v>7311632</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D156" t="n">
-        <v>974327</v>
+        <v>975827</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7426</v>
+        <v>7430</v>
       </c>
       <c r="D160" t="n">
-        <v>9209161</v>
+        <v>9212472</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>2848</v>
+        <v>2850</v>
       </c>
       <c r="D163" t="n">
-        <v>4175958</v>
+        <v>4178958</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D164" t="n">
-        <v>2009932</v>
+        <v>2011432</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5604</v>
+        <v>5606</v>
       </c>
       <c r="D168" t="n">
-        <v>7055122</v>
+        <v>7056757</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>15944</v>
+        <v>15952</v>
       </c>
       <c r="D178" t="n">
-        <v>20034454</v>
+        <v>20043666</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6382</v>
+        <v>6389</v>
       </c>
       <c r="D183" t="n">
-        <v>9322294</v>
+        <v>9332359</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D186" t="n">
-        <v>738655</v>
+        <v>740155</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3061</v>
+        <v>3064</v>
       </c>
       <c r="D188" t="n">
-        <v>3845491</v>
+        <v>3846137</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D190" t="n">
-        <v>2152242</v>
+        <v>2153742</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9694,10 +9694,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D195" t="n">
-        <v>68525</v>
+        <v>70025</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9195</v>
+        <v>9199</v>
       </c>
       <c r="D196" t="n">
-        <v>11482026</v>
+        <v>11486616</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>3426</v>
+        <v>3429</v>
       </c>
       <c r="D200" t="n">
-        <v>5033576</v>
+        <v>5038076</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>1610</v>
+        <v>1612</v>
       </c>
       <c r="D201" t="n">
-        <v>2321680</v>
+        <v>2324680</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10126,10 +10126,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D204" t="n">
-        <v>296097</v>
+        <v>297597</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>17227</v>
+        <v>17237</v>
       </c>
       <c r="D205" t="n">
-        <v>21518714</v>
+        <v>21531557</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>7678</v>
+        <v>7682</v>
       </c>
       <c r="D209" t="n">
-        <v>11275801</v>
+        <v>11280996</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D211" t="n">
-        <v>394905</v>
+        <v>395577</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>26095</v>
+        <v>26109</v>
       </c>
       <c r="D213" t="n">
-        <v>32919425</v>
+        <v>32931061</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>10483</v>
+        <v>10487</v>
       </c>
       <c r="D217" t="n">
-        <v>15310852</v>
+        <v>15315853</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2632</v>
+        <v>2635</v>
       </c>
       <c r="D219" t="n">
-        <v>3795522</v>
+        <v>3800022</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D222" t="n">
-        <v>843266</v>
+        <v>844766</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>28428</v>
+        <v>28456</v>
       </c>
       <c r="D223" t="n">
-        <v>35885586</v>
+        <v>35915098</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>14720</v>
+        <v>14722</v>
       </c>
       <c r="D228" t="n">
-        <v>21599928</v>
+        <v>21602928</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2650</v>
+        <v>2655</v>
       </c>
       <c r="D230" t="n">
-        <v>3804675</v>
+        <v>3812175</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D232" t="n">
-        <v>509584</v>
+        <v>511084</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D233" t="n">
-        <v>1019228</v>
+        <v>1022228</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24237</v>
+        <v>24254</v>
       </c>
       <c r="D234" t="n">
-        <v>30577910</v>
+        <v>30595219</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D238" t="n">
-        <v>330775</v>
+        <v>332275</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>11167</v>
+        <v>11170</v>
       </c>
       <c r="D240" t="n">
-        <v>16371249</v>
+        <v>16375749</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2505</v>
+        <v>2506</v>
       </c>
       <c r="D242" t="n">
-        <v>3580847</v>
+        <v>3582347</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12094,10 +12094,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D245" t="n">
-        <v>621324</v>
+        <v>622824</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -12142,10 +12142,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>7862</v>
+        <v>7866</v>
       </c>
       <c r="D246" t="n">
-        <v>9837056</v>
+        <v>9840680</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>2697</v>
+        <v>2700</v>
       </c>
       <c r="D250" t="n">
-        <v>3958650</v>
+        <v>3963150</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12478,10 +12478,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D253" t="n">
-        <v>1452615</v>
+        <v>1454115</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>9791</v>
+        <v>9796</v>
       </c>
       <c r="D256" t="n">
-        <v>12488092</v>
+        <v>12493927</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="D262" t="n">
-        <v>3140102</v>
+        <v>3141602</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>5532</v>
+        <v>5540</v>
       </c>
       <c r="D265" t="n">
-        <v>6858043</v>
+        <v>6870043</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13438,10 +13438,10 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D273" t="n">
-        <v>230656</v>
+        <v>232156</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -13486,10 +13486,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>19041</v>
+        <v>19056</v>
       </c>
       <c r="D274" t="n">
-        <v>24062909</v>
+        <v>24079422</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>7918</v>
+        <v>7924</v>
       </c>
       <c r="D278" t="n">
-        <v>11609705</v>
+        <v>11618608</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>2492</v>
+        <v>2493</v>
       </c>
       <c r="D280" t="n">
-        <v>3579559</v>
+        <v>3581059</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D283" t="n">
-        <v>650745</v>
+        <v>652245</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>16578</v>
+        <v>16594</v>
       </c>
       <c r="D285" t="n">
-        <v>20539922</v>
+        <v>20556883</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>7178</v>
+        <v>7181</v>
       </c>
       <c r="D289" t="n">
-        <v>10528612</v>
+        <v>10533112</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>9331</v>
+        <v>9342</v>
       </c>
       <c r="D294" t="n">
-        <v>11727079</v>
+        <v>11739335</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>3910</v>
+        <v>3911</v>
       </c>
       <c r="D298" t="n">
-        <v>5722832</v>
+        <v>5724332</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D299" t="n">
-        <v>1811009</v>
+        <v>1812509</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>9186</v>
+        <v>9193</v>
       </c>
       <c r="D304" t="n">
-        <v>11996036</v>
+        <v>12003485</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>3735</v>
+        <v>3739</v>
       </c>
       <c r="D308" t="n">
-        <v>5460349</v>
+        <v>5466349</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>11053</v>
+        <v>11059</v>
       </c>
       <c r="D312" t="n">
-        <v>14515336</v>
+        <v>14523278</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2696</v>
+        <v>2702</v>
       </c>
       <c r="D318" t="n">
-        <v>3909138</v>
+        <v>3918138</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D320" t="n">
-        <v>233286</v>
+        <v>234786</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6801</v>
+        <v>6808</v>
       </c>
       <c r="D321" t="n">
-        <v>8409391</v>
+        <v>8416301</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D328" t="n">
-        <v>1128842</v>
+        <v>1130275</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>7512</v>
+        <v>7522</v>
       </c>
       <c r="D331" t="n">
-        <v>9404046</v>
+        <v>9418179</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16462,10 +16462,10 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>3126</v>
+        <v>3127</v>
       </c>
       <c r="D336" t="n">
-        <v>4567315</v>
+        <v>4568815</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="D337" t="n">
-        <v>1845695</v>
+        <v>1848361</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>31944</v>
+        <v>31982</v>
       </c>
       <c r="D340" t="n">
-        <v>40132719</v>
+        <v>40177718</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>16518</v>
+        <v>16524</v>
       </c>
       <c r="D346" t="n">
-        <v>24154379</v>
+        <v>24161739</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>8029</v>
+        <v>8042</v>
       </c>
       <c r="D349" t="n">
-        <v>11563034</v>
+        <v>11582205</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D350" t="n">
-        <v>914171</v>
+        <v>915671</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>3887</v>
+        <v>3893</v>
       </c>
       <c r="D352" t="n">
-        <v>4842945</v>
+        <v>4850212</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D355" t="n">
-        <v>2203157</v>
+        <v>2204657</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>19354</v>
+        <v>19368</v>
       </c>
       <c r="D360" t="n">
-        <v>24134344</v>
+        <v>24150044</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>9895</v>
+        <v>9901</v>
       </c>
       <c r="D364" t="n">
-        <v>14507235</v>
+        <v>14516235</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>4733</v>
+        <v>4737</v>
       </c>
       <c r="D366" t="n">
-        <v>6844409</v>
+        <v>6850409</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D367" t="n">
-        <v>868460</v>
+        <v>871460</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -17998,10 +17998,10 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D368" t="n">
-        <v>500984</v>
+        <v>502484</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>13902</v>
+        <v>13917</v>
       </c>
       <c r="D369" t="n">
-        <v>17393938</v>
+        <v>17408534</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>6436</v>
+        <v>6441</v>
       </c>
       <c r="D373" t="n">
-        <v>9422958</v>
+        <v>9430458</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18334,10 +18334,10 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>2478</v>
+        <v>2481</v>
       </c>
       <c r="D375" t="n">
-        <v>3561087</v>
+        <v>3565183</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>17963</v>
+        <v>17981</v>
       </c>
       <c r="D378" t="n">
-        <v>22405293</v>
+        <v>22423439</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>7136</v>
+        <v>7139</v>
       </c>
       <c r="D382" t="n">
-        <v>10489215</v>
+        <v>10493715</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>2834</v>
+        <v>2836</v>
       </c>
       <c r="D384" t="n">
-        <v>4123192</v>
+        <v>4125151</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D387" t="n">
-        <v>555654</v>
+        <v>557154</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>4088</v>
+        <v>4090</v>
       </c>
       <c r="D388" t="n">
-        <v>5129292</v>
+        <v>5132292</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>22248</v>
+        <v>22268</v>
       </c>
       <c r="D395" t="n">
-        <v>27599752</v>
+        <v>27623557</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>9360</v>
+        <v>9364</v>
       </c>
       <c r="D398" t="n">
-        <v>13779417</v>
+        <v>13785017</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>6203</v>
+        <v>6207</v>
       </c>
       <c r="D400" t="n">
-        <v>9023736</v>
+        <v>9028491</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>11130</v>
+        <v>11131</v>
       </c>
       <c r="D403" t="n">
-        <v>13721686</v>
+        <v>13722637</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1840</v>
+        <v>1842</v>
       </c>
       <c r="D410" t="n">
-        <v>2672364</v>
+        <v>2675364</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>32054</v>
+        <v>32126</v>
       </c>
       <c r="D413" t="n">
-        <v>43432262</v>
+        <v>43525558</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>7792</v>
+        <v>7802</v>
       </c>
       <c r="D417" t="n">
-        <v>11457470</v>
+        <v>11472470</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>7088</v>
+        <v>7098</v>
       </c>
       <c r="D419" t="n">
-        <v>10275127</v>
+        <v>10290127</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>8791</v>
+        <v>8823</v>
       </c>
       <c r="D423" t="n">
-        <v>12200726</v>
+        <v>12245320</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2210</v>
+        <v>2218</v>
       </c>
       <c r="D425" t="n">
-        <v>3256352</v>
+        <v>3267382</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>2979</v>
+        <v>2988</v>
       </c>
       <c r="D427" t="n">
-        <v>4351241</v>
+        <v>4364741</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D430" t="n">
-        <v>247086</v>
+        <v>248586</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21022,10 +21022,10 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>11019</v>
+        <v>11022</v>
       </c>
       <c r="D431" t="n">
-        <v>13603731</v>
+        <v>13608231</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>3785</v>
+        <v>3786</v>
       </c>
       <c r="D434" t="n">
-        <v>5555841</v>
+        <v>5556304</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>1868</v>
+        <v>1871</v>
       </c>
       <c r="D436" t="n">
-        <v>2680227</v>
+        <v>2684727</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>62838</v>
+        <v>62901</v>
       </c>
       <c r="D439" t="n">
-        <v>77883850</v>
+        <v>77955041</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D441" t="n">
-        <v>38487</v>
+        <v>39757</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>24913</v>
+        <v>24916</v>
       </c>
       <c r="D443" t="n">
-        <v>36518620</v>
+        <v>36523120</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>12907</v>
+        <v>12923</v>
       </c>
       <c r="D445" t="n">
-        <v>18716968</v>
+        <v>18740027</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="D449" t="n">
-        <v>1458294</v>
+        <v>1460899</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>18881</v>
+        <v>18889</v>
       </c>
       <c r="D451" t="n">
-        <v>23868117</v>
+        <v>23878757</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>7700</v>
+        <v>7702</v>
       </c>
       <c r="D455" t="n">
-        <v>11302393</v>
+        <v>11305393</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>4851</v>
+        <v>4856</v>
       </c>
       <c r="D457" t="n">
-        <v>7039422</v>
+        <v>7046922</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>32195</v>
+        <v>32218</v>
       </c>
       <c r="D460" t="n">
-        <v>39355427</v>
+        <v>39380080</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>11446</v>
+        <v>11448</v>
       </c>
       <c r="D464" t="n">
-        <v>16747270</v>
+        <v>16749849</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>4902</v>
+        <v>4905</v>
       </c>
       <c r="D466" t="n">
-        <v>7113393</v>
+        <v>7116582</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D467" t="n">
-        <v>522044</v>
+        <v>523484</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>14386</v>
+        <v>14395</v>
       </c>
       <c r="D469" t="n">
-        <v>17592872</v>
+        <v>17602746</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23182,10 +23182,10 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>2067</v>
+        <v>2069</v>
       </c>
       <c r="D476" t="n">
-        <v>2981283</v>
+        <v>2984283</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>35933</v>
+        <v>35970</v>
       </c>
       <c r="D479" t="n">
-        <v>46821562</v>
+        <v>46870036</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>13546</v>
+        <v>13552</v>
       </c>
       <c r="D483" t="n">
-        <v>19929300</v>
+        <v>19938300</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>11975</v>
+        <v>11987</v>
       </c>
       <c r="D485" t="n">
-        <v>17476788</v>
+        <v>17494788</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D487" t="n">
-        <v>424726</v>
+        <v>426226</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>62242</v>
+        <v>62307</v>
       </c>
       <c r="D488" t="n">
-        <v>82418291</v>
+        <v>82499286</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>23081</v>
+        <v>23099</v>
       </c>
       <c r="D493" t="n">
-        <v>33867084</v>
+        <v>33893984</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>22396</v>
+        <v>22419</v>
       </c>
       <c r="D495" t="n">
-        <v>32516840</v>
+        <v>32549416</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>150578</v>
+        <v>150775</v>
       </c>
       <c r="D499" t="n">
-        <v>198052522</v>
+        <v>198306113</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>81520</v>
+        <v>81585</v>
       </c>
       <c r="D506" t="n">
-        <v>119762852</v>
+        <v>119852991</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>59923</v>
+        <v>60006</v>
       </c>
       <c r="D509" t="n">
-        <v>86984598</v>
+        <v>87103422</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1071</v>
+        <v>1076</v>
       </c>
       <c r="D511" t="n">
-        <v>1527607</v>
+        <v>1534107</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>2774</v>
+        <v>2778</v>
       </c>
       <c r="D513" t="n">
-        <v>3926678</v>
+        <v>3932678</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>41080</v>
+        <v>41168</v>
       </c>
       <c r="D515" t="n">
-        <v>53397909</v>
+        <v>53512578</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>15224</v>
+        <v>15240</v>
       </c>
       <c r="D520" t="n">
-        <v>22364249</v>
+        <v>22385856</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>12911</v>
+        <v>12926</v>
       </c>
       <c r="D522" t="n">
-        <v>18714398</v>
+        <v>18735030</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>66077</v>
+        <v>66137</v>
       </c>
       <c r="D527" t="n">
-        <v>88810669</v>
+        <v>88888705</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>23284</v>
+        <v>23306</v>
       </c>
       <c r="D531" t="n">
-        <v>34358402</v>
+        <v>34389681</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>24054</v>
+        <v>24074</v>
       </c>
       <c r="D533" t="n">
-        <v>35206129</v>
+        <v>35234416</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="D536" t="n">
-        <v>1214969</v>
+        <v>1217969</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>54978</v>
+        <v>55027</v>
       </c>
       <c r="D537" t="n">
-        <v>72921520</v>
+        <v>72983757</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>17760</v>
+        <v>17770</v>
       </c>
       <c r="D542" t="n">
-        <v>26096526</v>
+        <v>26111526</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>18293</v>
+        <v>18302</v>
       </c>
       <c r="D544" t="n">
-        <v>26590367</v>
+        <v>26603867</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26542,10 +26542,10 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D546" t="n">
-        <v>877253</v>
+        <v>877715</v>
       </c>
       <c r="E546" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>41505</v>
+        <v>41550</v>
       </c>
       <c r="D547" t="n">
-        <v>55118312</v>
+        <v>55175648</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>14204</v>
+        <v>14212</v>
       </c>
       <c r="D551" t="n">
-        <v>20949169</v>
+        <v>20961121</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>14382</v>
+        <v>14398</v>
       </c>
       <c r="D553" t="n">
-        <v>20885178</v>
+        <v>20908148</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D554" t="n">
-        <v>245479</v>
+        <v>251479</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>41269</v>
+        <v>41301</v>
       </c>
       <c r="D556" t="n">
-        <v>53498484</v>
+        <v>53542148</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>16179</v>
+        <v>16191</v>
       </c>
       <c r="D560" t="n">
-        <v>23738426</v>
+        <v>23756426</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>12984</v>
+        <v>12998</v>
       </c>
       <c r="D562" t="n">
-        <v>18779347</v>
+        <v>18798447</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27406,10 +27406,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D564" t="n">
-        <v>372060</v>
+        <v>374160</v>
       </c>
       <c r="E564" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D565" t="n">
-        <v>495767</v>
+        <v>497267</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>43790</v>
+        <v>43856</v>
       </c>
       <c r="D566" t="n">
-        <v>58473348</v>
+        <v>58552963</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>13896</v>
+        <v>13905</v>
       </c>
       <c r="D572" t="n">
-        <v>20382249</v>
+        <v>20395249</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>3696</v>
+        <v>3702</v>
       </c>
       <c r="D573" t="n">
-        <v>5330140</v>
+        <v>5338019</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27982,10 +27982,10 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D576" t="n">
-        <v>565431</v>
+        <v>568431</v>
       </c>
       <c r="E576" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>17254</v>
+        <v>17264</v>
       </c>
       <c r="D579" t="n">
-        <v>22797660</v>
+        <v>22809991</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>7046</v>
+        <v>7059</v>
       </c>
       <c r="D583" t="n">
-        <v>10247481</v>
+        <v>10266288</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28414,10 +28414,10 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>4909</v>
+        <v>4913</v>
       </c>
       <c r="D585" t="n">
-        <v>7066936</v>
+        <v>7071877</v>
       </c>
       <c r="E585" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>15353</v>
+        <v>15462</v>
       </c>
       <c r="D590" t="n">
-        <v>22279946</v>
+        <v>22435556</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>1737</v>
+        <v>1744</v>
       </c>
       <c r="D591" t="n">
-        <v>2584030</v>
+        <v>2593730</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>21973</v>
+        <v>21988</v>
       </c>
       <c r="D596" t="n">
-        <v>27570223</v>
+        <v>27588072</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>8977</v>
+        <v>8982</v>
       </c>
       <c r="D601" t="n">
-        <v>13153008</v>
+        <v>13158665</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29374,10 +29374,10 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D605" t="n">
-        <v>646439</v>
+        <v>647939</v>
       </c>
       <c r="E605" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>14613</v>
+        <v>14626</v>
       </c>
       <c r="D607" t="n">
-        <v>18322064</v>
+        <v>18339100</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>5780</v>
+        <v>5782</v>
       </c>
       <c r="D611" t="n">
-        <v>8489151</v>
+        <v>8492151</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>2668</v>
+        <v>2669</v>
       </c>
       <c r="D613" t="n">
-        <v>3845587</v>
+        <v>3847087</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>13734</v>
+        <v>13737</v>
       </c>
       <c r="D616" t="n">
-        <v>17348881</v>
+        <v>17352334</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -30094,10 +30094,10 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>5218</v>
+        <v>5221</v>
       </c>
       <c r="D620" t="n">
-        <v>7648220</v>
+        <v>7652720</v>
       </c>
       <c r="E620" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1159</v>
+        <v>1162</v>
       </c>
       <c r="D621" t="n">
-        <v>1678855</v>
+        <v>1683355</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D624" t="n">
-        <v>364466</v>
+        <v>365966</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>7485</v>
+        <v>7495</v>
       </c>
       <c r="D625" t="n">
-        <v>9629769</v>
+        <v>9641387</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30622,10 +30622,10 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D631" t="n">
-        <v>1220614</v>
+        <v>1222114</v>
       </c>
       <c r="E631" t="inlineStr">
         <is>
@@ -30670,10 +30670,10 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D632" t="n">
-        <v>248518</v>
+        <v>250018</v>
       </c>
       <c r="E632" t="inlineStr">
         <is>
@@ -30718,10 +30718,10 @@
         </is>
       </c>
       <c r="C633" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D633" t="n">
-        <v>183956</v>
+        <v>186825</v>
       </c>
       <c r="E633" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>28752</v>
+        <v>28767</v>
       </c>
       <c r="D634" t="n">
-        <v>35412814</v>
+        <v>35431583</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>11001</v>
+        <v>11005</v>
       </c>
       <c r="D638" t="n">
-        <v>16141462</v>
+        <v>16147115</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4814</v>
+        <v>4818</v>
       </c>
       <c r="D640" t="n">
-        <v>6985323</v>
+        <v>6990353</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>11283</v>
+        <v>11294</v>
       </c>
       <c r="D644" t="n">
-        <v>13676576</v>
+        <v>13689706</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>28237</v>
+        <v>28263</v>
       </c>
       <c r="D654" t="n">
-        <v>35109819</v>
+        <v>35140545</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>10724</v>
+        <v>10730</v>
       </c>
       <c r="D658" t="n">
-        <v>15757964</v>
+        <v>15765836</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>3070</v>
+        <v>3074</v>
       </c>
       <c r="D660" t="n">
-        <v>4426977</v>
+        <v>4432477</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D663" t="n">
-        <v>662175</v>
+        <v>666675</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>7474</v>
+        <v>7481</v>
       </c>
       <c r="D664" t="n">
-        <v>9483499</v>
+        <v>9492436</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="D666" t="n">
-        <v>3861707</v>
+        <v>3864665</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32398,10 +32398,10 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="D668" t="n">
-        <v>1867872</v>
+        <v>1870872</v>
       </c>
       <c r="E668" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3768</v>
+        <v>3770</v>
       </c>
       <c r="D672" t="n">
-        <v>4566767</v>
+        <v>4569767</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32926,10 +32926,10 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D679" t="n">
-        <v>171745</v>
+        <v>174745</v>
       </c>
       <c r="E679" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D680" t="n">
-        <v>204932</v>
+        <v>206432</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>9283</v>
+        <v>9296</v>
       </c>
       <c r="D681" t="n">
-        <v>11585981</v>
+        <v>11599362</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>3463</v>
+        <v>3464</v>
       </c>
       <c r="D685" t="n">
-        <v>5105017</v>
+        <v>5106517</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D686" t="n">
-        <v>1077102</v>
+        <v>1078602</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D689" t="n">
-        <v>379569</v>
+        <v>381069</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>19167</v>
+        <v>19187</v>
       </c>
       <c r="D690" t="n">
-        <v>23462813</v>
+        <v>23481704</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>5699</v>
+        <v>5703</v>
       </c>
       <c r="D694" t="n">
-        <v>8323980</v>
+        <v>8329980</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>2239</v>
+        <v>2242</v>
       </c>
       <c r="D696" t="n">
-        <v>3221514</v>
+        <v>3226014</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>74156</v>
+        <v>74249</v>
       </c>
       <c r="D701" t="n">
-        <v>93360823</v>
+        <v>93471953</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>26448</v>
+        <v>26463</v>
       </c>
       <c r="D706" t="n">
-        <v>38836419</v>
+        <v>38853677</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>13110</v>
+        <v>13123</v>
       </c>
       <c r="D709" t="n">
-        <v>18909654</v>
+        <v>18928093</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="D712" t="n">
-        <v>2777047</v>
+        <v>2778547</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>1189</v>
+        <v>1196</v>
       </c>
       <c r="D714" t="n">
-        <v>1659039</v>
+        <v>1669243</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>11098</v>
+        <v>11133</v>
       </c>
       <c r="D715" t="n">
-        <v>13577363</v>
+        <v>13624063</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>4091</v>
+        <v>4095</v>
       </c>
       <c r="D718" t="n">
-        <v>5984583</v>
+        <v>5990583</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>1486</v>
+        <v>1488</v>
       </c>
       <c r="D720" t="n">
-        <v>2141500</v>
+        <v>2144500</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -35038,10 +35038,10 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>17519</v>
+        <v>17537</v>
       </c>
       <c r="D723" t="n">
-        <v>21610384</v>
+        <v>21633227</v>
       </c>
       <c r="E723" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>6826</v>
+        <v>6831</v>
       </c>
       <c r="D727" t="n">
-        <v>9977829</v>
+        <v>9985329</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35326,10 +35326,10 @@
         </is>
       </c>
       <c r="C729" t="n">
-        <v>2173</v>
+        <v>2176</v>
       </c>
       <c r="D729" t="n">
-        <v>3115538</v>
+        <v>3120038</v>
       </c>
       <c r="E729" t="inlineStr">
         <is>
@@ -35422,10 +35422,10 @@
         </is>
       </c>
       <c r="C731" t="n">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D731" t="n">
-        <v>452489</v>
+        <v>453989</v>
       </c>
       <c r="E731" t="inlineStr">
         <is>
@@ -35470,10 +35470,10 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D732" t="n">
-        <v>450219</v>
+        <v>451719</v>
       </c>
       <c r="E732" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>11461</v>
+        <v>11473</v>
       </c>
       <c r="D734" t="n">
-        <v>14154539</v>
+        <v>14167854</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35758,10 +35758,10 @@
         </is>
       </c>
       <c r="C738" t="n">
-        <v>4228</v>
+        <v>4229</v>
       </c>
       <c r="D738" t="n">
-        <v>6198245</v>
+        <v>6199745</v>
       </c>
       <c r="E738" t="inlineStr">
         <is>
@@ -35854,10 +35854,10 @@
         </is>
       </c>
       <c r="C740" t="n">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D740" t="n">
-        <v>2317034</v>
+        <v>2318534</v>
       </c>
       <c r="E740" t="inlineStr">
         <is>
@@ -35902,10 +35902,10 @@
         </is>
       </c>
       <c r="C741" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D741" t="n">
-        <v>314713</v>
+        <v>316213</v>
       </c>
       <c r="E741" t="inlineStr">
         <is>
@@ -35950,10 +35950,10 @@
         </is>
       </c>
       <c r="C742" t="n">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D742" t="n">
-        <v>426423</v>
+        <v>428909</v>
       </c>
       <c r="E742" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>29435</v>
+        <v>29454</v>
       </c>
       <c r="D743" t="n">
-        <v>36586956</v>
+        <v>36609190</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36190,10 +36190,10 @@
         </is>
       </c>
       <c r="C747" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D747" t="n">
-        <v>166395</v>
+        <v>167895</v>
       </c>
       <c r="E747" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>12682</v>
+        <v>12688</v>
       </c>
       <c r="D748" t="n">
-        <v>18561366</v>
+        <v>18569699</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36334,10 +36334,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>4199</v>
+        <v>4204</v>
       </c>
       <c r="D750" t="n">
-        <v>5999119</v>
+        <v>6006619</v>
       </c>
       <c r="E750" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D753" t="n">
-        <v>952004</v>
+        <v>953504</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>12272</v>
+        <v>12277</v>
       </c>
       <c r="D755" t="n">
-        <v>15194684</v>
+        <v>15200121</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36718,10 +36718,10 @@
         </is>
       </c>
       <c r="C758" t="n">
-        <v>4648</v>
+        <v>4650</v>
       </c>
       <c r="D758" t="n">
-        <v>6793356</v>
+        <v>6796356</v>
       </c>
       <c r="E758" t="inlineStr">
         <is>
@@ -36862,10 +36862,10 @@
         </is>
       </c>
       <c r="C761" t="n">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D761" t="n">
-        <v>519162</v>
+        <v>522162</v>
       </c>
       <c r="E761" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>6690</v>
+        <v>6698</v>
       </c>
       <c r="D762" t="n">
-        <v>7864848</v>
+        <v>7872150</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37102,10 +37102,10 @@
         </is>
       </c>
       <c r="C766" t="n">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="D766" t="n">
-        <v>2470873</v>
+        <v>2472153</v>
       </c>
       <c r="E766" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="D767" t="n">
-        <v>1453344</v>
+        <v>1454844</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37246,10 +37246,10 @@
         </is>
       </c>
       <c r="C769" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D769" t="n">
-        <v>207515</v>
+        <v>209935</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>16722</v>
+        <v>16747</v>
       </c>
       <c r="D770" t="n">
-        <v>20285128</v>
+        <v>20319218</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>5519</v>
+        <v>5524</v>
       </c>
       <c r="D775" t="n">
-        <v>8086587</v>
+        <v>8094086</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37630,10 +37630,10 @@
         </is>
       </c>
       <c r="C777" t="n">
-        <v>3387</v>
+        <v>3388</v>
       </c>
       <c r="D777" t="n">
-        <v>4947277</v>
+        <v>4948222</v>
       </c>
       <c r="E777" t="inlineStr">
         <is>
@@ -37726,10 +37726,10 @@
         </is>
       </c>
       <c r="C779" t="n">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D779" t="n">
-        <v>527612</v>
+        <v>529112</v>
       </c>
       <c r="E779" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>11327</v>
+        <v>11345</v>
       </c>
       <c r="D781" t="n">
-        <v>14350175</v>
+        <v>14369076</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -38014,10 +38014,10 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>3947</v>
+        <v>3948</v>
       </c>
       <c r="D785" t="n">
-        <v>5771483</v>
+        <v>5772983</v>
       </c>
       <c r="E785" t="inlineStr">
         <is>
@@ -38110,10 +38110,10 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="D787" t="n">
-        <v>1809412</v>
+        <v>1812412</v>
       </c>
       <c r="E787" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>32009</v>
+        <v>32037</v>
       </c>
       <c r="D791" t="n">
-        <v>39488834</v>
+        <v>39518834</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38494,10 +38494,10 @@
         </is>
       </c>
       <c r="C795" t="n">
-        <v>13153</v>
+        <v>13159</v>
       </c>
       <c r="D795" t="n">
-        <v>19245934</v>
+        <v>19253227</v>
       </c>
       <c r="E795" t="inlineStr">
         <is>
@@ -38590,10 +38590,10 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>6019</v>
+        <v>6023</v>
       </c>
       <c r="D797" t="n">
-        <v>8698230</v>
+        <v>8704078</v>
       </c>
       <c r="E797" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D798" t="n">
-        <v>728817</v>
+        <v>731569</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38734,10 +38734,10 @@
         </is>
       </c>
       <c r="C800" t="n">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D800" t="n">
-        <v>907773</v>
+        <v>910773</v>
       </c>
       <c r="E800" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>7580</v>
+        <v>7590</v>
       </c>
       <c r="D801" t="n">
-        <v>9373636</v>
+        <v>9384537</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -39070,10 +39070,10 @@
         </is>
       </c>
       <c r="C807" t="n">
-        <v>2671</v>
+        <v>2676</v>
       </c>
       <c r="D807" t="n">
-        <v>3895984</v>
+        <v>3903484</v>
       </c>
       <c r="E807" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D808" t="n">
-        <v>1632938</v>
+        <v>1634438</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39166,10 +39166,10 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D809" t="n">
-        <v>537372</v>
+        <v>538872</v>
       </c>
       <c r="E809" t="inlineStr">
         <is>
@@ -39262,10 +39262,10 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>58581</v>
+        <v>58661</v>
       </c>
       <c r="D811" t="n">
-        <v>73224406</v>
+        <v>73327148</v>
       </c>
       <c r="E811" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>21082</v>
+        <v>21092</v>
       </c>
       <c r="D816" t="n">
-        <v>30845225</v>
+        <v>30859293</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>12555</v>
+        <v>12567</v>
       </c>
       <c r="D819" t="n">
-        <v>18123329</v>
+        <v>18140129</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39742,10 +39742,10 @@
         </is>
       </c>
       <c r="C821" t="n">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D821" t="n">
-        <v>644695</v>
+        <v>647695</v>
       </c>
       <c r="E821" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>1313</v>
+        <v>1316</v>
       </c>
       <c r="D824" t="n">
-        <v>1831685</v>
+        <v>1835325</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>11089</v>
+        <v>11104</v>
       </c>
       <c r="D825" t="n">
-        <v>13828181</v>
+        <v>13844329</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -40126,10 +40126,10 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>3900</v>
+        <v>3903</v>
       </c>
       <c r="D829" t="n">
-        <v>5671022</v>
+        <v>5674604</v>
       </c>
       <c r="E829" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>58273</v>
+        <v>58326</v>
       </c>
       <c r="D836" t="n">
-        <v>72056213</v>
+        <v>72119491</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>22267</v>
+        <v>22278</v>
       </c>
       <c r="D842" t="n">
-        <v>32672826</v>
+        <v>32688308</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>14269</v>
+        <v>14278</v>
       </c>
       <c r="D844" t="n">
-        <v>20657814</v>
+        <v>20670411</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>1233</v>
+        <v>1238</v>
       </c>
       <c r="D847" t="n">
-        <v>1717786</v>
+        <v>1720686</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>7710</v>
+        <v>7716</v>
       </c>
       <c r="D849" t="n">
-        <v>9462879</v>
+        <v>9467513</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41182,10 +41182,10 @@
         </is>
       </c>
       <c r="C851" t="n">
-        <v>2565</v>
+        <v>2567</v>
       </c>
       <c r="D851" t="n">
-        <v>3735062</v>
+        <v>3738062</v>
       </c>
       <c r="E851" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D853" t="n">
-        <v>429097</v>
+        <v>432097</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>3584</v>
+        <v>3591</v>
       </c>
       <c r="D855" t="n">
-        <v>4633813</v>
+        <v>4642111</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41518,10 +41518,10 @@
         </is>
       </c>
       <c r="C858" t="n">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D858" t="n">
-        <v>1705582</v>
+        <v>1707082</v>
       </c>
       <c r="E858" t="inlineStr">
         <is>
@@ -41614,10 +41614,10 @@
         </is>
       </c>
       <c r="C860" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D860" t="n">
-        <v>531939</v>
+        <v>532778</v>
       </c>
       <c r="E860" t="inlineStr">
         <is>
@@ -41662,10 +41662,10 @@
         </is>
       </c>
       <c r="C861" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D861" t="n">
-        <v>189582</v>
+        <v>192582</v>
       </c>
       <c r="E861" t="inlineStr">
         <is>
@@ -41758,10 +41758,10 @@
         </is>
       </c>
       <c r="C863" t="n">
-        <v>22271</v>
+        <v>22292</v>
       </c>
       <c r="D863" t="n">
-        <v>27903757</v>
+        <v>27930984</v>
       </c>
       <c r="E863" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>7729</v>
+        <v>7735</v>
       </c>
       <c r="D867" t="n">
-        <v>11282256</v>
+        <v>11291256</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -42046,10 +42046,10 @@
         </is>
       </c>
       <c r="C869" t="n">
-        <v>4610</v>
+        <v>4616</v>
       </c>
       <c r="D869" t="n">
-        <v>6665151</v>
+        <v>6674151</v>
       </c>
       <c r="E869" t="inlineStr">
         <is>
@@ -42142,10 +42142,10 @@
         </is>
       </c>
       <c r="C871" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D871" t="n">
-        <v>536062</v>
+        <v>537517</v>
       </c>
       <c r="E871" t="inlineStr">
         <is>
@@ -42190,10 +42190,10 @@
         </is>
       </c>
       <c r="C872" t="n">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D872" t="n">
-        <v>594055</v>
+        <v>597055</v>
       </c>
       <c r="E872" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>14461</v>
+        <v>14471</v>
       </c>
       <c r="D874" t="n">
-        <v>17437648</v>
+        <v>17450843</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="D880" t="n">
-        <v>3380003</v>
+        <v>3381503</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>9739</v>
+        <v>9749</v>
       </c>
       <c r="D884" t="n">
-        <v>11968265</v>
+        <v>11977889</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42910,10 +42910,10 @@
         </is>
       </c>
       <c r="C887" t="n">
-        <v>3340</v>
+        <v>3341</v>
       </c>
       <c r="D887" t="n">
-        <v>4893738</v>
+        <v>4895238</v>
       </c>
       <c r="E887" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>44392</v>
+        <v>44432</v>
       </c>
       <c r="D891" t="n">
-        <v>55772445</v>
+        <v>55814146</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>20996</v>
+        <v>21009</v>
       </c>
       <c r="D896" t="n">
-        <v>30786188</v>
+        <v>30804498</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43438,10 +43438,10 @@
         </is>
       </c>
       <c r="C898" t="n">
-        <v>5871</v>
+        <v>5873</v>
       </c>
       <c r="D898" t="n">
-        <v>8459669</v>
+        <v>8462669</v>
       </c>
       <c r="E898" t="inlineStr">
         <is>
@@ -43582,10 +43582,10 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="D901" t="n">
-        <v>1286884</v>
+        <v>1294062</v>
       </c>
       <c r="E901" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>21140</v>
+        <v>21150</v>
       </c>
       <c r="D902" t="n">
-        <v>26308361</v>
+        <v>26319772</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43774,10 +43774,10 @@
         </is>
       </c>
       <c r="C905" t="n">
-        <v>9753</v>
+        <v>9756</v>
       </c>
       <c r="D905" t="n">
-        <v>14292369</v>
+        <v>14296027</v>
       </c>
       <c r="E905" t="inlineStr">
         <is>
@@ -43870,10 +43870,10 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>2267</v>
+        <v>2268</v>
       </c>
       <c r="D907" t="n">
-        <v>3248665</v>
+        <v>3250165</v>
       </c>
       <c r="E907" t="inlineStr">
         <is>
@@ -44014,10 +44014,10 @@
         </is>
       </c>
       <c r="C910" t="n">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D910" t="n">
-        <v>881850</v>
+        <v>884850</v>
       </c>
       <c r="E910" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>7010</v>
+        <v>7018</v>
       </c>
       <c r="D911" t="n">
-        <v>8813292</v>
+        <v>8821161</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>3010</v>
+        <v>3012</v>
       </c>
       <c r="D916" t="n">
-        <v>4433020</v>
+        <v>4435089</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44350,10 +44350,10 @@
         </is>
       </c>
       <c r="C917" t="n">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D917" t="n">
-        <v>910949</v>
+        <v>912449</v>
       </c>
       <c r="E917" t="inlineStr">
         <is>
@@ -44494,10 +44494,10 @@
         </is>
       </c>
       <c r="C920" t="n">
-        <v>12976</v>
+        <v>12984</v>
       </c>
       <c r="D920" t="n">
-        <v>16175450</v>
+        <v>16180267</v>
       </c>
       <c r="E920" t="inlineStr">
         <is>
@@ -44686,10 +44686,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>5236</v>
+        <v>5237</v>
       </c>
       <c r="D924" t="n">
-        <v>7651678</v>
+        <v>7652857</v>
       </c>
       <c r="E924" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>19248</v>
+        <v>19259</v>
       </c>
       <c r="D931" t="n">
-        <v>24049207</v>
+        <v>24062318</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45214,10 +45214,10 @@
         </is>
       </c>
       <c r="C935" t="n">
-        <v>10058</v>
+        <v>10061</v>
       </c>
       <c r="D935" t="n">
-        <v>14703076</v>
+        <v>14707576</v>
       </c>
       <c r="E935" t="inlineStr">
         <is>
@@ -45310,10 +45310,10 @@
         </is>
       </c>
       <c r="C937" t="n">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="D937" t="n">
-        <v>2961819</v>
+        <v>2963319</v>
       </c>
       <c r="E937" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>8595</v>
+        <v>8606</v>
       </c>
       <c r="D940" t="n">
-        <v>10727197</v>
+        <v>10737251</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45502,10 +45502,10 @@
         </is>
       </c>
       <c r="C941" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D941" t="n">
-        <v>4442</v>
+        <v>4916</v>
       </c>
       <c r="E941" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>3192</v>
+        <v>3195</v>
       </c>
       <c r="D945" t="n">
-        <v>4656134</v>
+        <v>4660634</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>66895</v>
+        <v>66938</v>
       </c>
       <c r="D950" t="n">
-        <v>85891282</v>
+        <v>85937162</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>25501</v>
+        <v>25518</v>
       </c>
       <c r="D957" t="n">
-        <v>37376852</v>
+        <v>37401841</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46366,10 +46366,10 @@
         </is>
       </c>
       <c r="C959" t="n">
-        <v>17540</v>
+        <v>17553</v>
       </c>
       <c r="D959" t="n">
-        <v>25431342</v>
+        <v>25449522</v>
       </c>
       <c r="E959" t="inlineStr">
         <is>
@@ -46462,10 +46462,10 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D961" t="n">
-        <v>697823</v>
+        <v>699323</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>83493</v>
+        <v>83574</v>
       </c>
       <c r="D963" t="n">
-        <v>104839381</v>
+        <v>104927047</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>33725</v>
+        <v>33745</v>
       </c>
       <c r="D970" t="n">
-        <v>49470396</v>
+        <v>49496037</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -47038,10 +47038,10 @@
         </is>
       </c>
       <c r="C973" t="n">
-        <v>25115</v>
+        <v>25129</v>
       </c>
       <c r="D973" t="n">
-        <v>36426461</v>
+        <v>36447237</v>
       </c>
       <c r="E973" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="D976" t="n">
-        <v>2787617</v>
+        <v>2789117</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>10716</v>
+        <v>10726</v>
       </c>
       <c r="D977" t="n">
-        <v>13982476</v>
+        <v>13993663</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47422,10 +47422,10 @@
         </is>
       </c>
       <c r="C981" t="n">
-        <v>3455</v>
+        <v>3456</v>
       </c>
       <c r="D981" t="n">
-        <v>5046922</v>
+        <v>5048422</v>
       </c>
       <c r="E981" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>55825</v>
+        <v>55861</v>
       </c>
       <c r="D987" t="n">
-        <v>69893337</v>
+        <v>69938241</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>18474</v>
+        <v>18482</v>
       </c>
       <c r="D992" t="n">
-        <v>27055283</v>
+        <v>27067283</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -48046,10 +48046,10 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>12577</v>
+        <v>12587</v>
       </c>
       <c r="D994" t="n">
-        <v>18188477</v>
+        <v>18202855</v>
       </c>
       <c r="E994" t="inlineStr">
         <is>
@@ -48094,10 +48094,10 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D995" t="n">
-        <v>677973</v>
+        <v>679473</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
@@ -48190,10 +48190,10 @@
         </is>
       </c>
       <c r="C997" t="n">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="D997" t="n">
-        <v>1029924</v>
+        <v>1034424</v>
       </c>
       <c r="E997" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>28146</v>
+        <v>28166</v>
       </c>
       <c r="D998" t="n">
-        <v>35021979</v>
+        <v>35049665</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48478,10 +48478,10 @@
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>10473</v>
+        <v>10479</v>
       </c>
       <c r="D1003" t="n">
-        <v>15338750</v>
+        <v>15347750</v>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>6203</v>
+        <v>6205</v>
       </c>
       <c r="D1005" t="n">
-        <v>8994605</v>
+        <v>8997605</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D1006" t="n">
-        <v>744918</v>
+        <v>745918</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-11 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16338</v>
+        <v>16350</v>
       </c>
       <c r="D2" t="n">
-        <v>20540918</v>
+        <v>20554322</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6240</v>
+        <v>6241</v>
       </c>
       <c r="D6" t="n">
-        <v>9125238</v>
+        <v>9126738</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3287</v>
+        <v>3288</v>
       </c>
       <c r="D8" t="n">
-        <v>4756880</v>
+        <v>4758380</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10978</v>
+        <v>10986</v>
       </c>
       <c r="D12" t="n">
-        <v>13854426</v>
+        <v>13863620</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3224</v>
+        <v>3226</v>
       </c>
       <c r="D16" t="n">
-        <v>4697627</v>
+        <v>4700627</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D18" t="n">
-        <v>2092220</v>
+        <v>2093720</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D19" t="n">
-        <v>545821</v>
+        <v>547321</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14232</v>
+        <v>14240</v>
       </c>
       <c r="D21" t="n">
-        <v>17457173</v>
+        <v>17463355</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4935</v>
+        <v>4937</v>
       </c>
       <c r="D25" t="n">
-        <v>7216928</v>
+        <v>7219928</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6545</v>
+        <v>6548</v>
       </c>
       <c r="D31" t="n">
-        <v>8694275</v>
+        <v>8696969</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="D34" t="n">
-        <v>2318620</v>
+        <v>2320120</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>21836</v>
+        <v>21852</v>
       </c>
       <c r="D40" t="n">
-        <v>26876126</v>
+        <v>26894204</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7798</v>
+        <v>7802</v>
       </c>
       <c r="D46" t="n">
-        <v>11454460</v>
+        <v>11460460</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3831</v>
+        <v>3835</v>
       </c>
       <c r="D48" t="n">
-        <v>5545155</v>
+        <v>5551155</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D51" t="n">
-        <v>827066</v>
+        <v>828566</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>8132</v>
+        <v>8138</v>
       </c>
       <c r="D52" t="n">
-        <v>10377641</v>
+        <v>10384450</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2779</v>
+        <v>2780</v>
       </c>
       <c r="D56" t="n">
-        <v>4042043</v>
+        <v>4043543</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>36089</v>
+        <v>36117</v>
       </c>
       <c r="D61" t="n">
-        <v>46464294</v>
+        <v>46498503</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>13144</v>
+        <v>13148</v>
       </c>
       <c r="D66" t="n">
-        <v>19277835</v>
+        <v>19283835</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5153</v>
+        <v>5159</v>
       </c>
       <c r="D68" t="n">
-        <v>7452815</v>
+        <v>7461584</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>46187</v>
+        <v>46220</v>
       </c>
       <c r="D74" t="n">
-        <v>59055149</v>
+        <v>59091847</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4078,10 +4078,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>18104</v>
+        <v>18108</v>
       </c>
       <c r="D78" t="n">
-        <v>26523304</v>
+        <v>26529304</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9324</v>
+        <v>9328</v>
       </c>
       <c r="D80" t="n">
-        <v>13460833</v>
+        <v>13466833</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>24901</v>
+        <v>24928</v>
       </c>
       <c r="D85" t="n">
-        <v>31390628</v>
+        <v>31424802</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8676</v>
+        <v>8677</v>
       </c>
       <c r="D89" t="n">
-        <v>12735886</v>
+        <v>12737386</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4895</v>
+        <v>4900</v>
       </c>
       <c r="D91" t="n">
-        <v>7074639</v>
+        <v>7082139</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>21931</v>
+        <v>21948</v>
       </c>
       <c r="D94" t="n">
-        <v>27531701</v>
+        <v>27555399</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -5038,10 +5038,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9149</v>
+        <v>9151</v>
       </c>
       <c r="D98" t="n">
-        <v>13393205</v>
+        <v>13394849</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -5134,10 +5134,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>3312</v>
+        <v>3324</v>
       </c>
       <c r="D100" t="n">
-        <v>4744746</v>
+        <v>4761769</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>81519</v>
+        <v>81616</v>
       </c>
       <c r="D105" t="n">
-        <v>104466700</v>
+        <v>104586681</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>30573</v>
+        <v>30582</v>
       </c>
       <c r="D112" t="n">
-        <v>44864473</v>
+        <v>44877917</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20797</v>
+        <v>20811</v>
       </c>
       <c r="D114" t="n">
-        <v>30009159</v>
+        <v>30029999</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1882</v>
+        <v>1891</v>
       </c>
       <c r="D121" t="n">
-        <v>2647383</v>
+        <v>2660707</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>27666</v>
+        <v>27683</v>
       </c>
       <c r="D122" t="n">
-        <v>36514011</v>
+        <v>36535103</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>9863</v>
+        <v>9867</v>
       </c>
       <c r="D126" t="n">
-        <v>14464979</v>
+        <v>14470370</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3263</v>
+        <v>3264</v>
       </c>
       <c r="D128" t="n">
-        <v>4744157</v>
+        <v>4745657</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6622,10 +6622,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D131" t="n">
-        <v>491802</v>
+        <v>493302</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15722</v>
+        <v>15732</v>
       </c>
       <c r="D132" t="n">
-        <v>19564614</v>
+        <v>19576121</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6814,10 +6814,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7754</v>
+        <v>7757</v>
       </c>
       <c r="D135" t="n">
-        <v>11347635</v>
+        <v>11350849</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2210</v>
+        <v>2212</v>
       </c>
       <c r="D137" t="n">
-        <v>3155610</v>
+        <v>3158610</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>13514</v>
+        <v>13522</v>
       </c>
       <c r="D142" t="n">
-        <v>16887463</v>
+        <v>16896463</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6239</v>
+        <v>6240</v>
       </c>
       <c r="D146" t="n">
-        <v>9140755</v>
+        <v>9142255</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="D148" t="n">
-        <v>2871499</v>
+        <v>2872999</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7582,10 +7582,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D151" t="n">
-        <v>506408</v>
+        <v>507908</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7630,10 +7630,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>5978</v>
+        <v>5982</v>
       </c>
       <c r="D152" t="n">
-        <v>7311632</v>
+        <v>7316232</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -7966,10 +7966,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D159" t="n">
-        <v>127567</v>
+        <v>129067</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7430</v>
+        <v>7432</v>
       </c>
       <c r="D160" t="n">
-        <v>9212472</v>
+        <v>9213335</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D164" t="n">
-        <v>2011432</v>
+        <v>2012281</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5606</v>
+        <v>5611</v>
       </c>
       <c r="D168" t="n">
-        <v>7056757</v>
+        <v>7061634</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8638,10 +8638,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="D173" t="n">
-        <v>2960041</v>
+        <v>2963041</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>15952</v>
+        <v>15958</v>
       </c>
       <c r="D178" t="n">
-        <v>20043666</v>
+        <v>20051654</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6389</v>
+        <v>6391</v>
       </c>
       <c r="D183" t="n">
-        <v>9332359</v>
+        <v>9335359</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>2224</v>
+        <v>2225</v>
       </c>
       <c r="D184" t="n">
-        <v>3192491</v>
+        <v>3193991</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3064</v>
+        <v>3071</v>
       </c>
       <c r="D188" t="n">
-        <v>3846137</v>
+        <v>3854537</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>1472</v>
+        <v>1474</v>
       </c>
       <c r="D190" t="n">
-        <v>2153742</v>
+        <v>2156742</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9199</v>
+        <v>9202</v>
       </c>
       <c r="D196" t="n">
-        <v>11486616</v>
+        <v>11489814</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>17237</v>
+        <v>17254</v>
       </c>
       <c r="D205" t="n">
-        <v>21531557</v>
+        <v>21548500</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>7682</v>
+        <v>7687</v>
       </c>
       <c r="D209" t="n">
-        <v>11280996</v>
+        <v>11287615</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>26109</v>
+        <v>26124</v>
       </c>
       <c r="D213" t="n">
-        <v>32931061</v>
+        <v>32949473</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>10487</v>
+        <v>10492</v>
       </c>
       <c r="D217" t="n">
-        <v>15315853</v>
+        <v>15323353</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2635</v>
+        <v>2638</v>
       </c>
       <c r="D219" t="n">
-        <v>3800022</v>
+        <v>3804522</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D222" t="n">
-        <v>844766</v>
+        <v>847766</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>28456</v>
+        <v>28472</v>
       </c>
       <c r="D223" t="n">
-        <v>35915098</v>
+        <v>35930563</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>14722</v>
+        <v>14726</v>
       </c>
       <c r="D228" t="n">
-        <v>21602928</v>
+        <v>21607618</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2655</v>
+        <v>2656</v>
       </c>
       <c r="D230" t="n">
-        <v>3812175</v>
+        <v>3813675</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D232" t="n">
-        <v>511084</v>
+        <v>512382</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24254</v>
+        <v>24270</v>
       </c>
       <c r="D234" t="n">
-        <v>30595219</v>
+        <v>30615933</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>11170</v>
+        <v>11175</v>
       </c>
       <c r="D240" t="n">
-        <v>16375749</v>
+        <v>16382837</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2506</v>
+        <v>2509</v>
       </c>
       <c r="D242" t="n">
-        <v>3582347</v>
+        <v>3585748</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12142,10 +12142,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>7866</v>
+        <v>7870</v>
       </c>
       <c r="D246" t="n">
-        <v>9840680</v>
+        <v>9845747</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>2700</v>
+        <v>2701</v>
       </c>
       <c r="D250" t="n">
-        <v>3963150</v>
+        <v>3964650</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12478,10 +12478,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="D253" t="n">
-        <v>1454115</v>
+        <v>1455615</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>9796</v>
+        <v>9806</v>
       </c>
       <c r="D256" t="n">
-        <v>12493927</v>
+        <v>12507997</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>2170</v>
+        <v>2171</v>
       </c>
       <c r="D262" t="n">
-        <v>3141602</v>
+        <v>3143102</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>5540</v>
+        <v>5541</v>
       </c>
       <c r="D265" t="n">
-        <v>6870043</v>
+        <v>6871543</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13486,10 +13486,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>19056</v>
+        <v>19075</v>
       </c>
       <c r="D274" t="n">
-        <v>24079422</v>
+        <v>24099822</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>7924</v>
+        <v>7928</v>
       </c>
       <c r="D278" t="n">
-        <v>11618608</v>
+        <v>11624608</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>2493</v>
+        <v>2495</v>
       </c>
       <c r="D280" t="n">
-        <v>3581059</v>
+        <v>3584059</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>16594</v>
+        <v>16614</v>
       </c>
       <c r="D285" t="n">
-        <v>20556883</v>
+        <v>20580279</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>7181</v>
+        <v>7184</v>
       </c>
       <c r="D289" t="n">
-        <v>10533112</v>
+        <v>10536614</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>3328</v>
+        <v>3329</v>
       </c>
       <c r="D290" t="n">
-        <v>4823299</v>
+        <v>4824799</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D293" t="n">
-        <v>467443</v>
+        <v>468587</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>9342</v>
+        <v>9349</v>
       </c>
       <c r="D294" t="n">
-        <v>11739335</v>
+        <v>11746732</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D300" t="n">
-        <v>313165</v>
+        <v>314665</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14878,10 +14878,10 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D303" t="n">
-        <v>288729</v>
+        <v>290229</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>9193</v>
+        <v>9197</v>
       </c>
       <c r="D304" t="n">
-        <v>12003485</v>
+        <v>12008790</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>3739</v>
+        <v>3744</v>
       </c>
       <c r="D308" t="n">
-        <v>5466349</v>
+        <v>5473849</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="D309" t="n">
-        <v>3419468</v>
+        <v>3420968</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>11059</v>
+        <v>11068</v>
       </c>
       <c r="D312" t="n">
-        <v>14523278</v>
+        <v>14533022</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2702</v>
+        <v>2704</v>
       </c>
       <c r="D318" t="n">
-        <v>3918138</v>
+        <v>3920296</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6808</v>
+        <v>6811</v>
       </c>
       <c r="D321" t="n">
-        <v>8416301</v>
+        <v>8420246</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15982,10 +15982,10 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>2297</v>
+        <v>2299</v>
       </c>
       <c r="D326" t="n">
-        <v>3370084</v>
+        <v>3372584</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="D328" t="n">
-        <v>1130275</v>
+        <v>1133275</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>7522</v>
+        <v>7529</v>
       </c>
       <c r="D331" t="n">
-        <v>9418179</v>
+        <v>9424650</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16462,10 +16462,10 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>3127</v>
+        <v>3128</v>
       </c>
       <c r="D336" t="n">
-        <v>4568815</v>
+        <v>4570315</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D337" t="n">
-        <v>1848361</v>
+        <v>1849861</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>31982</v>
+        <v>32013</v>
       </c>
       <c r="D340" t="n">
-        <v>40177718</v>
+        <v>40214418</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>16524</v>
+        <v>16534</v>
       </c>
       <c r="D346" t="n">
-        <v>24161739</v>
+        <v>24176270</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>8042</v>
+        <v>8047</v>
       </c>
       <c r="D349" t="n">
-        <v>11582205</v>
+        <v>11588516</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D350" t="n">
-        <v>915671</v>
+        <v>917053</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17182,10 +17182,10 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D351" t="n">
-        <v>1109890</v>
+        <v>1110589</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>3893</v>
+        <v>3894</v>
       </c>
       <c r="D352" t="n">
-        <v>4850212</v>
+        <v>4851412</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D355" t="n">
-        <v>2204657</v>
+        <v>2206157</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>19368</v>
+        <v>19384</v>
       </c>
       <c r="D360" t="n">
-        <v>24150044</v>
+        <v>24169548</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>9901</v>
+        <v>9907</v>
       </c>
       <c r="D364" t="n">
-        <v>14516235</v>
+        <v>14525235</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>4737</v>
+        <v>4739</v>
       </c>
       <c r="D366" t="n">
-        <v>6850409</v>
+        <v>6853409</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>13917</v>
+        <v>13929</v>
       </c>
       <c r="D369" t="n">
-        <v>17408534</v>
+        <v>17424352</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>6441</v>
+        <v>6443</v>
       </c>
       <c r="D373" t="n">
-        <v>9430458</v>
+        <v>9433376</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18334,10 +18334,10 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>2481</v>
+        <v>2482</v>
       </c>
       <c r="D375" t="n">
-        <v>3565183</v>
+        <v>3566683</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D376" t="n">
-        <v>1019501</v>
+        <v>1021001</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>17981</v>
+        <v>17996</v>
       </c>
       <c r="D378" t="n">
-        <v>22423439</v>
+        <v>22440658</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>7139</v>
+        <v>7141</v>
       </c>
       <c r="D382" t="n">
-        <v>10493715</v>
+        <v>10496715</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>2836</v>
+        <v>2838</v>
       </c>
       <c r="D384" t="n">
-        <v>4125151</v>
+        <v>4128151</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D387" t="n">
-        <v>557154</v>
+        <v>557454</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>4090</v>
+        <v>4096</v>
       </c>
       <c r="D388" t="n">
-        <v>5132292</v>
+        <v>5139992</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D391" t="n">
-        <v>2029076</v>
+        <v>2030576</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>22268</v>
+        <v>22284</v>
       </c>
       <c r="D395" t="n">
-        <v>27623557</v>
+        <v>27641651</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>9364</v>
+        <v>9366</v>
       </c>
       <c r="D398" t="n">
-        <v>13785017</v>
+        <v>13788017</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>6207</v>
+        <v>6209</v>
       </c>
       <c r="D400" t="n">
-        <v>9028491</v>
+        <v>9031491</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D402" t="n">
-        <v>486802</v>
+        <v>489802</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>11131</v>
+        <v>11138</v>
       </c>
       <c r="D403" t="n">
-        <v>13722637</v>
+        <v>13731862</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="D410" t="n">
-        <v>2675364</v>
+        <v>2676864</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>32126</v>
+        <v>32245</v>
       </c>
       <c r="D413" t="n">
-        <v>43525558</v>
+        <v>43682165</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>7802</v>
+        <v>7820</v>
       </c>
       <c r="D417" t="n">
-        <v>11472470</v>
+        <v>11498881</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>7098</v>
+        <v>7130</v>
       </c>
       <c r="D419" t="n">
-        <v>10290127</v>
+        <v>10336819</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20542,10 +20542,10 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="D421" t="n">
-        <v>734905</v>
+        <v>748405</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>8823</v>
+        <v>8855</v>
       </c>
       <c r="D423" t="n">
-        <v>12245320</v>
+        <v>12290720</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2218</v>
+        <v>2227</v>
       </c>
       <c r="D425" t="n">
-        <v>3267382</v>
+        <v>3280802</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>2988</v>
+        <v>2996</v>
       </c>
       <c r="D427" t="n">
-        <v>4364741</v>
+        <v>4376451</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -21022,10 +21022,10 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>11022</v>
+        <v>11026</v>
       </c>
       <c r="D431" t="n">
-        <v>13608231</v>
+        <v>13613278</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>3786</v>
+        <v>3788</v>
       </c>
       <c r="D434" t="n">
-        <v>5556304</v>
+        <v>5559304</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="D436" t="n">
-        <v>2684727</v>
+        <v>2686227</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>62901</v>
+        <v>62963</v>
       </c>
       <c r="D439" t="n">
-        <v>77955041</v>
+        <v>78029261</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D440" t="n">
-        <v>16482</v>
+        <v>17982</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>24916</v>
+        <v>24922</v>
       </c>
       <c r="D443" t="n">
-        <v>36523120</v>
+        <v>36532120</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>12923</v>
+        <v>12935</v>
       </c>
       <c r="D445" t="n">
-        <v>18740027</v>
+        <v>18757013</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="D449" t="n">
-        <v>1460899</v>
+        <v>1463799</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>18889</v>
+        <v>18905</v>
       </c>
       <c r="D451" t="n">
-        <v>23878757</v>
+        <v>23897374</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>7702</v>
+        <v>7706</v>
       </c>
       <c r="D455" t="n">
-        <v>11305393</v>
+        <v>11311393</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>4856</v>
+        <v>4857</v>
       </c>
       <c r="D457" t="n">
-        <v>7046922</v>
+        <v>7048197</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>32218</v>
+        <v>32230</v>
       </c>
       <c r="D460" t="n">
-        <v>39380080</v>
+        <v>39395110</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>11448</v>
+        <v>11453</v>
       </c>
       <c r="D464" t="n">
-        <v>16749849</v>
+        <v>16757349</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>4905</v>
+        <v>4908</v>
       </c>
       <c r="D466" t="n">
-        <v>7116582</v>
+        <v>7121082</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D467" t="n">
-        <v>523484</v>
+        <v>524984</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>14395</v>
+        <v>14404</v>
       </c>
       <c r="D469" t="n">
-        <v>17602746</v>
+        <v>17609840</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>4380</v>
+        <v>4382</v>
       </c>
       <c r="D474" t="n">
-        <v>6434922</v>
+        <v>6437922</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>35970</v>
+        <v>36015</v>
       </c>
       <c r="D479" t="n">
-        <v>46870036</v>
+        <v>46929744</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>13552</v>
+        <v>13562</v>
       </c>
       <c r="D483" t="n">
-        <v>19938300</v>
+        <v>19953300</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>11987</v>
+        <v>11997</v>
       </c>
       <c r="D485" t="n">
-        <v>17494788</v>
+        <v>17509678</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>62307</v>
+        <v>62396</v>
       </c>
       <c r="D488" t="n">
-        <v>82499286</v>
+        <v>82620108</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>23099</v>
+        <v>23114</v>
       </c>
       <c r="D493" t="n">
-        <v>33893984</v>
+        <v>33916484</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>22419</v>
+        <v>22440</v>
       </c>
       <c r="D495" t="n">
-        <v>32549416</v>
+        <v>32578711</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>150775</v>
+        <v>150987</v>
       </c>
       <c r="D499" t="n">
-        <v>198306113</v>
+        <v>198571677</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24526,10 +24526,10 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D504" t="n">
-        <v>697555</v>
+        <v>699055</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>81585</v>
+        <v>81645</v>
       </c>
       <c r="D506" t="n">
-        <v>119852991</v>
+        <v>119935894</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D507" t="n">
-        <v>344842</v>
+        <v>346342</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>60006</v>
+        <v>60076</v>
       </c>
       <c r="D509" t="n">
-        <v>87103422</v>
+        <v>87207210</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="D511" t="n">
-        <v>1534107</v>
+        <v>1535607</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>2778</v>
+        <v>2786</v>
       </c>
       <c r="D513" t="n">
-        <v>3932678</v>
+        <v>3944013</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>41168</v>
+        <v>41216</v>
       </c>
       <c r="D515" t="n">
-        <v>53512578</v>
+        <v>53575179</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>15240</v>
+        <v>15256</v>
       </c>
       <c r="D520" t="n">
-        <v>22385856</v>
+        <v>22408613</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>12926</v>
+        <v>12935</v>
       </c>
       <c r="D522" t="n">
-        <v>18735030</v>
+        <v>18748530</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25534,10 +25534,10 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D525" t="n">
-        <v>493648</v>
+        <v>496156</v>
       </c>
       <c r="E525" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>66137</v>
+        <v>66230</v>
       </c>
       <c r="D527" t="n">
-        <v>88888705</v>
+        <v>89010595</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>23306</v>
+        <v>23328</v>
       </c>
       <c r="D531" t="n">
-        <v>34389681</v>
+        <v>34422343</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>24074</v>
+        <v>24105</v>
       </c>
       <c r="D533" t="n">
-        <v>35234416</v>
+        <v>35278463</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="D536" t="n">
-        <v>1217969</v>
+        <v>1220969</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>55027</v>
+        <v>55099</v>
       </c>
       <c r="D537" t="n">
-        <v>72983757</v>
+        <v>73077699</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>17770</v>
+        <v>17787</v>
       </c>
       <c r="D542" t="n">
-        <v>26111526</v>
+        <v>26137026</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>18302</v>
+        <v>18324</v>
       </c>
       <c r="D544" t="n">
-        <v>26603867</v>
+        <v>26636847</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26542,10 +26542,10 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D546" t="n">
-        <v>877715</v>
+        <v>882204</v>
       </c>
       <c r="E546" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>41550</v>
+        <v>41596</v>
       </c>
       <c r="D547" t="n">
-        <v>55175648</v>
+        <v>55237547</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>14212</v>
+        <v>14223</v>
       </c>
       <c r="D551" t="n">
-        <v>20961121</v>
+        <v>20977621</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>14398</v>
+        <v>14414</v>
       </c>
       <c r="D553" t="n">
-        <v>20908148</v>
+        <v>20930756</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D554" t="n">
-        <v>251479</v>
+        <v>257479</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>41301</v>
+        <v>41339</v>
       </c>
       <c r="D556" t="n">
-        <v>53542148</v>
+        <v>53593514</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>16191</v>
+        <v>16201</v>
       </c>
       <c r="D560" t="n">
-        <v>23756426</v>
+        <v>23771426</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>12998</v>
+        <v>13010</v>
       </c>
       <c r="D562" t="n">
-        <v>18798447</v>
+        <v>18815967</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>43856</v>
+        <v>43912</v>
       </c>
       <c r="D566" t="n">
-        <v>58552963</v>
+        <v>58625733</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>13905</v>
+        <v>13916</v>
       </c>
       <c r="D572" t="n">
-        <v>20395249</v>
+        <v>20410330</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>17264</v>
+        <v>17288</v>
       </c>
       <c r="D579" t="n">
-        <v>22809991</v>
+        <v>22842544</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>7059</v>
+        <v>7066</v>
       </c>
       <c r="D583" t="n">
-        <v>10266288</v>
+        <v>10276203</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28414,10 +28414,10 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>4913</v>
+        <v>4921</v>
       </c>
       <c r="D585" t="n">
-        <v>7071877</v>
+        <v>7081742</v>
       </c>
       <c r="E585" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D588" t="n">
-        <v>372274</v>
+        <v>373774</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>15462</v>
+        <v>15577</v>
       </c>
       <c r="D590" t="n">
-        <v>22435556</v>
+        <v>22604690</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>1744</v>
+        <v>1755</v>
       </c>
       <c r="D591" t="n">
-        <v>2593730</v>
+        <v>2610230</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D595" t="n">
-        <v>116949</v>
+        <v>118449</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>21988</v>
+        <v>22005</v>
       </c>
       <c r="D596" t="n">
-        <v>27588072</v>
+        <v>27609086</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D597" t="n">
-        <v>7229</v>
+        <v>7481</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>8982</v>
+        <v>8985</v>
       </c>
       <c r="D601" t="n">
-        <v>13158665</v>
+        <v>13163165</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29278,10 +29278,10 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>3347</v>
+        <v>3348</v>
       </c>
       <c r="D603" t="n">
-        <v>4807159</v>
+        <v>4808659</v>
       </c>
       <c r="E603" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>14626</v>
+        <v>14637</v>
       </c>
       <c r="D607" t="n">
-        <v>18339100</v>
+        <v>18352138</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>5782</v>
+        <v>5786</v>
       </c>
       <c r="D611" t="n">
-        <v>8492151</v>
+        <v>8498151</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>2669</v>
+        <v>2672</v>
       </c>
       <c r="D613" t="n">
-        <v>3847087</v>
+        <v>3851587</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D614" t="n">
-        <v>255209</v>
+        <v>256709</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D615" t="n">
-        <v>260636</v>
+        <v>262136</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>13737</v>
+        <v>13744</v>
       </c>
       <c r="D616" t="n">
-        <v>17352334</v>
+        <v>17361851</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -30094,10 +30094,10 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>5221</v>
+        <v>5225</v>
       </c>
       <c r="D620" t="n">
-        <v>7652720</v>
+        <v>7658720</v>
       </c>
       <c r="E620" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D624" t="n">
-        <v>365966</v>
+        <v>367466</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>7495</v>
+        <v>7501</v>
       </c>
       <c r="D625" t="n">
-        <v>9641387</v>
+        <v>9648223</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>28767</v>
+        <v>28778</v>
       </c>
       <c r="D634" t="n">
-        <v>35431583</v>
+        <v>35443958</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>11005</v>
+        <v>11015</v>
       </c>
       <c r="D638" t="n">
-        <v>16147115</v>
+        <v>16161785</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4818</v>
+        <v>4823</v>
       </c>
       <c r="D640" t="n">
-        <v>6990353</v>
+        <v>6997853</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>11294</v>
+        <v>11306</v>
       </c>
       <c r="D644" t="n">
-        <v>13689706</v>
+        <v>13703369</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>3636</v>
+        <v>3638</v>
       </c>
       <c r="D649" t="n">
-        <v>5322719</v>
+        <v>5325719</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>28263</v>
+        <v>28273</v>
       </c>
       <c r="D654" t="n">
-        <v>35140545</v>
+        <v>35151553</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>10730</v>
+        <v>10732</v>
       </c>
       <c r="D658" t="n">
-        <v>15765836</v>
+        <v>15768836</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>3074</v>
+        <v>3075</v>
       </c>
       <c r="D660" t="n">
-        <v>4432477</v>
+        <v>4433977</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32110,10 +32110,10 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D662" t="n">
-        <v>711551</v>
+        <v>713051</v>
       </c>
       <c r="E662" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D663" t="n">
-        <v>666675</v>
+        <v>671175</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>7481</v>
+        <v>7489</v>
       </c>
       <c r="D664" t="n">
-        <v>9492436</v>
+        <v>9501760</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D669" t="n">
-        <v>364484</v>
+        <v>365984</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3770</v>
+        <v>3771</v>
       </c>
       <c r="D672" t="n">
-        <v>4569767</v>
+        <v>4571267</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D680" t="n">
-        <v>206432</v>
+        <v>207932</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>9296</v>
+        <v>9308</v>
       </c>
       <c r="D681" t="n">
-        <v>11599362</v>
+        <v>11611033</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>3464</v>
+        <v>3465</v>
       </c>
       <c r="D685" t="n">
-        <v>5106517</v>
+        <v>5108017</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D686" t="n">
-        <v>1078602</v>
+        <v>1080102</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>19187</v>
+        <v>19197</v>
       </c>
       <c r="D690" t="n">
-        <v>23481704</v>
+        <v>23493583</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>5703</v>
+        <v>5706</v>
       </c>
       <c r="D694" t="n">
-        <v>8329980</v>
+        <v>8334480</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>2242</v>
+        <v>2243</v>
       </c>
       <c r="D696" t="n">
-        <v>3226014</v>
+        <v>3227514</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33838,10 +33838,10 @@
         </is>
       </c>
       <c r="C698" t="n">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D698" t="n">
-        <v>509462</v>
+        <v>510962</v>
       </c>
       <c r="E698" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>74249</v>
+        <v>74360</v>
       </c>
       <c r="D701" t="n">
-        <v>93471953</v>
+        <v>93615310</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>26463</v>
+        <v>26475</v>
       </c>
       <c r="D706" t="n">
-        <v>38853677</v>
+        <v>38871677</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>13123</v>
+        <v>13132</v>
       </c>
       <c r="D709" t="n">
-        <v>18928093</v>
+        <v>18939335</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>1928</v>
+        <v>1934</v>
       </c>
       <c r="D712" t="n">
-        <v>2778547</v>
+        <v>2783827</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>1196</v>
+        <v>1199</v>
       </c>
       <c r="D714" t="n">
-        <v>1669243</v>
+        <v>1673743</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>11133</v>
+        <v>11146</v>
       </c>
       <c r="D715" t="n">
-        <v>13624063</v>
+        <v>13636360</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>4095</v>
+        <v>4100</v>
       </c>
       <c r="D718" t="n">
-        <v>5990583</v>
+        <v>5997133</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>1488</v>
+        <v>1490</v>
       </c>
       <c r="D720" t="n">
-        <v>2144500</v>
+        <v>2147500</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -34990,10 +34990,10 @@
         </is>
       </c>
       <c r="C722" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D722" t="n">
-        <v>335382</v>
+        <v>336882</v>
       </c>
       <c r="E722" t="inlineStr">
         <is>
@@ -35038,10 +35038,10 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>17537</v>
+        <v>17566</v>
       </c>
       <c r="D723" t="n">
-        <v>21633227</v>
+        <v>21665775</v>
       </c>
       <c r="E723" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>6831</v>
+        <v>6836</v>
       </c>
       <c r="D727" t="n">
-        <v>9985329</v>
+        <v>9992329</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35326,10 +35326,10 @@
         </is>
       </c>
       <c r="C729" t="n">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="D729" t="n">
-        <v>3120038</v>
+        <v>3121538</v>
       </c>
       <c r="E729" t="inlineStr">
         <is>
@@ -35422,10 +35422,10 @@
         </is>
       </c>
       <c r="C731" t="n">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D731" t="n">
-        <v>453989</v>
+        <v>459189</v>
       </c>
       <c r="E731" t="inlineStr">
         <is>
@@ -35470,10 +35470,10 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D732" t="n">
-        <v>451719</v>
+        <v>455679</v>
       </c>
       <c r="E732" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>11473</v>
+        <v>11491</v>
       </c>
       <c r="D734" t="n">
-        <v>14167854</v>
+        <v>14188870</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35758,10 +35758,10 @@
         </is>
       </c>
       <c r="C738" t="n">
-        <v>4229</v>
+        <v>4231</v>
       </c>
       <c r="D738" t="n">
-        <v>6199745</v>
+        <v>6201994</v>
       </c>
       <c r="E738" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>29454</v>
+        <v>29473</v>
       </c>
       <c r="D743" t="n">
-        <v>36609190</v>
+        <v>36632831</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>12688</v>
+        <v>12694</v>
       </c>
       <c r="D748" t="n">
-        <v>18569699</v>
+        <v>18578590</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36334,10 +36334,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>4204</v>
+        <v>4207</v>
       </c>
       <c r="D750" t="n">
-        <v>6006619</v>
+        <v>6011119</v>
       </c>
       <c r="E750" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D753" t="n">
-        <v>953504</v>
+        <v>958004</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>12277</v>
+        <v>12287</v>
       </c>
       <c r="D755" t="n">
-        <v>15200121</v>
+        <v>15210614</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36718,10 +36718,10 @@
         </is>
       </c>
       <c r="C758" t="n">
-        <v>4650</v>
+        <v>4651</v>
       </c>
       <c r="D758" t="n">
-        <v>6796356</v>
+        <v>6797856</v>
       </c>
       <c r="E758" t="inlineStr">
         <is>
@@ -36766,10 +36766,10 @@
         </is>
       </c>
       <c r="C759" t="n">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D759" t="n">
-        <v>1643486</v>
+        <v>1644986</v>
       </c>
       <c r="E759" t="inlineStr">
         <is>
@@ -36862,10 +36862,10 @@
         </is>
       </c>
       <c r="C761" t="n">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D761" t="n">
-        <v>522162</v>
+        <v>525162</v>
       </c>
       <c r="E761" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>6698</v>
+        <v>6708</v>
       </c>
       <c r="D762" t="n">
-        <v>7872150</v>
+        <v>7883669</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37102,10 +37102,10 @@
         </is>
       </c>
       <c r="C766" t="n">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="D766" t="n">
-        <v>2472153</v>
+        <v>2473653</v>
       </c>
       <c r="E766" t="inlineStr">
         <is>
@@ -37246,10 +37246,10 @@
         </is>
       </c>
       <c r="C769" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D769" t="n">
-        <v>209935</v>
+        <v>210947</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>16747</v>
+        <v>16762</v>
       </c>
       <c r="D770" t="n">
-        <v>20319218</v>
+        <v>20334664</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>5524</v>
+        <v>5529</v>
       </c>
       <c r="D775" t="n">
-        <v>8094086</v>
+        <v>8101586</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37630,10 +37630,10 @@
         </is>
       </c>
       <c r="C777" t="n">
-        <v>3388</v>
+        <v>3391</v>
       </c>
       <c r="D777" t="n">
-        <v>4948222</v>
+        <v>4952722</v>
       </c>
       <c r="E777" t="inlineStr">
         <is>
@@ -37774,10 +37774,10 @@
         </is>
       </c>
       <c r="C780" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D780" t="n">
-        <v>391348</v>
+        <v>392848</v>
       </c>
       <c r="E780" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>11345</v>
+        <v>11351</v>
       </c>
       <c r="D781" t="n">
-        <v>14369076</v>
+        <v>14372659</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -38014,10 +38014,10 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>3948</v>
+        <v>3949</v>
       </c>
       <c r="D785" t="n">
-        <v>5772983</v>
+        <v>5774483</v>
       </c>
       <c r="E785" t="inlineStr">
         <is>
@@ -38110,10 +38110,10 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="D787" t="n">
-        <v>1812412</v>
+        <v>1815412</v>
       </c>
       <c r="E787" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>32037</v>
+        <v>32063</v>
       </c>
       <c r="D791" t="n">
-        <v>39518834</v>
+        <v>39551293</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38494,10 +38494,10 @@
         </is>
       </c>
       <c r="C795" t="n">
-        <v>13159</v>
+        <v>13164</v>
       </c>
       <c r="D795" t="n">
-        <v>19253227</v>
+        <v>19260319</v>
       </c>
       <c r="E795" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D798" t="n">
-        <v>731569</v>
+        <v>733069</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38734,10 +38734,10 @@
         </is>
       </c>
       <c r="C800" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D800" t="n">
-        <v>910773</v>
+        <v>912273</v>
       </c>
       <c r="E800" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>7590</v>
+        <v>7595</v>
       </c>
       <c r="D801" t="n">
-        <v>9384537</v>
+        <v>9392037</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -39070,10 +39070,10 @@
         </is>
       </c>
       <c r="C807" t="n">
-        <v>2676</v>
+        <v>2677</v>
       </c>
       <c r="D807" t="n">
-        <v>3903484</v>
+        <v>3904984</v>
       </c>
       <c r="E807" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="D808" t="n">
-        <v>1634438</v>
+        <v>1637438</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39262,10 +39262,10 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>58661</v>
+        <v>58732</v>
       </c>
       <c r="D811" t="n">
-        <v>73327148</v>
+        <v>73414309</v>
       </c>
       <c r="E811" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>21092</v>
+        <v>21113</v>
       </c>
       <c r="D816" t="n">
-        <v>30859293</v>
+        <v>30888769</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>12567</v>
+        <v>12577</v>
       </c>
       <c r="D819" t="n">
-        <v>18140129</v>
+        <v>18153682</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>1316</v>
+        <v>1320</v>
       </c>
       <c r="D824" t="n">
-        <v>1835325</v>
+        <v>1840607</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>11104</v>
+        <v>11112</v>
       </c>
       <c r="D825" t="n">
-        <v>13844329</v>
+        <v>13854013</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -40030,10 +40030,10 @@
         </is>
       </c>
       <c r="C827" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D827" t="n">
-        <v>40366</v>
+        <v>43366</v>
       </c>
       <c r="E827" t="inlineStr">
         <is>
@@ -40126,10 +40126,10 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>3903</v>
+        <v>3909</v>
       </c>
       <c r="D829" t="n">
-        <v>5674604</v>
+        <v>5682219</v>
       </c>
       <c r="E829" t="inlineStr">
         <is>
@@ -40222,10 +40222,10 @@
         </is>
       </c>
       <c r="C831" t="n">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="D831" t="n">
-        <v>1766049</v>
+        <v>1770549</v>
       </c>
       <c r="E831" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>58326</v>
+        <v>58378</v>
       </c>
       <c r="D836" t="n">
-        <v>72119491</v>
+        <v>72178291</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40702,10 +40702,10 @@
         </is>
       </c>
       <c r="C841" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D841" t="n">
-        <v>130658</v>
+        <v>132158</v>
       </c>
       <c r="E841" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>22278</v>
+        <v>22289</v>
       </c>
       <c r="D842" t="n">
-        <v>32688308</v>
+        <v>32704808</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40798,10 +40798,10 @@
         </is>
       </c>
       <c r="C843" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D843" t="n">
-        <v>22500</v>
+        <v>24000</v>
       </c>
       <c r="E843" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>14278</v>
+        <v>14292</v>
       </c>
       <c r="D844" t="n">
-        <v>20670411</v>
+        <v>20689917</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -40942,10 +40942,10 @@
         </is>
       </c>
       <c r="C846" t="n">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="D846" t="n">
-        <v>1272101</v>
+        <v>1273601</v>
       </c>
       <c r="E846" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="D847" t="n">
-        <v>1720686</v>
+        <v>1723686</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>7716</v>
+        <v>7722</v>
       </c>
       <c r="D849" t="n">
-        <v>9467513</v>
+        <v>9476513</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D853" t="n">
-        <v>432097</v>
+        <v>433597</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>3591</v>
+        <v>3598</v>
       </c>
       <c r="D855" t="n">
-        <v>4642111</v>
+        <v>4652489</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41614,10 +41614,10 @@
         </is>
       </c>
       <c r="C860" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D860" t="n">
-        <v>532778</v>
+        <v>534278</v>
       </c>
       <c r="E860" t="inlineStr">
         <is>
@@ -41662,10 +41662,10 @@
         </is>
       </c>
       <c r="C861" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D861" t="n">
-        <v>192582</v>
+        <v>196729</v>
       </c>
       <c r="E861" t="inlineStr">
         <is>
@@ -41758,10 +41758,10 @@
         </is>
       </c>
       <c r="C863" t="n">
-        <v>22292</v>
+        <v>22306</v>
       </c>
       <c r="D863" t="n">
-        <v>27930984</v>
+        <v>27949560</v>
       </c>
       <c r="E863" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>7735</v>
+        <v>7737</v>
       </c>
       <c r="D867" t="n">
-        <v>11291256</v>
+        <v>11294256</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -42046,10 +42046,10 @@
         </is>
       </c>
       <c r="C869" t="n">
-        <v>4616</v>
+        <v>4618</v>
       </c>
       <c r="D869" t="n">
-        <v>6674151</v>
+        <v>6677151</v>
       </c>
       <c r="E869" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>14471</v>
+        <v>14482</v>
       </c>
       <c r="D874" t="n">
-        <v>17450843</v>
+        <v>17464679</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42478,10 +42478,10 @@
         </is>
       </c>
       <c r="C878" t="n">
-        <v>5231</v>
+        <v>5235</v>
       </c>
       <c r="D878" t="n">
-        <v>7629110</v>
+        <v>7635110</v>
       </c>
       <c r="E878" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>2352</v>
+        <v>2355</v>
       </c>
       <c r="D880" t="n">
-        <v>3381503</v>
+        <v>3386003</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42670,10 +42670,10 @@
         </is>
       </c>
       <c r="C882" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D882" t="n">
-        <v>315049</v>
+        <v>316549</v>
       </c>
       <c r="E882" t="inlineStr">
         <is>
@@ -42718,10 +42718,10 @@
         </is>
       </c>
       <c r="C883" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D883" t="n">
-        <v>409885</v>
+        <v>411385</v>
       </c>
       <c r="E883" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>9749</v>
+        <v>9755</v>
       </c>
       <c r="D884" t="n">
-        <v>11977889</v>
+        <v>11982326</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42910,10 +42910,10 @@
         </is>
       </c>
       <c r="C887" t="n">
-        <v>3341</v>
+        <v>3343</v>
       </c>
       <c r="D887" t="n">
-        <v>4895238</v>
+        <v>4898238</v>
       </c>
       <c r="E887" t="inlineStr">
         <is>
@@ -42958,10 +42958,10 @@
         </is>
       </c>
       <c r="C888" t="n">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D888" t="n">
-        <v>2143219</v>
+        <v>2144719</v>
       </c>
       <c r="E888" t="inlineStr">
         <is>
@@ -43054,10 +43054,10 @@
         </is>
       </c>
       <c r="C890" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D890" t="n">
-        <v>267889</v>
+        <v>269389</v>
       </c>
       <c r="E890" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>44432</v>
+        <v>44476</v>
       </c>
       <c r="D891" t="n">
-        <v>55814146</v>
+        <v>55863362</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>21009</v>
+        <v>21024</v>
       </c>
       <c r="D896" t="n">
-        <v>30804498</v>
+        <v>30826907</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43438,10 +43438,10 @@
         </is>
       </c>
       <c r="C898" t="n">
-        <v>5873</v>
+        <v>5875</v>
       </c>
       <c r="D898" t="n">
-        <v>8462669</v>
+        <v>8465669</v>
       </c>
       <c r="E898" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D899" t="n">
-        <v>887955</v>
+        <v>889455</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43582,10 +43582,10 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D901" t="n">
-        <v>1294062</v>
+        <v>1297062</v>
       </c>
       <c r="E901" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>21150</v>
+        <v>21167</v>
       </c>
       <c r="D902" t="n">
-        <v>26319772</v>
+        <v>26339893</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43966,10 +43966,10 @@
         </is>
       </c>
       <c r="C909" t="n">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D909" t="n">
-        <v>885933</v>
+        <v>886879</v>
       </c>
       <c r="E909" t="inlineStr">
         <is>
@@ -44014,10 +44014,10 @@
         </is>
       </c>
       <c r="C910" t="n">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D910" t="n">
-        <v>884850</v>
+        <v>886350</v>
       </c>
       <c r="E910" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>7018</v>
+        <v>7022</v>
       </c>
       <c r="D911" t="n">
-        <v>8821161</v>
+        <v>8826461</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>3012</v>
+        <v>3013</v>
       </c>
       <c r="D916" t="n">
-        <v>4435089</v>
+        <v>4436589</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44350,10 +44350,10 @@
         </is>
       </c>
       <c r="C917" t="n">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D917" t="n">
-        <v>912449</v>
+        <v>913949</v>
       </c>
       <c r="E917" t="inlineStr">
         <is>
@@ -44446,10 +44446,10 @@
         </is>
       </c>
       <c r="C919" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D919" t="n">
-        <v>251925</v>
+        <v>253425</v>
       </c>
       <c r="E919" t="inlineStr">
         <is>
@@ -44494,10 +44494,10 @@
         </is>
       </c>
       <c r="C920" t="n">
-        <v>12984</v>
+        <v>13000</v>
       </c>
       <c r="D920" t="n">
-        <v>16180267</v>
+        <v>16192898</v>
       </c>
       <c r="E920" t="inlineStr">
         <is>
@@ -44782,10 +44782,10 @@
         </is>
       </c>
       <c r="C926" t="n">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D926" t="n">
-        <v>1981867</v>
+        <v>1982188</v>
       </c>
       <c r="E926" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>19259</v>
+        <v>19266</v>
       </c>
       <c r="D931" t="n">
-        <v>24062318</v>
+        <v>24071479</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45214,10 +45214,10 @@
         </is>
       </c>
       <c r="C935" t="n">
-        <v>10061</v>
+        <v>10064</v>
       </c>
       <c r="D935" t="n">
-        <v>14707576</v>
+        <v>14712076</v>
       </c>
       <c r="E935" t="inlineStr">
         <is>
@@ -45310,10 +45310,10 @@
         </is>
       </c>
       <c r="C937" t="n">
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="D937" t="n">
-        <v>2963319</v>
+        <v>2966319</v>
       </c>
       <c r="E937" t="inlineStr">
         <is>
@@ -45406,10 +45406,10 @@
         </is>
       </c>
       <c r="C939" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D939" t="n">
-        <v>620294</v>
+        <v>621794</v>
       </c>
       <c r="E939" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>8606</v>
+        <v>8612</v>
       </c>
       <c r="D940" t="n">
-        <v>10737251</v>
+        <v>10744932</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>1493</v>
+        <v>1495</v>
       </c>
       <c r="D946" t="n">
-        <v>2153309</v>
+        <v>2156309</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45838,10 +45838,10 @@
         </is>
       </c>
       <c r="C948" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D948" t="n">
-        <v>223575</v>
+        <v>225075</v>
       </c>
       <c r="E948" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>66938</v>
+        <v>66997</v>
       </c>
       <c r="D950" t="n">
-        <v>85937162</v>
+        <v>86006111</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>25518</v>
+        <v>25527</v>
       </c>
       <c r="D957" t="n">
-        <v>37401841</v>
+        <v>37414241</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46366,10 +46366,10 @@
         </is>
       </c>
       <c r="C959" t="n">
-        <v>17553</v>
+        <v>17568</v>
       </c>
       <c r="D959" t="n">
-        <v>25449522</v>
+        <v>25469848</v>
       </c>
       <c r="E959" t="inlineStr">
         <is>
@@ -46462,10 +46462,10 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D961" t="n">
-        <v>699323</v>
+        <v>702323</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
@@ -46510,10 +46510,10 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="D962" t="n">
-        <v>1233721</v>
+        <v>1236721</v>
       </c>
       <c r="E962" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>83574</v>
+        <v>83672</v>
       </c>
       <c r="D963" t="n">
-        <v>104927047</v>
+        <v>105034161</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>33745</v>
+        <v>33761</v>
       </c>
       <c r="D970" t="n">
-        <v>49496037</v>
+        <v>49519300</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -47038,10 +47038,10 @@
         </is>
       </c>
       <c r="C973" t="n">
-        <v>25129</v>
+        <v>25147</v>
       </c>
       <c r="D973" t="n">
-        <v>36447237</v>
+        <v>36474237</v>
       </c>
       <c r="E973" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D974" t="n">
-        <v>872652</v>
+        <v>874152</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>1981</v>
+        <v>1983</v>
       </c>
       <c r="D976" t="n">
-        <v>2789117</v>
+        <v>2791805</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>10726</v>
+        <v>10741</v>
       </c>
       <c r="D977" t="n">
-        <v>13993663</v>
+        <v>14012137</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47662,10 +47662,10 @@
         </is>
       </c>
       <c r="C986" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D986" t="n">
-        <v>249033</v>
+        <v>252033</v>
       </c>
       <c r="E986" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>55861</v>
+        <v>55893</v>
       </c>
       <c r="D987" t="n">
-        <v>69938241</v>
+        <v>69975469</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>18482</v>
+        <v>18486</v>
       </c>
       <c r="D992" t="n">
-        <v>27067283</v>
+        <v>27073283</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -48046,10 +48046,10 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>12587</v>
+        <v>12598</v>
       </c>
       <c r="D994" t="n">
-        <v>18202855</v>
+        <v>18218821</v>
       </c>
       <c r="E994" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>28166</v>
+        <v>28193</v>
       </c>
       <c r="D998" t="n">
-        <v>35049665</v>
+        <v>35083463</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48430,10 +48430,10 @@
         </is>
       </c>
       <c r="C1002" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1002" t="n">
-        <v>107760</v>
+        <v>109260</v>
       </c>
       <c r="E1002" t="inlineStr">
         <is>
@@ -48478,10 +48478,10 @@
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>10479</v>
+        <v>10483</v>
       </c>
       <c r="D1003" t="n">
-        <v>15347750</v>
+        <v>15353684</v>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>6205</v>
+        <v>6210</v>
       </c>
       <c r="D1005" t="n">
-        <v>8997605</v>
+        <v>9005105</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48670,10 +48670,10 @@
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D1007" t="n">
-        <v>716129</v>
+        <v>718816</v>
       </c>
       <c r="E1007" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-13 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16359</v>
+        <v>16375</v>
       </c>
       <c r="D2" t="n">
-        <v>20565248</v>
+        <v>20583012</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6242</v>
+        <v>6244</v>
       </c>
       <c r="D6" t="n">
-        <v>9128238</v>
+        <v>9131238</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3288</v>
+        <v>3290</v>
       </c>
       <c r="D8" t="n">
-        <v>4758380</v>
+        <v>4760205</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10990</v>
+        <v>10999</v>
       </c>
       <c r="D12" t="n">
-        <v>13868664</v>
+        <v>13880448</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3226</v>
+        <v>3232</v>
       </c>
       <c r="D16" t="n">
-        <v>4700627</v>
+        <v>4708073</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D18" t="n">
-        <v>2093720</v>
+        <v>2095220</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D19" t="n">
-        <v>548178</v>
+        <v>551178</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D21" t="n">
-        <v>284753</v>
+        <v>286253</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>14244</v>
+        <v>14251</v>
       </c>
       <c r="D22" t="n">
-        <v>17465716</v>
+        <v>17473314</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6554</v>
+        <v>6556</v>
       </c>
       <c r="D32" t="n">
-        <v>8705969</v>
+        <v>8708786</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>21866</v>
+        <v>21875</v>
       </c>
       <c r="D41" t="n">
-        <v>26911428</v>
+        <v>26919421</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7807</v>
+        <v>7810</v>
       </c>
       <c r="D47" t="n">
-        <v>11467960</v>
+        <v>11472460</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3836</v>
+        <v>3841</v>
       </c>
       <c r="D49" t="n">
-        <v>5552655</v>
+        <v>5559069</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2780</v>
+        <v>2781</v>
       </c>
       <c r="D57" t="n">
-        <v>4043543</v>
+        <v>4045043</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="D59" t="n">
-        <v>1443584</v>
+        <v>1445084</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D61" t="n">
-        <v>351461</v>
+        <v>352961</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>36141</v>
+        <v>36160</v>
       </c>
       <c r="D62" t="n">
-        <v>46529577</v>
+        <v>46551041</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>13156</v>
+        <v>13160</v>
       </c>
       <c r="D67" t="n">
-        <v>19294885</v>
+        <v>19300885</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5160</v>
+        <v>5162</v>
       </c>
       <c r="D69" t="n">
-        <v>7463084</v>
+        <v>7466084</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>46254</v>
+        <v>46276</v>
       </c>
       <c r="D75" t="n">
-        <v>59130315</v>
+        <v>59152284</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18109</v>
+        <v>18115</v>
       </c>
       <c r="D79" t="n">
-        <v>26530804</v>
+        <v>26538880</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9333</v>
+        <v>9339</v>
       </c>
       <c r="D81" t="n">
-        <v>13472947</v>
+        <v>13481947</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>24938</v>
+        <v>24951</v>
       </c>
       <c r="D86" t="n">
-        <v>31437832</v>
+        <v>31454264</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8678</v>
+        <v>8682</v>
       </c>
       <c r="D90" t="n">
-        <v>12738886</v>
+        <v>12744886</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4902</v>
+        <v>4903</v>
       </c>
       <c r="D92" t="n">
-        <v>7085139</v>
+        <v>7086639</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D94" t="n">
-        <v>1061815</v>
+        <v>1063315</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>21962</v>
+        <v>21967</v>
       </c>
       <c r="D95" t="n">
-        <v>27572164</v>
+        <v>27577683</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9154</v>
+        <v>9157</v>
       </c>
       <c r="D99" t="n">
-        <v>13399349</v>
+        <v>13403849</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5182,10 +5182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3327</v>
+        <v>3328</v>
       </c>
       <c r="D101" t="n">
-        <v>4765390</v>
+        <v>4765848</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>81682</v>
+        <v>81746</v>
       </c>
       <c r="D106" t="n">
-        <v>104667041</v>
+        <v>104746625</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>30600</v>
+        <v>30611</v>
       </c>
       <c r="D113" t="n">
-        <v>44904917</v>
+        <v>44921417</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>20821</v>
+        <v>20834</v>
       </c>
       <c r="D115" t="n">
-        <v>30044999</v>
+        <v>30063184</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -5998,10 +5998,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D118" t="n">
-        <v>971267</v>
+        <v>972767</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>27697</v>
+        <v>27713</v>
       </c>
       <c r="D123" t="n">
-        <v>36553455</v>
+        <v>36572723</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6430,10 +6430,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>9868</v>
+        <v>9870</v>
       </c>
       <c r="D127" t="n">
-        <v>14471870</v>
+        <v>14474870</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -6526,10 +6526,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3267</v>
+        <v>3273</v>
       </c>
       <c r="D129" t="n">
-        <v>4750157</v>
+        <v>4759157</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D130" t="n">
-        <v>314867</v>
+        <v>316308</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>15743</v>
+        <v>15755</v>
       </c>
       <c r="D133" t="n">
-        <v>19586933</v>
+        <v>19601897</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6862,10 +6862,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>7760</v>
+        <v>7762</v>
       </c>
       <c r="D136" t="n">
-        <v>11354916</v>
+        <v>11357916</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -6958,10 +6958,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>2214</v>
+        <v>2216</v>
       </c>
       <c r="D138" t="n">
-        <v>3161610</v>
+        <v>3163547</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>13529</v>
+        <v>13540</v>
       </c>
       <c r="D143" t="n">
-        <v>16904522</v>
+        <v>16910677</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7390,10 +7390,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6243</v>
+        <v>6244</v>
       </c>
       <c r="D147" t="n">
-        <v>9146755</v>
+        <v>9148255</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="D149" t="n">
-        <v>2874499</v>
+        <v>2875999</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>5982</v>
+        <v>5985</v>
       </c>
       <c r="D153" t="n">
-        <v>7316232</v>
+        <v>7320084</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D157" t="n">
-        <v>977327</v>
+        <v>978827</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -8062,10 +8062,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>7438</v>
+        <v>7440</v>
       </c>
       <c r="D161" t="n">
-        <v>9218550</v>
+        <v>9219088</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D168" t="n">
-        <v>201865</v>
+        <v>204865</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>5612</v>
+        <v>5614</v>
       </c>
       <c r="D169" t="n">
-        <v>7062664</v>
+        <v>7065664</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8926,10 +8926,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>15971</v>
+        <v>15976</v>
       </c>
       <c r="D179" t="n">
-        <v>20068126</v>
+        <v>20073496</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>6393</v>
+        <v>6394</v>
       </c>
       <c r="D184" t="n">
-        <v>9338359</v>
+        <v>9339859</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D188" t="n">
-        <v>630912</v>
+        <v>632412</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D191" t="n">
-        <v>2156742</v>
+        <v>2158242</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>9204</v>
+        <v>9210</v>
       </c>
       <c r="D197" t="n">
-        <v>11492602</v>
+        <v>11499830</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>3429</v>
+        <v>3430</v>
       </c>
       <c r="D201" t="n">
-        <v>5038076</v>
+        <v>5039576</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>17262</v>
+        <v>17271</v>
       </c>
       <c r="D206" t="n">
-        <v>21555356</v>
+        <v>21566631</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>7690</v>
+        <v>7691</v>
       </c>
       <c r="D210" t="n">
-        <v>11292115</v>
+        <v>11293615</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D211" t="n">
-        <v>1776154</v>
+        <v>1777654</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>26135</v>
+        <v>26149</v>
       </c>
       <c r="D214" t="n">
-        <v>32964466</v>
+        <v>32980786</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>10492</v>
+        <v>10494</v>
       </c>
       <c r="D218" t="n">
-        <v>15323353</v>
+        <v>15326353</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D223" t="n">
-        <v>849159</v>
+        <v>850659</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>28486</v>
+        <v>28506</v>
       </c>
       <c r="D224" t="n">
-        <v>35944850</v>
+        <v>35965555</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11326,10 +11326,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>14730</v>
+        <v>14734</v>
       </c>
       <c r="D229" t="n">
-        <v>21613596</v>
+        <v>21619219</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -11422,10 +11422,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>2657</v>
+        <v>2658</v>
       </c>
       <c r="D231" t="n">
-        <v>3815175</v>
+        <v>3816675</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>24285</v>
+        <v>24297</v>
       </c>
       <c r="D235" t="n">
-        <v>30633422</v>
+        <v>30645473</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11902,10 +11902,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>11177</v>
+        <v>11186</v>
       </c>
       <c r="D241" t="n">
-        <v>16384567</v>
+        <v>16395490</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>2509</v>
+        <v>2512</v>
       </c>
       <c r="D243" t="n">
-        <v>3585748</v>
+        <v>3588818</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>2701</v>
+        <v>2702</v>
       </c>
       <c r="D251" t="n">
-        <v>3964650</v>
+        <v>3966150</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D256" t="n">
-        <v>205667</v>
+        <v>207167</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12670,10 +12670,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>9810</v>
+        <v>9817</v>
       </c>
       <c r="D257" t="n">
-        <v>12511114</v>
+        <v>12521232</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>4194</v>
+        <v>4197</v>
       </c>
       <c r="D261" t="n">
-        <v>6156670</v>
+        <v>6160460</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -12958,10 +12958,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>2172</v>
+        <v>2174</v>
       </c>
       <c r="D263" t="n">
-        <v>3144602</v>
+        <v>3147387</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -13102,10 +13102,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>5547</v>
+        <v>5554</v>
       </c>
       <c r="D266" t="n">
-        <v>6879537</v>
+        <v>6887700</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13342,10 +13342,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D271" t="n">
-        <v>1031372</v>
+        <v>1032872</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13534,10 +13534,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>19093</v>
+        <v>19106</v>
       </c>
       <c r="D275" t="n">
-        <v>24122516</v>
+        <v>24135703</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>7932</v>
+        <v>7933</v>
       </c>
       <c r="D279" t="n">
-        <v>11629896</v>
+        <v>11631396</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>2498</v>
+        <v>2499</v>
       </c>
       <c r="D281" t="n">
-        <v>3588559</v>
+        <v>3590059</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>16626</v>
+        <v>16635</v>
       </c>
       <c r="D286" t="n">
-        <v>20591785</v>
+        <v>20604385</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>7189</v>
+        <v>7191</v>
       </c>
       <c r="D290" t="n">
-        <v>10544114</v>
+        <v>10547114</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>3333</v>
+        <v>3334</v>
       </c>
       <c r="D291" t="n">
-        <v>4830799</v>
+        <v>4832299</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>9355</v>
+        <v>9357</v>
       </c>
       <c r="D295" t="n">
-        <v>11752972</v>
+        <v>11754524</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>3913</v>
+        <v>3915</v>
       </c>
       <c r="D299" t="n">
-        <v>5727332</v>
+        <v>5730332</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D304" t="n">
-        <v>291729</v>
+        <v>293229</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>9205</v>
+        <v>9209</v>
       </c>
       <c r="D305" t="n">
-        <v>12020429</v>
+        <v>12026229</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>3746</v>
+        <v>3747</v>
       </c>
       <c r="D309" t="n">
-        <v>5476849</v>
+        <v>5478349</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>2356</v>
+        <v>2358</v>
       </c>
       <c r="D310" t="n">
-        <v>3426950</v>
+        <v>3429950</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D311" t="n">
-        <v>329165</v>
+        <v>332165</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>11074</v>
+        <v>11076</v>
       </c>
       <c r="D313" t="n">
-        <v>14540643</v>
+        <v>14543643</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15550,10 +15550,10 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>3779</v>
+        <v>3782</v>
       </c>
       <c r="D317" t="n">
-        <v>5540181</v>
+        <v>5544672</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2704</v>
+        <v>2707</v>
       </c>
       <c r="D319" t="n">
-        <v>3920296</v>
+        <v>3923728</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>6819</v>
+        <v>6822</v>
       </c>
       <c r="D322" t="n">
-        <v>8430616</v>
+        <v>8433859</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>2300</v>
+        <v>2301</v>
       </c>
       <c r="D327" t="n">
-        <v>3374084</v>
+        <v>3375584</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>7534</v>
+        <v>7542</v>
       </c>
       <c r="D332" t="n">
-        <v>9427893</v>
+        <v>9439350</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16558,10 +16558,10 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D338" t="n">
-        <v>1849861</v>
+        <v>1851361</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -16702,10 +16702,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>32032</v>
+        <v>32050</v>
       </c>
       <c r="D341" t="n">
-        <v>40235461</v>
+        <v>40258516</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>16542</v>
+        <v>16546</v>
       </c>
       <c r="D347" t="n">
-        <v>24187878</v>
+        <v>24193878</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>8053</v>
+        <v>8057</v>
       </c>
       <c r="D350" t="n">
-        <v>11597294</v>
+        <v>11603232</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17182,10 +17182,10 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D351" t="n">
-        <v>918553</v>
+        <v>919163</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>3894</v>
+        <v>3896</v>
       </c>
       <c r="D353" t="n">
-        <v>4851412</v>
+        <v>4854412</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>19392</v>
+        <v>19406</v>
       </c>
       <c r="D361" t="n">
-        <v>24179730</v>
+        <v>24195917</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17854,10 +17854,10 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>9915</v>
+        <v>9918</v>
       </c>
       <c r="D365" t="n">
-        <v>14537235</v>
+        <v>14541735</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>4740</v>
+        <v>4742</v>
       </c>
       <c r="D367" t="n">
-        <v>6854017</v>
+        <v>6855662</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>13947</v>
+        <v>13955</v>
       </c>
       <c r="D370" t="n">
-        <v>17442027</v>
+        <v>17449386</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>6444</v>
+        <v>6447</v>
       </c>
       <c r="D374" t="n">
-        <v>9434876</v>
+        <v>9439376</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>2484</v>
+        <v>2485</v>
       </c>
       <c r="D376" t="n">
-        <v>3568690</v>
+        <v>3570190</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>18003</v>
+        <v>18016</v>
       </c>
       <c r="D379" t="n">
-        <v>22449776</v>
+        <v>22461904</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>7141</v>
+        <v>7143</v>
       </c>
       <c r="D383" t="n">
-        <v>10496715</v>
+        <v>10499715</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -19006,10 +19006,10 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>4097</v>
+        <v>4098</v>
       </c>
       <c r="D389" t="n">
-        <v>5141492</v>
+        <v>5142992</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -19342,10 +19342,10 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>22294</v>
+        <v>22309</v>
       </c>
       <c r="D396" t="n">
-        <v>27655273</v>
+        <v>27675052</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>9369</v>
+        <v>9373</v>
       </c>
       <c r="D399" t="n">
-        <v>13791657</v>
+        <v>13797657</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>6211</v>
+        <v>6219</v>
       </c>
       <c r="D401" t="n">
-        <v>9034133</v>
+        <v>9046133</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19726,10 +19726,10 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>11143</v>
+        <v>11147</v>
       </c>
       <c r="D404" t="n">
-        <v>13736366</v>
+        <v>13741257</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="D411" t="n">
-        <v>2676864</v>
+        <v>2678364</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>32324</v>
+        <v>32399</v>
       </c>
       <c r="D414" t="n">
-        <v>43785476</v>
+        <v>43887633</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20398,10 +20398,10 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>7825</v>
+        <v>7836</v>
       </c>
       <c r="D418" t="n">
-        <v>11506381</v>
+        <v>11521581</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>7149</v>
+        <v>7155</v>
       </c>
       <c r="D420" t="n">
-        <v>10364336</v>
+        <v>10373082</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D422" t="n">
-        <v>748405</v>
+        <v>749905</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D423" t="n">
-        <v>695443</v>
+        <v>696943</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>8877</v>
+        <v>8921</v>
       </c>
       <c r="D424" t="n">
-        <v>12321466</v>
+        <v>12384334</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>2235</v>
+        <v>2240</v>
       </c>
       <c r="D426" t="n">
-        <v>3292802</v>
+        <v>3300302</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3000</v>
+        <v>3010</v>
       </c>
       <c r="D428" t="n">
-        <v>4382451</v>
+        <v>4396550</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D430" t="n">
-        <v>186120</v>
+        <v>190620</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21070,10 +21070,10 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>11034</v>
+        <v>11039</v>
       </c>
       <c r="D432" t="n">
-        <v>13623653</v>
+        <v>13629418</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>3793</v>
+        <v>3794</v>
       </c>
       <c r="D435" t="n">
-        <v>5566481</v>
+        <v>5567312</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="D437" t="n">
-        <v>2686227</v>
+        <v>2687727</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>63006</v>
+        <v>63042</v>
       </c>
       <c r="D440" t="n">
-        <v>78080039</v>
+        <v>78120140</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21646,10 +21646,10 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>24930</v>
+        <v>24944</v>
       </c>
       <c r="D444" t="n">
-        <v>36544120</v>
+        <v>36563113</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>12943</v>
+        <v>12951</v>
       </c>
       <c r="D446" t="n">
-        <v>18767797</v>
+        <v>18779697</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21790,10 +21790,10 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D447" t="n">
-        <v>659056</v>
+        <v>660537</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>18919</v>
+        <v>18934</v>
       </c>
       <c r="D452" t="n">
-        <v>23916000</v>
+        <v>23933669</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22222,10 +22222,10 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>7706</v>
+        <v>7710</v>
       </c>
       <c r="D456" t="n">
-        <v>11311393</v>
+        <v>11317393</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>4858</v>
+        <v>4864</v>
       </c>
       <c r="D458" t="n">
-        <v>7049697</v>
+        <v>7058697</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22462,10 +22462,10 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>32245</v>
+        <v>32262</v>
       </c>
       <c r="D461" t="n">
-        <v>39412080</v>
+        <v>39432217</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -22654,10 +22654,10 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>11455</v>
+        <v>11464</v>
       </c>
       <c r="D465" t="n">
-        <v>16760349</v>
+        <v>16773849</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>4910</v>
+        <v>4912</v>
       </c>
       <c r="D467" t="n">
-        <v>7124082</v>
+        <v>7127082</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22894,10 +22894,10 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>14412</v>
+        <v>14419</v>
       </c>
       <c r="D470" t="n">
-        <v>17621162</v>
+        <v>17627915</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>2075</v>
+        <v>2077</v>
       </c>
       <c r="D477" t="n">
-        <v>2991793</v>
+        <v>2994793</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23278,10 +23278,10 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D478" t="n">
-        <v>198369</v>
+        <v>198855</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D479" t="n">
-        <v>465848</v>
+        <v>467348</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23374,10 +23374,10 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>36037</v>
+        <v>36071</v>
       </c>
       <c r="D480" t="n">
-        <v>46956220</v>
+        <v>47004868</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -23566,10 +23566,10 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>13572</v>
+        <v>13575</v>
       </c>
       <c r="D484" t="n">
-        <v>19968000</v>
+        <v>19972500</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -23662,10 +23662,10 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>12008</v>
+        <v>12015</v>
       </c>
       <c r="D486" t="n">
-        <v>17526178</v>
+        <v>17536678</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D487" t="n">
-        <v>271421</v>
+        <v>272921</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D488" t="n">
-        <v>426226</v>
+        <v>427726</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>62447</v>
+        <v>62497</v>
       </c>
       <c r="D489" t="n">
-        <v>82681841</v>
+        <v>82745387</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>23131</v>
+        <v>23145</v>
       </c>
       <c r="D494" t="n">
-        <v>33941984</v>
+        <v>33962984</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24142,10 +24142,10 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>22466</v>
+        <v>22484</v>
       </c>
       <c r="D496" t="n">
-        <v>32616473</v>
+        <v>32643143</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D499" t="n">
-        <v>888101</v>
+        <v>889143</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>151145</v>
+        <v>151297</v>
       </c>
       <c r="D500" t="n">
-        <v>198772534</v>
+        <v>198970076</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D502" t="n">
-        <v>179220</v>
+        <v>180720</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>81711</v>
+        <v>81768</v>
       </c>
       <c r="D507" t="n">
-        <v>120031632</v>
+        <v>120115560</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>60137</v>
+        <v>60194</v>
       </c>
       <c r="D510" t="n">
-        <v>87293764</v>
+        <v>87376325</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>2790</v>
+        <v>2793</v>
       </c>
       <c r="D514" t="n">
-        <v>3950013</v>
+        <v>3954513</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>41265</v>
+        <v>41313</v>
       </c>
       <c r="D516" t="n">
-        <v>53635609</v>
+        <v>53701725</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25342,10 +25342,10 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>15266</v>
+        <v>15273</v>
       </c>
       <c r="D521" t="n">
-        <v>22422873</v>
+        <v>22432718</v>
       </c>
       <c r="E521" t="inlineStr">
         <is>
@@ -25438,10 +25438,10 @@
         </is>
       </c>
       <c r="C523" t="n">
-        <v>12942</v>
+        <v>12953</v>
       </c>
       <c r="D523" t="n">
-        <v>18759030</v>
+        <v>18775072</v>
       </c>
       <c r="E523" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>66289</v>
+        <v>66347</v>
       </c>
       <c r="D528" t="n">
-        <v>89086297</v>
+        <v>89166735</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>23338</v>
+        <v>23352</v>
       </c>
       <c r="D532" t="n">
-        <v>34436135</v>
+        <v>34457135</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -25966,10 +25966,10 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>24118</v>
+        <v>24137</v>
       </c>
       <c r="D534" t="n">
-        <v>35297963</v>
+        <v>35325491</v>
       </c>
       <c r="E534" t="inlineStr">
         <is>
@@ -26158,10 +26158,10 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>55145</v>
+        <v>55181</v>
       </c>
       <c r="D538" t="n">
-        <v>73138016</v>
+        <v>73184883</v>
       </c>
       <c r="E538" t="inlineStr">
         <is>
@@ -26398,10 +26398,10 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>17799</v>
+        <v>17809</v>
       </c>
       <c r="D543" t="n">
-        <v>26155026</v>
+        <v>26168586</v>
       </c>
       <c r="E543" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>18334</v>
+        <v>18345</v>
       </c>
       <c r="D545" t="n">
-        <v>26651587</v>
+        <v>26668087</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D547" t="n">
-        <v>882204</v>
+        <v>883704</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>41633</v>
+        <v>41661</v>
       </c>
       <c r="D548" t="n">
-        <v>55283230</v>
+        <v>55317529</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>14227</v>
+        <v>14232</v>
       </c>
       <c r="D552" t="n">
-        <v>20983621</v>
+        <v>20991121</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>14425</v>
+        <v>14434</v>
       </c>
       <c r="D554" t="n">
-        <v>20947256</v>
+        <v>20960035</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>41368</v>
+        <v>41393</v>
       </c>
       <c r="D557" t="n">
-        <v>53634298</v>
+        <v>53664137</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>16213</v>
+        <v>16226</v>
       </c>
       <c r="D561" t="n">
-        <v>23788075</v>
+        <v>23805655</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27358,10 +27358,10 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>13021</v>
+        <v>13034</v>
       </c>
       <c r="D563" t="n">
-        <v>18831609</v>
+        <v>18850615</v>
       </c>
       <c r="E563" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D565" t="n">
-        <v>374160</v>
+        <v>375660</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D566" t="n">
-        <v>498767</v>
+        <v>500267</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>43948</v>
+        <v>43975</v>
       </c>
       <c r="D567" t="n">
-        <v>58667555</v>
+        <v>58702970</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>13929</v>
+        <v>13933</v>
       </c>
       <c r="D573" t="n">
-        <v>20427111</v>
+        <v>20432676</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27886,10 +27886,10 @@
         </is>
       </c>
       <c r="C574" t="n">
-        <v>3707</v>
+        <v>3710</v>
       </c>
       <c r="D574" t="n">
-        <v>5345180</v>
+        <v>5349680</v>
       </c>
       <c r="E574" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D577" t="n">
-        <v>569931</v>
+        <v>571431</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>17317</v>
+        <v>17344</v>
       </c>
       <c r="D580" t="n">
-        <v>22880660</v>
+        <v>22914662</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>7076</v>
+        <v>7085</v>
       </c>
       <c r="D584" t="n">
-        <v>10291203</v>
+        <v>10304703</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>4925</v>
+        <v>4931</v>
       </c>
       <c r="D586" t="n">
-        <v>7086563</v>
+        <v>7095563</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D588" t="n">
-        <v>378731</v>
+        <v>380231</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D589" t="n">
-        <v>375864</v>
+        <v>377364</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>15613</v>
+        <v>15649</v>
       </c>
       <c r="D591" t="n">
-        <v>22651655</v>
+        <v>22705655</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="D592" t="n">
-        <v>2616230</v>
+        <v>2617730</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D593" t="n">
-        <v>347302</v>
+        <v>348802</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>22021</v>
+        <v>22038</v>
       </c>
       <c r="D597" t="n">
-        <v>27629741</v>
+        <v>27649547</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>8989</v>
+        <v>8993</v>
       </c>
       <c r="D602" t="n">
-        <v>13169165</v>
+        <v>13173968</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>3349</v>
+        <v>3350</v>
       </c>
       <c r="D604" t="n">
-        <v>4810159</v>
+        <v>4811659</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29374,10 +29374,10 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D605" t="n">
-        <v>500984</v>
+        <v>502484</v>
       </c>
       <c r="E605" t="inlineStr">
         <is>
@@ -29422,10 +29422,10 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D606" t="n">
-        <v>649439</v>
+        <v>650939</v>
       </c>
       <c r="E606" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>14648</v>
+        <v>14657</v>
       </c>
       <c r="D608" t="n">
-        <v>18362547</v>
+        <v>18373396</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>5787</v>
+        <v>5790</v>
       </c>
       <c r="D612" t="n">
-        <v>8499651</v>
+        <v>8504151</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>2673</v>
+        <v>2675</v>
       </c>
       <c r="D614" t="n">
-        <v>3851928</v>
+        <v>3854928</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D616" t="n">
-        <v>262136</v>
+        <v>263636</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -29950,10 +29950,10 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>13753</v>
+        <v>13760</v>
       </c>
       <c r="D617" t="n">
-        <v>17369488</v>
+        <v>17376579</v>
       </c>
       <c r="E617" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>5226</v>
+        <v>5228</v>
       </c>
       <c r="D621" t="n">
-        <v>7660220</v>
+        <v>7662187</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D622" t="n">
-        <v>1683355</v>
+        <v>1684855</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>7507</v>
+        <v>7510</v>
       </c>
       <c r="D626" t="n">
-        <v>9657223</v>
+        <v>9661164</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>28797</v>
+        <v>28815</v>
       </c>
       <c r="D635" t="n">
-        <v>35467437</v>
+        <v>35490213</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -31006,10 +31006,10 @@
         </is>
       </c>
       <c r="C639" t="n">
-        <v>11022</v>
+        <v>11028</v>
       </c>
       <c r="D639" t="n">
-        <v>16172149</v>
+        <v>16180409</v>
       </c>
       <c r="E639" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>4830</v>
+        <v>4833</v>
       </c>
       <c r="D641" t="n">
-        <v>7008353</v>
+        <v>7012853</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D644" t="n">
-        <v>801936</v>
+        <v>803436</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>11309</v>
+        <v>11312</v>
       </c>
       <c r="D645" t="n">
-        <v>13706798</v>
+        <v>13710058</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D654" t="n">
-        <v>319290</v>
+        <v>320790</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31774,10 +31774,10 @@
         </is>
       </c>
       <c r="C655" t="n">
-        <v>28296</v>
+        <v>28311</v>
       </c>
       <c r="D655" t="n">
-        <v>35176769</v>
+        <v>35195290</v>
       </c>
       <c r="E655" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>10735</v>
+        <v>10736</v>
       </c>
       <c r="D659" t="n">
-        <v>15773336</v>
+        <v>15774836</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32062,10 +32062,10 @@
         </is>
       </c>
       <c r="C661" t="n">
-        <v>3077</v>
+        <v>3080</v>
       </c>
       <c r="D661" t="n">
-        <v>4436427</v>
+        <v>4440927</v>
       </c>
       <c r="E661" t="inlineStr">
         <is>
@@ -32254,10 +32254,10 @@
         </is>
       </c>
       <c r="C665" t="n">
-        <v>7495</v>
+        <v>7499</v>
       </c>
       <c r="D665" t="n">
-        <v>9508814</v>
+        <v>9512825</v>
       </c>
       <c r="E665" t="inlineStr">
         <is>
@@ -32350,10 +32350,10 @@
         </is>
       </c>
       <c r="C667" t="n">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="D667" t="n">
-        <v>3866165</v>
+        <v>3869165</v>
       </c>
       <c r="E667" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D670" t="n">
-        <v>367484</v>
+        <v>368984</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D672" t="n">
-        <v>229998</v>
+        <v>231070</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32638,10 +32638,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>3772</v>
+        <v>3774</v>
       </c>
       <c r="D673" t="n">
-        <v>4572767</v>
+        <v>4573898</v>
       </c>
       <c r="E673" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>9310</v>
+        <v>9311</v>
       </c>
       <c r="D682" t="n">
-        <v>11613188</v>
+        <v>11614688</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33502,10 +33502,10 @@
         </is>
       </c>
       <c r="C691" t="n">
-        <v>19205</v>
+        <v>19214</v>
       </c>
       <c r="D691" t="n">
-        <v>23503923</v>
+        <v>23515032</v>
       </c>
       <c r="E691" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>5706</v>
+        <v>5708</v>
       </c>
       <c r="D695" t="n">
-        <v>8334480</v>
+        <v>8337480</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>74419</v>
+        <v>74483</v>
       </c>
       <c r="D702" t="n">
-        <v>93687667</v>
+        <v>93763826</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>26485</v>
+        <v>26492</v>
       </c>
       <c r="D707" t="n">
-        <v>38885465</v>
+        <v>38894744</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>13143</v>
+        <v>13148</v>
       </c>
       <c r="D710" t="n">
-        <v>18954831</v>
+        <v>18962331</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34558,10 +34558,10 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>1943</v>
+        <v>1946</v>
       </c>
       <c r="D713" t="n">
-        <v>2796483</v>
+        <v>2800539</v>
       </c>
       <c r="E713" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="D715" t="n">
-        <v>1675243</v>
+        <v>1678243</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34702,10 +34702,10 @@
         </is>
       </c>
       <c r="C716" t="n">
-        <v>11150</v>
+        <v>11157</v>
       </c>
       <c r="D716" t="n">
-        <v>13642091</v>
+        <v>13648658</v>
       </c>
       <c r="E716" t="inlineStr">
         <is>
@@ -34846,10 +34846,10 @@
         </is>
       </c>
       <c r="C719" t="n">
-        <v>4101</v>
+        <v>4102</v>
       </c>
       <c r="D719" t="n">
-        <v>5998633</v>
+        <v>6000133</v>
       </c>
       <c r="E719" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>17576</v>
+        <v>17591</v>
       </c>
       <c r="D724" t="n">
-        <v>21678208</v>
+        <v>21693662</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35278,10 +35278,10 @@
         </is>
       </c>
       <c r="C728" t="n">
-        <v>6839</v>
+        <v>6842</v>
       </c>
       <c r="D728" t="n">
-        <v>9996829</v>
+        <v>10000329</v>
       </c>
       <c r="E728" t="inlineStr">
         <is>
@@ -35518,10 +35518,10 @@
         </is>
       </c>
       <c r="C733" t="n">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D733" t="n">
-        <v>456614</v>
+        <v>460114</v>
       </c>
       <c r="E733" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>11497</v>
+        <v>11506</v>
       </c>
       <c r="D735" t="n">
-        <v>14195199</v>
+        <v>14201708</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>4231</v>
+        <v>4233</v>
       </c>
       <c r="D739" t="n">
-        <v>6201994</v>
+        <v>6204994</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -36046,10 +36046,10 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>29484</v>
+        <v>29502</v>
       </c>
       <c r="D744" t="n">
-        <v>36645279</v>
+        <v>36669407</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
@@ -36286,10 +36286,10 @@
         </is>
       </c>
       <c r="C749" t="n">
-        <v>12698</v>
+        <v>12704</v>
       </c>
       <c r="D749" t="n">
-        <v>18584590</v>
+        <v>18593590</v>
       </c>
       <c r="E749" t="inlineStr">
         <is>
@@ -36382,10 +36382,10 @@
         </is>
       </c>
       <c r="C751" t="n">
-        <v>4209</v>
+        <v>4215</v>
       </c>
       <c r="D751" t="n">
-        <v>6014119</v>
+        <v>6022585</v>
       </c>
       <c r="E751" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D753" t="n">
-        <v>1075657</v>
+        <v>1078657</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36526,10 +36526,10 @@
         </is>
       </c>
       <c r="C754" t="n">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D754" t="n">
-        <v>959504</v>
+        <v>962896</v>
       </c>
       <c r="E754" t="inlineStr">
         <is>
@@ -36622,10 +36622,10 @@
         </is>
       </c>
       <c r="C756" t="n">
-        <v>12296</v>
+        <v>12303</v>
       </c>
       <c r="D756" t="n">
-        <v>15219498</v>
+        <v>15226784</v>
       </c>
       <c r="E756" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D760" t="n">
-        <v>1647986</v>
+        <v>1649486</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -36958,10 +36958,10 @@
         </is>
       </c>
       <c r="C763" t="n">
-        <v>6714</v>
+        <v>6715</v>
       </c>
       <c r="D763" t="n">
-        <v>7890153</v>
+        <v>7891653</v>
       </c>
       <c r="E763" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>1698</v>
+        <v>1700</v>
       </c>
       <c r="D767" t="n">
-        <v>2475153</v>
+        <v>2478153</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37198,10 +37198,10 @@
         </is>
       </c>
       <c r="C768" t="n">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D768" t="n">
-        <v>1454844</v>
+        <v>1456344</v>
       </c>
       <c r="E768" t="inlineStr">
         <is>
@@ -37342,10 +37342,10 @@
         </is>
       </c>
       <c r="C771" t="n">
-        <v>16769</v>
+        <v>16777</v>
       </c>
       <c r="D771" t="n">
-        <v>20343418</v>
+        <v>20351695</v>
       </c>
       <c r="E771" t="inlineStr">
         <is>
@@ -37582,10 +37582,10 @@
         </is>
       </c>
       <c r="C776" t="n">
-        <v>5530</v>
+        <v>5531</v>
       </c>
       <c r="D776" t="n">
-        <v>8103086</v>
+        <v>8104586</v>
       </c>
       <c r="E776" t="inlineStr">
         <is>
@@ -37678,10 +37678,10 @@
         </is>
       </c>
       <c r="C778" t="n">
-        <v>3394</v>
+        <v>3395</v>
       </c>
       <c r="D778" t="n">
-        <v>4957222</v>
+        <v>4958722</v>
       </c>
       <c r="E778" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>11359</v>
+        <v>11362</v>
       </c>
       <c r="D782" t="n">
-        <v>14379030</v>
+        <v>14381335</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38062,10 +38062,10 @@
         </is>
       </c>
       <c r="C786" t="n">
-        <v>3951</v>
+        <v>3955</v>
       </c>
       <c r="D786" t="n">
-        <v>5776458</v>
+        <v>5782458</v>
       </c>
       <c r="E786" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D791" t="n">
-        <v>318881</v>
+        <v>323381</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38350,10 +38350,10 @@
         </is>
       </c>
       <c r="C792" t="n">
-        <v>32074</v>
+        <v>32097</v>
       </c>
       <c r="D792" t="n">
-        <v>39564763</v>
+        <v>39589823</v>
       </c>
       <c r="E792" t="inlineStr">
         <is>
@@ -38542,10 +38542,10 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>13165</v>
+        <v>13166</v>
       </c>
       <c r="D796" t="n">
-        <v>19261819</v>
+        <v>19263319</v>
       </c>
       <c r="E796" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>6029</v>
+        <v>6034</v>
       </c>
       <c r="D798" t="n">
-        <v>8713078</v>
+        <v>8717657</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D801" t="n">
-        <v>919124</v>
+        <v>920624</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -38830,10 +38830,10 @@
         </is>
       </c>
       <c r="C802" t="n">
-        <v>7601</v>
+        <v>7603</v>
       </c>
       <c r="D802" t="n">
-        <v>9400273</v>
+        <v>9401568</v>
       </c>
       <c r="E802" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>2679</v>
+        <v>2681</v>
       </c>
       <c r="D808" t="n">
-        <v>3907984</v>
+        <v>3910984</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39166,10 +39166,10 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D809" t="n">
-        <v>1637438</v>
+        <v>1640438</v>
       </c>
       <c r="E809" t="inlineStr">
         <is>
@@ -39310,10 +39310,10 @@
         </is>
       </c>
       <c r="C812" t="n">
-        <v>58796</v>
+        <v>58857</v>
       </c>
       <c r="D812" t="n">
-        <v>73490977</v>
+        <v>73559800</v>
       </c>
       <c r="E812" t="inlineStr">
         <is>
@@ -39550,10 +39550,10 @@
         </is>
       </c>
       <c r="C817" t="n">
-        <v>21122</v>
+        <v>21127</v>
       </c>
       <c r="D817" t="n">
-        <v>30900891</v>
+        <v>30906181</v>
       </c>
       <c r="E817" t="inlineStr">
         <is>
@@ -39694,10 +39694,10 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>12588</v>
+        <v>12595</v>
       </c>
       <c r="D820" t="n">
-        <v>18169533</v>
+        <v>18180033</v>
       </c>
       <c r="E820" t="inlineStr">
         <is>
@@ -39790,10 +39790,10 @@
         </is>
       </c>
       <c r="C822" t="n">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D822" t="n">
-        <v>647695</v>
+        <v>649195</v>
       </c>
       <c r="E822" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="D825" t="n">
-        <v>1840607</v>
+        <v>1843607</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -39982,10 +39982,10 @@
         </is>
       </c>
       <c r="C826" t="n">
-        <v>11117</v>
+        <v>11128</v>
       </c>
       <c r="D826" t="n">
-        <v>13857020</v>
+        <v>13872406</v>
       </c>
       <c r="E826" t="inlineStr">
         <is>
@@ -40174,10 +40174,10 @@
         </is>
       </c>
       <c r="C830" t="n">
-        <v>3910</v>
+        <v>3912</v>
       </c>
       <c r="D830" t="n">
-        <v>5683719</v>
+        <v>5686719</v>
       </c>
       <c r="E830" t="inlineStr">
         <is>
@@ -40366,10 +40366,10 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D834" t="n">
-        <v>194065</v>
+        <v>195335</v>
       </c>
       <c r="E834" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D836" t="n">
-        <v>369237</v>
+        <v>370737</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>58425</v>
+        <v>58462</v>
       </c>
       <c r="D837" t="n">
-        <v>72238343</v>
+        <v>72283358</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40798,10 +40798,10 @@
         </is>
       </c>
       <c r="C843" t="n">
-        <v>22302</v>
+        <v>22306</v>
       </c>
       <c r="D843" t="n">
-        <v>32724274</v>
+        <v>32730274</v>
       </c>
       <c r="E843" t="inlineStr">
         <is>
@@ -40894,10 +40894,10 @@
         </is>
       </c>
       <c r="C845" t="n">
-        <v>14302</v>
+        <v>14312</v>
       </c>
       <c r="D845" t="n">
-        <v>20704747</v>
+        <v>20718592</v>
       </c>
       <c r="E845" t="inlineStr">
         <is>
@@ -41038,10 +41038,10 @@
         </is>
       </c>
       <c r="C848" t="n">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="D848" t="n">
-        <v>1729686</v>
+        <v>1731936</v>
       </c>
       <c r="E848" t="inlineStr">
         <is>
@@ -41134,10 +41134,10 @@
         </is>
       </c>
       <c r="C850" t="n">
-        <v>7725</v>
+        <v>7731</v>
       </c>
       <c r="D850" t="n">
-        <v>9479100</v>
+        <v>9484026</v>
       </c>
       <c r="E850" t="inlineStr">
         <is>
@@ -41230,10 +41230,10 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>2567</v>
+        <v>2571</v>
       </c>
       <c r="D852" t="n">
-        <v>3738062</v>
+        <v>3743395</v>
       </c>
       <c r="E852" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="D853" t="n">
-        <v>1552979</v>
+        <v>1555976</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41422,10 +41422,10 @@
         </is>
       </c>
       <c r="C856" t="n">
-        <v>3599</v>
+        <v>3600</v>
       </c>
       <c r="D856" t="n">
-        <v>4652868</v>
+        <v>4653131</v>
       </c>
       <c r="E856" t="inlineStr">
         <is>
@@ -41806,10 +41806,10 @@
         </is>
       </c>
       <c r="C864" t="n">
-        <v>22317</v>
+        <v>22329</v>
       </c>
       <c r="D864" t="n">
-        <v>27964550</v>
+        <v>27979097</v>
       </c>
       <c r="E864" t="inlineStr">
         <is>
@@ -41998,10 +41998,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>7739</v>
+        <v>7742</v>
       </c>
       <c r="D868" t="n">
-        <v>11296769</v>
+        <v>11301269</v>
       </c>
       <c r="E868" t="inlineStr">
         <is>
@@ -42094,10 +42094,10 @@
         </is>
       </c>
       <c r="C870" t="n">
-        <v>4621</v>
+        <v>4623</v>
       </c>
       <c r="D870" t="n">
-        <v>6681651</v>
+        <v>6684651</v>
       </c>
       <c r="E870" t="inlineStr">
         <is>
@@ -42238,10 +42238,10 @@
         </is>
       </c>
       <c r="C873" t="n">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D873" t="n">
-        <v>597055</v>
+        <v>600055</v>
       </c>
       <c r="E873" t="inlineStr">
         <is>
@@ -42334,10 +42334,10 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>14488</v>
+        <v>14499</v>
       </c>
       <c r="D875" t="n">
-        <v>17470469</v>
+        <v>17481011</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
@@ -42526,10 +42526,10 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>5237</v>
+        <v>5238</v>
       </c>
       <c r="D879" t="n">
-        <v>7638110</v>
+        <v>7639610</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
@@ -42622,10 +42622,10 @@
         </is>
       </c>
       <c r="C881" t="n">
-        <v>2355</v>
+        <v>2358</v>
       </c>
       <c r="D881" t="n">
-        <v>3386003</v>
+        <v>3390503</v>
       </c>
       <c r="E881" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D884" t="n">
-        <v>412885</v>
+        <v>413475</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42814,10 +42814,10 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>9765</v>
+        <v>9772</v>
       </c>
       <c r="D885" t="n">
-        <v>11996126</v>
+        <v>12004088</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
@@ -42958,10 +42958,10 @@
         </is>
       </c>
       <c r="C888" t="n">
-        <v>3345</v>
+        <v>3346</v>
       </c>
       <c r="D888" t="n">
-        <v>4901238</v>
+        <v>4902156</v>
       </c>
       <c r="E888" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D891" t="n">
-        <v>269389</v>
+        <v>270819</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43150,10 +43150,10 @@
         </is>
       </c>
       <c r="C892" t="n">
-        <v>44509</v>
+        <v>44533</v>
       </c>
       <c r="D892" t="n">
-        <v>55905121</v>
+        <v>55932024</v>
       </c>
       <c r="E892" t="inlineStr">
         <is>
@@ -43390,10 +43390,10 @@
         </is>
       </c>
       <c r="C897" t="n">
-        <v>21035</v>
+        <v>21043</v>
       </c>
       <c r="D897" t="n">
-        <v>30843407</v>
+        <v>30854047</v>
       </c>
       <c r="E897" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>5883</v>
+        <v>5884</v>
       </c>
       <c r="D899" t="n">
-        <v>8477587</v>
+        <v>8479087</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43678,10 +43678,10 @@
         </is>
       </c>
       <c r="C903" t="n">
-        <v>21178</v>
+        <v>21185</v>
       </c>
       <c r="D903" t="n">
-        <v>26352082</v>
+        <v>26361307</v>
       </c>
       <c r="E903" t="inlineStr">
         <is>
@@ -43822,10 +43822,10 @@
         </is>
       </c>
       <c r="C906" t="n">
-        <v>9758</v>
+        <v>9760</v>
       </c>
       <c r="D906" t="n">
-        <v>14298696</v>
+        <v>14301696</v>
       </c>
       <c r="E906" t="inlineStr">
         <is>
@@ -43918,10 +43918,10 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>2272</v>
+        <v>2273</v>
       </c>
       <c r="D908" t="n">
-        <v>3256165</v>
+        <v>3257665</v>
       </c>
       <c r="E908" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D911" t="n">
-        <v>889350</v>
+        <v>890850</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44110,10 +44110,10 @@
         </is>
       </c>
       <c r="C912" t="n">
-        <v>7024</v>
+        <v>7031</v>
       </c>
       <c r="D912" t="n">
-        <v>8828638</v>
+        <v>8837517</v>
       </c>
       <c r="E912" t="inlineStr">
         <is>
@@ -44350,10 +44350,10 @@
         </is>
       </c>
       <c r="C917" t="n">
-        <v>3014</v>
+        <v>3015</v>
       </c>
       <c r="D917" t="n">
-        <v>4438089</v>
+        <v>4439589</v>
       </c>
       <c r="E917" t="inlineStr">
         <is>
@@ -44542,10 +44542,10 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>13009</v>
+        <v>13016</v>
       </c>
       <c r="D921" t="n">
-        <v>16202141</v>
+        <v>16209487</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
@@ -44734,10 +44734,10 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>5240</v>
+        <v>5246</v>
       </c>
       <c r="D925" t="n">
-        <v>7657357</v>
+        <v>7666357</v>
       </c>
       <c r="E925" t="inlineStr">
         <is>
@@ -44830,10 +44830,10 @@
         </is>
       </c>
       <c r="C927" t="n">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D927" t="n">
-        <v>1983688</v>
+        <v>1985188</v>
       </c>
       <c r="E927" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D931" t="n">
-        <v>358184</v>
+        <v>368934</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45070,10 +45070,10 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>19272</v>
+        <v>19278</v>
       </c>
       <c r="D932" t="n">
-        <v>24079394</v>
+        <v>24085043</v>
       </c>
       <c r="E932" t="inlineStr">
         <is>
@@ -45262,10 +45262,10 @@
         </is>
       </c>
       <c r="C936" t="n">
-        <v>10066</v>
+        <v>10070</v>
       </c>
       <c r="D936" t="n">
-        <v>14714036</v>
+        <v>14719216</v>
       </c>
       <c r="E936" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D940" t="n">
-        <v>621794</v>
+        <v>623294</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45502,10 +45502,10 @@
         </is>
       </c>
       <c r="C941" t="n">
-        <v>8616</v>
+        <v>8617</v>
       </c>
       <c r="D941" t="n">
-        <v>10749514</v>
+        <v>10751014</v>
       </c>
       <c r="E941" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>3198</v>
+        <v>3199</v>
       </c>
       <c r="D946" t="n">
-        <v>4664785</v>
+        <v>4666285</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45982,10 +45982,10 @@
         </is>
       </c>
       <c r="C951" t="n">
-        <v>67057</v>
+        <v>67105</v>
       </c>
       <c r="D951" t="n">
-        <v>86074088</v>
+        <v>86134181</v>
       </c>
       <c r="E951" t="inlineStr">
         <is>
@@ -46030,10 +46030,10 @@
         </is>
       </c>
       <c r="C952" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D952" t="n">
-        <v>68769</v>
+        <v>70269</v>
       </c>
       <c r="E952" t="inlineStr">
         <is>
@@ -46318,10 +46318,10 @@
         </is>
       </c>
       <c r="C958" t="n">
-        <v>25537</v>
+        <v>25554</v>
       </c>
       <c r="D958" t="n">
-        <v>37429241</v>
+        <v>37450876</v>
       </c>
       <c r="E958" t="inlineStr">
         <is>
@@ -46414,10 +46414,10 @@
         </is>
       </c>
       <c r="C960" t="n">
-        <v>17579</v>
+        <v>17590</v>
       </c>
       <c r="D960" t="n">
-        <v>25486145</v>
+        <v>25500565</v>
       </c>
       <c r="E960" t="inlineStr">
         <is>
@@ -46510,10 +46510,10 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D962" t="n">
-        <v>703823</v>
+        <v>705323</v>
       </c>
       <c r="E962" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="D963" t="n">
-        <v>1238221</v>
+        <v>1241221</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46606,10 +46606,10 @@
         </is>
       </c>
       <c r="C964" t="n">
-        <v>83725</v>
+        <v>83779</v>
       </c>
       <c r="D964" t="n">
-        <v>105089644</v>
+        <v>105155137</v>
       </c>
       <c r="E964" t="inlineStr">
         <is>
@@ -46942,10 +46942,10 @@
         </is>
       </c>
       <c r="C971" t="n">
-        <v>33779</v>
+        <v>33799</v>
       </c>
       <c r="D971" t="n">
-        <v>49544240</v>
+        <v>49571179</v>
       </c>
       <c r="E971" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>25157</v>
+        <v>25174</v>
       </c>
       <c r="D974" t="n">
-        <v>36488873</v>
+        <v>36511784</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D977" t="n">
-        <v>2793305</v>
+        <v>2794805</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47278,10 +47278,10 @@
         </is>
       </c>
       <c r="C978" t="n">
-        <v>10750</v>
+        <v>10759</v>
       </c>
       <c r="D978" t="n">
-        <v>14020211</v>
+        <v>14032677</v>
       </c>
       <c r="E978" t="inlineStr">
         <is>
@@ -47470,10 +47470,10 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>3459</v>
+        <v>3461</v>
       </c>
       <c r="D982" t="n">
-        <v>5052922</v>
+        <v>5054695</v>
       </c>
       <c r="E982" t="inlineStr">
         <is>
@@ -47518,10 +47518,10 @@
         </is>
       </c>
       <c r="C983" t="n">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D983" t="n">
-        <v>1607189</v>
+        <v>1608689</v>
       </c>
       <c r="E983" t="inlineStr">
         <is>
@@ -47758,10 +47758,10 @@
         </is>
       </c>
       <c r="C988" t="n">
-        <v>55915</v>
+        <v>55938</v>
       </c>
       <c r="D988" t="n">
-        <v>70000971</v>
+        <v>70027988</v>
       </c>
       <c r="E988" t="inlineStr">
         <is>
@@ -47998,10 +47998,10 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>18491</v>
+        <v>18494</v>
       </c>
       <c r="D993" t="n">
-        <v>27080783</v>
+        <v>27085283</v>
       </c>
       <c r="E993" t="inlineStr">
         <is>
@@ -48094,10 +48094,10 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>12606</v>
+        <v>12607</v>
       </c>
       <c r="D995" t="n">
-        <v>18229686</v>
+        <v>18231186</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="D998" t="n">
-        <v>1035924</v>
+        <v>1039501</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48286,10 +48286,10 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>28201</v>
+        <v>28223</v>
       </c>
       <c r="D999" t="n">
-        <v>35091914</v>
+        <v>35117724</v>
       </c>
       <c r="E999" t="inlineStr">
         <is>
@@ -48526,10 +48526,10 @@
         </is>
       </c>
       <c r="C1004" t="n">
-        <v>10488</v>
+        <v>10491</v>
       </c>
       <c r="D1004" t="n">
-        <v>15361184</v>
+        <v>15365684</v>
       </c>
       <c r="E1004" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>6213</v>
+        <v>6215</v>
       </c>
       <c r="D1006" t="n">
-        <v>9009605</v>
+        <v>9012605</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>
@@ -48670,10 +48670,10 @@
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D1007" t="n">
-        <v>745918</v>
+        <v>747418</v>
       </c>
       <c r="E1007" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-14 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16375</v>
+        <v>16391</v>
       </c>
       <c r="D2" t="n">
-        <v>20583012</v>
+        <v>20604717</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6244</v>
+        <v>6248</v>
       </c>
       <c r="D6" t="n">
-        <v>9131238</v>
+        <v>9136405</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3290</v>
+        <v>3291</v>
       </c>
       <c r="D8" t="n">
-        <v>4760205</v>
+        <v>4761705</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D11" t="n">
-        <v>518208</v>
+        <v>519708</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10999</v>
+        <v>11013</v>
       </c>
       <c r="D12" t="n">
-        <v>13880448</v>
+        <v>13899574</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3232</v>
+        <v>3235</v>
       </c>
       <c r="D16" t="n">
-        <v>4708073</v>
+        <v>4712573</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D19" t="n">
-        <v>551178</v>
+        <v>552678</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>14251</v>
+        <v>14258</v>
       </c>
       <c r="D22" t="n">
-        <v>17473314</v>
+        <v>17482321</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1582,10 +1582,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4938</v>
+        <v>4940</v>
       </c>
       <c r="D26" t="n">
-        <v>7221428</v>
+        <v>7224129</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6556</v>
+        <v>6558</v>
       </c>
       <c r="D32" t="n">
-        <v>8708786</v>
+        <v>8711786</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1609</v>
+        <v>1612</v>
       </c>
       <c r="D35" t="n">
-        <v>2320120</v>
+        <v>2323410</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2158,10 +2158,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D38" t="n">
-        <v>747809</v>
+        <v>749309</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>21875</v>
+        <v>21882</v>
       </c>
       <c r="D41" t="n">
-        <v>26919421</v>
+        <v>26926380</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3841</v>
+        <v>3845</v>
       </c>
       <c r="D49" t="n">
-        <v>5559069</v>
+        <v>5564669</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D52" t="n">
-        <v>830066</v>
+        <v>832178</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8141</v>
+        <v>8143</v>
       </c>
       <c r="D53" t="n">
-        <v>10386756</v>
+        <v>10389725</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2781</v>
+        <v>2782</v>
       </c>
       <c r="D57" t="n">
-        <v>4045043</v>
+        <v>4046543</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>36160</v>
+        <v>36177</v>
       </c>
       <c r="D62" t="n">
-        <v>46551041</v>
+        <v>46571800</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>13160</v>
+        <v>13170</v>
       </c>
       <c r="D67" t="n">
-        <v>19300885</v>
+        <v>19315885</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5162</v>
+        <v>5163</v>
       </c>
       <c r="D69" t="n">
-        <v>7466084</v>
+        <v>7466914</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D73" t="n">
-        <v>485676</v>
+        <v>487176</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>46276</v>
+        <v>46300</v>
       </c>
       <c r="D75" t="n">
-        <v>59152284</v>
+        <v>59181823</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4078,10 +4078,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D78" t="n">
-        <v>105841</v>
+        <v>107341</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18115</v>
+        <v>18119</v>
       </c>
       <c r="D79" t="n">
-        <v>26538880</v>
+        <v>26544880</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9339</v>
+        <v>9347</v>
       </c>
       <c r="D81" t="n">
-        <v>13481947</v>
+        <v>13493183</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="D85" t="n">
-        <v>1125723</v>
+        <v>1127223</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>24951</v>
+        <v>24967</v>
       </c>
       <c r="D86" t="n">
-        <v>31454264</v>
+        <v>31476158</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8682</v>
+        <v>8684</v>
       </c>
       <c r="D90" t="n">
-        <v>12744886</v>
+        <v>12747886</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4903</v>
+        <v>4906</v>
       </c>
       <c r="D92" t="n">
-        <v>7086639</v>
+        <v>7090565</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>21967</v>
+        <v>21974</v>
       </c>
       <c r="D95" t="n">
-        <v>27577683</v>
+        <v>27586390</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9157</v>
+        <v>9160</v>
       </c>
       <c r="D99" t="n">
-        <v>13403849</v>
+        <v>13408349</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5182,10 +5182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3328</v>
+        <v>3329</v>
       </c>
       <c r="D101" t="n">
-        <v>4765848</v>
+        <v>4767348</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>81746</v>
+        <v>81814</v>
       </c>
       <c r="D106" t="n">
-        <v>104746625</v>
+        <v>104835322</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>30611</v>
+        <v>30628</v>
       </c>
       <c r="D113" t="n">
-        <v>44921417</v>
+        <v>44946150</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>20834</v>
+        <v>20854</v>
       </c>
       <c r="D115" t="n">
-        <v>30063184</v>
+        <v>30090682</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -5998,10 +5998,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="D118" t="n">
-        <v>972767</v>
+        <v>977267</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>27713</v>
+        <v>27718</v>
       </c>
       <c r="D123" t="n">
-        <v>36572723</v>
+        <v>36579963</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6430,10 +6430,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>9870</v>
+        <v>9873</v>
       </c>
       <c r="D127" t="n">
-        <v>14474870</v>
+        <v>14479051</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>15755</v>
+        <v>15759</v>
       </c>
       <c r="D133" t="n">
-        <v>19601897</v>
+        <v>19605957</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6862,10 +6862,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>7762</v>
+        <v>7765</v>
       </c>
       <c r="D136" t="n">
-        <v>11357916</v>
+        <v>11361516</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D142" t="n">
-        <v>544999</v>
+        <v>545415</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>13540</v>
+        <v>13548</v>
       </c>
       <c r="D143" t="n">
-        <v>16910677</v>
+        <v>16919336</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7390,10 +7390,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6244</v>
+        <v>6245</v>
       </c>
       <c r="D147" t="n">
-        <v>9148255</v>
+        <v>9149085</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>5985</v>
+        <v>5986</v>
       </c>
       <c r="D153" t="n">
-        <v>7320084</v>
+        <v>7321584</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -8062,10 +8062,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>7440</v>
+        <v>7443</v>
       </c>
       <c r="D161" t="n">
-        <v>9219088</v>
+        <v>9223200</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>2852</v>
+        <v>2854</v>
       </c>
       <c r="D164" t="n">
-        <v>4181958</v>
+        <v>4184958</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D165" t="n">
-        <v>2013387</v>
+        <v>2014887</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D166" t="n">
-        <v>217210</v>
+        <v>218710</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>5614</v>
+        <v>5616</v>
       </c>
       <c r="D169" t="n">
-        <v>7065664</v>
+        <v>7068664</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8686,10 +8686,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="D174" t="n">
-        <v>2963041</v>
+        <v>2964541</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -8926,10 +8926,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>15976</v>
+        <v>15979</v>
       </c>
       <c r="D179" t="n">
-        <v>20073496</v>
+        <v>20075978</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>6394</v>
+        <v>6396</v>
       </c>
       <c r="D184" t="n">
-        <v>9339859</v>
+        <v>9341635</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>3073</v>
+        <v>3074</v>
       </c>
       <c r="D189" t="n">
-        <v>3857537</v>
+        <v>3859016</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D191" t="n">
-        <v>2158242</v>
+        <v>2159742</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>9210</v>
+        <v>9216</v>
       </c>
       <c r="D197" t="n">
-        <v>11499830</v>
+        <v>11504976</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>3430</v>
+        <v>3431</v>
       </c>
       <c r="D201" t="n">
-        <v>5039576</v>
+        <v>5041076</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10030,10 +10030,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="D202" t="n">
-        <v>2327680</v>
+        <v>2329180</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D203" t="n">
-        <v>257630</v>
+        <v>259130</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>17271</v>
+        <v>17274</v>
       </c>
       <c r="D206" t="n">
-        <v>21566631</v>
+        <v>21569673</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D212" t="n">
-        <v>395577</v>
+        <v>397077</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>26149</v>
+        <v>26159</v>
       </c>
       <c r="D214" t="n">
-        <v>32980786</v>
+        <v>32993513</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>10494</v>
+        <v>10496</v>
       </c>
       <c r="D218" t="n">
-        <v>15326353</v>
+        <v>15329353</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D221" t="n">
-        <v>443807</v>
+        <v>445307</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D223" t="n">
-        <v>850659</v>
+        <v>851117</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>28506</v>
+        <v>28528</v>
       </c>
       <c r="D224" t="n">
-        <v>35965555</v>
+        <v>35989501</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11326,10 +11326,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>14734</v>
+        <v>14739</v>
       </c>
       <c r="D229" t="n">
-        <v>21619219</v>
+        <v>21626719</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -11422,10 +11422,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>2658</v>
+        <v>2659</v>
       </c>
       <c r="D231" t="n">
-        <v>3816675</v>
+        <v>3818175</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D234" t="n">
-        <v>1022228</v>
+        <v>1023728</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>24297</v>
+        <v>24303</v>
       </c>
       <c r="D235" t="n">
-        <v>30645473</v>
+        <v>30653948</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11902,10 +11902,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>11186</v>
+        <v>11188</v>
       </c>
       <c r="D241" t="n">
-        <v>16395490</v>
+        <v>16398490</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -12190,10 +12190,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>7872</v>
+        <v>7874</v>
       </c>
       <c r="D247" t="n">
-        <v>9846521</v>
+        <v>9849521</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -12670,10 +12670,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>9817</v>
+        <v>9819</v>
       </c>
       <c r="D257" t="n">
-        <v>12521232</v>
+        <v>12524232</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>4197</v>
+        <v>4198</v>
       </c>
       <c r="D261" t="n">
-        <v>6160460</v>
+        <v>6161960</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -12958,10 +12958,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>2174</v>
+        <v>2176</v>
       </c>
       <c r="D263" t="n">
-        <v>3147387</v>
+        <v>3150387</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D265" t="n">
-        <v>171681</v>
+        <v>173181</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13102,10 +13102,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>5554</v>
+        <v>5555</v>
       </c>
       <c r="D266" t="n">
-        <v>6887700</v>
+        <v>6888150</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13342,10 +13342,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D271" t="n">
-        <v>1032872</v>
+        <v>1034372</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13534,10 +13534,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>19106</v>
+        <v>19114</v>
       </c>
       <c r="D275" t="n">
-        <v>24135703</v>
+        <v>24145404</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>7933</v>
+        <v>7935</v>
       </c>
       <c r="D279" t="n">
-        <v>11631396</v>
+        <v>11634396</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13966,10 +13966,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D284" t="n">
-        <v>652245</v>
+        <v>653745</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>16635</v>
+        <v>16646</v>
       </c>
       <c r="D286" t="n">
-        <v>20604385</v>
+        <v>20618786</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>7191</v>
+        <v>7193</v>
       </c>
       <c r="D290" t="n">
-        <v>10547114</v>
+        <v>10550114</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>3334</v>
+        <v>3335</v>
       </c>
       <c r="D291" t="n">
-        <v>4832299</v>
+        <v>4833799</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>9357</v>
+        <v>9366</v>
       </c>
       <c r="D295" t="n">
-        <v>11754524</v>
+        <v>11762589</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>3915</v>
+        <v>3916</v>
       </c>
       <c r="D299" t="n">
-        <v>5730332</v>
+        <v>5731832</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="D300" t="n">
-        <v>1814009</v>
+        <v>1817009</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>9209</v>
+        <v>9216</v>
       </c>
       <c r="D305" t="n">
-        <v>12026229</v>
+        <v>12034217</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>3747</v>
+        <v>3750</v>
       </c>
       <c r="D309" t="n">
-        <v>5478349</v>
+        <v>5482849</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>2358</v>
+        <v>2359</v>
       </c>
       <c r="D310" t="n">
-        <v>3429950</v>
+        <v>3431450</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>11076</v>
+        <v>11080</v>
       </c>
       <c r="D313" t="n">
-        <v>14543643</v>
+        <v>14549143</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15550,10 +15550,10 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>3782</v>
+        <v>3783</v>
       </c>
       <c r="D317" t="n">
-        <v>5544672</v>
+        <v>5546172</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2707</v>
+        <v>2712</v>
       </c>
       <c r="D319" t="n">
-        <v>3923728</v>
+        <v>3931228</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>6822</v>
+        <v>6827</v>
       </c>
       <c r="D322" t="n">
-        <v>8433859</v>
+        <v>8439202</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>2301</v>
+        <v>2302</v>
       </c>
       <c r="D327" t="n">
-        <v>3375584</v>
+        <v>3376167</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D331" t="n">
-        <v>185289</v>
+        <v>186789</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>7542</v>
+        <v>7544</v>
       </c>
       <c r="D332" t="n">
-        <v>9439350</v>
+        <v>9442111</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>3132</v>
+        <v>3133</v>
       </c>
       <c r="D337" t="n">
-        <v>4574562</v>
+        <v>4576062</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16702,10 +16702,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>32050</v>
+        <v>32081</v>
       </c>
       <c r="D341" t="n">
-        <v>40258516</v>
+        <v>40300119</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>16546</v>
+        <v>16554</v>
       </c>
       <c r="D347" t="n">
-        <v>24193878</v>
+        <v>24205878</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>8057</v>
+        <v>8062</v>
       </c>
       <c r="D350" t="n">
-        <v>11603232</v>
+        <v>11610732</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D352" t="n">
-        <v>1112089</v>
+        <v>1112739</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>3896</v>
+        <v>3897</v>
       </c>
       <c r="D353" t="n">
-        <v>4854412</v>
+        <v>4855870</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>19406</v>
+        <v>19414</v>
       </c>
       <c r="D361" t="n">
-        <v>24195917</v>
+        <v>24200777</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17854,10 +17854,10 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>9918</v>
+        <v>9919</v>
       </c>
       <c r="D365" t="n">
-        <v>14541735</v>
+        <v>14543235</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>4742</v>
+        <v>4744</v>
       </c>
       <c r="D367" t="n">
-        <v>6855662</v>
+        <v>6858662</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>13955</v>
+        <v>13969</v>
       </c>
       <c r="D370" t="n">
-        <v>17449386</v>
+        <v>17464735</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>6447</v>
+        <v>6449</v>
       </c>
       <c r="D374" t="n">
-        <v>9439376</v>
+        <v>9442376</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>18016</v>
+        <v>18023</v>
       </c>
       <c r="D379" t="n">
-        <v>22461904</v>
+        <v>22471941</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>7143</v>
+        <v>7144</v>
       </c>
       <c r="D383" t="n">
-        <v>10499715</v>
+        <v>10501215</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>2838</v>
+        <v>2840</v>
       </c>
       <c r="D385" t="n">
-        <v>4128151</v>
+        <v>4131151</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -19006,10 +19006,10 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>4098</v>
+        <v>4099</v>
       </c>
       <c r="D389" t="n">
-        <v>5142992</v>
+        <v>5144492</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D392" t="n">
-        <v>2030576</v>
+        <v>2031746</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19342,10 +19342,10 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>22309</v>
+        <v>22327</v>
       </c>
       <c r="D396" t="n">
-        <v>27675052</v>
+        <v>27696139</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>9373</v>
+        <v>9376</v>
       </c>
       <c r="D399" t="n">
-        <v>13797657</v>
+        <v>13802157</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="D401" t="n">
-        <v>9046133</v>
+        <v>9053633</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D403" t="n">
-        <v>489802</v>
+        <v>491302</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19726,10 +19726,10 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>11147</v>
+        <v>11150</v>
       </c>
       <c r="D404" t="n">
-        <v>13741257</v>
+        <v>13744607</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>5328</v>
+        <v>5330</v>
       </c>
       <c r="D409" t="n">
-        <v>7786544</v>
+        <v>7789544</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>32399</v>
+        <v>32464</v>
       </c>
       <c r="D414" t="n">
-        <v>43887633</v>
+        <v>43975596</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20398,10 +20398,10 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>7836</v>
+        <v>7852</v>
       </c>
       <c r="D418" t="n">
-        <v>11521581</v>
+        <v>11545581</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>7155</v>
+        <v>7173</v>
       </c>
       <c r="D420" t="n">
-        <v>10373082</v>
+        <v>10400082</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D422" t="n">
-        <v>749905</v>
+        <v>750705</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D423" t="n">
-        <v>696943</v>
+        <v>698443</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>8921</v>
+        <v>8947</v>
       </c>
       <c r="D424" t="n">
-        <v>12384334</v>
+        <v>12421784</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>2240</v>
+        <v>2249</v>
       </c>
       <c r="D426" t="n">
-        <v>3300302</v>
+        <v>3313802</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3010</v>
+        <v>3015</v>
       </c>
       <c r="D428" t="n">
-        <v>4396550</v>
+        <v>4402834</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -21070,10 +21070,10 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>11039</v>
+        <v>11045</v>
       </c>
       <c r="D432" t="n">
-        <v>13629418</v>
+        <v>13635603</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D439" t="n">
-        <v>222511</v>
+        <v>224011</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>63042</v>
+        <v>63087</v>
       </c>
       <c r="D440" t="n">
-        <v>78120140</v>
+        <v>78167814</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21646,10 +21646,10 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>24944</v>
+        <v>24954</v>
       </c>
       <c r="D444" t="n">
-        <v>36563113</v>
+        <v>36576135</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>12951</v>
+        <v>12957</v>
       </c>
       <c r="D446" t="n">
-        <v>18779697</v>
+        <v>18788197</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21934,10 +21934,10 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="D450" t="n">
-        <v>1468299</v>
+        <v>1469799</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>18934</v>
+        <v>18949</v>
       </c>
       <c r="D452" t="n">
-        <v>23933669</v>
+        <v>23953680</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22222,10 +22222,10 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>7710</v>
+        <v>7715</v>
       </c>
       <c r="D456" t="n">
-        <v>11317393</v>
+        <v>11324720</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>4864</v>
+        <v>4872</v>
       </c>
       <c r="D458" t="n">
-        <v>7058697</v>
+        <v>7070214</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22462,10 +22462,10 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>32262</v>
+        <v>32282</v>
       </c>
       <c r="D461" t="n">
-        <v>39432217</v>
+        <v>39453301</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -22654,10 +22654,10 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>11464</v>
+        <v>11470</v>
       </c>
       <c r="D465" t="n">
-        <v>16773849</v>
+        <v>16782849</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>4912</v>
+        <v>4915</v>
       </c>
       <c r="D467" t="n">
-        <v>7127082</v>
+        <v>7131582</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22894,10 +22894,10 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>14419</v>
+        <v>14427</v>
       </c>
       <c r="D470" t="n">
-        <v>17627915</v>
+        <v>17635138</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -23374,10 +23374,10 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>36071</v>
+        <v>36103</v>
       </c>
       <c r="D480" t="n">
-        <v>47004868</v>
+        <v>47046249</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -23566,10 +23566,10 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>13575</v>
+        <v>13577</v>
       </c>
       <c r="D484" t="n">
-        <v>19972500</v>
+        <v>19975500</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -23662,10 +23662,10 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>12015</v>
+        <v>12027</v>
       </c>
       <c r="D486" t="n">
-        <v>17536678</v>
+        <v>17552596</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>62497</v>
+        <v>62588</v>
       </c>
       <c r="D489" t="n">
-        <v>82745387</v>
+        <v>82863170</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>23145</v>
+        <v>23155</v>
       </c>
       <c r="D494" t="n">
-        <v>33962984</v>
+        <v>33977984</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24142,10 +24142,10 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>22484</v>
+        <v>22503</v>
       </c>
       <c r="D496" t="n">
-        <v>32643143</v>
+        <v>32670675</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D499" t="n">
-        <v>889143</v>
+        <v>891555</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>151297</v>
+        <v>151428</v>
       </c>
       <c r="D500" t="n">
-        <v>198970076</v>
+        <v>199142828</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>81768</v>
+        <v>81813</v>
       </c>
       <c r="D507" t="n">
-        <v>120115560</v>
+        <v>120181730</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>60194</v>
+        <v>60239</v>
       </c>
       <c r="D510" t="n">
-        <v>87376325</v>
+        <v>87442561</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -24910,10 +24910,10 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="D512" t="n">
-        <v>1536703</v>
+        <v>1539703</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>2793</v>
+        <v>2799</v>
       </c>
       <c r="D514" t="n">
-        <v>3954513</v>
+        <v>3962925</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>41313</v>
+        <v>41340</v>
       </c>
       <c r="D516" t="n">
-        <v>53701725</v>
+        <v>53738072</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25342,10 +25342,10 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>15273</v>
+        <v>15282</v>
       </c>
       <c r="D521" t="n">
-        <v>22432718</v>
+        <v>22446218</v>
       </c>
       <c r="E521" t="inlineStr">
         <is>
@@ -25438,10 +25438,10 @@
         </is>
       </c>
       <c r="C523" t="n">
-        <v>12953</v>
+        <v>12961</v>
       </c>
       <c r="D523" t="n">
-        <v>18775072</v>
+        <v>18785623</v>
       </c>
       <c r="E523" t="inlineStr">
         <is>
@@ -25582,10 +25582,10 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D526" t="n">
-        <v>497656</v>
+        <v>499156</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>66347</v>
+        <v>66415</v>
       </c>
       <c r="D528" t="n">
-        <v>89166735</v>
+        <v>89256453</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>23352</v>
+        <v>23370</v>
       </c>
       <c r="D532" t="n">
-        <v>34457135</v>
+        <v>34483955</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -25966,10 +25966,10 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>24137</v>
+        <v>24157</v>
       </c>
       <c r="D534" t="n">
-        <v>35325491</v>
+        <v>35355491</v>
       </c>
       <c r="E534" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="D537" t="n">
-        <v>1221710</v>
+        <v>1227410</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26158,10 +26158,10 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>55181</v>
+        <v>55223</v>
       </c>
       <c r="D538" t="n">
-        <v>73184883</v>
+        <v>73241200</v>
       </c>
       <c r="E538" t="inlineStr">
         <is>
@@ -26398,10 +26398,10 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>17809</v>
+        <v>17816</v>
       </c>
       <c r="D543" t="n">
-        <v>26168586</v>
+        <v>26179086</v>
       </c>
       <c r="E543" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>18345</v>
+        <v>18360</v>
       </c>
       <c r="D545" t="n">
-        <v>26668087</v>
+        <v>26690256</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D547" t="n">
-        <v>883704</v>
+        <v>885204</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>41661</v>
+        <v>41705</v>
       </c>
       <c r="D548" t="n">
-        <v>55317529</v>
+        <v>55376130</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>14232</v>
+        <v>14240</v>
       </c>
       <c r="D552" t="n">
-        <v>20991121</v>
+        <v>21001740</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>14434</v>
+        <v>14444</v>
       </c>
       <c r="D554" t="n">
-        <v>20960035</v>
+        <v>20974294</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>41393</v>
+        <v>41415</v>
       </c>
       <c r="D557" t="n">
-        <v>53664137</v>
+        <v>53690244</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>16226</v>
+        <v>16234</v>
       </c>
       <c r="D561" t="n">
-        <v>23805655</v>
+        <v>23817655</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27358,10 +27358,10 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>13034</v>
+        <v>13040</v>
       </c>
       <c r="D563" t="n">
-        <v>18850615</v>
+        <v>18859007</v>
       </c>
       <c r="E563" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>43975</v>
+        <v>44006</v>
       </c>
       <c r="D567" t="n">
-        <v>58702970</v>
+        <v>58741729</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>13933</v>
+        <v>13939</v>
       </c>
       <c r="D573" t="n">
-        <v>20432676</v>
+        <v>20440478</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27886,10 +27886,10 @@
         </is>
       </c>
       <c r="C574" t="n">
-        <v>3710</v>
+        <v>3712</v>
       </c>
       <c r="D574" t="n">
-        <v>5349680</v>
+        <v>5352680</v>
       </c>
       <c r="E574" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>17344</v>
+        <v>17363</v>
       </c>
       <c r="D580" t="n">
-        <v>22914662</v>
+        <v>22940196</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D583" t="n">
-        <v>77906</v>
+        <v>79406</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>7085</v>
+        <v>7089</v>
       </c>
       <c r="D584" t="n">
-        <v>10304703</v>
+        <v>10309713</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>4931</v>
+        <v>4936</v>
       </c>
       <c r="D586" t="n">
-        <v>7095563</v>
+        <v>7103063</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D589" t="n">
-        <v>377364</v>
+        <v>378864</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>15649</v>
+        <v>15685</v>
       </c>
       <c r="D591" t="n">
-        <v>22705655</v>
+        <v>22757845</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>1760</v>
+        <v>1765</v>
       </c>
       <c r="D592" t="n">
-        <v>2617730</v>
+        <v>2625230</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D596" t="n">
-        <v>119949</v>
+        <v>124449</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>22038</v>
+        <v>22051</v>
       </c>
       <c r="D597" t="n">
-        <v>27649547</v>
+        <v>27662132</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>8993</v>
+        <v>8997</v>
       </c>
       <c r="D602" t="n">
-        <v>13173968</v>
+        <v>13179968</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>3350</v>
+        <v>3352</v>
       </c>
       <c r="D604" t="n">
-        <v>4811659</v>
+        <v>4814659</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>14657</v>
+        <v>14659</v>
       </c>
       <c r="D608" t="n">
-        <v>18373396</v>
+        <v>18376226</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>5790</v>
+        <v>5792</v>
       </c>
       <c r="D612" t="n">
-        <v>8504151</v>
+        <v>8507151</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>2675</v>
+        <v>2676</v>
       </c>
       <c r="D614" t="n">
-        <v>3854928</v>
+        <v>3856428</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D615" t="n">
-        <v>256709</v>
+        <v>258209</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -29950,10 +29950,10 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>13760</v>
+        <v>13763</v>
       </c>
       <c r="D617" t="n">
-        <v>17376579</v>
+        <v>17379691</v>
       </c>
       <c r="E617" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>5228</v>
+        <v>5229</v>
       </c>
       <c r="D621" t="n">
-        <v>7662187</v>
+        <v>7663687</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D625" t="n">
-        <v>367466</v>
+        <v>368966</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>7510</v>
+        <v>7513</v>
       </c>
       <c r="D626" t="n">
-        <v>9661164</v>
+        <v>9663780</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D634" t="n">
-        <v>187185</v>
+        <v>188685</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>28815</v>
+        <v>28827</v>
       </c>
       <c r="D635" t="n">
-        <v>35490213</v>
+        <v>35503690</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -31006,10 +31006,10 @@
         </is>
       </c>
       <c r="C639" t="n">
-        <v>11028</v>
+        <v>11034</v>
       </c>
       <c r="D639" t="n">
-        <v>16180409</v>
+        <v>16189409</v>
       </c>
       <c r="E639" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>4833</v>
+        <v>4836</v>
       </c>
       <c r="D641" t="n">
-        <v>7012853</v>
+        <v>7017353</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>11312</v>
+        <v>11319</v>
       </c>
       <c r="D645" t="n">
-        <v>13710058</v>
+        <v>13718772</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>3639</v>
+        <v>3641</v>
       </c>
       <c r="D650" t="n">
-        <v>5327219</v>
+        <v>5330219</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31774,10 +31774,10 @@
         </is>
       </c>
       <c r="C655" t="n">
-        <v>28311</v>
+        <v>28320</v>
       </c>
       <c r="D655" t="n">
-        <v>35195290</v>
+        <v>35205815</v>
       </c>
       <c r="E655" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>10736</v>
+        <v>10740</v>
       </c>
       <c r="D659" t="n">
-        <v>15774836</v>
+        <v>15779395</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32062,10 +32062,10 @@
         </is>
       </c>
       <c r="C661" t="n">
-        <v>3080</v>
+        <v>3082</v>
       </c>
       <c r="D661" t="n">
-        <v>4440927</v>
+        <v>4443927</v>
       </c>
       <c r="E661" t="inlineStr">
         <is>
@@ -32254,10 +32254,10 @@
         </is>
       </c>
       <c r="C665" t="n">
-        <v>7499</v>
+        <v>7505</v>
       </c>
       <c r="D665" t="n">
-        <v>9512825</v>
+        <v>9520828</v>
       </c>
       <c r="E665" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D669" t="n">
-        <v>1870872</v>
+        <v>1872372</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D670" t="n">
-        <v>368984</v>
+        <v>371984</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32638,10 +32638,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>3774</v>
+        <v>3777</v>
       </c>
       <c r="D673" t="n">
-        <v>4573898</v>
+        <v>4577611</v>
       </c>
       <c r="E673" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D681" t="n">
-        <v>207932</v>
+        <v>209432</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>9311</v>
+        <v>9315</v>
       </c>
       <c r="D682" t="n">
-        <v>11614688</v>
+        <v>11620067</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D690" t="n">
-        <v>381069</v>
+        <v>382569</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33502,10 +33502,10 @@
         </is>
       </c>
       <c r="C691" t="n">
-        <v>19214</v>
+        <v>19228</v>
       </c>
       <c r="D691" t="n">
-        <v>23515032</v>
+        <v>23532234</v>
       </c>
       <c r="E691" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>5708</v>
+        <v>5710</v>
       </c>
       <c r="D695" t="n">
-        <v>8337480</v>
+        <v>8340480</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>74483</v>
+        <v>74574</v>
       </c>
       <c r="D702" t="n">
-        <v>93763826</v>
+        <v>93875242</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>26492</v>
+        <v>26499</v>
       </c>
       <c r="D707" t="n">
-        <v>38894744</v>
+        <v>38905204</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>13148</v>
+        <v>13156</v>
       </c>
       <c r="D710" t="n">
-        <v>18962331</v>
+        <v>18973081</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34558,10 +34558,10 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="D713" t="n">
-        <v>2800539</v>
+        <v>2801089</v>
       </c>
       <c r="E713" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D715" t="n">
-        <v>1678243</v>
+        <v>1679743</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34702,10 +34702,10 @@
         </is>
       </c>
       <c r="C716" t="n">
-        <v>11157</v>
+        <v>11166</v>
       </c>
       <c r="D716" t="n">
-        <v>13648658</v>
+        <v>13658972</v>
       </c>
       <c r="E716" t="inlineStr">
         <is>
@@ -34846,10 +34846,10 @@
         </is>
       </c>
       <c r="C719" t="n">
-        <v>4102</v>
+        <v>4104</v>
       </c>
       <c r="D719" t="n">
-        <v>6000133</v>
+        <v>6003133</v>
       </c>
       <c r="E719" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>17591</v>
+        <v>17602</v>
       </c>
       <c r="D724" t="n">
-        <v>21693662</v>
+        <v>21703189</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35278,10 +35278,10 @@
         </is>
       </c>
       <c r="C728" t="n">
-        <v>6842</v>
+        <v>6845</v>
       </c>
       <c r="D728" t="n">
-        <v>10000329</v>
+        <v>10004829</v>
       </c>
       <c r="E728" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>11506</v>
+        <v>11514</v>
       </c>
       <c r="D735" t="n">
-        <v>14201708</v>
+        <v>14209730</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>4233</v>
+        <v>4235</v>
       </c>
       <c r="D739" t="n">
-        <v>6204994</v>
+        <v>6207994</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -35902,10 +35902,10 @@
         </is>
       </c>
       <c r="C741" t="n">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D741" t="n">
-        <v>2319054</v>
+        <v>2320554</v>
       </c>
       <c r="E741" t="inlineStr">
         <is>
@@ -35950,10 +35950,10 @@
         </is>
       </c>
       <c r="C742" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D742" t="n">
-        <v>316213</v>
+        <v>317713</v>
       </c>
       <c r="E742" t="inlineStr">
         <is>
@@ -36046,10 +36046,10 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>29502</v>
+        <v>29517</v>
       </c>
       <c r="D744" t="n">
-        <v>36669407</v>
+        <v>36689619</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
@@ -36286,10 +36286,10 @@
         </is>
       </c>
       <c r="C749" t="n">
-        <v>12704</v>
+        <v>12705</v>
       </c>
       <c r="D749" t="n">
-        <v>18593590</v>
+        <v>18595090</v>
       </c>
       <c r="E749" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D753" t="n">
-        <v>1078657</v>
+        <v>1080157</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36526,10 +36526,10 @@
         </is>
       </c>
       <c r="C754" t="n">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D754" t="n">
-        <v>962896</v>
+        <v>967396</v>
       </c>
       <c r="E754" t="inlineStr">
         <is>
@@ -36622,10 +36622,10 @@
         </is>
       </c>
       <c r="C756" t="n">
-        <v>12303</v>
+        <v>12308</v>
       </c>
       <c r="D756" t="n">
-        <v>15226784</v>
+        <v>15234109</v>
       </c>
       <c r="E756" t="inlineStr">
         <is>
@@ -36766,10 +36766,10 @@
         </is>
       </c>
       <c r="C759" t="n">
-        <v>4651</v>
+        <v>4653</v>
       </c>
       <c r="D759" t="n">
-        <v>6797856</v>
+        <v>6800856</v>
       </c>
       <c r="E759" t="inlineStr">
         <is>
@@ -36958,10 +36958,10 @@
         </is>
       </c>
       <c r="C763" t="n">
-        <v>6715</v>
+        <v>6720</v>
       </c>
       <c r="D763" t="n">
-        <v>7891653</v>
+        <v>7894316</v>
       </c>
       <c r="E763" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="D767" t="n">
-        <v>2478153</v>
+        <v>2479653</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37342,10 +37342,10 @@
         </is>
       </c>
       <c r="C771" t="n">
-        <v>16777</v>
+        <v>16786</v>
       </c>
       <c r="D771" t="n">
-        <v>20351695</v>
+        <v>20363022</v>
       </c>
       <c r="E771" t="inlineStr">
         <is>
@@ -37582,10 +37582,10 @@
         </is>
       </c>
       <c r="C776" t="n">
-        <v>5531</v>
+        <v>5532</v>
       </c>
       <c r="D776" t="n">
-        <v>8104586</v>
+        <v>8106086</v>
       </c>
       <c r="E776" t="inlineStr">
         <is>
@@ -37678,10 +37678,10 @@
         </is>
       </c>
       <c r="C778" t="n">
-        <v>3395</v>
+        <v>3396</v>
       </c>
       <c r="D778" t="n">
-        <v>4958722</v>
+        <v>4960222</v>
       </c>
       <c r="E778" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D781" t="n">
-        <v>394189</v>
+        <v>395128</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>11362</v>
+        <v>11363</v>
       </c>
       <c r="D782" t="n">
-        <v>14381335</v>
+        <v>14382835</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38062,10 +38062,10 @@
         </is>
       </c>
       <c r="C786" t="n">
-        <v>3955</v>
+        <v>3956</v>
       </c>
       <c r="D786" t="n">
-        <v>5782458</v>
+        <v>5783958</v>
       </c>
       <c r="E786" t="inlineStr">
         <is>
@@ -38158,10 +38158,10 @@
         </is>
       </c>
       <c r="C788" t="n">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D788" t="n">
-        <v>1815412</v>
+        <v>1816912</v>
       </c>
       <c r="E788" t="inlineStr">
         <is>
@@ -38350,10 +38350,10 @@
         </is>
       </c>
       <c r="C792" t="n">
-        <v>32097</v>
+        <v>32118</v>
       </c>
       <c r="D792" t="n">
-        <v>39589823</v>
+        <v>39615701</v>
       </c>
       <c r="E792" t="inlineStr">
         <is>
@@ -38542,10 +38542,10 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>13166</v>
+        <v>13170</v>
       </c>
       <c r="D796" t="n">
-        <v>19263319</v>
+        <v>19268099</v>
       </c>
       <c r="E796" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>6034</v>
+        <v>6036</v>
       </c>
       <c r="D798" t="n">
-        <v>8717657</v>
+        <v>8720657</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38686,10 +38686,10 @@
         </is>
       </c>
       <c r="C799" t="n">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D799" t="n">
-        <v>733069</v>
+        <v>734569</v>
       </c>
       <c r="E799" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D801" t="n">
-        <v>920624</v>
+        <v>922124</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -38830,10 +38830,10 @@
         </is>
       </c>
       <c r="C802" t="n">
-        <v>7603</v>
+        <v>7608</v>
       </c>
       <c r="D802" t="n">
-        <v>9401568</v>
+        <v>9405973</v>
       </c>
       <c r="E802" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>2681</v>
+        <v>2682</v>
       </c>
       <c r="D808" t="n">
-        <v>3910984</v>
+        <v>3912484</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39166,10 +39166,10 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D809" t="n">
-        <v>1640438</v>
+        <v>1641938</v>
       </c>
       <c r="E809" t="inlineStr">
         <is>
@@ -39310,10 +39310,10 @@
         </is>
       </c>
       <c r="C812" t="n">
-        <v>58857</v>
+        <v>58902</v>
       </c>
       <c r="D812" t="n">
-        <v>73559800</v>
+        <v>73614614</v>
       </c>
       <c r="E812" t="inlineStr">
         <is>
@@ -39550,10 +39550,10 @@
         </is>
       </c>
       <c r="C817" t="n">
-        <v>21127</v>
+        <v>21140</v>
       </c>
       <c r="D817" t="n">
-        <v>30906181</v>
+        <v>30925681</v>
       </c>
       <c r="E817" t="inlineStr">
         <is>
@@ -39694,10 +39694,10 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>12595</v>
+        <v>12599</v>
       </c>
       <c r="D820" t="n">
-        <v>18180033</v>
+        <v>18185310</v>
       </c>
       <c r="E820" t="inlineStr">
         <is>
@@ -39790,10 +39790,10 @@
         </is>
       </c>
       <c r="C822" t="n">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D822" t="n">
-        <v>649195</v>
+        <v>650645</v>
       </c>
       <c r="E822" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D825" t="n">
-        <v>1843607</v>
+        <v>1845107</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -39982,10 +39982,10 @@
         </is>
       </c>
       <c r="C826" t="n">
-        <v>11128</v>
+        <v>11129</v>
       </c>
       <c r="D826" t="n">
-        <v>13872406</v>
+        <v>13873906</v>
       </c>
       <c r="E826" t="inlineStr">
         <is>
@@ -40078,10 +40078,10 @@
         </is>
       </c>
       <c r="C828" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D828" t="n">
-        <v>44866</v>
+        <v>46366</v>
       </c>
       <c r="E828" t="inlineStr">
         <is>
@@ -40174,10 +40174,10 @@
         </is>
       </c>
       <c r="C830" t="n">
-        <v>3912</v>
+        <v>3914</v>
       </c>
       <c r="D830" t="n">
-        <v>5686719</v>
+        <v>5688557</v>
       </c>
       <c r="E830" t="inlineStr">
         <is>
@@ -40270,10 +40270,10 @@
         </is>
       </c>
       <c r="C832" t="n">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D832" t="n">
-        <v>1770549</v>
+        <v>1772049</v>
       </c>
       <c r="E832" t="inlineStr">
         <is>
@@ -40366,10 +40366,10 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D834" t="n">
-        <v>195335</v>
+        <v>196600</v>
       </c>
       <c r="E834" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>58462</v>
+        <v>58494</v>
       </c>
       <c r="D837" t="n">
-        <v>72283358</v>
+        <v>72324914</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40798,10 +40798,10 @@
         </is>
       </c>
       <c r="C843" t="n">
-        <v>22306</v>
+        <v>22312</v>
       </c>
       <c r="D843" t="n">
-        <v>32730274</v>
+        <v>32738574</v>
       </c>
       <c r="E843" t="inlineStr">
         <is>
@@ -40894,10 +40894,10 @@
         </is>
       </c>
       <c r="C845" t="n">
-        <v>14312</v>
+        <v>14319</v>
       </c>
       <c r="D845" t="n">
-        <v>20718592</v>
+        <v>20729092</v>
       </c>
       <c r="E845" t="inlineStr">
         <is>
@@ -41134,10 +41134,10 @@
         </is>
       </c>
       <c r="C850" t="n">
-        <v>7731</v>
+        <v>7743</v>
       </c>
       <c r="D850" t="n">
-        <v>9484026</v>
+        <v>9499796</v>
       </c>
       <c r="E850" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="D853" t="n">
-        <v>1555976</v>
+        <v>1557476</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41422,10 +41422,10 @@
         </is>
       </c>
       <c r="C856" t="n">
-        <v>3600</v>
+        <v>3603</v>
       </c>
       <c r="D856" t="n">
-        <v>4653131</v>
+        <v>4656638</v>
       </c>
       <c r="E856" t="inlineStr">
         <is>
@@ -41806,10 +41806,10 @@
         </is>
       </c>
       <c r="C864" t="n">
-        <v>22329</v>
+        <v>22340</v>
       </c>
       <c r="D864" t="n">
-        <v>27979097</v>
+        <v>27988441</v>
       </c>
       <c r="E864" t="inlineStr">
         <is>
@@ -41998,10 +41998,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>7742</v>
+        <v>7744</v>
       </c>
       <c r="D868" t="n">
-        <v>11301269</v>
+        <v>11304269</v>
       </c>
       <c r="E868" t="inlineStr">
         <is>
@@ -42094,10 +42094,10 @@
         </is>
       </c>
       <c r="C870" t="n">
-        <v>4623</v>
+        <v>4627</v>
       </c>
       <c r="D870" t="n">
-        <v>6684651</v>
+        <v>6690651</v>
       </c>
       <c r="E870" t="inlineStr">
         <is>
@@ -42334,10 +42334,10 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>14499</v>
+        <v>14507</v>
       </c>
       <c r="D875" t="n">
-        <v>17481011</v>
+        <v>17490637</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
@@ -42526,10 +42526,10 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>5238</v>
+        <v>5239</v>
       </c>
       <c r="D879" t="n">
-        <v>7639610</v>
+        <v>7641110</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
@@ -42622,10 +42622,10 @@
         </is>
       </c>
       <c r="C881" t="n">
-        <v>2358</v>
+        <v>2359</v>
       </c>
       <c r="D881" t="n">
-        <v>3390503</v>
+        <v>3392003</v>
       </c>
       <c r="E881" t="inlineStr">
         <is>
@@ -42814,10 +42814,10 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>9772</v>
+        <v>9777</v>
       </c>
       <c r="D885" t="n">
-        <v>12004088</v>
+        <v>12011588</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
@@ -42958,10 +42958,10 @@
         </is>
       </c>
       <c r="C888" t="n">
-        <v>3346</v>
+        <v>3349</v>
       </c>
       <c r="D888" t="n">
-        <v>4902156</v>
+        <v>4906656</v>
       </c>
       <c r="E888" t="inlineStr">
         <is>
@@ -43150,10 +43150,10 @@
         </is>
       </c>
       <c r="C892" t="n">
-        <v>44533</v>
+        <v>44551</v>
       </c>
       <c r="D892" t="n">
-        <v>55932024</v>
+        <v>55949661</v>
       </c>
       <c r="E892" t="inlineStr">
         <is>
@@ -43294,10 +43294,10 @@
         </is>
       </c>
       <c r="C895" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D895" t="n">
-        <v>235011</v>
+        <v>236511</v>
       </c>
       <c r="E895" t="inlineStr">
         <is>
@@ -43390,10 +43390,10 @@
         </is>
       </c>
       <c r="C897" t="n">
-        <v>21043</v>
+        <v>21045</v>
       </c>
       <c r="D897" t="n">
-        <v>30854047</v>
+        <v>30857047</v>
       </c>
       <c r="E897" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>5884</v>
+        <v>5885</v>
       </c>
       <c r="D899" t="n">
-        <v>8479087</v>
+        <v>8480587</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43534,10 +43534,10 @@
         </is>
       </c>
       <c r="C900" t="n">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D900" t="n">
-        <v>889455</v>
+        <v>890955</v>
       </c>
       <c r="E900" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="D902" t="n">
-        <v>1297062</v>
+        <v>1301562</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43678,10 +43678,10 @@
         </is>
       </c>
       <c r="C903" t="n">
-        <v>21185</v>
+        <v>21199</v>
       </c>
       <c r="D903" t="n">
-        <v>26361307</v>
+        <v>26375725</v>
       </c>
       <c r="E903" t="inlineStr">
         <is>
@@ -43822,10 +43822,10 @@
         </is>
       </c>
       <c r="C906" t="n">
-        <v>9760</v>
+        <v>9761</v>
       </c>
       <c r="D906" t="n">
-        <v>14301696</v>
+        <v>14303196</v>
       </c>
       <c r="E906" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D911" t="n">
-        <v>890850</v>
+        <v>893850</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44110,10 +44110,10 @@
         </is>
       </c>
       <c r="C912" t="n">
-        <v>7031</v>
+        <v>7037</v>
       </c>
       <c r="D912" t="n">
-        <v>8837517</v>
+        <v>8844554</v>
       </c>
       <c r="E912" t="inlineStr">
         <is>
@@ -44542,10 +44542,10 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>13016</v>
+        <v>13022</v>
       </c>
       <c r="D921" t="n">
-        <v>16209487</v>
+        <v>16215305</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
@@ -44830,10 +44830,10 @@
         </is>
       </c>
       <c r="C927" t="n">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D927" t="n">
-        <v>1985188</v>
+        <v>1986057</v>
       </c>
       <c r="E927" t="inlineStr">
         <is>
@@ -44926,10 +44926,10 @@
         </is>
       </c>
       <c r="C929" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D929" t="n">
-        <v>200821</v>
+        <v>202321</v>
       </c>
       <c r="E929" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D931" t="n">
-        <v>368934</v>
+        <v>370434</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45070,10 +45070,10 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>19278</v>
+        <v>19288</v>
       </c>
       <c r="D932" t="n">
-        <v>24085043</v>
+        <v>24096516</v>
       </c>
       <c r="E932" t="inlineStr">
         <is>
@@ -45262,10 +45262,10 @@
         </is>
       </c>
       <c r="C936" t="n">
-        <v>10070</v>
+        <v>10074</v>
       </c>
       <c r="D936" t="n">
-        <v>14719216</v>
+        <v>14725216</v>
       </c>
       <c r="E936" t="inlineStr">
         <is>
@@ -45358,10 +45358,10 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>2057</v>
+        <v>2060</v>
       </c>
       <c r="D938" t="n">
-        <v>2966319</v>
+        <v>2970819</v>
       </c>
       <c r="E938" t="inlineStr">
         <is>
@@ -45406,10 +45406,10 @@
         </is>
       </c>
       <c r="C939" t="n">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D939" t="n">
-        <v>494147</v>
+        <v>495647</v>
       </c>
       <c r="E939" t="inlineStr">
         <is>
@@ -45502,10 +45502,10 @@
         </is>
       </c>
       <c r="C941" t="n">
-        <v>8617</v>
+        <v>8621</v>
       </c>
       <c r="D941" t="n">
-        <v>10751014</v>
+        <v>10755778</v>
       </c>
       <c r="E941" t="inlineStr">
         <is>
@@ -45742,10 +45742,10 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>3199</v>
+        <v>3200</v>
       </c>
       <c r="D946" t="n">
-        <v>4666285</v>
+        <v>4667785</v>
       </c>
       <c r="E946" t="inlineStr">
         <is>
@@ -45982,10 +45982,10 @@
         </is>
       </c>
       <c r="C951" t="n">
-        <v>67105</v>
+        <v>67151</v>
       </c>
       <c r="D951" t="n">
-        <v>86134181</v>
+        <v>86191107</v>
       </c>
       <c r="E951" t="inlineStr">
         <is>
@@ -46318,10 +46318,10 @@
         </is>
       </c>
       <c r="C958" t="n">
-        <v>25554</v>
+        <v>25567</v>
       </c>
       <c r="D958" t="n">
-        <v>37450876</v>
+        <v>37469849</v>
       </c>
       <c r="E958" t="inlineStr">
         <is>
@@ -46414,10 +46414,10 @@
         </is>
       </c>
       <c r="C960" t="n">
-        <v>17590</v>
+        <v>17598</v>
       </c>
       <c r="D960" t="n">
-        <v>25500565</v>
+        <v>25510105</v>
       </c>
       <c r="E960" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="D963" t="n">
-        <v>1241221</v>
+        <v>1245721</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46606,10 +46606,10 @@
         </is>
       </c>
       <c r="C964" t="n">
-        <v>83779</v>
+        <v>83836</v>
       </c>
       <c r="D964" t="n">
-        <v>105155137</v>
+        <v>105226811</v>
       </c>
       <c r="E964" t="inlineStr">
         <is>
@@ -46942,10 +46942,10 @@
         </is>
       </c>
       <c r="C971" t="n">
-        <v>33799</v>
+        <v>33813</v>
       </c>
       <c r="D971" t="n">
-        <v>49571179</v>
+        <v>49592179</v>
       </c>
       <c r="E971" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>25174</v>
+        <v>25192</v>
       </c>
       <c r="D974" t="n">
-        <v>36511784</v>
+        <v>36537605</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47134,10 +47134,10 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D975" t="n">
-        <v>874152</v>
+        <v>875552</v>
       </c>
       <c r="E975" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>1985</v>
+        <v>1988</v>
       </c>
       <c r="D977" t="n">
-        <v>2794805</v>
+        <v>2799305</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47278,10 +47278,10 @@
         </is>
       </c>
       <c r="C978" t="n">
-        <v>10759</v>
+        <v>10764</v>
       </c>
       <c r="D978" t="n">
-        <v>14032677</v>
+        <v>14038986</v>
       </c>
       <c r="E978" t="inlineStr">
         <is>
@@ -47470,10 +47470,10 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>3461</v>
+        <v>3463</v>
       </c>
       <c r="D982" t="n">
-        <v>5054695</v>
+        <v>5057695</v>
       </c>
       <c r="E982" t="inlineStr">
         <is>
@@ -47758,10 +47758,10 @@
         </is>
       </c>
       <c r="C988" t="n">
-        <v>55938</v>
+        <v>55967</v>
       </c>
       <c r="D988" t="n">
-        <v>70027988</v>
+        <v>70058738</v>
       </c>
       <c r="E988" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D992" t="n">
-        <v>256663</v>
+        <v>257676</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -47998,10 +47998,10 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>18494</v>
+        <v>18497</v>
       </c>
       <c r="D993" t="n">
-        <v>27085283</v>
+        <v>27089783</v>
       </c>
       <c r="E993" t="inlineStr">
         <is>
@@ -48094,10 +48094,10 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>12607</v>
+        <v>12611</v>
       </c>
       <c r="D995" t="n">
-        <v>18231186</v>
+        <v>18237186</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D998" t="n">
-        <v>1039501</v>
+        <v>1041001</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48286,10 +48286,10 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>28223</v>
+        <v>28241</v>
       </c>
       <c r="D999" t="n">
-        <v>35117724</v>
+        <v>35143128</v>
       </c>
       <c r="E999" t="inlineStr">
         <is>
@@ -48526,10 +48526,10 @@
         </is>
       </c>
       <c r="C1004" t="n">
-        <v>10491</v>
+        <v>10493</v>
       </c>
       <c r="D1004" t="n">
-        <v>15365684</v>
+        <v>15368236</v>
       </c>
       <c r="E1004" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>6215</v>
+        <v>6216</v>
       </c>
       <c r="D1006" t="n">
-        <v>9012605</v>
+        <v>9014105</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>
@@ -48670,10 +48670,10 @@
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D1007" t="n">
-        <v>747418</v>
+        <v>748918</v>
       </c>
       <c r="E1007" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16742</v>
+        <v>16759</v>
       </c>
       <c r="D2" t="n">
-        <v>21028591</v>
+        <v>21046625</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6327</v>
+        <v>6329</v>
       </c>
       <c r="D6" t="n">
-        <v>9253697</v>
+        <v>9256486</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3367</v>
+        <v>3373</v>
       </c>
       <c r="D8" t="n">
-        <v>4872524</v>
+        <v>4881524</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D11" t="n">
-        <v>548998</v>
+        <v>553498</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11227</v>
+        <v>11236</v>
       </c>
       <c r="D12" t="n">
-        <v>14167382</v>
+        <v>14178093</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3282</v>
+        <v>3284</v>
       </c>
       <c r="D16" t="n">
-        <v>4777927</v>
+        <v>4780927</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D18" t="n">
-        <v>2143220</v>
+        <v>2144720</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D19" t="n">
-        <v>565380</v>
+        <v>566880</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D21" t="n">
-        <v>309475</v>
+        <v>312475</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>14591</v>
+        <v>14608</v>
       </c>
       <c r="D22" t="n">
-        <v>17857740</v>
+        <v>17873238</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1582,10 +1582,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5017</v>
+        <v>5018</v>
       </c>
       <c r="D26" t="n">
-        <v>7332355</v>
+        <v>7333855</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="D28" t="n">
-        <v>2511434</v>
+        <v>2512934</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D31" t="n">
-        <v>503734</v>
+        <v>506734</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6719</v>
+        <v>6722</v>
       </c>
       <c r="D32" t="n">
-        <v>8923223</v>
+        <v>8927723</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1635</v>
+        <v>1640</v>
       </c>
       <c r="D35" t="n">
-        <v>2357910</v>
+        <v>2365410</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2062,10 +2062,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D36" t="n">
-        <v>10513</v>
+        <v>12013</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>22351</v>
+        <v>22378</v>
       </c>
       <c r="D41" t="n">
-        <v>27498500</v>
+        <v>27529109</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7907</v>
+        <v>7914</v>
       </c>
       <c r="D47" t="n">
-        <v>11615210</v>
+        <v>11625472</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3928</v>
+        <v>3934</v>
       </c>
       <c r="D49" t="n">
-        <v>5684734</v>
+        <v>5691315</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="D52" t="n">
-        <v>884833</v>
+        <v>890238</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8300</v>
+        <v>8302</v>
       </c>
       <c r="D53" t="n">
-        <v>10584847</v>
+        <v>10587017</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2822</v>
+        <v>2823</v>
       </c>
       <c r="D57" t="n">
-        <v>4104328</v>
+        <v>4105828</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="D59" t="n">
-        <v>1465221</v>
+        <v>1468221</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>37119</v>
+        <v>37178</v>
       </c>
       <c r="D62" t="n">
-        <v>47776961</v>
+        <v>47854739</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>13435</v>
+        <v>13442</v>
       </c>
       <c r="D67" t="n">
-        <v>19700151</v>
+        <v>19710651</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5294</v>
+        <v>5297</v>
       </c>
       <c r="D69" t="n">
-        <v>7652234</v>
+        <v>7656734</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D73" t="n">
-        <v>504516</v>
+        <v>507516</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>47261</v>
+        <v>47318</v>
       </c>
       <c r="D75" t="n">
-        <v>60375986</v>
+        <v>60438594</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18433</v>
+        <v>18451</v>
       </c>
       <c r="D79" t="n">
-        <v>27000116</v>
+        <v>27027116</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9570</v>
+        <v>9575</v>
       </c>
       <c r="D81" t="n">
-        <v>13814988</v>
+        <v>13822488</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="D85" t="n">
-        <v>1193505</v>
+        <v>1199329</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>25436</v>
+        <v>25467</v>
       </c>
       <c r="D86" t="n">
-        <v>32061466</v>
+        <v>32098166</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8803</v>
+        <v>8807</v>
       </c>
       <c r="D90" t="n">
-        <v>12922818</v>
+        <v>12928818</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>5019</v>
+        <v>5025</v>
       </c>
       <c r="D92" t="n">
-        <v>7253940</v>
+        <v>7260757</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="D94" t="n">
-        <v>1131891</v>
+        <v>1137246</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>22448</v>
+        <v>22464</v>
       </c>
       <c r="D95" t="n">
-        <v>28152028</v>
+        <v>28168480</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9300</v>
+        <v>9305</v>
       </c>
       <c r="D99" t="n">
-        <v>13613739</v>
+        <v>13621239</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5182,10 +5182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3389</v>
+        <v>3393</v>
       </c>
       <c r="D101" t="n">
-        <v>4853936</v>
+        <v>4859936</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D105" t="n">
-        <v>657560</v>
+        <v>659060</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>84572</v>
+        <v>84686</v>
       </c>
       <c r="D106" t="n">
-        <v>108384694</v>
+        <v>108520405</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>31148</v>
+        <v>31170</v>
       </c>
       <c r="D113" t="n">
-        <v>45709973</v>
+        <v>45742019</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>21476</v>
+        <v>21505</v>
       </c>
       <c r="D115" t="n">
-        <v>30993790</v>
+        <v>31034752</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2000</v>
+        <v>2009</v>
       </c>
       <c r="D122" t="n">
-        <v>2813867</v>
+        <v>2827367</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>28221</v>
+        <v>28252</v>
       </c>
       <c r="D123" t="n">
-        <v>37220005</v>
+        <v>37262772</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6430,10 +6430,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>10046</v>
+        <v>10055</v>
       </c>
       <c r="D127" t="n">
-        <v>14732917</v>
+        <v>14746417</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -6526,10 +6526,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3355</v>
+        <v>3360</v>
       </c>
       <c r="D129" t="n">
-        <v>4880934</v>
+        <v>4888434</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D132" t="n">
-        <v>509152</v>
+        <v>512152</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>16136</v>
+        <v>16144</v>
       </c>
       <c r="D133" t="n">
-        <v>20040338</v>
+        <v>20048405</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7889</v>
+        <v>7894</v>
       </c>
       <c r="D137" t="n">
-        <v>11539295</v>
+        <v>11546795</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7006,10 +7006,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2270</v>
+        <v>2273</v>
       </c>
       <c r="D139" t="n">
-        <v>3239613</v>
+        <v>3243230</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D143" t="n">
-        <v>582640</v>
+        <v>588408</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>13858</v>
+        <v>13867</v>
       </c>
       <c r="D144" t="n">
-        <v>17296579</v>
+        <v>17305833</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>6340</v>
+        <v>6347</v>
       </c>
       <c r="D148" t="n">
-        <v>9284813</v>
+        <v>9295313</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>2025</v>
+        <v>2028</v>
       </c>
       <c r="D150" t="n">
-        <v>2925174</v>
+        <v>2929674</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D153" t="n">
-        <v>531932</v>
+        <v>533432</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>6125</v>
+        <v>6133</v>
       </c>
       <c r="D154" t="n">
-        <v>7495708</v>
+        <v>7506945</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="D157" t="n">
-        <v>3054497</v>
+        <v>3055997</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D158" t="n">
-        <v>998327</v>
+        <v>999827</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7601</v>
+        <v>7604</v>
       </c>
       <c r="D162" t="n">
-        <v>9411002</v>
+        <v>9413422</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>2902</v>
+        <v>2905</v>
       </c>
       <c r="D165" t="n">
-        <v>4254605</v>
+        <v>4258823</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -8494,10 +8494,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>5726</v>
+        <v>5728</v>
       </c>
       <c r="D170" t="n">
-        <v>7191663</v>
+        <v>7194048</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -8734,10 +8734,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="D175" t="n">
-        <v>2990432</v>
+        <v>2991932</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -8974,10 +8974,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>16370</v>
+        <v>16382</v>
       </c>
       <c r="D180" t="n">
-        <v>20535169</v>
+        <v>20548885</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -9214,10 +9214,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>6487</v>
+        <v>6489</v>
       </c>
       <c r="D185" t="n">
-        <v>9477188</v>
+        <v>9480090</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>2272</v>
+        <v>2275</v>
       </c>
       <c r="D186" t="n">
-        <v>3263037</v>
+        <v>3267537</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D189" t="n">
-        <v>675912</v>
+        <v>677102</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>3142</v>
+        <v>3144</v>
       </c>
       <c r="D190" t="n">
-        <v>3943566</v>
+        <v>3946566</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D197" t="n">
-        <v>74165</v>
+        <v>75665</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>9390</v>
+        <v>9401</v>
       </c>
       <c r="D198" t="n">
-        <v>11722151</v>
+        <v>11731864</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -10030,10 +10030,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>3479</v>
+        <v>3481</v>
       </c>
       <c r="D202" t="n">
-        <v>5109719</v>
+        <v>5112719</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="D203" t="n">
-        <v>2371673</v>
+        <v>2374673</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D206" t="n">
-        <v>315891</v>
+        <v>317391</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>17589</v>
+        <v>17599</v>
       </c>
       <c r="D207" t="n">
-        <v>21941376</v>
+        <v>21952733</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>7781</v>
+        <v>7783</v>
       </c>
       <c r="D211" t="n">
-        <v>11425683</v>
+        <v>11428041</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="D214" t="n">
-        <v>706218</v>
+        <v>711245</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>26611</v>
+        <v>26630</v>
       </c>
       <c r="D215" t="n">
-        <v>33518064</v>
+        <v>33538854</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>10611</v>
+        <v>10619</v>
       </c>
       <c r="D219" t="n">
-        <v>15498825</v>
+        <v>15510825</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2692</v>
+        <v>2694</v>
       </c>
       <c r="D221" t="n">
-        <v>3880420</v>
+        <v>3883420</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D224" t="n">
-        <v>894052</v>
+        <v>897998</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11134,10 +11134,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>29203</v>
+        <v>29229</v>
       </c>
       <c r="D225" t="n">
-        <v>36811155</v>
+        <v>36845874</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>14981</v>
+        <v>14995</v>
       </c>
       <c r="D230" t="n">
-        <v>21983837</v>
+        <v>22003646</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>2730</v>
+        <v>2736</v>
       </c>
       <c r="D232" t="n">
-        <v>3919538</v>
+        <v>3928005</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="D235" t="n">
-        <v>1097008</v>
+        <v>1100008</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11662,10 +11662,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>24837</v>
+        <v>24857</v>
       </c>
       <c r="D236" t="n">
-        <v>31295019</v>
+        <v>31316453</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>11322</v>
+        <v>11331</v>
       </c>
       <c r="D242" t="n">
-        <v>16592721</v>
+        <v>16606221</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12046,10 +12046,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2568</v>
+        <v>2574</v>
       </c>
       <c r="D244" t="n">
-        <v>3664854</v>
+        <v>3671364</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -12190,10 +12190,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D247" t="n">
-        <v>666570</v>
+        <v>668070</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -12238,10 +12238,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>8022</v>
+        <v>8028</v>
       </c>
       <c r="D248" t="n">
-        <v>10032218</v>
+        <v>10041088</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D251" t="n">
-        <v>55209</v>
+        <v>58209</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12574,10 +12574,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D255" t="n">
-        <v>1493115</v>
+        <v>1496115</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -12718,10 +12718,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>10046</v>
+        <v>10057</v>
       </c>
       <c r="D258" t="n">
-        <v>12823134</v>
+        <v>12836194</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>4277</v>
+        <v>4278</v>
       </c>
       <c r="D262" t="n">
-        <v>6278873</v>
+        <v>6280373</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>2235</v>
+        <v>2239</v>
       </c>
       <c r="D264" t="n">
-        <v>3237318</v>
+        <v>3241402</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D265" t="n">
-        <v>143696</v>
+        <v>145196</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13102,10 +13102,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D266" t="n">
-        <v>189441</v>
+        <v>190941</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>5674</v>
+        <v>5675</v>
       </c>
       <c r="D267" t="n">
-        <v>7022756</v>
+        <v>7023956</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="D270" t="n">
-        <v>2996230</v>
+        <v>2997730</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13390,10 +13390,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D272" t="n">
-        <v>1059650</v>
+        <v>1061150</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -13582,10 +13582,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>19537</v>
+        <v>19544</v>
       </c>
       <c r="D276" t="n">
-        <v>24659805</v>
+        <v>24664874</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>8090</v>
+        <v>8097</v>
       </c>
       <c r="D280" t="n">
-        <v>11860814</v>
+        <v>11869956</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13870,10 +13870,10 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>2557</v>
+        <v>2561</v>
       </c>
       <c r="D282" t="n">
-        <v>3674894</v>
+        <v>3680894</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D283" t="n">
-        <v>712598</v>
+        <v>714098</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D285" t="n">
-        <v>702669</v>
+        <v>703636</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14110,10 +14110,10 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>16988</v>
+        <v>17003</v>
       </c>
       <c r="D287" t="n">
-        <v>21039209</v>
+        <v>21056074</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>7317</v>
+        <v>7325</v>
       </c>
       <c r="D292" t="n">
-        <v>10732825</v>
+        <v>10744825</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>3422</v>
+        <v>3426</v>
       </c>
       <c r="D293" t="n">
-        <v>4958125</v>
+        <v>4964125</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D296" t="n">
-        <v>484545</v>
+        <v>485252</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14590,10 +14590,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>9568</v>
+        <v>9575</v>
       </c>
       <c r="D297" t="n">
-        <v>12008619</v>
+        <v>12017343</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="D302" t="n">
-        <v>1862733</v>
+        <v>1865733</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>9382</v>
+        <v>9389</v>
       </c>
       <c r="D307" t="n">
-        <v>12254297</v>
+        <v>12262630</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3809</v>
+        <v>3810</v>
       </c>
       <c r="D311" t="n">
-        <v>5570040</v>
+        <v>5571540</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>2412</v>
+        <v>2413</v>
       </c>
       <c r="D312" t="n">
-        <v>3510064</v>
+        <v>3511564</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D313" t="n">
-        <v>336665</v>
+        <v>338165</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>11333</v>
+        <v>11350</v>
       </c>
       <c r="D315" t="n">
-        <v>14873461</v>
+        <v>14894960</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>3860</v>
+        <v>3862</v>
       </c>
       <c r="D319" t="n">
-        <v>5660316</v>
+        <v>5663316</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15838,10 +15838,10 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D323" t="n">
-        <v>247696</v>
+        <v>252196</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>6957</v>
+        <v>6962</v>
       </c>
       <c r="D324" t="n">
-        <v>8597081</v>
+        <v>8604032</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>2332</v>
+        <v>2333</v>
       </c>
       <c r="D329" t="n">
-        <v>3420759</v>
+        <v>3422259</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16318,10 +16318,10 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D333" t="n">
-        <v>192551</v>
+        <v>194051</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -16366,10 +16366,10 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>7697</v>
+        <v>7706</v>
       </c>
       <c r="D334" t="n">
-        <v>9623635</v>
+        <v>9634365</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -16606,10 +16606,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>3186</v>
+        <v>3192</v>
       </c>
       <c r="D339" t="n">
-        <v>4653308</v>
+        <v>4661518</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D340" t="n">
-        <v>1899567</v>
+        <v>1901067</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>32859</v>
+        <v>32900</v>
       </c>
       <c r="D343" t="n">
-        <v>41291806</v>
+        <v>41344025</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>16858</v>
+        <v>16878</v>
       </c>
       <c r="D349" t="n">
-        <v>24647431</v>
+        <v>24677063</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>8251</v>
+        <v>8258</v>
       </c>
       <c r="D352" t="n">
-        <v>11885244</v>
+        <v>11895482</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D353" t="n">
-        <v>933263</v>
+        <v>934763</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c r="D354" t="n">
-        <v>1184226</v>
+        <v>1193805</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>4010</v>
+        <v>4012</v>
       </c>
       <c r="D355" t="n">
-        <v>4990718</v>
+        <v>4993164</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17518,10 +17518,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1515</v>
+        <v>1517</v>
       </c>
       <c r="D358" t="n">
-        <v>2234310</v>
+        <v>2237091</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D362" t="n">
-        <v>121595</v>
+        <v>124595</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>19868</v>
+        <v>19890</v>
       </c>
       <c r="D363" t="n">
-        <v>24742671</v>
+        <v>24764785</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>10095</v>
+        <v>10105</v>
       </c>
       <c r="D367" t="n">
-        <v>14800926</v>
+        <v>14814806</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>4847</v>
+        <v>4848</v>
       </c>
       <c r="D369" t="n">
-        <v>7013106</v>
+        <v>7014606</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>14274</v>
+        <v>14286</v>
       </c>
       <c r="D372" t="n">
-        <v>17837739</v>
+        <v>17851779</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>6556</v>
+        <v>6564</v>
       </c>
       <c r="D376" t="n">
-        <v>9598427</v>
+        <v>9610427</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>2550</v>
+        <v>2551</v>
       </c>
       <c r="D378" t="n">
-        <v>3660281</v>
+        <v>3661781</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18622,10 +18622,10 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>18442</v>
+        <v>18462</v>
       </c>
       <c r="D381" t="n">
-        <v>22969027</v>
+        <v>22994631</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>7257</v>
+        <v>7262</v>
       </c>
       <c r="D385" t="n">
-        <v>10663790</v>
+        <v>10671290</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>2900</v>
+        <v>2904</v>
       </c>
       <c r="D387" t="n">
-        <v>4217701</v>
+        <v>4223701</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D390" t="n">
-        <v>586489</v>
+        <v>589489</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>4190</v>
+        <v>4193</v>
       </c>
       <c r="D391" t="n">
-        <v>5252995</v>
+        <v>5256753</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19390,10 +19390,10 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D397" t="n">
-        <v>124310</v>
+        <v>127310</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>22799</v>
+        <v>22819</v>
       </c>
       <c r="D398" t="n">
-        <v>28242516</v>
+        <v>28267587</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>9506</v>
+        <v>9515</v>
       </c>
       <c r="D401" t="n">
-        <v>13995028</v>
+        <v>14008528</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>6350</v>
+        <v>6352</v>
       </c>
       <c r="D403" t="n">
-        <v>9234034</v>
+        <v>9237034</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D405" t="n">
-        <v>522070</v>
+        <v>523570</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>11436</v>
+        <v>11449</v>
       </c>
       <c r="D406" t="n">
-        <v>14079071</v>
+        <v>14096170</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>5418</v>
+        <v>5423</v>
       </c>
       <c r="D411" t="n">
-        <v>7918983</v>
+        <v>7926483</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="D413" t="n">
-        <v>2726842</v>
+        <v>2728342</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D414" t="n">
-        <v>203582</v>
+        <v>204733</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>33857</v>
+        <v>33925</v>
       </c>
       <c r="D416" t="n">
-        <v>45886126</v>
+        <v>45982281</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D419" t="n">
-        <v>43314</v>
+        <v>44814</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>8212</v>
+        <v>8226</v>
       </c>
       <c r="D420" t="n">
-        <v>12072127</v>
+        <v>12091517</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>7549</v>
+        <v>7571</v>
       </c>
       <c r="D422" t="n">
-        <v>10951980</v>
+        <v>10984190</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D425" t="n">
-        <v>725891</v>
+        <v>727391</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>10635</v>
+        <v>10692</v>
       </c>
       <c r="D426" t="n">
-        <v>16360661</v>
+        <v>16480189</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>2610</v>
+        <v>2627</v>
       </c>
       <c r="D428" t="n">
-        <v>4285676</v>
+        <v>4329376</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>3539</v>
+        <v>3578</v>
       </c>
       <c r="D430" t="n">
-        <v>5817151</v>
+        <v>5911207</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>11273</v>
+        <v>11285</v>
       </c>
       <c r="D434" t="n">
-        <v>13924552</v>
+        <v>13941052</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>3865</v>
+        <v>3867</v>
       </c>
       <c r="D437" t="n">
-        <v>5671558</v>
+        <v>5674558</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>1915</v>
+        <v>1917</v>
       </c>
       <c r="D439" t="n">
-        <v>2743942</v>
+        <v>2746942</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D441" t="n">
-        <v>235364</v>
+        <v>236864</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21550,10 +21550,10 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>64729</v>
+        <v>64785</v>
       </c>
       <c r="D442" t="n">
-        <v>80187229</v>
+        <v>80259550</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>25393</v>
+        <v>25401</v>
       </c>
       <c r="D446" t="n">
-        <v>37212117</v>
+        <v>37222442</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21838,10 +21838,10 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>13390</v>
+        <v>13402</v>
       </c>
       <c r="D448" t="n">
-        <v>19420429</v>
+        <v>19438149</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="D452" t="n">
-        <v>1552555</v>
+        <v>1555555</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>19515</v>
+        <v>19545</v>
       </c>
       <c r="D454" t="n">
-        <v>24696884</v>
+        <v>24738036</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>7851</v>
+        <v>7858</v>
       </c>
       <c r="D458" t="n">
-        <v>11519923</v>
+        <v>11530423</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>5069</v>
+        <v>5076</v>
       </c>
       <c r="D460" t="n">
-        <v>7358259</v>
+        <v>7368759</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22558,10 +22558,10 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>32944</v>
+        <v>32969</v>
       </c>
       <c r="D463" t="n">
-        <v>40245541</v>
+        <v>40274492</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>11643</v>
+        <v>11649</v>
       </c>
       <c r="D467" t="n">
-        <v>17033315</v>
+        <v>17041025</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>4985</v>
+        <v>4989</v>
       </c>
       <c r="D469" t="n">
-        <v>7234822</v>
+        <v>7238586</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -22990,10 +22990,10 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>14718</v>
+        <v>14735</v>
       </c>
       <c r="D472" t="n">
-        <v>17987870</v>
+        <v>18004950</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>4460</v>
+        <v>4462</v>
       </c>
       <c r="D477" t="n">
-        <v>6553821</v>
+        <v>6555661</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23470,10 +23470,10 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>37834</v>
+        <v>37923</v>
       </c>
       <c r="D482" t="n">
-        <v>49394389</v>
+        <v>49517301</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -23662,10 +23662,10 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>13880</v>
+        <v>13888</v>
       </c>
       <c r="D486" t="n">
-        <v>20418867</v>
+        <v>20430142</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>12611</v>
+        <v>12636</v>
       </c>
       <c r="D488" t="n">
-        <v>18415150</v>
+        <v>18451199</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D489" t="n">
-        <v>275921</v>
+        <v>276374</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -23854,10 +23854,10 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D490" t="n">
-        <v>446240</v>
+        <v>446522</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -23902,10 +23902,10 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>66302</v>
+        <v>66441</v>
       </c>
       <c r="D491" t="n">
-        <v>87926945</v>
+        <v>88104482</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D494" t="n">
-        <v>202955</v>
+        <v>204455</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24142,10 +24142,10 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>23848</v>
+        <v>23890</v>
       </c>
       <c r="D496" t="n">
-        <v>35000155</v>
+        <v>35062053</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -24238,10 +24238,10 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>23805</v>
+        <v>23857</v>
       </c>
       <c r="D498" t="n">
-        <v>34579738</v>
+        <v>34656316</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="D501" t="n">
-        <v>955377</v>
+        <v>958377</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>158803</v>
+        <v>159190</v>
       </c>
       <c r="D502" t="n">
-        <v>208793321</v>
+        <v>209283303</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D507" t="n">
-        <v>712555</v>
+        <v>715555</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>84385</v>
+        <v>84552</v>
       </c>
       <c r="D509" t="n">
-        <v>123965190</v>
+        <v>124213496</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D510" t="n">
-        <v>370302</v>
+        <v>373302</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -24910,10 +24910,10 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>62829</v>
+        <v>62956</v>
       </c>
       <c r="D512" t="n">
-        <v>91248189</v>
+        <v>91434253</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>2967</v>
+        <v>2992</v>
       </c>
       <c r="D516" t="n">
-        <v>4197701</v>
+        <v>4234190</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25246,10 +25246,10 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>43354</v>
+        <v>43447</v>
       </c>
       <c r="D519" t="n">
-        <v>56469030</v>
+        <v>56588097</v>
       </c>
       <c r="E519" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>15626</v>
+        <v>15649</v>
       </c>
       <c r="D524" t="n">
-        <v>22950518</v>
+        <v>22983733</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25582,10 +25582,10 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>13527</v>
+        <v>13551</v>
       </c>
       <c r="D526" t="n">
-        <v>19611122</v>
+        <v>19646960</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>71104</v>
+        <v>71298</v>
       </c>
       <c r="D531" t="n">
-        <v>95837710</v>
+        <v>96103777</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>24002</v>
+        <v>24040</v>
       </c>
       <c r="D535" t="n">
-        <v>35414502</v>
+        <v>35470018</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>25772</v>
+        <v>25843</v>
       </c>
       <c r="D537" t="n">
-        <v>37724141</v>
+        <v>37826766</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26206,10 +26206,10 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D539" t="n">
-        <v>372110</v>
+        <v>373610</v>
       </c>
       <c r="E539" t="inlineStr">
         <is>
@@ -26254,10 +26254,10 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="D540" t="n">
-        <v>1287255</v>
+        <v>1294755</v>
       </c>
       <c r="E540" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>58459</v>
+        <v>58594</v>
       </c>
       <c r="D541" t="n">
-        <v>77666282</v>
+        <v>77836915</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26542,10 +26542,10 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>18298</v>
+        <v>18330</v>
       </c>
       <c r="D546" t="n">
-        <v>26888887</v>
+        <v>26935555</v>
       </c>
       <c r="E546" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>19380</v>
+        <v>19426</v>
       </c>
       <c r="D548" t="n">
-        <v>28193658</v>
+        <v>28259264</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26734,10 +26734,10 @@
         </is>
       </c>
       <c r="C550" t="n">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D550" t="n">
-        <v>924829</v>
+        <v>927829</v>
       </c>
       <c r="E550" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>44405</v>
+        <v>44505</v>
       </c>
       <c r="D551" t="n">
-        <v>59144156</v>
+        <v>59280064</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>14543</v>
+        <v>14556</v>
       </c>
       <c r="D555" t="n">
-        <v>21449835</v>
+        <v>21466769</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>15275</v>
+        <v>15311</v>
       </c>
       <c r="D557" t="n">
-        <v>22194019</v>
+        <v>22245698</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="D559" t="n">
-        <v>425559</v>
+        <v>435891</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>43169</v>
+        <v>43250</v>
       </c>
       <c r="D560" t="n">
-        <v>56068307</v>
+        <v>56177188</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27406,10 +27406,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>16567</v>
+        <v>16596</v>
       </c>
       <c r="D564" t="n">
-        <v>24304977</v>
+        <v>24343763</v>
       </c>
       <c r="E564" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>13598</v>
+        <v>13626</v>
       </c>
       <c r="D566" t="n">
-        <v>19680064</v>
+        <v>19721716</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27646,10 +27646,10 @@
         </is>
       </c>
       <c r="C569" t="n">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D569" t="n">
-        <v>525731</v>
+        <v>528731</v>
       </c>
       <c r="E569" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>45408</v>
+        <v>45474</v>
       </c>
       <c r="D570" t="n">
-        <v>60617729</v>
+        <v>60698389</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27982,10 +27982,10 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>14244</v>
+        <v>14260</v>
       </c>
       <c r="D576" t="n">
-        <v>20883723</v>
+        <v>20907241</v>
       </c>
       <c r="E576" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>3815</v>
+        <v>3819</v>
       </c>
       <c r="D577" t="n">
-        <v>5501740</v>
+        <v>5507100</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D580" t="n">
-        <v>581216</v>
+        <v>582716</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28270,10 +28270,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D582" t="n">
-        <v>562763</v>
+        <v>564263</v>
       </c>
       <c r="E582" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>17900</v>
+        <v>17938</v>
       </c>
       <c r="D583" t="n">
-        <v>23657680</v>
+        <v>23708075</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28510,10 +28510,10 @@
         </is>
       </c>
       <c r="C587" t="n">
-        <v>7289</v>
+        <v>7298</v>
       </c>
       <c r="D587" t="n">
-        <v>10605404</v>
+        <v>10618344</v>
       </c>
       <c r="E587" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>5095</v>
+        <v>5099</v>
       </c>
       <c r="D589" t="n">
-        <v>7334996</v>
+        <v>7340996</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D592" t="n">
-        <v>389364</v>
+        <v>392364</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>18907</v>
+        <v>18987</v>
       </c>
       <c r="D594" t="n">
-        <v>30982945</v>
+        <v>31173397</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>2054</v>
+        <v>2067</v>
       </c>
       <c r="D595" t="n">
-        <v>3385072</v>
+        <v>3417822</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -29086,10 +29086,10 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D599" t="n">
-        <v>182949</v>
+        <v>188949</v>
       </c>
       <c r="E599" t="inlineStr">
         <is>
@@ -29134,10 +29134,10 @@
         </is>
       </c>
       <c r="C600" t="n">
-        <v>22578</v>
+        <v>22595</v>
       </c>
       <c r="D600" t="n">
-        <v>28290879</v>
+        <v>28306812</v>
       </c>
       <c r="E600" t="inlineStr">
         <is>
@@ -29374,10 +29374,10 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>9156</v>
+        <v>9158</v>
       </c>
       <c r="D605" t="n">
-        <v>13411248</v>
+        <v>13413879</v>
       </c>
       <c r="E605" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>3424</v>
+        <v>3425</v>
       </c>
       <c r="D607" t="n">
-        <v>4917669</v>
+        <v>4919169</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D608" t="n">
-        <v>505484</v>
+        <v>506984</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>15025</v>
+        <v>15041</v>
       </c>
       <c r="D611" t="n">
-        <v>18821991</v>
+        <v>18840368</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>5888</v>
+        <v>5892</v>
       </c>
       <c r="D615" t="n">
-        <v>8646917</v>
+        <v>8652917</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -29950,10 +29950,10 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>2754</v>
+        <v>2755</v>
       </c>
       <c r="D617" t="n">
-        <v>3971874</v>
+        <v>3973374</v>
       </c>
       <c r="E617" t="inlineStr">
         <is>
@@ -30046,10 +30046,10 @@
         </is>
       </c>
       <c r="C619" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D619" t="n">
-        <v>277056</v>
+        <v>278658</v>
       </c>
       <c r="E619" t="inlineStr">
         <is>
@@ -30094,10 +30094,10 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>14060</v>
+        <v>14070</v>
       </c>
       <c r="D620" t="n">
-        <v>17733155</v>
+        <v>17744890</v>
       </c>
       <c r="E620" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>5302</v>
+        <v>5303</v>
       </c>
       <c r="D624" t="n">
-        <v>7768105</v>
+        <v>7769605</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D625" t="n">
-        <v>1731187</v>
+        <v>1732687</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30526,10 +30526,10 @@
         </is>
       </c>
       <c r="C629" t="n">
-        <v>7684</v>
+        <v>7688</v>
       </c>
       <c r="D629" t="n">
-        <v>9875274</v>
+        <v>9879528</v>
       </c>
       <c r="E629" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>2599</v>
+        <v>2601</v>
       </c>
       <c r="D634" t="n">
-        <v>3807854</v>
+        <v>3810854</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="D635" t="n">
-        <v>1244614</v>
+        <v>1246114</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D636" t="n">
-        <v>251518</v>
+        <v>252928</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>29457</v>
+        <v>29476</v>
       </c>
       <c r="D638" t="n">
-        <v>36258485</v>
+        <v>36279521</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31198,10 +31198,10 @@
         </is>
       </c>
       <c r="C643" t="n">
-        <v>11230</v>
+        <v>11235</v>
       </c>
       <c r="D643" t="n">
-        <v>16478579</v>
+        <v>16486079</v>
       </c>
       <c r="E643" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>4961</v>
+        <v>4963</v>
       </c>
       <c r="D645" t="n">
-        <v>7196013</v>
+        <v>7199013</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31438,10 +31438,10 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D648" t="n">
-        <v>838259</v>
+        <v>842289</v>
       </c>
       <c r="E648" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>11564</v>
+        <v>11575</v>
       </c>
       <c r="D649" t="n">
-        <v>13979783</v>
+        <v>13993360</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D658" t="n">
-        <v>339496</v>
+        <v>340996</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>28812</v>
+        <v>28832</v>
       </c>
       <c r="D659" t="n">
-        <v>35801813</v>
+        <v>35828329</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>10856</v>
+        <v>10862</v>
       </c>
       <c r="D663" t="n">
-        <v>15950798</v>
+        <v>15959698</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32398,10 +32398,10 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D668" t="n">
-        <v>699657</v>
+        <v>700090</v>
       </c>
       <c r="E668" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>7614</v>
+        <v>7621</v>
       </c>
       <c r="D669" t="n">
-        <v>9650614</v>
+        <v>9661114</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D676" t="n">
-        <v>242490</v>
+        <v>242703</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32830,10 +32830,10 @@
         </is>
       </c>
       <c r="C677" t="n">
-        <v>3866</v>
+        <v>3869</v>
       </c>
       <c r="D677" t="n">
-        <v>4677089</v>
+        <v>4680334</v>
       </c>
       <c r="E677" t="inlineStr">
         <is>
@@ -33118,10 +33118,10 @@
         </is>
       </c>
       <c r="C683" t="n">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D683" t="n">
-        <v>651745</v>
+        <v>653245</v>
       </c>
       <c r="E683" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>9495</v>
+        <v>9501</v>
       </c>
       <c r="D686" t="n">
-        <v>11821969</v>
+        <v>11827324</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>3519</v>
+        <v>3522</v>
       </c>
       <c r="D690" t="n">
-        <v>5188223</v>
+        <v>5192723</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D694" t="n">
-        <v>404579</v>
+        <v>407579</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>19622</v>
+        <v>19640</v>
       </c>
       <c r="D695" t="n">
-        <v>24006420</v>
+        <v>24022502</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33886,10 +33886,10 @@
         </is>
       </c>
       <c r="C699" t="n">
-        <v>5806</v>
+        <v>5809</v>
       </c>
       <c r="D699" t="n">
-        <v>8481510</v>
+        <v>8486010</v>
       </c>
       <c r="E699" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>2299</v>
+        <v>2301</v>
       </c>
       <c r="D701" t="n">
-        <v>3307317</v>
+        <v>3310317</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>76439</v>
+        <v>76513</v>
       </c>
       <c r="D706" t="n">
-        <v>96242420</v>
+        <v>96331435</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34462,10 +34462,10 @@
         </is>
       </c>
       <c r="C711" t="n">
-        <v>26978</v>
+        <v>27002</v>
       </c>
       <c r="D711" t="n">
-        <v>39603491</v>
+        <v>39638711</v>
       </c>
       <c r="E711" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>13481</v>
+        <v>13503</v>
       </c>
       <c r="D714" t="n">
-        <v>19448441</v>
+        <v>19481260</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>
@@ -34846,10 +34846,10 @@
         </is>
       </c>
       <c r="C719" t="n">
-        <v>1273</v>
+        <v>1277</v>
       </c>
       <c r="D719" t="n">
-        <v>1775231</v>
+        <v>1781231</v>
       </c>
       <c r="E719" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>11394</v>
+        <v>11404</v>
       </c>
       <c r="D720" t="n">
-        <v>13930808</v>
+        <v>13939855</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -35038,10 +35038,10 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>4165</v>
+        <v>4167</v>
       </c>
       <c r="D723" t="n">
-        <v>6092773</v>
+        <v>6095773</v>
       </c>
       <c r="E723" t="inlineStr">
         <is>
@@ -35134,10 +35134,10 @@
         </is>
       </c>
       <c r="C725" t="n">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="D725" t="n">
-        <v>2199840</v>
+        <v>2204340</v>
       </c>
       <c r="E725" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D727" t="n">
-        <v>358949</v>
+        <v>361475</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35278,10 +35278,10 @@
         </is>
       </c>
       <c r="C728" t="n">
-        <v>17967</v>
+        <v>17984</v>
       </c>
       <c r="D728" t="n">
-        <v>22140879</v>
+        <v>22161310</v>
       </c>
       <c r="E728" t="inlineStr">
         <is>
@@ -35470,10 +35470,10 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>6956</v>
+        <v>6960</v>
       </c>
       <c r="D732" t="n">
-        <v>10167316</v>
+        <v>10173316</v>
       </c>
       <c r="E732" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>2223</v>
+        <v>2225</v>
       </c>
       <c r="D734" t="n">
-        <v>3188117</v>
+        <v>3191117</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35662,10 +35662,10 @@
         </is>
       </c>
       <c r="C736" t="n">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D736" t="n">
-        <v>465189</v>
+        <v>467789</v>
       </c>
       <c r="E736" t="inlineStr">
         <is>
@@ -35710,10 +35710,10 @@
         </is>
       </c>
       <c r="C737" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D737" t="n">
-        <v>490010</v>
+        <v>491510</v>
       </c>
       <c r="E737" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>11761</v>
+        <v>11768</v>
       </c>
       <c r="D739" t="n">
-        <v>14509258</v>
+        <v>14515353</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>4290</v>
+        <v>4291</v>
       </c>
       <c r="D743" t="n">
-        <v>6289385</v>
+        <v>6290885</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36190,10 +36190,10 @@
         </is>
       </c>
       <c r="C747" t="n">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D747" t="n">
-        <v>452413</v>
+        <v>453281</v>
       </c>
       <c r="E747" t="inlineStr">
         <is>
@@ -36238,10 +36238,10 @@
         </is>
       </c>
       <c r="C748" t="n">
-        <v>30079</v>
+        <v>30112</v>
       </c>
       <c r="D748" t="n">
-        <v>37381757</v>
+        <v>37420883</v>
       </c>
       <c r="E748" t="inlineStr">
         <is>
@@ -36478,10 +36478,10 @@
         </is>
       </c>
       <c r="C753" t="n">
-        <v>12877</v>
+        <v>12885</v>
       </c>
       <c r="D753" t="n">
-        <v>18847738</v>
+        <v>18859738</v>
       </c>
       <c r="E753" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>4298</v>
+        <v>4303</v>
       </c>
       <c r="D755" t="n">
-        <v>6141651</v>
+        <v>6148027</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36718,10 +36718,10 @@
         </is>
       </c>
       <c r="C758" t="n">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="D758" t="n">
-        <v>1000546</v>
+        <v>1005046</v>
       </c>
       <c r="E758" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>12562</v>
+        <v>12564</v>
       </c>
       <c r="D760" t="n">
-        <v>15537092</v>
+        <v>15538887</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -36958,10 +36958,10 @@
         </is>
       </c>
       <c r="C763" t="n">
-        <v>4729</v>
+        <v>4731</v>
       </c>
       <c r="D763" t="n">
-        <v>6912723</v>
+        <v>6914698</v>
       </c>
       <c r="E763" t="inlineStr">
         <is>
@@ -37102,10 +37102,10 @@
         </is>
       </c>
       <c r="C766" t="n">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D766" t="n">
-        <v>563304</v>
+        <v>566304</v>
       </c>
       <c r="E766" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>6877</v>
+        <v>6885</v>
       </c>
       <c r="D767" t="n">
-        <v>8076044</v>
+        <v>8084220</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37342,10 +37342,10 @@
         </is>
       </c>
       <c r="C771" t="n">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="D771" t="n">
-        <v>2518058</v>
+        <v>2519558</v>
       </c>
       <c r="E771" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>17130</v>
+        <v>17144</v>
       </c>
       <c r="D775" t="n">
-        <v>20783778</v>
+        <v>20801117</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37774,10 +37774,10 @@
         </is>
       </c>
       <c r="C780" t="n">
-        <v>5622</v>
+        <v>5628</v>
       </c>
       <c r="D780" t="n">
-        <v>8239136</v>
+        <v>8248136</v>
       </c>
       <c r="E780" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>3478</v>
+        <v>3483</v>
       </c>
       <c r="D782" t="n">
-        <v>5078771</v>
+        <v>5085435</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38062,10 +38062,10 @@
         </is>
       </c>
       <c r="C786" t="n">
-        <v>11551</v>
+        <v>11564</v>
       </c>
       <c r="D786" t="n">
-        <v>14609217</v>
+        <v>14624380</v>
       </c>
       <c r="E786" t="inlineStr">
         <is>
@@ -38494,10 +38494,10 @@
         </is>
       </c>
       <c r="C795" t="n">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D795" t="n">
-        <v>337366</v>
+        <v>339677</v>
       </c>
       <c r="E795" t="inlineStr">
         <is>
@@ -38542,10 +38542,10 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>32776</v>
+        <v>32807</v>
       </c>
       <c r="D796" t="n">
-        <v>40407221</v>
+        <v>40443737</v>
       </c>
       <c r="E796" t="inlineStr">
         <is>
@@ -38734,10 +38734,10 @@
         </is>
       </c>
       <c r="C800" t="n">
-        <v>13347</v>
+        <v>13353</v>
       </c>
       <c r="D800" t="n">
-        <v>19527700</v>
+        <v>19536700</v>
       </c>
       <c r="E800" t="inlineStr">
         <is>
@@ -38830,10 +38830,10 @@
         </is>
       </c>
       <c r="C802" t="n">
-        <v>6154</v>
+        <v>6163</v>
       </c>
       <c r="D802" t="n">
-        <v>8892072</v>
+        <v>8905572</v>
       </c>
       <c r="E802" t="inlineStr">
         <is>
@@ -38878,10 +38878,10 @@
         </is>
       </c>
       <c r="C803" t="n">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D803" t="n">
-        <v>746333</v>
+        <v>746558</v>
       </c>
       <c r="E803" t="inlineStr">
         <is>
@@ -38974,10 +38974,10 @@
         </is>
       </c>
       <c r="C805" t="n">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D805" t="n">
-        <v>972636</v>
+        <v>975636</v>
       </c>
       <c r="E805" t="inlineStr">
         <is>
@@ -39022,10 +39022,10 @@
         </is>
       </c>
       <c r="C806" t="n">
-        <v>7798</v>
+        <v>7809</v>
       </c>
       <c r="D806" t="n">
-        <v>9636653</v>
+        <v>9650335</v>
       </c>
       <c r="E806" t="inlineStr">
         <is>
@@ -39310,10 +39310,10 @@
         </is>
       </c>
       <c r="C812" t="n">
-        <v>2740</v>
+        <v>2743</v>
       </c>
       <c r="D812" t="n">
-        <v>3997740</v>
+        <v>4001127</v>
       </c>
       <c r="E812" t="inlineStr">
         <is>
@@ -39358,10 +39358,10 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D813" t="n">
-        <v>1681970</v>
+        <v>1683470</v>
       </c>
       <c r="E813" t="inlineStr">
         <is>
@@ -39454,10 +39454,10 @@
         </is>
       </c>
       <c r="C815" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D815" t="n">
-        <v>350537</v>
+        <v>351747</v>
       </c>
       <c r="E815" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>60746</v>
+        <v>60818</v>
       </c>
       <c r="D816" t="n">
-        <v>75904747</v>
+        <v>75996494</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39742,10 +39742,10 @@
         </is>
       </c>
       <c r="C821" t="n">
-        <v>21579</v>
+        <v>21595</v>
       </c>
       <c r="D821" t="n">
-        <v>31569519</v>
+        <v>31591468</v>
       </c>
       <c r="E821" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>12965</v>
+        <v>12982</v>
       </c>
       <c r="D824" t="n">
-        <v>18714720</v>
+        <v>18738860</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -40126,10 +40126,10 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>1411</v>
+        <v>1416</v>
       </c>
       <c r="D829" t="n">
-        <v>1968600</v>
+        <v>1976100</v>
       </c>
       <c r="E829" t="inlineStr">
         <is>
@@ -40174,10 +40174,10 @@
         </is>
       </c>
       <c r="C830" t="n">
-        <v>11475</v>
+        <v>11487</v>
       </c>
       <c r="D830" t="n">
-        <v>14312012</v>
+        <v>14327719</v>
       </c>
       <c r="E830" t="inlineStr">
         <is>
@@ -40366,10 +40366,10 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>4054</v>
+        <v>4058</v>
       </c>
       <c r="D834" t="n">
-        <v>5890649</v>
+        <v>5895731</v>
       </c>
       <c r="E834" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D836" t="n">
-        <v>1828602</v>
+        <v>1830102</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40702,10 +40702,10 @@
         </is>
       </c>
       <c r="C841" t="n">
-        <v>59742</v>
+        <v>59794</v>
       </c>
       <c r="D841" t="n">
-        <v>73859950</v>
+        <v>73915991</v>
       </c>
       <c r="E841" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>22655</v>
+        <v>22672</v>
       </c>
       <c r="D847" t="n">
-        <v>33240262</v>
+        <v>33265762</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>14637</v>
+        <v>14643</v>
       </c>
       <c r="D849" t="n">
-        <v>21196137</v>
+        <v>21203370</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41230,10 +41230,10 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>1328</v>
+        <v>1339</v>
       </c>
       <c r="D852" t="n">
-        <v>1846277</v>
+        <v>1862309</v>
       </c>
       <c r="E852" t="inlineStr">
         <is>
@@ -41326,10 +41326,10 @@
         </is>
       </c>
       <c r="C854" t="n">
-        <v>7909</v>
+        <v>7919</v>
       </c>
       <c r="D854" t="n">
-        <v>9686564</v>
+        <v>9696703</v>
       </c>
       <c r="E854" t="inlineStr">
         <is>
@@ -41422,10 +41422,10 @@
         </is>
       </c>
       <c r="C856" t="n">
-        <v>2607</v>
+        <v>2608</v>
       </c>
       <c r="D856" t="n">
-        <v>3797242</v>
+        <v>3798742</v>
       </c>
       <c r="E856" t="inlineStr">
         <is>
@@ -41470,10 +41470,10 @@
         </is>
       </c>
       <c r="C857" t="n">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D857" t="n">
-        <v>1578071</v>
+        <v>1579571</v>
       </c>
       <c r="E857" t="inlineStr">
         <is>
@@ -41566,10 +41566,10 @@
         </is>
       </c>
       <c r="C859" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D859" t="n">
-        <v>258962</v>
+        <v>260462</v>
       </c>
       <c r="E859" t="inlineStr">
         <is>
@@ -41758,10 +41758,10 @@
         </is>
       </c>
       <c r="C863" t="n">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D863" t="n">
-        <v>1717582</v>
+        <v>1719082</v>
       </c>
       <c r="E863" t="inlineStr">
         <is>
@@ -41998,10 +41998,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>22698</v>
+        <v>22716</v>
       </c>
       <c r="D868" t="n">
-        <v>28439143</v>
+        <v>28458953</v>
       </c>
       <c r="E868" t="inlineStr">
         <is>
@@ -42190,10 +42190,10 @@
         </is>
       </c>
       <c r="C872" t="n">
-        <v>7841</v>
+        <v>7844</v>
       </c>
       <c r="D872" t="n">
-        <v>11448009</v>
+        <v>11452509</v>
       </c>
       <c r="E872" t="inlineStr">
         <is>
@@ -42286,10 +42286,10 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>4720</v>
+        <v>4725</v>
       </c>
       <c r="D874" t="n">
-        <v>6825845</v>
+        <v>6832616</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
@@ -42526,10 +42526,10 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>14816</v>
+        <v>14827</v>
       </c>
       <c r="D879" t="n">
-        <v>17858525</v>
+        <v>17871767</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
@@ -42718,10 +42718,10 @@
         </is>
       </c>
       <c r="C883" t="n">
-        <v>5318</v>
+        <v>5322</v>
       </c>
       <c r="D883" t="n">
-        <v>7757306</v>
+        <v>7762126</v>
       </c>
       <c r="E883" t="inlineStr">
         <is>
@@ -42814,10 +42814,10 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>2424</v>
+        <v>2427</v>
       </c>
       <c r="D885" t="n">
-        <v>3485133</v>
+        <v>3489633</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
@@ -42958,10 +42958,10 @@
         </is>
       </c>
       <c r="C888" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D888" t="n">
-        <v>432036</v>
+        <v>433536</v>
       </c>
       <c r="E888" t="inlineStr">
         <is>
@@ -43006,10 +43006,10 @@
         </is>
       </c>
       <c r="C889" t="n">
-        <v>10020</v>
+        <v>10024</v>
       </c>
       <c r="D889" t="n">
-        <v>12318577</v>
+        <v>12323810</v>
       </c>
       <c r="E889" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>45848</v>
+        <v>45886</v>
       </c>
       <c r="D896" t="n">
-        <v>57542103</v>
+        <v>57587058</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43582,10 +43582,10 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>21455</v>
+        <v>21466</v>
       </c>
       <c r="D901" t="n">
-        <v>31461189</v>
+        <v>31477689</v>
       </c>
       <c r="E901" t="inlineStr">
         <is>
@@ -43678,10 +43678,10 @@
         </is>
       </c>
       <c r="C903" t="n">
-        <v>6099</v>
+        <v>6102</v>
       </c>
       <c r="D903" t="n">
-        <v>8786451</v>
+        <v>8790951</v>
       </c>
       <c r="E903" t="inlineStr">
         <is>
@@ -43822,10 +43822,10 @@
         </is>
       </c>
       <c r="C906" t="n">
-        <v>978</v>
+        <v>983</v>
       </c>
       <c r="D906" t="n">
-        <v>1377188</v>
+        <v>1384194</v>
       </c>
       <c r="E906" t="inlineStr">
         <is>
@@ -43870,10 +43870,10 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>21580</v>
+        <v>21594</v>
       </c>
       <c r="D907" t="n">
-        <v>26834975</v>
+        <v>26851578</v>
       </c>
       <c r="E907" t="inlineStr">
         <is>
@@ -44014,10 +44014,10 @@
         </is>
       </c>
       <c r="C910" t="n">
-        <v>9898</v>
+        <v>9905</v>
       </c>
       <c r="D910" t="n">
-        <v>14503804</v>
+        <v>14514304</v>
       </c>
       <c r="E910" t="inlineStr">
         <is>
@@ -44158,10 +44158,10 @@
         </is>
       </c>
       <c r="C913" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D913" t="n">
-        <v>4352</v>
+        <v>5331</v>
       </c>
       <c r="E913" t="inlineStr">
         <is>
@@ -44254,10 +44254,10 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D915" t="n">
-        <v>928685</v>
+        <v>930185</v>
       </c>
       <c r="E915" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>7200</v>
+        <v>7207</v>
       </c>
       <c r="D916" t="n">
-        <v>9035848</v>
+        <v>9046348</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44542,10 +44542,10 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>3058</v>
+        <v>3059</v>
       </c>
       <c r="D921" t="n">
-        <v>4502126</v>
+        <v>4503626</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
@@ -44734,10 +44734,10 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>13294</v>
+        <v>13305</v>
       </c>
       <c r="D925" t="n">
-        <v>16532244</v>
+        <v>16542875</v>
       </c>
       <c r="E925" t="inlineStr">
         <is>
@@ -44926,10 +44926,10 @@
         </is>
       </c>
       <c r="C929" t="n">
-        <v>5334</v>
+        <v>5336</v>
       </c>
       <c r="D929" t="n">
-        <v>7789859</v>
+        <v>7792859</v>
       </c>
       <c r="E929" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="D931" t="n">
-        <v>2043991</v>
+        <v>2046991</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45262,10 +45262,10 @@
         </is>
       </c>
       <c r="C936" t="n">
-        <v>19717</v>
+        <v>19732</v>
       </c>
       <c r="D936" t="n">
-        <v>24608716</v>
+        <v>24623961</v>
       </c>
       <c r="E936" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>10209</v>
+        <v>10212</v>
       </c>
       <c r="D940" t="n">
-        <v>14922785</v>
+        <v>14926659</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45550,10 +45550,10 @@
         </is>
       </c>
       <c r="C942" t="n">
-        <v>2121</v>
+        <v>2122</v>
       </c>
       <c r="D942" t="n">
-        <v>3059252</v>
+        <v>3060752</v>
       </c>
       <c r="E942" t="inlineStr">
         <is>
@@ -45646,10 +45646,10 @@
         </is>
       </c>
       <c r="C944" t="n">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D944" t="n">
-        <v>663794</v>
+        <v>666794</v>
       </c>
       <c r="E944" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>8821</v>
+        <v>8831</v>
       </c>
       <c r="D945" t="n">
-        <v>10993610</v>
+        <v>11003760</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>3255</v>
+        <v>3257</v>
       </c>
       <c r="D950" t="n">
-        <v>4749806</v>
+        <v>4752806</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -45982,10 +45982,10 @@
         </is>
       </c>
       <c r="C951" t="n">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="D951" t="n">
-        <v>2208795</v>
+        <v>2213295</v>
       </c>
       <c r="E951" t="inlineStr">
         <is>
@@ -46078,10 +46078,10 @@
         </is>
       </c>
       <c r="C953" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D953" t="n">
-        <v>226575</v>
+        <v>228075</v>
       </c>
       <c r="E953" t="inlineStr">
         <is>
@@ -46126,10 +46126,10 @@
         </is>
       </c>
       <c r="C954" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D954" t="n">
-        <v>315573</v>
+        <v>317073</v>
       </c>
       <c r="E954" t="inlineStr">
         <is>
@@ -46174,10 +46174,10 @@
         </is>
       </c>
       <c r="C955" t="n">
-        <v>69317</v>
+        <v>69410</v>
       </c>
       <c r="D955" t="n">
-        <v>89053009</v>
+        <v>89166146</v>
       </c>
       <c r="E955" t="inlineStr">
         <is>
@@ -46510,10 +46510,10 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>26125</v>
+        <v>26153</v>
       </c>
       <c r="D962" t="n">
-        <v>38290377</v>
+        <v>38330642</v>
       </c>
       <c r="E962" t="inlineStr">
         <is>
@@ -46606,10 +46606,10 @@
         </is>
       </c>
       <c r="C964" t="n">
-        <v>18269</v>
+        <v>18294</v>
       </c>
       <c r="D964" t="n">
-        <v>26490993</v>
+        <v>26527861</v>
       </c>
       <c r="E964" t="inlineStr">
         <is>
@@ -46750,10 +46750,10 @@
         </is>
       </c>
       <c r="C967" t="n">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="D967" t="n">
-        <v>1308769</v>
+        <v>1313269</v>
       </c>
       <c r="E967" t="inlineStr">
         <is>
@@ -46798,10 +46798,10 @@
         </is>
       </c>
       <c r="C968" t="n">
-        <v>86155</v>
+        <v>86277</v>
       </c>
       <c r="D968" t="n">
-        <v>108137767</v>
+        <v>108285089</v>
       </c>
       <c r="E968" t="inlineStr">
         <is>
@@ -47134,10 +47134,10 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>34451</v>
+        <v>34477</v>
       </c>
       <c r="D975" t="n">
-        <v>50525437</v>
+        <v>50564389</v>
       </c>
       <c r="E975" t="inlineStr">
         <is>
@@ -47278,10 +47278,10 @@
         </is>
       </c>
       <c r="C978" t="n">
-        <v>25876</v>
+        <v>25912</v>
       </c>
       <c r="D978" t="n">
-        <v>37542287</v>
+        <v>37594427</v>
       </c>
       <c r="E978" t="inlineStr">
         <is>
@@ -47422,10 +47422,10 @@
         </is>
       </c>
       <c r="C981" t="n">
-        <v>2092</v>
+        <v>2102</v>
       </c>
       <c r="D981" t="n">
-        <v>2947941</v>
+        <v>2961420</v>
       </c>
       <c r="E981" t="inlineStr">
         <is>
@@ -47470,10 +47470,10 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>10984</v>
+        <v>10998</v>
       </c>
       <c r="D982" t="n">
-        <v>14317000</v>
+        <v>14335273</v>
       </c>
       <c r="E982" t="inlineStr">
         <is>
@@ -47662,10 +47662,10 @@
         </is>
       </c>
       <c r="C986" t="n">
-        <v>3533</v>
+        <v>3535</v>
       </c>
       <c r="D986" t="n">
-        <v>5160511</v>
+        <v>5163511</v>
       </c>
       <c r="E986" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="D987" t="n">
-        <v>1649740</v>
+        <v>1651240</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47854,10 +47854,10 @@
         </is>
       </c>
       <c r="C990" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D990" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E990" t="inlineStr">
         <is>
@@ -47902,10 +47902,10 @@
         </is>
       </c>
       <c r="C991" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D991" t="n">
-        <v>255033</v>
+        <v>256533</v>
       </c>
       <c r="E991" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>57052</v>
+        <v>57106</v>
       </c>
       <c r="D992" t="n">
-        <v>71367825</v>
+        <v>71430839</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -47998,10 +47998,10 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D993" t="n">
-        <v>42835</v>
+        <v>43583</v>
       </c>
       <c r="E993" t="inlineStr">
         <is>
@@ -48190,10 +48190,10 @@
         </is>
       </c>
       <c r="C997" t="n">
-        <v>18717</v>
+        <v>18728</v>
       </c>
       <c r="D997" t="n">
-        <v>27412231</v>
+        <v>27428731</v>
       </c>
       <c r="E997" t="inlineStr">
         <is>
@@ -48286,10 +48286,10 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>12874</v>
+        <v>12892</v>
       </c>
       <c r="D999" t="n">
-        <v>18613854</v>
+        <v>18640854</v>
       </c>
       <c r="E999" t="inlineStr">
         <is>
@@ -48430,10 +48430,10 @@
         </is>
       </c>
       <c r="C1002" t="n">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="D1002" t="n">
-        <v>1085308</v>
+        <v>1090708</v>
       </c>
       <c r="E1002" t="inlineStr">
         <is>
@@ -48478,10 +48478,10 @@
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>28882</v>
+        <v>28927</v>
       </c>
       <c r="D1003" t="n">
-        <v>35925087</v>
+        <v>35975907</v>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
@@ -48718,10 +48718,10 @@
         </is>
       </c>
       <c r="C1008" t="n">
-        <v>10699</v>
+        <v>10710</v>
       </c>
       <c r="D1008" t="n">
-        <v>15670508</v>
+        <v>15687008</v>
       </c>
       <c r="E1008" t="inlineStr">
         <is>
@@ -48814,10 +48814,10 @@
         </is>
       </c>
       <c r="C1010" t="n">
-        <v>6373</v>
+        <v>6378</v>
       </c>
       <c r="D1010" t="n">
-        <v>9239042</v>
+        <v>9246004</v>
       </c>
       <c r="E1010" t="inlineStr">
         <is>
@@ -48862,10 +48862,10 @@
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D1011" t="n">
-        <v>757953</v>
+        <v>759453</v>
       </c>
       <c r="E1011" t="inlineStr">
         <is>
@@ -48910,10 +48910,10 @@
         </is>
       </c>
       <c r="C1012" t="n">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="D1012" t="n">
-        <v>777513</v>
+        <v>787680</v>
       </c>
       <c r="E1012" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-06 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16991</v>
+        <v>17013</v>
       </c>
       <c r="D2" t="n">
-        <v>21329954</v>
+        <v>21360014</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6387</v>
+        <v>6392</v>
       </c>
       <c r="D6" t="n">
-        <v>9342599</v>
+        <v>9350099</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3423</v>
+        <v>3425</v>
       </c>
       <c r="D8" t="n">
-        <v>4953260</v>
+        <v>4955704</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D11" t="n">
-        <v>576406</v>
+        <v>577906</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11333</v>
+        <v>11349</v>
       </c>
       <c r="D12" t="n">
-        <v>14287327</v>
+        <v>14306079</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3308</v>
+        <v>3310</v>
       </c>
       <c r="D16" t="n">
-        <v>4816927</v>
+        <v>4819927</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1513</v>
+        <v>1517</v>
       </c>
       <c r="D18" t="n">
-        <v>2179220</v>
+        <v>2184702</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D21" t="n">
-        <v>319591</v>
+        <v>322339</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>14753</v>
+        <v>14776</v>
       </c>
       <c r="D22" t="n">
-        <v>18050552</v>
+        <v>18077688</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1582,10 +1582,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5068</v>
+        <v>5070</v>
       </c>
       <c r="D26" t="n">
-        <v>7408513</v>
+        <v>7411513</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1787</v>
+        <v>1789</v>
       </c>
       <c r="D28" t="n">
-        <v>2553434</v>
+        <v>2556434</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D31" t="n">
-        <v>515420</v>
+        <v>518443</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6785</v>
+        <v>6792</v>
       </c>
       <c r="D32" t="n">
-        <v>9010214</v>
+        <v>9020714</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="D35" t="n">
-        <v>2386110</v>
+        <v>2387610</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D37" t="n">
-        <v>831311</v>
+        <v>832811</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D40" t="n">
-        <v>192391</v>
+        <v>195391</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>22647</v>
+        <v>22674</v>
       </c>
       <c r="D41" t="n">
-        <v>27848685</v>
+        <v>27882704</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7976</v>
+        <v>7978</v>
       </c>
       <c r="D47" t="n">
-        <v>11715989</v>
+        <v>11718989</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3970</v>
+        <v>3975</v>
       </c>
       <c r="D49" t="n">
-        <v>5743605</v>
+        <v>5750834</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D52" t="n">
-        <v>932961</v>
+        <v>934461</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8384</v>
+        <v>8393</v>
       </c>
       <c r="D53" t="n">
-        <v>10678642</v>
+        <v>10689696</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2844</v>
+        <v>2846</v>
       </c>
       <c r="D57" t="n">
-        <v>4136761</v>
+        <v>4139761</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="D59" t="n">
-        <v>1489861</v>
+        <v>1495861</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>37642</v>
+        <v>37704</v>
       </c>
       <c r="D62" t="n">
-        <v>48448419</v>
+        <v>48520263</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>13572</v>
+        <v>13581</v>
       </c>
       <c r="D67" t="n">
-        <v>19900139</v>
+        <v>19910575</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5363</v>
+        <v>5366</v>
       </c>
       <c r="D69" t="n">
-        <v>7751755</v>
+        <v>7756236</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>47926</v>
+        <v>47981</v>
       </c>
       <c r="D75" t="n">
-        <v>61202646</v>
+        <v>61276262</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18618</v>
+        <v>18632</v>
       </c>
       <c r="D79" t="n">
-        <v>27273931</v>
+        <v>27293555</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9714</v>
+        <v>9730</v>
       </c>
       <c r="D81" t="n">
-        <v>14022894</v>
+        <v>14046317</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="D85" t="n">
-        <v>1242252</v>
+        <v>1249752</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>25716</v>
+        <v>25748</v>
       </c>
       <c r="D86" t="n">
-        <v>32397740</v>
+        <v>32433170</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8900</v>
+        <v>8909</v>
       </c>
       <c r="D90" t="n">
-        <v>13063963</v>
+        <v>13076513</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D91" t="n">
-        <v>17685</v>
+        <v>19185</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>5080</v>
+        <v>5081</v>
       </c>
       <c r="D92" t="n">
-        <v>7341330</v>
+        <v>7342830</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>22744</v>
+        <v>22772</v>
       </c>
       <c r="D95" t="n">
-        <v>28501159</v>
+        <v>28534656</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9392</v>
+        <v>9402</v>
       </c>
       <c r="D99" t="n">
-        <v>13748621</v>
+        <v>13763281</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5182,10 +5182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3438</v>
+        <v>3445</v>
       </c>
       <c r="D101" t="n">
-        <v>4923881</v>
+        <v>4934131</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D105" t="n">
-        <v>672535</v>
+        <v>674035</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>86237</v>
+        <v>86466</v>
       </c>
       <c r="D106" t="n">
-        <v>110486984</v>
+        <v>110781804</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>31529</v>
+        <v>31563</v>
       </c>
       <c r="D113" t="n">
-        <v>46265366</v>
+        <v>46314270</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>21918</v>
+        <v>21951</v>
       </c>
       <c r="D115" t="n">
-        <v>31627551</v>
+        <v>31674372</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -5998,10 +5998,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="D118" t="n">
-        <v>989267</v>
+        <v>990767</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2092</v>
+        <v>2108</v>
       </c>
       <c r="D122" t="n">
-        <v>2939727</v>
+        <v>2960943</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>28589</v>
+        <v>28628</v>
       </c>
       <c r="D123" t="n">
-        <v>37695293</v>
+        <v>37745020</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6430,10 +6430,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>10147</v>
+        <v>10150</v>
       </c>
       <c r="D127" t="n">
-        <v>14879324</v>
+        <v>14882374</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D128" t="n">
-        <v>19290</v>
+        <v>20790</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6526,10 +6526,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3405</v>
+        <v>3411</v>
       </c>
       <c r="D129" t="n">
-        <v>4954397</v>
+        <v>4963213</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>16331</v>
+        <v>16352</v>
       </c>
       <c r="D133" t="n">
-        <v>20267368</v>
+        <v>20288043</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7957</v>
+        <v>7964</v>
       </c>
       <c r="D137" t="n">
-        <v>11638781</v>
+        <v>11649122</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7006,10 +7006,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2304</v>
+        <v>2312</v>
       </c>
       <c r="D139" t="n">
-        <v>3289559</v>
+        <v>3301559</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D143" t="n">
-        <v>612448</v>
+        <v>618448</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>14041</v>
+        <v>14057</v>
       </c>
       <c r="D144" t="n">
-        <v>17514815</v>
+        <v>17535081</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>6386</v>
+        <v>6389</v>
       </c>
       <c r="D148" t="n">
-        <v>9351268</v>
+        <v>9354865</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>2054</v>
+        <v>2059</v>
       </c>
       <c r="D150" t="n">
-        <v>2966985</v>
+        <v>2974135</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>6190</v>
+        <v>6194</v>
       </c>
       <c r="D154" t="n">
-        <v>7576728</v>
+        <v>7580169</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>2089</v>
+        <v>2092</v>
       </c>
       <c r="D157" t="n">
-        <v>3063497</v>
+        <v>3067997</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="D158" t="n">
-        <v>1011827</v>
+        <v>1014827</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7694</v>
+        <v>7706</v>
       </c>
       <c r="D162" t="n">
-        <v>9516645</v>
+        <v>9528792</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="D165" t="n">
-        <v>4305568</v>
+        <v>4308568</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1438</v>
+        <v>1440</v>
       </c>
       <c r="D166" t="n">
-        <v>2066211</v>
+        <v>2069161</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D169" t="n">
-        <v>218365</v>
+        <v>219865</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8494,10 +8494,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>5766</v>
+        <v>5775</v>
       </c>
       <c r="D170" t="n">
-        <v>7238048</v>
+        <v>7247844</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -8734,10 +8734,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>2064</v>
+        <v>2067</v>
       </c>
       <c r="D175" t="n">
-        <v>3010685</v>
+        <v>3014125</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -8830,10 +8830,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D177" t="n">
-        <v>1025972</v>
+        <v>1027472</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -8926,10 +8926,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D179" t="n">
-        <v>156068</v>
+        <v>157568</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -8974,10 +8974,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>16562</v>
+        <v>16586</v>
       </c>
       <c r="D180" t="n">
-        <v>20762484</v>
+        <v>20793859</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -9214,10 +9214,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>6538</v>
+        <v>6541</v>
       </c>
       <c r="D185" t="n">
-        <v>9551352</v>
+        <v>9555852</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>2304</v>
+        <v>2310</v>
       </c>
       <c r="D186" t="n">
-        <v>3308982</v>
+        <v>3317982</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D189" t="n">
-        <v>704900</v>
+        <v>706400</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>3179</v>
+        <v>3187</v>
       </c>
       <c r="D190" t="n">
-        <v>3988898</v>
+        <v>3994866</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9550,10 +9550,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>1515</v>
+        <v>1517</v>
       </c>
       <c r="D192" t="n">
-        <v>2218242</v>
+        <v>2221242</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -9646,10 +9646,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D194" t="n">
-        <v>833048</v>
+        <v>834081</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>9538</v>
+        <v>9554</v>
       </c>
       <c r="D198" t="n">
-        <v>11904479</v>
+        <v>11923960</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -10030,10 +10030,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>3515</v>
+        <v>3519</v>
       </c>
       <c r="D202" t="n">
-        <v>5161788</v>
+        <v>5166788</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="D203" t="n">
-        <v>2413522</v>
+        <v>2418022</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>17759</v>
+        <v>17773</v>
       </c>
       <c r="D207" t="n">
-        <v>22142938</v>
+        <v>22160849</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>7838</v>
+        <v>7841</v>
       </c>
       <c r="D211" t="n">
-        <v>11509202</v>
+        <v>11513702</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>1279</v>
+        <v>1284</v>
       </c>
       <c r="D212" t="n">
-        <v>1832296</v>
+        <v>1838595</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>26840</v>
+        <v>26883</v>
       </c>
       <c r="D215" t="n">
-        <v>33784997</v>
+        <v>33830121</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>10689</v>
+        <v>10694</v>
       </c>
       <c r="D219" t="n">
-        <v>15609308</v>
+        <v>15616808</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2718</v>
+        <v>2724</v>
       </c>
       <c r="D221" t="n">
-        <v>3917746</v>
+        <v>3925975</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="D224" t="n">
-        <v>928155</v>
+        <v>931155</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11134,10 +11134,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>29570</v>
+        <v>29620</v>
       </c>
       <c r="D225" t="n">
-        <v>37255927</v>
+        <v>37311990</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>15156</v>
+        <v>15170</v>
       </c>
       <c r="D230" t="n">
-        <v>22239359</v>
+        <v>22257730</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>2777</v>
+        <v>2781</v>
       </c>
       <c r="D232" t="n">
-        <v>3984100</v>
+        <v>3990100</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="D235" t="n">
-        <v>1141499</v>
+        <v>1144499</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11662,10 +11662,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>25134</v>
+        <v>25158</v>
       </c>
       <c r="D236" t="n">
-        <v>31649809</v>
+        <v>31680256</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>11409</v>
+        <v>11413</v>
       </c>
       <c r="D242" t="n">
-        <v>16717664</v>
+        <v>16722903</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12046,10 +12046,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2614</v>
+        <v>2617</v>
       </c>
       <c r="D244" t="n">
-        <v>3729587</v>
+        <v>3732453</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -12238,10 +12238,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>8111</v>
+        <v>8125</v>
       </c>
       <c r="D248" t="n">
-        <v>10141634</v>
+        <v>10159353</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12430,10 +12430,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>2774</v>
+        <v>2777</v>
       </c>
       <c r="D252" t="n">
-        <v>4070807</v>
+        <v>4075307</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -12718,10 +12718,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>10189</v>
+        <v>10202</v>
       </c>
       <c r="D258" t="n">
-        <v>13008470</v>
+        <v>13023565</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>4308</v>
+        <v>4314</v>
       </c>
       <c r="D262" t="n">
-        <v>6324981</v>
+        <v>6333981</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>2276</v>
+        <v>2278</v>
       </c>
       <c r="D264" t="n">
-        <v>3294103</v>
+        <v>3297103</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>5749</v>
+        <v>5758</v>
       </c>
       <c r="D267" t="n">
-        <v>7110773</v>
+        <v>7122321</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="D270" t="n">
-        <v>3021938</v>
+        <v>3023438</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13390,10 +13390,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D272" t="n">
-        <v>1080500</v>
+        <v>1083500</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -13534,10 +13534,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D275" t="n">
-        <v>261758</v>
+        <v>262770</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13582,10 +13582,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>19760</v>
+        <v>19786</v>
       </c>
       <c r="D276" t="n">
-        <v>24928459</v>
+        <v>24960320</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>8180</v>
+        <v>8191</v>
       </c>
       <c r="D280" t="n">
-        <v>11992429</v>
+        <v>12005564</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13870,10 +13870,10 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>2586</v>
+        <v>2588</v>
       </c>
       <c r="D282" t="n">
-        <v>3714848</v>
+        <v>3717848</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D283" t="n">
-        <v>715598</v>
+        <v>718598</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D285" t="n">
-        <v>727636</v>
+        <v>729136</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14110,10 +14110,10 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>17184</v>
+        <v>17209</v>
       </c>
       <c r="D287" t="n">
-        <v>21271168</v>
+        <v>21303668</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>7391</v>
+        <v>7404</v>
       </c>
       <c r="D292" t="n">
-        <v>10843413</v>
+        <v>10862815</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>3471</v>
+        <v>3472</v>
       </c>
       <c r="D293" t="n">
-        <v>5027719</v>
+        <v>5029219</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14590,10 +14590,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>9663</v>
+        <v>9678</v>
       </c>
       <c r="D297" t="n">
-        <v>12125905</v>
+        <v>12140255</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -14782,10 +14782,10 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>3996</v>
+        <v>4002</v>
       </c>
       <c r="D301" t="n">
-        <v>5848552</v>
+        <v>5857552</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D302" t="n">
-        <v>1889733</v>
+        <v>1889859</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -15022,10 +15022,10 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D306" t="n">
-        <v>313439</v>
+        <v>314939</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>9478</v>
+        <v>9485</v>
       </c>
       <c r="D307" t="n">
-        <v>12384239</v>
+        <v>12393588</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3838</v>
+        <v>3843</v>
       </c>
       <c r="D311" t="n">
-        <v>5613285</v>
+        <v>5620785</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>2439</v>
+        <v>2442</v>
       </c>
       <c r="D312" t="n">
-        <v>3550559</v>
+        <v>3553859</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>11468</v>
+        <v>11485</v>
       </c>
       <c r="D315" t="n">
-        <v>15044509</v>
+        <v>15064795</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>3903</v>
+        <v>3906</v>
       </c>
       <c r="D319" t="n">
-        <v>5724015</v>
+        <v>5728363</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>2797</v>
+        <v>2802</v>
       </c>
       <c r="D321" t="n">
-        <v>4053935</v>
+        <v>4061435</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>7044</v>
+        <v>7055</v>
       </c>
       <c r="D324" t="n">
-        <v>8704166</v>
+        <v>8717939</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="D329" t="n">
-        <v>3448915</v>
+        <v>3450415</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="D331" t="n">
-        <v>1181735</v>
+        <v>1184735</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16366,10 +16366,10 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>7782</v>
+        <v>7801</v>
       </c>
       <c r="D334" t="n">
-        <v>9734262</v>
+        <v>9756278</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -16606,10 +16606,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>3223</v>
+        <v>3226</v>
       </c>
       <c r="D339" t="n">
-        <v>4706365</v>
+        <v>4710865</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D340" t="n">
-        <v>1911567</v>
+        <v>1913067</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>33251</v>
+        <v>33290</v>
       </c>
       <c r="D343" t="n">
-        <v>41789794</v>
+        <v>41838018</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>17033</v>
+        <v>17043</v>
       </c>
       <c r="D349" t="n">
-        <v>24904841</v>
+        <v>24919093</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>8351</v>
+        <v>8365</v>
       </c>
       <c r="D352" t="n">
-        <v>12031254</v>
+        <v>12052254</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>860</v>
+        <v>868</v>
       </c>
       <c r="D354" t="n">
-        <v>1216557</v>
+        <v>1227460</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>4052</v>
+        <v>4055</v>
       </c>
       <c r="D355" t="n">
-        <v>5043787</v>
+        <v>5046681</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17518,10 +17518,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1530</v>
+        <v>1532</v>
       </c>
       <c r="D358" t="n">
-        <v>2256591</v>
+        <v>2259591</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D362" t="n">
-        <v>124595</v>
+        <v>127155</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>20133</v>
+        <v>20160</v>
       </c>
       <c r="D363" t="n">
-        <v>25055916</v>
+        <v>25090413</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>10204</v>
+        <v>10210</v>
       </c>
       <c r="D367" t="n">
-        <v>14960864</v>
+        <v>14969156</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>4911</v>
+        <v>4920</v>
       </c>
       <c r="D369" t="n">
-        <v>7107651</v>
+        <v>7121151</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>14450</v>
+        <v>14476</v>
       </c>
       <c r="D372" t="n">
-        <v>18042514</v>
+        <v>18075590</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>6629</v>
+        <v>6635</v>
       </c>
       <c r="D376" t="n">
-        <v>9705525</v>
+        <v>9714525</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>2601</v>
+        <v>2603</v>
       </c>
       <c r="D378" t="n">
-        <v>3733417</v>
+        <v>3736417</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D380" t="n">
-        <v>377912</v>
+        <v>379412</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18622,10 +18622,10 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>18659</v>
+        <v>18683</v>
       </c>
       <c r="D381" t="n">
-        <v>23231382</v>
+        <v>23260033</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>7323</v>
+        <v>7328</v>
       </c>
       <c r="D385" t="n">
-        <v>10757699</v>
+        <v>10765199</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="D387" t="n">
-        <v>4271659</v>
+        <v>4274659</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D390" t="n">
-        <v>615008</v>
+        <v>620387</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>4250</v>
+        <v>4258</v>
       </c>
       <c r="D391" t="n">
-        <v>5321524</v>
+        <v>5331676</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>1417</v>
+        <v>1420</v>
       </c>
       <c r="D394" t="n">
-        <v>2066622</v>
+        <v>2071122</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D395" t="n">
-        <v>854658</v>
+        <v>856158</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>23067</v>
+        <v>23094</v>
       </c>
       <c r="D398" t="n">
-        <v>28575608</v>
+        <v>28604902</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>9585</v>
+        <v>9588</v>
       </c>
       <c r="D401" t="n">
-        <v>14109560</v>
+        <v>14114060</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>6416</v>
+        <v>6422</v>
       </c>
       <c r="D403" t="n">
-        <v>9327459</v>
+        <v>9333825</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>11574</v>
+        <v>11584</v>
       </c>
       <c r="D406" t="n">
-        <v>14244660</v>
+        <v>14255226</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>5457</v>
+        <v>5459</v>
       </c>
       <c r="D411" t="n">
-        <v>7977283</v>
+        <v>7980283</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="D413" t="n">
-        <v>2755192</v>
+        <v>2756692</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>34624</v>
+        <v>34744</v>
       </c>
       <c r="D416" t="n">
-        <v>46951793</v>
+        <v>47110522</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>8394</v>
+        <v>8419</v>
       </c>
       <c r="D420" t="n">
-        <v>12339821</v>
+        <v>12376097</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>7779</v>
+        <v>7806</v>
       </c>
       <c r="D422" t="n">
-        <v>11290347</v>
+        <v>11330807</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D424" t="n">
-        <v>786156</v>
+        <v>787656</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D425" t="n">
-        <v>756550</v>
+        <v>758050</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>11642</v>
+        <v>11789</v>
       </c>
       <c r="D426" t="n">
-        <v>18764262</v>
+        <v>19125984</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>2827</v>
+        <v>2857</v>
       </c>
       <c r="D428" t="n">
-        <v>4893970</v>
+        <v>4980170</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>3891</v>
+        <v>3937</v>
       </c>
       <c r="D430" t="n">
-        <v>6764869</v>
+        <v>6892269</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D433" t="n">
-        <v>364530</v>
+        <v>370530</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>11442</v>
+        <v>11453</v>
       </c>
       <c r="D434" t="n">
-        <v>14137365</v>
+        <v>14149475</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>3907</v>
+        <v>3908</v>
       </c>
       <c r="D437" t="n">
-        <v>5734008</v>
+        <v>5735508</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="D439" t="n">
-        <v>2784692</v>
+        <v>2786112</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21550,10 +21550,10 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>65805</v>
+        <v>65899</v>
       </c>
       <c r="D442" t="n">
-        <v>81554079</v>
+        <v>81670996</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>25703</v>
+        <v>25721</v>
       </c>
       <c r="D446" t="n">
-        <v>37661291</v>
+        <v>37685283</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21838,10 +21838,10 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>13686</v>
+        <v>13715</v>
       </c>
       <c r="D448" t="n">
-        <v>19852768</v>
+        <v>19894420</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="D452" t="n">
-        <v>1620863</v>
+        <v>1623863</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>19892</v>
+        <v>19936</v>
       </c>
       <c r="D454" t="n">
-        <v>25181277</v>
+        <v>25240579</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>7935</v>
+        <v>7943</v>
       </c>
       <c r="D458" t="n">
-        <v>11642763</v>
+        <v>11654555</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>5193</v>
+        <v>5202</v>
       </c>
       <c r="D460" t="n">
-        <v>7538167</v>
+        <v>7551667</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22558,10 +22558,10 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>33275</v>
+        <v>33310</v>
       </c>
       <c r="D463" t="n">
-        <v>40659255</v>
+        <v>40696867</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>11727</v>
+        <v>11732</v>
       </c>
       <c r="D467" t="n">
-        <v>17153202</v>
+        <v>17159952</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>5042</v>
+        <v>5050</v>
       </c>
       <c r="D469" t="n">
-        <v>7315491</v>
+        <v>7326229</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -22990,10 +22990,10 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>14914</v>
+        <v>14925</v>
       </c>
       <c r="D472" t="n">
-        <v>18201293</v>
+        <v>18214490</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>4505</v>
+        <v>4508</v>
       </c>
       <c r="D477" t="n">
-        <v>6618285</v>
+        <v>6622163</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>2158</v>
+        <v>2161</v>
       </c>
       <c r="D479" t="n">
-        <v>3109318</v>
+        <v>3113522</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23470,10 +23470,10 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>38965</v>
+        <v>39110</v>
       </c>
       <c r="D482" t="n">
-        <v>50931963</v>
+        <v>51122316</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D485" t="n">
-        <v>150888</v>
+        <v>152388</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23662,10 +23662,10 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>14064</v>
+        <v>14080</v>
       </c>
       <c r="D486" t="n">
-        <v>20685457</v>
+        <v>20708952</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>13022</v>
+        <v>13057</v>
       </c>
       <c r="D488" t="n">
-        <v>19015948</v>
+        <v>19067004</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23854,10 +23854,10 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D490" t="n">
-        <v>463724</v>
+        <v>468718</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -23902,10 +23902,10 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>68902</v>
+        <v>69190</v>
       </c>
       <c r="D491" t="n">
-        <v>91415011</v>
+        <v>91787346</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -24142,10 +24142,10 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>24366</v>
+        <v>24429</v>
       </c>
       <c r="D496" t="n">
-        <v>35759542</v>
+        <v>35853207</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -24238,10 +24238,10 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>24729</v>
+        <v>24829</v>
       </c>
       <c r="D498" t="n">
-        <v>35913546</v>
+        <v>36055339</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="D501" t="n">
-        <v>990786</v>
+        <v>996786</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>163459</v>
+        <v>164052</v>
       </c>
       <c r="D502" t="n">
-        <v>214838578</v>
+        <v>215593135</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D507" t="n">
-        <v>722587</v>
+        <v>724087</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>86164</v>
+        <v>86366</v>
       </c>
       <c r="D509" t="n">
-        <v>126575725</v>
+        <v>126870132</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24910,10 +24910,10 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>64634</v>
+        <v>64820</v>
       </c>
       <c r="D512" t="n">
-        <v>93886798</v>
+        <v>94159596</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="D514" t="n">
-        <v>1567759</v>
+        <v>1569259</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>3098</v>
+        <v>3105</v>
       </c>
       <c r="D516" t="n">
-        <v>4378888</v>
+        <v>4388930</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25246,10 +25246,10 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>44629</v>
+        <v>44802</v>
       </c>
       <c r="D519" t="n">
-        <v>58184794</v>
+        <v>58412715</v>
       </c>
       <c r="E519" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>15844</v>
+        <v>15869</v>
       </c>
       <c r="D524" t="n">
-        <v>23268981</v>
+        <v>23304865</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25582,10 +25582,10 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>13937</v>
+        <v>13972</v>
       </c>
       <c r="D526" t="n">
-        <v>20208509</v>
+        <v>20260137</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D529" t="n">
-        <v>537022</v>
+        <v>543022</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>74091</v>
+        <v>74465</v>
       </c>
       <c r="D531" t="n">
-        <v>100001141</v>
+        <v>100508018</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>24471</v>
+        <v>24533</v>
       </c>
       <c r="D535" t="n">
-        <v>36100581</v>
+        <v>36188317</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>26898</v>
+        <v>27054</v>
       </c>
       <c r="D537" t="n">
-        <v>39364494</v>
+        <v>39589658</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="D541" t="n">
-        <v>1339623</v>
+        <v>1349138</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>60411</v>
+        <v>60710</v>
       </c>
       <c r="D542" t="n">
-        <v>80294633</v>
+        <v>80680864</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26542,10 +26542,10 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D546" t="n">
-        <v>148109</v>
+        <v>149609</v>
       </c>
       <c r="E546" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>18592</v>
+        <v>18615</v>
       </c>
       <c r="D547" t="n">
-        <v>27316240</v>
+        <v>27348180</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26686,10 +26686,10 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>20126</v>
+        <v>20216</v>
       </c>
       <c r="D549" t="n">
-        <v>29275383</v>
+        <v>29407413</v>
       </c>
       <c r="E549" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="D551" t="n">
-        <v>954780</v>
+        <v>959280</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>46102</v>
+        <v>46318</v>
       </c>
       <c r="D552" t="n">
-        <v>61517589</v>
+        <v>61815024</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>14749</v>
+        <v>14784</v>
       </c>
       <c r="D556" t="n">
-        <v>21747424</v>
+        <v>21795716</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27118,10 +27118,10 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>15897</v>
+        <v>15954</v>
       </c>
       <c r="D558" t="n">
-        <v>23092811</v>
+        <v>23173524</v>
       </c>
       <c r="E558" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D560" t="n">
-        <v>448242</v>
+        <v>450012</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>44339</v>
+        <v>44488</v>
       </c>
       <c r="D561" t="n">
-        <v>57619239</v>
+        <v>57821411</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>16779</v>
+        <v>16801</v>
       </c>
       <c r="D565" t="n">
-        <v>24613884</v>
+        <v>24645972</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>14009</v>
+        <v>14044</v>
       </c>
       <c r="D567" t="n">
-        <v>20276287</v>
+        <v>20327517</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D570" t="n">
-        <v>541490</v>
+        <v>542990</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27742,10 +27742,10 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>46189</v>
+        <v>46259</v>
       </c>
       <c r="D571" t="n">
-        <v>61642790</v>
+        <v>61739950</v>
       </c>
       <c r="E571" t="inlineStr">
         <is>
@@ -27934,10 +27934,10 @@
         </is>
       </c>
       <c r="C575" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D575" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E575" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>14434</v>
+        <v>14444</v>
       </c>
       <c r="D577" t="n">
-        <v>21156239</v>
+        <v>21170094</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>3873</v>
+        <v>3880</v>
       </c>
       <c r="D578" t="n">
-        <v>5585482</v>
+        <v>5594931</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28222,10 +28222,10 @@
         </is>
       </c>
       <c r="C581" t="n">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D581" t="n">
-        <v>584216</v>
+        <v>585716</v>
       </c>
       <c r="E581" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D583" t="n">
-        <v>586813</v>
+        <v>588313</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>18205</v>
+        <v>18250</v>
       </c>
       <c r="D584" t="n">
-        <v>24065567</v>
+        <v>24130080</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>7427</v>
+        <v>7452</v>
       </c>
       <c r="D588" t="n">
-        <v>10808593</v>
+        <v>10846728</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>5196</v>
+        <v>5214</v>
       </c>
       <c r="D590" t="n">
-        <v>7479538</v>
+        <v>7505821</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D593" t="n">
-        <v>397164</v>
+        <v>401664</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>21301</v>
+        <v>21587</v>
       </c>
       <c r="D595" t="n">
-        <v>37579924</v>
+        <v>38346680</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>2271</v>
+        <v>2295</v>
       </c>
       <c r="D596" t="n">
-        <v>3998571</v>
+        <v>4067571</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D597" t="n">
-        <v>510089</v>
+        <v>522089</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>22812</v>
+        <v>22836</v>
       </c>
       <c r="D601" t="n">
-        <v>28559938</v>
+        <v>28588130</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29422,10 +29422,10 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>9254</v>
+        <v>9261</v>
       </c>
       <c r="D606" t="n">
-        <v>13553295</v>
+        <v>13563252</v>
       </c>
       <c r="E606" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>3468</v>
+        <v>3481</v>
       </c>
       <c r="D608" t="n">
-        <v>4979857</v>
+        <v>4999083</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29566,10 +29566,10 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D609" t="n">
-        <v>512168</v>
+        <v>513668</v>
       </c>
       <c r="E609" t="inlineStr">
         <is>
@@ -29614,10 +29614,10 @@
         </is>
       </c>
       <c r="C610" t="n">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D610" t="n">
-        <v>717771</v>
+        <v>719271</v>
       </c>
       <c r="E610" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>15244</v>
+        <v>15268</v>
       </c>
       <c r="D612" t="n">
-        <v>19075212</v>
+        <v>19106385</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D614" t="n">
-        <v>8820</v>
+        <v>9889</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>5942</v>
+        <v>5945</v>
       </c>
       <c r="D616" t="n">
-        <v>8723804</v>
+        <v>8727318</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -29998,10 +29998,10 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>2800</v>
+        <v>2803</v>
       </c>
       <c r="D618" t="n">
-        <v>4037703</v>
+        <v>4041403</v>
       </c>
       <c r="E618" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>14223</v>
+        <v>14246</v>
       </c>
       <c r="D621" t="n">
-        <v>17921725</v>
+        <v>17950212</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>5349</v>
+        <v>5351</v>
       </c>
       <c r="D625" t="n">
-        <v>7838548</v>
+        <v>7841548</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D626" t="n">
-        <v>1758087</v>
+        <v>1759587</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30574,10 +30574,10 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>7785</v>
+        <v>7791</v>
       </c>
       <c r="D630" t="n">
-        <v>9995283</v>
+        <v>10000941</v>
       </c>
       <c r="E630" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>2624</v>
+        <v>2625</v>
       </c>
       <c r="D635" t="n">
-        <v>3844970</v>
+        <v>3846470</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -31006,10 +31006,10 @@
         </is>
       </c>
       <c r="C639" t="n">
-        <v>29807</v>
+        <v>29836</v>
       </c>
       <c r="D639" t="n">
-        <v>36684650</v>
+        <v>36719221</v>
       </c>
       <c r="E639" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>11339</v>
+        <v>11350</v>
       </c>
       <c r="D644" t="n">
-        <v>16637141</v>
+        <v>16653641</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D645" t="n">
-        <v>22500</v>
+        <v>25500</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31342,10 +31342,10 @@
         </is>
       </c>
       <c r="C646" t="n">
-        <v>5028</v>
+        <v>5037</v>
       </c>
       <c r="D646" t="n">
-        <v>7294059</v>
+        <v>7307559</v>
       </c>
       <c r="E646" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D649" t="n">
-        <v>857289</v>
+        <v>858789</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>11694</v>
+        <v>11704</v>
       </c>
       <c r="D650" t="n">
-        <v>14129526</v>
+        <v>14139835</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>29101</v>
+        <v>29147</v>
       </c>
       <c r="D660" t="n">
-        <v>36148393</v>
+        <v>36200370</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>10938</v>
+        <v>10943</v>
       </c>
       <c r="D664" t="n">
-        <v>16072095</v>
+        <v>16079595</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>3149</v>
+        <v>3154</v>
       </c>
       <c r="D666" t="n">
-        <v>4539115</v>
+        <v>4545814</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>7685</v>
+        <v>7686</v>
       </c>
       <c r="D670" t="n">
-        <v>9741125</v>
+        <v>9741361</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>3930</v>
+        <v>3935</v>
       </c>
       <c r="D678" t="n">
-        <v>4749306</v>
+        <v>4754703</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D684" t="n">
-        <v>662245</v>
+        <v>663745</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D686" t="n">
-        <v>217342</v>
+        <v>220776</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>9623</v>
+        <v>9635</v>
       </c>
       <c r="D687" t="n">
-        <v>11972902</v>
+        <v>11986340</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33502,10 +33502,10 @@
         </is>
       </c>
       <c r="C691" t="n">
-        <v>3543</v>
+        <v>3546</v>
       </c>
       <c r="D691" t="n">
-        <v>5223710</v>
+        <v>5228210</v>
       </c>
       <c r="E691" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>19844</v>
+        <v>19860</v>
       </c>
       <c r="D696" t="n">
-        <v>24277407</v>
+        <v>24298438</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>5851</v>
+        <v>5854</v>
       </c>
       <c r="D700" t="n">
-        <v>8544751</v>
+        <v>8549251</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>2318</v>
+        <v>2322</v>
       </c>
       <c r="D702" t="n">
-        <v>3334311</v>
+        <v>3340311</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>77521</v>
+        <v>77633</v>
       </c>
       <c r="D707" t="n">
-        <v>97584755</v>
+        <v>97729855</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D709" t="n">
-        <v>40798</v>
+        <v>42298</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>27293</v>
+        <v>27340</v>
       </c>
       <c r="D712" t="n">
-        <v>40060566</v>
+        <v>40126235</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>13714</v>
+        <v>13742</v>
       </c>
       <c r="D715" t="n">
-        <v>19786604</v>
+        <v>19824307</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="D718" t="n">
-        <v>2867467</v>
+        <v>2868967</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>1318</v>
+        <v>1322</v>
       </c>
       <c r="D720" t="n">
-        <v>1840670</v>
+        <v>1845823</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -34942,10 +34942,10 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>11517</v>
+        <v>11528</v>
       </c>
       <c r="D721" t="n">
-        <v>14073870</v>
+        <v>14088313</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>4203</v>
+        <v>4205</v>
       </c>
       <c r="D724" t="n">
-        <v>6148340</v>
+        <v>6151340</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35182,10 +35182,10 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D726" t="n">
-        <v>2226840</v>
+        <v>2228340</v>
       </c>
       <c r="E726" t="inlineStr">
         <is>
@@ -35278,10 +35278,10 @@
         </is>
       </c>
       <c r="C728" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D728" t="n">
-        <v>369460</v>
+        <v>371847</v>
       </c>
       <c r="E728" t="inlineStr">
         <is>
@@ -35326,10 +35326,10 @@
         </is>
       </c>
       <c r="C729" t="n">
-        <v>18180</v>
+        <v>18214</v>
       </c>
       <c r="D729" t="n">
-        <v>22394629</v>
+        <v>22426901</v>
       </c>
       <c r="E729" t="inlineStr">
         <is>
@@ -35518,10 +35518,10 @@
         </is>
       </c>
       <c r="C733" t="n">
-        <v>7015</v>
+        <v>7018</v>
       </c>
       <c r="D733" t="n">
-        <v>10253206</v>
+        <v>10257706</v>
       </c>
       <c r="E733" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>2250</v>
+        <v>2252</v>
       </c>
       <c r="D735" t="n">
-        <v>3226679</v>
+        <v>3229679</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35854,10 +35854,10 @@
         </is>
       </c>
       <c r="C740" t="n">
-        <v>11890</v>
+        <v>11908</v>
       </c>
       <c r="D740" t="n">
-        <v>14665071</v>
+        <v>14687234</v>
       </c>
       <c r="E740" t="inlineStr">
         <is>
@@ -36046,10 +36046,10 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>4327</v>
+        <v>4331</v>
       </c>
       <c r="D744" t="n">
-        <v>6343847</v>
+        <v>6349847</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
@@ -36286,10 +36286,10 @@
         </is>
       </c>
       <c r="C749" t="n">
-        <v>30378</v>
+        <v>30416</v>
       </c>
       <c r="D749" t="n">
-        <v>37751844</v>
+        <v>37796441</v>
       </c>
       <c r="E749" t="inlineStr">
         <is>
@@ -36526,10 +36526,10 @@
         </is>
       </c>
       <c r="C754" t="n">
-        <v>12994</v>
+        <v>13002</v>
       </c>
       <c r="D754" t="n">
-        <v>19014409</v>
+        <v>19025308</v>
       </c>
       <c r="E754" t="inlineStr">
         <is>
@@ -36622,10 +36622,10 @@
         </is>
       </c>
       <c r="C756" t="n">
-        <v>4355</v>
+        <v>4359</v>
       </c>
       <c r="D756" t="n">
-        <v>6222382</v>
+        <v>6228026</v>
       </c>
       <c r="E756" t="inlineStr">
         <is>
@@ -36766,10 +36766,10 @@
         </is>
       </c>
       <c r="C759" t="n">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D759" t="n">
-        <v>1032406</v>
+        <v>1033406</v>
       </c>
       <c r="E759" t="inlineStr">
         <is>
@@ -36862,10 +36862,10 @@
         </is>
       </c>
       <c r="C761" t="n">
-        <v>12727</v>
+        <v>12737</v>
       </c>
       <c r="D761" t="n">
-        <v>15734258</v>
+        <v>15744302</v>
       </c>
       <c r="E761" t="inlineStr">
         <is>
@@ -37006,10 +37006,10 @@
         </is>
       </c>
       <c r="C764" t="n">
-        <v>4767</v>
+        <v>4770</v>
       </c>
       <c r="D764" t="n">
-        <v>6964632</v>
+        <v>6969132</v>
       </c>
       <c r="E764" t="inlineStr">
         <is>
@@ -37054,10 +37054,10 @@
         </is>
       </c>
       <c r="C765" t="n">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D765" t="n">
-        <v>1706948</v>
+        <v>1708448</v>
       </c>
       <c r="E765" t="inlineStr">
         <is>
@@ -37198,10 +37198,10 @@
         </is>
       </c>
       <c r="C768" t="n">
-        <v>6957</v>
+        <v>6970</v>
       </c>
       <c r="D768" t="n">
-        <v>8162473</v>
+        <v>8177057</v>
       </c>
       <c r="E768" t="inlineStr">
         <is>
@@ -37390,10 +37390,10 @@
         </is>
       </c>
       <c r="C772" t="n">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="D772" t="n">
-        <v>2542364</v>
+        <v>2543864</v>
       </c>
       <c r="E772" t="inlineStr">
         <is>
@@ -37438,10 +37438,10 @@
         </is>
       </c>
       <c r="C773" t="n">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="D773" t="n">
-        <v>1502915</v>
+        <v>1504400</v>
       </c>
       <c r="E773" t="inlineStr">
         <is>
@@ -37534,10 +37534,10 @@
         </is>
       </c>
       <c r="C775" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D775" t="n">
-        <v>230487</v>
+        <v>231987</v>
       </c>
       <c r="E775" t="inlineStr">
         <is>
@@ -37582,10 +37582,10 @@
         </is>
       </c>
       <c r="C776" t="n">
-        <v>17292</v>
+        <v>17317</v>
       </c>
       <c r="D776" t="n">
-        <v>20981681</v>
+        <v>21009873</v>
       </c>
       <c r="E776" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>5676</v>
+        <v>5679</v>
       </c>
       <c r="D781" t="n">
-        <v>8319926</v>
+        <v>8324426</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -37918,10 +37918,10 @@
         </is>
       </c>
       <c r="C783" t="n">
-        <v>3521</v>
+        <v>3523</v>
       </c>
       <c r="D783" t="n">
-        <v>5139734</v>
+        <v>5142543</v>
       </c>
       <c r="E783" t="inlineStr">
         <is>
@@ -38110,10 +38110,10 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>11661</v>
+        <v>11672</v>
       </c>
       <c r="D787" t="n">
-        <v>14738962</v>
+        <v>14751774</v>
       </c>
       <c r="E787" t="inlineStr">
         <is>
@@ -38302,10 +38302,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>4037</v>
+        <v>4042</v>
       </c>
       <c r="D791" t="n">
-        <v>5901401</v>
+        <v>5908901</v>
       </c>
       <c r="E791" t="inlineStr">
         <is>
@@ -38398,10 +38398,10 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D793" t="n">
-        <v>1867745</v>
+        <v>1869245</v>
       </c>
       <c r="E793" t="inlineStr">
         <is>
@@ -38590,10 +38590,10 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>33157</v>
+        <v>33199</v>
       </c>
       <c r="D797" t="n">
-        <v>40865134</v>
+        <v>40917493</v>
       </c>
       <c r="E797" t="inlineStr">
         <is>
@@ -38782,10 +38782,10 @@
         </is>
       </c>
       <c r="C801" t="n">
-        <v>13472</v>
+        <v>13484</v>
       </c>
       <c r="D801" t="n">
-        <v>19705207</v>
+        <v>19723207</v>
       </c>
       <c r="E801" t="inlineStr">
         <is>
@@ -38878,10 +38878,10 @@
         </is>
       </c>
       <c r="C803" t="n">
-        <v>6252</v>
+        <v>6254</v>
       </c>
       <c r="D803" t="n">
-        <v>9034307</v>
+        <v>9037307</v>
       </c>
       <c r="E803" t="inlineStr">
         <is>
@@ -39022,10 +39022,10 @@
         </is>
       </c>
       <c r="C806" t="n">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D806" t="n">
-        <v>1001894</v>
+        <v>1003472</v>
       </c>
       <c r="E806" t="inlineStr">
         <is>
@@ -39070,10 +39070,10 @@
         </is>
       </c>
       <c r="C807" t="n">
-        <v>7905</v>
+        <v>7910</v>
       </c>
       <c r="D807" t="n">
-        <v>9759722</v>
+        <v>9766502</v>
       </c>
       <c r="E807" t="inlineStr">
         <is>
@@ -39358,10 +39358,10 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>2770</v>
+        <v>2771</v>
       </c>
       <c r="D813" t="n">
-        <v>4041339</v>
+        <v>4042839</v>
       </c>
       <c r="E813" t="inlineStr">
         <is>
@@ -39502,10 +39502,10 @@
         </is>
       </c>
       <c r="C816" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D816" t="n">
-        <v>369980</v>
+        <v>371380</v>
       </c>
       <c r="E816" t="inlineStr">
         <is>
@@ -39550,10 +39550,10 @@
         </is>
       </c>
       <c r="C817" t="n">
-        <v>61751</v>
+        <v>61855</v>
       </c>
       <c r="D817" t="n">
-        <v>77173457</v>
+        <v>77299261</v>
       </c>
       <c r="E817" t="inlineStr">
         <is>
@@ -39790,10 +39790,10 @@
         </is>
       </c>
       <c r="C822" t="n">
-        <v>21861</v>
+        <v>21880</v>
       </c>
       <c r="D822" t="n">
-        <v>31978684</v>
+        <v>32006619</v>
       </c>
       <c r="E822" t="inlineStr">
         <is>
@@ -39934,10 +39934,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>13247</v>
+        <v>13263</v>
       </c>
       <c r="D825" t="n">
-        <v>19120509</v>
+        <v>19144509</v>
       </c>
       <c r="E825" t="inlineStr">
         <is>
@@ -40174,10 +40174,10 @@
         </is>
       </c>
       <c r="C830" t="n">
-        <v>1456</v>
+        <v>1463</v>
       </c>
       <c r="D830" t="n">
-        <v>2032133</v>
+        <v>2040524</v>
       </c>
       <c r="E830" t="inlineStr">
         <is>
@@ -40222,10 +40222,10 @@
         </is>
       </c>
       <c r="C831" t="n">
-        <v>11659</v>
+        <v>11682</v>
       </c>
       <c r="D831" t="n">
-        <v>14546761</v>
+        <v>14575313</v>
       </c>
       <c r="E831" t="inlineStr">
         <is>
@@ -40366,10 +40366,10 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D834" t="n">
-        <v>53659</v>
+        <v>56659</v>
       </c>
       <c r="E834" t="inlineStr">
         <is>
@@ -40414,10 +40414,10 @@
         </is>
       </c>
       <c r="C835" t="n">
-        <v>4111</v>
+        <v>4116</v>
       </c>
       <c r="D835" t="n">
-        <v>5974691</v>
+        <v>5982191</v>
       </c>
       <c r="E835" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D836" t="n">
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>1301</v>
+        <v>1307</v>
       </c>
       <c r="D837" t="n">
-        <v>1862742</v>
+        <v>1871567</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>60466</v>
+        <v>60563</v>
       </c>
       <c r="D842" t="n">
-        <v>74730800</v>
+        <v>74849524</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -41038,10 +41038,10 @@
         </is>
       </c>
       <c r="C848" t="n">
-        <v>22870</v>
+        <v>22897</v>
       </c>
       <c r="D848" t="n">
-        <v>33560046</v>
+        <v>33600546</v>
       </c>
       <c r="E848" t="inlineStr">
         <is>
@@ -41134,10 +41134,10 @@
         </is>
       </c>
       <c r="C850" t="n">
-        <v>14863</v>
+        <v>14888</v>
       </c>
       <c r="D850" t="n">
-        <v>21519869</v>
+        <v>21557048</v>
       </c>
       <c r="E850" t="inlineStr">
         <is>
@@ -41278,10 +41278,10 @@
         </is>
       </c>
       <c r="C853" t="n">
-        <v>1398</v>
+        <v>1404</v>
       </c>
       <c r="D853" t="n">
-        <v>1947586</v>
+        <v>1955836</v>
       </c>
       <c r="E853" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>8007</v>
+        <v>8016</v>
       </c>
       <c r="D855" t="n">
-        <v>9804252</v>
+        <v>9814075</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41470,10 +41470,10 @@
         </is>
       </c>
       <c r="C857" t="n">
-        <v>2627</v>
+        <v>2629</v>
       </c>
       <c r="D857" t="n">
-        <v>3825977</v>
+        <v>3828977</v>
       </c>
       <c r="E857" t="inlineStr">
         <is>
@@ -41662,10 +41662,10 @@
         </is>
       </c>
       <c r="C861" t="n">
-        <v>3733</v>
+        <v>3737</v>
       </c>
       <c r="D861" t="n">
-        <v>4824429</v>
+        <v>4828694</v>
       </c>
       <c r="E861" t="inlineStr">
         <is>
@@ -42046,10 +42046,10 @@
         </is>
       </c>
       <c r="C869" t="n">
-        <v>22879</v>
+        <v>22903</v>
       </c>
       <c r="D869" t="n">
-        <v>28655324</v>
+        <v>28687200</v>
       </c>
       <c r="E869" t="inlineStr">
         <is>
@@ -42238,10 +42238,10 @@
         </is>
       </c>
       <c r="C873" t="n">
-        <v>7903</v>
+        <v>7909</v>
       </c>
       <c r="D873" t="n">
-        <v>11540279</v>
+        <v>11547727</v>
       </c>
       <c r="E873" t="inlineStr">
         <is>
@@ -42334,10 +42334,10 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>4792</v>
+        <v>4795</v>
       </c>
       <c r="D875" t="n">
-        <v>6926527</v>
+        <v>6931027</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
@@ -42478,10 +42478,10 @@
         </is>
       </c>
       <c r="C878" t="n">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="D878" t="n">
-        <v>648893</v>
+        <v>655893</v>
       </c>
       <c r="E878" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>14966</v>
+        <v>14984</v>
       </c>
       <c r="D880" t="n">
-        <v>18040449</v>
+        <v>18057580</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>5370</v>
+        <v>5378</v>
       </c>
       <c r="D884" t="n">
-        <v>7831780</v>
+        <v>7843780</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -43054,10 +43054,10 @@
         </is>
       </c>
       <c r="C890" t="n">
-        <v>10133</v>
+        <v>10146</v>
       </c>
       <c r="D890" t="n">
-        <v>12454991</v>
+        <v>12470470</v>
       </c>
       <c r="E890" t="inlineStr">
         <is>
@@ -43102,10 +43102,10 @@
         </is>
       </c>
       <c r="C891" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D891" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E891" t="inlineStr">
         <is>
@@ -43198,10 +43198,10 @@
         </is>
       </c>
       <c r="C893" t="n">
-        <v>3417</v>
+        <v>3419</v>
       </c>
       <c r="D893" t="n">
-        <v>5005004</v>
+        <v>5006847</v>
       </c>
       <c r="E893" t="inlineStr">
         <is>
@@ -43246,10 +43246,10 @@
         </is>
       </c>
       <c r="C894" t="n">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="D894" t="n">
-        <v>2230736</v>
+        <v>2235236</v>
       </c>
       <c r="E894" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D896" t="n">
-        <v>300819</v>
+        <v>302319</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43390,10 +43390,10 @@
         </is>
       </c>
       <c r="C897" t="n">
-        <v>46588</v>
+        <v>46660</v>
       </c>
       <c r="D897" t="n">
-        <v>58460184</v>
+        <v>58544946</v>
       </c>
       <c r="E897" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D899" t="n">
-        <v>35968</v>
+        <v>37468</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43630,10 +43630,10 @@
         </is>
       </c>
       <c r="C902" t="n">
-        <v>21686</v>
+        <v>21711</v>
       </c>
       <c r="D902" t="n">
-        <v>31800851</v>
+        <v>31838351</v>
       </c>
       <c r="E902" t="inlineStr">
         <is>
@@ -43726,10 +43726,10 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>6232</v>
+        <v>6242</v>
       </c>
       <c r="D904" t="n">
-        <v>8981455</v>
+        <v>8994987</v>
       </c>
       <c r="E904" t="inlineStr">
         <is>
@@ -43870,10 +43870,10 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="D907" t="n">
-        <v>1433125</v>
+        <v>1439125</v>
       </c>
       <c r="E907" t="inlineStr">
         <is>
@@ -43918,10 +43918,10 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>21825</v>
+        <v>21846</v>
       </c>
       <c r="D908" t="n">
-        <v>27134081</v>
+        <v>27160246</v>
       </c>
       <c r="E908" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>9993</v>
+        <v>10002</v>
       </c>
       <c r="D911" t="n">
-        <v>14640222</v>
+        <v>14653722</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44158,10 +44158,10 @@
         </is>
       </c>
       <c r="C913" t="n">
-        <v>2341</v>
+        <v>2344</v>
       </c>
       <c r="D913" t="n">
-        <v>3356847</v>
+        <v>3361347</v>
       </c>
       <c r="E913" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D916" t="n">
-        <v>945468</v>
+        <v>949968</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44350,10 +44350,10 @@
         </is>
       </c>
       <c r="C917" t="n">
-        <v>7312</v>
+        <v>7313</v>
       </c>
       <c r="D917" t="n">
-        <v>9175119</v>
+        <v>9176619</v>
       </c>
       <c r="E917" t="inlineStr">
         <is>
@@ -44590,10 +44590,10 @@
         </is>
       </c>
       <c r="C922" t="n">
-        <v>3090</v>
+        <v>3095</v>
       </c>
       <c r="D922" t="n">
-        <v>4550126</v>
+        <v>4557587</v>
       </c>
       <c r="E922" t="inlineStr">
         <is>
@@ -44638,10 +44638,10 @@
         </is>
       </c>
       <c r="C923" t="n">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D923" t="n">
-        <v>956793</v>
+        <v>961293</v>
       </c>
       <c r="E923" t="inlineStr">
         <is>
@@ -44734,10 +44734,10 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D925" t="n">
-        <v>271425</v>
+        <v>272925</v>
       </c>
       <c r="E925" t="inlineStr">
         <is>
@@ -44782,10 +44782,10 @@
         </is>
       </c>
       <c r="C926" t="n">
-        <v>13451</v>
+        <v>13465</v>
       </c>
       <c r="D926" t="n">
-        <v>16721818</v>
+        <v>16738461</v>
       </c>
       <c r="E926" t="inlineStr">
         <is>
@@ -44974,10 +44974,10 @@
         </is>
       </c>
       <c r="C930" t="n">
-        <v>5377</v>
+        <v>5384</v>
       </c>
       <c r="D930" t="n">
-        <v>7852904</v>
+        <v>7861844</v>
       </c>
       <c r="E930" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D931" t="n">
-        <v>13649</v>
+        <v>15149</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45070,10 +45070,10 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>1456</v>
+        <v>1460</v>
       </c>
       <c r="D932" t="n">
-        <v>2091426</v>
+        <v>2097426</v>
       </c>
       <c r="E932" t="inlineStr">
         <is>
@@ -45310,10 +45310,10 @@
         </is>
       </c>
       <c r="C937" t="n">
-        <v>19930</v>
+        <v>19959</v>
       </c>
       <c r="D937" t="n">
-        <v>24877007</v>
+        <v>24910341</v>
       </c>
       <c r="E937" t="inlineStr">
         <is>
@@ -45550,10 +45550,10 @@
         </is>
       </c>
       <c r="C942" t="n">
-        <v>10274</v>
+        <v>10277</v>
       </c>
       <c r="D942" t="n">
-        <v>15014351</v>
+        <v>15017388</v>
       </c>
       <c r="E942" t="inlineStr">
         <is>
@@ -45646,10 +45646,10 @@
         </is>
       </c>
       <c r="C944" t="n">
-        <v>2148</v>
+        <v>2150</v>
       </c>
       <c r="D944" t="n">
-        <v>3099014</v>
+        <v>3102014</v>
       </c>
       <c r="E944" t="inlineStr">
         <is>
@@ -45790,10 +45790,10 @@
         </is>
       </c>
       <c r="C947" t="n">
-        <v>8914</v>
+        <v>8921</v>
       </c>
       <c r="D947" t="n">
-        <v>11111288</v>
+        <v>11120011</v>
       </c>
       <c r="E947" t="inlineStr">
         <is>
@@ -46030,10 +46030,10 @@
         </is>
       </c>
       <c r="C952" t="n">
-        <v>3274</v>
+        <v>3279</v>
       </c>
       <c r="D952" t="n">
-        <v>4777341</v>
+        <v>4784841</v>
       </c>
       <c r="E952" t="inlineStr">
         <is>
@@ -46078,10 +46078,10 @@
         </is>
       </c>
       <c r="C953" t="n">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D953" t="n">
-        <v>2235795</v>
+        <v>2237295</v>
       </c>
       <c r="E953" t="inlineStr">
         <is>
@@ -46270,10 +46270,10 @@
         </is>
       </c>
       <c r="C957" t="n">
-        <v>70596</v>
+        <v>70763</v>
       </c>
       <c r="D957" t="n">
-        <v>90728193</v>
+        <v>90947250</v>
       </c>
       <c r="E957" t="inlineStr">
         <is>
@@ -46606,10 +46606,10 @@
         </is>
       </c>
       <c r="C964" t="n">
-        <v>26488</v>
+        <v>26524</v>
       </c>
       <c r="D964" t="n">
-        <v>38819416</v>
+        <v>38872991</v>
       </c>
       <c r="E964" t="inlineStr">
         <is>
@@ -46702,10 +46702,10 @@
         </is>
       </c>
       <c r="C966" t="n">
-        <v>18669</v>
+        <v>18709</v>
       </c>
       <c r="D966" t="n">
-        <v>27078845</v>
+        <v>27138426</v>
       </c>
       <c r="E966" t="inlineStr">
         <is>
@@ -46846,10 +46846,10 @@
         </is>
       </c>
       <c r="C969" t="n">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="D969" t="n">
-        <v>1346844</v>
+        <v>1349631</v>
       </c>
       <c r="E969" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>87586</v>
+        <v>87729</v>
       </c>
       <c r="D970" t="n">
-        <v>109929230</v>
+        <v>110102777</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>34868</v>
+        <v>34903</v>
       </c>
       <c r="D977" t="n">
-        <v>51131976</v>
+        <v>51181914</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47326,10 +47326,10 @@
         </is>
       </c>
       <c r="C979" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D979" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E979" t="inlineStr">
         <is>
@@ -47374,10 +47374,10 @@
         </is>
       </c>
       <c r="C980" t="n">
-        <v>26358</v>
+        <v>26413</v>
       </c>
       <c r="D980" t="n">
-        <v>38248025</v>
+        <v>38327542</v>
       </c>
       <c r="E980" t="inlineStr">
         <is>
@@ -47518,10 +47518,10 @@
         </is>
       </c>
       <c r="C983" t="n">
-        <v>2176</v>
+        <v>2181</v>
       </c>
       <c r="D983" t="n">
-        <v>3062942</v>
+        <v>3070442</v>
       </c>
       <c r="E983" t="inlineStr">
         <is>
@@ -47566,10 +47566,10 @@
         </is>
       </c>
       <c r="C984" t="n">
-        <v>11112</v>
+        <v>11137</v>
       </c>
       <c r="D984" t="n">
-        <v>14476348</v>
+        <v>14505615</v>
       </c>
       <c r="E984" t="inlineStr">
         <is>
@@ -47806,10 +47806,10 @@
         </is>
       </c>
       <c r="C989" t="n">
-        <v>3571</v>
+        <v>3577</v>
       </c>
       <c r="D989" t="n">
-        <v>5216061</v>
+        <v>5225061</v>
       </c>
       <c r="E989" t="inlineStr">
         <is>
@@ -48046,10 +48046,10 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D994" t="n">
-        <v>262533</v>
+        <v>267033</v>
       </c>
       <c r="E994" t="inlineStr">
         <is>
@@ -48094,10 +48094,10 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>57670</v>
+        <v>57733</v>
       </c>
       <c r="D995" t="n">
-        <v>72132195</v>
+        <v>72203130</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
@@ -48334,10 +48334,10 @@
         </is>
       </c>
       <c r="C1000" t="n">
-        <v>18868</v>
+        <v>18873</v>
       </c>
       <c r="D1000" t="n">
-        <v>27633352</v>
+        <v>27640852</v>
       </c>
       <c r="E1000" t="inlineStr">
         <is>
@@ -48430,10 +48430,10 @@
         </is>
       </c>
       <c r="C1002" t="n">
-        <v>13051</v>
+        <v>13069</v>
       </c>
       <c r="D1002" t="n">
-        <v>18874041</v>
+        <v>18899225</v>
       </c>
       <c r="E1002" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="D1005" t="n">
-        <v>1112578</v>
+        <v>1115578</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>29254</v>
+        <v>29307</v>
       </c>
       <c r="D1006" t="n">
-        <v>36362449</v>
+        <v>36435306</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>
@@ -48862,10 +48862,10 @@
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>10840</v>
+        <v>10846</v>
       </c>
       <c r="D1011" t="n">
-        <v>15875995</v>
+        <v>15884995</v>
       </c>
       <c r="E1011" t="inlineStr">
         <is>
@@ -48958,10 +48958,10 @@
         </is>
       </c>
       <c r="C1013" t="n">
-        <v>6474</v>
+        <v>6478</v>
       </c>
       <c r="D1013" t="n">
-        <v>9387129</v>
+        <v>9393129</v>
       </c>
       <c r="E1013" t="inlineStr">
         <is>
@@ -49006,10 +49006,10 @@
         </is>
       </c>
       <c r="C1014" t="n">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D1014" t="n">
-        <v>771253</v>
+        <v>772753</v>
       </c>
       <c r="E1014" t="inlineStr">
         <is>
@@ -49054,10 +49054,10 @@
         </is>
       </c>
       <c r="C1015" t="n">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D1015" t="n">
-        <v>830225</v>
+        <v>833225</v>
       </c>
       <c r="E1015" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-10-04 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17386</v>
+        <v>17396</v>
       </c>
       <c r="D2" t="n">
-        <v>21808528</v>
+        <v>21819363</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6512</v>
+        <v>6513</v>
       </c>
       <c r="D6" t="n">
-        <v>9528082</v>
+        <v>9529582</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3520</v>
+        <v>3528</v>
       </c>
       <c r="D8" t="n">
-        <v>5096998</v>
+        <v>5108155</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D11" t="n">
-        <v>633846</v>
+        <v>639846</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11650</v>
+        <v>11660</v>
       </c>
       <c r="D12" t="n">
-        <v>14680139</v>
+        <v>14692296</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3363</v>
+        <v>3368</v>
       </c>
       <c r="D16" t="n">
-        <v>4895655</v>
+        <v>4901793</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1560</v>
+        <v>1562</v>
       </c>
       <c r="D18" t="n">
-        <v>2249039</v>
+        <v>2252039</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D19" t="n">
-        <v>578880</v>
+        <v>580380</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15043</v>
+        <v>15051</v>
       </c>
       <c r="D22" t="n">
-        <v>18395166</v>
+        <v>18400730</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D31" t="n">
-        <v>566634</v>
+        <v>568134</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6888</v>
+        <v>6889</v>
       </c>
       <c r="D32" t="n">
-        <v>9132271</v>
+        <v>9133771</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D37" t="n">
-        <v>843798</v>
+        <v>846798</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D40" t="n">
-        <v>199891</v>
+        <v>200435</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>23122</v>
+        <v>23127</v>
       </c>
       <c r="D41" t="n">
-        <v>28388163</v>
+        <v>28394277</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>8100</v>
+        <v>8106</v>
       </c>
       <c r="D47" t="n">
-        <v>11900511</v>
+        <v>11908770</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4061</v>
+        <v>4063</v>
       </c>
       <c r="D49" t="n">
-        <v>5876155</v>
+        <v>5879155</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8545</v>
+        <v>8549</v>
       </c>
       <c r="D53" t="n">
-        <v>10871603</v>
+        <v>10877241</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2893</v>
+        <v>2894</v>
       </c>
       <c r="D57" t="n">
-        <v>4205597</v>
+        <v>4207097</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D61" t="n">
-        <v>402311</v>
+        <v>403811</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>38714</v>
+        <v>38745</v>
       </c>
       <c r="D62" t="n">
-        <v>49794325</v>
+        <v>49830534</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>13887</v>
+        <v>13895</v>
       </c>
       <c r="D67" t="n">
-        <v>20351482</v>
+        <v>20363482</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5568</v>
+        <v>5578</v>
       </c>
       <c r="D69" t="n">
-        <v>8049865</v>
+        <v>8064865</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D74" t="n">
-        <v>553912</v>
+        <v>554924</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3982,10 +3982,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>49131</v>
+        <v>49165</v>
       </c>
       <c r="D76" t="n">
-        <v>62663866</v>
+        <v>62700420</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>19049</v>
+        <v>19059</v>
       </c>
       <c r="D80" t="n">
-        <v>27892780</v>
+        <v>27907780</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>10011</v>
+        <v>10019</v>
       </c>
       <c r="D82" t="n">
-        <v>14453943</v>
+        <v>14465688</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>969</v>
+        <v>974</v>
       </c>
       <c r="D86" t="n">
-        <v>1368441</v>
+        <v>1375176</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4510,10 +4510,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>26211</v>
+        <v>26232</v>
       </c>
       <c r="D87" t="n">
-        <v>32980624</v>
+        <v>33002227</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>9065</v>
+        <v>9073</v>
       </c>
       <c r="D91" t="n">
-        <v>13303226</v>
+        <v>13314885</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5214</v>
+        <v>5223</v>
       </c>
       <c r="D93" t="n">
-        <v>7530850</v>
+        <v>7544350</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D94" t="n">
-        <v>528822</v>
+        <v>530322</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="D95" t="n">
-        <v>1253544</v>
+        <v>1256544</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>23200</v>
+        <v>23217</v>
       </c>
       <c r="D96" t="n">
-        <v>29027530</v>
+        <v>29045408</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -5134,10 +5134,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>9602</v>
+        <v>9610</v>
       </c>
       <c r="D100" t="n">
-        <v>14049919</v>
+        <v>14061919</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -5230,10 +5230,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>3533</v>
+        <v>3537</v>
       </c>
       <c r="D102" t="n">
-        <v>5060746</v>
+        <v>5066746</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D106" t="n">
-        <v>748079</v>
+        <v>749554</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5470,10 +5470,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>88917</v>
+        <v>88991</v>
       </c>
       <c r="D107" t="n">
-        <v>113778433</v>
+        <v>113865131</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>32273</v>
+        <v>32302</v>
       </c>
       <c r="D114" t="n">
-        <v>47329265</v>
+        <v>47371844</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -5902,10 +5902,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>22706</v>
+        <v>22733</v>
       </c>
       <c r="D116" t="n">
-        <v>32755734</v>
+        <v>32796234</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>2351</v>
+        <v>2367</v>
       </c>
       <c r="D123" t="n">
-        <v>3296693</v>
+        <v>3318544</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>29573</v>
+        <v>29617</v>
       </c>
       <c r="D124" t="n">
-        <v>38970608</v>
+        <v>39030191</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6334,10 +6334,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D125" t="n">
-        <v>135908</v>
+        <v>138908</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6430,10 +6430,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D127" t="n">
-        <v>149105</v>
+        <v>150605</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>10462</v>
+        <v>10470</v>
       </c>
       <c r="D128" t="n">
-        <v>15337057</v>
+        <v>15349057</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>3519</v>
+        <v>3524</v>
       </c>
       <c r="D130" t="n">
-        <v>5122700</v>
+        <v>5129745</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D133" t="n">
-        <v>575855</v>
+        <v>577855</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>16669</v>
+        <v>16675</v>
       </c>
       <c r="D134" t="n">
-        <v>20651931</v>
+        <v>20659699</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -6958,10 +6958,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>8116</v>
+        <v>8117</v>
       </c>
       <c r="D138" t="n">
-        <v>11868045</v>
+        <v>11869545</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -7054,10 +7054,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2380</v>
+        <v>2384</v>
       </c>
       <c r="D140" t="n">
-        <v>3397974</v>
+        <v>3403974</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D144" t="n">
-        <v>676946</v>
+        <v>678697</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7294,10 +7294,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>14427</v>
+        <v>14436</v>
       </c>
       <c r="D145" t="n">
-        <v>17964205</v>
+        <v>17977342</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>6502</v>
+        <v>6507</v>
       </c>
       <c r="D149" t="n">
-        <v>9522091</v>
+        <v>9529591</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7582,10 +7582,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>2109</v>
+        <v>2110</v>
       </c>
       <c r="D151" t="n">
-        <v>3045836</v>
+        <v>3047336</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D154" t="n">
-        <v>596085</v>
+        <v>597585</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>6301</v>
+        <v>6304</v>
       </c>
       <c r="D155" t="n">
-        <v>7707512</v>
+        <v>7712012</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D162" t="n">
-        <v>135103</v>
+        <v>136603</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>7840</v>
+        <v>7842</v>
       </c>
       <c r="D163" t="n">
-        <v>9681339</v>
+        <v>9682327</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>2989</v>
+        <v>2990</v>
       </c>
       <c r="D166" t="n">
-        <v>4382794</v>
+        <v>4384294</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8542,10 +8542,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>5920</v>
+        <v>5925</v>
       </c>
       <c r="D171" t="n">
-        <v>7415155</v>
+        <v>7421836</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -8782,10 +8782,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>2103</v>
+        <v>2104</v>
       </c>
       <c r="D176" t="n">
-        <v>3067061</v>
+        <v>3068561</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -9022,10 +9022,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>16950</v>
+        <v>16958</v>
       </c>
       <c r="D181" t="n">
-        <v>21223385</v>
+        <v>21233769</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>6653</v>
+        <v>6655</v>
       </c>
       <c r="D186" t="n">
-        <v>9718811</v>
+        <v>9720704</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>2368</v>
+        <v>2370</v>
       </c>
       <c r="D188" t="n">
-        <v>3403140</v>
+        <v>3406140</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="D191" t="n">
-        <v>744535</v>
+        <v>752035</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9550,10 +9550,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>3244</v>
+        <v>3245</v>
       </c>
       <c r="D192" t="n">
-        <v>4059113</v>
+        <v>4060613</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -9646,10 +9646,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="D194" t="n">
-        <v>2256872</v>
+        <v>2265062</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>9755</v>
+        <v>9772</v>
       </c>
       <c r="D200" t="n">
-        <v>12152857</v>
+        <v>12171738</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -10126,10 +10126,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>3585</v>
+        <v>3586</v>
       </c>
       <c r="D204" t="n">
-        <v>5261956</v>
+        <v>5263456</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D209" t="n">
-        <v>351471</v>
+        <v>352971</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>18068</v>
+        <v>18078</v>
       </c>
       <c r="D210" t="n">
-        <v>22497782</v>
+        <v>22506674</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D212" t="n">
-        <v>29047</v>
+        <v>30547</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D217" t="n">
-        <v>780092</v>
+        <v>781592</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>27379</v>
+        <v>27397</v>
       </c>
       <c r="D218" t="n">
-        <v>34404298</v>
+        <v>34426747</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>10862</v>
+        <v>10867</v>
       </c>
       <c r="D222" t="n">
-        <v>15856604</v>
+        <v>15864104</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2771</v>
+        <v>2772</v>
       </c>
       <c r="D224" t="n">
-        <v>3987254</v>
+        <v>3988754</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11230,10 +11230,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="D227" t="n">
-        <v>985461</v>
+        <v>988461</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>30303</v>
+        <v>30328</v>
       </c>
       <c r="D228" t="n">
-        <v>38122396</v>
+        <v>38152652</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>15473</v>
+        <v>15482</v>
       </c>
       <c r="D233" t="n">
-        <v>22695536</v>
+        <v>22709036</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>2877</v>
+        <v>2881</v>
       </c>
       <c r="D235" t="n">
-        <v>4127920</v>
+        <v>4131421</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="D238" t="n">
-        <v>1259230</v>
+        <v>1262230</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11806,10 +11806,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>25658</v>
+        <v>25674</v>
       </c>
       <c r="D239" t="n">
-        <v>32287528</v>
+        <v>32307500</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -12094,10 +12094,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>11606</v>
+        <v>11610</v>
       </c>
       <c r="D245" t="n">
-        <v>17004802</v>
+        <v>17010802</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -12190,10 +12190,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>2671</v>
+        <v>2673</v>
       </c>
       <c r="D247" t="n">
-        <v>3808349</v>
+        <v>3811349</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="D250" t="n">
-        <v>757156</v>
+        <v>763156</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>8266</v>
+        <v>8267</v>
       </c>
       <c r="D251" t="n">
-        <v>10337773</v>
+        <v>10338600</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12574,10 +12574,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2839</v>
+        <v>2841</v>
       </c>
       <c r="D255" t="n">
-        <v>4166922</v>
+        <v>4168534</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -12718,10 +12718,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="D258" t="n">
-        <v>1549513</v>
+        <v>1551013</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>10482</v>
+        <v>10488</v>
       </c>
       <c r="D261" t="n">
-        <v>13375346</v>
+        <v>13382052</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>4391</v>
+        <v>4393</v>
       </c>
       <c r="D265" t="n">
-        <v>6447587</v>
+        <v>6450587</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>2332</v>
+        <v>2335</v>
       </c>
       <c r="D267" t="n">
-        <v>3375601</v>
+        <v>3380101</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13246,10 +13246,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D269" t="n">
-        <v>210281</v>
+        <v>214781</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>5903</v>
+        <v>5906</v>
       </c>
       <c r="D270" t="n">
-        <v>7287414</v>
+        <v>7290498</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>20238</v>
+        <v>20248</v>
       </c>
       <c r="D279" t="n">
-        <v>25482693</v>
+        <v>25494242</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>8373</v>
+        <v>8378</v>
       </c>
       <c r="D283" t="n">
-        <v>12263378</v>
+        <v>12269778</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>2671</v>
+        <v>2672</v>
       </c>
       <c r="D285" t="n">
-        <v>3834992</v>
+        <v>3836492</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14158,10 +14158,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="D288" t="n">
-        <v>798829</v>
+        <v>802829</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>17548</v>
+        <v>17564</v>
       </c>
       <c r="D290" t="n">
-        <v>21704921</v>
+        <v>21723692</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>7526</v>
+        <v>7532</v>
       </c>
       <c r="D295" t="n">
-        <v>11037827</v>
+        <v>11046477</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>3565</v>
+        <v>3568</v>
       </c>
       <c r="D296" t="n">
-        <v>5163860</v>
+        <v>5168360</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>9866</v>
+        <v>9872</v>
       </c>
       <c r="D300" t="n">
-        <v>12357415</v>
+        <v>12366365</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>4058</v>
+        <v>4060</v>
       </c>
       <c r="D304" t="n">
-        <v>5939996</v>
+        <v>5942996</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="D305" t="n">
-        <v>1932846</v>
+        <v>1935846</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>9787</v>
+        <v>9796</v>
       </c>
       <c r="D310" t="n">
-        <v>12774920</v>
+        <v>12787717</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>3975</v>
+        <v>3983</v>
       </c>
       <c r="D314" t="n">
-        <v>5812611</v>
+        <v>5823769</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>2540</v>
+        <v>2543</v>
       </c>
       <c r="D315" t="n">
-        <v>3700151</v>
+        <v>3704651</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D316" t="n">
-        <v>361302</v>
+        <v>364302</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15550,10 +15550,10 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D317" t="n">
-        <v>175627</v>
+        <v>178627</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>11834</v>
+        <v>11844</v>
       </c>
       <c r="D318" t="n">
-        <v>15514223</v>
+        <v>15526384</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>4037</v>
+        <v>4042</v>
       </c>
       <c r="D322" t="n">
-        <v>5920535</v>
+        <v>5928035</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>2887</v>
+        <v>2890</v>
       </c>
       <c r="D324" t="n">
-        <v>4186832</v>
+        <v>4191332</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>7167</v>
+        <v>7169</v>
       </c>
       <c r="D327" t="n">
-        <v>8854815</v>
+        <v>8856059</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="D332" t="n">
-        <v>3521449</v>
+        <v>3522949</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>7936</v>
+        <v>7942</v>
       </c>
       <c r="D337" t="n">
-        <v>9916284</v>
+        <v>9923787</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>3286</v>
+        <v>3288</v>
       </c>
       <c r="D342" t="n">
-        <v>4798375</v>
+        <v>4801375</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>1365</v>
+        <v>1367</v>
       </c>
       <c r="D343" t="n">
-        <v>1956584</v>
+        <v>1959584</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>34338</v>
+        <v>34385</v>
       </c>
       <c r="D347" t="n">
-        <v>43089889</v>
+        <v>43144187</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>17381</v>
+        <v>17395</v>
       </c>
       <c r="D353" t="n">
-        <v>25400804</v>
+        <v>25421040</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>8579</v>
+        <v>8590</v>
       </c>
       <c r="D356" t="n">
-        <v>12351437</v>
+        <v>12366503</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17518,10 +17518,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>959</v>
+        <v>964</v>
       </c>
       <c r="D358" t="n">
-        <v>1355982</v>
+        <v>1362679</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>4154</v>
+        <v>4156</v>
       </c>
       <c r="D359" t="n">
-        <v>5153753</v>
+        <v>5155334</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D362" t="n">
-        <v>2292139</v>
+        <v>2293639</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>20560</v>
+        <v>20571</v>
       </c>
       <c r="D367" t="n">
-        <v>25569259</v>
+        <v>25582790</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>10370</v>
+        <v>10378</v>
       </c>
       <c r="D371" t="n">
-        <v>15203436</v>
+        <v>15215163</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>5029</v>
+        <v>5033</v>
       </c>
       <c r="D373" t="n">
-        <v>7283046</v>
+        <v>7287029</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>14920</v>
+        <v>14929</v>
       </c>
       <c r="D376" t="n">
-        <v>18612103</v>
+        <v>18622819</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>6798</v>
+        <v>6804</v>
       </c>
       <c r="D380" t="n">
-        <v>9949978</v>
+        <v>9958978</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>2685</v>
+        <v>2690</v>
       </c>
       <c r="D382" t="n">
-        <v>3855072</v>
+        <v>3862572</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="D383" t="n">
-        <v>1147621</v>
+        <v>1150261</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>19056</v>
+        <v>19072</v>
       </c>
       <c r="D385" t="n">
-        <v>23695409</v>
+        <v>23711094</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -19006,10 +19006,10 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>7459</v>
+        <v>7464</v>
       </c>
       <c r="D389" t="n">
-        <v>10953867</v>
+        <v>10961367</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>2984</v>
+        <v>2986</v>
       </c>
       <c r="D391" t="n">
-        <v>4342069</v>
+        <v>4345069</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D394" t="n">
-        <v>675822</v>
+        <v>678822</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>4325</v>
+        <v>4327</v>
       </c>
       <c r="D395" t="n">
-        <v>5401599</v>
+        <v>5404115</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D398" t="n">
-        <v>2103640</v>
+        <v>2105140</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D399" t="n">
-        <v>875628</v>
+        <v>877128</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D401" t="n">
-        <v>143747</v>
+        <v>146747</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>23542</v>
+        <v>23557</v>
       </c>
       <c r="D402" t="n">
-        <v>29113326</v>
+        <v>29130455</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>9746</v>
+        <v>9759</v>
       </c>
       <c r="D405" t="n">
-        <v>14340770</v>
+        <v>14359350</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>6530</v>
+        <v>6535</v>
       </c>
       <c r="D407" t="n">
-        <v>9489975</v>
+        <v>9497475</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D409" t="n">
-        <v>577550</v>
+        <v>579050</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>11804</v>
+        <v>11807</v>
       </c>
       <c r="D410" t="n">
-        <v>14497766</v>
+        <v>14502266</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>5530</v>
+        <v>5531</v>
       </c>
       <c r="D415" t="n">
-        <v>8082532</v>
+        <v>8084032</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>36020</v>
+        <v>36075</v>
       </c>
       <c r="D420" t="n">
-        <v>48844635</v>
+        <v>48918778</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>8782</v>
+        <v>8794</v>
       </c>
       <c r="D424" t="n">
-        <v>12904758</v>
+        <v>12922758</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>8160</v>
+        <v>8182</v>
       </c>
       <c r="D426" t="n">
-        <v>11837519</v>
+        <v>11869214</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D428" t="n">
-        <v>818876</v>
+        <v>820376</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>13721</v>
+        <v>13831</v>
       </c>
       <c r="D430" t="n">
-        <v>23711065</v>
+        <v>23978665</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>3267</v>
+        <v>3275</v>
       </c>
       <c r="D433" t="n">
-        <v>6092377</v>
+        <v>6116377</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>4547</v>
+        <v>4575</v>
       </c>
       <c r="D435" t="n">
-        <v>8499980</v>
+        <v>8579021</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D437" t="n">
-        <v>356290</v>
+        <v>363790</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21358,10 +21358,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="D438" t="n">
-        <v>490473</v>
+        <v>503191</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>11708</v>
+        <v>11714</v>
       </c>
       <c r="D440" t="n">
-        <v>14463854</v>
+        <v>14472314</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>3998</v>
+        <v>4001</v>
       </c>
       <c r="D443" t="n">
-        <v>5862484</v>
+        <v>5866984</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="D445" t="n">
-        <v>2880538</v>
+        <v>2883538</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21838,10 +21838,10 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>67442</v>
+        <v>67485</v>
       </c>
       <c r="D448" t="n">
-        <v>83498558</v>
+        <v>83548707</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>26321</v>
+        <v>26341</v>
       </c>
       <c r="D452" t="n">
-        <v>38546160</v>
+        <v>38575347</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>14182</v>
+        <v>14199</v>
       </c>
       <c r="D454" t="n">
-        <v>20567788</v>
+        <v>20592002</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="D458" t="n">
-        <v>1789588</v>
+        <v>1792588</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>20369</v>
+        <v>20379</v>
       </c>
       <c r="D460" t="n">
-        <v>25786003</v>
+        <v>25797203</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>8100</v>
+        <v>8107</v>
       </c>
       <c r="D464" t="n">
-        <v>11878513</v>
+        <v>11889013</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>5394</v>
+        <v>5406</v>
       </c>
       <c r="D466" t="n">
-        <v>7831253</v>
+        <v>7849253</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D467" t="n">
-        <v>248597</v>
+        <v>250097</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D468" t="n">
-        <v>456515</v>
+        <v>458015</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>33904</v>
+        <v>33926</v>
       </c>
       <c r="D469" t="n">
-        <v>41373373</v>
+        <v>41395399</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23038,10 +23038,10 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>11925</v>
+        <v>11931</v>
       </c>
       <c r="D473" t="n">
-        <v>17432870</v>
+        <v>17441870</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -23278,10 +23278,10 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>15191</v>
+        <v>15198</v>
       </c>
       <c r="D478" t="n">
-        <v>18508669</v>
+        <v>18517870</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>4588</v>
+        <v>4591</v>
       </c>
       <c r="D483" t="n">
-        <v>6737185</v>
+        <v>6741685</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>2225</v>
+        <v>2228</v>
       </c>
       <c r="D485" t="n">
-        <v>3205307</v>
+        <v>3209807</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D487" t="n">
-        <v>538232</v>
+        <v>539732</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>40410</v>
+        <v>40460</v>
       </c>
       <c r="D488" t="n">
-        <v>52814519</v>
+        <v>52876995</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23950,10 +23950,10 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>14434</v>
+        <v>14445</v>
       </c>
       <c r="D492" t="n">
-        <v>21223938</v>
+        <v>21238200</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>13542</v>
+        <v>13564</v>
       </c>
       <c r="D494" t="n">
-        <v>19771080</v>
+        <v>19802510</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24190,10 +24190,10 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>72534</v>
+        <v>72637</v>
       </c>
       <c r="D497" t="n">
-        <v>96104405</v>
+        <v>96232746</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>25455</v>
+        <v>25499</v>
       </c>
       <c r="D502" t="n">
-        <v>37328068</v>
+        <v>37392687</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24526,10 +24526,10 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>26119</v>
+        <v>26165</v>
       </c>
       <c r="D504" t="n">
-        <v>37914777</v>
+        <v>37980113</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="D507" t="n">
-        <v>1110311</v>
+        <v>1113311</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>173637</v>
+        <v>173888</v>
       </c>
       <c r="D508" t="n">
-        <v>227777180</v>
+        <v>228082654</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D513" t="n">
-        <v>763190</v>
+        <v>764690</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D514" t="n">
-        <v>36010</v>
+        <v>37510</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>90673</v>
+        <v>90861</v>
       </c>
       <c r="D515" t="n">
-        <v>133165447</v>
+        <v>133442530</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25198,10 +25198,10 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>68470</v>
+        <v>68600</v>
       </c>
       <c r="D518" t="n">
-        <v>99471365</v>
+        <v>99660092</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>3453</v>
+        <v>3469</v>
       </c>
       <c r="D522" t="n">
-        <v>4881333</v>
+        <v>4901166</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D524" t="n">
-        <v>18000</v>
+        <v>19500</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25534,10 +25534,10 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>46384</v>
+        <v>46431</v>
       </c>
       <c r="D525" t="n">
-        <v>60459135</v>
+        <v>60520543</v>
       </c>
       <c r="E525" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>16294</v>
+        <v>16309</v>
       </c>
       <c r="D530" t="n">
-        <v>23924833</v>
+        <v>23945480</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>14518</v>
+        <v>14538</v>
       </c>
       <c r="D532" t="n">
-        <v>21042490</v>
+        <v>21072399</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D535" t="n">
-        <v>586892</v>
+        <v>588655</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>78146</v>
+        <v>78305</v>
       </c>
       <c r="D537" t="n">
-        <v>105426401</v>
+        <v>105639172</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>25287</v>
+        <v>25330</v>
       </c>
       <c r="D541" t="n">
-        <v>37285367</v>
+        <v>37347260</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26398,10 +26398,10 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>28431</v>
+        <v>28504</v>
       </c>
       <c r="D543" t="n">
-        <v>41580914</v>
+        <v>41688135</v>
       </c>
       <c r="E543" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D545" t="n">
-        <v>375110</v>
+        <v>375620</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="D547" t="n">
-        <v>1459863</v>
+        <v>1468863</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>63194</v>
+        <v>63265</v>
       </c>
       <c r="D548" t="n">
-        <v>83899957</v>
+        <v>83986028</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>19267</v>
+        <v>19293</v>
       </c>
       <c r="D553" t="n">
-        <v>28299064</v>
+        <v>28338064</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>21135</v>
+        <v>21164</v>
       </c>
       <c r="D555" t="n">
-        <v>30740989</v>
+        <v>30783324</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D557" t="n">
-        <v>1053089</v>
+        <v>1054589</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27118,10 +27118,10 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>48132</v>
+        <v>48195</v>
       </c>
       <c r="D558" t="n">
-        <v>64220555</v>
+        <v>64297700</v>
       </c>
       <c r="E558" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>15158</v>
+        <v>15168</v>
       </c>
       <c r="D562" t="n">
-        <v>22334718</v>
+        <v>22349205</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27406,10 +27406,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>16634</v>
+        <v>16656</v>
       </c>
       <c r="D564" t="n">
-        <v>24154464</v>
+        <v>24185412</v>
       </c>
       <c r="E564" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D566" t="n">
-        <v>486595</v>
+        <v>487964</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>46024</v>
+        <v>46071</v>
       </c>
       <c r="D567" t="n">
-        <v>59781958</v>
+        <v>59842328</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27742,10 +27742,10 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>17217</v>
+        <v>17225</v>
       </c>
       <c r="D571" t="n">
-        <v>25247237</v>
+        <v>25257813</v>
       </c>
       <c r="E571" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>14559</v>
+        <v>14577</v>
       </c>
       <c r="D573" t="n">
-        <v>21064221</v>
+        <v>21087714</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27982,10 +27982,10 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D576" t="n">
-        <v>590774</v>
+        <v>592274</v>
       </c>
       <c r="E576" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>47705</v>
+        <v>47751</v>
       </c>
       <c r="D577" t="n">
-        <v>63608894</v>
+        <v>63669096</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>14786</v>
+        <v>14801</v>
       </c>
       <c r="D583" t="n">
-        <v>21667828</v>
+        <v>21690198</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>3993</v>
+        <v>3999</v>
       </c>
       <c r="D584" t="n">
-        <v>5761075</v>
+        <v>5770075</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D589" t="n">
-        <v>635398</v>
+        <v>639898</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>18799</v>
+        <v>18823</v>
       </c>
       <c r="D590" t="n">
-        <v>24859205</v>
+        <v>24888603</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>7730</v>
+        <v>7737</v>
       </c>
       <c r="D594" t="n">
-        <v>11249277</v>
+        <v>11257767</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>5441</v>
+        <v>5451</v>
       </c>
       <c r="D596" t="n">
-        <v>7837391</v>
+        <v>7852391</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>24253</v>
+        <v>24377</v>
       </c>
       <c r="D601" t="n">
-        <v>45224532</v>
+        <v>45524979</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>2491</v>
+        <v>2495</v>
       </c>
       <c r="D602" t="n">
-        <v>4598491</v>
+        <v>4608491</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>23270</v>
+        <v>23278</v>
       </c>
       <c r="D607" t="n">
-        <v>29097660</v>
+        <v>29107252</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>9418</v>
+        <v>9430</v>
       </c>
       <c r="D612" t="n">
-        <v>13784277</v>
+        <v>13802277</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29998,10 +29998,10 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>15573</v>
+        <v>15583</v>
       </c>
       <c r="D618" t="n">
-        <v>19479368</v>
+        <v>19487501</v>
       </c>
       <c r="E618" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>6084</v>
+        <v>6090</v>
       </c>
       <c r="D622" t="n">
-        <v>8929550</v>
+        <v>8938550</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>2884</v>
+        <v>2891</v>
       </c>
       <c r="D624" t="n">
-        <v>4157719</v>
+        <v>4166673</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D626" t="n">
-        <v>307020</v>
+        <v>311520</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30430,10 +30430,10 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>14502</v>
+        <v>14506</v>
       </c>
       <c r="D627" t="n">
-        <v>18252995</v>
+        <v>18257707</v>
       </c>
       <c r="E627" t="inlineStr">
         <is>
@@ -30622,10 +30622,10 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>5456</v>
+        <v>5459</v>
       </c>
       <c r="D631" t="n">
-        <v>7994323</v>
+        <v>7998823</v>
       </c>
       <c r="E631" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>7947</v>
+        <v>7952</v>
       </c>
       <c r="D636" t="n">
-        <v>10186343</v>
+        <v>10191559</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>2675</v>
+        <v>2676</v>
       </c>
       <c r="D641" t="n">
-        <v>3918610</v>
+        <v>3920110</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D644" t="n">
-        <v>224105</v>
+        <v>227105</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>30478</v>
+        <v>30487</v>
       </c>
       <c r="D645" t="n">
-        <v>37464551</v>
+        <v>37471990</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>11607</v>
+        <v>11615</v>
       </c>
       <c r="D650" t="n">
-        <v>17027653</v>
+        <v>17037629</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>5206</v>
+        <v>5215</v>
       </c>
       <c r="D652" t="n">
-        <v>7550654</v>
+        <v>7564154</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31726,10 +31726,10 @@
         </is>
       </c>
       <c r="C654" t="n">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D654" t="n">
-        <v>356147</v>
+        <v>359147</v>
       </c>
       <c r="E654" t="inlineStr">
         <is>
@@ -31774,10 +31774,10 @@
         </is>
       </c>
       <c r="C655" t="n">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D655" t="n">
-        <v>906656</v>
+        <v>909461</v>
       </c>
       <c r="E655" t="inlineStr">
         <is>
@@ -31822,10 +31822,10 @@
         </is>
       </c>
       <c r="C656" t="n">
-        <v>11933</v>
+        <v>11949</v>
       </c>
       <c r="D656" t="n">
-        <v>14391673</v>
+        <v>14407146</v>
       </c>
       <c r="E656" t="inlineStr">
         <is>
@@ -32110,10 +32110,10 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="D662" t="n">
-        <v>1659761</v>
+        <v>1662761</v>
       </c>
       <c r="E662" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>29659</v>
+        <v>29677</v>
       </c>
       <c r="D666" t="n">
-        <v>36790350</v>
+        <v>36812381</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D669" t="n">
-        <v>187451</v>
+        <v>188951</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>11090</v>
+        <v>11098</v>
       </c>
       <c r="D670" t="n">
-        <v>16294894</v>
+        <v>16305874</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="D672" t="n">
-        <v>4623207</v>
+        <v>4624707</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>7919</v>
+        <v>7929</v>
       </c>
       <c r="D676" t="n">
-        <v>10020592</v>
+        <v>10031080</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>2699</v>
+        <v>2701</v>
       </c>
       <c r="D678" t="n">
-        <v>3955048</v>
+        <v>3957404</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="D680" t="n">
-        <v>1972471</v>
+        <v>1975441</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>4030</v>
+        <v>4033</v>
       </c>
       <c r="D684" t="n">
-        <v>4860563</v>
+        <v>4864818</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D692" t="n">
-        <v>224614</v>
+        <v>226114</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>9815</v>
+        <v>9820</v>
       </c>
       <c r="D693" t="n">
-        <v>12189095</v>
+        <v>12194744</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>3610</v>
+        <v>3613</v>
       </c>
       <c r="D697" t="n">
-        <v>5322618</v>
+        <v>5327118</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>20289</v>
+        <v>20303</v>
       </c>
       <c r="D702" t="n">
-        <v>24782384</v>
+        <v>24799904</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>5953</v>
+        <v>5954</v>
       </c>
       <c r="D706" t="n">
-        <v>8695718</v>
+        <v>8696857</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D710" t="n">
-        <v>532375</v>
+        <v>535375</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34510,10 +34510,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D712" t="n">
-        <v>464677</v>
+        <v>466177</v>
       </c>
       <c r="E712" t="inlineStr">
         <is>
@@ -34558,10 +34558,10 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>79758</v>
+        <v>79820</v>
       </c>
       <c r="D713" t="n">
-        <v>100289527</v>
+        <v>100360083</v>
       </c>
       <c r="E713" t="inlineStr">
         <is>
@@ -34654,10 +34654,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D715" t="n">
-        <v>42298</v>
+        <v>44541</v>
       </c>
       <c r="E715" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>28001</v>
+        <v>28022</v>
       </c>
       <c r="D718" t="n">
-        <v>41076303</v>
+        <v>41107803</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34942,10 +34942,10 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>14230</v>
+        <v>14255</v>
       </c>
       <c r="D721" t="n">
-        <v>20528245</v>
+        <v>20565355</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>2045</v>
+        <v>2048</v>
       </c>
       <c r="D724" t="n">
-        <v>2944972</v>
+        <v>2949472</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35134,10 +35134,10 @@
         </is>
       </c>
       <c r="C725" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D725" t="n">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="E725" t="inlineStr">
         <is>
@@ -35182,10 +35182,10 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>1426</v>
+        <v>1429</v>
       </c>
       <c r="D726" t="n">
-        <v>1992878</v>
+        <v>1997378</v>
       </c>
       <c r="E726" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>11765</v>
+        <v>11770</v>
       </c>
       <c r="D727" t="n">
-        <v>14356945</v>
+        <v>14360586</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35566,10 +35566,10 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D734" t="n">
-        <v>413292</v>
+        <v>417792</v>
       </c>
       <c r="E734" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>18524</v>
+        <v>18534</v>
       </c>
       <c r="D735" t="n">
-        <v>22796014</v>
+        <v>22806639</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>7134</v>
+        <v>7136</v>
       </c>
       <c r="D739" t="n">
-        <v>10429069</v>
+        <v>10432069</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -36046,10 +36046,10 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D744" t="n">
-        <v>540280</v>
+        <v>541780</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
@@ -36142,10 +36142,10 @@
         </is>
       </c>
       <c r="C746" t="n">
-        <v>12145</v>
+        <v>12146</v>
       </c>
       <c r="D746" t="n">
-        <v>14959968</v>
+        <v>14960943</v>
       </c>
       <c r="E746" t="inlineStr">
         <is>
@@ -36334,10 +36334,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>4386</v>
+        <v>4388</v>
       </c>
       <c r="D750" t="n">
-        <v>6428752</v>
+        <v>6431752</v>
       </c>
       <c r="E750" t="inlineStr">
         <is>
@@ -36526,10 +36526,10 @@
         </is>
       </c>
       <c r="C754" t="n">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D754" t="n">
-        <v>487216</v>
+        <v>488716</v>
       </c>
       <c r="E754" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>30982</v>
+        <v>30994</v>
       </c>
       <c r="D755" t="n">
-        <v>38500619</v>
+        <v>38515712</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>13257</v>
+        <v>13263</v>
       </c>
       <c r="D760" t="n">
-        <v>19394415</v>
+        <v>19401840</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>4446</v>
+        <v>4455</v>
       </c>
       <c r="D762" t="n">
-        <v>6348902</v>
+        <v>6362402</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37006,10 +37006,10 @@
         </is>
       </c>
       <c r="C764" t="n">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D764" t="n">
-        <v>1100094</v>
+        <v>1101594</v>
       </c>
       <c r="E764" t="inlineStr">
         <is>
@@ -37054,10 +37054,10 @@
         </is>
       </c>
       <c r="C765" t="n">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="D765" t="n">
-        <v>1084552</v>
+        <v>1090552</v>
       </c>
       <c r="E765" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>12943</v>
+        <v>12948</v>
       </c>
       <c r="D767" t="n">
-        <v>15962848</v>
+        <v>15967576</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>4846</v>
+        <v>4852</v>
       </c>
       <c r="D770" t="n">
-        <v>7079475</v>
+        <v>7088475</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37438,10 +37438,10 @@
         </is>
       </c>
       <c r="C773" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D773" t="n">
-        <v>628053</v>
+        <v>629054</v>
       </c>
       <c r="E773" t="inlineStr">
         <is>
@@ -37486,10 +37486,10 @@
         </is>
       </c>
       <c r="C774" t="n">
-        <v>7114</v>
+        <v>7119</v>
       </c>
       <c r="D774" t="n">
-        <v>8326833</v>
+        <v>8332001</v>
       </c>
       <c r="E774" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D781" t="n">
-        <v>239487</v>
+        <v>240987</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>17730</v>
+        <v>17742</v>
       </c>
       <c r="D782" t="n">
-        <v>21503047</v>
+        <v>21519581</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38110,10 +38110,10 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>5806</v>
+        <v>5807</v>
       </c>
       <c r="D787" t="n">
-        <v>8512580</v>
+        <v>8514080</v>
       </c>
       <c r="E787" t="inlineStr">
         <is>
@@ -38206,10 +38206,10 @@
         </is>
       </c>
       <c r="C789" t="n">
-        <v>3623</v>
+        <v>3626</v>
       </c>
       <c r="D789" t="n">
-        <v>5289133</v>
+        <v>5293613</v>
       </c>
       <c r="E789" t="inlineStr">
         <is>
@@ -38350,10 +38350,10 @@
         </is>
       </c>
       <c r="C792" t="n">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D792" t="n">
-        <v>474541</v>
+        <v>479041</v>
       </c>
       <c r="E792" t="inlineStr">
         <is>
@@ -38398,10 +38398,10 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>11935</v>
+        <v>11952</v>
       </c>
       <c r="D793" t="n">
-        <v>15064971</v>
+        <v>15082690</v>
       </c>
       <c r="E793" t="inlineStr">
         <is>
@@ -38542,10 +38542,10 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D796" t="n">
-        <v>130669</v>
+        <v>132385</v>
       </c>
       <c r="E796" t="inlineStr">
         <is>
@@ -38590,10 +38590,10 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>4128</v>
+        <v>4130</v>
       </c>
       <c r="D797" t="n">
-        <v>6036823</v>
+        <v>6039823</v>
       </c>
       <c r="E797" t="inlineStr">
         <is>
@@ -38686,10 +38686,10 @@
         </is>
       </c>
       <c r="C799" t="n">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D799" t="n">
-        <v>1923053</v>
+        <v>1924553</v>
       </c>
       <c r="E799" t="inlineStr">
         <is>
@@ -38830,10 +38830,10 @@
         </is>
       </c>
       <c r="C802" t="n">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D802" t="n">
-        <v>388338</v>
+        <v>391338</v>
       </c>
       <c r="E802" t="inlineStr">
         <is>
@@ -38878,10 +38878,10 @@
         </is>
       </c>
       <c r="C803" t="n">
-        <v>34059</v>
+        <v>34080</v>
       </c>
       <c r="D803" t="n">
-        <v>41946938</v>
+        <v>41970877</v>
       </c>
       <c r="E803" t="inlineStr">
         <is>
@@ -39070,10 +39070,10 @@
         </is>
       </c>
       <c r="C807" t="n">
-        <v>13757</v>
+        <v>13763</v>
       </c>
       <c r="D807" t="n">
-        <v>20117828</v>
+        <v>20126431</v>
       </c>
       <c r="E807" t="inlineStr">
         <is>
@@ -39166,10 +39166,10 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>6400</v>
+        <v>6413</v>
       </c>
       <c r="D809" t="n">
-        <v>9247683</v>
+        <v>9266683</v>
       </c>
       <c r="E809" t="inlineStr">
         <is>
@@ -39214,10 +39214,10 @@
         </is>
       </c>
       <c r="C810" t="n">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D810" t="n">
-        <v>786278</v>
+        <v>789278</v>
       </c>
       <c r="E810" t="inlineStr">
         <is>
@@ -39310,10 +39310,10 @@
         </is>
       </c>
       <c r="C812" t="n">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="D812" t="n">
-        <v>1124104</v>
+        <v>1127104</v>
       </c>
       <c r="E812" t="inlineStr">
         <is>
@@ -39358,10 +39358,10 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>8089</v>
+        <v>8095</v>
       </c>
       <c r="D813" t="n">
-        <v>9978440</v>
+        <v>9986305</v>
       </c>
       <c r="E813" t="inlineStr">
         <is>
@@ -39646,10 +39646,10 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>2829</v>
+        <v>2832</v>
       </c>
       <c r="D819" t="n">
-        <v>4126266</v>
+        <v>4130766</v>
       </c>
       <c r="E819" t="inlineStr">
         <is>
@@ -39694,10 +39694,10 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D820" t="n">
-        <v>1752147</v>
+        <v>1753647</v>
       </c>
       <c r="E820" t="inlineStr">
         <is>
@@ -39742,10 +39742,10 @@
         </is>
       </c>
       <c r="C821" t="n">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D821" t="n">
-        <v>570650</v>
+        <v>572150</v>
       </c>
       <c r="E821" t="inlineStr">
         <is>
@@ -39790,10 +39790,10 @@
         </is>
       </c>
       <c r="C822" t="n">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D822" t="n">
-        <v>405898</v>
+        <v>410398</v>
       </c>
       <c r="E822" t="inlineStr">
         <is>
@@ -39838,10 +39838,10 @@
         </is>
       </c>
       <c r="C823" t="n">
-        <v>63467</v>
+        <v>63502</v>
       </c>
       <c r="D823" t="n">
-        <v>79221002</v>
+        <v>79261486</v>
       </c>
       <c r="E823" t="inlineStr">
         <is>
@@ -40078,10 +40078,10 @@
         </is>
       </c>
       <c r="C828" t="n">
-        <v>22437</v>
+        <v>22454</v>
       </c>
       <c r="D828" t="n">
-        <v>32810693</v>
+        <v>32836193</v>
       </c>
       <c r="E828" t="inlineStr">
         <is>
@@ -40222,10 +40222,10 @@
         </is>
       </c>
       <c r="C831" t="n">
-        <v>13660</v>
+        <v>13677</v>
       </c>
       <c r="D831" t="n">
-        <v>19702015</v>
+        <v>19727031</v>
       </c>
       <c r="E831" t="inlineStr">
         <is>
@@ -40462,10 +40462,10 @@
         </is>
       </c>
       <c r="C836" t="n">
-        <v>1603</v>
+        <v>1614</v>
       </c>
       <c r="D836" t="n">
-        <v>2238767</v>
+        <v>2251432</v>
       </c>
       <c r="E836" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>11969</v>
+        <v>11980</v>
       </c>
       <c r="D837" t="n">
-        <v>14933507</v>
+        <v>14946798</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40702,10 +40702,10 @@
         </is>
       </c>
       <c r="C841" t="n">
-        <v>4289</v>
+        <v>4298</v>
       </c>
       <c r="D841" t="n">
-        <v>6225797</v>
+        <v>6237197</v>
       </c>
       <c r="E841" t="inlineStr">
         <is>
@@ -40990,10 +40990,10 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D847" t="n">
-        <v>422889</v>
+        <v>425295</v>
       </c>
       <c r="E847" t="inlineStr">
         <is>
@@ -41038,10 +41038,10 @@
         </is>
       </c>
       <c r="C848" t="n">
-        <v>61925</v>
+        <v>61965</v>
       </c>
       <c r="D848" t="n">
-        <v>76485857</v>
+        <v>76528204</v>
       </c>
       <c r="E848" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D849" t="n">
-        <v>69929</v>
+        <v>71429</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41326,10 +41326,10 @@
         </is>
       </c>
       <c r="C854" t="n">
-        <v>23355</v>
+        <v>23368</v>
       </c>
       <c r="D854" t="n">
-        <v>34270710</v>
+        <v>34290156</v>
       </c>
       <c r="E854" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D855" t="n">
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41422,10 +41422,10 @@
         </is>
       </c>
       <c r="C856" t="n">
-        <v>15266</v>
+        <v>15281</v>
       </c>
       <c r="D856" t="n">
-        <v>22101290</v>
+        <v>22123634</v>
       </c>
       <c r="E856" t="inlineStr">
         <is>
@@ -41518,10 +41518,10 @@
         </is>
       </c>
       <c r="C858" t="n">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="D858" t="n">
-        <v>1305166</v>
+        <v>1306666</v>
       </c>
       <c r="E858" t="inlineStr">
         <is>
@@ -41566,10 +41566,10 @@
         </is>
       </c>
       <c r="C859" t="n">
-        <v>1566</v>
+        <v>1572</v>
       </c>
       <c r="D859" t="n">
-        <v>2181776</v>
+        <v>2190152</v>
       </c>
       <c r="E859" t="inlineStr">
         <is>
@@ -41662,10 +41662,10 @@
         </is>
       </c>
       <c r="C861" t="n">
-        <v>8173</v>
+        <v>8174</v>
       </c>
       <c r="D861" t="n">
-        <v>10004812</v>
+        <v>10006312</v>
       </c>
       <c r="E861" t="inlineStr">
         <is>
@@ -42334,10 +42334,10 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>23284</v>
+        <v>23298</v>
       </c>
       <c r="D875" t="n">
-        <v>29146307</v>
+        <v>29163767</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
@@ -42526,10 +42526,10 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>8054</v>
+        <v>8059</v>
       </c>
       <c r="D879" t="n">
-        <v>11756501</v>
+        <v>11764001</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
@@ -42622,10 +42622,10 @@
         </is>
       </c>
       <c r="C881" t="n">
-        <v>4897</v>
+        <v>4901</v>
       </c>
       <c r="D881" t="n">
-        <v>7076107</v>
+        <v>7082107</v>
       </c>
       <c r="E881" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="D884" t="n">
-        <v>732760</v>
+        <v>738529</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42862,10 +42862,10 @@
         </is>
       </c>
       <c r="C886" t="n">
-        <v>15273</v>
+        <v>15276</v>
       </c>
       <c r="D886" t="n">
-        <v>18382568</v>
+        <v>18386532</v>
       </c>
       <c r="E886" t="inlineStr">
         <is>
@@ -43054,10 +43054,10 @@
         </is>
       </c>
       <c r="C890" t="n">
-        <v>5465</v>
+        <v>5468</v>
       </c>
       <c r="D890" t="n">
-        <v>7966408</v>
+        <v>7970908</v>
       </c>
       <c r="E890" t="inlineStr">
         <is>
@@ -43150,10 +43150,10 @@
         </is>
       </c>
       <c r="C892" t="n">
-        <v>2535</v>
+        <v>2536</v>
       </c>
       <c r="D892" t="n">
-        <v>3643183</v>
+        <v>3644125</v>
       </c>
       <c r="E892" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>10324</v>
+        <v>10329</v>
       </c>
       <c r="D896" t="n">
-        <v>12673408</v>
+        <v>12680908</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43486,10 +43486,10 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>3461</v>
+        <v>3463</v>
       </c>
       <c r="D899" t="n">
-        <v>5064242</v>
+        <v>5067142</v>
       </c>
       <c r="E899" t="inlineStr">
         <is>
@@ -43678,10 +43678,10 @@
         </is>
       </c>
       <c r="C903" t="n">
-        <v>47854</v>
+        <v>47893</v>
       </c>
       <c r="D903" t="n">
-        <v>59972016</v>
+        <v>60010165</v>
       </c>
       <c r="E903" t="inlineStr">
         <is>
@@ -43918,10 +43918,10 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>22176</v>
+        <v>22186</v>
       </c>
       <c r="D908" t="n">
-        <v>32515331</v>
+        <v>32529229</v>
       </c>
       <c r="E908" t="inlineStr">
         <is>
@@ -44014,10 +44014,10 @@
         </is>
       </c>
       <c r="C910" t="n">
-        <v>6458</v>
+        <v>6460</v>
       </c>
       <c r="D910" t="n">
-        <v>9304119</v>
+        <v>9307119</v>
       </c>
       <c r="E910" t="inlineStr">
         <is>
@@ -44158,10 +44158,10 @@
         </is>
       </c>
       <c r="C913" t="n">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c r="D913" t="n">
-        <v>1537733</v>
+        <v>1541903</v>
       </c>
       <c r="E913" t="inlineStr">
         <is>
@@ -44206,10 +44206,10 @@
         </is>
       </c>
       <c r="C914" t="n">
-        <v>22361</v>
+        <v>22372</v>
       </c>
       <c r="D914" t="n">
-        <v>27782379</v>
+        <v>27792849</v>
       </c>
       <c r="E914" t="inlineStr">
         <is>
@@ -44302,10 +44302,10 @@
         </is>
       </c>
       <c r="C916" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D916" t="n">
-        <v>171923</v>
+        <v>173423</v>
       </c>
       <c r="E916" t="inlineStr">
         <is>
@@ -44350,10 +44350,10 @@
         </is>
       </c>
       <c r="C917" t="n">
-        <v>10174</v>
+        <v>10186</v>
       </c>
       <c r="D917" t="n">
-        <v>14904582</v>
+        <v>14921647</v>
       </c>
       <c r="E917" t="inlineStr">
         <is>
@@ -44446,10 +44446,10 @@
         </is>
       </c>
       <c r="C919" t="n">
-        <v>2439</v>
+        <v>2445</v>
       </c>
       <c r="D919" t="n">
-        <v>3495305</v>
+        <v>3504305</v>
       </c>
       <c r="E919" t="inlineStr">
         <is>
@@ -44542,10 +44542,10 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D921" t="n">
-        <v>895960</v>
+        <v>897460</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
@@ -44638,10 +44638,10 @@
         </is>
       </c>
       <c r="C923" t="n">
-        <v>7469</v>
+        <v>7477</v>
       </c>
       <c r="D923" t="n">
-        <v>9353094</v>
+        <v>9365094</v>
       </c>
       <c r="E923" t="inlineStr">
         <is>
@@ -44734,10 +44734,10 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D925" t="n">
-        <v>8300</v>
+        <v>9100</v>
       </c>
       <c r="E925" t="inlineStr">
         <is>
@@ -44878,10 +44878,10 @@
         </is>
       </c>
       <c r="C928" t="n">
-        <v>3174</v>
+        <v>3175</v>
       </c>
       <c r="D928" t="n">
-        <v>4674959</v>
+        <v>4676459</v>
       </c>
       <c r="E928" t="inlineStr">
         <is>
@@ -44926,10 +44926,10 @@
         </is>
       </c>
       <c r="C929" t="n">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D929" t="n">
-        <v>991293</v>
+        <v>992793</v>
       </c>
       <c r="E929" t="inlineStr">
         <is>
@@ -44974,10 +44974,10 @@
         </is>
       </c>
       <c r="C930" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D930" t="n">
-        <v>246580</v>
+        <v>248080</v>
       </c>
       <c r="E930" t="inlineStr">
         <is>
@@ -45070,10 +45070,10 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>13756</v>
+        <v>13762</v>
       </c>
       <c r="D932" t="n">
-        <v>17082316</v>
+        <v>17089473</v>
       </c>
       <c r="E932" t="inlineStr">
         <is>
@@ -45262,10 +45262,10 @@
         </is>
       </c>
       <c r="C936" t="n">
-        <v>5491</v>
+        <v>5498</v>
       </c>
       <c r="D936" t="n">
-        <v>8018793</v>
+        <v>8029293</v>
       </c>
       <c r="E936" t="inlineStr">
         <is>
@@ -45598,10 +45598,10 @@
         </is>
       </c>
       <c r="C943" t="n">
-        <v>20299</v>
+        <v>20308</v>
       </c>
       <c r="D943" t="n">
-        <v>25277678</v>
+        <v>25286812</v>
       </c>
       <c r="E943" t="inlineStr">
         <is>
@@ -45838,10 +45838,10 @@
         </is>
       </c>
       <c r="C948" t="n">
-        <v>10411</v>
+        <v>10418</v>
       </c>
       <c r="D948" t="n">
-        <v>15210715</v>
+        <v>15220215</v>
       </c>
       <c r="E948" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>2203</v>
+        <v>2205</v>
       </c>
       <c r="D950" t="n">
-        <v>3180378</v>
+        <v>3183378</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46030,10 +46030,10 @@
         </is>
       </c>
       <c r="C952" t="n">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D952" t="n">
-        <v>725394</v>
+        <v>728394</v>
       </c>
       <c r="E952" t="inlineStr">
         <is>
@@ -46078,10 +46078,10 @@
         </is>
       </c>
       <c r="C953" t="n">
-        <v>9095</v>
+        <v>9101</v>
       </c>
       <c r="D953" t="n">
-        <v>11317900</v>
+        <v>11326212</v>
       </c>
       <c r="E953" t="inlineStr">
         <is>
@@ -46318,10 +46318,10 @@
         </is>
       </c>
       <c r="C958" t="n">
-        <v>3331</v>
+        <v>3332</v>
       </c>
       <c r="D958" t="n">
-        <v>4861178</v>
+        <v>4862678</v>
       </c>
       <c r="E958" t="inlineStr">
         <is>
@@ -46366,10 +46366,10 @@
         </is>
       </c>
       <c r="C959" t="n">
-        <v>1581</v>
+        <v>1585</v>
       </c>
       <c r="D959" t="n">
-        <v>2277776</v>
+        <v>2283776</v>
       </c>
       <c r="E959" t="inlineStr">
         <is>
@@ -46558,10 +46558,10 @@
         </is>
       </c>
       <c r="C963" t="n">
-        <v>72917</v>
+        <v>72983</v>
       </c>
       <c r="D963" t="n">
-        <v>93687614</v>
+        <v>93761576</v>
       </c>
       <c r="E963" t="inlineStr">
         <is>
@@ -46894,10 +46894,10 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>27243</v>
+        <v>27282</v>
       </c>
       <c r="D970" t="n">
-        <v>39926047</v>
+        <v>39981444</v>
       </c>
       <c r="E970" t="inlineStr">
         <is>
@@ -46990,10 +46990,10 @@
         </is>
       </c>
       <c r="C972" t="n">
-        <v>19354</v>
+        <v>19366</v>
       </c>
       <c r="D972" t="n">
-        <v>28072437</v>
+        <v>28090025</v>
       </c>
       <c r="E972" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="D974" t="n">
-        <v>740416</v>
+        <v>746225</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47134,10 +47134,10 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="D975" t="n">
-        <v>1450004</v>
+        <v>1453004</v>
       </c>
       <c r="E975" t="inlineStr">
         <is>
@@ -47182,10 +47182,10 @@
         </is>
       </c>
       <c r="C976" t="n">
-        <v>89901</v>
+        <v>89998</v>
       </c>
       <c r="D976" t="n">
-        <v>112731234</v>
+        <v>112831607</v>
       </c>
       <c r="E976" t="inlineStr">
         <is>
@@ -47518,10 +47518,10 @@
         </is>
       </c>
       <c r="C983" t="n">
-        <v>35733</v>
+        <v>35787</v>
       </c>
       <c r="D983" t="n">
-        <v>52380049</v>
+        <v>52460975</v>
       </c>
       <c r="E983" t="inlineStr">
         <is>
@@ -47662,10 +47662,10 @@
         </is>
       </c>
       <c r="C986" t="n">
-        <v>27199</v>
+        <v>27246</v>
       </c>
       <c r="D986" t="n">
-        <v>39462444</v>
+        <v>39530441</v>
       </c>
       <c r="E986" t="inlineStr">
         <is>
@@ -47710,10 +47710,10 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D987" t="n">
-        <v>907481</v>
+        <v>908981</v>
       </c>
       <c r="E987" t="inlineStr">
         <is>
@@ -47806,10 +47806,10 @@
         </is>
       </c>
       <c r="C989" t="n">
-        <v>2350</v>
+        <v>2355</v>
       </c>
       <c r="D989" t="n">
-        <v>3304445</v>
+        <v>3311945</v>
       </c>
       <c r="E989" t="inlineStr">
         <is>
@@ -47854,10 +47854,10 @@
         </is>
       </c>
       <c r="C990" t="n">
-        <v>11456</v>
+        <v>11464</v>
       </c>
       <c r="D990" t="n">
-        <v>14909362</v>
+        <v>14921228</v>
       </c>
       <c r="E990" t="inlineStr">
         <is>
@@ -48094,10 +48094,10 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>3660</v>
+        <v>3664</v>
       </c>
       <c r="D995" t="n">
-        <v>5348274</v>
+        <v>5354274</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
@@ -48142,10 +48142,10 @@
         </is>
       </c>
       <c r="C996" t="n">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D996" t="n">
-        <v>1724022</v>
+        <v>1725522</v>
       </c>
       <c r="E996" t="inlineStr">
         <is>
@@ -48382,10 +48382,10 @@
         </is>
       </c>
       <c r="C1001" t="n">
-        <v>58754</v>
+        <v>58793</v>
       </c>
       <c r="D1001" t="n">
-        <v>73408688</v>
+        <v>73458215</v>
       </c>
       <c r="E1001" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D1005" t="n">
-        <v>272017</v>
+        <v>273517</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48622,10 +48622,10 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>19142</v>
+        <v>19146</v>
       </c>
       <c r="D1006" t="n">
-        <v>28033404</v>
+        <v>28039404</v>
       </c>
       <c r="E1006" t="inlineStr">
         <is>
@@ -48718,10 +48718,10 @@
         </is>
       </c>
       <c r="C1008" t="n">
-        <v>13339</v>
+        <v>13348</v>
       </c>
       <c r="D1008" t="n">
-        <v>19292840</v>
+        <v>19305612</v>
       </c>
       <c r="E1008" t="inlineStr">
         <is>
@@ -48862,10 +48862,10 @@
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D1011" t="n">
-        <v>1186648</v>
+        <v>1188148</v>
       </c>
       <c r="E1011" t="inlineStr">
         <is>
@@ -48910,10 +48910,10 @@
         </is>
       </c>
       <c r="C1012" t="n">
-        <v>29921</v>
+        <v>29943</v>
       </c>
       <c r="D1012" t="n">
-        <v>37195342</v>
+        <v>37221536</v>
       </c>
       <c r="E1012" t="inlineStr">
         <is>
@@ -49150,10 +49150,10 @@
         </is>
       </c>
       <c r="C1017" t="n">
-        <v>11089</v>
+        <v>11092</v>
       </c>
       <c r="D1017" t="n">
-        <v>16235575</v>
+        <v>16240075</v>
       </c>
       <c r="E1017" t="inlineStr">
         <is>
@@ -49246,10 +49246,10 @@
         </is>
       </c>
       <c r="C1019" t="n">
-        <v>6648</v>
+        <v>6656</v>
       </c>
       <c r="D1019" t="n">
-        <v>9634212</v>
+        <v>9645526</v>
       </c>
       <c r="E1019" t="inlineStr">
         <is>
@@ -49342,10 +49342,10 @@
         </is>
       </c>
       <c r="C1021" t="n">
-        <v>691</v>
+        <v>698</v>
       </c>
       <c r="D1021" t="n">
-        <v>957558</v>
+        <v>966741</v>
       </c>
       <c r="E1021" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-11-09 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17915</v>
+        <v>17931</v>
       </c>
       <c r="D2" t="n">
-        <v>22440383</v>
+        <v>22455118</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6646</v>
+        <v>6648</v>
       </c>
       <c r="D6" t="n">
-        <v>9728980</v>
+        <v>9731980</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3643</v>
+        <v>3648</v>
       </c>
       <c r="D8" t="n">
-        <v>5277872</v>
+        <v>5285372</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D11" t="n">
-        <v>691789</v>
+        <v>693389</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12063</v>
+        <v>12070</v>
       </c>
       <c r="D12" t="n">
-        <v>15188050</v>
+        <v>15195206</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -958,10 +958,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
-        <v>16952</v>
+        <v>18452</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15538</v>
+        <v>15548</v>
       </c>
       <c r="D22" t="n">
-        <v>18971763</v>
+        <v>18983614</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1582,10 +1582,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5263</v>
+        <v>5265</v>
       </c>
       <c r="D26" t="n">
-        <v>7685748</v>
+        <v>7688748</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D28" t="n">
-        <v>2705651</v>
+        <v>2707151</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D31" t="n">
-        <v>627587</v>
+        <v>629087</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6995</v>
+        <v>6998</v>
       </c>
       <c r="D32" t="n">
-        <v>9261374</v>
+        <v>9263795</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>23864</v>
+        <v>23888</v>
       </c>
       <c r="D41" t="n">
-        <v>29249294</v>
+        <v>29278355</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>8284</v>
+        <v>8289</v>
       </c>
       <c r="D47" t="n">
-        <v>12165219</v>
+        <v>12172719</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4176</v>
+        <v>4178</v>
       </c>
       <c r="D49" t="n">
-        <v>6041978</v>
+        <v>6044978</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="D52" t="n">
-        <v>1109410</v>
+        <v>1113910</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8793</v>
+        <v>8796</v>
       </c>
       <c r="D53" t="n">
-        <v>11166195</v>
+        <v>11169360</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2950</v>
+        <v>2953</v>
       </c>
       <c r="D57" t="n">
-        <v>4288574</v>
+        <v>4293074</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D59" t="n">
-        <v>1563565</v>
+        <v>1566565</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3310,10 +3310,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>40364</v>
+        <v>40424</v>
       </c>
       <c r="D62" t="n">
-        <v>51852844</v>
+        <v>51921535</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>14286</v>
+        <v>14298</v>
       </c>
       <c r="D67" t="n">
-        <v>20939169</v>
+        <v>20955069</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3646,10 +3646,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5831</v>
+        <v>5832</v>
       </c>
       <c r="D69" t="n">
-        <v>8427746</v>
+        <v>8429246</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D74" t="n">
-        <v>606956</v>
+        <v>611456</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3982,10 +3982,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>50829</v>
+        <v>50887</v>
       </c>
       <c r="D76" t="n">
-        <v>64725097</v>
+        <v>64785307</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>19638</v>
+        <v>19646</v>
       </c>
       <c r="D80" t="n">
-        <v>28735995</v>
+        <v>28745554</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>10469</v>
+        <v>10486</v>
       </c>
       <c r="D82" t="n">
-        <v>15126801</v>
+        <v>15149061</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c r="D86" t="n">
-        <v>1531035</v>
+        <v>1536931</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4510,10 +4510,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>26955</v>
+        <v>26966</v>
       </c>
       <c r="D87" t="n">
-        <v>33874925</v>
+        <v>33888864</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>9299</v>
+        <v>9307</v>
       </c>
       <c r="D91" t="n">
-        <v>13643564</v>
+        <v>13655564</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5403</v>
+        <v>5408</v>
       </c>
       <c r="D93" t="n">
-        <v>7800866</v>
+        <v>7808366</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>23981</v>
+        <v>24007</v>
       </c>
       <c r="D96" t="n">
-        <v>29951618</v>
+        <v>29980555</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -5134,10 +5134,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>9848</v>
+        <v>9852</v>
       </c>
       <c r="D100" t="n">
-        <v>14411178</v>
+        <v>14417178</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D106" t="n">
-        <v>820400</v>
+        <v>823400</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5470,10 +5470,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>93078</v>
+        <v>93175</v>
       </c>
       <c r="D107" t="n">
-        <v>118919543</v>
+        <v>119031783</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>33276</v>
+        <v>33303</v>
       </c>
       <c r="D114" t="n">
-        <v>48793636</v>
+        <v>48834058</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D115" t="n">
-        <v>40500</v>
+        <v>42000</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -5902,10 +5902,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>23805</v>
+        <v>23840</v>
       </c>
       <c r="D116" t="n">
-        <v>34352764</v>
+        <v>34401962</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>2630</v>
+        <v>2639</v>
       </c>
       <c r="D123" t="n">
-        <v>3677285</v>
+        <v>3688374</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>30845</v>
+        <v>30879</v>
       </c>
       <c r="D124" t="n">
-        <v>40608350</v>
+        <v>40648596</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>10945</v>
+        <v>10961</v>
       </c>
       <c r="D128" t="n">
-        <v>16049038</v>
+        <v>16073038</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>3676</v>
+        <v>3684</v>
       </c>
       <c r="D130" t="n">
-        <v>5350604</v>
+        <v>5362604</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6622,10 +6622,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D131" t="n">
-        <v>339662</v>
+        <v>342662</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -6718,10 +6718,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D133" t="n">
-        <v>646747</v>
+        <v>649747</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>17164</v>
+        <v>17181</v>
       </c>
       <c r="D134" t="n">
-        <v>21229067</v>
+        <v>21247089</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -6958,10 +6958,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>8320</v>
+        <v>8326</v>
       </c>
       <c r="D138" t="n">
-        <v>12165326</v>
+        <v>12174098</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -7054,10 +7054,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2481</v>
+        <v>2486</v>
       </c>
       <c r="D140" t="n">
-        <v>3543891</v>
+        <v>3551391</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D142" t="n">
-        <v>457739</v>
+        <v>459213</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="D144" t="n">
-        <v>736714</v>
+        <v>742336</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7294,10 +7294,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>14893</v>
+        <v>14901</v>
       </c>
       <c r="D145" t="n">
-        <v>18499623</v>
+        <v>18508062</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>6637</v>
+        <v>6640</v>
       </c>
       <c r="D149" t="n">
-        <v>9720428</v>
+        <v>9723814</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>6466</v>
+        <v>6468</v>
       </c>
       <c r="D155" t="n">
-        <v>7899715</v>
+        <v>7902015</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>2146</v>
+        <v>2147</v>
       </c>
       <c r="D158" t="n">
-        <v>3147279</v>
+        <v>3148779</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>8097</v>
+        <v>8101</v>
       </c>
       <c r="D163" t="n">
-        <v>9969433</v>
+        <v>9974160</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>3071</v>
+        <v>3077</v>
       </c>
       <c r="D166" t="n">
-        <v>4504740</v>
+        <v>4513740</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8350,10 +8350,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D167" t="n">
-        <v>2168730</v>
+        <v>2170230</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -8494,10 +8494,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D170" t="n">
-        <v>248722</v>
+        <v>250222</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -8542,10 +8542,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>6125</v>
+        <v>6132</v>
       </c>
       <c r="D171" t="n">
-        <v>7641632</v>
+        <v>7648187</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D178" t="n">
-        <v>1078697</v>
+        <v>1081697</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -9022,10 +9022,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>17457</v>
+        <v>17470</v>
       </c>
       <c r="D181" t="n">
-        <v>21830426</v>
+        <v>21845241</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -9262,10 +9262,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>6799</v>
+        <v>6806</v>
       </c>
       <c r="D186" t="n">
-        <v>9930545</v>
+        <v>9940519</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -9358,10 +9358,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>2454</v>
+        <v>2459</v>
       </c>
       <c r="D188" t="n">
-        <v>3529538</v>
+        <v>3537038</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -9550,10 +9550,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>3323</v>
+        <v>3328</v>
       </c>
       <c r="D192" t="n">
-        <v>4152724</v>
+        <v>4156895</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>10089</v>
+        <v>10104</v>
       </c>
       <c r="D200" t="n">
-        <v>12562168</v>
+        <v>12581380</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -10126,10 +10126,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>3678</v>
+        <v>3682</v>
       </c>
       <c r="D204" t="n">
-        <v>5398547</v>
+        <v>5403810</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1790</v>
+        <v>1792</v>
       </c>
       <c r="D206" t="n">
-        <v>2572843</v>
+        <v>2575843</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D207" t="n">
-        <v>287843</v>
+        <v>289343</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D209" t="n">
-        <v>385682</v>
+        <v>387182</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>18553</v>
+        <v>18571</v>
       </c>
       <c r="D210" t="n">
-        <v>23041603</v>
+        <v>23059572</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>8113</v>
+        <v>8116</v>
       </c>
       <c r="D214" t="n">
-        <v>11909908</v>
+        <v>11914408</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="D215" t="n">
-        <v>1918762</v>
+        <v>1921762</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10702,10 +10702,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D216" t="n">
-        <v>411363</v>
+        <v>412863</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>28076</v>
+        <v>28097</v>
       </c>
       <c r="D218" t="n">
-        <v>35184034</v>
+        <v>35203473</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>11050</v>
+        <v>11053</v>
       </c>
       <c r="D222" t="n">
-        <v>16127494</v>
+        <v>16131994</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2869</v>
+        <v>2873</v>
       </c>
       <c r="D224" t="n">
-        <v>4128059</v>
+        <v>4134059</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11230,10 +11230,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="D227" t="n">
-        <v>1040371</v>
+        <v>1043178</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>31444</v>
+        <v>31479</v>
       </c>
       <c r="D228" t="n">
-        <v>39448627</v>
+        <v>39489835</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>15903</v>
+        <v>15910</v>
       </c>
       <c r="D233" t="n">
-        <v>23324234</v>
+        <v>23333772</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D234" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3001</v>
+        <v>3004</v>
       </c>
       <c r="D235" t="n">
-        <v>4304861</v>
+        <v>4309361</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="D238" t="n">
-        <v>1377650</v>
+        <v>1381628</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11806,10 +11806,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>26428</v>
+        <v>26444</v>
       </c>
       <c r="D239" t="n">
-        <v>33190394</v>
+        <v>33210234</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D243" t="n">
-        <v>339775</v>
+        <v>341275</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -12094,10 +12094,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>11810</v>
+        <v>11815</v>
       </c>
       <c r="D245" t="n">
-        <v>17297042</v>
+        <v>17304542</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D250" t="n">
-        <v>814621</v>
+        <v>816121</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>8482</v>
+        <v>8494</v>
       </c>
       <c r="D251" t="n">
-        <v>10592598</v>
+        <v>10607602</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>10850</v>
+        <v>10861</v>
       </c>
       <c r="D261" t="n">
-        <v>13846050</v>
+        <v>13857556</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>4529</v>
+        <v>4535</v>
       </c>
       <c r="D265" t="n">
-        <v>6643195</v>
+        <v>6652195</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>2425</v>
+        <v>2428</v>
       </c>
       <c r="D267" t="n">
-        <v>3509876</v>
+        <v>3514376</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13198,10 +13198,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D268" t="n">
-        <v>151487</v>
+        <v>152890</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>6112</v>
+        <v>6117</v>
       </c>
       <c r="D270" t="n">
-        <v>7512678</v>
+        <v>7516200</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>20932</v>
+        <v>20960</v>
       </c>
       <c r="D279" t="n">
-        <v>26326659</v>
+        <v>26356883</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>8621</v>
+        <v>8630</v>
       </c>
       <c r="D283" t="n">
-        <v>12619372</v>
+        <v>12632872</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14158,10 +14158,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D288" t="n">
-        <v>868347</v>
+        <v>869847</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>18090</v>
+        <v>18100</v>
       </c>
       <c r="D290" t="n">
-        <v>22352857</v>
+        <v>22362294</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>7741</v>
+        <v>7748</v>
       </c>
       <c r="D295" t="n">
-        <v>11349799</v>
+        <v>11360210</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>3684</v>
+        <v>3688</v>
       </c>
       <c r="D296" t="n">
-        <v>5332467</v>
+        <v>5336467</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D299" t="n">
-        <v>598138</v>
+        <v>599638</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>10177</v>
+        <v>10181</v>
       </c>
       <c r="D300" t="n">
-        <v>12727642</v>
+        <v>12731893</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>4142</v>
+        <v>4144</v>
       </c>
       <c r="D304" t="n">
-        <v>6059836</v>
+        <v>6062836</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="D305" t="n">
-        <v>2023558</v>
+        <v>2028058</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D309" t="n">
-        <v>364047</v>
+        <v>365547</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>10159</v>
+        <v>10166</v>
       </c>
       <c r="D310" t="n">
-        <v>13228984</v>
+        <v>13239484</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>4092</v>
+        <v>4093</v>
       </c>
       <c r="D314" t="n">
-        <v>5980732</v>
+        <v>5982232</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>2660</v>
+        <v>2665</v>
       </c>
       <c r="D315" t="n">
-        <v>3877064</v>
+        <v>3884564</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>12315</v>
+        <v>12328</v>
       </c>
       <c r="D318" t="n">
-        <v>16125985</v>
+        <v>16139024</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>4186</v>
+        <v>4191</v>
       </c>
       <c r="D322" t="n">
-        <v>6140294</v>
+        <v>6148292</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>3017</v>
+        <v>3018</v>
       </c>
       <c r="D324" t="n">
-        <v>4377867</v>
+        <v>4379367</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -15934,10 +15934,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D325" t="n">
-        <v>401756</v>
+        <v>404716</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -15982,10 +15982,10 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D326" t="n">
-        <v>306921</v>
+        <v>308321</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>7346</v>
+        <v>7348</v>
       </c>
       <c r="D327" t="n">
-        <v>9062675</v>
+        <v>9065131</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>2460</v>
+        <v>2463</v>
       </c>
       <c r="D332" t="n">
-        <v>3607867</v>
+        <v>3611287</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16366,10 +16366,10 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D334" t="n">
-        <v>1250235</v>
+        <v>1251735</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>8233</v>
+        <v>8235</v>
       </c>
       <c r="D337" t="n">
-        <v>10259570</v>
+        <v>10260182</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>3384</v>
+        <v>3387</v>
       </c>
       <c r="D342" t="n">
-        <v>4942617</v>
+        <v>4947117</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>1419</v>
+        <v>1421</v>
       </c>
       <c r="D343" t="n">
-        <v>2037544</v>
+        <v>2040544</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>35735</v>
+        <v>35778</v>
       </c>
       <c r="D347" t="n">
-        <v>44743212</v>
+        <v>44792355</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>17827</v>
+        <v>17835</v>
       </c>
       <c r="D353" t="n">
-        <v>26049183</v>
+        <v>26061142</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>8841</v>
+        <v>8844</v>
       </c>
       <c r="D356" t="n">
-        <v>12732036</v>
+        <v>12736536</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17518,10 +17518,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D358" t="n">
-        <v>1505096</v>
+        <v>1508096</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>4278</v>
+        <v>4279</v>
       </c>
       <c r="D359" t="n">
-        <v>5292960</v>
+        <v>5294460</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>21140</v>
+        <v>21161</v>
       </c>
       <c r="D367" t="n">
-        <v>26249391</v>
+        <v>26273570</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>10601</v>
+        <v>10608</v>
       </c>
       <c r="D371" t="n">
-        <v>15539075</v>
+        <v>15549575</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>5183</v>
+        <v>5190</v>
       </c>
       <c r="D373" t="n">
-        <v>7506242</v>
+        <v>7516742</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18334,10 +18334,10 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D375" t="n">
-        <v>624281</v>
+        <v>627281</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>15483</v>
+        <v>15495</v>
       </c>
       <c r="D376" t="n">
-        <v>19295114</v>
+        <v>19305303</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>6983</v>
+        <v>6985</v>
       </c>
       <c r="D380" t="n">
-        <v>10222595</v>
+        <v>10225595</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>2812</v>
+        <v>2816</v>
       </c>
       <c r="D382" t="n">
-        <v>4035632</v>
+        <v>4041632</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D383" t="n">
-        <v>1215176</v>
+        <v>1216676</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>19680</v>
+        <v>19700</v>
       </c>
       <c r="D385" t="n">
-        <v>24393851</v>
+        <v>24414653</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -19006,10 +19006,10 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>7627</v>
+        <v>7631</v>
       </c>
       <c r="D389" t="n">
-        <v>11200533</v>
+        <v>11206533</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>3062</v>
+        <v>3066</v>
       </c>
       <c r="D391" t="n">
-        <v>4458060</v>
+        <v>4464060</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D394" t="n">
-        <v>730479</v>
+        <v>731979</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>4443</v>
+        <v>4448</v>
       </c>
       <c r="D395" t="n">
-        <v>5538996</v>
+        <v>5543957</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>24188</v>
+        <v>24209</v>
       </c>
       <c r="D402" t="n">
-        <v>29823354</v>
+        <v>29843487</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>9947</v>
+        <v>9950</v>
       </c>
       <c r="D405" t="n">
-        <v>14631439</v>
+        <v>14635939</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>6698</v>
+        <v>6701</v>
       </c>
       <c r="D407" t="n">
-        <v>9736351</v>
+        <v>9740851</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D409" t="n">
-        <v>620182</v>
+        <v>623932</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>12140</v>
+        <v>12149</v>
       </c>
       <c r="D410" t="n">
-        <v>14874294</v>
+        <v>14881741</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>5651</v>
+        <v>5657</v>
       </c>
       <c r="D415" t="n">
-        <v>8252500</v>
+        <v>8260371</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="D417" t="n">
-        <v>2894189</v>
+        <v>2895689</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D419" t="n">
-        <v>344446</v>
+        <v>346560</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>37814</v>
+        <v>37839</v>
       </c>
       <c r="D420" t="n">
-        <v>51291641</v>
+        <v>51324684</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>9361</v>
+        <v>9383</v>
       </c>
       <c r="D424" t="n">
-        <v>13751758</v>
+        <v>13784762</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>8722</v>
+        <v>8725</v>
       </c>
       <c r="D426" t="n">
-        <v>12655426</v>
+        <v>12659926</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="D428" t="n">
-        <v>841550</v>
+        <v>845430</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20926,10 +20926,10 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D429" t="n">
-        <v>825060</v>
+        <v>826560</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>16485</v>
+        <v>16517</v>
       </c>
       <c r="D430" t="n">
-        <v>30791225</v>
+        <v>30882945</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>3809</v>
+        <v>3831</v>
       </c>
       <c r="D433" t="n">
-        <v>7627695</v>
+        <v>7680181</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>5421</v>
+        <v>5437</v>
       </c>
       <c r="D435" t="n">
-        <v>10978084</v>
+        <v>11023520</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D437" t="n">
-        <v>499340</v>
+        <v>507340</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21358,10 +21358,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D438" t="n">
-        <v>621150</v>
+        <v>626650</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>12064</v>
+        <v>12073</v>
       </c>
       <c r="D440" t="n">
-        <v>14905588</v>
+        <v>14918717</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>4117</v>
+        <v>4123</v>
       </c>
       <c r="D443" t="n">
-        <v>6037738</v>
+        <v>6046107</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21838,10 +21838,10 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>69878</v>
+        <v>69938</v>
       </c>
       <c r="D448" t="n">
-        <v>86410132</v>
+        <v>86471835</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -22030,10 +22030,10 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>27182</v>
+        <v>27202</v>
       </c>
       <c r="D452" t="n">
-        <v>39792478</v>
+        <v>39820781</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>14909</v>
+        <v>14926</v>
       </c>
       <c r="D454" t="n">
-        <v>21632184</v>
+        <v>21656040</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>1375</v>
+        <v>1379</v>
       </c>
       <c r="D458" t="n">
-        <v>1942640</v>
+        <v>1948640</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>21171</v>
+        <v>21193</v>
       </c>
       <c r="D460" t="n">
-        <v>26802484</v>
+        <v>26827407</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>8320</v>
+        <v>8328</v>
       </c>
       <c r="D464" t="n">
-        <v>12197916</v>
+        <v>12209916</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>5750</v>
+        <v>5757</v>
       </c>
       <c r="D466" t="n">
-        <v>8346420</v>
+        <v>8356920</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D468" t="n">
-        <v>512510</v>
+        <v>514010</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>34921</v>
+        <v>34952</v>
       </c>
       <c r="D469" t="n">
-        <v>42533380</v>
+        <v>42564306</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23038,10 +23038,10 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>12192</v>
+        <v>12200</v>
       </c>
       <c r="D473" t="n">
-        <v>17822048</v>
+        <v>17834048</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -23134,10 +23134,10 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>5328</v>
+        <v>5330</v>
       </c>
       <c r="D475" t="n">
-        <v>7723145</v>
+        <v>7726145</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D477" t="n">
-        <v>675266</v>
+        <v>676766</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23278,10 +23278,10 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>15616</v>
+        <v>15634</v>
       </c>
       <c r="D478" t="n">
-        <v>19003646</v>
+        <v>19024145</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>4701</v>
+        <v>4705</v>
       </c>
       <c r="D483" t="n">
-        <v>6903543</v>
+        <v>6909543</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>2307</v>
+        <v>2310</v>
       </c>
       <c r="D485" t="n">
-        <v>3322793</v>
+        <v>3327293</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D487" t="n">
-        <v>561528</v>
+        <v>562950</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>43114</v>
+        <v>43178</v>
       </c>
       <c r="D488" t="n">
-        <v>56382846</v>
+        <v>56465289</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -23950,10 +23950,10 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>15022</v>
+        <v>15049</v>
       </c>
       <c r="D492" t="n">
-        <v>22075974</v>
+        <v>22116474</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>14569</v>
+        <v>14605</v>
       </c>
       <c r="D494" t="n">
-        <v>21268478</v>
+        <v>21321081</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24190,10 +24190,10 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>78462</v>
+        <v>78607</v>
       </c>
       <c r="D497" t="n">
-        <v>103926571</v>
+        <v>104096529</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>27088</v>
+        <v>27140</v>
       </c>
       <c r="D502" t="n">
-        <v>39724334</v>
+        <v>39800419</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24526,10 +24526,10 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>28452</v>
+        <v>28501</v>
       </c>
       <c r="D504" t="n">
-        <v>41334766</v>
+        <v>41407398</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="D507" t="n">
-        <v>1227925</v>
+        <v>1233014</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>187899</v>
+        <v>188195</v>
       </c>
       <c r="D508" t="n">
-        <v>245964034</v>
+        <v>246314825</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="D513" t="n">
-        <v>837149</v>
+        <v>844649</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>96900</v>
+        <v>97117</v>
       </c>
       <c r="D515" t="n">
-        <v>142283793</v>
+        <v>142600856</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D516" t="n">
-        <v>525699</v>
+        <v>527199</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25198,10 +25198,10 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>74144</v>
+        <v>74301</v>
       </c>
       <c r="D518" t="n">
-        <v>107738267</v>
+        <v>107970139</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="D520" t="n">
-        <v>1683009</v>
+        <v>1686009</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>3914</v>
+        <v>3934</v>
       </c>
       <c r="D522" t="n">
-        <v>5520612</v>
+        <v>5547158</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25534,10 +25534,10 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>49254</v>
+        <v>49313</v>
       </c>
       <c r="D525" t="n">
-        <v>64267689</v>
+        <v>64334161</v>
       </c>
       <c r="E525" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D527" t="n">
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>16890</v>
+        <v>16909</v>
       </c>
       <c r="D530" t="n">
-        <v>24799860</v>
+        <v>24827510</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>15460</v>
+        <v>15494</v>
       </c>
       <c r="D532" t="n">
-        <v>22406231</v>
+        <v>22451548</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="D535" t="n">
-        <v>635985</v>
+        <v>640485</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>86172</v>
+        <v>86393</v>
       </c>
       <c r="D537" t="n">
-        <v>116525916</v>
+        <v>116801557</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>26662</v>
+        <v>26701</v>
       </c>
       <c r="D541" t="n">
-        <v>39301198</v>
+        <v>39359219</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26398,10 +26398,10 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>31291</v>
+        <v>31355</v>
       </c>
       <c r="D543" t="n">
-        <v>45771610</v>
+        <v>45864678</v>
       </c>
       <c r="E543" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>1146</v>
+        <v>1151</v>
       </c>
       <c r="D547" t="n">
-        <v>1619637</v>
+        <v>1627137</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>68073</v>
+        <v>68178</v>
       </c>
       <c r="D548" t="n">
-        <v>90314449</v>
+        <v>90449502</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>20222</v>
+        <v>20235</v>
       </c>
       <c r="D553" t="n">
-        <v>29699207</v>
+        <v>29718707</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>23026</v>
+        <v>23064</v>
       </c>
       <c r="D555" t="n">
-        <v>33475213</v>
+        <v>33526413</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>838</v>
+        <v>847</v>
       </c>
       <c r="D557" t="n">
-        <v>1180569</v>
+        <v>1193850</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27118,10 +27118,10 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>51888</v>
+        <v>51977</v>
       </c>
       <c r="D558" t="n">
-        <v>69362514</v>
+        <v>69474315</v>
       </c>
       <c r="E558" t="inlineStr">
         <is>
@@ -27310,10 +27310,10 @@
         </is>
       </c>
       <c r="C562" t="n">
-        <v>15804</v>
+        <v>15814</v>
       </c>
       <c r="D562" t="n">
-        <v>23278604</v>
+        <v>23291891</v>
       </c>
       <c r="E562" t="inlineStr">
         <is>
@@ -27406,10 +27406,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>18068</v>
+        <v>18110</v>
       </c>
       <c r="D564" t="n">
-        <v>26236254</v>
+        <v>26292617</v>
       </c>
       <c r="E564" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D566" t="n">
-        <v>543098</v>
+        <v>546098</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>48770</v>
+        <v>48823</v>
       </c>
       <c r="D567" t="n">
-        <v>63359876</v>
+        <v>63424986</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D570" t="n">
-        <v>211248</v>
+        <v>212748</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27742,10 +27742,10 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>17828</v>
+        <v>17844</v>
       </c>
       <c r="D571" t="n">
-        <v>26139152</v>
+        <v>26162144</v>
       </c>
       <c r="E571" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>15455</v>
+        <v>15467</v>
       </c>
       <c r="D573" t="n">
-        <v>22357195</v>
+        <v>22374553</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27982,10 +27982,10 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D576" t="n">
-        <v>634238</v>
+        <v>635738</v>
       </c>
       <c r="E576" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>49504</v>
+        <v>49534</v>
       </c>
       <c r="D577" t="n">
-        <v>65998563</v>
+        <v>66040199</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D578" t="n">
-        <v>45036</v>
+        <v>45310</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>15269</v>
+        <v>15278</v>
       </c>
       <c r="D583" t="n">
-        <v>22376939</v>
+        <v>22390110</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>4146</v>
+        <v>4149</v>
       </c>
       <c r="D584" t="n">
-        <v>5983326</v>
+        <v>5987826</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D589" t="n">
-        <v>703366</v>
+        <v>704259</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>19758</v>
+        <v>19793</v>
       </c>
       <c r="D590" t="n">
-        <v>26121567</v>
+        <v>26168853</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D593" t="n">
-        <v>82406</v>
+        <v>83906</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>8181</v>
+        <v>8193</v>
       </c>
       <c r="D594" t="n">
-        <v>11901340</v>
+        <v>11919200</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>5804</v>
+        <v>5815</v>
       </c>
       <c r="D596" t="n">
-        <v>8353327</v>
+        <v>8369992</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>28701</v>
+        <v>28736</v>
       </c>
       <c r="D601" t="n">
-        <v>57766848</v>
+        <v>57862448</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>2860</v>
+        <v>2867</v>
       </c>
       <c r="D602" t="n">
-        <v>5681227</v>
+        <v>5702117</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>23967</v>
+        <v>23994</v>
       </c>
       <c r="D607" t="n">
-        <v>29918977</v>
+        <v>29951506</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>9690</v>
+        <v>9694</v>
       </c>
       <c r="D612" t="n">
-        <v>14178843</v>
+        <v>14184143</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>3693</v>
+        <v>3694</v>
       </c>
       <c r="D614" t="n">
-        <v>5306123</v>
+        <v>5307623</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29998,10 +29998,10 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>16104</v>
+        <v>16118</v>
       </c>
       <c r="D618" t="n">
-        <v>20104519</v>
+        <v>20122240</v>
       </c>
       <c r="E618" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>6245</v>
+        <v>6256</v>
       </c>
       <c r="D622" t="n">
-        <v>9165170</v>
+        <v>9181581</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30430,10 +30430,10 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>14923</v>
+        <v>14934</v>
       </c>
       <c r="D627" t="n">
-        <v>18742638</v>
+        <v>18752497</v>
       </c>
       <c r="E627" t="inlineStr">
         <is>
@@ -30622,10 +30622,10 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>5564</v>
+        <v>5566</v>
       </c>
       <c r="D631" t="n">
-        <v>8152896</v>
+        <v>8155896</v>
       </c>
       <c r="E631" t="inlineStr">
         <is>
@@ -30670,10 +30670,10 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D632" t="n">
-        <v>1871191</v>
+        <v>1872691</v>
       </c>
       <c r="E632" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D635" t="n">
-        <v>460107</v>
+        <v>461607</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>8166</v>
+        <v>8167</v>
       </c>
       <c r="D636" t="n">
-        <v>10453331</v>
+        <v>10454815</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>2723</v>
+        <v>2724</v>
       </c>
       <c r="D641" t="n">
-        <v>3988557</v>
+        <v>3990057</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>31366</v>
+        <v>31394</v>
       </c>
       <c r="D645" t="n">
-        <v>38474469</v>
+        <v>38503569</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>11910</v>
+        <v>11916</v>
       </c>
       <c r="D650" t="n">
-        <v>17468671</v>
+        <v>17476959</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>5452</v>
+        <v>5459</v>
       </c>
       <c r="D652" t="n">
-        <v>7907427</v>
+        <v>7917767</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31822,10 +31822,10 @@
         </is>
       </c>
       <c r="C656" t="n">
-        <v>12341</v>
+        <v>12344</v>
       </c>
       <c r="D656" t="n">
-        <v>14840253</v>
+        <v>14843512</v>
       </c>
       <c r="E656" t="inlineStr">
         <is>
@@ -32062,10 +32062,10 @@
         </is>
       </c>
       <c r="C661" t="n">
-        <v>3859</v>
+        <v>3861</v>
       </c>
       <c r="D661" t="n">
-        <v>5648407</v>
+        <v>5651407</v>
       </c>
       <c r="E661" t="inlineStr">
         <is>
@@ -32110,10 +32110,10 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D662" t="n">
-        <v>1716822</v>
+        <v>1718322</v>
       </c>
       <c r="E662" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>30390</v>
+        <v>30411</v>
       </c>
       <c r="D666" t="n">
-        <v>37652035</v>
+        <v>37670715</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>11312</v>
+        <v>11320</v>
       </c>
       <c r="D670" t="n">
-        <v>16612907</v>
+        <v>16624907</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>3304</v>
+        <v>3307</v>
       </c>
       <c r="D672" t="n">
-        <v>4762162</v>
+        <v>4766250</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>8156</v>
+        <v>8164</v>
       </c>
       <c r="D676" t="n">
-        <v>10300955</v>
+        <v>10307342</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D680" t="n">
-        <v>2026195</v>
+        <v>2027695</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33118,10 +33118,10 @@
         </is>
       </c>
       <c r="C683" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D683" t="n">
-        <v>283868</v>
+        <v>286868</v>
       </c>
       <c r="E683" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>4159</v>
+        <v>4167</v>
       </c>
       <c r="D684" t="n">
-        <v>4999062</v>
+        <v>5006263</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="D688" t="n">
-        <v>1244565</v>
+        <v>1247565</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D690" t="n">
-        <v>695077</v>
+        <v>696577</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D692" t="n">
-        <v>239110</v>
+        <v>240106</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>10138</v>
+        <v>10151</v>
       </c>
       <c r="D693" t="n">
-        <v>12551437</v>
+        <v>12567302</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>3686</v>
+        <v>3688</v>
       </c>
       <c r="D697" t="n">
-        <v>5434439</v>
+        <v>5436890</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>20882</v>
+        <v>20895</v>
       </c>
       <c r="D702" t="n">
-        <v>25497044</v>
+        <v>25511319</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34222,10 +34222,10 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>6105</v>
+        <v>6110</v>
       </c>
       <c r="D706" t="n">
-        <v>8910334</v>
+        <v>8917834</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
@@ -34318,10 +34318,10 @@
         </is>
       </c>
       <c r="C708" t="n">
-        <v>2458</v>
+        <v>2460</v>
       </c>
       <c r="D708" t="n">
-        <v>3538202</v>
+        <v>3539928</v>
       </c>
       <c r="E708" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D710" t="n">
-        <v>542065</v>
+        <v>543565</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34558,10 +34558,10 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>82899</v>
+        <v>82986</v>
       </c>
       <c r="D713" t="n">
-        <v>104060575</v>
+        <v>104160335</v>
       </c>
       <c r="E713" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>29006</v>
+        <v>29028</v>
       </c>
       <c r="D718" t="n">
-        <v>42548560</v>
+        <v>42581230</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34942,10 +34942,10 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>14924</v>
+        <v>14947</v>
       </c>
       <c r="D721" t="n">
-        <v>21530095</v>
+        <v>21561991</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>2146</v>
+        <v>2151</v>
       </c>
       <c r="D724" t="n">
-        <v>3094940</v>
+        <v>3101809</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>
@@ -35182,10 +35182,10 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>1578</v>
+        <v>1587</v>
       </c>
       <c r="D726" t="n">
-        <v>2202610</v>
+        <v>2214080</v>
       </c>
       <c r="E726" t="inlineStr">
         <is>
@@ -35230,10 +35230,10 @@
         </is>
       </c>
       <c r="C727" t="n">
-        <v>12095</v>
+        <v>12103</v>
       </c>
       <c r="D727" t="n">
-        <v>14718977</v>
+        <v>14726862</v>
       </c>
       <c r="E727" t="inlineStr">
         <is>
@@ -35470,10 +35470,10 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="D732" t="n">
-        <v>2342791</v>
+        <v>2346289</v>
       </c>
       <c r="E732" t="inlineStr">
         <is>
@@ -35614,10 +35614,10 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>19040</v>
+        <v>19051</v>
       </c>
       <c r="D735" t="n">
-        <v>23388199</v>
+        <v>23399348</v>
       </c>
       <c r="E735" t="inlineStr">
         <is>
@@ -35806,10 +35806,10 @@
         </is>
       </c>
       <c r="C739" t="n">
-        <v>7306</v>
+        <v>7311</v>
       </c>
       <c r="D739" t="n">
-        <v>10684349</v>
+        <v>10691849</v>
       </c>
       <c r="E739" t="inlineStr">
         <is>
@@ -35902,10 +35902,10 @@
         </is>
       </c>
       <c r="C741" t="n">
-        <v>2402</v>
+        <v>2405</v>
       </c>
       <c r="D741" t="n">
-        <v>3447522</v>
+        <v>3449950</v>
       </c>
       <c r="E741" t="inlineStr">
         <is>
@@ -35998,10 +35998,10 @@
         </is>
       </c>
       <c r="C743" t="n">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D743" t="n">
-        <v>480274</v>
+        <v>484774</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
@@ -36046,10 +36046,10 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D744" t="n">
-        <v>590079</v>
+        <v>591579</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
@@ -36142,10 +36142,10 @@
         </is>
       </c>
       <c r="C746" t="n">
-        <v>12497</v>
+        <v>12505</v>
       </c>
       <c r="D746" t="n">
-        <v>15366141</v>
+        <v>15372061</v>
       </c>
       <c r="E746" t="inlineStr">
         <is>
@@ -36334,10 +36334,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>4520</v>
+        <v>4525</v>
       </c>
       <c r="D750" t="n">
-        <v>6620887</v>
+        <v>6627787</v>
       </c>
       <c r="E750" t="inlineStr">
         <is>
@@ -36574,10 +36574,10 @@
         </is>
       </c>
       <c r="C755" t="n">
-        <v>31839</v>
+        <v>31848</v>
       </c>
       <c r="D755" t="n">
-        <v>39525295</v>
+        <v>39533836</v>
       </c>
       <c r="E755" t="inlineStr">
         <is>
@@ -36814,10 +36814,10 @@
         </is>
       </c>
       <c r="C760" t="n">
-        <v>13565</v>
+        <v>13574</v>
       </c>
       <c r="D760" t="n">
-        <v>19838542</v>
+        <v>19852042</v>
       </c>
       <c r="E760" t="inlineStr">
         <is>
@@ -36910,10 +36910,10 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>4591</v>
+        <v>4596</v>
       </c>
       <c r="D762" t="n">
-        <v>6560080</v>
+        <v>6567580</v>
       </c>
       <c r="E762" t="inlineStr">
         <is>
@@ -37054,10 +37054,10 @@
         </is>
       </c>
       <c r="C765" t="n">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="D765" t="n">
-        <v>1153911</v>
+        <v>1158411</v>
       </c>
       <c r="E765" t="inlineStr">
         <is>
@@ -37150,10 +37150,10 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>13320</v>
+        <v>13330</v>
       </c>
       <c r="D767" t="n">
-        <v>16379041</v>
+        <v>16389243</v>
       </c>
       <c r="E767" t="inlineStr">
         <is>
@@ -37246,10 +37246,10 @@
         </is>
       </c>
       <c r="C769" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D769" t="n">
-        <v>124215</v>
+        <v>127215</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
@@ -37294,10 +37294,10 @@
         </is>
       </c>
       <c r="C770" t="n">
-        <v>4952</v>
+        <v>4956</v>
       </c>
       <c r="D770" t="n">
-        <v>7234643</v>
+        <v>7240643</v>
       </c>
       <c r="E770" t="inlineStr">
         <is>
@@ -37342,10 +37342,10 @@
         </is>
       </c>
       <c r="C771" t="n">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="D771" t="n">
-        <v>1816582</v>
+        <v>1821082</v>
       </c>
       <c r="E771" t="inlineStr">
         <is>
@@ -37438,10 +37438,10 @@
         </is>
       </c>
       <c r="C773" t="n">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="D773" t="n">
-        <v>682271</v>
+        <v>686324</v>
       </c>
       <c r="E773" t="inlineStr">
         <is>
@@ -37486,10 +37486,10 @@
         </is>
       </c>
       <c r="C774" t="n">
-        <v>7372</v>
+        <v>7384</v>
       </c>
       <c r="D774" t="n">
-        <v>8590695</v>
+        <v>8600349</v>
       </c>
       <c r="E774" t="inlineStr">
         <is>
@@ -37726,10 +37726,10 @@
         </is>
       </c>
       <c r="C779" t="n">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="D779" t="n">
-        <v>1603892</v>
+        <v>1606892</v>
       </c>
       <c r="E779" t="inlineStr">
         <is>
@@ -37774,10 +37774,10 @@
         </is>
       </c>
       <c r="C780" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D780" t="n">
-        <v>224240</v>
+        <v>225740</v>
       </c>
       <c r="E780" t="inlineStr">
         <is>
@@ -37822,10 +37822,10 @@
         </is>
       </c>
       <c r="C781" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D781" t="n">
-        <v>261737</v>
+        <v>261890</v>
       </c>
       <c r="E781" t="inlineStr">
         <is>
@@ -37870,10 +37870,10 @@
         </is>
       </c>
       <c r="C782" t="n">
-        <v>18340</v>
+        <v>18364</v>
       </c>
       <c r="D782" t="n">
-        <v>22217876</v>
+        <v>22245706</v>
       </c>
       <c r="E782" t="inlineStr">
         <is>
@@ -38206,10 +38206,10 @@
         </is>
       </c>
       <c r="C789" t="n">
-        <v>3745</v>
+        <v>3748</v>
       </c>
       <c r="D789" t="n">
-        <v>5467744</v>
+        <v>5471520</v>
       </c>
       <c r="E789" t="inlineStr">
         <is>
@@ -38350,10 +38350,10 @@
         </is>
       </c>
       <c r="C792" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D792" t="n">
-        <v>509458</v>
+        <v>510958</v>
       </c>
       <c r="E792" t="inlineStr">
         <is>
@@ -38398,10 +38398,10 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>12312</v>
+        <v>12322</v>
       </c>
       <c r="D793" t="n">
-        <v>15491511</v>
+        <v>15499893</v>
       </c>
       <c r="E793" t="inlineStr">
         <is>
@@ -38638,10 +38638,10 @@
         </is>
       </c>
       <c r="C798" t="n">
-        <v>4208</v>
+        <v>4209</v>
       </c>
       <c r="D798" t="n">
-        <v>6155110</v>
+        <v>6156352</v>
       </c>
       <c r="E798" t="inlineStr">
         <is>
@@ -38926,10 +38926,10 @@
         </is>
       </c>
       <c r="C804" t="n">
-        <v>35277</v>
+        <v>35297</v>
       </c>
       <c r="D804" t="n">
-        <v>43360795</v>
+        <v>43381640</v>
       </c>
       <c r="E804" t="inlineStr">
         <is>
@@ -39118,10 +39118,10 @@
         </is>
       </c>
       <c r="C808" t="n">
-        <v>14136</v>
+        <v>14139</v>
       </c>
       <c r="D808" t="n">
-        <v>20670396</v>
+        <v>20673982</v>
       </c>
       <c r="E808" t="inlineStr">
         <is>
@@ -39214,10 +39214,10 @@
         </is>
       </c>
       <c r="C810" t="n">
-        <v>6650</v>
+        <v>6652</v>
       </c>
       <c r="D810" t="n">
-        <v>9599609</v>
+        <v>9599995</v>
       </c>
       <c r="E810" t="inlineStr">
         <is>
@@ -39262,10 +39262,10 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D811" t="n">
-        <v>814537</v>
+        <v>816037</v>
       </c>
       <c r="E811" t="inlineStr">
         <is>
@@ -39358,10 +39358,10 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D813" t="n">
-        <v>1249131</v>
+        <v>1252131</v>
       </c>
       <c r="E813" t="inlineStr">
         <is>
@@ -39406,10 +39406,10 @@
         </is>
       </c>
       <c r="C814" t="n">
-        <v>8360</v>
+        <v>8362</v>
       </c>
       <c r="D814" t="n">
-        <v>10296334</v>
+        <v>10297641</v>
       </c>
       <c r="E814" t="inlineStr">
         <is>
@@ -39694,10 +39694,10 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>2912</v>
+        <v>2913</v>
       </c>
       <c r="D820" t="n">
-        <v>4248869</v>
+        <v>4250369</v>
       </c>
       <c r="E820" t="inlineStr">
         <is>
@@ -39886,10 +39886,10 @@
         </is>
       </c>
       <c r="C824" t="n">
-        <v>65926</v>
+        <v>65977</v>
       </c>
       <c r="D824" t="n">
-        <v>82144522</v>
+        <v>82200165</v>
       </c>
       <c r="E824" t="inlineStr">
         <is>
@@ -40126,10 +40126,10 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>23158</v>
+        <v>23176</v>
       </c>
       <c r="D829" t="n">
-        <v>33864196</v>
+        <v>33890510</v>
       </c>
       <c r="E829" t="inlineStr">
         <is>
@@ -40270,10 +40270,10 @@
         </is>
       </c>
       <c r="C832" t="n">
-        <v>14265</v>
+        <v>14280</v>
       </c>
       <c r="D832" t="n">
-        <v>20577909</v>
+        <v>20599275</v>
       </c>
       <c r="E832" t="inlineStr">
         <is>
@@ -40510,10 +40510,10 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>1790</v>
+        <v>1797</v>
       </c>
       <c r="D837" t="n">
-        <v>2491747</v>
+        <v>2501987</v>
       </c>
       <c r="E837" t="inlineStr">
         <is>
@@ -40558,10 +40558,10 @@
         </is>
       </c>
       <c r="C838" t="n">
-        <v>12426</v>
+        <v>12435</v>
       </c>
       <c r="D838" t="n">
-        <v>15501786</v>
+        <v>15508900</v>
       </c>
       <c r="E838" t="inlineStr">
         <is>
@@ -40750,10 +40750,10 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>4509</v>
+        <v>4511</v>
       </c>
       <c r="D842" t="n">
-        <v>6542383</v>
+        <v>6543931</v>
       </c>
       <c r="E842" t="inlineStr">
         <is>
@@ -40846,10 +40846,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>1403</v>
+        <v>1405</v>
       </c>
       <c r="D844" t="n">
-        <v>2013436</v>
+        <v>2016436</v>
       </c>
       <c r="E844" t="inlineStr">
         <is>
@@ -41038,10 +41038,10 @@
         </is>
       </c>
       <c r="C848" t="n">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D848" t="n">
-        <v>453167</v>
+        <v>460667</v>
       </c>
       <c r="E848" t="inlineStr">
         <is>
@@ -41086,10 +41086,10 @@
         </is>
       </c>
       <c r="C849" t="n">
-        <v>64025</v>
+        <v>64093</v>
       </c>
       <c r="D849" t="n">
-        <v>78958109</v>
+        <v>79024179</v>
       </c>
       <c r="E849" t="inlineStr">
         <is>
@@ -41374,10 +41374,10 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>24072</v>
+        <v>24089</v>
       </c>
       <c r="D855" t="n">
-        <v>35318940</v>
+        <v>35341921</v>
       </c>
       <c r="E855" t="inlineStr">
         <is>
@@ -41470,10 +41470,10 @@
         </is>
       </c>
       <c r="C857" t="n">
-        <v>15908</v>
+        <v>15922</v>
       </c>
       <c r="D857" t="n">
-        <v>23034477</v>
+        <v>23055308</v>
       </c>
       <c r="E857" t="inlineStr">
         <is>
@@ -41566,10 +41566,10 @@
         </is>
       </c>
       <c r="C859" t="n">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="D859" t="n">
-        <v>1338849</v>
+        <v>1342872</v>
       </c>
       <c r="E859" t="inlineStr">
         <is>
@@ -41614,10 +41614,10 @@
         </is>
       </c>
       <c r="C860" t="n">
-        <v>1737</v>
+        <v>1743</v>
       </c>
       <c r="D860" t="n">
-        <v>2418792</v>
+        <v>2427792</v>
       </c>
       <c r="E860" t="inlineStr">
         <is>
@@ -41710,10 +41710,10 @@
         </is>
       </c>
       <c r="C862" t="n">
-        <v>8396</v>
+        <v>8400</v>
       </c>
       <c r="D862" t="n">
-        <v>10257102</v>
+        <v>10262052</v>
       </c>
       <c r="E862" t="inlineStr">
         <is>
@@ -41806,10 +41806,10 @@
         </is>
       </c>
       <c r="C864" t="n">
-        <v>2728</v>
+        <v>2730</v>
       </c>
       <c r="D864" t="n">
-        <v>3973305</v>
+        <v>3976305</v>
       </c>
       <c r="E864" t="inlineStr">
         <is>
@@ -41854,10 +41854,10 @@
         </is>
       </c>
       <c r="C865" t="n">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="D865" t="n">
-        <v>1643445</v>
+        <v>1646445</v>
       </c>
       <c r="E865" t="inlineStr">
         <is>
@@ -41950,10 +41950,10 @@
         </is>
       </c>
       <c r="C867" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D867" t="n">
-        <v>293362</v>
+        <v>294862</v>
       </c>
       <c r="E867" t="inlineStr">
         <is>
@@ -41998,10 +41998,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>3868</v>
+        <v>3871</v>
       </c>
       <c r="D868" t="n">
-        <v>4973941</v>
+        <v>4976276</v>
       </c>
       <c r="E868" t="inlineStr">
         <is>
@@ -42382,10 +42382,10 @@
         </is>
       </c>
       <c r="C876" t="n">
-        <v>23987</v>
+        <v>24011</v>
       </c>
       <c r="D876" t="n">
-        <v>29988280</v>
+        <v>30015302</v>
       </c>
       <c r="E876" t="inlineStr">
         <is>
@@ -42526,10 +42526,10 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D879" t="n">
-        <v>60039</v>
+        <v>61539</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
@@ -42574,10 +42574,10 @@
         </is>
       </c>
       <c r="C880" t="n">
-        <v>8230</v>
+        <v>8235</v>
       </c>
       <c r="D880" t="n">
-        <v>12012905</v>
+        <v>12020405</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
@@ -42670,10 +42670,10 @@
         </is>
       </c>
       <c r="C882" t="n">
-        <v>5087</v>
+        <v>5093</v>
       </c>
       <c r="D882" t="n">
-        <v>7349968</v>
+        <v>7357353</v>
       </c>
       <c r="E882" t="inlineStr">
         <is>
@@ -42766,10 +42766,10 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D884" t="n">
-        <v>555594</v>
+        <v>557094</v>
       </c>
       <c r="E884" t="inlineStr">
         <is>
@@ -42814,10 +42814,10 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D885" t="n">
-        <v>794827</v>
+        <v>797827</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
@@ -42910,10 +42910,10 @@
         </is>
       </c>
       <c r="C887" t="n">
-        <v>15770</v>
+        <v>15782</v>
       </c>
       <c r="D887" t="n">
-        <v>18936120</v>
+        <v>18943002</v>
       </c>
       <c r="E887" t="inlineStr">
         <is>
@@ -43198,10 +43198,10 @@
         </is>
       </c>
       <c r="C893" t="n">
-        <v>2619</v>
+        <v>2620</v>
       </c>
       <c r="D893" t="n">
-        <v>3765455</v>
+        <v>3766955</v>
       </c>
       <c r="E893" t="inlineStr">
         <is>
@@ -43342,10 +43342,10 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D896" t="n">
-        <v>518157</v>
+        <v>522657</v>
       </c>
       <c r="E896" t="inlineStr">
         <is>
@@ -43390,10 +43390,10 @@
         </is>
       </c>
       <c r="C897" t="n">
-        <v>10637</v>
+        <v>10648</v>
       </c>
       <c r="D897" t="n">
-        <v>13048895</v>
+        <v>13062267</v>
       </c>
       <c r="E897" t="inlineStr">
         <is>
@@ -43534,10 +43534,10 @@
         </is>
       </c>
       <c r="C900" t="n">
-        <v>3516</v>
+        <v>3517</v>
       </c>
       <c r="D900" t="n">
-        <v>5142130</v>
+        <v>5143630</v>
       </c>
       <c r="E900" t="inlineStr">
         <is>
@@ -43582,10 +43582,10 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>1647</v>
+        <v>1649</v>
       </c>
       <c r="D901" t="n">
-        <v>2366092</v>
+        <v>2369092</v>
       </c>
       <c r="E901" t="inlineStr">
         <is>
@@ -43726,10 +43726,10 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>49741</v>
+        <v>49818</v>
       </c>
       <c r="D904" t="n">
-        <v>62219484</v>
+        <v>62302610</v>
       </c>
       <c r="E904" t="inlineStr">
         <is>
@@ -43966,10 +43966,10 @@
         </is>
       </c>
       <c r="C909" t="n">
-        <v>22781</v>
+        <v>22802</v>
       </c>
       <c r="D909" t="n">
-        <v>33397544</v>
+        <v>33423957</v>
       </c>
       <c r="E909" t="inlineStr">
         <is>
@@ -44062,10 +44062,10 @@
         </is>
       </c>
       <c r="C911" t="n">
-        <v>6781</v>
+        <v>6791</v>
       </c>
       <c r="D911" t="n">
-        <v>9770111</v>
+        <v>9785111</v>
       </c>
       <c r="E911" t="inlineStr">
         <is>
@@ -44206,10 +44206,10 @@
         </is>
       </c>
       <c r="C914" t="n">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="D914" t="n">
-        <v>1664450</v>
+        <v>1668818</v>
       </c>
       <c r="E914" t="inlineStr">
         <is>
@@ -44254,10 +44254,10 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>23105</v>
+        <v>23120</v>
       </c>
       <c r="D915" t="n">
-        <v>28669975</v>
+        <v>28685278</v>
       </c>
       <c r="E915" t="inlineStr">
         <is>
@@ -44446,10 +44446,10 @@
         </is>
       </c>
       <c r="C919" t="n">
-        <v>10426</v>
+        <v>10435</v>
       </c>
       <c r="D919" t="n">
-        <v>15269609</v>
+        <v>15283109</v>
       </c>
       <c r="E919" t="inlineStr">
         <is>
@@ -44686,10 +44686,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D924" t="n">
-        <v>1091091</v>
+        <v>1092017</v>
       </c>
       <c r="E924" t="inlineStr">
         <is>
@@ -44734,10 +44734,10 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>7706</v>
+        <v>7707</v>
       </c>
       <c r="D925" t="n">
-        <v>9639813</v>
+        <v>9640324</v>
       </c>
       <c r="E925" t="inlineStr">
         <is>
@@ -44974,10 +44974,10 @@
         </is>
       </c>
       <c r="C930" t="n">
-        <v>3234</v>
+        <v>3235</v>
       </c>
       <c r="D930" t="n">
-        <v>4762851</v>
+        <v>4764351</v>
       </c>
       <c r="E930" t="inlineStr">
         <is>
@@ -45022,10 +45022,10 @@
         </is>
       </c>
       <c r="C931" t="n">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="D931" t="n">
-        <v>1040425</v>
+        <v>1046425</v>
       </c>
       <c r="E931" t="inlineStr">
         <is>
@@ -45118,10 +45118,10 @@
         </is>
       </c>
       <c r="C933" t="n">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D933" t="n">
-        <v>311888</v>
+        <v>314888</v>
       </c>
       <c r="E933" t="inlineStr">
         <is>
@@ -45166,10 +45166,10 @@
         </is>
       </c>
       <c r="C934" t="n">
-        <v>14170</v>
+        <v>14182</v>
       </c>
       <c r="D934" t="n">
-        <v>17559175</v>
+        <v>17573506</v>
       </c>
       <c r="E934" t="inlineStr">
         <is>
@@ -45358,10 +45358,10 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>5617</v>
+        <v>5619</v>
       </c>
       <c r="D938" t="n">
-        <v>8202776</v>
+        <v>8205776</v>
       </c>
       <c r="E938" t="inlineStr">
         <is>
@@ -45454,10 +45454,10 @@
         </is>
       </c>
       <c r="C940" t="n">
-        <v>1572</v>
+        <v>1577</v>
       </c>
       <c r="D940" t="n">
-        <v>2258981</v>
+        <v>2266481</v>
       </c>
       <c r="E940" t="inlineStr">
         <is>
@@ -45694,10 +45694,10 @@
         </is>
       </c>
       <c r="C945" t="n">
-        <v>20866</v>
+        <v>20887</v>
       </c>
       <c r="D945" t="n">
-        <v>25919225</v>
+        <v>25938437</v>
       </c>
       <c r="E945" t="inlineStr">
         <is>
@@ -45934,10 +45934,10 @@
         </is>
       </c>
       <c r="C950" t="n">
-        <v>10589</v>
+        <v>10592</v>
       </c>
       <c r="D950" t="n">
-        <v>15467965</v>
+        <v>15472465</v>
       </c>
       <c r="E950" t="inlineStr">
         <is>
@@ -46126,10 +46126,10 @@
         </is>
       </c>
       <c r="C954" t="n">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D954" t="n">
-        <v>774505</v>
+        <v>778096</v>
       </c>
       <c r="E954" t="inlineStr">
         <is>
@@ -46174,10 +46174,10 @@
         </is>
       </c>
       <c r="C955" t="n">
-        <v>9367</v>
+        <v>9374</v>
       </c>
       <c r="D955" t="n">
-        <v>11639886</v>
+        <v>11646531</v>
       </c>
       <c r="E955" t="inlineStr">
         <is>
@@ -46462,10 +46462,10 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="D961" t="n">
-        <v>2343388</v>
+        <v>2347888</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
@@ -46510,10 +46510,10 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D962" t="n">
-        <v>7489</v>
+        <v>8989</v>
       </c>
       <c r="E962" t="inlineStr">
         <is>
@@ -46654,10 +46654,10 @@
         </is>
       </c>
       <c r="C965" t="n">
-        <v>76695</v>
+        <v>76771</v>
       </c>
       <c r="D965" t="n">
-        <v>98516653</v>
+        <v>98605644</v>
       </c>
       <c r="E965" t="inlineStr">
         <is>
@@ -46990,10 +46990,10 @@
         </is>
       </c>
       <c r="C972" t="n">
-        <v>28519</v>
+        <v>28546</v>
       </c>
       <c r="D972" t="n">
-        <v>41805814</v>
+        <v>41845048</v>
       </c>
       <c r="E972" t="inlineStr">
         <is>
@@ -47086,10 +47086,10 @@
         </is>
       </c>
       <c r="C974" t="n">
-        <v>20627</v>
+        <v>20650</v>
       </c>
       <c r="D974" t="n">
-        <v>29915656</v>
+        <v>29947039</v>
       </c>
       <c r="E974" t="inlineStr">
         <is>
@@ -47230,10 +47230,10 @@
         </is>
       </c>
       <c r="C977" t="n">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="D977" t="n">
-        <v>1642257</v>
+        <v>1646757</v>
       </c>
       <c r="E977" t="inlineStr">
         <is>
@@ -47278,10 +47278,10 @@
         </is>
       </c>
       <c r="C978" t="n">
-        <v>93870</v>
+        <v>93995</v>
       </c>
       <c r="D978" t="n">
-        <v>117579645</v>
+        <v>117740009</v>
       </c>
       <c r="E978" t="inlineStr">
         <is>
@@ -47614,10 +47614,10 @@
         </is>
       </c>
       <c r="C985" t="n">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D985" t="n">
-        <v>471248</v>
+        <v>475758</v>
       </c>
       <c r="E985" t="inlineStr">
         <is>
@@ -47662,10 +47662,10 @@
         </is>
       </c>
       <c r="C986" t="n">
-        <v>37578</v>
+        <v>37668</v>
       </c>
       <c r="D986" t="n">
-        <v>55069531</v>
+        <v>55196424</v>
       </c>
       <c r="E986" t="inlineStr">
         <is>
@@ -47806,10 +47806,10 @@
         </is>
       </c>
       <c r="C989" t="n">
-        <v>28982</v>
+        <v>29066</v>
       </c>
       <c r="D989" t="n">
-        <v>42050030</v>
+        <v>42174321</v>
       </c>
       <c r="E989" t="inlineStr">
         <is>
@@ -47854,10 +47854,10 @@
         </is>
       </c>
       <c r="C990" t="n">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D990" t="n">
-        <v>929434</v>
+        <v>929689</v>
       </c>
       <c r="E990" t="inlineStr">
         <is>
@@ -47950,10 +47950,10 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>2645</v>
+        <v>2657</v>
       </c>
       <c r="D992" t="n">
-        <v>3715693</v>
+        <v>3729835</v>
       </c>
       <c r="E992" t="inlineStr">
         <is>
@@ -47998,10 +47998,10 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>11937</v>
+        <v>11948</v>
       </c>
       <c r="D993" t="n">
-        <v>15503401</v>
+        <v>15513958</v>
       </c>
       <c r="E993" t="inlineStr">
         <is>
@@ -48238,10 +48238,10 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>3803</v>
+        <v>3806</v>
       </c>
       <c r="D998" t="n">
-        <v>5550621</v>
+        <v>5555121</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
@@ -48286,10 +48286,10 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>1255</v>
+        <v>1260</v>
       </c>
       <c r="D999" t="n">
-        <v>1811357</v>
+        <v>1818857</v>
       </c>
       <c r="E999" t="inlineStr">
         <is>
@@ -48526,10 +48526,10 @@
         </is>
       </c>
       <c r="C1004" t="n">
-        <v>60466</v>
+        <v>60517</v>
       </c>
       <c r="D1004" t="n">
-        <v>75470481</v>
+        <v>75529627</v>
       </c>
       <c r="E1004" t="inlineStr">
         <is>
@@ -48574,10 +48574,10 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D1005" t="n">
-        <v>59118</v>
+        <v>59556</v>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
@@ -48766,10 +48766,10 @@
         </is>
       </c>
       <c r="C1009" t="n">
-        <v>19575</v>
+        <v>19583</v>
       </c>
       <c r="D1009" t="n">
-        <v>28665710</v>
+        <v>28677106</v>
       </c>
       <c r="E1009" t="inlineStr">
         <is>
@@ -48862,10 +48862,10 @@
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>13820</v>
+        <v>13838</v>
       </c>
       <c r="D1011" t="n">
-        <v>19983999</v>
+        <v>20010705</v>
       </c>
       <c r="E1011" t="inlineStr">
         <is>
@@ -49006,10 +49006,10 @@
         </is>
       </c>
       <c r="C1014" t="n">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="D1014" t="n">
-        <v>1315296</v>
+        <v>1321296</v>
       </c>
       <c r="E1014" t="inlineStr">
         <is>
@@ -49054,10 +49054,10 @@
         </is>
       </c>
       <c r="C1015" t="n">
-        <v>30961</v>
+        <v>30982</v>
       </c>
       <c r="D1015" t="n">
-        <v>38448635</v>
+        <v>38469858</v>
       </c>
       <c r="E1015" t="inlineStr">
         <is>
@@ -49294,10 +49294,10 @@
         </is>
       </c>
       <c r="C1020" t="n">
-        <v>11454</v>
+        <v>11459</v>
       </c>
       <c r="D1020" t="n">
-        <v>16768873</v>
+        <v>16775428</v>
       </c>
       <c r="E1020" t="inlineStr">
         <is>
@@ -49390,10 +49390,10 @@
         </is>
       </c>
       <c r="C1022" t="n">
-        <v>6932</v>
+        <v>6937</v>
       </c>
       <c r="D1022" t="n">
-        <v>10041118</v>
+        <v>10048618</v>
       </c>
       <c r="E1022" t="inlineStr">
         <is>
@@ -49486,10 +49486,10 @@
         </is>
       </c>
       <c r="C1024" t="n">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D1024" t="n">
-        <v>1059149</v>
+        <v>1060121</v>
       </c>
       <c r="E1024" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[PGE] Add 2021-01-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1302,13 +1302,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>22048</v>
+        <v>22047</v>
       </c>
       <c r="D19" t="n">
         <v>6688</v>
       </c>
       <c r="E19" t="n">
-        <v>32930122</v>
+        <v>32930047</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -2220,13 +2220,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>33664</v>
+        <v>33662</v>
       </c>
       <c r="D37" t="n">
-        <v>10429</v>
+        <v>10428</v>
       </c>
       <c r="E37" t="n">
-        <v>49424802</v>
+        <v>49422067</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3138,13 +3138,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>58151</v>
+        <v>58152</v>
       </c>
       <c r="D55" t="n">
         <v>17719</v>
       </c>
       <c r="E55" t="n">
-        <v>91763033</v>
+        <v>91763268</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -3699,13 +3699,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>70595</v>
+        <v>70589</v>
       </c>
       <c r="D66" t="n">
         <v>22047</v>
       </c>
       <c r="E66" t="n">
-        <v>105656424</v>
+        <v>105647624</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -4317,7 +4317,7 @@
         <v>11590</v>
       </c>
       <c r="E78" t="n">
-        <v>57752067</v>
+        <v>57752877</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -4719,13 +4719,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>33634</v>
+        <v>33635</v>
       </c>
       <c r="D86" t="n">
-        <v>10338</v>
+        <v>10339</v>
       </c>
       <c r="E86" t="n">
-        <v>50613204</v>
+        <v>50614523</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -5235,7 +5235,7 @@
         <v>36592</v>
       </c>
       <c r="E96" t="n">
-        <v>195863757</v>
+        <v>195863097</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -5892,13 +5892,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>47407</v>
+        <v>47406</v>
       </c>
       <c r="D109" t="n">
         <v>13423</v>
       </c>
       <c r="E109" t="n">
-        <v>78516727</v>
+        <v>78515227</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -6402,13 +6402,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>23973</v>
+        <v>23970</v>
       </c>
       <c r="D119" t="n">
         <v>7467</v>
       </c>
       <c r="E119" t="n">
-        <v>35378648</v>
+        <v>35374148</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -8085,13 +8085,13 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>8673</v>
+        <v>8674</v>
       </c>
       <c r="D152" t="n">
         <v>2710</v>
       </c>
       <c r="E152" t="n">
-        <v>13786142</v>
+        <v>13787642</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -8442,13 +8442,13 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>25078</v>
+        <v>25079</v>
       </c>
       <c r="D159" t="n">
         <v>7854</v>
       </c>
       <c r="E159" t="n">
-        <v>39637990</v>
+        <v>39638350</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -10431,13 +10431,13 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>43322</v>
+        <v>43323</v>
       </c>
       <c r="D198" t="n">
         <v>13996</v>
       </c>
       <c r="E198" t="n">
-        <v>66259935</v>
+        <v>66251883</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -11451,13 +11451,13 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>11755</v>
+        <v>11756</v>
       </c>
       <c r="D218" t="n">
         <v>3764</v>
       </c>
       <c r="E218" t="n">
-        <v>18688366</v>
+        <v>18688473</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
@@ -14511,13 +14511,13 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>16970</v>
+        <v>16971</v>
       </c>
       <c r="D278" t="n">
         <v>4790</v>
       </c>
       <c r="E278" t="n">
-        <v>27497893</v>
+        <v>27498705</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>
@@ -15429,13 +15429,13 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>12510</v>
+        <v>12511</v>
       </c>
       <c r="D296" t="n">
         <v>4074</v>
       </c>
       <c r="E296" t="n">
-        <v>22202471</v>
+        <v>22202911</v>
       </c>
       <c r="F296" t="inlineStr">
         <is>
@@ -15891,7 +15891,7 @@
         <v>49201</v>
       </c>
       <c r="D305" t="n">
-        <v>15227</v>
+        <v>15228</v>
       </c>
       <c r="E305" t="n">
         <v>73268628</v>
@@ -16857,13 +16857,13 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>28699</v>
+        <v>28698</v>
       </c>
       <c r="D324" t="n">
         <v>9040</v>
       </c>
       <c r="E324" t="n">
-        <v>42890591</v>
+        <v>42889341</v>
       </c>
       <c r="F324" t="inlineStr">
         <is>
@@ -18693,13 +18693,13 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>33115</v>
+        <v>33114</v>
       </c>
       <c r="D360" t="n">
         <v>10429</v>
       </c>
       <c r="E360" t="n">
-        <v>49891241</v>
+        <v>49889741</v>
       </c>
       <c r="F360" t="inlineStr">
         <is>
@@ -20784,13 +20784,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>97756</v>
+        <v>97757</v>
       </c>
       <c r="D401" t="n">
         <v>29686</v>
       </c>
       <c r="E401" t="n">
-        <v>145933173</v>
+        <v>145934805</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21345,13 +21345,13 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>29336</v>
+        <v>29328</v>
       </c>
       <c r="D412" t="n">
         <v>8933</v>
       </c>
       <c r="E412" t="n">
-        <v>45394106</v>
+        <v>45383476</v>
       </c>
       <c r="F412" t="inlineStr">
         <is>
@@ -22671,13 +22671,13 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>59715</v>
+        <v>59716</v>
       </c>
       <c r="D438" t="n">
-        <v>15778</v>
+        <v>15779</v>
       </c>
       <c r="E438" t="n">
-        <v>96954689</v>
+        <v>96956189</v>
       </c>
       <c r="F438" t="inlineStr">
         <is>
@@ -23079,13 +23079,13 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>108993</v>
+        <v>108992</v>
       </c>
       <c r="D446" t="n">
-        <v>26322</v>
+        <v>26324</v>
       </c>
       <c r="E446" t="n">
-        <v>180648503</v>
+        <v>180641979</v>
       </c>
       <c r="F446" t="inlineStr">
         <is>
@@ -23538,13 +23538,13 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>265641</v>
+        <v>265634</v>
       </c>
       <c r="D455" t="n">
-        <v>67476</v>
+        <v>67475</v>
       </c>
       <c r="E455" t="n">
-        <v>421241688</v>
+        <v>421218549</v>
       </c>
       <c r="F455" t="inlineStr">
         <is>
@@ -24405,13 +24405,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>68582</v>
+        <v>68580</v>
       </c>
       <c r="D472" t="n">
-        <v>18407</v>
+        <v>18408</v>
       </c>
       <c r="E472" t="n">
-        <v>108738449</v>
+        <v>108736485</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24864,13 +24864,13 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>121763</v>
+        <v>121760</v>
       </c>
       <c r="D481" t="n">
-        <v>26741</v>
+        <v>26742</v>
       </c>
       <c r="E481" t="n">
-        <v>212460706</v>
+        <v>212448611</v>
       </c>
       <c r="F481" t="inlineStr">
         <is>
@@ -25323,13 +25323,13 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>94218</v>
+        <v>94214</v>
       </c>
       <c r="D490" t="n">
         <v>22809</v>
       </c>
       <c r="E490" t="n">
-        <v>153847830</v>
+        <v>153842183</v>
       </c>
       <c r="F490" t="inlineStr">
         <is>
@@ -25782,13 +25782,13 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>71745</v>
+        <v>71741</v>
       </c>
       <c r="D499" t="n">
         <v>17096</v>
       </c>
       <c r="E499" t="n">
-        <v>120301721</v>
+        <v>120296901</v>
       </c>
       <c r="F499" t="inlineStr">
         <is>
@@ -26190,13 +26190,13 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>66754</v>
+        <v>66755</v>
       </c>
       <c r="D507" t="n">
-        <v>18642</v>
+        <v>18643</v>
       </c>
       <c r="E507" t="n">
-        <v>105583201</v>
+        <v>105583800</v>
       </c>
       <c r="F507" t="inlineStr">
         <is>
@@ -27873,13 +27873,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>33558</v>
+        <v>33560</v>
       </c>
       <c r="D540" t="n">
-        <v>10533</v>
+        <v>10534</v>
       </c>
       <c r="E540" t="n">
-        <v>51726195</v>
+        <v>51736035</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -29148,13 +29148,13 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>11318</v>
+        <v>11319</v>
       </c>
       <c r="D565" t="n">
-        <v>3572</v>
+        <v>3573</v>
       </c>
       <c r="E565" t="n">
-        <v>18204575</v>
+        <v>18206075</v>
       </c>
       <c r="F565" t="inlineStr">
         <is>
@@ -29505,13 +29505,13 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>44266</v>
+        <v>44267</v>
       </c>
       <c r="D572" t="n">
-        <v>13804</v>
+        <v>13805</v>
       </c>
       <c r="E572" t="n">
-        <v>67917267</v>
+        <v>67917933</v>
       </c>
       <c r="F572" t="inlineStr">
         <is>
@@ -30423,13 +30423,13 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>41003</v>
+        <v>41002</v>
       </c>
       <c r="D590" t="n">
         <v>13343</v>
       </c>
       <c r="E590" t="n">
-        <v>60348102</v>
+        <v>60347867</v>
       </c>
       <c r="F590" t="inlineStr">
         <is>
@@ -32514,13 +32514,13 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>111161</v>
+        <v>111160</v>
       </c>
       <c r="D631" t="n">
         <v>34682</v>
       </c>
       <c r="E631" t="n">
-        <v>166159778</v>
+        <v>166159428</v>
       </c>
       <c r="F631" t="inlineStr">
         <is>
@@ -33585,13 +33585,13 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>26088</v>
+        <v>26090</v>
       </c>
       <c r="D652" t="n">
         <v>8468</v>
       </c>
       <c r="E652" t="n">
-        <v>38442470</v>
+        <v>38444729</v>
       </c>
       <c r="F652" t="inlineStr">
         <is>
@@ -34452,13 +34452,13 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>44258</v>
+        <v>44259</v>
       </c>
       <c r="D669" t="n">
-        <v>14319</v>
+        <v>14320</v>
       </c>
       <c r="E669" t="n">
-        <v>64154552</v>
+        <v>64155643</v>
       </c>
       <c r="F669" t="inlineStr">
         <is>
@@ -35370,13 +35370,13 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>10283</v>
+        <v>10284</v>
       </c>
       <c r="D687" t="n">
-        <v>3367</v>
+        <v>3368</v>
       </c>
       <c r="E687" t="n">
-        <v>14072716</v>
+        <v>14072791</v>
       </c>
       <c r="F687" t="inlineStr">
         <is>
@@ -35676,13 +35676,13 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>25100</v>
+        <v>25101</v>
       </c>
       <c r="D693" t="n">
-        <v>7661</v>
+        <v>7662</v>
       </c>
       <c r="E693" t="n">
-        <v>36647129</v>
+        <v>36647614</v>
       </c>
       <c r="F693" t="inlineStr">
         <is>
@@ -36543,13 +36543,13 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>50173</v>
+        <v>50172</v>
       </c>
       <c r="D710" t="n">
         <v>15118</v>
       </c>
       <c r="E710" t="n">
-        <v>71963356</v>
+        <v>71962122</v>
       </c>
       <c r="F710" t="inlineStr">
         <is>
@@ -37359,13 +37359,13 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>91329</v>
+        <v>91327</v>
       </c>
       <c r="D726" t="n">
         <v>27803</v>
       </c>
       <c r="E726" t="n">
-        <v>133672564</v>
+        <v>133670667</v>
       </c>
       <c r="F726" t="inlineStr">
         <is>
@@ -38538,7 +38538,7 @@
         <v>27143</v>
       </c>
       <c r="E749" t="n">
-        <v>126256567</v>
+        <v>126256866</v>
       </c>
       <c r="F749" t="inlineStr">
         <is>
@@ -39042,13 +39042,13 @@
         </is>
       </c>
       <c r="C759" t="n">
-        <v>11624</v>
+        <v>11625</v>
       </c>
       <c r="D759" t="n">
-        <v>3762</v>
+        <v>3763</v>
       </c>
       <c r="E759" t="n">
-        <v>17284227</v>
+        <v>17284624</v>
       </c>
       <c r="F759" t="inlineStr">
         <is>
@@ -39348,13 +39348,13 @@
         </is>
       </c>
       <c r="C765" t="n">
-        <v>5406</v>
+        <v>5407</v>
       </c>
       <c r="D765" t="n">
         <v>1800</v>
       </c>
       <c r="E765" t="n">
-        <v>8778245</v>
+        <v>8778745</v>
       </c>
       <c r="F765" t="inlineStr">
         <is>
@@ -40980,13 +40980,13 @@
         </is>
       </c>
       <c r="C797" t="n">
-        <v>66461</v>
+        <v>66460</v>
       </c>
       <c r="D797" t="n">
-        <v>21676</v>
+        <v>21675</v>
       </c>
       <c r="E797" t="n">
-        <v>100767663</v>
+        <v>100767215</v>
       </c>
       <c r="F797" t="inlineStr">
         <is>
@@ -42153,13 +42153,13 @@
         </is>
       </c>
       <c r="C820" t="n">
-        <v>19696</v>
+        <v>19697</v>
       </c>
       <c r="D820" t="n">
-        <v>6164</v>
+        <v>6165</v>
       </c>
       <c r="E820" t="n">
-        <v>30611963</v>
+        <v>30618101</v>
       </c>
       <c r="F820" t="inlineStr">
         <is>
@@ -43071,13 +43071,13 @@
         </is>
       </c>
       <c r="C838" t="n">
-        <v>13108</v>
+        <v>13109</v>
       </c>
       <c r="D838" t="n">
-        <v>4045</v>
+        <v>4046</v>
       </c>
       <c r="E838" t="n">
-        <v>20176478</v>
+        <v>20176940</v>
       </c>
       <c r="F838" t="inlineStr">
         <is>
@@ -43530,13 +43530,13 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>108075</v>
+        <v>108076</v>
       </c>
       <c r="D847" t="n">
         <v>29724</v>
       </c>
       <c r="E847" t="n">
-        <v>164181601</v>
+        <v>164182835</v>
       </c>
       <c r="F847" t="inlineStr">
         <is>
@@ -44244,13 +44244,13 @@
         </is>
       </c>
       <c r="C861" t="n">
-        <v>134233</v>
+        <v>134231</v>
       </c>
       <c r="D861" t="n">
         <v>39112</v>
       </c>
       <c r="E861" t="n">
-        <v>201918433</v>
+        <v>201915733</v>
       </c>
       <c r="F861" t="inlineStr">
         <is>
@@ -44907,13 +44907,13 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>18234</v>
+        <v>18236</v>
       </c>
       <c r="D874" t="n">
         <v>5203</v>
       </c>
       <c r="E874" t="n">
-        <v>29207727</v>
+        <v>29210227</v>
       </c>
       <c r="F874" t="inlineStr">
         <is>
@@ -45468,13 +45468,13 @@
         </is>
       </c>
       <c r="C885" t="n">
-        <v>85282</v>
+        <v>85283</v>
       </c>
       <c r="D885" t="n">
-        <v>26090</v>
+        <v>26091</v>
       </c>
       <c r="E885" t="n">
-        <v>125687534</v>
+        <v>125689469</v>
       </c>
       <c r="F885" t="inlineStr">
         <is>
@@ -45978,13 +45978,13 @@
         </is>
       </c>
       <c r="C895" t="n">
-        <v>43342</v>
+        <v>43340</v>
       </c>
       <c r="D895" t="n">
         <v>12998</v>
       </c>
       <c r="E895" t="n">
-        <v>63855858</v>
+        <v>63854196</v>
       </c>
       <c r="F895" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-15-v2 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3138,13 +3138,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>60647</v>
+        <v>60645</v>
       </c>
       <c r="D55" t="n">
-        <v>17919</v>
+        <v>17918</v>
       </c>
       <c r="E55" t="n">
-        <v>97793882</v>
+        <v>97791087</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -9411,13 +9411,13 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>14370</v>
+        <v>14369</v>
       </c>
       <c r="D178" t="n">
         <v>4390</v>
       </c>
       <c r="E178" t="n">
-        <v>22425917</v>
+        <v>22424417</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -10176,13 +10176,13 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>39445</v>
+        <v>39446</v>
       </c>
       <c r="D193" t="n">
         <v>12934</v>
       </c>
       <c r="E193" t="n">
-        <v>63771141</v>
+        <v>63772555</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -10635,13 +10635,13 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>44525</v>
+        <v>44526</v>
       </c>
       <c r="D202" t="n">
-        <v>14097</v>
+        <v>14098</v>
       </c>
       <c r="E202" t="n">
-        <v>69270050</v>
+        <v>69271353</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -11145,13 +11145,13 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>37253</v>
+        <v>37252</v>
       </c>
       <c r="D212" t="n">
         <v>11827</v>
       </c>
       <c r="E212" t="n">
-        <v>59192747</v>
+        <v>59191444</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -23334,13 +23334,13 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>111857</v>
+        <v>111856</v>
       </c>
       <c r="D451" t="n">
         <v>26484</v>
       </c>
       <c r="E451" t="n">
-        <v>187047768</v>
+        <v>187037768</v>
       </c>
       <c r="F451" t="inlineStr">
         <is>
@@ -23793,13 +23793,13 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>273972</v>
+        <v>273968</v>
       </c>
       <c r="D460" t="n">
         <v>68000</v>
       </c>
       <c r="E460" t="n">
-        <v>439570918</v>
+        <v>439566794</v>
       </c>
       <c r="F460" t="inlineStr">
         <is>
@@ -25119,13 +25119,13 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>125107</v>
+        <v>125109</v>
       </c>
       <c r="D486" t="n">
-        <v>26908</v>
+        <v>26909</v>
       </c>
       <c r="E486" t="n">
-        <v>220619170</v>
+        <v>220622220</v>
       </c>
       <c r="F486" t="inlineStr">
         <is>
@@ -25578,13 +25578,13 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>96731</v>
+        <v>96734</v>
       </c>
       <c r="D495" t="n">
-        <v>22943</v>
+        <v>22944</v>
       </c>
       <c r="E495" t="n">
-        <v>159632149</v>
+        <v>159634859</v>
       </c>
       <c r="F495" t="inlineStr">
         <is>
@@ -29454,13 +29454,13 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>11687</v>
+        <v>11686</v>
       </c>
       <c r="D571" t="n">
         <v>3596</v>
       </c>
       <c r="E571" t="n">
-        <v>19458618</v>
+        <v>19458515</v>
       </c>
       <c r="F571" t="inlineStr">
         <is>
@@ -32871,13 +32871,13 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>114345</v>
+        <v>114343</v>
       </c>
       <c r="D638" t="n">
-        <v>34971</v>
+        <v>34970</v>
       </c>
       <c r="E638" t="n">
-        <v>173489735</v>
+        <v>173488085</v>
       </c>
       <c r="F638" t="inlineStr">
         <is>
@@ -34860,13 +34860,13 @@
         </is>
       </c>
       <c r="C677" t="n">
-        <v>45615</v>
+        <v>45618</v>
       </c>
       <c r="D677" t="n">
-        <v>14409</v>
+        <v>14410</v>
       </c>
       <c r="E677" t="n">
-        <v>67262267</v>
+        <v>67266562</v>
       </c>
       <c r="F677" t="inlineStr">
         <is>
@@ -37767,13 +37767,13 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>93865</v>
+        <v>93863</v>
       </c>
       <c r="D734" t="n">
-        <v>27952</v>
+        <v>27951</v>
       </c>
       <c r="E734" t="n">
-        <v>138584381</v>
+        <v>138581739</v>
       </c>
       <c r="F734" t="inlineStr">
         <is>
@@ -38328,13 +38328,13 @@
         </is>
       </c>
       <c r="C745" t="n">
-        <v>18634</v>
+        <v>18636</v>
       </c>
       <c r="D745" t="n">
         <v>5268</v>
       </c>
       <c r="E745" t="n">
-        <v>30425937</v>
+        <v>30428579</v>
       </c>
       <c r="F745" t="inlineStr">
         <is>
@@ -39450,13 +39450,13 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>11959</v>
+        <v>11960</v>
       </c>
       <c r="D767" t="n">
-        <v>3791</v>
+        <v>3792</v>
       </c>
       <c r="E767" t="n">
-        <v>18095195</v>
+        <v>18095345</v>
       </c>
       <c r="F767" t="inlineStr">
         <is>
@@ -42612,13 +42612,13 @@
         </is>
       </c>
       <c r="C829" t="n">
-        <v>20262</v>
+        <v>20263</v>
       </c>
       <c r="D829" t="n">
-        <v>6199</v>
+        <v>6200</v>
       </c>
       <c r="E829" t="n">
-        <v>32164373</v>
+        <v>32164476</v>
       </c>
       <c r="F829" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2021-07-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -8135,13 +8135,13 @@
         <v>12</v>
       </c>
       <c r="C201">
-        <v>53603</v>
+        <v>53602</v>
       </c>
       <c r="D201">
         <v>13160</v>
       </c>
       <c r="E201">
-        <v>107871483</v>
+        <v>107871396</v>
       </c>
       <c r="F201" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-02-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1267,13 +1267,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4550</v>
+        <v>4548</v>
       </c>
       <c r="D17" t="n">
         <v>831</v>
       </c>
       <c r="E17" t="n">
-        <v>22865659</v>
+        <v>22857743</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>186331</v>
+        <v>186330</v>
       </c>
       <c r="D100" t="n">
         <v>37747</v>
       </c>
       <c r="E100" t="n">
-        <v>306246904</v>
+        <v>306246664</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>84944</v>
+        <v>84939</v>
       </c>
       <c r="D105" t="n">
         <v>16087</v>
       </c>
       <c r="E105" t="n">
-        <v>401454980</v>
+        <v>401394388</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62491</v>
+        <v>62490</v>
       </c>
       <c r="D108" t="n">
         <v>10954</v>
       </c>
       <c r="E108" t="n">
-        <v>340002241</v>
+        <v>339992241</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -10192,13 +10192,13 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>37579</v>
+        <v>37577</v>
       </c>
       <c r="D192" t="n">
         <v>8493</v>
       </c>
       <c r="E192" t="n">
-        <v>76083396</v>
+        <v>76083324</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -12895,13 +12895,13 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="D245" t="n">
         <v>1133</v>
       </c>
       <c r="E245" t="n">
-        <v>24343308</v>
+        <v>24337561</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -15088,13 +15088,13 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>14205</v>
+        <v>14204</v>
       </c>
       <c r="D288" t="n">
         <v>2289</v>
       </c>
       <c r="E288" t="n">
-        <v>94111398</v>
+        <v>94110798</v>
       </c>
       <c r="F288" t="inlineStr">
         <is>
@@ -16006,13 +16006,13 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>6084</v>
+        <v>6083</v>
       </c>
       <c r="D306" t="n">
         <v>1239</v>
       </c>
       <c r="E306" t="n">
-        <v>26906084</v>
+        <v>26900708</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
@@ -16771,13 +16771,13 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>76025</v>
+        <v>76024</v>
       </c>
       <c r="D321" t="n">
         <v>15907</v>
       </c>
       <c r="E321" t="n">
-        <v>132426430</v>
+        <v>132420461</v>
       </c>
       <c r="F321" t="inlineStr">
         <is>
@@ -17077,13 +17077,13 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>47891</v>
+        <v>47890</v>
       </c>
       <c r="D327" t="n">
         <v>9067</v>
       </c>
       <c r="E327" t="n">
-        <v>240487313</v>
+        <v>240480465</v>
       </c>
       <c r="F327" t="inlineStr">
         <is>
@@ -17995,13 +17995,13 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D345" t="n">
         <v>21</v>
       </c>
       <c r="E345" t="n">
-        <v>5675074</v>
+        <v>5633874</v>
       </c>
       <c r="F345" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18405</v>
+        <v>18404</v>
       </c>
       <c r="D399" t="n">
         <v>3382</v>
       </c>
       <c r="E399" t="n">
-        <v>72117092</v>
+        <v>72097061</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16555</v>
+        <v>16554</v>
       </c>
       <c r="D401" t="n">
         <v>2942</v>
       </c>
       <c r="E401" t="n">
-        <v>48245887</v>
+        <v>48244387</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -22075,13 +22075,13 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>70510</v>
+        <v>70509</v>
       </c>
       <c r="D425" t="n">
         <v>13142</v>
       </c>
       <c r="E425" t="n">
-        <v>343031318</v>
+        <v>343021318</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -22585,13 +22585,13 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>20231</v>
+        <v>20230</v>
       </c>
       <c r="D435" t="n">
         <v>4036</v>
       </c>
       <c r="E435" t="n">
-        <v>93020853</v>
+        <v>93010853</v>
       </c>
       <c r="F435" t="inlineStr">
         <is>
@@ -22687,13 +22687,13 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>14442</v>
+        <v>14441</v>
       </c>
       <c r="D437" t="n">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="E437" t="n">
-        <v>69130582</v>
+        <v>69127602</v>
       </c>
       <c r="F437" t="inlineStr">
         <is>
@@ -23044,13 +23044,13 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>31759</v>
+        <v>31758</v>
       </c>
       <c r="D444" t="n">
         <v>6195</v>
       </c>
       <c r="E444" t="n">
-        <v>161385286</v>
+        <v>161380032</v>
       </c>
       <c r="F444" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35036</v>
+        <v>35033</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>159879837</v>
+        <v>159828648</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416409</v>
+        <v>416403</v>
       </c>
       <c r="D477" t="n">
         <v>70491</v>
       </c>
       <c r="E477" t="n">
-        <v>723871781</v>
+        <v>723832135</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24982,13 +24982,13 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>4135</v>
+        <v>4134</v>
       </c>
       <c r="D482" t="n">
         <v>520</v>
       </c>
       <c r="E482" t="n">
-        <v>69649630</v>
+        <v>69648130</v>
       </c>
       <c r="F482" t="inlineStr">
         <is>
@@ -25033,13 +25033,13 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D483" t="n">
         <v>33</v>
       </c>
       <c r="E483" t="n">
-        <v>5333530</v>
+        <v>5323530</v>
       </c>
       <c r="F483" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291449</v>
+        <v>291440</v>
       </c>
       <c r="D484" t="n">
         <v>42556</v>
       </c>
       <c r="E484" t="n">
-        <v>1761471642</v>
+        <v>1761369173</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>98202958</v>
+        <v>98156372</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230083</v>
+        <v>230080</v>
       </c>
       <c r="D487" t="n">
         <v>33834</v>
       </c>
       <c r="E487" t="n">
-        <v>1801990470</v>
+        <v>1801816842</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12209</v>
+        <v>12207</v>
       </c>
       <c r="D491" t="n">
         <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>74110981</v>
+        <v>74107425</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184197</v>
+        <v>184196</v>
       </c>
       <c r="D505" t="n">
         <v>27732</v>
       </c>
       <c r="E505" t="n">
-        <v>332561206</v>
+        <v>332557721</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56033</v>
+        <v>56031</v>
       </c>
       <c r="D520" t="n">
         <v>8768</v>
       </c>
       <c r="E520" t="n">
-        <v>252149237</v>
+        <v>252086256</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27889,13 +27889,13 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="D539" t="n">
         <v>248</v>
       </c>
       <c r="E539" t="n">
-        <v>7581562</v>
+        <v>7569421</v>
       </c>
       <c r="F539" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>24513</v>
+        <v>24512</v>
       </c>
       <c r="D545" t="n">
         <v>6169</v>
       </c>
       <c r="E545" t="n">
-        <v>88165149</v>
+        <v>88163649</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39269</v>
+        <v>39255</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>59810882</v>
+        <v>59799025</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>17975</v>
+        <v>17967</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>69519959</v>
+        <v>69446902</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28858,13 +28858,13 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D558" t="n">
         <v>133</v>
       </c>
       <c r="E558" t="n">
-        <v>1388087</v>
+        <v>1385587</v>
       </c>
       <c r="F558" t="inlineStr">
         <is>
@@ -31153,13 +31153,13 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>32182</v>
+        <v>32181</v>
       </c>
       <c r="D603" t="n">
         <v>6078</v>
       </c>
       <c r="E603" t="n">
-        <v>170257117</v>
+        <v>170255679</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -41863,13 +41863,13 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>50343</v>
+        <v>50342</v>
       </c>
       <c r="D813" t="n">
         <v>10678</v>
       </c>
       <c r="E813" t="n">
-        <v>86497731</v>
+        <v>86496231</v>
       </c>
       <c r="F813" t="inlineStr">
         <is>
@@ -43444,13 +43444,13 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>58388</v>
+        <v>58387</v>
       </c>
       <c r="D844" t="n">
         <v>11374</v>
       </c>
       <c r="E844" t="n">
-        <v>290384699</v>
+        <v>290383199</v>
       </c>
       <c r="F844" t="inlineStr">
         <is>
@@ -44923,13 +44923,13 @@
         </is>
       </c>
       <c r="C873" t="n">
-        <v>41827</v>
+        <v>41825</v>
       </c>
       <c r="D873" t="n">
         <v>9646</v>
       </c>
       <c r="E873" t="n">
-        <v>75019853</v>
+        <v>75018942</v>
       </c>
       <c r="F873" t="inlineStr">
         <is>
@@ -45994,13 +45994,13 @@
         </is>
       </c>
       <c r="C894" t="n">
-        <v>167269</v>
+        <v>167268</v>
       </c>
       <c r="D894" t="n">
         <v>30742</v>
       </c>
       <c r="E894" t="n">
-        <v>280748586</v>
+        <v>280746100</v>
       </c>
       <c r="F894" t="inlineStr">
         <is>
@@ -47065,13 +47065,13 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>96838</v>
+        <v>96837</v>
       </c>
       <c r="D915" t="n">
         <v>17575</v>
       </c>
       <c r="E915" t="n">
-        <v>463179168</v>
+        <v>463177376</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79063</v>
+        <v>79062</v>
       </c>
       <c r="D918" t="n">
         <v>13382</v>
       </c>
       <c r="E918" t="n">
-        <v>390375033</v>
+        <v>390373035</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -47932,13 +47932,13 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>127919</v>
+        <v>127918</v>
       </c>
       <c r="D932" t="n">
         <v>26954</v>
       </c>
       <c r="E932" t="n">
-        <v>215181430</v>
+        <v>215179588</v>
       </c>
       <c r="F932" t="inlineStr">
         <is>
@@ -48646,13 +48646,13 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>29823</v>
+        <v>29822</v>
       </c>
       <c r="D946" t="n">
         <v>5383</v>
       </c>
       <c r="E946" t="n">
-        <v>141907706</v>
+        <v>141897706</v>
       </c>
       <c r="F946" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-02-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1267,13 +1267,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4548</v>
+        <v>4550</v>
       </c>
       <c r="D17" t="n">
         <v>831</v>
       </c>
       <c r="E17" t="n">
-        <v>22857743</v>
+        <v>22865659</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>186330</v>
+        <v>186331</v>
       </c>
       <c r="D100" t="n">
         <v>37747</v>
       </c>
       <c r="E100" t="n">
-        <v>306246664</v>
+        <v>306246904</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>84939</v>
+        <v>84944</v>
       </c>
       <c r="D105" t="n">
         <v>16087</v>
       </c>
       <c r="E105" t="n">
-        <v>401394388</v>
+        <v>401454980</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62490</v>
+        <v>62491</v>
       </c>
       <c r="D108" t="n">
         <v>10954</v>
       </c>
       <c r="E108" t="n">
-        <v>339992241</v>
+        <v>340002241</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -10192,13 +10192,13 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>37577</v>
+        <v>37579</v>
       </c>
       <c r="D192" t="n">
         <v>8493</v>
       </c>
       <c r="E192" t="n">
-        <v>76083324</v>
+        <v>76083396</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -12895,13 +12895,13 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>5775</v>
+        <v>5776</v>
       </c>
       <c r="D245" t="n">
         <v>1133</v>
       </c>
       <c r="E245" t="n">
-        <v>24337561</v>
+        <v>24343308</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -15088,13 +15088,13 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>14204</v>
+        <v>14205</v>
       </c>
       <c r="D288" t="n">
         <v>2289</v>
       </c>
       <c r="E288" t="n">
-        <v>94110798</v>
+        <v>94111398</v>
       </c>
       <c r="F288" t="inlineStr">
         <is>
@@ -16006,13 +16006,13 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>6083</v>
+        <v>6084</v>
       </c>
       <c r="D306" t="n">
         <v>1239</v>
       </c>
       <c r="E306" t="n">
-        <v>26900708</v>
+        <v>26906084</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
@@ -16771,13 +16771,13 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>76024</v>
+        <v>76025</v>
       </c>
       <c r="D321" t="n">
         <v>15907</v>
       </c>
       <c r="E321" t="n">
-        <v>132420461</v>
+        <v>132426430</v>
       </c>
       <c r="F321" t="inlineStr">
         <is>
@@ -17077,13 +17077,13 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>47890</v>
+        <v>47891</v>
       </c>
       <c r="D327" t="n">
         <v>9067</v>
       </c>
       <c r="E327" t="n">
-        <v>240480465</v>
+        <v>240487313</v>
       </c>
       <c r="F327" t="inlineStr">
         <is>
@@ -17995,13 +17995,13 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D345" t="n">
         <v>21</v>
       </c>
       <c r="E345" t="n">
-        <v>5633874</v>
+        <v>5675074</v>
       </c>
       <c r="F345" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18404</v>
+        <v>18405</v>
       </c>
       <c r="D399" t="n">
         <v>3382</v>
       </c>
       <c r="E399" t="n">
-        <v>72097061</v>
+        <v>72117092</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16554</v>
+        <v>16555</v>
       </c>
       <c r="D401" t="n">
         <v>2942</v>
       </c>
       <c r="E401" t="n">
-        <v>48244387</v>
+        <v>48245887</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -22075,13 +22075,13 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>70509</v>
+        <v>70510</v>
       </c>
       <c r="D425" t="n">
         <v>13142</v>
       </c>
       <c r="E425" t="n">
-        <v>343021318</v>
+        <v>343031318</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -22585,13 +22585,13 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>20230</v>
+        <v>20231</v>
       </c>
       <c r="D435" t="n">
         <v>4036</v>
       </c>
       <c r="E435" t="n">
-        <v>93010853</v>
+        <v>93020853</v>
       </c>
       <c r="F435" t="inlineStr">
         <is>
@@ -22687,13 +22687,13 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>14441</v>
+        <v>14442</v>
       </c>
       <c r="D437" t="n">
-        <v>2513</v>
+        <v>2514</v>
       </c>
       <c r="E437" t="n">
-        <v>69127602</v>
+        <v>69130582</v>
       </c>
       <c r="F437" t="inlineStr">
         <is>
@@ -23044,13 +23044,13 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>31758</v>
+        <v>31759</v>
       </c>
       <c r="D444" t="n">
         <v>6195</v>
       </c>
       <c r="E444" t="n">
-        <v>161380032</v>
+        <v>161385286</v>
       </c>
       <c r="F444" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35033</v>
+        <v>35036</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>159828648</v>
+        <v>159879837</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416403</v>
+        <v>416409</v>
       </c>
       <c r="D477" t="n">
         <v>70491</v>
       </c>
       <c r="E477" t="n">
-        <v>723832135</v>
+        <v>723871781</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24982,13 +24982,13 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>4134</v>
+        <v>4135</v>
       </c>
       <c r="D482" t="n">
         <v>520</v>
       </c>
       <c r="E482" t="n">
-        <v>69648130</v>
+        <v>69649630</v>
       </c>
       <c r="F482" t="inlineStr">
         <is>
@@ -25033,13 +25033,13 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D483" t="n">
         <v>33</v>
       </c>
       <c r="E483" t="n">
-        <v>5323530</v>
+        <v>5333530</v>
       </c>
       <c r="F483" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291440</v>
+        <v>291449</v>
       </c>
       <c r="D484" t="n">
         <v>42556</v>
       </c>
       <c r="E484" t="n">
-        <v>1761369173</v>
+        <v>1761471642</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3036</v>
+        <v>3037</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>98156372</v>
+        <v>98202958</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230080</v>
+        <v>230083</v>
       </c>
       <c r="D487" t="n">
         <v>33834</v>
       </c>
       <c r="E487" t="n">
-        <v>1801816842</v>
+        <v>1801990470</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12207</v>
+        <v>12209</v>
       </c>
       <c r="D491" t="n">
         <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>74107425</v>
+        <v>74110981</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184196</v>
+        <v>184197</v>
       </c>
       <c r="D505" t="n">
         <v>27732</v>
       </c>
       <c r="E505" t="n">
-        <v>332557721</v>
+        <v>332561206</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56031</v>
+        <v>56033</v>
       </c>
       <c r="D520" t="n">
         <v>8768</v>
       </c>
       <c r="E520" t="n">
-        <v>252086256</v>
+        <v>252149237</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27889,13 +27889,13 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D539" t="n">
         <v>248</v>
       </c>
       <c r="E539" t="n">
-        <v>7569421</v>
+        <v>7581562</v>
       </c>
       <c r="F539" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>24512</v>
+        <v>24513</v>
       </c>
       <c r="D545" t="n">
         <v>6169</v>
       </c>
       <c r="E545" t="n">
-        <v>88163649</v>
+        <v>88165149</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39255</v>
+        <v>39269</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>59799025</v>
+        <v>59810882</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>17967</v>
+        <v>17975</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>69446902</v>
+        <v>69519959</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28858,13 +28858,13 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D558" t="n">
         <v>133</v>
       </c>
       <c r="E558" t="n">
-        <v>1385587</v>
+        <v>1388087</v>
       </c>
       <c r="F558" t="inlineStr">
         <is>
@@ -31153,13 +31153,13 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>32181</v>
+        <v>32182</v>
       </c>
       <c r="D603" t="n">
         <v>6078</v>
       </c>
       <c r="E603" t="n">
-        <v>170255679</v>
+        <v>170257117</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -41863,13 +41863,13 @@
         </is>
       </c>
       <c r="C813" t="n">
-        <v>50342</v>
+        <v>50343</v>
       </c>
       <c r="D813" t="n">
         <v>10678</v>
       </c>
       <c r="E813" t="n">
-        <v>86496231</v>
+        <v>86497731</v>
       </c>
       <c r="F813" t="inlineStr">
         <is>
@@ -43444,13 +43444,13 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>58387</v>
+        <v>58388</v>
       </c>
       <c r="D844" t="n">
         <v>11374</v>
       </c>
       <c r="E844" t="n">
-        <v>290383199</v>
+        <v>290384699</v>
       </c>
       <c r="F844" t="inlineStr">
         <is>
@@ -44923,13 +44923,13 @@
         </is>
       </c>
       <c r="C873" t="n">
-        <v>41825</v>
+        <v>41827</v>
       </c>
       <c r="D873" t="n">
         <v>9646</v>
       </c>
       <c r="E873" t="n">
-        <v>75018942</v>
+        <v>75019853</v>
       </c>
       <c r="F873" t="inlineStr">
         <is>
@@ -45994,13 +45994,13 @@
         </is>
       </c>
       <c r="C894" t="n">
-        <v>167268</v>
+        <v>167269</v>
       </c>
       <c r="D894" t="n">
         <v>30742</v>
       </c>
       <c r="E894" t="n">
-        <v>280746100</v>
+        <v>280748586</v>
       </c>
       <c r="F894" t="inlineStr">
         <is>
@@ -47065,13 +47065,13 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>96837</v>
+        <v>96838</v>
       </c>
       <c r="D915" t="n">
         <v>17575</v>
       </c>
       <c r="E915" t="n">
-        <v>463177376</v>
+        <v>463179168</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79062</v>
+        <v>79063</v>
       </c>
       <c r="D918" t="n">
         <v>13382</v>
       </c>
       <c r="E918" t="n">
-        <v>390373035</v>
+        <v>390375033</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -47932,13 +47932,13 @@
         </is>
       </c>
       <c r="C932" t="n">
-        <v>127918</v>
+        <v>127919</v>
       </c>
       <c r="D932" t="n">
         <v>26954</v>
       </c>
       <c r="E932" t="n">
-        <v>215179588</v>
+        <v>215181430</v>
       </c>
       <c r="F932" t="inlineStr">
         <is>
@@ -48646,13 +48646,13 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>29822</v>
+        <v>29823</v>
       </c>
       <c r="D946" t="n">
         <v>5383</v>
       </c>
       <c r="E946" t="n">
-        <v>141897706</v>
+        <v>141907706</v>
       </c>
       <c r="F946" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-10 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105817</v>
+        <v>105816</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186616008</v>
+        <v>186614253</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>186356</v>
+        <v>186357</v>
       </c>
       <c r="D100" t="n">
         <v>37749</v>
       </c>
       <c r="E100" t="n">
-        <v>306308327</v>
+        <v>306312150</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62513</v>
+        <v>62514</v>
       </c>
       <c r="D108" t="n">
         <v>10954</v>
       </c>
       <c r="E108" t="n">
-        <v>340290180</v>
+        <v>340490180</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88466</v>
+        <v>88468</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216744449</v>
+        <v>216749459</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -6571,13 +6571,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>14631</v>
+        <v>14632</v>
       </c>
       <c r="D121" t="n">
         <v>2285</v>
       </c>
       <c r="E121" t="n">
-        <v>166810085</v>
+        <v>166992531</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -14629,13 +14629,13 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>10477</v>
+        <v>10478</v>
       </c>
       <c r="D279" t="n">
         <v>2119</v>
       </c>
       <c r="E279" t="n">
-        <v>50258881</v>
+        <v>50264281</v>
       </c>
       <c r="F279" t="inlineStr">
         <is>
@@ -15649,13 +15649,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>9029</v>
+        <v>9026</v>
       </c>
       <c r="D299" t="n">
         <v>1438</v>
       </c>
       <c r="E299" t="n">
-        <v>49918414</v>
+        <v>49891360</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -17944,13 +17944,13 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>28868</v>
+        <v>28869</v>
       </c>
       <c r="D344" t="n">
         <v>5352</v>
       </c>
       <c r="E344" t="n">
-        <v>158914675</v>
+        <v>158938232</v>
       </c>
       <c r="F344" t="inlineStr">
         <is>
@@ -20341,13 +20341,13 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>13983</v>
+        <v>13984</v>
       </c>
       <c r="D391" t="n">
         <v>2759</v>
       </c>
       <c r="E391" t="n">
-        <v>63992975</v>
+        <v>63997173</v>
       </c>
       <c r="F391" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71234</v>
+        <v>71246</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110272213</v>
+        <v>110277178</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18837</v>
+        <v>18836</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75052351</v>
+        <v>75024804</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16904</v>
+        <v>16911</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50383889</v>
+        <v>50425027</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9325</v>
+        <v>9326</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23677096</v>
+        <v>23686296</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -21871,13 +21871,13 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>145340</v>
+        <v>145341</v>
       </c>
       <c r="D421" t="n">
         <v>30579</v>
       </c>
       <c r="E421" t="n">
-        <v>246833634</v>
+        <v>246840415</v>
       </c>
       <c r="F421" t="inlineStr">
         <is>
@@ -22228,13 +22228,13 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>40397</v>
+        <v>40398</v>
       </c>
       <c r="D428" t="n">
         <v>6930</v>
       </c>
       <c r="E428" t="n">
-        <v>214794795</v>
+        <v>214795790</v>
       </c>
       <c r="F428" t="inlineStr">
         <is>
@@ -23554,13 +23554,13 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>12239</v>
+        <v>12238</v>
       </c>
       <c r="D454" t="n">
         <v>2377</v>
       </c>
       <c r="E454" t="n">
-        <v>66592456</v>
+        <v>66590896</v>
       </c>
       <c r="F454" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35046</v>
+        <v>35048</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>160107500</v>
+        <v>160117921</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24268,13 +24268,13 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>164675</v>
+        <v>164676</v>
       </c>
       <c r="D468" t="n">
-        <v>27309</v>
+        <v>27310</v>
       </c>
       <c r="E468" t="n">
-        <v>287058129</v>
+        <v>287059661</v>
       </c>
       <c r="F468" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73739</v>
+        <v>73741</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386230756</v>
+        <v>386233213</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74974</v>
+        <v>74975</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>434143030</v>
+        <v>434343030</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416589</v>
+        <v>416585</v>
       </c>
       <c r="D477" t="n">
-        <v>70494</v>
+        <v>70495</v>
       </c>
       <c r="E477" t="n">
-        <v>724710605</v>
+        <v>724623272</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291783</v>
+        <v>291772</v>
       </c>
       <c r="D484" t="n">
         <v>42562</v>
       </c>
       <c r="E484" t="n">
-        <v>1766328544</v>
+        <v>1766246969</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>99344175</v>
+        <v>99339705</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230419</v>
+        <v>230414</v>
       </c>
       <c r="D487" t="n">
         <v>33842</v>
       </c>
       <c r="E487" t="n">
-        <v>1812330499</v>
+        <v>1812124067</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12241</v>
+        <v>12240</v>
       </c>
       <c r="D491" t="n">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>75399746</v>
+        <v>75396798</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62165</v>
+        <v>62166</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>298500853</v>
+        <v>298518861</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71168</v>
+        <v>71160</v>
       </c>
       <c r="D511" t="n">
         <v>10922</v>
       </c>
       <c r="E511" t="n">
-        <v>286903932</v>
+        <v>286488150</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56087</v>
+        <v>56085</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253210292</v>
+        <v>253185332</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27481,13 +27481,13 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>98235</v>
+        <v>98236</v>
       </c>
       <c r="D531" t="n">
         <v>19246</v>
       </c>
       <c r="E531" t="n">
-        <v>165241680</v>
+        <v>165243320</v>
       </c>
       <c r="F531" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76626</v>
+        <v>76627</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114123502</v>
+        <v>114124865</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25034</v>
+        <v>25047</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92043375</v>
+        <v>92100271</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39903</v>
+        <v>39911</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60347848</v>
+        <v>60347099</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18422</v>
+        <v>18423</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72341763</v>
+        <v>72343317</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12388</v>
+        <v>12389</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>39959770</v>
+        <v>39983570</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -30490,13 +30490,13 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D590" t="n">
         <v>157</v>
       </c>
       <c r="E590" t="n">
-        <v>4605934</v>
+        <v>4694818</v>
       </c>
       <c r="F590" t="inlineStr">
         <is>
@@ -30949,13 +30949,13 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>66143</v>
+        <v>66144</v>
       </c>
       <c r="D599" t="n">
         <v>14270</v>
       </c>
       <c r="E599" t="n">
-        <v>120502250</v>
+        <v>120508743</v>
       </c>
       <c r="F599" t="inlineStr">
         <is>
@@ -31612,13 +31612,13 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>9698</v>
+        <v>9699</v>
       </c>
       <c r="D612" t="n">
         <v>1964</v>
       </c>
       <c r="E612" t="n">
-        <v>47949364</v>
+        <v>47994364</v>
       </c>
       <c r="F612" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163430</v>
+        <v>163429</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278422088</v>
+        <v>278421637</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73196</v>
+        <v>73197</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367141670</v>
+        <v>367142267</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -37936,13 +37936,13 @@
         </is>
       </c>
       <c r="C736" t="n">
-        <v>26808</v>
+        <v>26809</v>
       </c>
       <c r="D736" t="n">
         <v>5726</v>
       </c>
       <c r="E736" t="n">
-        <v>51203410</v>
+        <v>51206159</v>
       </c>
       <c r="F736" t="inlineStr">
         <is>
@@ -43444,13 +43444,13 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>58392</v>
+        <v>58391</v>
       </c>
       <c r="D844" t="n">
-        <v>11375</v>
+        <v>11374</v>
       </c>
       <c r="E844" t="n">
-        <v>290405101</v>
+        <v>290395101</v>
       </c>
       <c r="F844" t="inlineStr">
         <is>
@@ -43852,13 +43852,13 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>27076</v>
+        <v>27074</v>
       </c>
       <c r="D852" t="n">
         <v>5532</v>
       </c>
       <c r="E852" t="n">
-        <v>133385704</v>
+        <v>133339983</v>
       </c>
       <c r="F852" t="inlineStr">
         <is>
@@ -46351,13 +46351,13 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>81808</v>
+        <v>81809</v>
       </c>
       <c r="D901" t="n">
         <v>13203</v>
       </c>
       <c r="E901" t="n">
-        <v>443358990</v>
+        <v>443365592</v>
       </c>
       <c r="F901" t="inlineStr">
         <is>
@@ -47320,13 +47320,13 @@
         </is>
       </c>
       <c r="C920" t="n">
-        <v>8093</v>
+        <v>8094</v>
       </c>
       <c r="D920" t="n">
         <v>1180</v>
       </c>
       <c r="E920" t="n">
-        <v>30412786</v>
+        <v>30424296</v>
       </c>
       <c r="F920" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-11 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105819</v>
+        <v>105821</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186621981</v>
+        <v>186623631</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -5296,13 +5296,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>10187</v>
+        <v>10188</v>
       </c>
       <c r="D96" t="n">
         <v>1862</v>
       </c>
       <c r="E96" t="n">
-        <v>57988922</v>
+        <v>57991098</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88468</v>
+        <v>88469</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216749459</v>
+        <v>216751125</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -13660,13 +13660,13 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>22633</v>
+        <v>22634</v>
       </c>
       <c r="D260" t="n">
         <v>4189</v>
       </c>
       <c r="E260" t="n">
-        <v>112140012</v>
+        <v>112152305</v>
       </c>
       <c r="F260" t="inlineStr">
         <is>
@@ -15088,13 +15088,13 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>14211</v>
+        <v>14212</v>
       </c>
       <c r="D288" t="n">
         <v>2289</v>
       </c>
       <c r="E288" t="n">
-        <v>94252714</v>
+        <v>94261000</v>
       </c>
       <c r="F288" t="inlineStr">
         <is>
@@ -15649,13 +15649,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>9026</v>
+        <v>9027</v>
       </c>
       <c r="D299" t="n">
         <v>1438</v>
       </c>
       <c r="E299" t="n">
-        <v>49891360</v>
+        <v>49908539</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -17995,13 +17995,13 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D345" t="n">
         <v>21</v>
       </c>
       <c r="E345" t="n">
-        <v>5675074</v>
+        <v>5870275</v>
       </c>
       <c r="F345" t="inlineStr">
         <is>
@@ -20443,13 +20443,13 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>5430</v>
+        <v>5431</v>
       </c>
       <c r="D393" t="n">
         <v>1019</v>
       </c>
       <c r="E393" t="n">
-        <v>28228173</v>
+        <v>28230358</v>
       </c>
       <c r="F393" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71248</v>
+        <v>71256</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110277738</v>
+        <v>110281502</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18836</v>
+        <v>18840</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75024804</v>
+        <v>75078847</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -21004,13 +21004,13 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>29539</v>
+        <v>29541</v>
       </c>
       <c r="D404" t="n">
         <v>3814</v>
       </c>
       <c r="E404" t="n">
-        <v>56426825</v>
+        <v>56427433</v>
       </c>
       <c r="F404" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9326</v>
+        <v>9328</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23686296</v>
+        <v>23689436</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -22075,13 +22075,13 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>70533</v>
+        <v>70534</v>
       </c>
       <c r="D425" t="n">
         <v>13142</v>
       </c>
       <c r="E425" t="n">
-        <v>343478433</v>
+        <v>343483488</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -22228,13 +22228,13 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>40398</v>
+        <v>40399</v>
       </c>
       <c r="D428" t="n">
         <v>6930</v>
       </c>
       <c r="E428" t="n">
-        <v>214795790</v>
+        <v>214995790</v>
       </c>
       <c r="F428" t="inlineStr">
         <is>
@@ -22840,13 +22840,13 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>73244</v>
+        <v>73245</v>
       </c>
       <c r="D440" t="n">
         <v>15804</v>
       </c>
       <c r="E440" t="n">
-        <v>130263162</v>
+        <v>130263838</v>
       </c>
       <c r="F440" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416598</v>
+        <v>416600</v>
       </c>
       <c r="D477" t="n">
         <v>70496</v>
       </c>
       <c r="E477" t="n">
-        <v>724660973</v>
+        <v>724664616</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291792</v>
+        <v>291809</v>
       </c>
       <c r="D484" t="n">
         <v>42562</v>
       </c>
       <c r="E484" t="n">
-        <v>1766503326</v>
+        <v>1766757877</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230422</v>
+        <v>230432</v>
       </c>
       <c r="D487" t="n">
         <v>33844</v>
       </c>
       <c r="E487" t="n">
-        <v>1812181711</v>
+        <v>1812295997</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184233</v>
+        <v>184235</v>
       </c>
       <c r="D505" t="n">
         <v>27735</v>
       </c>
       <c r="E505" t="n">
-        <v>332672964</v>
+        <v>332674960</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71160</v>
+        <v>71162</v>
       </c>
       <c r="D511" t="n">
         <v>10922</v>
       </c>
       <c r="E511" t="n">
-        <v>286488150</v>
+        <v>286499687</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -27736,13 +27736,13 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>37773</v>
+        <v>37774</v>
       </c>
       <c r="D536" t="n">
         <v>6687</v>
       </c>
       <c r="E536" t="n">
-        <v>172977992</v>
+        <v>173177992</v>
       </c>
       <c r="F536" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76627</v>
+        <v>76633</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114124865</v>
+        <v>114126711</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25048</v>
+        <v>25055</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92102558</v>
+        <v>92126085</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28246,13 +28246,13 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D546" t="n">
         <v>14</v>
       </c>
       <c r="E546" t="n">
-        <v>6189889</v>
+        <v>6360066</v>
       </c>
       <c r="F546" t="inlineStr">
         <is>
@@ -28297,13 +28297,13 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>7433</v>
+        <v>7437</v>
       </c>
       <c r="D547" t="n">
         <v>1667</v>
       </c>
       <c r="E547" t="n">
-        <v>37655642</v>
+        <v>37677476</v>
       </c>
       <c r="F547" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39913</v>
+        <v>39917</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60354039</v>
+        <v>60356678</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18423</v>
+        <v>18426</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72343317</v>
+        <v>72350486</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12389</v>
+        <v>12390</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>39983570</v>
+        <v>39995711</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -28960,13 +28960,13 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>43845</v>
+        <v>43846</v>
       </c>
       <c r="D560" t="n">
         <v>5415</v>
       </c>
       <c r="E560" t="n">
-        <v>101309981</v>
+        <v>101311481</v>
       </c>
       <c r="F560" t="inlineStr">
         <is>
@@ -31612,13 +31612,13 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>9699</v>
+        <v>9700</v>
       </c>
       <c r="D612" t="n">
         <v>1964</v>
       </c>
       <c r="E612" t="n">
-        <v>47994364</v>
+        <v>48001469</v>
       </c>
       <c r="F612" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73197</v>
+        <v>73198</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367142267</v>
+        <v>367142864</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -36355,13 +36355,13 @@
         </is>
       </c>
       <c r="C705" t="n">
-        <v>13799</v>
+        <v>13800</v>
       </c>
       <c r="D705" t="n">
         <v>2476</v>
       </c>
       <c r="E705" t="n">
-        <v>77906892</v>
+        <v>78001970</v>
       </c>
       <c r="F705" t="inlineStr">
         <is>
@@ -37885,13 +37885,13 @@
         </is>
       </c>
       <c r="C735" t="n">
-        <v>1166</v>
+        <v>1179</v>
       </c>
       <c r="D735" t="n">
         <v>175</v>
       </c>
       <c r="E735" t="n">
-        <v>4744845</v>
+        <v>4792653</v>
       </c>
       <c r="F735" t="inlineStr">
         <is>
@@ -40843,13 +40843,13 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>63449</v>
+        <v>63451</v>
       </c>
       <c r="D793" t="n">
         <v>11594</v>
       </c>
       <c r="E793" t="n">
-        <v>307268920</v>
+        <v>307274782</v>
       </c>
       <c r="F793" t="inlineStr">
         <is>
@@ -43240,13 +43240,13 @@
         </is>
       </c>
       <c r="C840" t="n">
-        <v>95913</v>
+        <v>95914</v>
       </c>
       <c r="D840" t="n">
         <v>22285</v>
       </c>
       <c r="E840" t="n">
-        <v>162851256</v>
+        <v>162851683</v>
       </c>
       <c r="F840" t="inlineStr">
         <is>
@@ -47065,13 +47065,13 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>96852</v>
+        <v>96854</v>
       </c>
       <c r="D915" t="n">
         <v>17575</v>
       </c>
       <c r="E915" t="n">
-        <v>463299858</v>
+        <v>463304681</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79075</v>
+        <v>79076</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391005220</v>
+        <v>391015220</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -48136,13 +48136,13 @@
         </is>
       </c>
       <c r="C936" t="n">
-        <v>53208</v>
+        <v>53209</v>
       </c>
       <c r="D936" t="n">
         <v>10126</v>
       </c>
       <c r="E936" t="n">
-        <v>267696103</v>
+        <v>267701946</v>
       </c>
       <c r="F936" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-12 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3511,13 +3511,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>47710</v>
+        <v>47712</v>
       </c>
       <c r="D61" t="n">
         <v>8058</v>
       </c>
       <c r="E61" t="n">
-        <v>305736686</v>
+        <v>305766805</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -6520,13 +6520,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D120" t="n">
         <v>50</v>
       </c>
       <c r="E120" t="n">
-        <v>17480759</v>
+        <v>17611036</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -6571,13 +6571,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>14632</v>
+        <v>14633</v>
       </c>
       <c r="D121" t="n">
         <v>2285</v>
       </c>
       <c r="E121" t="n">
-        <v>166992531</v>
+        <v>167108722</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71256</v>
+        <v>71261</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110281502</v>
+        <v>110287231</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18840</v>
+        <v>18845</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75078847</v>
+        <v>75099352</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16911</v>
+        <v>16917</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50425027</v>
+        <v>50434566</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21106,13 +21106,13 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>6284</v>
+        <v>6285</v>
       </c>
       <c r="D406" t="n">
         <v>911</v>
       </c>
       <c r="E406" t="n">
-        <v>19289207</v>
+        <v>19290013</v>
       </c>
       <c r="F406" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9328</v>
+        <v>9333</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23689436</v>
+        <v>23704653</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -22075,13 +22075,13 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>70534</v>
+        <v>70535</v>
       </c>
       <c r="D425" t="n">
         <v>13142</v>
       </c>
       <c r="E425" t="n">
-        <v>343483488</v>
+        <v>343510010</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -22330,13 +22330,13 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>4612</v>
+        <v>4613</v>
       </c>
       <c r="D430" t="n">
         <v>698</v>
       </c>
       <c r="E430" t="n">
-        <v>21810497</v>
+        <v>21811728</v>
       </c>
       <c r="F430" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73743</v>
+        <v>73745</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386286610</v>
+        <v>386330290</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74978</v>
+        <v>74979</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>434640907</v>
+        <v>434681221</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416603</v>
+        <v>416617</v>
       </c>
       <c r="D477" t="n">
         <v>70497</v>
       </c>
       <c r="E477" t="n">
-        <v>724677058</v>
+        <v>724724257</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291829</v>
+        <v>291839</v>
       </c>
       <c r="D484" t="n">
         <v>42562</v>
       </c>
       <c r="E484" t="n">
-        <v>1767125717</v>
+        <v>1767314795</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3047</v>
+        <v>3048</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>99339705</v>
+        <v>99419703</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230438</v>
+        <v>230458</v>
       </c>
       <c r="D487" t="n">
-        <v>33844</v>
+        <v>33845</v>
       </c>
       <c r="E487" t="n">
-        <v>1812326466</v>
+        <v>1813660978</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184237</v>
+        <v>184238</v>
       </c>
       <c r="D505" t="n">
         <v>27736</v>
       </c>
       <c r="E505" t="n">
-        <v>332677072</v>
+        <v>332679772</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56087</v>
+        <v>56089</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253261587</v>
+        <v>253510639</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27736,13 +27736,13 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>37774</v>
+        <v>37777</v>
       </c>
       <c r="D536" t="n">
         <v>6687</v>
       </c>
       <c r="E536" t="n">
-        <v>173177992</v>
+        <v>173248686</v>
       </c>
       <c r="F536" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76633</v>
+        <v>76637</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114126711</v>
+        <v>114129393</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25055</v>
+        <v>25065</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92126085</v>
+        <v>92331999</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28246,13 +28246,13 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D546" t="n">
         <v>14</v>
       </c>
       <c r="E546" t="n">
-        <v>6360066</v>
+        <v>6534296</v>
       </c>
       <c r="F546" t="inlineStr">
         <is>
@@ -28297,13 +28297,13 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>7437</v>
+        <v>7438</v>
       </c>
       <c r="D547" t="n">
         <v>1667</v>
       </c>
       <c r="E547" t="n">
-        <v>37677476</v>
+        <v>37681278</v>
       </c>
       <c r="F547" t="inlineStr">
         <is>
@@ -28501,13 +28501,13 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="D551" t="n">
         <v>175</v>
       </c>
       <c r="E551" t="n">
-        <v>2011806</v>
+        <v>2015502</v>
       </c>
       <c r="F551" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39917</v>
+        <v>39920</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60356678</v>
+        <v>60358891</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18429</v>
+        <v>18430</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72553333</v>
+        <v>72554723</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12390</v>
+        <v>12394</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>39995711</v>
+        <v>40027556</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -31612,13 +31612,13 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>9700</v>
+        <v>9701</v>
       </c>
       <c r="D612" t="n">
         <v>1964</v>
       </c>
       <c r="E612" t="n">
-        <v>48001469</v>
+        <v>48023701</v>
       </c>
       <c r="F612" t="inlineStr">
         <is>
@@ -31816,13 +31816,13 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D616" t="n">
         <v>142</v>
       </c>
       <c r="E616" t="n">
-        <v>3300738</v>
+        <v>3305706</v>
       </c>
       <c r="F616" t="inlineStr">
         <is>
@@ -34978,13 +34978,13 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>11103</v>
+        <v>11107</v>
       </c>
       <c r="D678" t="n">
         <v>2218</v>
       </c>
       <c r="E678" t="n">
-        <v>55909400</v>
+        <v>55930968</v>
       </c>
       <c r="F678" t="inlineStr">
         <is>
@@ -43444,13 +43444,13 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>58391</v>
+        <v>58393</v>
       </c>
       <c r="D844" t="n">
         <v>11374</v>
       </c>
       <c r="E844" t="n">
-        <v>290395101</v>
+        <v>290406601</v>
       </c>
       <c r="F844" t="inlineStr">
         <is>
@@ -44515,13 +44515,13 @@
         </is>
       </c>
       <c r="C865" t="n">
-        <v>28824</v>
+        <v>28825</v>
       </c>
       <c r="D865" t="n">
         <v>6343</v>
       </c>
       <c r="E865" t="n">
-        <v>53403627</v>
+        <v>53407166</v>
       </c>
       <c r="F865" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79078</v>
+        <v>79080</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391231708</v>
+        <v>391401403</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -48238,13 +48238,13 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>38551</v>
+        <v>38552</v>
       </c>
       <c r="D938" t="n">
         <v>6910</v>
       </c>
       <c r="E938" t="n">
-        <v>195227309</v>
+        <v>195262936</v>
       </c>
       <c r="F938" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-13 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105822</v>
+        <v>105825</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186626159</v>
+        <v>186635544</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -4276,13 +4276,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>28518</v>
+        <v>28519</v>
       </c>
       <c r="D76" t="n">
         <v>5076</v>
       </c>
       <c r="E76" t="n">
-        <v>158498679</v>
+        <v>158500134</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>84958</v>
+        <v>84959</v>
       </c>
       <c r="D105" t="n">
         <v>16087</v>
       </c>
       <c r="E105" t="n">
-        <v>401635674</v>
+        <v>401645674</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -6571,13 +6571,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>14633</v>
+        <v>14634</v>
       </c>
       <c r="D121" t="n">
-        <v>2285</v>
+        <v>2286</v>
       </c>
       <c r="E121" t="n">
-        <v>167108722</v>
+        <v>167168716</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -12793,13 +12793,13 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>10445</v>
+        <v>10446</v>
       </c>
       <c r="D243" t="n">
         <v>2230</v>
       </c>
       <c r="E243" t="n">
-        <v>48577712</v>
+        <v>48587712</v>
       </c>
       <c r="F243" t="inlineStr">
         <is>
@@ -19882,13 +19882,13 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>25390</v>
+        <v>25391</v>
       </c>
       <c r="D382" t="n">
         <v>5083</v>
       </c>
       <c r="E382" t="n">
-        <v>129164110</v>
+        <v>129169663</v>
       </c>
       <c r="F382" t="inlineStr">
         <is>
@@ -19984,13 +19984,13 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>16791</v>
+        <v>16792</v>
       </c>
       <c r="D384" t="n">
         <v>3259</v>
       </c>
       <c r="E384" t="n">
-        <v>80747329</v>
+        <v>80750829</v>
       </c>
       <c r="F384" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71261</v>
+        <v>71264</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110287231</v>
+        <v>110294557</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18845</v>
+        <v>18848</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75099352</v>
+        <v>75117834</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16921</v>
+        <v>16923</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50436644</v>
+        <v>50452265</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73745</v>
+        <v>73746</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386330290</v>
+        <v>386348384</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416619</v>
+        <v>416626</v>
       </c>
       <c r="D477" t="n">
-        <v>70497</v>
+        <v>70498</v>
       </c>
       <c r="E477" t="n">
-        <v>724734682</v>
+        <v>724749754</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24778,13 +24778,13 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D478" t="n">
         <v>23</v>
       </c>
       <c r="E478" t="n">
-        <v>664607</v>
+        <v>665363</v>
       </c>
       <c r="F478" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291845</v>
+        <v>291855</v>
       </c>
       <c r="D484" t="n">
         <v>42564</v>
       </c>
       <c r="E484" t="n">
-        <v>1767518345</v>
+        <v>1767581398</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230475</v>
+        <v>230488</v>
       </c>
       <c r="D487" t="n">
         <v>33846</v>
       </c>
       <c r="E487" t="n">
-        <v>1814465772</v>
+        <v>1815156171</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12242</v>
+        <v>12245</v>
       </c>
       <c r="D491" t="n">
         <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>75403155</v>
+        <v>75461668</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71163</v>
+        <v>71164</v>
       </c>
       <c r="D511" t="n">
         <v>10922</v>
       </c>
       <c r="E511" t="n">
-        <v>286509687</v>
+        <v>286576209</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26614,13 +26614,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>142803</v>
+        <v>142804</v>
       </c>
       <c r="D514" t="n">
         <v>23612</v>
       </c>
       <c r="E514" t="n">
-        <v>244567071</v>
+        <v>244568983</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76637</v>
+        <v>76639</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114129393</v>
+        <v>114131597</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25065</v>
+        <v>25068</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92331999</v>
+        <v>92362703</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39920</v>
+        <v>39921</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60358891</v>
+        <v>60359605</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18430</v>
+        <v>18438</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72554723</v>
+        <v>72659539</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12394</v>
+        <v>12397</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40027556</v>
+        <v>40042868</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -28909,13 +28909,13 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D559" t="n">
         <v>132</v>
       </c>
       <c r="E559" t="n">
-        <v>1762560</v>
+        <v>1762994</v>
       </c>
       <c r="F559" t="inlineStr">
         <is>
@@ -28960,13 +28960,13 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>43846</v>
+        <v>43847</v>
       </c>
       <c r="D560" t="n">
         <v>5415</v>
       </c>
       <c r="E560" t="n">
-        <v>101311481</v>
+        <v>101312981</v>
       </c>
       <c r="F560" t="inlineStr">
         <is>
@@ -35692,13 +35692,13 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>24461</v>
+        <v>24462</v>
       </c>
       <c r="D692" t="n">
         <v>5606</v>
       </c>
       <c r="E692" t="n">
-        <v>41128650</v>
+        <v>41133626</v>
       </c>
       <c r="F692" t="inlineStr">
         <is>
@@ -42169,13 +42169,13 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>14926</v>
+        <v>14927</v>
       </c>
       <c r="D819" t="n">
         <v>2491</v>
       </c>
       <c r="E819" t="n">
-        <v>82016836</v>
+        <v>82037653</v>
       </c>
       <c r="F819" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-16 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71264</v>
+        <v>71266</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110294557</v>
+        <v>110295157</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18848</v>
+        <v>18857</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75117834</v>
+        <v>75163013</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -21055,13 +21055,13 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D405" t="n">
         <v>4</v>
       </c>
       <c r="E405" t="n">
-        <v>286089</v>
+        <v>354577</v>
       </c>
       <c r="F405" t="inlineStr">
         <is>
@@ -21106,13 +21106,13 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>6285</v>
+        <v>6295</v>
       </c>
       <c r="D406" t="n">
         <v>911</v>
       </c>
       <c r="E406" t="n">
-        <v>19290013</v>
+        <v>19452171</v>
       </c>
       <c r="F406" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9336</v>
+        <v>9339</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23720836</v>
+        <v>23760393</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -24268,13 +24268,13 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>164676</v>
+        <v>164677</v>
       </c>
       <c r="D468" t="n">
         <v>27310</v>
       </c>
       <c r="E468" t="n">
-        <v>287059661</v>
+        <v>287066961</v>
       </c>
       <c r="F468" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73746</v>
+        <v>73747</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386348384</v>
+        <v>386472202</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74979</v>
+        <v>74982</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>434681221</v>
+        <v>434912217</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416628</v>
+        <v>416632</v>
       </c>
       <c r="D477" t="n">
         <v>70498</v>
       </c>
       <c r="E477" t="n">
-        <v>724755492</v>
+        <v>724771273</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24778,13 +24778,13 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D478" t="n">
         <v>23</v>
       </c>
       <c r="E478" t="n">
-        <v>665363</v>
+        <v>671308</v>
       </c>
       <c r="F478" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291864</v>
+        <v>291874</v>
       </c>
       <c r="D484" t="n">
         <v>42564</v>
       </c>
       <c r="E484" t="n">
-        <v>1767661264</v>
+        <v>1767732203</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230490</v>
+        <v>230512</v>
       </c>
       <c r="D487" t="n">
         <v>33847</v>
       </c>
       <c r="E487" t="n">
-        <v>1815247172</v>
+        <v>1815879720</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12245</v>
+        <v>12246</v>
       </c>
       <c r="D491" t="n">
         <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>75461668</v>
+        <v>75473984</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184241</v>
+        <v>184243</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332689980</v>
+        <v>332690915</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62169</v>
+        <v>62171</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>298586676</v>
+        <v>298721711</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26563,13 +26563,13 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>3269</v>
+        <v>3270</v>
       </c>
       <c r="D513" t="n">
         <v>540</v>
       </c>
       <c r="E513" t="n">
-        <v>14285083</v>
+        <v>14294035</v>
       </c>
       <c r="F513" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56089</v>
+        <v>56090</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253510639</v>
+        <v>253515671</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="D534" t="n">
-        <v>8565</v>
+        <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>219686913</v>
+        <v>219749837</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -27736,13 +27736,13 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>37777</v>
+        <v>37779</v>
       </c>
       <c r="D536" t="n">
         <v>6687</v>
       </c>
       <c r="E536" t="n">
-        <v>173248686</v>
+        <v>173272231</v>
       </c>
       <c r="F536" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76639</v>
+        <v>76641</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114131597</v>
+        <v>114132538</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25069</v>
+        <v>25074</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92411535</v>
+        <v>92430892</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28297,13 +28297,13 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>7438</v>
+        <v>7440</v>
       </c>
       <c r="D547" t="n">
         <v>1667</v>
       </c>
       <c r="E547" t="n">
-        <v>37681278</v>
+        <v>37684204</v>
       </c>
       <c r="F547" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39921</v>
+        <v>39928</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60359605</v>
+        <v>60363412</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18438</v>
+        <v>18453</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72659539</v>
+        <v>72760118</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12397</v>
+        <v>12398</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40042868</v>
+        <v>40047588</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -31153,13 +31153,13 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>32186</v>
+        <v>32187</v>
       </c>
       <c r="D603" t="n">
         <v>6078</v>
       </c>
       <c r="E603" t="n">
-        <v>170277785</v>
+        <v>170477785</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -34519,13 +34519,13 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>39554</v>
+        <v>39555</v>
       </c>
       <c r="D669" t="n">
         <v>7193</v>
       </c>
       <c r="E669" t="n">
-        <v>209539933</v>
+        <v>209549933</v>
       </c>
       <c r="F669" t="inlineStr">
         <is>
@@ -44005,13 +44005,13 @@
         </is>
       </c>
       <c r="C855" t="n">
-        <v>7434</v>
+        <v>7435</v>
       </c>
       <c r="D855" t="n">
         <v>1362</v>
       </c>
       <c r="E855" t="n">
-        <v>45727097</v>
+        <v>45731389</v>
       </c>
       <c r="F855" t="inlineStr">
         <is>
@@ -46708,13 +46708,13 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>198891</v>
+        <v>198893</v>
       </c>
       <c r="D908" t="n">
-        <v>40344</v>
+        <v>40345</v>
       </c>
       <c r="E908" t="n">
-        <v>322719679</v>
+        <v>322739607</v>
       </c>
       <c r="F908" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79081</v>
+        <v>79082</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391402903</v>
+        <v>391405598</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -47371,13 +47371,13 @@
         </is>
       </c>
       <c r="C921" t="n">
-        <v>32195</v>
+        <v>32197</v>
       </c>
       <c r="D921" t="n">
         <v>5510</v>
       </c>
       <c r="E921" t="n">
-        <v>70560754</v>
+        <v>70565470</v>
       </c>
       <c r="F921" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-18 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -5194,13 +5194,13 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>25840</v>
+        <v>25841</v>
       </c>
       <c r="D94" t="n">
         <v>4834</v>
       </c>
       <c r="E94" t="n">
-        <v>122618879</v>
+        <v>122619668</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>186357</v>
+        <v>186361</v>
       </c>
       <c r="D100" t="n">
         <v>37749</v>
       </c>
       <c r="E100" t="n">
-        <v>306312150</v>
+        <v>306314845</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>84959</v>
+        <v>84960</v>
       </c>
       <c r="D105" t="n">
         <v>16087</v>
       </c>
       <c r="E105" t="n">
-        <v>401645674</v>
+        <v>401647390</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62514</v>
+        <v>62516</v>
       </c>
       <c r="D108" t="n">
         <v>10954</v>
       </c>
       <c r="E108" t="n">
-        <v>340490180</v>
+        <v>340502701</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -20443,13 +20443,13 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>5431</v>
+        <v>5433</v>
       </c>
       <c r="D393" t="n">
         <v>1019</v>
       </c>
       <c r="E393" t="n">
-        <v>28230358</v>
+        <v>28232237</v>
       </c>
       <c r="F393" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71266</v>
+        <v>71267</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110295157</v>
+        <v>110296657</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18857</v>
+        <v>18858</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75163013</v>
+        <v>75166047</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73747</v>
+        <v>73749</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386472202</v>
+        <v>386489016</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74983</v>
+        <v>74984</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>434922217</v>
+        <v>434931632</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416632</v>
+        <v>416637</v>
       </c>
       <c r="D477" t="n">
         <v>70498</v>
       </c>
       <c r="E477" t="n">
-        <v>724771273</v>
+        <v>724789528</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291875</v>
+        <v>291906</v>
       </c>
       <c r="D484" t="n">
         <v>42564</v>
       </c>
       <c r="E484" t="n">
-        <v>1767734486</v>
+        <v>1767978145</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230516</v>
+        <v>230544</v>
       </c>
       <c r="D487" t="n">
         <v>33847</v>
       </c>
       <c r="E487" t="n">
-        <v>1816060513</v>
+        <v>1816575326</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12246</v>
+        <v>12248</v>
       </c>
       <c r="D491" t="n">
         <v>1838</v>
       </c>
       <c r="E491" t="n">
-        <v>75473984</v>
+        <v>75585376</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71169</v>
+        <v>71172</v>
       </c>
       <c r="D511" t="n">
         <v>10923</v>
       </c>
       <c r="E511" t="n">
-        <v>286732560</v>
+        <v>286745637</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39928</v>
+        <v>39929</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60363412</v>
+        <v>60367248</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18453</v>
+        <v>18454</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72760118</v>
+        <v>72765909</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12399</v>
+        <v>12401</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40081638</v>
+        <v>40224583</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -29011,13 +29011,13 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>4230</v>
+        <v>4231</v>
       </c>
       <c r="D561" t="n">
         <v>682</v>
       </c>
       <c r="E561" t="n">
-        <v>12505869</v>
+        <v>12512655</v>
       </c>
       <c r="F561" t="inlineStr">
         <is>
@@ -29623,13 +29623,13 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="D573" t="n">
         <v>319</v>
       </c>
       <c r="E573" t="n">
-        <v>9436652</v>
+        <v>9445286</v>
       </c>
       <c r="F573" t="inlineStr">
         <is>
@@ -38701,13 +38701,13 @@
         </is>
       </c>
       <c r="C751" t="n">
-        <v>18144</v>
+        <v>18145</v>
       </c>
       <c r="D751" t="n">
         <v>3259</v>
       </c>
       <c r="E751" t="n">
-        <v>83154544</v>
+        <v>83163396</v>
       </c>
       <c r="F751" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-19 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3001,13 +3001,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>7303</v>
+        <v>7306</v>
       </c>
       <c r="D51" t="n">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="E51" t="n">
-        <v>32823377</v>
+        <v>32827877</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -7336,13 +7336,13 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>30532</v>
+        <v>30535</v>
       </c>
       <c r="D136" t="n">
-        <v>6640</v>
+        <v>6641</v>
       </c>
       <c r="E136" t="n">
-        <v>53099204</v>
+        <v>53103920</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -17944,13 +17944,13 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>28869</v>
+        <v>28870</v>
       </c>
       <c r="D344" t="n">
         <v>5352</v>
       </c>
       <c r="E344" t="n">
-        <v>158938232</v>
+        <v>158991044</v>
       </c>
       <c r="F344" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73749</v>
+        <v>73751</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>386489016</v>
+        <v>386646478</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74984</v>
+        <v>74989</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>434931632</v>
+        <v>435084940</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416641</v>
+        <v>416654</v>
       </c>
       <c r="D477" t="n">
         <v>70498</v>
       </c>
       <c r="E477" t="n">
-        <v>724796013</v>
+        <v>724839211</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291917</v>
+        <v>291940</v>
       </c>
       <c r="D484" t="n">
         <v>42564</v>
       </c>
       <c r="E484" t="n">
-        <v>1768100752</v>
+        <v>1768526023</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230547</v>
+        <v>230557</v>
       </c>
       <c r="D487" t="n">
         <v>33847</v>
       </c>
       <c r="E487" t="n">
-        <v>1816582631</v>
+        <v>1816992371</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62171</v>
+        <v>62173</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>298721711</v>
+        <v>298815941</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25076</v>
+        <v>25079</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92439338</v>
+        <v>92448942</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18454</v>
+        <v>18455</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>72765909</v>
+        <v>72768683</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12401</v>
+        <v>12402</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40224583</v>
+        <v>40299139</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -37018,13 +37018,13 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="D718" t="n">
         <v>236</v>
       </c>
       <c r="E718" t="n">
-        <v>5186675</v>
+        <v>5191274</v>
       </c>
       <c r="F718" t="inlineStr">
         <is>
@@ -46708,13 +46708,13 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>198893</v>
+        <v>198894</v>
       </c>
       <c r="D908" t="n">
         <v>40345</v>
       </c>
       <c r="E908" t="n">
-        <v>322739607</v>
+        <v>322749607</v>
       </c>
       <c r="F908" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-20 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3256,13 +3256,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>97640</v>
+        <v>97641</v>
       </c>
       <c r="D56" t="n">
         <v>18772</v>
       </c>
       <c r="E56" t="n">
-        <v>200339074</v>
+        <v>200343303</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>186361</v>
+        <v>186362</v>
       </c>
       <c r="D100" t="n">
         <v>37749</v>
       </c>
       <c r="E100" t="n">
-        <v>306314845</v>
+        <v>306316796</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71267</v>
+        <v>71268</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110296657</v>
+        <v>110298182</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35050</v>
+        <v>35051</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>160289217</v>
+        <v>160291457</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416664</v>
+        <v>416672</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>724875392</v>
+        <v>724905891</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291952</v>
+        <v>291972</v>
       </c>
       <c r="D484" t="n">
-        <v>42564</v>
+        <v>42565</v>
       </c>
       <c r="E484" t="n">
-        <v>1768728441</v>
+        <v>1768884931</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230557</v>
+        <v>230572</v>
       </c>
       <c r="D487" t="n">
-        <v>33847</v>
+        <v>33848</v>
       </c>
       <c r="E487" t="n">
-        <v>1816992371</v>
+        <v>1817278836</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25339,13 +25339,13 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>3147</v>
+        <v>3149</v>
       </c>
       <c r="D489" t="n">
         <v>608</v>
       </c>
       <c r="E489" t="n">
-        <v>8190949</v>
+        <v>8198315</v>
       </c>
       <c r="F489" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184244</v>
+        <v>184252</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332692745</v>
+        <v>332715568</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71172</v>
+        <v>71173</v>
       </c>
       <c r="D511" t="n">
         <v>10923</v>
       </c>
       <c r="E511" t="n">
-        <v>286745637</v>
+        <v>286945637</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26614,13 +26614,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>142805</v>
+        <v>142806</v>
       </c>
       <c r="D514" t="n">
         <v>23612</v>
       </c>
       <c r="E514" t="n">
-        <v>244574428</v>
+        <v>244576163</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39929</v>
+        <v>39930</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60367248</v>
+        <v>60367935</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12402</v>
+        <v>12405</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40299139</v>
+        <v>40365216</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -29776,13 +29776,13 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>15016</v>
+        <v>15017</v>
       </c>
       <c r="D576" t="n">
         <v>3117</v>
       </c>
       <c r="E576" t="n">
-        <v>67287568</v>
+        <v>67297568</v>
       </c>
       <c r="F576" t="inlineStr">
         <is>
@@ -35845,13 +35845,13 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>11033</v>
+        <v>11034</v>
       </c>
       <c r="D695" t="n">
         <v>2192</v>
       </c>
       <c r="E695" t="n">
-        <v>48728368</v>
+        <v>48734023</v>
       </c>
       <c r="F695" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-23 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105826</v>
+        <v>105827</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186640864</v>
+        <v>186642619</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -15649,13 +15649,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>9029</v>
+        <v>9032</v>
       </c>
       <c r="D299" t="n">
         <v>1438</v>
       </c>
       <c r="E299" t="n">
-        <v>50036881</v>
+        <v>50063935</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71268</v>
+        <v>71270</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110298182</v>
+        <v>110301078</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18863</v>
+        <v>18866</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75211295</v>
+        <v>75241295</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -23554,13 +23554,13 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>12238</v>
+        <v>12239</v>
       </c>
       <c r="D454" t="n">
         <v>2377</v>
       </c>
       <c r="E454" t="n">
-        <v>66590896</v>
+        <v>66592456</v>
       </c>
       <c r="F454" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416674</v>
+        <v>416682</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>724909969</v>
+        <v>725016776</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291982</v>
+        <v>291996</v>
       </c>
       <c r="D484" t="n">
         <v>42565</v>
       </c>
       <c r="E484" t="n">
-        <v>1769201775</v>
+        <v>1769311893</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3049</v>
+        <v>3050</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>99508589</v>
+        <v>99513059</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230589</v>
+        <v>230601</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1818119337</v>
+        <v>1818390513</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12248</v>
+        <v>12249</v>
       </c>
       <c r="D491" t="n">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="E491" t="n">
-        <v>75585376</v>
+        <v>75588324</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62178</v>
+        <v>62179</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>298934889</v>
+        <v>298944889</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71178</v>
+        <v>71186</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>286985272</v>
+        <v>287401054</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56095</v>
+        <v>56097</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253584096</v>
+        <v>253609056</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27940,13 +27940,13 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>76641</v>
+        <v>76643</v>
       </c>
       <c r="D540" t="n">
         <v>17494</v>
       </c>
       <c r="E540" t="n">
-        <v>114132538</v>
+        <v>114133158</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39930</v>
+        <v>39931</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60367935</v>
+        <v>60378307</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18458</v>
+        <v>18459</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>73368683</v>
+        <v>73371235</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163433</v>
+        <v>163434</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278426270</v>
+        <v>278426721</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -43444,13 +43444,13 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>58393</v>
+        <v>58394</v>
       </c>
       <c r="D844" t="n">
-        <v>11374</v>
+        <v>11375</v>
       </c>
       <c r="E844" t="n">
-        <v>290406601</v>
+        <v>290416601</v>
       </c>
       <c r="F844" t="inlineStr">
         <is>
@@ -43852,13 +43852,13 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>27075</v>
+        <v>27077</v>
       </c>
       <c r="D852" t="n">
         <v>5532</v>
       </c>
       <c r="E852" t="n">
-        <v>133341228</v>
+        <v>133386949</v>
       </c>
       <c r="F852" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-09 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1165,13 +1165,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8966</v>
+        <v>8967</v>
       </c>
       <c r="D15" t="n">
         <v>1806</v>
       </c>
       <c r="E15" t="n">
-        <v>40509823</v>
+        <v>40512006</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -3256,13 +3256,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>97641</v>
+        <v>97642</v>
       </c>
       <c r="D56" t="n">
         <v>18772</v>
       </c>
       <c r="E56" t="n">
-        <v>200343303</v>
+        <v>200344803</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -19066,13 +19066,13 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>18845</v>
+        <v>18846</v>
       </c>
       <c r="D366" t="n">
         <v>3811</v>
       </c>
       <c r="E366" t="n">
-        <v>86393610</v>
+        <v>86458324</v>
       </c>
       <c r="F366" t="inlineStr">
         <is>
@@ -19882,13 +19882,13 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>25392</v>
+        <v>25393</v>
       </c>
       <c r="D382" t="n">
         <v>5083</v>
       </c>
       <c r="E382" t="n">
-        <v>129195897</v>
+        <v>129197360</v>
       </c>
       <c r="F382" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35051</v>
+        <v>35052</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>160291457</v>
+        <v>160307087</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416682</v>
+        <v>416686</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>725016776</v>
+        <v>725025361</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24982,13 +24982,13 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>4145</v>
+        <v>4149</v>
       </c>
       <c r="D482" t="n">
         <v>521</v>
       </c>
       <c r="E482" t="n">
-        <v>69750394</v>
+        <v>69788450</v>
       </c>
       <c r="F482" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>291996</v>
+        <v>292004</v>
       </c>
       <c r="D484" t="n">
         <v>42565</v>
       </c>
       <c r="E484" t="n">
-        <v>1769311893</v>
+        <v>1769404137</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230601</v>
+        <v>230605</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1818390513</v>
+        <v>1818417273</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184255</v>
+        <v>184256</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332722779</v>
+        <v>332723639</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56097</v>
+        <v>56099</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253609056</v>
+        <v>253683580</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44037</v>
+        <v>44039</v>
       </c>
       <c r="D534" t="n">
         <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>219881172</v>
+        <v>219932787</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25079</v>
+        <v>25080</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92448942</v>
+        <v>92483431</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79083</v>
+        <v>79085</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391605598</v>
+        <v>391609737</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -47575,13 +47575,13 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>12199</v>
+        <v>12200</v>
       </c>
       <c r="D925" t="n">
         <v>1959</v>
       </c>
       <c r="E925" t="n">
-        <v>76244390</v>
+        <v>76251330</v>
       </c>
       <c r="F925" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-31 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105828</v>
+        <v>105831</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186643959</v>
+        <v>186651687</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71271</v>
+        <v>71273</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110302626</v>
+        <v>110303186</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -22075,13 +22075,13 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>70536</v>
+        <v>70537</v>
       </c>
       <c r="D425" t="n">
         <v>13142</v>
       </c>
       <c r="E425" t="n">
-        <v>343514088</v>
+        <v>343712541</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -24115,13 +24115,13 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>34719</v>
+        <v>34720</v>
       </c>
       <c r="D465" t="n">
         <v>6013</v>
       </c>
       <c r="E465" t="n">
-        <v>152625095</v>
+        <v>152635095</v>
       </c>
       <c r="F465" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73756</v>
+        <v>73757</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>387088234</v>
+        <v>387133975</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74991</v>
+        <v>74992</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>435132289</v>
+        <v>435318545</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416718</v>
+        <v>416731</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>725132137</v>
+        <v>725169838</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292041</v>
+        <v>292061</v>
       </c>
       <c r="D484" t="n">
         <v>42565</v>
       </c>
       <c r="E484" t="n">
-        <v>1769873779</v>
+        <v>1770130136</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230638</v>
+        <v>230646</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1819528910</v>
+        <v>1819586554</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25951,13 +25951,13 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>38088</v>
+        <v>38089</v>
       </c>
       <c r="D501" t="n">
         <v>6578</v>
       </c>
       <c r="E501" t="n">
-        <v>177066943</v>
+        <v>177109909</v>
       </c>
       <c r="F501" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184256</v>
+        <v>184258</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332723639</v>
+        <v>332729119</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56099</v>
+        <v>56101</v>
       </c>
       <c r="D520" t="n">
         <v>8769</v>
       </c>
       <c r="E520" t="n">
-        <v>253683580</v>
+        <v>253759835</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25080</v>
+        <v>25081</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92483431</v>
+        <v>92485718</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28297,13 +28297,13 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>7440</v>
+        <v>7441</v>
       </c>
       <c r="D547" t="n">
         <v>1667</v>
       </c>
       <c r="E547" t="n">
-        <v>37684204</v>
+        <v>37756696</v>
       </c>
       <c r="F547" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39931</v>
+        <v>39933</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60378307</v>
+        <v>60385247</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163434</v>
+        <v>163436</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278426721</v>
+        <v>278429721</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-01 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105831</v>
+        <v>105832</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186651687</v>
+        <v>186654215</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88473</v>
+        <v>88474</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216759407</v>
+        <v>216759422</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -6265,13 +6265,13 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="D115" t="n">
         <v>76</v>
       </c>
       <c r="E115" t="n">
-        <v>1094111</v>
+        <v>1104375</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -12232,13 +12232,13 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>17578</v>
+        <v>17579</v>
       </c>
       <c r="D232" t="n">
         <v>3904</v>
       </c>
       <c r="E232" t="n">
-        <v>34529253</v>
+        <v>34539253</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
@@ -22585,13 +22585,13 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>20235</v>
+        <v>20236</v>
       </c>
       <c r="D435" t="n">
         <v>4036</v>
       </c>
       <c r="E435" t="n">
-        <v>93031589</v>
+        <v>93034525</v>
       </c>
       <c r="F435" t="inlineStr">
         <is>
@@ -24115,13 +24115,13 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>34720</v>
+        <v>34721</v>
       </c>
       <c r="D465" t="n">
         <v>6013</v>
       </c>
       <c r="E465" t="n">
-        <v>152635095</v>
+        <v>152637895</v>
       </c>
       <c r="F465" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73757</v>
+        <v>73758</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>387133975</v>
+        <v>387141631</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74992</v>
+        <v>74994</v>
       </c>
       <c r="D474" t="n">
         <v>11549</v>
       </c>
       <c r="E474" t="n">
-        <v>435318545</v>
+        <v>435430166</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416733</v>
+        <v>416736</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>725177470</v>
+        <v>725189912</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292067</v>
+        <v>292087</v>
       </c>
       <c r="D484" t="n">
         <v>42565</v>
       </c>
       <c r="E484" t="n">
-        <v>1770153973</v>
+        <v>1770521813</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25186,13 +25186,13 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D486" t="n">
         <v>49</v>
       </c>
       <c r="E486" t="n">
-        <v>17455226</v>
+        <v>17518019</v>
       </c>
       <c r="F486" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230653</v>
+        <v>230659</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1820025477</v>
+        <v>1820055946</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12255</v>
+        <v>12257</v>
       </c>
       <c r="D491" t="n">
         <v>1839</v>
       </c>
       <c r="E491" t="n">
-        <v>76165173</v>
+        <v>76171530</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -25492,13 +25492,13 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D492" t="n">
         <v>7</v>
       </c>
       <c r="E492" t="n">
-        <v>2058873</v>
+        <v>2246560</v>
       </c>
       <c r="F492" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184259</v>
+        <v>184261</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332734069</v>
+        <v>332736181</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18459</v>
+        <v>18462</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>73371235</v>
+        <v>73574082</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -36253,13 +36253,13 @@
         </is>
       </c>
       <c r="C703" t="n">
-        <v>36230</v>
+        <v>36231</v>
       </c>
       <c r="D703" t="n">
         <v>6909</v>
       </c>
       <c r="E703" t="n">
-        <v>183952297</v>
+        <v>183977808</v>
       </c>
       <c r="F703" t="inlineStr">
         <is>
@@ -43852,13 +43852,13 @@
         </is>
       </c>
       <c r="C852" t="n">
-        <v>27077</v>
+        <v>27078</v>
       </c>
       <c r="D852" t="n">
         <v>5532</v>
       </c>
       <c r="E852" t="n">
-        <v>133386949</v>
+        <v>133388194</v>
       </c>
       <c r="F852" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79085</v>
+        <v>79087</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391609737</v>
+        <v>391826225</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-03 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88474</v>
+        <v>88477</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216759422</v>
+        <v>216767689</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16937</v>
+        <v>16941</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50658037</v>
+        <v>50660115</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9342</v>
+        <v>9344</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23821759</v>
+        <v>23829850</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -22228,13 +22228,13 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>40404</v>
+        <v>40406</v>
       </c>
       <c r="D428" t="n">
         <v>6930</v>
       </c>
       <c r="E428" t="n">
-        <v>215158895</v>
+        <v>215219541</v>
       </c>
       <c r="F428" t="inlineStr">
         <is>
@@ -23809,13 +23809,13 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>88337</v>
+        <v>88339</v>
       </c>
       <c r="D459" t="n">
         <v>16394</v>
       </c>
       <c r="E459" t="n">
-        <v>151555713</v>
+        <v>151567802</v>
       </c>
       <c r="F459" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416744</v>
+        <v>416746</v>
       </c>
       <c r="D477" t="n">
         <v>70499</v>
       </c>
       <c r="E477" t="n">
-        <v>725211927</v>
+        <v>725222352</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292094</v>
+        <v>292100</v>
       </c>
       <c r="D484" t="n">
         <v>42566</v>
       </c>
       <c r="E484" t="n">
-        <v>1770780754</v>
+        <v>1770984304</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25135,13 +25135,13 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>3053</v>
+        <v>3054</v>
       </c>
       <c r="D485" t="n">
         <v>420</v>
       </c>
       <c r="E485" t="n">
-        <v>99913911</v>
+        <v>100002797</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230666</v>
+        <v>230683</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1820098168</v>
+        <v>1820902962</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25951,13 +25951,13 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>38089</v>
+        <v>38091</v>
       </c>
       <c r="D501" t="n">
         <v>6578</v>
       </c>
       <c r="E501" t="n">
-        <v>177109909</v>
+        <v>177160205</v>
       </c>
       <c r="F501" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184262</v>
+        <v>184265</v>
       </c>
       <c r="D505" t="n">
         <v>27737</v>
       </c>
       <c r="E505" t="n">
-        <v>332736481</v>
+        <v>332746689</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62184</v>
+        <v>62186</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>298981780</v>
+        <v>299005841</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71189</v>
+        <v>71190</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287409316</v>
+        <v>287419316</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26563,13 +26563,13 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>3276</v>
+        <v>3277</v>
       </c>
       <c r="D513" t="n">
         <v>540</v>
       </c>
       <c r="E513" t="n">
-        <v>14354035</v>
+        <v>14364035</v>
       </c>
       <c r="F513" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="D534" t="n">
         <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>219932787</v>
+        <v>220132787</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163436</v>
+        <v>163437</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278429721</v>
+        <v>278430785</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -47065,13 +47065,13 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>96857</v>
+        <v>96858</v>
       </c>
       <c r="D915" t="n">
         <v>17575</v>
       </c>
       <c r="E915" t="n">
-        <v>463317154</v>
+        <v>463319404</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>
@@ -47575,13 +47575,13 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>12200</v>
+        <v>12203</v>
       </c>
       <c r="D925" t="n">
         <v>1959</v>
       </c>
       <c r="E925" t="n">
-        <v>76251330</v>
+        <v>76281330</v>
       </c>
       <c r="F925" t="inlineStr">
         <is>
@@ -48238,13 +48238,13 @@
         </is>
       </c>
       <c r="C938" t="n">
-        <v>38554</v>
+        <v>38556</v>
       </c>
       <c r="D938" t="n">
         <v>6911</v>
       </c>
       <c r="E938" t="n">
-        <v>195385199</v>
+        <v>195507462</v>
       </c>
       <c r="F938" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-07 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -4174,13 +4174,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>50228</v>
+        <v>50229</v>
       </c>
       <c r="D74" t="n">
         <v>9675</v>
       </c>
       <c r="E74" t="n">
-        <v>249887928</v>
+        <v>249889845</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -7795,13 +7795,13 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D145" t="n">
         <v>225</v>
       </c>
       <c r="E145" t="n">
-        <v>7286063</v>
+        <v>7370100</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -10651,13 +10651,13 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>56180</v>
+        <v>56181</v>
       </c>
       <c r="D201" t="n">
         <v>13193</v>
       </c>
       <c r="E201" t="n">
-        <v>111926430</v>
+        <v>111929074</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -15547,13 +15547,13 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>12890</v>
+        <v>12891</v>
       </c>
       <c r="D297" t="n">
         <v>1973</v>
       </c>
       <c r="E297" t="n">
-        <v>74448110</v>
+        <v>74449610</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
@@ -21004,13 +21004,13 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>29543</v>
+        <v>29544</v>
       </c>
       <c r="D404" t="n">
         <v>3814</v>
       </c>
       <c r="E404" t="n">
-        <v>56432511</v>
+        <v>56437349</v>
       </c>
       <c r="F404" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9344</v>
+        <v>9345</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23829850</v>
+        <v>23837942</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -21361,13 +21361,13 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D411" t="n">
         <v>79</v>
       </c>
       <c r="E411" t="n">
-        <v>994952</v>
+        <v>996792</v>
       </c>
       <c r="F411" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416754</v>
+        <v>416757</v>
       </c>
       <c r="D477" t="n">
         <v>70500</v>
       </c>
       <c r="E477" t="n">
-        <v>725253751</v>
+        <v>725262336</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292111</v>
+        <v>292120</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1771052582</v>
+        <v>1771132448</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230706</v>
+        <v>230708</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1821668003</v>
+        <v>1821759004</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25798,13 +25798,13 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>40859</v>
+        <v>40860</v>
       </c>
       <c r="D498" t="n">
         <v>7972</v>
       </c>
       <c r="E498" t="n">
-        <v>194519587</v>
+        <v>194557004</v>
       </c>
       <c r="F498" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62187</v>
+        <v>62188</v>
       </c>
       <c r="D509" t="n">
         <v>11277</v>
       </c>
       <c r="E509" t="n">
-        <v>299015841</v>
+        <v>299059595</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71191</v>
+        <v>71195</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287435462</v>
+        <v>287589147</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25082</v>
+        <v>25083</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92493053</v>
+        <v>92541885</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -32071,13 +32071,13 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>30120</v>
+        <v>30121</v>
       </c>
       <c r="D621" t="n">
         <v>5930</v>
       </c>
       <c r="E621" t="n">
-        <v>163612704</v>
+        <v>163621818</v>
       </c>
       <c r="F621" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163437</v>
+        <v>163438</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278430785</v>
+        <v>278431354</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73205</v>
+        <v>73207</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367188525</v>
+        <v>367202185</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -46351,13 +46351,13 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>81810</v>
+        <v>81811</v>
       </c>
       <c r="D901" t="n">
         <v>13203</v>
       </c>
       <c r="E901" t="n">
-        <v>443371787</v>
+        <v>443377982</v>
       </c>
       <c r="F901" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79087</v>
+        <v>79088</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391826225</v>
+        <v>391827725</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-09 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -16771,13 +16771,13 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>76030</v>
+        <v>76032</v>
       </c>
       <c r="D321" t="n">
         <v>15908</v>
       </c>
       <c r="E321" t="n">
-        <v>132447839</v>
+        <v>132462902</v>
       </c>
       <c r="F321" t="inlineStr">
         <is>
@@ -22228,13 +22228,13 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>40406</v>
+        <v>40408</v>
       </c>
       <c r="D428" t="n">
         <v>6930</v>
       </c>
       <c r="E428" t="n">
-        <v>215219541</v>
+        <v>215280187</v>
       </c>
       <c r="F428" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35052</v>
+        <v>35054</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>160307087</v>
+        <v>160478383</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74995</v>
+        <v>74996</v>
       </c>
       <c r="D474" t="n">
         <v>11550</v>
       </c>
       <c r="E474" t="n">
-        <v>435440166</v>
+        <v>435450166</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292127</v>
+        <v>292128</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1771208912</v>
+        <v>1771211195</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230715</v>
+        <v>230719</v>
       </c>
       <c r="D487" t="n">
         <v>33849</v>
       </c>
       <c r="E487" t="n">
-        <v>1821795286</v>
+        <v>1821976079</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184268</v>
+        <v>184269</v>
       </c>
       <c r="D505" t="n">
         <v>27738</v>
       </c>
       <c r="E505" t="n">
-        <v>332750448</v>
+        <v>332752278</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71195</v>
+        <v>71196</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287589147</v>
+        <v>287591813</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26563,13 +26563,13 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>3277</v>
+        <v>3280</v>
       </c>
       <c r="D513" t="n">
         <v>540</v>
       </c>
       <c r="E513" t="n">
-        <v>14364035</v>
+        <v>14394035</v>
       </c>
       <c r="F513" t="inlineStr">
         <is>
@@ -27226,13 +27226,13 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>35988</v>
+        <v>35989</v>
       </c>
       <c r="D526" t="n">
         <v>7104</v>
       </c>
       <c r="E526" t="n">
-        <v>162590347</v>
+        <v>162620811</v>
       </c>
       <c r="F526" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25083</v>
+        <v>25085</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92541885</v>
+        <v>92550331</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12408</v>
+        <v>12409</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40519203</v>
+        <v>40553253</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -46504,13 +46504,13 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>59759</v>
+        <v>59760</v>
       </c>
       <c r="D904" t="n">
         <v>8975</v>
       </c>
       <c r="E904" t="n">
-        <v>334677919</v>
+        <v>334732534</v>
       </c>
       <c r="F904" t="inlineStr">
         <is>
@@ -48748,13 +48748,13 @@
         </is>
       </c>
       <c r="C948" t="n">
-        <v>19065</v>
+        <v>19071</v>
       </c>
       <c r="D948" t="n">
         <v>3311</v>
       </c>
       <c r="E948" t="n">
-        <v>93803672</v>
+        <v>93863672</v>
       </c>
       <c r="F948" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-10 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -10855,13 +10855,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>29940</v>
+        <v>29941</v>
       </c>
       <c r="D205" t="n">
         <v>5716</v>
       </c>
       <c r="E205" t="n">
-        <v>156325110</v>
+        <v>156347147</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -12232,13 +12232,13 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>17579</v>
+        <v>17580</v>
       </c>
       <c r="D232" t="n">
         <v>3904</v>
       </c>
       <c r="E232" t="n">
-        <v>34539253</v>
+        <v>34543636</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
@@ -15547,13 +15547,13 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>12891</v>
+        <v>12893</v>
       </c>
       <c r="D297" t="n">
         <v>1973</v>
       </c>
       <c r="E297" t="n">
-        <v>74449610</v>
+        <v>74453702</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
@@ -15649,13 +15649,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>9032</v>
+        <v>9033</v>
       </c>
       <c r="D299" t="n">
         <v>1438</v>
       </c>
       <c r="E299" t="n">
-        <v>50063935</v>
+        <v>50072268</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -15802,13 +15802,13 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>15276</v>
+        <v>15277</v>
       </c>
       <c r="D302" t="n">
         <v>3339</v>
       </c>
       <c r="E302" t="n">
-        <v>28784971</v>
+        <v>28787352</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
@@ -18097,13 +18097,13 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>14620</v>
+        <v>14621</v>
       </c>
       <c r="D347" t="n">
         <v>2663</v>
       </c>
       <c r="E347" t="n">
-        <v>85179235</v>
+        <v>85181223</v>
       </c>
       <c r="F347" t="inlineStr">
         <is>
@@ -22432,13 +22432,13 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>43535</v>
+        <v>43536</v>
       </c>
       <c r="D432" t="n">
-        <v>9207</v>
+        <v>9208</v>
       </c>
       <c r="E432" t="n">
-        <v>76686195</v>
+        <v>76686270</v>
       </c>
       <c r="F432" t="inlineStr">
         <is>
@@ -23809,13 +23809,13 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>88339</v>
+        <v>88343</v>
       </c>
       <c r="D459" t="n">
         <v>16394</v>
       </c>
       <c r="E459" t="n">
-        <v>151567802</v>
+        <v>151573170</v>
       </c>
       <c r="F459" t="inlineStr">
         <is>
@@ -24268,13 +24268,13 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>164679</v>
+        <v>164680</v>
       </c>
       <c r="D468" t="n">
         <v>27310</v>
       </c>
       <c r="E468" t="n">
-        <v>287071522</v>
+        <v>287073022</v>
       </c>
       <c r="F468" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416773</v>
+        <v>416779</v>
       </c>
       <c r="D477" t="n">
-        <v>70500</v>
+        <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725320314</v>
+        <v>725332455</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292139</v>
+        <v>292150</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1771562858</v>
+        <v>1771685465</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230731</v>
+        <v>230734</v>
       </c>
       <c r="D487" t="n">
         <v>33850</v>
       </c>
       <c r="E487" t="n">
-        <v>1822246752</v>
+        <v>1822254057</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26614,13 +26614,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>142807</v>
+        <v>142808</v>
       </c>
       <c r="D514" t="n">
         <v>23612</v>
       </c>
       <c r="E514" t="n">
-        <v>244580153</v>
+        <v>244585598</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56106</v>
+        <v>56110</v>
       </c>
       <c r="D520" t="n">
         <v>8770</v>
       </c>
       <c r="E520" t="n">
-        <v>254037273</v>
+        <v>254093530</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44040</v>
+        <v>44042</v>
       </c>
       <c r="D534" t="n">
         <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>220132787</v>
+        <v>220226017</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73207</v>
+        <v>73208</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367202185</v>
+        <v>367211591</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -34519,13 +34519,13 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>39558</v>
+        <v>39559</v>
       </c>
       <c r="D669" t="n">
         <v>7193</v>
       </c>
       <c r="E669" t="n">
-        <v>209612091</v>
+        <v>209622091</v>
       </c>
       <c r="F669" t="inlineStr">
         <is>
@@ -40843,13 +40843,13 @@
         </is>
       </c>
       <c r="C793" t="n">
-        <v>63454</v>
+        <v>63457</v>
       </c>
       <c r="D793" t="n">
         <v>11594</v>
       </c>
       <c r="E793" t="n">
-        <v>307291486</v>
+        <v>307308190</v>
       </c>
       <c r="F793" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79088</v>
+        <v>79089</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>391827725</v>
+        <v>392027725</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -48646,13 +48646,13 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>29831</v>
+        <v>29832</v>
       </c>
       <c r="D946" t="n">
         <v>5384</v>
       </c>
       <c r="E946" t="n">
-        <v>141956650</v>
+        <v>141958150</v>
       </c>
       <c r="F946" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-14 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105832</v>
+        <v>105833</v>
       </c>
       <c r="D69" t="n">
         <v>22855</v>
       </c>
       <c r="E69" t="n">
-        <v>186654215</v>
+        <v>186659535</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -6571,13 +6571,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>14643</v>
+        <v>14647</v>
       </c>
       <c r="D121" t="n">
         <v>2286</v>
       </c>
       <c r="E121" t="n">
-        <v>168858937</v>
+        <v>169549158</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -6673,13 +6673,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="D123" t="n">
         <v>242</v>
       </c>
       <c r="E123" t="n">
-        <v>3796100</v>
+        <v>3797642</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
@@ -7030,13 +7030,13 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>22275</v>
+        <v>22276</v>
       </c>
       <c r="D130" t="n">
         <v>4180</v>
       </c>
       <c r="E130" t="n">
-        <v>116853588</v>
+        <v>116865350</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -15649,13 +15649,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>9033</v>
+        <v>9034</v>
       </c>
       <c r="D299" t="n">
         <v>1438</v>
       </c>
       <c r="E299" t="n">
-        <v>50072268</v>
+        <v>50192277</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -19882,13 +19882,13 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>25393</v>
+        <v>25394</v>
       </c>
       <c r="D382" t="n">
         <v>5083</v>
       </c>
       <c r="E382" t="n">
-        <v>129197360</v>
+        <v>129223594</v>
       </c>
       <c r="F382" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18875</v>
+        <v>18876</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75303711</v>
+        <v>75305211</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -23809,13 +23809,13 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>88343</v>
+        <v>88345</v>
       </c>
       <c r="D459" t="n">
         <v>16394</v>
       </c>
       <c r="E459" t="n">
-        <v>151573170</v>
+        <v>151574915</v>
       </c>
       <c r="F459" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74996</v>
+        <v>74997</v>
       </c>
       <c r="D474" t="n">
         <v>11550</v>
       </c>
       <c r="E474" t="n">
-        <v>435450166</v>
+        <v>435453342</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416792</v>
+        <v>416802</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725391121</v>
+        <v>725427302</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292166</v>
+        <v>292178</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1771833259</v>
+        <v>1772035677</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62193</v>
+        <v>62194</v>
       </c>
       <c r="D509" t="n">
         <v>11278</v>
       </c>
       <c r="E509" t="n">
-        <v>299103395</v>
+        <v>299163826</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56110</v>
+        <v>56111</v>
       </c>
       <c r="D520" t="n">
         <v>8770</v>
       </c>
       <c r="E520" t="n">
-        <v>254093530</v>
+        <v>254105698</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D534" t="n">
         <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>220226017</v>
+        <v>220264122</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -28705,13 +28705,13 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>18462</v>
+        <v>18465</v>
       </c>
       <c r="D555" t="n">
         <v>3296</v>
       </c>
       <c r="E555" t="n">
-        <v>73574082</v>
+        <v>74174082</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -48646,13 +48646,13 @@
         </is>
       </c>
       <c r="C946" t="n">
-        <v>29832</v>
+        <v>29833</v>
       </c>
       <c r="D946" t="n">
         <v>5384</v>
       </c>
       <c r="E946" t="n">
-        <v>141958150</v>
+        <v>141963607</v>
       </c>
       <c r="F946" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-15 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -13813,13 +13813,13 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>7912</v>
+        <v>7913</v>
       </c>
       <c r="D263" t="n">
         <v>1455</v>
       </c>
       <c r="E263" t="n">
-        <v>44690774</v>
+        <v>44890774</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18876</v>
+        <v>18880</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75305211</v>
+        <v>75348959</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16941</v>
+        <v>16946</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50660115</v>
+        <v>50673087</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21004,13 +21004,13 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>29544</v>
+        <v>29545</v>
       </c>
       <c r="D404" t="n">
         <v>3814</v>
       </c>
       <c r="E404" t="n">
-        <v>56437349</v>
+        <v>56437589</v>
       </c>
       <c r="F404" t="inlineStr">
         <is>
@@ -21106,13 +21106,13 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>6298</v>
+        <v>6300</v>
       </c>
       <c r="D406" t="n">
         <v>911</v>
       </c>
       <c r="E406" t="n">
-        <v>19477128</v>
+        <v>19499128</v>
       </c>
       <c r="F406" t="inlineStr">
         <is>
@@ -22228,13 +22228,13 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>40408</v>
+        <v>40409</v>
       </c>
       <c r="D428" t="n">
         <v>6930</v>
       </c>
       <c r="E428" t="n">
-        <v>215280187</v>
+        <v>215322000</v>
       </c>
       <c r="F428" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73759</v>
+        <v>73763</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>387151631</v>
+        <v>387497603</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416809</v>
+        <v>416811</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725452946</v>
+        <v>725457024</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292185</v>
+        <v>292195</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1772328458</v>
+        <v>1772645302</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230753</v>
+        <v>230770</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1822785565</v>
+        <v>1823626066</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184271</v>
+        <v>184274</v>
       </c>
       <c r="D505" t="n">
         <v>27738</v>
       </c>
       <c r="E505" t="n">
-        <v>332753046</v>
+        <v>332760257</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62197</v>
+        <v>62201</v>
       </c>
       <c r="D509" t="n">
         <v>11278</v>
       </c>
       <c r="E509" t="n">
-        <v>299200303</v>
+        <v>299258820</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71200</v>
+        <v>71205</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287631813</v>
+        <v>287671448</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26563,13 +26563,13 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>3280</v>
+        <v>3283</v>
       </c>
       <c r="D513" t="n">
         <v>540</v>
       </c>
       <c r="E513" t="n">
-        <v>14394035</v>
+        <v>14424035</v>
       </c>
       <c r="F513" t="inlineStr">
         <is>
@@ -27736,13 +27736,13 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>37781</v>
+        <v>37782</v>
       </c>
       <c r="D536" t="n">
         <v>6687</v>
       </c>
       <c r="E536" t="n">
-        <v>173282736</v>
+        <v>173283241</v>
       </c>
       <c r="F536" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73208</v>
+        <v>73209</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367211591</v>
+        <v>367212686</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -34519,13 +34519,13 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>39559</v>
+        <v>39560</v>
       </c>
       <c r="D669" t="n">
         <v>7193</v>
       </c>
       <c r="E669" t="n">
-        <v>209622091</v>
+        <v>209653170</v>
       </c>
       <c r="F669" t="inlineStr">
         <is>
@@ -40537,13 +40537,13 @@
         </is>
       </c>
       <c r="C787" t="n">
-        <v>133967</v>
+        <v>133970</v>
       </c>
       <c r="D787" t="n">
         <v>28168</v>
       </c>
       <c r="E787" t="n">
-        <v>211459201</v>
+        <v>211464673</v>
       </c>
       <c r="F787" t="inlineStr">
         <is>
@@ -44515,13 +44515,13 @@
         </is>
       </c>
       <c r="C865" t="n">
-        <v>28827</v>
+        <v>28829</v>
       </c>
       <c r="D865" t="n">
         <v>6343</v>
       </c>
       <c r="E865" t="n">
-        <v>53423670</v>
+        <v>53440174</v>
       </c>
       <c r="F865" t="inlineStr">
         <is>
@@ -47065,13 +47065,13 @@
         </is>
       </c>
       <c r="C915" t="n">
-        <v>96858</v>
+        <v>96859</v>
       </c>
       <c r="D915" t="n">
         <v>17575</v>
       </c>
       <c r="E915" t="n">
-        <v>463319404</v>
+        <v>463325082</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-16 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -1165,13 +1165,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8967</v>
+        <v>8968</v>
       </c>
       <c r="D15" t="n">
         <v>1806</v>
       </c>
       <c r="E15" t="n">
-        <v>40512006</v>
+        <v>40514189</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -3256,13 +3256,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>97646</v>
+        <v>97647</v>
       </c>
       <c r="D56" t="n">
         <v>18772</v>
       </c>
       <c r="E56" t="n">
-        <v>200355723</v>
+        <v>200357223</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -19066,13 +19066,13 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>18846</v>
+        <v>18847</v>
       </c>
       <c r="D366" t="n">
         <v>3811</v>
       </c>
       <c r="E366" t="n">
-        <v>86458324</v>
+        <v>86523038</v>
       </c>
       <c r="F366" t="inlineStr">
         <is>
@@ -19882,13 +19882,13 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>25394</v>
+        <v>25395</v>
       </c>
       <c r="D382" t="n">
         <v>5083</v>
       </c>
       <c r="E382" t="n">
-        <v>129223594</v>
+        <v>129225057</v>
       </c>
       <c r="F382" t="inlineStr">
         <is>
@@ -24013,13 +24013,13 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>35054</v>
+        <v>35055</v>
       </c>
       <c r="D463" t="n">
         <v>7039</v>
       </c>
       <c r="E463" t="n">
-        <v>160478383</v>
+        <v>160494013</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416823</v>
+        <v>416827</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725487387</v>
+        <v>725495972</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24982,13 +24982,13 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>4150</v>
+        <v>4154</v>
       </c>
       <c r="D482" t="n">
         <v>521</v>
       </c>
       <c r="E482" t="n">
-        <v>69888184</v>
+        <v>69926240</v>
       </c>
       <c r="F482" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292200</v>
+        <v>292208</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1772732127</v>
+        <v>1772824371</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230779</v>
+        <v>230783</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1823728544</v>
+        <v>1823755304</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184274</v>
+        <v>184275</v>
       </c>
       <c r="D505" t="n">
         <v>27738</v>
       </c>
       <c r="E505" t="n">
-        <v>332760257</v>
+        <v>332761117</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56111</v>
+        <v>56113</v>
       </c>
       <c r="D520" t="n">
         <v>8770</v>
       </c>
       <c r="E520" t="n">
-        <v>254105698</v>
+        <v>254180222</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -27634,13 +27634,13 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D534" t="n">
         <v>8566</v>
       </c>
       <c r="E534" t="n">
-        <v>220264122</v>
+        <v>220315737</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25085</v>
+        <v>25086</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92550331</v>
+        <v>92584820</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -47218,13 +47218,13 @@
         </is>
       </c>
       <c r="C918" t="n">
-        <v>79090</v>
+        <v>79092</v>
       </c>
       <c r="D918" t="n">
         <v>13383</v>
       </c>
       <c r="E918" t="n">
-        <v>392037725</v>
+        <v>392041864</v>
       </c>
       <c r="F918" t="inlineStr">
         <is>
@@ -47575,13 +47575,13 @@
         </is>
       </c>
       <c r="C925" t="n">
-        <v>12203</v>
+        <v>12204</v>
       </c>
       <c r="D925" t="n">
         <v>1959</v>
       </c>
       <c r="E925" t="n">
-        <v>76281330</v>
+        <v>76288270</v>
       </c>
       <c r="F925" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-05-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3868,13 +3868,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1795</v>
+        <v>1797</v>
       </c>
       <c r="D68" t="n">
         <v>299</v>
       </c>
       <c r="E68" t="n">
-        <v>15915294</v>
+        <v>16009548</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62518</v>
+        <v>62519</v>
       </c>
       <c r="D108" t="n">
         <v>10955</v>
       </c>
       <c r="E108" t="n">
-        <v>340663237</v>
+        <v>340664380</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88477</v>
+        <v>88479</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216767689</v>
+        <v>216769579</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -9886,13 +9886,13 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>20398</v>
+        <v>20399</v>
       </c>
       <c r="D186" t="n">
         <v>4510</v>
       </c>
       <c r="E186" t="n">
-        <v>37267359</v>
+        <v>37274929</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -10855,13 +10855,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>29941</v>
+        <v>29942</v>
       </c>
       <c r="D205" t="n">
         <v>5716</v>
       </c>
       <c r="E205" t="n">
-        <v>156347147</v>
+        <v>156350725</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -14323,13 +14323,13 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>9011</v>
+        <v>9012</v>
       </c>
       <c r="D273" t="n">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="E273" t="n">
-        <v>43986444</v>
+        <v>43996444</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
@@ -19984,13 +19984,13 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>16792</v>
+        <v>16793</v>
       </c>
       <c r="D384" t="n">
         <v>3259</v>
       </c>
       <c r="E384" t="n">
-        <v>80750829</v>
+        <v>80758794</v>
       </c>
       <c r="F384" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71277</v>
+        <v>71278</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110315180</v>
+        <v>110315721</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416827</v>
+        <v>416828</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725495972</v>
+        <v>725501172</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292208</v>
+        <v>292218</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1772824371</v>
+        <v>1772898069</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230783</v>
+        <v>230784</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1823755304</v>
+        <v>1823763804</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184275</v>
+        <v>184280</v>
       </c>
       <c r="D505" t="n">
-        <v>27738</v>
+        <v>27739</v>
       </c>
       <c r="E505" t="n">
-        <v>332761117</v>
+        <v>332783436</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71212</v>
+        <v>71213</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287766959</v>
+        <v>287772436</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26614,13 +26614,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>142811</v>
+        <v>142812</v>
       </c>
       <c r="D514" t="n">
         <v>23613</v>
       </c>
       <c r="E514" t="n">
-        <v>244601927</v>
+        <v>244603015</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56113</v>
+        <v>56114</v>
       </c>
       <c r="D520" t="n">
         <v>8770</v>
       </c>
       <c r="E520" t="n">
-        <v>254180222</v>
+        <v>254184625</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39933</v>
+        <v>39935</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60385247</v>
+        <v>60390275</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12411</v>
+        <v>12412</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40580089</v>
+        <v>40642757</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -31153,13 +31153,13 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>32187</v>
+        <v>32191</v>
       </c>
       <c r="D603" t="n">
-        <v>6078</v>
+        <v>6079</v>
       </c>
       <c r="E603" t="n">
-        <v>170477785</v>
+        <v>170496846</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163438</v>
+        <v>163439</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278431354</v>
+        <v>278442560</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73210</v>
+        <v>73212</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367230138</v>
+        <v>367246535</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -35845,13 +35845,13 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>11037</v>
+        <v>11038</v>
       </c>
       <c r="D695" t="n">
         <v>2194</v>
       </c>
       <c r="E695" t="n">
-        <v>48904037</v>
+        <v>48914037</v>
       </c>
       <c r="F695" t="inlineStr">
         <is>
@@ -46351,13 +46351,13 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>81811</v>
+        <v>81813</v>
       </c>
       <c r="D901" t="n">
         <v>13203</v>
       </c>
       <c r="E901" t="n">
-        <v>443377982</v>
+        <v>443486042</v>
       </c>
       <c r="F901" t="inlineStr">
         <is>
@@ -46504,13 +46504,13 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>59760</v>
+        <v>59761</v>
       </c>
       <c r="D904" t="n">
         <v>8975</v>
       </c>
       <c r="E904" t="n">
-        <v>334732534</v>
+        <v>334806309</v>
       </c>
       <c r="F904" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-23 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62519</v>
+        <v>62520</v>
       </c>
       <c r="D108" t="n">
         <v>10955</v>
       </c>
       <c r="E108" t="n">
-        <v>340664380</v>
+        <v>340718916</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71279</v>
+        <v>71283</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110317269</v>
+        <v>110329263</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18880</v>
+        <v>18884</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75348959</v>
+        <v>75370883</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -20851,13 +20851,13 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>16950</v>
+        <v>16953</v>
       </c>
       <c r="D401" t="n">
         <v>2945</v>
       </c>
       <c r="E401" t="n">
-        <v>50842697</v>
+        <v>50862471</v>
       </c>
       <c r="F401" t="inlineStr">
         <is>
@@ -21106,13 +21106,13 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>6300</v>
+        <v>6301</v>
       </c>
       <c r="D406" t="n">
         <v>911</v>
       </c>
       <c r="E406" t="n">
-        <v>19499128</v>
+        <v>19502085</v>
       </c>
       <c r="F406" t="inlineStr">
         <is>
@@ -21208,13 +21208,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>9346</v>
+        <v>9348</v>
       </c>
       <c r="D408" t="n">
         <v>1304</v>
       </c>
       <c r="E408" t="n">
-        <v>23840698</v>
+        <v>23899308</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -24523,13 +24523,13 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D473" t="n">
         <v>66</v>
       </c>
       <c r="E473" t="n">
-        <v>18624611</v>
+        <v>18988775</v>
       </c>
       <c r="F473" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416845</v>
+        <v>416847</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725561174</v>
+        <v>725568806</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -24778,13 +24778,13 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D478" t="n">
         <v>23</v>
       </c>
       <c r="E478" t="n">
-        <v>737225</v>
+        <v>770088</v>
       </c>
       <c r="F478" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292235</v>
+        <v>292241</v>
       </c>
       <c r="D484" t="n">
         <v>42567</v>
       </c>
       <c r="E484" t="n">
-        <v>1773134394</v>
+        <v>1773158231</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230793</v>
+        <v>230800</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1823854114</v>
+        <v>1824293037</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -25441,13 +25441,13 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>12261</v>
+        <v>12262</v>
       </c>
       <c r="D491" t="n">
         <v>1839</v>
       </c>
       <c r="E491" t="n">
-        <v>76190156</v>
+        <v>76195954</v>
       </c>
       <c r="F491" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184280</v>
+        <v>184281</v>
       </c>
       <c r="D505" t="n">
         <v>27739</v>
       </c>
       <c r="E505" t="n">
-        <v>332783436</v>
+        <v>332788386</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62229</v>
+        <v>62230</v>
       </c>
       <c r="D509" t="n">
         <v>11293</v>
       </c>
       <c r="E509" t="n">
-        <v>299519446</v>
+        <v>299538829</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -33550,13 +33550,13 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>43792</v>
+        <v>43796</v>
       </c>
       <c r="D650" t="n">
         <v>9334</v>
       </c>
       <c r="E650" t="n">
-        <v>79590543</v>
+        <v>79596543</v>
       </c>
       <c r="F650" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -4837,13 +4837,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>14392</v>
+        <v>14393</v>
       </c>
       <c r="D87" t="n">
         <v>2776</v>
       </c>
       <c r="E87" t="n">
-        <v>69662774</v>
+        <v>69668520</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -12640,13 +12640,13 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>21378</v>
+        <v>21379</v>
       </c>
       <c r="D240" t="n">
         <v>4844</v>
       </c>
       <c r="E240" t="n">
-        <v>39860171</v>
+        <v>39860848</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -17230,13 +17230,13 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>24068</v>
+        <v>24069</v>
       </c>
       <c r="D330" t="n">
         <v>4530</v>
       </c>
       <c r="E330" t="n">
-        <v>149828624</v>
+        <v>149830687</v>
       </c>
       <c r="F330" t="inlineStr">
         <is>
@@ -20749,13 +20749,13 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>18884</v>
+        <v>18886</v>
       </c>
       <c r="D399" t="n">
         <v>3383</v>
       </c>
       <c r="E399" t="n">
-        <v>75370883</v>
+        <v>75390235</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -24472,13 +24472,13 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>73763</v>
+        <v>73764</v>
       </c>
       <c r="D472" t="n">
         <v>11997</v>
       </c>
       <c r="E472" t="n">
-        <v>387497603</v>
+        <v>387507603</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -24574,13 +24574,13 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>74998</v>
+        <v>74999</v>
       </c>
       <c r="D474" t="n">
         <v>11550</v>
       </c>
       <c r="E474" t="n">
-        <v>435635809</v>
+        <v>435645809</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416849</v>
+        <v>416857</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725578248</v>
+        <v>725600263</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292247</v>
+        <v>292254</v>
       </c>
       <c r="D484" t="n">
         <v>42568</v>
       </c>
       <c r="E484" t="n">
-        <v>1773216731</v>
+        <v>1773475672</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230801</v>
+        <v>230808</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1824493037</v>
+        <v>1824535259</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184282</v>
+        <v>184283</v>
       </c>
       <c r="D505" t="n">
         <v>27740</v>
       </c>
       <c r="E505" t="n">
-        <v>332790736</v>
+        <v>332791036</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26359,13 +26359,13 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>62276</v>
+        <v>62279</v>
       </c>
       <c r="D509" t="n">
         <v>11318</v>
       </c>
       <c r="E509" t="n">
-        <v>299983793</v>
+        <v>299998072</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71227</v>
+        <v>71230</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>287875047</v>
+        <v>287883309</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -28195,13 +28195,13 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>25087</v>
+        <v>25088</v>
       </c>
       <c r="D545" t="n">
         <v>6170</v>
       </c>
       <c r="E545" t="n">
-        <v>92608318</v>
+        <v>92615653</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -35845,13 +35845,13 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>11038</v>
+        <v>11039</v>
       </c>
       <c r="D695" t="n">
         <v>2194</v>
       </c>
       <c r="E695" t="n">
-        <v>48914037</v>
+        <v>49064700</v>
       </c>
       <c r="F695" t="inlineStr">
         <is>
@@ -40996,13 +40996,13 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="D796" t="n">
         <v>7448</v>
       </c>
       <c r="E796" t="n">
-        <v>210446178</v>
+        <v>210456178</v>
       </c>
       <c r="F796" t="inlineStr">
         <is>
@@ -42169,13 +42169,13 @@
         </is>
       </c>
       <c r="C819" t="n">
-        <v>14928</v>
+        <v>14929</v>
       </c>
       <c r="D819" t="n">
         <v>2491</v>
       </c>
       <c r="E819" t="n">
-        <v>82089300</v>
+        <v>82140947</v>
       </c>
       <c r="F819" t="inlineStr">
         <is>
@@ -46657,13 +46657,13 @@
         </is>
       </c>
       <c r="C907" t="n">
-        <v>3558</v>
+        <v>3559</v>
       </c>
       <c r="D907" t="n">
         <v>486</v>
       </c>
       <c r="E907" t="n">
-        <v>13887813</v>
+        <v>13897813</v>
       </c>
       <c r="F907" t="inlineStr">
         <is>
@@ -48748,13 +48748,13 @@
         </is>
       </c>
       <c r="C948" t="n">
-        <v>19073</v>
+        <v>19074</v>
       </c>
       <c r="D948" t="n">
         <v>3311</v>
       </c>
       <c r="E948" t="n">
-        <v>93868358</v>
+        <v>93883351</v>
       </c>
       <c r="F948" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2022-06-21 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-categorie-juridique-latest.xlsx
@@ -3868,13 +3868,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1799</v>
+        <v>1801</v>
       </c>
       <c r="D68" t="n">
         <v>299</v>
       </c>
       <c r="E68" t="n">
-        <v>16082974</v>
+        <v>16177228</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -5908,13 +5908,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>62521</v>
+        <v>62522</v>
       </c>
       <c r="D108" t="n">
         <v>10955</v>
       </c>
       <c r="E108" t="n">
-        <v>340824916</v>
+        <v>340826059</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -6214,13 +6214,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>88479</v>
+        <v>88481</v>
       </c>
       <c r="D114" t="n">
         <v>14314</v>
       </c>
       <c r="E114" t="n">
-        <v>216769579</v>
+        <v>216771469</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -9886,13 +9886,13 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>20400</v>
+        <v>20401</v>
       </c>
       <c r="D186" t="n">
         <v>4510</v>
       </c>
       <c r="E186" t="n">
-        <v>37276429</v>
+        <v>37283999</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -10855,13 +10855,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>29942</v>
+        <v>29943</v>
       </c>
       <c r="D205" t="n">
         <v>5716</v>
       </c>
       <c r="E205" t="n">
-        <v>156350725</v>
+        <v>156354303</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -14323,13 +14323,13 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>9013</v>
+        <v>9014</v>
       </c>
       <c r="D273" t="n">
         <v>1763</v>
       </c>
       <c r="E273" t="n">
-        <v>43997558</v>
+        <v>44007558</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
@@ -19984,13 +19984,13 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>16793</v>
+        <v>16794</v>
       </c>
       <c r="D384" t="n">
         <v>3259</v>
       </c>
       <c r="E384" t="n">
-        <v>80758794</v>
+        <v>80766759</v>
       </c>
       <c r="F384" t="inlineStr">
         <is>
@@ -20596,13 +20596,13 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>71283</v>
+        <v>71284</v>
       </c>
       <c r="D396" t="n">
         <v>12436</v>
       </c>
       <c r="E396" t="n">
-        <v>110329263</v>
+        <v>110329804</v>
       </c>
       <c r="F396" t="inlineStr">
         <is>
@@ -24727,13 +24727,13 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>416913</v>
+        <v>416914</v>
       </c>
       <c r="D477" t="n">
         <v>70501</v>
       </c>
       <c r="E477" t="n">
-        <v>725804313</v>
+        <v>725809513</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -25084,13 +25084,13 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>292311</v>
+        <v>292321</v>
       </c>
       <c r="D484" t="n">
         <v>42568</v>
       </c>
       <c r="E484" t="n">
-        <v>1774499477</v>
+        <v>1774573175</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -25237,13 +25237,13 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>230878</v>
+        <v>230879</v>
       </c>
       <c r="D487" t="n">
         <v>33851</v>
       </c>
       <c r="E487" t="n">
-        <v>1826241241</v>
+        <v>1826249741</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -26155,13 +26155,13 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>184288</v>
+        <v>184293</v>
       </c>
       <c r="D505" t="n">
         <v>27740</v>
       </c>
       <c r="E505" t="n">
-        <v>332795563</v>
+        <v>332817882</v>
       </c>
       <c r="F505" t="inlineStr">
         <is>
@@ -26461,13 +26461,13 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>71242</v>
+        <v>71243</v>
       </c>
       <c r="D511" t="n">
         <v>10924</v>
       </c>
       <c r="E511" t="n">
-        <v>288034966</v>
+        <v>288040443</v>
       </c>
       <c r="F511" t="inlineStr">
         <is>
@@ -26614,13 +26614,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>142816</v>
+        <v>142817</v>
       </c>
       <c r="D514" t="n">
         <v>23613</v>
       </c>
       <c r="E514" t="n">
-        <v>244623334</v>
+        <v>244624422</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -26920,13 +26920,13 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>56120</v>
+        <v>56121</v>
       </c>
       <c r="D520" t="n">
         <v>8770</v>
       </c>
       <c r="E520" t="n">
-        <v>254526317</v>
+        <v>254530720</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -28552,13 +28552,13 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>39935</v>
+        <v>39937</v>
       </c>
       <c r="D552" t="n">
         <v>7155</v>
       </c>
       <c r="E552" t="n">
-        <v>60390275</v>
+        <v>60395303</v>
       </c>
       <c r="F552" t="inlineStr">
         <is>
@@ -28807,13 +28807,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>12417</v>
+        <v>12418</v>
       </c>
       <c r="D557" t="n">
         <v>2144</v>
       </c>
       <c r="E557" t="n">
-        <v>40823580</v>
+        <v>40886248</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -31153,13 +31153,13 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>32191</v>
+        <v>32195</v>
       </c>
       <c r="D603" t="n">
         <v>6079</v>
       </c>
       <c r="E603" t="n">
-        <v>170496846</v>
+        <v>170515907</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -34009,13 +34009,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>163439</v>
+        <v>163440</v>
       </c>
       <c r="D659" t="n">
         <v>36203</v>
       </c>
       <c r="E659" t="n">
-        <v>278442560</v>
+        <v>278453766</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -34366,13 +34366,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>73214</v>
+        <v>73216</v>
       </c>
       <c r="D666" t="n">
         <v>14361</v>
       </c>
       <c r="E666" t="n">
-        <v>367268472</v>
+        <v>367284869</v>
       </c>
       <c r="F666" t="inlineStr">
         <is>
@@ -35845,13 +35845,13 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>11041</v>
+        <v>11042</v>
       </c>
       <c r="D695" t="n">
         <v>2194</v>
       </c>
       <c r="E695" t="n">
-        <v>49084051</v>
+        <v>49094051</v>
       </c>
       <c r="F695" t="inlineStr">
         <is>
@@ -46351,13 +46351,13 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>81813</v>
+        <v>81815</v>
       </c>
       <c r="D901" t="n">
         <v>13203</v>
       </c>
       <c r="E901" t="n">
-        <v>443486042</v>
+        <v>443594102</v>
       </c>
       <c r="F901" t="inlineStr">
         <is>
@@ -46504,13 +46504,13 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>59762</v>
+        <v>59763</v>
       </c>
       <c r="D904" t="n">
         <v>8975</v>
       </c>
       <c r="E904" t="n">
-        <v>334901835</v>
+        <v>334975610</v>
       </c>
       <c r="F904" t="inlineStr">
         <is>

</xml_diff>